<commit_message>
2nd half of initial DoE
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0974C12-65FD-2C4B-9A60-6DC99E3A6D76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E318CC59-D727-CD41-9DE9-3190D0D95337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
   <si>
     <t>Sample</t>
   </si>
@@ -204,16 +204,13 @@
     <t>Arlypon TT</t>
   </si>
   <si>
-    <t>Viscosity_10/Pa.s</t>
+    <t>Stability_Test</t>
   </si>
   <si>
-    <t>Viscosity_1/Pa.s</t>
+    <t>Viscosity_1/cP</t>
   </si>
   <si>
-    <t>Shear_thinning</t>
-  </si>
-  <si>
-    <t>Stability_Test</t>
+    <t>Viscosity_10/cP</t>
   </si>
 </sst>
 </file>
@@ -288,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -318,9 +315,6 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -637,11 +631,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:X79"/>
+  <dimension ref="A1:W79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="112" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Q81" sqref="Q81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="V50" sqref="V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,10 +662,9 @@
     <col min="21" max="21" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>36</v>
       </c>
@@ -730,22 +723,19 @@
         <v>54</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="U1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="15" t="s">
+      <c r="V1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="W1" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="X1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -818,12 +808,8 @@
         <f>IF(T2=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
-      <c r="X2" s="2" t="str">
-        <f>IF(T2=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10">
         <v>2</v>
       </c>
@@ -896,12 +882,8 @@
         <f t="shared" ref="W3:W43" si="2">IF(T3=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
-      <c r="X3" s="2" t="str">
-        <f t="shared" ref="X3:X43" si="3">IF(T3=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -974,12 +956,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X4" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="10">
         <v>4</v>
       </c>
@@ -1052,12 +1030,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X5" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>5</v>
       </c>
@@ -1130,12 +1104,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X6" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="10">
         <v>6</v>
       </c>
@@ -1208,12 +1178,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X7" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>7</v>
       </c>
@@ -1286,12 +1252,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X8" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -1364,12 +1326,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X9" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>9</v>
       </c>
@@ -1442,12 +1400,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X10" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10">
         <v>10</v>
       </c>
@@ -1520,12 +1474,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X11" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>11</v>
       </c>
@@ -1598,12 +1548,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X12" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10">
         <v>12</v>
       </c>
@@ -1676,12 +1622,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X13" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>13</v>
       </c>
@@ -1754,12 +1696,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X14" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10">
         <v>14</v>
       </c>
@@ -1832,12 +1770,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X15" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>15</v>
       </c>
@@ -1910,12 +1844,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X16" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="17" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10">
         <v>16</v>
       </c>
@@ -1988,12 +1918,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X17" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="18" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>17</v>
       </c>
@@ -2066,12 +1992,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X18" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="19" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="10">
         <v>18</v>
       </c>
@@ -2144,12 +2066,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X19" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="20" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>19</v>
       </c>
@@ -2222,12 +2140,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X20" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="21" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="10">
         <v>20</v>
       </c>
@@ -2300,12 +2214,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X21" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="22" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>21</v>
       </c>
@@ -2378,12 +2288,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X22" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="23" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -2456,12 +2362,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X23" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="24" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>23</v>
       </c>
@@ -2534,12 +2436,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X24" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="25" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="10">
         <v>24</v>
       </c>
@@ -2612,12 +2510,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X25" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="26" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
         <v>25</v>
       </c>
@@ -2690,12 +2584,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X26" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="27" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="10">
         <v>26</v>
       </c>
@@ -2768,12 +2658,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X27" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="28" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <v>27</v>
       </c>
@@ -2846,12 +2732,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X28" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10">
         <v>28</v>
       </c>
@@ -2924,12 +2806,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X29" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <v>29</v>
       </c>
@@ -3002,12 +2880,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X30" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10">
         <v>30</v>
       </c>
@@ -3080,12 +2954,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X31" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -3158,12 +3028,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X32" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="33" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="10">
         <v>32</v>
       </c>
@@ -3236,12 +3102,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X33" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="34" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>33</v>
       </c>
@@ -3314,12 +3176,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X34" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="35" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="10">
         <v>34</v>
       </c>
@@ -3392,12 +3250,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X35" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="36" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <v>35</v>
       </c>
@@ -3470,12 +3324,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X36" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="10">
         <v>36</v>
       </c>
@@ -3548,12 +3398,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X37" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10">
         <v>37</v>
       </c>
@@ -3617,20 +3463,14 @@
       <c r="U38" s="2">
         <v>23</v>
       </c>
-      <c r="V38" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="W38" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="X38" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="V38" s="2">
+        <v>92</v>
+      </c>
+      <c r="W38" s="2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="10">
         <v>38</v>
       </c>
@@ -3703,12 +3543,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X39" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <v>39</v>
       </c>
@@ -3781,12 +3617,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X40" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10">
         <v>40</v>
       </c>
@@ -3850,20 +3682,14 @@
       <c r="U41" s="2">
         <v>1229</v>
       </c>
-      <c r="V41" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="W41" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="X41" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="V41" s="2">
+        <v>5</v>
+      </c>
+      <c r="W41" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10">
         <v>41</v>
       </c>
@@ -3936,12 +3762,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X42" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:23" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10">
         <v>42</v>
       </c>
@@ -4014,12 +3836,8 @@
         <f t="shared" si="2"/>
         <v>NA</v>
       </c>
-      <c r="X43" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
         <v>43</v>
       </c>
@@ -4092,12 +3910,8 @@
         <f>IF(T44=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
-      <c r="X44" s="2" t="str">
-        <f>IF(T44=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A45" s="10">
         <v>44</v>
       </c>
@@ -4159,23 +3973,19 @@
         <v>0</v>
       </c>
       <c r="U45" s="2" t="str">
-        <f t="shared" ref="U45:U79" si="4">IF(T45=FALSE, "NA", "")</f>
+        <f t="shared" ref="U45:U79" si="3">IF(T45=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V45" s="2" t="str">
-        <f t="shared" ref="V45:V67" si="5">IF(T45=FALSE, "NA", "")</f>
+        <f t="shared" ref="V45:V79" si="4">IF(T45=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W45" s="2" t="str">
-        <f t="shared" ref="W45:W67" si="6">IF(T45=FALSE, "NA", "")</f>
+        <f t="shared" ref="W45:W79" si="5">IF(T45=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
-      <c r="X45" s="2" t="str">
-        <f t="shared" ref="X45:X67" si="7">IF(T45=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A46" s="10">
         <v>45</v>
       </c>
@@ -4237,23 +4047,19 @@
         <v>0</v>
       </c>
       <c r="U46" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V46" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V46" s="2" t="str">
+      <c r="W46" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W46" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X46" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A47" s="10">
         <v>46</v>
       </c>
@@ -4315,23 +4121,19 @@
         <v>0</v>
       </c>
       <c r="U47" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V47" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V47" s="2" t="str">
+      <c r="W47" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W47" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X47" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
         <v>47</v>
       </c>
@@ -4393,23 +4195,19 @@
         <v>0</v>
       </c>
       <c r="U48" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V48" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V48" s="2" t="str">
+      <c r="W48" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W48" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X48" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A49" s="10">
         <v>48</v>
       </c>
@@ -4471,23 +4269,19 @@
         <v>0</v>
       </c>
       <c r="U49" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V49" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V49" s="2" t="str">
+      <c r="W49" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W49" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X49" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A50" s="10">
         <v>49</v>
       </c>
@@ -4552,19 +4346,15 @@
         <v>491</v>
       </c>
       <c r="V50" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W50" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W50" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X50" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A51" s="10">
         <v>50</v>
       </c>
@@ -4629,19 +4419,15 @@
         <v>299</v>
       </c>
       <c r="V51" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W51" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W51" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X51" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A52" s="10">
         <v>51</v>
       </c>
@@ -4703,23 +4489,19 @@
         <v>0</v>
       </c>
       <c r="U52" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V52" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V52" s="2" t="str">
+      <c r="W52" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W52" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X52" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A53" s="10">
         <v>52</v>
       </c>
@@ -4781,23 +4563,19 @@
         <v>0</v>
       </c>
       <c r="U53" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V53" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V53" s="2" t="str">
+      <c r="W53" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W53" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X53" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A54" s="10">
         <v>53</v>
       </c>
@@ -4862,19 +4640,15 @@
         <v>25</v>
       </c>
       <c r="V54" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W54" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W54" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X54" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A55" s="10">
         <v>54</v>
       </c>
@@ -4936,23 +4710,19 @@
         <v>0</v>
       </c>
       <c r="U55" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V55" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V55" s="2" t="str">
+      <c r="W55" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W55" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X55" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A56" s="10">
         <v>55</v>
       </c>
@@ -5014,23 +4784,19 @@
         <v>0</v>
       </c>
       <c r="U56" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V56" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V56" s="2" t="str">
+      <c r="W56" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W56" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X56" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A57" s="10">
         <v>56</v>
       </c>
@@ -5095,19 +4861,15 @@
         <v>33</v>
       </c>
       <c r="V57" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W57" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W57" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X57" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A58" s="10">
         <v>57</v>
       </c>
@@ -5172,19 +4934,15 @@
         <v>35</v>
       </c>
       <c r="V58" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W58" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W58" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X58" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A59" s="10">
         <v>58</v>
       </c>
@@ -5249,19 +5007,15 @@
         <v>16</v>
       </c>
       <c r="V59" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W59" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W59" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X59" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="10">
         <v>59</v>
       </c>
@@ -5326,19 +5080,15 @@
         <v>48</v>
       </c>
       <c r="V60" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W60" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W60" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X60" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A61" s="10">
         <v>60</v>
       </c>
@@ -5403,19 +5153,15 @@
         <v>332</v>
       </c>
       <c r="V61" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W61" s="2" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="W61" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="X61" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A62" s="10">
         <v>61</v>
       </c>
@@ -5477,23 +5223,19 @@
         <v>0</v>
       </c>
       <c r="U62" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V62" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V62" s="2" t="str">
+      <c r="W62" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W62" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X62" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A63" s="10">
         <v>62</v>
       </c>
@@ -5555,23 +5297,19 @@
         <v>0</v>
       </c>
       <c r="U63" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V63" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V63" s="2" t="str">
+      <c r="W63" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W63" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X63" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A64" s="10">
         <v>63</v>
       </c>
@@ -5633,23 +5371,19 @@
         <v>0</v>
       </c>
       <c r="U64" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V64" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V64" s="2" t="str">
+      <c r="W64" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W64" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X64" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A65" s="10">
         <v>64</v>
       </c>
@@ -5711,23 +5445,19 @@
         <v>0</v>
       </c>
       <c r="U65" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V65" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V65" s="2" t="str">
+      <c r="W65" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W65" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X65" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A66" s="10">
         <v>65</v>
       </c>
@@ -5789,23 +5519,19 @@
         <v>0</v>
       </c>
       <c r="U66" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V66" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V66" s="2" t="str">
+      <c r="W66" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W66" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X66" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A67" s="10">
         <v>66</v>
       </c>
@@ -5867,80 +5593,898 @@
         <v>0</v>
       </c>
       <c r="U67" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V67" s="2" t="str">
         <f t="shared" si="4"/>
         <v>NA</v>
       </c>
-      <c r="V67" s="2" t="str">
+      <c r="W67" s="2" t="str">
         <f t="shared" si="5"/>
         <v>NA</v>
       </c>
-      <c r="W67" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
-      </c>
-      <c r="X67" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A68" s="10">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B68" s="11">
+        <v>0</v>
+      </c>
+      <c r="C68" s="11">
+        <v>11.960952337720601</v>
+      </c>
+      <c r="D68" s="11">
+        <v>0</v>
+      </c>
+      <c r="E68" s="11">
+        <v>0</v>
+      </c>
+      <c r="F68" s="11">
+        <v>0</v>
+      </c>
+      <c r="G68" s="11">
+        <v>12.314377303011</v>
+      </c>
+      <c r="H68" s="11">
+        <v>0</v>
+      </c>
+      <c r="I68" s="11">
+        <v>0</v>
+      </c>
+      <c r="J68" s="11">
+        <v>0</v>
+      </c>
+      <c r="K68" s="11">
+        <v>0</v>
+      </c>
+      <c r="L68" s="11">
+        <v>0</v>
+      </c>
+      <c r="M68" s="11">
+        <v>0</v>
+      </c>
+      <c r="N68" s="11">
+        <v>1.7938994450346699</v>
+      </c>
+      <c r="O68" s="11">
+        <v>0</v>
+      </c>
+      <c r="P68" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="11">
+        <v>0</v>
+      </c>
+      <c r="R68" s="11">
+        <v>0</v>
+      </c>
+      <c r="S68" s="11">
+        <v>2.3464302103302099</v>
+      </c>
+      <c r="T68" t="b">
+        <v>1</v>
+      </c>
+      <c r="U68" s="2">
+        <v>32</v>
+      </c>
+      <c r="V68" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W68" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="69" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A69" s="10">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B69" s="11">
+        <v>0</v>
+      </c>
+      <c r="C69" s="11">
+        <v>13.433824587522601</v>
+      </c>
+      <c r="D69" s="11">
+        <v>0</v>
+      </c>
+      <c r="E69" s="11">
+        <v>0</v>
+      </c>
+      <c r="F69" s="11">
+        <v>0</v>
+      </c>
+      <c r="G69" s="11">
+        <v>9.6518228363670708</v>
+      </c>
+      <c r="H69" s="11">
+        <v>0</v>
+      </c>
+      <c r="I69" s="11">
+        <v>0</v>
+      </c>
+      <c r="J69" s="11">
+        <v>0</v>
+      </c>
+      <c r="K69" s="11">
+        <v>0</v>
+      </c>
+      <c r="L69" s="11">
+        <v>0</v>
+      </c>
+      <c r="M69" s="11">
+        <v>0</v>
+      </c>
+      <c r="N69" s="11">
+        <v>2.1466719123267102</v>
+      </c>
+      <c r="O69" s="11">
+        <v>0</v>
+      </c>
+      <c r="P69" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="11">
+        <v>0</v>
+      </c>
+      <c r="R69" s="11">
+        <v>0</v>
+      </c>
+      <c r="S69" s="11">
+        <v>4.3512316065588701</v>
+      </c>
+      <c r="T69" t="b">
+        <v>1</v>
+      </c>
+      <c r="U69" s="2">
+        <v>1404</v>
+      </c>
+      <c r="V69" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W69" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A70" s="10">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B70" s="11">
+        <v>0</v>
+      </c>
+      <c r="C70" s="11">
+        <v>8.8808327727084997</v>
+      </c>
+      <c r="D70" s="11">
+        <v>0</v>
+      </c>
+      <c r="E70" s="11">
+        <v>0</v>
+      </c>
+      <c r="F70" s="11">
+        <v>0</v>
+      </c>
+      <c r="G70" s="11">
+        <v>13.0731223318641</v>
+      </c>
+      <c r="H70" s="11">
+        <v>0</v>
+      </c>
+      <c r="I70" s="11">
+        <v>0</v>
+      </c>
+      <c r="J70" s="11">
+        <v>0</v>
+      </c>
+      <c r="K70" s="11">
+        <v>0</v>
+      </c>
+      <c r="L70" s="11">
+        <v>0</v>
+      </c>
+      <c r="M70" s="11">
+        <v>0</v>
+      </c>
+      <c r="N70" s="11">
+        <v>1.30889296393886</v>
+      </c>
+      <c r="O70" s="11">
+        <v>0</v>
+      </c>
+      <c r="P70" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q70" s="11">
+        <v>0</v>
+      </c>
+      <c r="R70" s="11">
+        <v>0</v>
+      </c>
+      <c r="S70" s="11">
+        <v>2.1890725874475301</v>
+      </c>
+      <c r="T70" t="b">
+        <v>1</v>
+      </c>
+      <c r="U70" s="2">
+        <v>36</v>
+      </c>
+      <c r="V70" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W70" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A71" s="10">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B71" s="11">
+        <v>0</v>
+      </c>
+      <c r="C71" s="11">
+        <v>11.6816632747274</v>
+      </c>
+      <c r="D71" s="11">
+        <v>0</v>
+      </c>
+      <c r="E71" s="11">
+        <v>0</v>
+      </c>
+      <c r="F71" s="11">
+        <v>0</v>
+      </c>
+      <c r="G71" s="11">
+        <v>9.8591083673005304</v>
+      </c>
+      <c r="H71" s="11">
+        <v>0</v>
+      </c>
+      <c r="I71" s="11">
+        <v>0</v>
+      </c>
+      <c r="J71" s="11">
+        <v>0</v>
+      </c>
+      <c r="K71" s="11">
+        <v>0</v>
+      </c>
+      <c r="L71" s="11">
+        <v>0</v>
+      </c>
+      <c r="M71" s="11">
+        <v>0</v>
+      </c>
+      <c r="N71" s="11">
+        <v>1.4907441195312801</v>
+      </c>
+      <c r="O71" s="11">
+        <v>0</v>
+      </c>
+      <c r="P71" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q71" s="11">
+        <v>0</v>
+      </c>
+      <c r="R71" s="11">
+        <v>0</v>
+      </c>
+      <c r="S71" s="11">
+        <v>1.6590539394784201</v>
+      </c>
+      <c r="T71" t="b">
+        <v>1</v>
+      </c>
+      <c r="U71" s="2">
+        <v>20</v>
+      </c>
+      <c r="V71" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W71" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A72" s="10">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B72" s="11">
+        <v>0</v>
+      </c>
+      <c r="C72" s="11">
+        <v>10.144285854046201</v>
+      </c>
+      <c r="D72" s="11">
+        <v>0</v>
+      </c>
+      <c r="E72" s="11">
+        <v>0</v>
+      </c>
+      <c r="F72" s="11">
+        <v>0</v>
+      </c>
+      <c r="G72" s="11">
+        <v>13.263972089495701</v>
+      </c>
+      <c r="H72" s="11">
+        <v>0</v>
+      </c>
+      <c r="I72" s="11">
+        <v>0</v>
+      </c>
+      <c r="J72" s="11">
+        <v>0</v>
+      </c>
+      <c r="K72" s="11">
+        <v>0</v>
+      </c>
+      <c r="L72" s="11">
+        <v>0</v>
+      </c>
+      <c r="M72" s="11">
+        <v>0</v>
+      </c>
+      <c r="N72" s="11">
+        <v>2.4104254733546702</v>
+      </c>
+      <c r="O72" s="11">
+        <v>0</v>
+      </c>
+      <c r="P72" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="11">
+        <v>0</v>
+      </c>
+      <c r="R72" s="11">
+        <v>0</v>
+      </c>
+      <c r="S72" s="11">
+        <v>3.1833533014789399</v>
+      </c>
+      <c r="T72" t="b">
+        <v>1</v>
+      </c>
+      <c r="U72" s="2">
+        <v>479</v>
+      </c>
+      <c r="V72" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W72" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A73" s="10">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B73" s="11">
+        <v>0</v>
+      </c>
+      <c r="C73" s="11">
+        <v>8.5422370363173599</v>
+      </c>
+      <c r="D73" s="11">
+        <v>0</v>
+      </c>
+      <c r="E73" s="11">
+        <v>0</v>
+      </c>
+      <c r="F73" s="11">
+        <v>0</v>
+      </c>
+      <c r="G73" s="11">
+        <v>12.609230126374699</v>
+      </c>
+      <c r="H73" s="11">
+        <v>0</v>
+      </c>
+      <c r="I73" s="11">
+        <v>0</v>
+      </c>
+      <c r="J73" s="11">
+        <v>0</v>
+      </c>
+      <c r="K73" s="11">
+        <v>0</v>
+      </c>
+      <c r="L73" s="11">
+        <v>0</v>
+      </c>
+      <c r="M73" s="11">
+        <v>0</v>
+      </c>
+      <c r="N73" s="11">
+        <v>2.7818756383172101</v>
+      </c>
+      <c r="O73" s="11">
+        <v>0</v>
+      </c>
+      <c r="P73" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q73" s="11">
+        <v>0</v>
+      </c>
+      <c r="R73" s="11">
+        <v>0</v>
+      </c>
+      <c r="S73" s="11">
+        <v>4.3637264914777898</v>
+      </c>
+      <c r="T73" t="b">
+        <v>0</v>
+      </c>
+      <c r="U73" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V73" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W73" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A74" s="10">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B74" s="11">
+        <v>0</v>
+      </c>
+      <c r="C74" s="11">
+        <v>0</v>
+      </c>
+      <c r="D74" s="11">
+        <v>7.9909864833298299</v>
+      </c>
+      <c r="E74" s="11">
+        <v>0</v>
+      </c>
+      <c r="F74" s="11">
+        <v>12.5605679587618</v>
+      </c>
+      <c r="G74" s="11">
+        <v>0</v>
+      </c>
+      <c r="H74" s="11">
+        <v>0</v>
+      </c>
+      <c r="I74" s="11">
+        <v>0</v>
+      </c>
+      <c r="J74" s="11">
+        <v>0</v>
+      </c>
+      <c r="K74" s="11">
+        <v>0</v>
+      </c>
+      <c r="L74" s="11">
+        <v>0</v>
+      </c>
+      <c r="M74" s="11">
+        <v>0</v>
+      </c>
+      <c r="N74" s="11">
+        <v>1.8185325618674899</v>
+      </c>
+      <c r="O74" s="11">
+        <v>0</v>
+      </c>
+      <c r="P74" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="11">
+        <v>0</v>
+      </c>
+      <c r="R74" s="11">
+        <v>0</v>
+      </c>
+      <c r="S74" s="11">
+        <v>1.9454653806294899</v>
+      </c>
+      <c r="T74" t="b">
+        <v>0</v>
+      </c>
+      <c r="U74" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V74" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W74" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A75" s="10">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B75" s="11">
+        <v>0</v>
+      </c>
+      <c r="C75" s="11">
+        <v>0</v>
+      </c>
+      <c r="D75" s="11">
+        <v>12.680121593136599</v>
+      </c>
+      <c r="E75" s="11">
+        <v>0</v>
+      </c>
+      <c r="F75" s="11">
+        <v>9.8108759221831505</v>
+      </c>
+      <c r="G75" s="11">
+        <v>0</v>
+      </c>
+      <c r="H75" s="11">
+        <v>0</v>
+      </c>
+      <c r="I75" s="11">
+        <v>0</v>
+      </c>
+      <c r="J75" s="11">
+        <v>0</v>
+      </c>
+      <c r="K75" s="11">
+        <v>0</v>
+      </c>
+      <c r="L75" s="11">
+        <v>0</v>
+      </c>
+      <c r="M75" s="11">
+        <v>0</v>
+      </c>
+      <c r="N75" s="11">
+        <v>2.5422325153993399</v>
+      </c>
+      <c r="O75" s="11">
+        <v>0</v>
+      </c>
+      <c r="P75" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q75" s="11">
+        <v>0</v>
+      </c>
+      <c r="R75" s="11">
+        <v>0</v>
+      </c>
+      <c r="S75" s="11">
+        <v>4.0136714015013402</v>
+      </c>
+      <c r="T75" t="b">
+        <v>0</v>
+      </c>
+      <c r="U75" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V75" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W75" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A76" s="10">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B76" s="11">
+        <v>0</v>
+      </c>
+      <c r="C76" s="11">
+        <v>0</v>
+      </c>
+      <c r="D76" s="11">
+        <v>12.138035073527501</v>
+      </c>
+      <c r="E76" s="11">
+        <v>0</v>
+      </c>
+      <c r="F76" s="11">
+        <v>12.5785359544683</v>
+      </c>
+      <c r="G76" s="11">
+        <v>0</v>
+      </c>
+      <c r="H76" s="11">
+        <v>0</v>
+      </c>
+      <c r="I76" s="11">
+        <v>0</v>
+      </c>
+      <c r="J76" s="11">
+        <v>0</v>
+      </c>
+      <c r="K76" s="11">
+        <v>0</v>
+      </c>
+      <c r="L76" s="11">
+        <v>0</v>
+      </c>
+      <c r="M76" s="11">
+        <v>0</v>
+      </c>
+      <c r="N76" s="11">
+        <v>1.2106638682445701</v>
+      </c>
+      <c r="O76" s="11">
+        <v>0</v>
+      </c>
+      <c r="P76" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="11">
+        <v>0</v>
+      </c>
+      <c r="R76" s="11">
+        <v>0</v>
+      </c>
+      <c r="S76" s="11">
+        <v>4.8236273571708104</v>
+      </c>
+      <c r="T76" t="b">
+        <v>1</v>
+      </c>
+      <c r="U76" s="2">
+        <v>1065</v>
+      </c>
+      <c r="V76" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="W76" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A77" s="10">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B77" s="11">
+        <v>0</v>
+      </c>
+      <c r="C77" s="11">
+        <v>0</v>
+      </c>
+      <c r="D77" s="11">
+        <v>9.0092814854214804</v>
+      </c>
+      <c r="E77" s="11">
+        <v>0</v>
+      </c>
+      <c r="F77" s="11">
+        <v>8.8782587245092195</v>
+      </c>
+      <c r="G77" s="11">
+        <v>0</v>
+      </c>
+      <c r="H77" s="11">
+        <v>0</v>
+      </c>
+      <c r="I77" s="11">
+        <v>0</v>
+      </c>
+      <c r="J77" s="11">
+        <v>0</v>
+      </c>
+      <c r="K77" s="11">
+        <v>0</v>
+      </c>
+      <c r="L77" s="11">
+        <v>0</v>
+      </c>
+      <c r="M77" s="11">
+        <v>0</v>
+      </c>
+      <c r="N77" s="11">
+        <v>2.29412054321371</v>
+      </c>
+      <c r="O77" s="11">
+        <v>0</v>
+      </c>
+      <c r="P77" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="11">
+        <v>0</v>
+      </c>
+      <c r="R77" s="11">
+        <v>0</v>
+      </c>
+      <c r="S77" s="11">
+        <v>2.1853423182023799</v>
+      </c>
+      <c r="T77" t="b">
+        <v>0</v>
+      </c>
+      <c r="U77" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V77" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W77" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A78" s="10">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="B78" s="11">
+        <v>0</v>
+      </c>
+      <c r="C78" s="11">
+        <v>0</v>
+      </c>
+      <c r="D78" s="11">
+        <v>13.1129778481016</v>
+      </c>
+      <c r="E78" s="11">
+        <v>0</v>
+      </c>
+      <c r="F78" s="11">
+        <v>9.2781320911583691</v>
+      </c>
+      <c r="G78" s="11">
+        <v>0</v>
+      </c>
+      <c r="H78" s="11">
+        <v>0</v>
+      </c>
+      <c r="I78" s="11">
+        <v>0</v>
+      </c>
+      <c r="J78" s="11">
+        <v>0</v>
+      </c>
+      <c r="K78" s="11">
+        <v>0</v>
+      </c>
+      <c r="L78" s="11">
+        <v>0</v>
+      </c>
+      <c r="M78" s="11">
+        <v>0</v>
+      </c>
+      <c r="N78" s="11">
+        <v>2.9322035359157002</v>
+      </c>
+      <c r="O78" s="11">
+        <v>0</v>
+      </c>
+      <c r="P78" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q78" s="11">
+        <v>0</v>
+      </c>
+      <c r="R78" s="11">
+        <v>0</v>
+      </c>
+      <c r="S78" s="11">
+        <v>3.5903550887042899</v>
+      </c>
+      <c r="T78" t="b">
+        <v>0</v>
+      </c>
+      <c r="U78" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V78" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W78" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A79" s="10">
         <v>78</v>
+      </c>
+      <c r="B79" s="11">
+        <v>0</v>
+      </c>
+      <c r="C79" s="11">
+        <v>0</v>
+      </c>
+      <c r="D79" s="11">
+        <v>9.1634562147604406</v>
+      </c>
+      <c r="E79" s="11">
+        <v>0</v>
+      </c>
+      <c r="F79" s="11">
+        <v>9.2232327979173991</v>
+      </c>
+      <c r="G79" s="11">
+        <v>0</v>
+      </c>
+      <c r="H79" s="11">
+        <v>0</v>
+      </c>
+      <c r="I79" s="11">
+        <v>0</v>
+      </c>
+      <c r="J79" s="11">
+        <v>0</v>
+      </c>
+      <c r="K79" s="11">
+        <v>0</v>
+      </c>
+      <c r="L79" s="11">
+        <v>0</v>
+      </c>
+      <c r="M79" s="11">
+        <v>0</v>
+      </c>
+      <c r="N79" s="11">
+        <v>2.67769694223428</v>
+      </c>
+      <c r="O79" s="11">
+        <v>0</v>
+      </c>
+      <c r="P79" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q79" s="11">
+        <v>0</v>
+      </c>
+      <c r="R79" s="11">
+        <v>0</v>
+      </c>
+      <c r="S79" s="11">
+        <v>5.0761098484075804</v>
+      </c>
+      <c r="T79" t="b">
+        <v>0</v>
+      </c>
+      <c r="U79" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V79" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W79" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Master dataset new samples
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C5DC667-1BB1-534C-96D9-78114D1B844B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E7CA94-4EEB-984B-8813-874A36F771EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="59">
   <si>
     <t>Sample</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Viscosity_10/cP</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -631,11 +634,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W129"/>
+  <dimension ref="A1:W139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="66" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="66" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L106" sqref="L106"/>
+      <selection pane="topRight" activeCell="U113" sqref="U113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8307,19 +8310,18 @@
         <v>105</v>
       </c>
       <c r="T106" t="b">
-        <v>0</v>
-      </c>
-      <c r="U106" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>NA</v>
+        <v>1</v>
+      </c>
+      <c r="U106" s="2">
+        <v>153</v>
       </c>
       <c r="V106" s="2" t="str">
         <f t="shared" si="4"/>
-        <v>NA</v>
+        <v/>
       </c>
       <c r="W106" s="2" t="str">
         <f t="shared" si="5"/>
-        <v>NA</v>
+        <v/>
       </c>
     </row>
     <row r="107" spans="1:23" x14ac:dyDescent="0.2">
@@ -8370,15 +8372,15 @@
         <v>0</v>
       </c>
       <c r="U109" s="2" t="str">
-        <f t="shared" ref="U109:U129" si="6">IF(T109=FALSE, "NA", "")</f>
+        <f t="shared" ref="U109:U139" si="6">IF(T109=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V109" s="2" t="str">
-        <f t="shared" ref="V109:V129" si="7">IF(T109=FALSE, "NA", "")</f>
+        <f t="shared" ref="V109:V139" si="7">IF(T109=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W109" s="2" t="str">
-        <f t="shared" ref="W109:W129" si="8">IF(T109=FALSE, "NA", "")</f>
+        <f t="shared" ref="W109:W139" si="8">IF(T109=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -8387,19 +8389,18 @@
         <v>109</v>
       </c>
       <c r="T110" t="b">
-        <v>0</v>
-      </c>
-      <c r="U110" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
+        <v>1</v>
+      </c>
+      <c r="U110" s="2">
+        <v>19</v>
       </c>
       <c r="V110" s="2" t="str">
         <f t="shared" si="7"/>
-        <v>NA</v>
+        <v/>
       </c>
       <c r="W110" s="2" t="str">
         <f t="shared" si="8"/>
-        <v>NA</v>
+        <v/>
       </c>
     </row>
     <row r="111" spans="1:23" x14ac:dyDescent="0.2">
@@ -8429,9 +8430,8 @@
       <c r="T112" t="b">
         <v>0</v>
       </c>
-      <c r="U112" s="2" t="str">
-        <f t="shared" si="6"/>
-        <v>NA</v>
+      <c r="U112" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="V112" s="2" t="str">
         <f t="shared" si="7"/>
@@ -8506,9 +8506,6 @@
       <c r="A116" s="10">
         <v>115</v>
       </c>
-      <c r="T116" t="b">
-        <v>0</v>
-      </c>
       <c r="U116" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8526,9 +8523,6 @@
       <c r="A117" s="10">
         <v>116</v>
       </c>
-      <c r="T117" t="b">
-        <v>0</v>
-      </c>
       <c r="U117" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8546,9 +8540,6 @@
       <c r="A118" s="10">
         <v>117</v>
       </c>
-      <c r="T118" t="b">
-        <v>0</v>
-      </c>
       <c r="U118" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8566,9 +8557,6 @@
       <c r="A119" s="10">
         <v>118</v>
       </c>
-      <c r="T119" t="b">
-        <v>0</v>
-      </c>
       <c r="U119" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8586,9 +8574,6 @@
       <c r="A120" s="10">
         <v>119</v>
       </c>
-      <c r="T120" t="b">
-        <v>0</v>
-      </c>
       <c r="U120" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8606,9 +8591,6 @@
       <c r="A121" s="10">
         <v>120</v>
       </c>
-      <c r="T121" t="b">
-        <v>0</v>
-      </c>
       <c r="U121" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8626,9 +8608,6 @@
       <c r="A122" s="10">
         <v>121</v>
       </c>
-      <c r="T122" t="b">
-        <v>0</v>
-      </c>
       <c r="U122" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8646,9 +8625,6 @@
       <c r="A123" s="10">
         <v>122</v>
       </c>
-      <c r="T123" t="b">
-        <v>0</v>
-      </c>
       <c r="U123" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8666,9 +8642,6 @@
       <c r="A124" s="10">
         <v>123</v>
       </c>
-      <c r="T124" t="b">
-        <v>0</v>
-      </c>
       <c r="U124" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8686,9 +8659,6 @@
       <c r="A125" s="10">
         <v>124</v>
       </c>
-      <c r="T125" t="b">
-        <v>0</v>
-      </c>
       <c r="U125" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8706,9 +8676,6 @@
       <c r="A126" s="10">
         <v>125</v>
       </c>
-      <c r="T126" t="b">
-        <v>0</v>
-      </c>
       <c r="U126" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8726,9 +8693,6 @@
       <c r="A127" s="10">
         <v>126</v>
       </c>
-      <c r="T127" t="b">
-        <v>0</v>
-      </c>
       <c r="U127" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8746,9 +8710,6 @@
       <c r="A128" s="10">
         <v>127</v>
       </c>
-      <c r="T128" t="b">
-        <v>0</v>
-      </c>
       <c r="U128" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8766,9 +8727,6 @@
       <c r="A129" s="10">
         <v>128</v>
       </c>
-      <c r="T129" t="b">
-        <v>0</v>
-      </c>
       <c r="U129" s="2" t="str">
         <f t="shared" si="6"/>
         <v>NA</v>
@@ -8778,6 +8736,176 @@
         <v>NA</v>
       </c>
       <c r="W129" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A130" s="10">
+        <v>129</v>
+      </c>
+      <c r="U130" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V130" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W130" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A131" s="10">
+        <v>130</v>
+      </c>
+      <c r="U131" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V131" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W131" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A132" s="10">
+        <v>131</v>
+      </c>
+      <c r="U132" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V132" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W132" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A133" s="10">
+        <v>132</v>
+      </c>
+      <c r="U133" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V133" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W133" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A134" s="10">
+        <v>133</v>
+      </c>
+      <c r="U134" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V134" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W134" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A135" s="10">
+        <v>134</v>
+      </c>
+      <c r="U135" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V135" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W135" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A136" s="10">
+        <v>135</v>
+      </c>
+      <c r="U136" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V136" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W136" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A137" s="10">
+        <v>136</v>
+      </c>
+      <c r="U137" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V137" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W137" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A138" s="10">
+        <v>137</v>
+      </c>
+      <c r="U138" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V138" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W138" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A139" s="10">
+        <v>138</v>
+      </c>
+      <c r="U139" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V139" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W139" s="2" t="str">
         <f t="shared" si="8"/>
         <v>NA</v>
       </c>

</xml_diff>

<commit_message>
Compiled dataset upto S144
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E9EA951-D177-CA49-B8BD-770AB81CC3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F5BD23-53B8-C44D-AB2D-A668B4F3289E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
   <si>
     <t>Sample</t>
   </si>
@@ -687,11 +687,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W122"/>
+  <dimension ref="A1:W145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="56" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W121" sqref="W121"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="91" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W145" sqref="W145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5615,15 +5615,15 @@
         <v>0</v>
       </c>
       <c r="U67" s="2" t="str">
-        <f t="shared" ref="U67:U120" si="3">IF(T67=FALSE, "NA", "")</f>
+        <f t="shared" ref="U67:U130" si="3">IF(T67=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V67" s="2" t="str">
-        <f t="shared" ref="V67:V121" si="4">IF(T67=FALSE, "NA", "")</f>
+        <f t="shared" ref="V67:V130" si="4">IF(T67=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W67" s="2" t="str">
-        <f t="shared" ref="W67:W121" si="5">IF(T67=FALSE, "NA", "")</f>
+        <f t="shared" ref="W67:W130" si="5">IF(T67=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -9584,8 +9584,9 @@
       <c r="T121" t="b">
         <v>0</v>
       </c>
-      <c r="U121" s="2" t="s">
-        <v>57</v>
+      <c r="U121" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
       </c>
       <c r="V121" s="2" t="str">
         <f t="shared" si="4"/>
@@ -9597,12 +9598,1776 @@
       </c>
     </row>
     <row r="122" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="T122" s="22"/>
+      <c r="A122" s="10">
+        <v>121</v>
+      </c>
+      <c r="B122" s="19">
+        <v>0</v>
+      </c>
+      <c r="C122" s="19">
+        <v>0</v>
+      </c>
+      <c r="D122" s="19">
+        <v>0</v>
+      </c>
+      <c r="E122" s="19">
+        <v>0</v>
+      </c>
+      <c r="F122" s="19">
+        <v>0</v>
+      </c>
+      <c r="G122" s="19">
+        <v>0</v>
+      </c>
+      <c r="H122" s="19">
+        <v>0</v>
+      </c>
+      <c r="I122" s="19">
+        <v>0</v>
+      </c>
+      <c r="J122" s="19">
+        <v>11.110272393026801</v>
+      </c>
+      <c r="K122" s="19">
+        <v>0</v>
+      </c>
+      <c r="L122" s="19">
+        <v>12.9728478359823</v>
+      </c>
+      <c r="M122" s="19">
+        <v>0</v>
+      </c>
+      <c r="N122" s="19">
+        <v>2.55659712510655</v>
+      </c>
+      <c r="O122" s="19">
+        <v>0</v>
+      </c>
+      <c r="P122" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q122" s="19">
+        <v>0</v>
+      </c>
+      <c r="R122" s="19">
+        <v>0</v>
+      </c>
+      <c r="S122" s="19">
+        <v>1.49124545008624</v>
+      </c>
+      <c r="T122" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="U122" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V122" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W122" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="123" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A123" s="10">
+        <v>122</v>
+      </c>
+      <c r="B123" s="19">
+        <v>0</v>
+      </c>
+      <c r="C123" s="19">
+        <v>0</v>
+      </c>
+      <c r="D123" s="19">
+        <v>0</v>
+      </c>
+      <c r="E123" s="19">
+        <v>0</v>
+      </c>
+      <c r="F123" s="19">
+        <v>0</v>
+      </c>
+      <c r="G123" s="19">
+        <v>0</v>
+      </c>
+      <c r="H123" s="19">
+        <v>10.833398455257299</v>
+      </c>
+      <c r="I123" s="19">
+        <v>11.017586034112799</v>
+      </c>
+      <c r="J123" s="19">
+        <v>0</v>
+      </c>
+      <c r="K123" s="19">
+        <v>0</v>
+      </c>
+      <c r="L123" s="19">
+        <v>0</v>
+      </c>
+      <c r="M123" s="19">
+        <v>0</v>
+      </c>
+      <c r="N123" s="19">
+        <v>2.9621026626406901</v>
+      </c>
+      <c r="O123" s="19">
+        <v>0</v>
+      </c>
+      <c r="P123" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q123" s="19">
+        <v>0</v>
+      </c>
+      <c r="R123" s="19">
+        <v>0</v>
+      </c>
+      <c r="S123" s="19">
+        <v>3.38667483701823</v>
+      </c>
+      <c r="T123" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U123" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V123" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W123" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="124" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A124" s="10">
+        <v>123</v>
+      </c>
+      <c r="B124" s="19">
+        <v>0</v>
+      </c>
+      <c r="C124" s="19">
+        <v>0</v>
+      </c>
+      <c r="D124" s="19">
+        <v>0</v>
+      </c>
+      <c r="E124" s="19">
+        <v>0</v>
+      </c>
+      <c r="F124" s="19">
+        <v>0</v>
+      </c>
+      <c r="G124" s="19">
+        <v>0</v>
+      </c>
+      <c r="H124" s="19">
+        <v>12.525976188106601</v>
+      </c>
+      <c r="I124" s="19">
+        <v>12.0004709972716</v>
+      </c>
+      <c r="J124" s="19">
+        <v>0</v>
+      </c>
+      <c r="K124" s="19">
+        <v>0</v>
+      </c>
+      <c r="L124" s="19">
+        <v>0</v>
+      </c>
+      <c r="M124" s="19">
+        <v>0</v>
+      </c>
+      <c r="N124" s="19">
+        <v>1.60929982166093</v>
+      </c>
+      <c r="O124" s="19">
+        <v>0</v>
+      </c>
+      <c r="P124" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="19">
+        <v>0</v>
+      </c>
+      <c r="R124" s="19">
+        <v>0</v>
+      </c>
+      <c r="S124" s="19">
+        <v>1.99577107994824</v>
+      </c>
+      <c r="T124" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U124" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V124" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W124" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="125" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A125" s="10">
+        <v>124</v>
+      </c>
+      <c r="B125" s="19">
+        <v>0</v>
+      </c>
+      <c r="C125" s="19">
+        <v>0</v>
+      </c>
+      <c r="D125" s="19">
+        <v>0</v>
+      </c>
+      <c r="E125" s="19">
+        <v>12.016129507367699</v>
+      </c>
+      <c r="F125" s="19">
+        <v>0</v>
+      </c>
+      <c r="G125" s="19">
+        <v>0</v>
+      </c>
+      <c r="H125" s="19">
+        <v>0</v>
+      </c>
+      <c r="I125" s="19">
+        <v>0</v>
+      </c>
+      <c r="J125" s="19">
+        <v>13.182099327099399</v>
+      </c>
+      <c r="K125" s="19">
+        <v>0</v>
+      </c>
+      <c r="L125" s="19">
+        <v>0</v>
+      </c>
+      <c r="M125" s="19">
+        <v>0</v>
+      </c>
+      <c r="N125" s="19">
+        <v>1.12788537838368</v>
+      </c>
+      <c r="O125" s="19">
+        <v>0</v>
+      </c>
+      <c r="P125" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q125" s="19">
+        <v>0</v>
+      </c>
+      <c r="R125" s="19">
+        <v>0</v>
+      </c>
+      <c r="S125" s="19">
+        <v>2.7879764115022301</v>
+      </c>
+      <c r="T125" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U125" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V125" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W125" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="126" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A126" s="10">
+        <v>125</v>
+      </c>
+      <c r="B126" s="19">
+        <v>0</v>
+      </c>
+      <c r="C126" s="19">
+        <v>0</v>
+      </c>
+      <c r="D126" s="19">
+        <v>0</v>
+      </c>
+      <c r="E126" s="19">
+        <v>0</v>
+      </c>
+      <c r="F126" s="19">
+        <v>0</v>
+      </c>
+      <c r="G126" s="19">
+        <v>0</v>
+      </c>
+      <c r="H126" s="19">
+        <v>0</v>
+      </c>
+      <c r="I126" s="19">
+        <v>0</v>
+      </c>
+      <c r="J126" s="19">
+        <v>10.3959610193385</v>
+      </c>
+      <c r="K126" s="19">
+        <v>0</v>
+      </c>
+      <c r="L126" s="19">
+        <v>0</v>
+      </c>
+      <c r="M126" s="19">
+        <v>10.5472039438159</v>
+      </c>
+      <c r="N126" s="19">
+        <v>1.1679038329295599</v>
+      </c>
+      <c r="O126" s="19">
+        <v>0</v>
+      </c>
+      <c r="P126" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q126" s="19">
+        <v>0</v>
+      </c>
+      <c r="R126" s="19">
+        <v>0</v>
+      </c>
+      <c r="S126" s="19">
+        <v>5.2387762985085002</v>
+      </c>
+      <c r="T126" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U126" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V126" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W126" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="127" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A127" s="10">
+        <v>126</v>
+      </c>
+      <c r="B127" s="19">
+        <v>0</v>
+      </c>
+      <c r="C127" s="19">
+        <v>0</v>
+      </c>
+      <c r="D127" s="19">
+        <v>0</v>
+      </c>
+      <c r="E127" s="19">
+        <v>0</v>
+      </c>
+      <c r="F127" s="19">
+        <v>0</v>
+      </c>
+      <c r="G127" s="19">
+        <v>0</v>
+      </c>
+      <c r="H127" s="19">
+        <v>13.082716743206101</v>
+      </c>
+      <c r="I127" s="19">
+        <v>0</v>
+      </c>
+      <c r="J127" s="19">
+        <v>0</v>
+      </c>
+      <c r="K127" s="19">
+        <v>0</v>
+      </c>
+      <c r="L127" s="19">
+        <v>0</v>
+      </c>
+      <c r="M127" s="19">
+        <v>8.9478666689314093</v>
+      </c>
+      <c r="N127" s="19">
+        <v>2.15735581484011</v>
+      </c>
+      <c r="O127" s="19">
+        <v>0</v>
+      </c>
+      <c r="P127" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q127" s="19">
+        <v>0</v>
+      </c>
+      <c r="R127" s="19">
+        <v>0</v>
+      </c>
+      <c r="S127" s="19">
+        <v>5.52361716601445</v>
+      </c>
+      <c r="T127" t="b">
+        <v>0</v>
+      </c>
+      <c r="U127" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V127" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W127" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="128" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A128" s="10">
+        <v>127</v>
+      </c>
+      <c r="B128" s="19">
+        <v>0</v>
+      </c>
+      <c r="C128" s="19">
+        <v>0</v>
+      </c>
+      <c r="D128" s="19">
+        <v>0</v>
+      </c>
+      <c r="E128" s="19">
+        <v>0</v>
+      </c>
+      <c r="F128" s="19">
+        <v>0</v>
+      </c>
+      <c r="G128" s="19">
+        <v>0</v>
+      </c>
+      <c r="H128" s="19">
+        <v>9.6907433749692693</v>
+      </c>
+      <c r="I128" s="19">
+        <v>0</v>
+      </c>
+      <c r="J128" s="19">
+        <v>12.5051477490365</v>
+      </c>
+      <c r="K128" s="19">
+        <v>0</v>
+      </c>
+      <c r="L128" s="19">
+        <v>0</v>
+      </c>
+      <c r="M128" s="19">
+        <v>0</v>
+      </c>
+      <c r="N128" s="19">
+        <v>0.78841126420936003</v>
+      </c>
+      <c r="O128" s="19">
+        <v>0</v>
+      </c>
+      <c r="P128" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q128" s="19">
+        <v>0</v>
+      </c>
+      <c r="R128" s="19">
+        <v>0</v>
+      </c>
+      <c r="S128" s="19">
+        <v>3.4471230668585</v>
+      </c>
+      <c r="T128" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U128" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V128" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W128" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="129" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A129" s="10">
+        <v>128</v>
+      </c>
+      <c r="B129" s="19">
+        <v>0</v>
+      </c>
+      <c r="C129" s="19">
+        <v>12.901149495214799</v>
+      </c>
+      <c r="D129" s="19">
+        <v>0</v>
+      </c>
+      <c r="E129" s="19">
+        <v>0</v>
+      </c>
+      <c r="F129" s="19">
+        <v>0</v>
+      </c>
+      <c r="G129" s="19">
+        <v>0</v>
+      </c>
+      <c r="H129" s="19">
+        <v>0</v>
+      </c>
+      <c r="I129" s="19">
+        <v>10.4900987805032</v>
+      </c>
+      <c r="J129" s="19">
+        <v>0</v>
+      </c>
+      <c r="K129" s="19">
+        <v>0</v>
+      </c>
+      <c r="L129" s="19">
+        <v>0</v>
+      </c>
+      <c r="M129" s="19">
+        <v>0</v>
+      </c>
+      <c r="N129" s="19">
+        <v>1.5446257399849299</v>
+      </c>
+      <c r="O129" s="19">
+        <v>0</v>
+      </c>
+      <c r="P129" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q129" s="19">
+        <v>0</v>
+      </c>
+      <c r="R129" s="19">
+        <v>0</v>
+      </c>
+      <c r="S129" s="19">
+        <v>4.90223893779058</v>
+      </c>
+      <c r="T129" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U129" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V129" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W129" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="130" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A130" s="10">
+        <v>129</v>
+      </c>
+      <c r="B130" s="19">
+        <v>0</v>
+      </c>
+      <c r="C130" s="19">
+        <v>0</v>
+      </c>
+      <c r="D130" s="19">
+        <v>0</v>
+      </c>
+      <c r="E130" s="19">
+        <v>0</v>
+      </c>
+      <c r="F130" s="19">
+        <v>0</v>
+      </c>
+      <c r="G130" s="19">
+        <v>7.5859787297801304</v>
+      </c>
+      <c r="H130" s="19">
+        <v>0</v>
+      </c>
+      <c r="I130" s="19">
+        <v>0</v>
+      </c>
+      <c r="J130" s="19">
+        <v>0</v>
+      </c>
+      <c r="K130" s="19">
+        <v>0</v>
+      </c>
+      <c r="L130" s="19">
+        <v>0</v>
+      </c>
+      <c r="M130" s="19">
+        <v>10.808007164464801</v>
+      </c>
+      <c r="N130" s="19">
+        <v>2.7864781689534501</v>
+      </c>
+      <c r="O130" s="19">
+        <v>0</v>
+      </c>
+      <c r="P130" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q130" s="19">
+        <v>0</v>
+      </c>
+      <c r="R130" s="19">
+        <v>0</v>
+      </c>
+      <c r="S130" s="19">
+        <v>2.0671866576631301</v>
+      </c>
+      <c r="T130" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U130" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>NA</v>
+      </c>
+      <c r="V130" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>NA</v>
+      </c>
+      <c r="W130" s="12" t="str">
+        <f t="shared" si="5"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="131" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A131" s="10">
+        <v>130</v>
+      </c>
+      <c r="B131" s="19">
+        <v>0</v>
+      </c>
+      <c r="C131" s="19">
+        <v>0</v>
+      </c>
+      <c r="D131" s="19">
+        <v>0</v>
+      </c>
+      <c r="E131" s="19">
+        <v>0</v>
+      </c>
+      <c r="F131" s="19">
+        <v>0</v>
+      </c>
+      <c r="G131" s="19">
+        <v>0</v>
+      </c>
+      <c r="H131" s="19">
+        <v>0</v>
+      </c>
+      <c r="I131" s="19">
+        <v>0</v>
+      </c>
+      <c r="J131" s="19">
+        <v>0</v>
+      </c>
+      <c r="K131" s="19">
+        <v>0</v>
+      </c>
+      <c r="L131" s="19">
+        <v>12.140124251374599</v>
+      </c>
+      <c r="M131" s="19">
+        <v>12.5498089139169</v>
+      </c>
+      <c r="N131" s="19">
+        <v>2.3230307857924402</v>
+      </c>
+      <c r="O131" s="19">
+        <v>0</v>
+      </c>
+      <c r="P131" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q131" s="19">
+        <v>0</v>
+      </c>
+      <c r="R131" s="19">
+        <v>0</v>
+      </c>
+      <c r="S131" s="19">
+        <v>1.8505080167974499</v>
+      </c>
+      <c r="T131" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U131" s="2" t="str">
+        <f t="shared" ref="U131:U145" si="6">IF(T131=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V131" s="2" t="str">
+        <f t="shared" ref="V131:V145" si="7">IF(T131=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W131" s="12" t="str">
+        <f t="shared" ref="W131:W145" si="8">IF(T131=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="132" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A132" s="10">
+        <v>131</v>
+      </c>
+      <c r="B132" s="19">
+        <v>0</v>
+      </c>
+      <c r="C132" s="19">
+        <v>0</v>
+      </c>
+      <c r="D132" s="19">
+        <v>0</v>
+      </c>
+      <c r="E132" s="19">
+        <v>0</v>
+      </c>
+      <c r="F132" s="19">
+        <v>0</v>
+      </c>
+      <c r="G132" s="19">
+        <v>0</v>
+      </c>
+      <c r="H132" s="19">
+        <v>11.275260335924701</v>
+      </c>
+      <c r="I132" s="19">
+        <v>0</v>
+      </c>
+      <c r="J132" s="19">
+        <v>0</v>
+      </c>
+      <c r="K132" s="19">
+        <v>0</v>
+      </c>
+      <c r="L132" s="19">
+        <v>0</v>
+      </c>
+      <c r="M132" s="19">
+        <v>13.0213109861756</v>
+      </c>
+      <c r="N132" s="19">
+        <v>1.54557085273902</v>
+      </c>
+      <c r="O132" s="19">
+        <v>0</v>
+      </c>
+      <c r="P132" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q132" s="19">
+        <v>0</v>
+      </c>
+      <c r="R132" s="19">
+        <v>0</v>
+      </c>
+      <c r="S132" s="19">
+        <v>2.1628116086252298</v>
+      </c>
+      <c r="T132" s="20" t="b">
+        <v>1</v>
+      </c>
+      <c r="U132" s="2">
+        <v>252</v>
+      </c>
+      <c r="V132" s="2">
+        <v>130</v>
+      </c>
+      <c r="W132" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A133" s="10">
+        <v>132</v>
+      </c>
+      <c r="B133" s="19">
+        <v>0</v>
+      </c>
+      <c r="C133" s="19">
+        <v>0</v>
+      </c>
+      <c r="D133" s="19">
+        <v>0</v>
+      </c>
+      <c r="E133" s="19">
+        <v>0</v>
+      </c>
+      <c r="F133" s="19">
+        <v>0</v>
+      </c>
+      <c r="G133" s="19">
+        <v>0</v>
+      </c>
+      <c r="H133" s="19">
+        <v>0</v>
+      </c>
+      <c r="I133" s="19">
+        <v>12.8708931443248</v>
+      </c>
+      <c r="J133" s="19">
+        <v>0</v>
+      </c>
+      <c r="K133" s="19">
+        <v>0</v>
+      </c>
+      <c r="L133" s="19">
+        <v>0</v>
+      </c>
+      <c r="M133" s="19">
+        <v>12.9213362051379</v>
+      </c>
+      <c r="N133" s="19">
+        <v>2.9029486958113702</v>
+      </c>
+      <c r="O133" s="19">
+        <v>0</v>
+      </c>
+      <c r="P133" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q133" s="19">
+        <v>0</v>
+      </c>
+      <c r="R133" s="19">
+        <v>0</v>
+      </c>
+      <c r="S133" s="19">
+        <v>4.3222779559439699</v>
+      </c>
+      <c r="T133" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U133" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V133" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W133" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="134" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A134" s="10">
+        <v>133</v>
+      </c>
+      <c r="B134" s="19">
+        <v>0</v>
+      </c>
+      <c r="C134" s="19">
+        <v>0</v>
+      </c>
+      <c r="D134" s="19">
+        <v>0</v>
+      </c>
+      <c r="E134" s="19">
+        <v>0</v>
+      </c>
+      <c r="F134" s="19">
+        <v>0</v>
+      </c>
+      <c r="G134" s="19">
+        <v>9.2792650069644491</v>
+      </c>
+      <c r="H134" s="19">
+        <v>11.5637591583682</v>
+      </c>
+      <c r="I134" s="19">
+        <v>0</v>
+      </c>
+      <c r="J134" s="19">
+        <v>0</v>
+      </c>
+      <c r="K134" s="19">
+        <v>0</v>
+      </c>
+      <c r="L134" s="19">
+        <v>0</v>
+      </c>
+      <c r="M134" s="19">
+        <v>0</v>
+      </c>
+      <c r="N134" s="19">
+        <v>2.0434581286782199</v>
+      </c>
+      <c r="O134" s="19">
+        <v>0</v>
+      </c>
+      <c r="P134" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q134" s="19">
+        <v>0</v>
+      </c>
+      <c r="R134" s="19">
+        <v>0</v>
+      </c>
+      <c r="S134" s="19">
+        <v>2.2635993878237399</v>
+      </c>
+      <c r="T134" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U134" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V134" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W134" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="135" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A135" s="10">
+        <v>134</v>
+      </c>
+      <c r="B135" s="19">
+        <v>0</v>
+      </c>
+      <c r="C135" s="19">
+        <v>0</v>
+      </c>
+      <c r="D135" s="19">
+        <v>0</v>
+      </c>
+      <c r="E135" s="19">
+        <v>0</v>
+      </c>
+      <c r="F135" s="19">
+        <v>0</v>
+      </c>
+      <c r="G135" s="19">
+        <v>0</v>
+      </c>
+      <c r="H135" s="19">
+        <v>0</v>
+      </c>
+      <c r="I135" s="19">
+        <v>0</v>
+      </c>
+      <c r="J135" s="19">
+        <v>0</v>
+      </c>
+      <c r="K135" s="19">
+        <v>7.9129647458576402</v>
+      </c>
+      <c r="L135" s="19">
+        <v>0</v>
+      </c>
+      <c r="M135" s="19">
+        <v>12.901616482776801</v>
+      </c>
+      <c r="N135" s="19">
+        <v>2.7681360731649498</v>
+      </c>
+      <c r="O135" s="19">
+        <v>0</v>
+      </c>
+      <c r="P135" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q135" s="19">
+        <v>0</v>
+      </c>
+      <c r="R135" s="19">
+        <v>0</v>
+      </c>
+      <c r="S135" s="19">
+        <v>3.083493347323</v>
+      </c>
+      <c r="T135" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U135" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V135" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W135" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="136" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A136" s="10">
+        <v>135</v>
+      </c>
+      <c r="B136" s="19">
+        <v>0</v>
+      </c>
+      <c r="C136" s="19">
+        <v>0</v>
+      </c>
+      <c r="D136" s="19">
+        <v>0</v>
+      </c>
+      <c r="E136" s="19">
+        <v>0</v>
+      </c>
+      <c r="F136" s="19">
+        <v>0</v>
+      </c>
+      <c r="G136" s="19">
+        <v>0</v>
+      </c>
+      <c r="H136" s="19">
+        <v>0</v>
+      </c>
+      <c r="I136" s="19">
+        <v>10.953075839976</v>
+      </c>
+      <c r="J136" s="19">
+        <v>0</v>
+      </c>
+      <c r="K136" s="19">
+        <v>0</v>
+      </c>
+      <c r="L136" s="19">
+        <v>9.8937802921224005</v>
+      </c>
+      <c r="M136" s="19">
+        <v>0</v>
+      </c>
+      <c r="N136" s="19">
+        <v>1.7554613719166401</v>
+      </c>
+      <c r="O136" s="19">
+        <v>0</v>
+      </c>
+      <c r="P136" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q136" s="19">
+        <v>0</v>
+      </c>
+      <c r="R136" s="19">
+        <v>0</v>
+      </c>
+      <c r="S136" s="19">
+        <v>1.79057059935507</v>
+      </c>
+      <c r="T136" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U136" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V136" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W136" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="137" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A137" s="10">
+        <v>136</v>
+      </c>
+      <c r="B137" s="19">
+        <v>0</v>
+      </c>
+      <c r="C137" s="19">
+        <v>0</v>
+      </c>
+      <c r="D137" s="19">
+        <v>0</v>
+      </c>
+      <c r="E137" s="19">
+        <v>0</v>
+      </c>
+      <c r="F137" s="19">
+        <v>0</v>
+      </c>
+      <c r="G137" s="19">
+        <v>0</v>
+      </c>
+      <c r="H137" s="19">
+        <v>0</v>
+      </c>
+      <c r="I137" s="19">
+        <v>11.231561663514499</v>
+      </c>
+      <c r="J137" s="19">
+        <v>0</v>
+      </c>
+      <c r="K137" s="19">
+        <v>0</v>
+      </c>
+      <c r="L137" s="19">
+        <v>0</v>
+      </c>
+      <c r="M137" s="19">
+        <v>12.2672995684184</v>
+      </c>
+      <c r="N137" s="19">
+        <v>1.4544931822456499</v>
+      </c>
+      <c r="O137" s="19">
+        <v>0</v>
+      </c>
+      <c r="P137" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q137" s="19">
+        <v>0</v>
+      </c>
+      <c r="R137" s="19">
+        <v>0</v>
+      </c>
+      <c r="S137" s="19">
+        <v>2.4530634589832498</v>
+      </c>
+      <c r="T137" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U137" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V137" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W137" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="138" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A138" s="10">
+        <v>137</v>
+      </c>
+      <c r="B138" s="19">
+        <v>0</v>
+      </c>
+      <c r="C138" s="19">
+        <v>0</v>
+      </c>
+      <c r="D138" s="19">
+        <v>0</v>
+      </c>
+      <c r="E138" s="19">
+        <v>0</v>
+      </c>
+      <c r="F138" s="19">
+        <v>11.3242482032423</v>
+      </c>
+      <c r="G138" s="19">
+        <v>0</v>
+      </c>
+      <c r="H138" s="19">
+        <v>12.1362314150205</v>
+      </c>
+      <c r="I138" s="19">
+        <v>0</v>
+      </c>
+      <c r="J138" s="19">
+        <v>0</v>
+      </c>
+      <c r="K138" s="19">
+        <v>0</v>
+      </c>
+      <c r="L138" s="19">
+        <v>0</v>
+      </c>
+      <c r="M138" s="19">
+        <v>0</v>
+      </c>
+      <c r="N138" s="19">
+        <v>2.0546834622040402</v>
+      </c>
+      <c r="O138" s="19">
+        <v>0</v>
+      </c>
+      <c r="P138" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q138" s="19">
+        <v>0</v>
+      </c>
+      <c r="R138" s="19">
+        <v>0</v>
+      </c>
+      <c r="S138" s="19">
+        <v>1.89891323582752</v>
+      </c>
+      <c r="T138" t="b">
+        <v>1</v>
+      </c>
+      <c r="U138" s="2">
+        <v>430</v>
+      </c>
+      <c r="V138" s="2">
+        <v>1212</v>
+      </c>
+      <c r="W138" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A139" s="10">
+        <v>138</v>
+      </c>
+      <c r="B139" s="19">
+        <v>6.67779781956866</v>
+      </c>
+      <c r="C139" s="19">
+        <v>0</v>
+      </c>
+      <c r="D139" s="19">
+        <v>0</v>
+      </c>
+      <c r="E139" s="19">
+        <v>0</v>
+      </c>
+      <c r="F139" s="19">
+        <v>0</v>
+      </c>
+      <c r="G139" s="19">
+        <v>12.454888271272701</v>
+      </c>
+      <c r="H139" s="19">
+        <v>0</v>
+      </c>
+      <c r="I139" s="19">
+        <v>0</v>
+      </c>
+      <c r="J139" s="19">
+        <v>0</v>
+      </c>
+      <c r="K139" s="19">
+        <v>0</v>
+      </c>
+      <c r="L139" s="19">
+        <v>0</v>
+      </c>
+      <c r="M139" s="19">
+        <v>0</v>
+      </c>
+      <c r="N139" s="19">
+        <v>1.1296835941160801</v>
+      </c>
+      <c r="O139" s="19">
+        <v>0</v>
+      </c>
+      <c r="P139" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q139" s="19">
+        <v>0</v>
+      </c>
+      <c r="R139" s="19">
+        <v>0</v>
+      </c>
+      <c r="S139" s="19">
+        <v>1.88449460543139</v>
+      </c>
+      <c r="T139" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U139" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V139" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W139" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="140" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A140" s="10">
+        <v>139</v>
+      </c>
+      <c r="B140" s="19">
+        <v>0</v>
+      </c>
+      <c r="C140" s="19">
+        <v>0</v>
+      </c>
+      <c r="D140" s="19">
+        <v>0</v>
+      </c>
+      <c r="E140" s="19">
+        <v>0</v>
+      </c>
+      <c r="F140" s="19">
+        <v>0</v>
+      </c>
+      <c r="G140" s="19">
+        <v>0</v>
+      </c>
+      <c r="H140" s="19">
+        <v>0</v>
+      </c>
+      <c r="I140" s="19">
+        <v>0</v>
+      </c>
+      <c r="J140" s="19">
+        <v>12.5075369995233</v>
+      </c>
+      <c r="K140" s="19">
+        <v>0</v>
+      </c>
+      <c r="L140" s="19">
+        <v>9.0965717769884602</v>
+      </c>
+      <c r="M140" s="19">
+        <v>0</v>
+      </c>
+      <c r="N140" s="19">
+        <v>1.7356350653825801</v>
+      </c>
+      <c r="O140" s="19">
+        <v>0</v>
+      </c>
+      <c r="P140" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q140" s="19">
+        <v>0</v>
+      </c>
+      <c r="R140" s="19">
+        <v>0</v>
+      </c>
+      <c r="S140" s="19">
+        <v>2.4271479593432499</v>
+      </c>
+      <c r="T140" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U140" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V140" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W140" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="141" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A141" s="10">
+        <v>140</v>
+      </c>
+      <c r="B141" s="19">
+        <v>0</v>
+      </c>
+      <c r="C141" s="19">
+        <v>0</v>
+      </c>
+      <c r="D141" s="19">
+        <v>0</v>
+      </c>
+      <c r="E141" s="19">
+        <v>11.042077219383</v>
+      </c>
+      <c r="F141" s="19">
+        <v>0</v>
+      </c>
+      <c r="G141" s="19">
+        <v>10.5233879694841</v>
+      </c>
+      <c r="H141" s="19">
+        <v>0</v>
+      </c>
+      <c r="I141" s="19">
+        <v>0</v>
+      </c>
+      <c r="J141" s="19">
+        <v>0</v>
+      </c>
+      <c r="K141" s="19">
+        <v>0</v>
+      </c>
+      <c r="L141" s="19">
+        <v>0</v>
+      </c>
+      <c r="M141" s="19">
+        <v>0</v>
+      </c>
+      <c r="N141" s="19">
+        <v>2.9649931030743302</v>
+      </c>
+      <c r="O141" s="19">
+        <v>0</v>
+      </c>
+      <c r="P141" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q141" s="19">
+        <v>0</v>
+      </c>
+      <c r="R141" s="19">
+        <v>0</v>
+      </c>
+      <c r="S141" s="19">
+        <v>2.18006961769616</v>
+      </c>
+      <c r="T141" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U141" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V141" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W141" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="142" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A142" s="10">
+        <v>141</v>
+      </c>
+      <c r="B142" s="19">
+        <v>0</v>
+      </c>
+      <c r="C142" s="19">
+        <v>0</v>
+      </c>
+      <c r="D142" s="19">
+        <v>0</v>
+      </c>
+      <c r="E142" s="19">
+        <v>0</v>
+      </c>
+      <c r="F142" s="19">
+        <v>0</v>
+      </c>
+      <c r="G142" s="19">
+        <v>0</v>
+      </c>
+      <c r="H142" s="19">
+        <v>9.2046680113093906</v>
+      </c>
+      <c r="I142" s="19">
+        <v>0</v>
+      </c>
+      <c r="J142" s="19">
+        <v>0</v>
+      </c>
+      <c r="K142" s="19">
+        <v>0</v>
+      </c>
+      <c r="L142" s="19">
+        <v>0</v>
+      </c>
+      <c r="M142" s="19">
+        <v>11.8909057999747</v>
+      </c>
+      <c r="N142" s="19">
+        <v>2.36196765322285</v>
+      </c>
+      <c r="O142" s="19">
+        <v>0</v>
+      </c>
+      <c r="P142" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q142" s="19">
+        <v>0</v>
+      </c>
+      <c r="R142" s="19">
+        <v>0</v>
+      </c>
+      <c r="S142" s="19">
+        <v>3.7781474114051101</v>
+      </c>
+      <c r="T142" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="U142" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V142" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W142" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="143" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A143" s="10">
+        <v>142</v>
+      </c>
+      <c r="B143" s="19">
+        <v>0</v>
+      </c>
+      <c r="C143" s="19">
+        <v>0</v>
+      </c>
+      <c r="D143" s="19">
+        <v>0</v>
+      </c>
+      <c r="E143" s="19">
+        <v>10.126867607475999</v>
+      </c>
+      <c r="F143" s="19">
+        <v>8.84806174516293</v>
+      </c>
+      <c r="G143" s="19">
+        <v>0</v>
+      </c>
+      <c r="H143" s="19">
+        <v>0</v>
+      </c>
+      <c r="I143" s="19">
+        <v>0</v>
+      </c>
+      <c r="J143" s="19">
+        <v>0</v>
+      </c>
+      <c r="K143" s="19">
+        <v>0</v>
+      </c>
+      <c r="L143" s="19">
+        <v>0</v>
+      </c>
+      <c r="M143" s="19">
+        <v>0</v>
+      </c>
+      <c r="N143" s="19">
+        <v>2.0740757073729901</v>
+      </c>
+      <c r="O143" s="19">
+        <v>0</v>
+      </c>
+      <c r="P143" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q143" s="19">
+        <v>0</v>
+      </c>
+      <c r="R143" s="19">
+        <v>0</v>
+      </c>
+      <c r="S143" s="19">
+        <v>1.82757691381969</v>
+      </c>
+      <c r="T143" t="b">
+        <v>1</v>
+      </c>
+      <c r="U143" s="2">
+        <v>20</v>
+      </c>
+      <c r="V143" s="2">
+        <v>13</v>
+      </c>
+      <c r="W143" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A144" s="10">
+        <v>143</v>
+      </c>
+      <c r="B144" s="19">
+        <v>0</v>
+      </c>
+      <c r="C144" s="19">
+        <v>10.8370822177899</v>
+      </c>
+      <c r="D144" s="19">
+        <v>0</v>
+      </c>
+      <c r="E144" s="19">
+        <v>0</v>
+      </c>
+      <c r="F144" s="19">
+        <v>0</v>
+      </c>
+      <c r="G144" s="19">
+        <v>0</v>
+      </c>
+      <c r="H144" s="19">
+        <v>0</v>
+      </c>
+      <c r="I144" s="19">
+        <v>11.410962214088</v>
+      </c>
+      <c r="J144" s="19">
+        <v>0</v>
+      </c>
+      <c r="K144" s="19">
+        <v>0</v>
+      </c>
+      <c r="L144" s="19">
+        <v>0</v>
+      </c>
+      <c r="M144" s="19">
+        <v>0</v>
+      </c>
+      <c r="N144" s="19">
+        <v>1.2009707028250101</v>
+      </c>
+      <c r="O144" s="19">
+        <v>0</v>
+      </c>
+      <c r="P144" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q144" s="19">
+        <v>0</v>
+      </c>
+      <c r="R144" s="19">
+        <v>0</v>
+      </c>
+      <c r="S144" s="19">
+        <v>3.27718299445824</v>
+      </c>
+      <c r="T144" t="b">
+        <v>0</v>
+      </c>
+      <c r="U144" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V144" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W144" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="145" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A145" s="10">
+        <v>144</v>
+      </c>
+      <c r="B145" s="19">
+        <v>0</v>
+      </c>
+      <c r="C145" s="19">
+        <v>0</v>
+      </c>
+      <c r="D145" s="19">
+        <v>0</v>
+      </c>
+      <c r="E145" s="19">
+        <v>0</v>
+      </c>
+      <c r="F145" s="19">
+        <v>0</v>
+      </c>
+      <c r="G145" s="19">
+        <v>10.3969156372025</v>
+      </c>
+      <c r="H145" s="19">
+        <v>0</v>
+      </c>
+      <c r="I145" s="19">
+        <v>13.162464253496999</v>
+      </c>
+      <c r="J145" s="19">
+        <v>0</v>
+      </c>
+      <c r="K145" s="19">
+        <v>0</v>
+      </c>
+      <c r="L145" s="19">
+        <v>0</v>
+      </c>
+      <c r="M145" s="19">
+        <v>0</v>
+      </c>
+      <c r="N145" s="19">
+        <v>2.2192077183203001</v>
+      </c>
+      <c r="O145" s="19">
+        <v>0</v>
+      </c>
+      <c r="P145" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q145" s="19">
+        <v>0</v>
+      </c>
+      <c r="R145" s="19">
+        <v>0</v>
+      </c>
+      <c r="S145" s="19">
+        <v>2.5141351057222998</v>
+      </c>
+      <c r="T145" t="b">
+        <v>0</v>
+      </c>
+      <c r="U145" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V145" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W145" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:W121">
+  <conditionalFormatting sqref="A1:W145">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>$T2=TRUE</formula>
+      <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated dataset till S180
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF46F82A-1F57-1C4E-A504-07F8FA24DF69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1AEE6F-9E4F-C745-AEA0-CF5AC50B04F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4840" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -689,9 +689,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
   <dimension ref="A1:W181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T169" sqref="T169"/>
+    <sheetView tabSelected="1" topLeftCell="A144" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W181" sqref="W181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10325,15 +10325,15 @@
         <v>0</v>
       </c>
       <c r="U131" s="2" t="str">
-        <f t="shared" ref="U131:U157" si="6">IF(T131=FALSE, "NA", "")</f>
+        <f t="shared" ref="U131:U179" si="6">IF(T131=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V131" s="2" t="str">
-        <f t="shared" ref="V131:V157" si="7">IF(T131=FALSE, "NA", "")</f>
+        <f t="shared" ref="V131:V181" si="7">IF(T131=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W131" s="12" t="str">
-        <f t="shared" ref="W131:W157" si="8">IF(T131=FALSE, "NA", "")</f>
+        <f t="shared" ref="W131:W181" si="8">IF(T131=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -12289,6 +12289,18 @@
       <c r="S158" s="19">
         <v>4.2600556684542799</v>
       </c>
+      <c r="T158" t="b">
+        <v>1</v>
+      </c>
+      <c r="U158" s="2">
+        <v>142</v>
+      </c>
+      <c r="V158" s="2">
+        <v>262</v>
+      </c>
+      <c r="W158" s="12" t="b">
+        <v>0</v>
+      </c>
     </row>
     <row r="159" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A159" s="10">
@@ -12348,6 +12360,21 @@
       <c r="S159" s="19">
         <v>2.4526892080829499</v>
       </c>
+      <c r="T159" t="b">
+        <v>0</v>
+      </c>
+      <c r="U159" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V159" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W159" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="160" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A160" s="10">
@@ -12407,8 +12434,20 @@
       <c r="S160" s="19">
         <v>1.40260110331874</v>
       </c>
-    </row>
-    <row r="161" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T160" t="b">
+        <v>1</v>
+      </c>
+      <c r="U160" s="2">
+        <v>15</v>
+      </c>
+      <c r="V160" s="2">
+        <v>4</v>
+      </c>
+      <c r="W160" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A161" s="10">
         <v>160</v>
       </c>
@@ -12466,8 +12505,20 @@
       <c r="S161" s="19">
         <v>4.6282139228679204</v>
       </c>
-    </row>
-    <row r="162" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T161" t="b">
+        <v>1</v>
+      </c>
+      <c r="U161" s="2">
+        <v>20</v>
+      </c>
+      <c r="V161" s="2">
+        <v>242</v>
+      </c>
+      <c r="W161" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A162" s="10">
         <v>161</v>
       </c>
@@ -12525,8 +12576,23 @@
       <c r="S162" s="19">
         <v>1.62055980828711</v>
       </c>
-    </row>
-    <row r="163" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T162" t="b">
+        <v>0</v>
+      </c>
+      <c r="U162" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V162" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W162" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="163" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A163" s="10">
         <v>162</v>
       </c>
@@ -12584,8 +12650,23 @@
       <c r="S163" s="19">
         <v>3.3303020428669798</v>
       </c>
-    </row>
-    <row r="164" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T163" t="b">
+        <v>0</v>
+      </c>
+      <c r="U163" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V163" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W163" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="164" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A164" s="10">
         <v>163</v>
       </c>
@@ -12643,8 +12724,23 @@
       <c r="S164" s="19">
         <v>1.4343733496284301</v>
       </c>
-    </row>
-    <row r="165" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T164" t="b">
+        <v>0</v>
+      </c>
+      <c r="U164" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V164" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W164" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="165" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A165" s="10">
         <v>164</v>
       </c>
@@ -12702,8 +12798,20 @@
       <c r="S165" s="19">
         <v>1.64920222056957</v>
       </c>
-    </row>
-    <row r="166" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T165" t="b">
+        <v>1</v>
+      </c>
+      <c r="U165" s="2">
+        <v>14</v>
+      </c>
+      <c r="V165" s="2">
+        <v>4</v>
+      </c>
+      <c r="W165" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A166" s="10">
         <v>165</v>
       </c>
@@ -12761,8 +12869,23 @@
       <c r="S166" s="19">
         <v>2.1103429594241701</v>
       </c>
-    </row>
-    <row r="167" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T166" t="b">
+        <v>0</v>
+      </c>
+      <c r="U166" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V166" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W166" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="167" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A167" s="10">
         <v>166</v>
       </c>
@@ -12820,8 +12943,20 @@
       <c r="S167" s="19">
         <v>3.2817471050871898</v>
       </c>
-    </row>
-    <row r="168" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T167" t="b">
+        <v>1</v>
+      </c>
+      <c r="U167" s="2">
+        <v>31</v>
+      </c>
+      <c r="V167" s="2">
+        <v>233</v>
+      </c>
+      <c r="W167" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A168" s="10">
         <v>167</v>
       </c>
@@ -12879,8 +13014,20 @@
       <c r="S168" s="19">
         <v>2.0365729339234999</v>
       </c>
-    </row>
-    <row r="169" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T168" t="b">
+        <v>1</v>
+      </c>
+      <c r="U168" s="2">
+        <v>118</v>
+      </c>
+      <c r="V168" s="2">
+        <v>101</v>
+      </c>
+      <c r="W168" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A169" s="10">
         <v>168</v>
       </c>
@@ -12938,69 +13085,894 @@
       <c r="S169" s="19">
         <v>1.5872835854145499</v>
       </c>
-    </row>
-    <row r="170" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="T169" t="b">
+        <v>0</v>
+      </c>
+      <c r="U169" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V169" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W169" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="170" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A170" s="10">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B170" s="19">
+        <v>0</v>
+      </c>
+      <c r="C170" s="19">
+        <v>10.2653869809432</v>
+      </c>
+      <c r="D170" s="19">
+        <v>0</v>
+      </c>
+      <c r="E170" s="19">
+        <v>0</v>
+      </c>
+      <c r="F170" s="19">
+        <v>0</v>
+      </c>
+      <c r="G170" s="19">
+        <v>0</v>
+      </c>
+      <c r="H170" s="19">
+        <v>0</v>
+      </c>
+      <c r="I170" s="19">
+        <v>11.378166057468199</v>
+      </c>
+      <c r="J170" s="19">
+        <v>0</v>
+      </c>
+      <c r="K170" s="19">
+        <v>0</v>
+      </c>
+      <c r="L170" s="19">
+        <v>0</v>
+      </c>
+      <c r="M170" s="19">
+        <v>0</v>
+      </c>
+      <c r="N170" s="19">
+        <v>2.0678316544801598</v>
+      </c>
+      <c r="O170" s="19">
+        <v>0</v>
+      </c>
+      <c r="P170" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q170" s="19">
+        <v>0</v>
+      </c>
+      <c r="R170" s="19">
+        <v>0</v>
+      </c>
+      <c r="S170" s="19">
+        <v>1.1872955325422601</v>
+      </c>
+      <c r="T170" t="b">
+        <v>1</v>
+      </c>
+      <c r="U170" s="2">
+        <v>275</v>
+      </c>
+      <c r="V170" s="2">
+        <v>2</v>
+      </c>
+      <c r="W170" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A171" s="10">
         <v>170</v>
       </c>
-    </row>
-    <row r="172" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B171" s="19">
+        <v>0</v>
+      </c>
+      <c r="C171" s="19">
+        <v>0</v>
+      </c>
+      <c r="D171" s="19">
+        <v>0</v>
+      </c>
+      <c r="E171" s="19">
+        <v>0</v>
+      </c>
+      <c r="F171" s="19">
+        <v>0</v>
+      </c>
+      <c r="G171" s="19">
+        <v>0</v>
+      </c>
+      <c r="H171" s="19">
+        <v>0</v>
+      </c>
+      <c r="I171" s="19">
+        <v>8.9170384814845391</v>
+      </c>
+      <c r="J171" s="19">
+        <v>12.6791304878173</v>
+      </c>
+      <c r="K171" s="19">
+        <v>0</v>
+      </c>
+      <c r="L171" s="19">
+        <v>0</v>
+      </c>
+      <c r="M171" s="19">
+        <v>0</v>
+      </c>
+      <c r="N171" s="19">
+        <v>1.90058355697282</v>
+      </c>
+      <c r="O171" s="19">
+        <v>0</v>
+      </c>
+      <c r="P171" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q171" s="19">
+        <v>0</v>
+      </c>
+      <c r="R171" s="19">
+        <v>0</v>
+      </c>
+      <c r="S171" s="19">
+        <v>1.79547646371144</v>
+      </c>
+      <c r="T171" t="b">
+        <v>1</v>
+      </c>
+      <c r="U171" s="2">
+        <v>50</v>
+      </c>
+      <c r="V171" s="2">
+        <v>254</v>
+      </c>
+      <c r="W171" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A172" s="10">
         <v>171</v>
       </c>
-    </row>
-    <row r="173" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B172" s="19">
+        <v>0</v>
+      </c>
+      <c r="C172" s="19">
+        <v>0</v>
+      </c>
+      <c r="D172" s="19">
+        <v>0</v>
+      </c>
+      <c r="E172" s="19">
+        <v>0</v>
+      </c>
+      <c r="F172" s="19">
+        <v>0</v>
+      </c>
+      <c r="G172" s="19">
+        <v>0</v>
+      </c>
+      <c r="H172" s="19">
+        <v>0</v>
+      </c>
+      <c r="I172" s="19">
+        <v>0</v>
+      </c>
+      <c r="J172" s="19">
+        <v>12.890699125983801</v>
+      </c>
+      <c r="K172" s="19">
+        <v>0</v>
+      </c>
+      <c r="L172" s="19">
+        <v>0</v>
+      </c>
+      <c r="M172" s="19">
+        <v>9.7986766723475007</v>
+      </c>
+      <c r="N172" s="19">
+        <v>2.0750663836542702</v>
+      </c>
+      <c r="O172" s="19">
+        <v>0</v>
+      </c>
+      <c r="P172" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q172" s="19">
+        <v>0</v>
+      </c>
+      <c r="R172" s="19">
+        <v>0</v>
+      </c>
+      <c r="S172" s="19">
+        <v>2.4692546214092799</v>
+      </c>
+      <c r="T172" t="b">
+        <v>1</v>
+      </c>
+      <c r="U172" s="2">
+        <v>40</v>
+      </c>
+      <c r="V172" s="2">
+        <v>172</v>
+      </c>
+      <c r="W172" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A173" s="10">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B173" s="19">
+        <v>0</v>
+      </c>
+      <c r="C173" s="19">
+        <v>9.7946187873011699</v>
+      </c>
+      <c r="D173" s="19">
+        <v>0</v>
+      </c>
+      <c r="E173" s="19">
+        <v>0</v>
+      </c>
+      <c r="F173" s="19">
+        <v>0</v>
+      </c>
+      <c r="G173" s="19">
+        <v>0</v>
+      </c>
+      <c r="H173" s="19">
+        <v>0</v>
+      </c>
+      <c r="I173" s="19">
+        <v>0</v>
+      </c>
+      <c r="J173" s="19">
+        <v>12.1699227799109</v>
+      </c>
+      <c r="K173" s="19">
+        <v>0</v>
+      </c>
+      <c r="L173" s="19">
+        <v>0</v>
+      </c>
+      <c r="M173" s="19">
+        <v>0</v>
+      </c>
+      <c r="N173" s="19">
+        <v>1.1571497232649699</v>
+      </c>
+      <c r="O173" s="19">
+        <v>0</v>
+      </c>
+      <c r="P173" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q173" s="19">
+        <v>0</v>
+      </c>
+      <c r="R173" s="19">
+        <v>0</v>
+      </c>
+      <c r="S173" s="19">
+        <v>2.19810031113931</v>
+      </c>
+      <c r="T173" t="b">
+        <v>0</v>
+      </c>
+      <c r="U173" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V173" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W173" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="174" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A174" s="10">
         <v>173</v>
       </c>
-    </row>
-    <row r="175" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B174" s="19">
+        <v>0</v>
+      </c>
+      <c r="C174" s="19">
+        <v>0</v>
+      </c>
+      <c r="D174" s="19">
+        <v>0</v>
+      </c>
+      <c r="E174" s="19">
+        <v>10.4056318189722</v>
+      </c>
+      <c r="F174" s="19">
+        <v>0</v>
+      </c>
+      <c r="G174" s="19">
+        <v>0</v>
+      </c>
+      <c r="H174" s="19">
+        <v>9.8722123029058793</v>
+      </c>
+      <c r="I174" s="19">
+        <v>0</v>
+      </c>
+      <c r="J174" s="19">
+        <v>0</v>
+      </c>
+      <c r="K174" s="19">
+        <v>0</v>
+      </c>
+      <c r="L174" s="19">
+        <v>0</v>
+      </c>
+      <c r="M174" s="19">
+        <v>0</v>
+      </c>
+      <c r="N174" s="19">
+        <v>2.8152696681290199</v>
+      </c>
+      <c r="O174" s="19">
+        <v>0</v>
+      </c>
+      <c r="P174" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q174" s="19">
+        <v>0</v>
+      </c>
+      <c r="R174" s="19">
+        <v>0</v>
+      </c>
+      <c r="S174" s="19">
+        <v>1.7385524968094701</v>
+      </c>
+      <c r="T174" t="b">
+        <v>0</v>
+      </c>
+      <c r="U174" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V174" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W174" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="175" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A175" s="10">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B175" s="19">
+        <v>0</v>
+      </c>
+      <c r="C175" s="19">
+        <v>12.504551376244001</v>
+      </c>
+      <c r="D175" s="19">
+        <v>0</v>
+      </c>
+      <c r="E175" s="19">
+        <v>0</v>
+      </c>
+      <c r="F175" s="19">
+        <v>10.989200504366901</v>
+      </c>
+      <c r="G175" s="19">
+        <v>0</v>
+      </c>
+      <c r="H175" s="19">
+        <v>0</v>
+      </c>
+      <c r="I175" s="19">
+        <v>0</v>
+      </c>
+      <c r="J175" s="19">
+        <v>0</v>
+      </c>
+      <c r="K175" s="19">
+        <v>0</v>
+      </c>
+      <c r="L175" s="19">
+        <v>0</v>
+      </c>
+      <c r="M175" s="19">
+        <v>0</v>
+      </c>
+      <c r="N175" s="19">
+        <v>1.2753072794809499</v>
+      </c>
+      <c r="O175" s="19">
+        <v>0</v>
+      </c>
+      <c r="P175" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q175" s="19">
+        <v>0</v>
+      </c>
+      <c r="R175" s="19">
+        <v>0</v>
+      </c>
+      <c r="S175" s="19">
+        <v>1.48240846161887</v>
+      </c>
+      <c r="T175" t="b">
+        <v>0</v>
+      </c>
+      <c r="U175" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V175" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W175" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="176" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A176" s="10">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176" s="19">
+        <v>0</v>
+      </c>
+      <c r="C176" s="19">
+        <v>0</v>
+      </c>
+      <c r="D176" s="19">
+        <v>0</v>
+      </c>
+      <c r="E176" s="19">
+        <v>11.5571467949592</v>
+      </c>
+      <c r="F176" s="19">
+        <v>0</v>
+      </c>
+      <c r="G176" s="19">
+        <v>0</v>
+      </c>
+      <c r="H176" s="19">
+        <v>0</v>
+      </c>
+      <c r="I176" s="19">
+        <v>0</v>
+      </c>
+      <c r="J176" s="19">
+        <v>0</v>
+      </c>
+      <c r="K176" s="19">
+        <v>0</v>
+      </c>
+      <c r="L176" s="19">
+        <v>8.4657700985929605</v>
+      </c>
+      <c r="M176" s="19">
+        <v>0</v>
+      </c>
+      <c r="N176" s="19">
+        <v>2.2835169286266401</v>
+      </c>
+      <c r="O176" s="19">
+        <v>0</v>
+      </c>
+      <c r="P176" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q176" s="19">
+        <v>0</v>
+      </c>
+      <c r="R176" s="19">
+        <v>0</v>
+      </c>
+      <c r="S176" s="19">
+        <v>1.6457329014636799</v>
+      </c>
+      <c r="T176" t="b">
+        <v>0</v>
+      </c>
+      <c r="U176" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V176" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W176" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="177" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A177" s="10">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177" s="19">
+        <v>0</v>
+      </c>
+      <c r="C177" s="19">
+        <v>0</v>
+      </c>
+      <c r="D177" s="19">
+        <v>0</v>
+      </c>
+      <c r="E177" s="19">
+        <v>12.9213836121534</v>
+      </c>
+      <c r="F177" s="19">
+        <v>10.8954949044402</v>
+      </c>
+      <c r="G177" s="19">
+        <v>0</v>
+      </c>
+      <c r="H177" s="19">
+        <v>0</v>
+      </c>
+      <c r="I177" s="19">
+        <v>0</v>
+      </c>
+      <c r="J177" s="19">
+        <v>0</v>
+      </c>
+      <c r="K177" s="19">
+        <v>0</v>
+      </c>
+      <c r="L177" s="19">
+        <v>0</v>
+      </c>
+      <c r="M177" s="19">
+        <v>0</v>
+      </c>
+      <c r="N177" s="19">
+        <v>1.3710855656729899</v>
+      </c>
+      <c r="O177" s="19">
+        <v>0</v>
+      </c>
+      <c r="P177" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q177" s="19">
+        <v>0</v>
+      </c>
+      <c r="R177" s="19">
+        <v>0</v>
+      </c>
+      <c r="S177" s="19">
+        <v>2.6201884297736302</v>
+      </c>
+      <c r="T177" t="b">
+        <v>1</v>
+      </c>
+      <c r="U177" s="2">
+        <v>19</v>
+      </c>
+      <c r="V177" s="2">
+        <v>88</v>
+      </c>
+      <c r="W177" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A178" s="10">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B178" s="19">
+        <v>0</v>
+      </c>
+      <c r="C178" s="19">
+        <v>0</v>
+      </c>
+      <c r="D178" s="19">
+        <v>0</v>
+      </c>
+      <c r="E178" s="19">
+        <v>0</v>
+      </c>
+      <c r="F178" s="19">
+        <v>0</v>
+      </c>
+      <c r="G178" s="19">
+        <v>0</v>
+      </c>
+      <c r="H178" s="19">
+        <v>0</v>
+      </c>
+      <c r="I178" s="19">
+        <v>0</v>
+      </c>
+      <c r="J178" s="19">
+        <v>11.401479794604599</v>
+      </c>
+      <c r="K178" s="19">
+        <v>12.6407925269305</v>
+      </c>
+      <c r="L178" s="19">
+        <v>0</v>
+      </c>
+      <c r="M178" s="19">
+        <v>0</v>
+      </c>
+      <c r="N178" s="19">
+        <v>1.38633311219559</v>
+      </c>
+      <c r="O178" s="19">
+        <v>0</v>
+      </c>
+      <c r="P178" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q178" s="19">
+        <v>0</v>
+      </c>
+      <c r="R178" s="19">
+        <v>0</v>
+      </c>
+      <c r="S178" s="19">
+        <v>3.2610896340258502</v>
+      </c>
+      <c r="T178" t="b">
+        <v>0</v>
+      </c>
+      <c r="U178" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V178" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W178" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="179" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A179" s="10">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B179" s="19">
+        <v>0</v>
+      </c>
+      <c r="C179" s="19">
+        <v>0</v>
+      </c>
+      <c r="D179" s="19">
+        <v>0</v>
+      </c>
+      <c r="E179" s="19">
+        <v>0</v>
+      </c>
+      <c r="F179" s="19">
+        <v>0</v>
+      </c>
+      <c r="G179" s="19">
+        <v>0</v>
+      </c>
+      <c r="H179" s="19">
+        <v>9.9161968320794909</v>
+      </c>
+      <c r="I179" s="19">
+        <v>0</v>
+      </c>
+      <c r="J179" s="19">
+        <v>0</v>
+      </c>
+      <c r="K179" s="19">
+        <v>0</v>
+      </c>
+      <c r="L179" s="19">
+        <v>0</v>
+      </c>
+      <c r="M179" s="19">
+        <v>10.9467231225762</v>
+      </c>
+      <c r="N179" s="19">
+        <v>2.90677248686832</v>
+      </c>
+      <c r="O179" s="19">
+        <v>0</v>
+      </c>
+      <c r="P179" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q179" s="19">
+        <v>0</v>
+      </c>
+      <c r="R179" s="19">
+        <v>0</v>
+      </c>
+      <c r="S179" s="19">
+        <v>2.2196718260942201</v>
+      </c>
+      <c r="T179" t="b">
+        <v>0</v>
+      </c>
+      <c r="U179" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>NA</v>
+      </c>
+      <c r="V179" s="2" t="str">
+        <f t="shared" si="7"/>
+        <v>NA</v>
+      </c>
+      <c r="W179" s="12" t="str">
+        <f t="shared" si="8"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="180" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A180" s="10">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B180" s="19">
+        <v>0</v>
+      </c>
+      <c r="C180" s="19">
+        <v>0</v>
+      </c>
+      <c r="D180" s="19">
+        <v>0</v>
+      </c>
+      <c r="E180" s="19">
+        <v>0</v>
+      </c>
+      <c r="F180" s="19">
+        <v>0</v>
+      </c>
+      <c r="G180" s="19">
+        <v>0</v>
+      </c>
+      <c r="H180" s="19">
+        <v>9.5240633357233495</v>
+      </c>
+      <c r="I180" s="19">
+        <v>0</v>
+      </c>
+      <c r="J180" s="19">
+        <v>13.0756740244887</v>
+      </c>
+      <c r="K180" s="19">
+        <v>0</v>
+      </c>
+      <c r="L180" s="19">
+        <v>0</v>
+      </c>
+      <c r="M180" s="19">
+        <v>0</v>
+      </c>
+      <c r="N180" s="19">
+        <v>2.7853853778154201</v>
+      </c>
+      <c r="O180" s="19">
+        <v>0</v>
+      </c>
+      <c r="P180" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q180" s="19">
+        <v>0</v>
+      </c>
+      <c r="R180" s="19">
+        <v>0</v>
+      </c>
+      <c r="S180" s="19">
+        <v>1.6467980216207301</v>
+      </c>
+      <c r="T180" t="b">
+        <v>1</v>
+      </c>
+      <c r="U180" s="2">
+        <v>18</v>
+      </c>
+      <c r="V180" s="2">
+        <v>10</v>
+      </c>
+      <c r="W180" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A181" s="10">
         <v>180</v>
       </c>
+      <c r="B181" s="19">
+        <v>0</v>
+      </c>
+      <c r="C181" s="19">
+        <v>0</v>
+      </c>
+      <c r="D181" s="19">
+        <v>0</v>
+      </c>
+      <c r="E181" s="19">
+        <v>0</v>
+      </c>
+      <c r="F181" s="19">
+        <v>0</v>
+      </c>
+      <c r="G181" s="19">
+        <v>0</v>
+      </c>
+      <c r="H181" s="19">
+        <v>0</v>
+      </c>
+      <c r="I181" s="19">
+        <v>0</v>
+      </c>
+      <c r="J181" s="19">
+        <v>11.2839783019497</v>
+      </c>
+      <c r="K181" s="19">
+        <v>0</v>
+      </c>
+      <c r="L181" s="19">
+        <v>0</v>
+      </c>
+      <c r="M181" s="19">
+        <v>8.44565879048365</v>
+      </c>
+      <c r="N181" s="19">
+        <v>1.1496332517229999</v>
+      </c>
+      <c r="O181" s="19">
+        <v>0</v>
+      </c>
+      <c r="P181" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q181" s="19">
+        <v>0</v>
+      </c>
+      <c r="R181" s="19">
+        <v>0</v>
+      </c>
+      <c r="S181" s="19">
+        <v>1.5641942197824801</v>
+      </c>
+      <c r="T181" t="b">
+        <v>1</v>
+      </c>
+      <c r="U181" s="2">
+        <v>21</v>
+      </c>
+      <c r="V181" s="2">
+        <v>4</v>
+      </c>
+      <c r="W181" s="12" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W169">
+  <conditionalFormatting sqref="A1:W181">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated dataset till S252
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{420A1518-CEBF-7748-9D57-A5DE965EAB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74428456-2E2C-CE44-B7B5-248AA8A01BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="-38400" yWindow="-5300" windowWidth="38400" windowHeight="21600" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -356,17 +356,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -699,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
   <dimension ref="A1:W253"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" zoomScale="92" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="92" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="W253" sqref="W253"/>
     </sheetView>
   </sheetViews>
@@ -18419,13 +18409,11 @@
       <c r="U242" s="2">
         <v>23</v>
       </c>
-      <c r="V242" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="W242" s="12" t="str">
-        <f t="shared" ref="W242:W253" si="15">IF(T242=FALSE, "NA", "")</f>
-        <v/>
+      <c r="V242" s="2">
+        <v>73</v>
+      </c>
+      <c r="W242" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="243" spans="1:23" x14ac:dyDescent="0.2">
@@ -18498,7 +18486,7 @@
         <v>NA</v>
       </c>
       <c r="W243" s="12" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="W242:W253" si="15">IF(T243=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -18714,13 +18702,11 @@
       <c r="U246" s="2">
         <v>30</v>
       </c>
-      <c r="V246" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="W246" s="12" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+      <c r="V246" s="2">
+        <v>90</v>
+      </c>
+      <c r="W246" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:23" x14ac:dyDescent="0.2">
@@ -18787,13 +18773,11 @@
       <c r="U247" s="2">
         <v>17</v>
       </c>
-      <c r="V247" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="W247" s="12" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+      <c r="V247" s="2">
+        <v>8</v>
+      </c>
+      <c r="W247" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="248" spans="1:23" x14ac:dyDescent="0.2">
@@ -18860,13 +18844,11 @@
       <c r="U248" s="2">
         <v>22</v>
       </c>
-      <c r="V248" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="W248" s="12" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+      <c r="V248" s="2">
+        <v>21</v>
+      </c>
+      <c r="W248" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="249" spans="1:23" x14ac:dyDescent="0.2">
@@ -18933,13 +18915,11 @@
       <c r="U249" s="2">
         <v>21</v>
       </c>
-      <c r="V249" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="W249" s="12" t="str">
-        <f t="shared" si="15"/>
-        <v/>
+      <c r="V249" s="2">
+        <v>3</v>
+      </c>
+      <c r="W249" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="250" spans="1:23" x14ac:dyDescent="0.2">
@@ -29394,7 +29374,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S272
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74428456-2E2C-CE44-B7B5-248AA8A01BED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BD140D-E703-C943-A921-866D4C9C0906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5300" windowWidth="38400" windowHeight="21600" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="-38400" yWindow="-4840" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
   <si>
     <t>Sample</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>Percent stable</t>
+  </si>
+  <si>
+    <t>Newtonian</t>
   </si>
 </sst>
 </file>
@@ -687,11 +690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W253"/>
+  <dimension ref="A1:W277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A212" zoomScale="92" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W253" sqref="W253"/>
+    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W277" sqref="A1:W277"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,7 +791,7 @@
         <v>56</v>
       </c>
       <c r="W1" s="11" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -16785,11 +16788,11 @@
         <v>0</v>
       </c>
       <c r="U220" s="2" t="str">
-        <f t="shared" ref="U220:U253" si="12">IF(T220=FALSE, "NA", "")</f>
+        <f t="shared" ref="U220:U277" si="12">IF(T220=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V220" s="2" t="str">
-        <f t="shared" ref="V220:V253" si="13">IF(T220=FALSE, "NA", "")</f>
+        <f t="shared" ref="V220:V277" si="13">IF(T220=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W220" s="12" t="str">
@@ -18486,7 +18489,7 @@
         <v>NA</v>
       </c>
       <c r="W243" s="12" t="str">
-        <f t="shared" ref="W242:W253" si="15">IF(T243=FALSE, "NA", "")</f>
+        <f t="shared" ref="W243:W276" si="15">IF(T243=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -19218,8 +19221,1751 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="254" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A254" s="10">
+        <v>253</v>
+      </c>
+      <c r="B254" s="7">
+        <v>0</v>
+      </c>
+      <c r="C254" s="7">
+        <v>0</v>
+      </c>
+      <c r="D254" s="7">
+        <v>0</v>
+      </c>
+      <c r="E254" s="7">
+        <v>0</v>
+      </c>
+      <c r="F254" s="7">
+        <v>12.295247162772799</v>
+      </c>
+      <c r="G254" s="7">
+        <v>0</v>
+      </c>
+      <c r="H254" s="7">
+        <v>0</v>
+      </c>
+      <c r="I254" s="7">
+        <v>0</v>
+      </c>
+      <c r="J254" s="7">
+        <v>0</v>
+      </c>
+      <c r="K254" s="7">
+        <v>0</v>
+      </c>
+      <c r="L254" s="7">
+        <v>0</v>
+      </c>
+      <c r="M254" s="7">
+        <v>8.2751854684037607</v>
+      </c>
+      <c r="N254" s="7">
+        <v>2.5244166959849599</v>
+      </c>
+      <c r="O254" s="7">
+        <v>0</v>
+      </c>
+      <c r="P254" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q254" s="7">
+        <v>0</v>
+      </c>
+      <c r="R254" s="7">
+        <v>1.0352734146981399</v>
+      </c>
+      <c r="S254" s="7">
+        <v>0</v>
+      </c>
+      <c r="T254" t="b">
+        <v>1</v>
+      </c>
+      <c r="U254" s="2">
+        <v>19</v>
+      </c>
+      <c r="V254" s="2">
+        <v>5</v>
+      </c>
+      <c r="W254" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A255" s="10">
+        <v>254</v>
+      </c>
+      <c r="B255" s="7">
+        <v>0</v>
+      </c>
+      <c r="C255" s="7">
+        <v>0</v>
+      </c>
+      <c r="D255" s="7">
+        <v>0</v>
+      </c>
+      <c r="E255" s="7">
+        <v>6.7450675030102101</v>
+      </c>
+      <c r="F255" s="7">
+        <v>0</v>
+      </c>
+      <c r="G255" s="7">
+        <v>0</v>
+      </c>
+      <c r="H255" s="7">
+        <v>0</v>
+      </c>
+      <c r="I255" s="7">
+        <v>0</v>
+      </c>
+      <c r="J255" s="7">
+        <v>0</v>
+      </c>
+      <c r="K255" s="7">
+        <v>0</v>
+      </c>
+      <c r="L255" s="7">
+        <v>0</v>
+      </c>
+      <c r="M255" s="7">
+        <v>13.303807174445399</v>
+      </c>
+      <c r="N255" s="7">
+        <v>2.9220736289545202</v>
+      </c>
+      <c r="O255" s="7">
+        <v>0</v>
+      </c>
+      <c r="P255" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q255" s="7">
+        <v>0</v>
+      </c>
+      <c r="R255" s="7">
+        <v>1.42012022984085</v>
+      </c>
+      <c r="S255" s="7">
+        <v>0</v>
+      </c>
+      <c r="T255" t="b">
+        <v>1</v>
+      </c>
+      <c r="U255" s="2">
+        <v>21</v>
+      </c>
+      <c r="V255" s="2">
+        <v>9</v>
+      </c>
+      <c r="W255" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A256" s="10">
+        <v>255</v>
+      </c>
+      <c r="B256" s="7">
+        <v>0</v>
+      </c>
+      <c r="C256" s="7">
+        <v>0</v>
+      </c>
+      <c r="D256" s="7">
+        <v>0</v>
+      </c>
+      <c r="E256" s="7">
+        <v>0</v>
+      </c>
+      <c r="F256" s="7">
+        <v>0</v>
+      </c>
+      <c r="G256" s="7">
+        <v>0</v>
+      </c>
+      <c r="H256" s="7">
+        <v>0</v>
+      </c>
+      <c r="I256" s="7">
+        <v>0</v>
+      </c>
+      <c r="J256" s="7">
+        <v>0</v>
+      </c>
+      <c r="K256" s="7">
+        <v>8.7695469536642907</v>
+      </c>
+      <c r="L256" s="7">
+        <v>0</v>
+      </c>
+      <c r="M256" s="7">
+        <v>10.544787136032699</v>
+      </c>
+      <c r="N256" s="7">
+        <v>1.4440646907389301</v>
+      </c>
+      <c r="O256" s="7">
+        <v>0</v>
+      </c>
+      <c r="P256" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q256" s="7">
+        <v>0</v>
+      </c>
+      <c r="R256" s="7">
+        <v>1.2210383062330501</v>
+      </c>
+      <c r="S256" s="7">
+        <v>0</v>
+      </c>
+      <c r="T256" t="b">
+        <v>0</v>
+      </c>
+      <c r="U256" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V256" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W256" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="257" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A257" s="10">
+        <v>256</v>
+      </c>
+      <c r="B257" s="7">
+        <v>0</v>
+      </c>
+      <c r="C257" s="7">
+        <v>0</v>
+      </c>
+      <c r="D257" s="7">
+        <v>0</v>
+      </c>
+      <c r="E257" s="7">
+        <v>13.8205367068784</v>
+      </c>
+      <c r="F257" s="7">
+        <v>0</v>
+      </c>
+      <c r="G257" s="7">
+        <v>0</v>
+      </c>
+      <c r="H257" s="7">
+        <v>0</v>
+      </c>
+      <c r="I257" s="7">
+        <v>0</v>
+      </c>
+      <c r="J257" s="7">
+        <v>0</v>
+      </c>
+      <c r="K257" s="7">
+        <v>0</v>
+      </c>
+      <c r="L257" s="7">
+        <v>0</v>
+      </c>
+      <c r="M257" s="7">
+        <v>10.410784129214001</v>
+      </c>
+      <c r="N257" s="7">
+        <v>1.05358901590432</v>
+      </c>
+      <c r="O257" s="7">
+        <v>0</v>
+      </c>
+      <c r="P257" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q257" s="7">
+        <v>0</v>
+      </c>
+      <c r="R257" s="7">
+        <v>2.8308305572839298</v>
+      </c>
+      <c r="S257" s="7">
+        <v>0</v>
+      </c>
+      <c r="T257" t="b">
+        <v>1</v>
+      </c>
+      <c r="U257" s="2">
+        <v>25</v>
+      </c>
+      <c r="V257" s="2">
+        <v>340</v>
+      </c>
+      <c r="W257" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A258" s="10">
+        <v>257</v>
+      </c>
+      <c r="B258" s="7">
+        <v>0</v>
+      </c>
+      <c r="C258" s="7">
+        <v>0</v>
+      </c>
+      <c r="D258" s="7">
+        <v>0</v>
+      </c>
+      <c r="E258" s="7">
+        <v>10.1030826800597</v>
+      </c>
+      <c r="F258" s="7">
+        <v>0</v>
+      </c>
+      <c r="G258" s="7">
+        <v>0</v>
+      </c>
+      <c r="H258" s="7">
+        <v>0</v>
+      </c>
+      <c r="I258" s="7">
+        <v>0</v>
+      </c>
+      <c r="J258" s="7">
+        <v>7.9649584843580401</v>
+      </c>
+      <c r="K258" s="7">
+        <v>0</v>
+      </c>
+      <c r="L258" s="7">
+        <v>0</v>
+      </c>
+      <c r="M258" s="7">
+        <v>0</v>
+      </c>
+      <c r="N258" s="7">
+        <v>2.6020614777392099</v>
+      </c>
+      <c r="O258" s="7">
+        <v>0</v>
+      </c>
+      <c r="P258" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q258" s="7">
+        <v>0</v>
+      </c>
+      <c r="R258" s="7">
+        <v>2.1648755178905801</v>
+      </c>
+      <c r="S258" s="7">
+        <v>0</v>
+      </c>
+      <c r="T258" t="b">
+        <v>0</v>
+      </c>
+      <c r="U258" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V258" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W258" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="259" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A259" s="10">
+        <v>258</v>
+      </c>
+      <c r="B259" s="7">
+        <v>0</v>
+      </c>
+      <c r="C259" s="7">
+        <v>9.3877584210417897</v>
+      </c>
+      <c r="D259" s="7">
+        <v>0</v>
+      </c>
+      <c r="E259" s="7">
+        <v>0</v>
+      </c>
+      <c r="F259" s="7">
+        <v>0</v>
+      </c>
+      <c r="G259" s="7">
+        <v>0</v>
+      </c>
+      <c r="H259" s="7">
+        <v>0</v>
+      </c>
+      <c r="I259" s="7">
+        <v>0</v>
+      </c>
+      <c r="J259" s="7">
+        <v>0</v>
+      </c>
+      <c r="K259" s="7">
+        <v>0</v>
+      </c>
+      <c r="L259" s="7">
+        <v>0</v>
+      </c>
+      <c r="M259" s="7">
+        <v>12.883147416252999</v>
+      </c>
+      <c r="N259" s="7">
+        <v>2.06760723683978</v>
+      </c>
+      <c r="O259" s="7">
+        <v>0</v>
+      </c>
+      <c r="P259" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q259" s="7">
+        <v>0</v>
+      </c>
+      <c r="R259" s="7">
+        <v>1.1750880382761</v>
+      </c>
+      <c r="S259" s="7">
+        <v>0</v>
+      </c>
+      <c r="T259" t="b">
+        <v>0</v>
+      </c>
+      <c r="U259" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V259" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W259" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="260" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A260" s="10">
+        <v>259</v>
+      </c>
+      <c r="B260" s="7">
+        <v>0</v>
+      </c>
+      <c r="C260" s="7">
+        <v>0</v>
+      </c>
+      <c r="D260" s="7">
+        <v>0</v>
+      </c>
+      <c r="E260" s="7">
+        <v>0</v>
+      </c>
+      <c r="F260" s="7">
+        <v>0</v>
+      </c>
+      <c r="G260" s="7">
+        <v>0</v>
+      </c>
+      <c r="H260" s="7">
+        <v>0</v>
+      </c>
+      <c r="I260" s="7">
+        <v>0</v>
+      </c>
+      <c r="J260" s="7">
+        <v>12.222394850928501</v>
+      </c>
+      <c r="K260" s="7">
+        <v>0</v>
+      </c>
+      <c r="L260" s="7">
+        <v>0</v>
+      </c>
+      <c r="M260" s="7">
+        <v>8.5352369347823291</v>
+      </c>
+      <c r="N260" s="7">
+        <v>1.54428685250946</v>
+      </c>
+      <c r="O260" s="7">
+        <v>0</v>
+      </c>
+      <c r="P260" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q260" s="7">
+        <v>0</v>
+      </c>
+      <c r="R260" s="7">
+        <v>2.9954382306213598</v>
+      </c>
+      <c r="S260" s="7">
+        <v>0</v>
+      </c>
+      <c r="T260" t="b">
+        <v>1</v>
+      </c>
+      <c r="U260" s="2">
+        <v>19</v>
+      </c>
+      <c r="V260" s="2">
+        <v>64</v>
+      </c>
+      <c r="W260" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A261" s="10">
+        <v>260</v>
+      </c>
+      <c r="B261" s="7">
+        <v>0</v>
+      </c>
+      <c r="C261" s="7">
+        <v>0</v>
+      </c>
+      <c r="D261" s="7">
+        <v>0</v>
+      </c>
+      <c r="E261" s="7">
+        <v>7.2676482967029701</v>
+      </c>
+      <c r="F261" s="7">
+        <v>8.0636969501242497</v>
+      </c>
+      <c r="G261" s="7">
+        <v>0</v>
+      </c>
+      <c r="H261" s="7">
+        <v>0</v>
+      </c>
+      <c r="I261" s="7">
+        <v>0</v>
+      </c>
+      <c r="J261" s="7">
+        <v>0</v>
+      </c>
+      <c r="K261" s="7">
+        <v>0</v>
+      </c>
+      <c r="L261" s="7">
+        <v>0</v>
+      </c>
+      <c r="M261" s="7">
+        <v>0</v>
+      </c>
+      <c r="N261" s="7">
+        <v>2.9059863391099001</v>
+      </c>
+      <c r="O261" s="7">
+        <v>0</v>
+      </c>
+      <c r="P261" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q261" s="7">
+        <v>0</v>
+      </c>
+      <c r="R261" s="7">
+        <v>5.08387939765149</v>
+      </c>
+      <c r="S261" s="7">
+        <v>0</v>
+      </c>
+      <c r="T261" t="b">
+        <v>0</v>
+      </c>
+      <c r="U261" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V261" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W261" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="262" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A262" s="10">
+        <v>261</v>
+      </c>
+      <c r="B262" s="7">
+        <v>0</v>
+      </c>
+      <c r="C262" s="7">
+        <v>0</v>
+      </c>
+      <c r="D262" s="7">
+        <v>0</v>
+      </c>
+      <c r="E262" s="7">
+        <v>0</v>
+      </c>
+      <c r="F262" s="7">
+        <v>0</v>
+      </c>
+      <c r="G262" s="7">
+        <v>9.2089215699919595</v>
+      </c>
+      <c r="H262" s="7">
+        <v>0</v>
+      </c>
+      <c r="I262" s="7">
+        <v>0</v>
+      </c>
+      <c r="J262" s="7">
+        <v>0</v>
+      </c>
+      <c r="K262" s="7">
+        <v>0</v>
+      </c>
+      <c r="L262" s="7">
+        <v>0</v>
+      </c>
+      <c r="M262" s="7">
+        <v>11.821111030922999</v>
+      </c>
+      <c r="N262" s="7">
+        <v>1.5686187673729901</v>
+      </c>
+      <c r="O262" s="7">
+        <v>0</v>
+      </c>
+      <c r="P262" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q262" s="7">
+        <v>0</v>
+      </c>
+      <c r="R262" s="7">
+        <v>2.7607690305763799</v>
+      </c>
+      <c r="S262" s="7">
+        <v>0</v>
+      </c>
+      <c r="T262" t="b">
+        <v>0</v>
+      </c>
+      <c r="U262" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V262" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W262" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="263" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A263" s="10">
+        <v>262</v>
+      </c>
+      <c r="B263" s="7">
+        <v>0</v>
+      </c>
+      <c r="C263" s="7">
+        <v>0</v>
+      </c>
+      <c r="D263" s="7">
+        <v>0</v>
+      </c>
+      <c r="E263" s="7">
+        <v>0</v>
+      </c>
+      <c r="F263" s="7">
+        <v>0</v>
+      </c>
+      <c r="G263" s="7">
+        <v>0</v>
+      </c>
+      <c r="H263" s="7">
+        <v>0</v>
+      </c>
+      <c r="I263" s="7">
+        <v>6.7817476999314001</v>
+      </c>
+      <c r="J263" s="7">
+        <v>0</v>
+      </c>
+      <c r="K263" s="7">
+        <v>0</v>
+      </c>
+      <c r="L263" s="7">
+        <v>0</v>
+      </c>
+      <c r="M263" s="7">
+        <v>9.1778771151222909</v>
+      </c>
+      <c r="N263" s="7">
+        <v>1.9798311565906701</v>
+      </c>
+      <c r="O263" s="7">
+        <v>0</v>
+      </c>
+      <c r="P263" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q263" s="7">
+        <v>0</v>
+      </c>
+      <c r="R263" s="7">
+        <v>1.9722066463599399</v>
+      </c>
+      <c r="S263" s="7">
+        <v>0</v>
+      </c>
+      <c r="T263" t="b">
+        <v>0</v>
+      </c>
+      <c r="U263" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V263" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W263" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="264" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A264" s="10">
+        <v>263</v>
+      </c>
+      <c r="B264" s="7">
+        <v>0</v>
+      </c>
+      <c r="C264" s="7">
+        <v>0</v>
+      </c>
+      <c r="D264" s="7">
+        <v>0</v>
+      </c>
+      <c r="E264" s="7">
+        <v>0</v>
+      </c>
+      <c r="F264" s="7">
+        <v>0</v>
+      </c>
+      <c r="G264" s="7">
+        <v>0</v>
+      </c>
+      <c r="H264" s="7">
+        <v>0</v>
+      </c>
+      <c r="I264" s="7">
+        <v>12.5558385585202</v>
+      </c>
+      <c r="J264" s="7">
+        <v>0</v>
+      </c>
+      <c r="K264" s="7">
+        <v>0</v>
+      </c>
+      <c r="L264" s="7">
+        <v>0</v>
+      </c>
+      <c r="M264" s="7">
+        <v>12.486452855583799</v>
+      </c>
+      <c r="N264" s="7">
+        <v>1.4310801230649699</v>
+      </c>
+      <c r="O264" s="7">
+        <v>0</v>
+      </c>
+      <c r="P264" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q264" s="7">
+        <v>0</v>
+      </c>
+      <c r="R264" s="7">
+        <v>2.5276220355432799</v>
+      </c>
+      <c r="S264" s="7">
+        <v>0</v>
+      </c>
+      <c r="T264" t="b">
+        <v>0</v>
+      </c>
+      <c r="U264" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V264" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W264" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="265" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A265" s="10">
+        <v>264</v>
+      </c>
+      <c r="B265" s="7">
+        <v>0</v>
+      </c>
+      <c r="C265" s="7">
+        <v>0</v>
+      </c>
+      <c r="D265" s="7">
+        <v>0</v>
+      </c>
+      <c r="E265" s="7">
+        <v>0</v>
+      </c>
+      <c r="F265" s="7">
+        <v>10.8515169605094</v>
+      </c>
+      <c r="G265" s="7">
+        <v>0</v>
+      </c>
+      <c r="H265" s="7">
+        <v>0</v>
+      </c>
+      <c r="I265" s="7">
+        <v>0</v>
+      </c>
+      <c r="J265" s="7">
+        <v>0</v>
+      </c>
+      <c r="K265" s="7">
+        <v>0</v>
+      </c>
+      <c r="L265" s="7">
+        <v>0</v>
+      </c>
+      <c r="M265" s="7">
+        <v>12.8603566290085</v>
+      </c>
+      <c r="N265" s="7">
+        <v>2.6354821716309602</v>
+      </c>
+      <c r="O265" s="7">
+        <v>0</v>
+      </c>
+      <c r="P265" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q265" s="7">
+        <v>0</v>
+      </c>
+      <c r="R265" s="7">
+        <v>3.3049294843491701</v>
+      </c>
+      <c r="S265" s="7">
+        <v>0</v>
+      </c>
+      <c r="T265" t="b">
+        <v>1</v>
+      </c>
+      <c r="U265" s="2">
+        <v>24</v>
+      </c>
+      <c r="V265" s="2">
+        <v>357</v>
+      </c>
+      <c r="W265" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="266" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A266" s="10">
+        <v>265</v>
+      </c>
+      <c r="B266" s="7">
+        <v>0</v>
+      </c>
+      <c r="C266" s="7">
+        <v>0</v>
+      </c>
+      <c r="D266" s="7">
+        <v>0</v>
+      </c>
+      <c r="E266" s="7">
+        <v>8.7030684296429399</v>
+      </c>
+      <c r="F266" s="7">
+        <v>0</v>
+      </c>
+      <c r="G266" s="7">
+        <v>0</v>
+      </c>
+      <c r="H266" s="7">
+        <v>0</v>
+      </c>
+      <c r="I266" s="7">
+        <v>0</v>
+      </c>
+      <c r="J266" s="7">
+        <v>0</v>
+      </c>
+      <c r="K266" s="7">
+        <v>0</v>
+      </c>
+      <c r="L266" s="7">
+        <v>0</v>
+      </c>
+      <c r="M266" s="7">
+        <v>8.6297365481994408</v>
+      </c>
+      <c r="N266" s="7">
+        <v>2.5793470799381399</v>
+      </c>
+      <c r="O266" s="7">
+        <v>0</v>
+      </c>
+      <c r="P266" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q266" s="7">
+        <v>0</v>
+      </c>
+      <c r="R266" s="7">
+        <v>4.3999128866071002</v>
+      </c>
+      <c r="S266" s="7">
+        <v>0</v>
+      </c>
+      <c r="T266" t="b">
+        <v>0</v>
+      </c>
+      <c r="U266" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V266" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W266" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="267" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A267" s="10">
+        <v>266</v>
+      </c>
+      <c r="B267" s="7">
+        <v>0</v>
+      </c>
+      <c r="C267" s="7">
+        <v>0</v>
+      </c>
+      <c r="D267" s="7">
+        <v>0</v>
+      </c>
+      <c r="E267" s="7">
+        <v>13.3222133000941</v>
+      </c>
+      <c r="F267" s="7">
+        <v>6.7216799284721196</v>
+      </c>
+      <c r="G267" s="7">
+        <v>0</v>
+      </c>
+      <c r="H267" s="7">
+        <v>0</v>
+      </c>
+      <c r="I267" s="7">
+        <v>0</v>
+      </c>
+      <c r="J267" s="7">
+        <v>0</v>
+      </c>
+      <c r="K267" s="7">
+        <v>0</v>
+      </c>
+      <c r="L267" s="7">
+        <v>0</v>
+      </c>
+      <c r="M267" s="7">
+        <v>0</v>
+      </c>
+      <c r="N267" s="7">
+        <v>1.2297841002854599</v>
+      </c>
+      <c r="O267" s="7">
+        <v>0</v>
+      </c>
+      <c r="P267" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q267" s="7">
+        <v>0</v>
+      </c>
+      <c r="R267" s="7">
+        <v>4.5771904745483099</v>
+      </c>
+      <c r="S267" s="7">
+        <v>0</v>
+      </c>
+      <c r="T267" t="b">
+        <v>0</v>
+      </c>
+      <c r="U267" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V267" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W267" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="268" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A268" s="10">
+        <v>267</v>
+      </c>
+      <c r="B268" s="7">
+        <v>0</v>
+      </c>
+      <c r="C268" s="7">
+        <v>0</v>
+      </c>
+      <c r="D268" s="7">
+        <v>0</v>
+      </c>
+      <c r="E268" s="7">
+        <v>0</v>
+      </c>
+      <c r="F268" s="7">
+        <v>0</v>
+      </c>
+      <c r="G268" s="7">
+        <v>0</v>
+      </c>
+      <c r="H268" s="7">
+        <v>0</v>
+      </c>
+      <c r="I268" s="7">
+        <v>0</v>
+      </c>
+      <c r="J268" s="7">
+        <v>8.5500400063464692</v>
+      </c>
+      <c r="K268" s="7">
+        <v>0</v>
+      </c>
+      <c r="L268" s="7">
+        <v>0</v>
+      </c>
+      <c r="M268" s="7">
+        <v>11.251948716217299</v>
+      </c>
+      <c r="N268" s="7">
+        <v>0.99195074394791105</v>
+      </c>
+      <c r="O268" s="7">
+        <v>0</v>
+      </c>
+      <c r="P268" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q268" s="7">
+        <v>0</v>
+      </c>
+      <c r="R268" s="7">
+        <v>2.4317178388836602</v>
+      </c>
+      <c r="S268" s="7">
+        <v>0</v>
+      </c>
+      <c r="T268" t="b">
+        <v>1</v>
+      </c>
+      <c r="U268" s="2">
+        <v>20</v>
+      </c>
+      <c r="V268" s="2">
+        <v>23</v>
+      </c>
+      <c r="W268" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A269" s="10">
+        <v>268</v>
+      </c>
+      <c r="B269" s="7">
+        <v>0</v>
+      </c>
+      <c r="C269" s="7">
+        <v>0</v>
+      </c>
+      <c r="D269" s="7">
+        <v>0</v>
+      </c>
+      <c r="E269" s="7">
+        <v>8.50924547642866</v>
+      </c>
+      <c r="F269" s="7">
+        <v>0</v>
+      </c>
+      <c r="G269" s="7">
+        <v>0</v>
+      </c>
+      <c r="H269" s="7">
+        <v>0</v>
+      </c>
+      <c r="I269" s="7">
+        <v>0</v>
+      </c>
+      <c r="J269" s="7">
+        <v>11.530174839340701</v>
+      </c>
+      <c r="K269" s="7">
+        <v>0</v>
+      </c>
+      <c r="L269" s="7">
+        <v>0</v>
+      </c>
+      <c r="M269" s="7">
+        <v>0</v>
+      </c>
+      <c r="N269" s="7">
+        <v>2.2487668624992101</v>
+      </c>
+      <c r="O269" s="7">
+        <v>0</v>
+      </c>
+      <c r="P269" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q269" s="7">
+        <v>0</v>
+      </c>
+      <c r="R269" s="7">
+        <v>1.39367111609324</v>
+      </c>
+      <c r="S269" s="7">
+        <v>0</v>
+      </c>
+      <c r="T269" t="b">
+        <v>1</v>
+      </c>
+      <c r="U269" s="2">
+        <v>31</v>
+      </c>
+      <c r="V269" s="2">
+        <v>18</v>
+      </c>
+      <c r="W269" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A270" s="10">
+        <v>269</v>
+      </c>
+      <c r="B270" s="7">
+        <v>0</v>
+      </c>
+      <c r="C270" s="7">
+        <v>0</v>
+      </c>
+      <c r="D270" s="7">
+        <v>0</v>
+      </c>
+      <c r="E270" s="7">
+        <v>0</v>
+      </c>
+      <c r="F270" s="7">
+        <v>9.7566016571435199</v>
+      </c>
+      <c r="G270" s="7">
+        <v>0</v>
+      </c>
+      <c r="H270" s="7">
+        <v>0</v>
+      </c>
+      <c r="I270" s="7">
+        <v>0</v>
+      </c>
+      <c r="J270" s="7">
+        <v>0</v>
+      </c>
+      <c r="K270" s="7">
+        <v>0</v>
+      </c>
+      <c r="L270" s="7">
+        <v>0</v>
+      </c>
+      <c r="M270" s="7">
+        <v>11.4170259497181</v>
+      </c>
+      <c r="N270" s="7">
+        <v>1.64730525746613</v>
+      </c>
+      <c r="O270" s="7">
+        <v>0</v>
+      </c>
+      <c r="P270" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q270" s="7">
+        <v>0</v>
+      </c>
+      <c r="R270" s="7">
+        <v>4.2178935517994001</v>
+      </c>
+      <c r="S270" s="7">
+        <v>0</v>
+      </c>
+      <c r="T270" t="b">
+        <v>0</v>
+      </c>
+      <c r="U270" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V270" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W270" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="271" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A271" s="10">
+        <v>270</v>
+      </c>
+      <c r="B271" s="7">
+        <v>0</v>
+      </c>
+      <c r="C271" s="7">
+        <v>0</v>
+      </c>
+      <c r="D271" s="7">
+        <v>0</v>
+      </c>
+      <c r="E271" s="7">
+        <v>0</v>
+      </c>
+      <c r="F271" s="7">
+        <v>10.844081307943901</v>
+      </c>
+      <c r="G271" s="7">
+        <v>0</v>
+      </c>
+      <c r="H271" s="7">
+        <v>0</v>
+      </c>
+      <c r="I271" s="7">
+        <v>0</v>
+      </c>
+      <c r="J271" s="7">
+        <v>12.5849371700888</v>
+      </c>
+      <c r="K271" s="7">
+        <v>0</v>
+      </c>
+      <c r="L271" s="7">
+        <v>0</v>
+      </c>
+      <c r="M271" s="7">
+        <v>0</v>
+      </c>
+      <c r="N271" s="7">
+        <v>1.8452484011755299</v>
+      </c>
+      <c r="O271" s="7">
+        <v>0</v>
+      </c>
+      <c r="P271" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q271" s="7">
+        <v>0</v>
+      </c>
+      <c r="R271" s="7">
+        <v>3.7493095003964201</v>
+      </c>
+      <c r="S271" s="7">
+        <v>0</v>
+      </c>
+      <c r="T271" t="b">
+        <v>0</v>
+      </c>
+      <c r="U271" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V271" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W271" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="272" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A272" s="10">
+        <v>271</v>
+      </c>
+      <c r="B272" s="7">
+        <v>0</v>
+      </c>
+      <c r="C272" s="7">
+        <v>0</v>
+      </c>
+      <c r="D272" s="7">
+        <v>0</v>
+      </c>
+      <c r="E272" s="7">
+        <v>0</v>
+      </c>
+      <c r="F272" s="7">
+        <v>0</v>
+      </c>
+      <c r="G272" s="7">
+        <v>11.7073117612775</v>
+      </c>
+      <c r="H272" s="7">
+        <v>0</v>
+      </c>
+      <c r="I272" s="7">
+        <v>0</v>
+      </c>
+      <c r="J272" s="7">
+        <v>0</v>
+      </c>
+      <c r="K272" s="7">
+        <v>0</v>
+      </c>
+      <c r="L272" s="7">
+        <v>0</v>
+      </c>
+      <c r="M272" s="7">
+        <v>12.844216032162199</v>
+      </c>
+      <c r="N272" s="7">
+        <v>1.0145569582829399</v>
+      </c>
+      <c r="O272" s="7">
+        <v>0</v>
+      </c>
+      <c r="P272" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q272" s="7">
+        <v>0</v>
+      </c>
+      <c r="R272" s="7">
+        <v>1.34607063762339</v>
+      </c>
+      <c r="S272" s="7">
+        <v>0</v>
+      </c>
+      <c r="T272" t="b">
+        <v>1</v>
+      </c>
+      <c r="U272" s="2">
+        <v>28</v>
+      </c>
+      <c r="V272" s="2">
+        <v>1030</v>
+      </c>
+      <c r="W272" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A273" s="10">
+        <v>272</v>
+      </c>
+      <c r="B273" s="7">
+        <v>0</v>
+      </c>
+      <c r="C273" s="7">
+        <v>0</v>
+      </c>
+      <c r="D273" s="7">
+        <v>0</v>
+      </c>
+      <c r="E273" s="7">
+        <v>0</v>
+      </c>
+      <c r="F273" s="7">
+        <v>0</v>
+      </c>
+      <c r="G273" s="7">
+        <v>0</v>
+      </c>
+      <c r="H273" s="7">
+        <v>7.9663250903729201</v>
+      </c>
+      <c r="I273" s="7">
+        <v>0</v>
+      </c>
+      <c r="J273" s="7">
+        <v>0</v>
+      </c>
+      <c r="K273" s="7">
+        <v>0</v>
+      </c>
+      <c r="L273" s="7">
+        <v>0</v>
+      </c>
+      <c r="M273" s="7">
+        <v>8.2400957005273892</v>
+      </c>
+      <c r="N273" s="7">
+        <v>1.60740317184714</v>
+      </c>
+      <c r="O273" s="7">
+        <v>0</v>
+      </c>
+      <c r="P273" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q273" s="7">
+        <v>0</v>
+      </c>
+      <c r="R273" s="7">
+        <v>1.54870235671367</v>
+      </c>
+      <c r="S273" s="7">
+        <v>0</v>
+      </c>
+      <c r="T273" t="b">
+        <v>1</v>
+      </c>
+      <c r="U273" s="2">
+        <v>28</v>
+      </c>
+      <c r="V273" s="2">
+        <v>170</v>
+      </c>
+      <c r="W273" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A274" s="10">
+        <v>273</v>
+      </c>
+      <c r="B274" s="7">
+        <v>0</v>
+      </c>
+      <c r="C274" s="7">
+        <v>0</v>
+      </c>
+      <c r="D274" s="7">
+        <v>0</v>
+      </c>
+      <c r="E274" s="7">
+        <v>12.067036914070799</v>
+      </c>
+      <c r="F274" s="7">
+        <v>8.19803190383276</v>
+      </c>
+      <c r="G274" s="7">
+        <v>0</v>
+      </c>
+      <c r="H274" s="7">
+        <v>0</v>
+      </c>
+      <c r="I274" s="7">
+        <v>0</v>
+      </c>
+      <c r="J274" s="7">
+        <v>0</v>
+      </c>
+      <c r="K274" s="7">
+        <v>0</v>
+      </c>
+      <c r="L274" s="7">
+        <v>0</v>
+      </c>
+      <c r="M274" s="7">
+        <v>0</v>
+      </c>
+      <c r="N274" s="7">
+        <v>1.9021101345115501</v>
+      </c>
+      <c r="O274" s="7">
+        <v>0</v>
+      </c>
+      <c r="P274" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q274" s="7">
+        <v>0</v>
+      </c>
+      <c r="R274" s="7">
+        <v>2.2800211249326399</v>
+      </c>
+      <c r="S274" s="7">
+        <v>0</v>
+      </c>
+      <c r="T274" t="b">
+        <v>1</v>
+      </c>
+      <c r="U274" s="2">
+        <v>25</v>
+      </c>
+      <c r="V274" s="2">
+        <v>60</v>
+      </c>
+      <c r="W274" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A275" s="10">
+        <v>274</v>
+      </c>
+      <c r="B275" s="7">
+        <v>0</v>
+      </c>
+      <c r="C275" s="7">
+        <v>0</v>
+      </c>
+      <c r="D275" s="7">
+        <v>0</v>
+      </c>
+      <c r="E275" s="7">
+        <v>12.395699611050601</v>
+      </c>
+      <c r="F275" s="7">
+        <v>0</v>
+      </c>
+      <c r="G275" s="7">
+        <v>0</v>
+      </c>
+      <c r="H275" s="7">
+        <v>0</v>
+      </c>
+      <c r="I275" s="7">
+        <v>0</v>
+      </c>
+      <c r="J275" s="7">
+        <v>10.549177265007501</v>
+      </c>
+      <c r="K275" s="7">
+        <v>0</v>
+      </c>
+      <c r="L275" s="7">
+        <v>0</v>
+      </c>
+      <c r="M275" s="7">
+        <v>0</v>
+      </c>
+      <c r="N275" s="7">
+        <v>2.9216195740444801</v>
+      </c>
+      <c r="O275" s="7">
+        <v>0</v>
+      </c>
+      <c r="P275" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q275" s="7">
+        <v>0</v>
+      </c>
+      <c r="R275" s="7">
+        <v>3.56080038613627</v>
+      </c>
+      <c r="S275" s="7">
+        <v>0</v>
+      </c>
+      <c r="T275" t="b">
+        <v>0</v>
+      </c>
+      <c r="U275" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V275" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W275" s="12" t="str">
+        <f t="shared" si="15"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="276" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A276" s="10">
+        <v>275</v>
+      </c>
+      <c r="B276" s="7">
+        <v>0</v>
+      </c>
+      <c r="C276" s="7">
+        <v>0</v>
+      </c>
+      <c r="D276" s="7">
+        <v>0</v>
+      </c>
+      <c r="E276" s="7">
+        <v>9.8631375515323398</v>
+      </c>
+      <c r="F276" s="7">
+        <v>12.375013646398701</v>
+      </c>
+      <c r="G276" s="7">
+        <v>0</v>
+      </c>
+      <c r="H276" s="7">
+        <v>0</v>
+      </c>
+      <c r="I276" s="7">
+        <v>0</v>
+      </c>
+      <c r="J276" s="7">
+        <v>0</v>
+      </c>
+      <c r="K276" s="7">
+        <v>0</v>
+      </c>
+      <c r="L276" s="7">
+        <v>0</v>
+      </c>
+      <c r="M276" s="7">
+        <v>0</v>
+      </c>
+      <c r="N276" s="7">
+        <v>2.4277404392616901</v>
+      </c>
+      <c r="O276" s="7">
+        <v>0</v>
+      </c>
+      <c r="P276" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q276" s="7">
+        <v>0</v>
+      </c>
+      <c r="R276" s="7">
+        <v>1.7656294103721699</v>
+      </c>
+      <c r="S276" s="7">
+        <v>0</v>
+      </c>
+      <c r="T276" t="b">
+        <v>1</v>
+      </c>
+      <c r="U276" s="2">
+        <v>29</v>
+      </c>
+      <c r="V276" s="2">
+        <v>15</v>
+      </c>
+      <c r="W276" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A277" s="10">
+        <v>276</v>
+      </c>
+      <c r="B277" s="7">
+        <v>0</v>
+      </c>
+      <c r="C277" s="7">
+        <v>0</v>
+      </c>
+      <c r="D277" s="7">
+        <v>0</v>
+      </c>
+      <c r="E277" s="7">
+        <v>0</v>
+      </c>
+      <c r="F277" s="7">
+        <v>0</v>
+      </c>
+      <c r="G277" s="7">
+        <v>0</v>
+      </c>
+      <c r="H277" s="7">
+        <v>10.334694882431201</v>
+      </c>
+      <c r="I277" s="7">
+        <v>0</v>
+      </c>
+      <c r="J277" s="7">
+        <v>0</v>
+      </c>
+      <c r="K277" s="7">
+        <v>0</v>
+      </c>
+      <c r="L277" s="7">
+        <v>0</v>
+      </c>
+      <c r="M277" s="7">
+        <v>9.2808018797427998</v>
+      </c>
+      <c r="N277" s="7">
+        <v>2.2617059382718798</v>
+      </c>
+      <c r="O277" s="7">
+        <v>0</v>
+      </c>
+      <c r="P277" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q277" s="7">
+        <v>0</v>
+      </c>
+      <c r="R277" s="7">
+        <v>2.2852524658483402</v>
+      </c>
+      <c r="S277" s="7">
+        <v>0</v>
+      </c>
+      <c r="T277" t="b">
+        <v>0</v>
+      </c>
+      <c r="U277" s="2" t="str">
+        <f t="shared" si="12"/>
+        <v>NA</v>
+      </c>
+      <c r="V277" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v>NA</v>
+      </c>
+      <c r="W277" s="12" t="str">
+        <f>IF(T277=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W253">
+  <conditionalFormatting sqref="A1:W277">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
@@ -36855,7 +38601,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updated dataset till S300
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25BD140D-E703-C943-A921-866D4C9C0906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E2E639C-6D40-7A47-A8AF-84D2C817CA54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4840" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -359,7 +359,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -690,11 +700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W277"/>
+  <dimension ref="A1:W301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="92" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W277" sqref="A1:W277"/>
+    <sheetView tabSelected="1" topLeftCell="A261" zoomScale="92" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W301" sqref="W301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16788,11 +16798,11 @@
         <v>0</v>
       </c>
       <c r="U220" s="2" t="str">
-        <f t="shared" ref="U220:U277" si="12">IF(T220=FALSE, "NA", "")</f>
+        <f t="shared" ref="U220:U283" si="12">IF(T220=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V220" s="2" t="str">
-        <f t="shared" ref="V220:V277" si="13">IF(T220=FALSE, "NA", "")</f>
+        <f t="shared" ref="V220:V283" si="13">IF(T220=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W220" s="12" t="str">
@@ -18489,7 +18499,7 @@
         <v>NA</v>
       </c>
       <c r="W243" s="12" t="str">
-        <f t="shared" ref="W243:W276" si="15">IF(T243=FALSE, "NA", "")</f>
+        <f t="shared" ref="W243:W275" si="15">IF(T243=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -20964,8 +20974,1760 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="278" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A278" s="10">
+        <v>277</v>
+      </c>
+      <c r="B278" s="7">
+        <v>0</v>
+      </c>
+      <c r="C278" s="7">
+        <v>0</v>
+      </c>
+      <c r="D278" s="7">
+        <v>0</v>
+      </c>
+      <c r="E278" s="7">
+        <v>9.0479424430514506</v>
+      </c>
+      <c r="F278" s="7">
+        <v>0</v>
+      </c>
+      <c r="G278" s="7">
+        <v>0</v>
+      </c>
+      <c r="H278" s="7">
+        <v>0</v>
+      </c>
+      <c r="I278" s="7">
+        <v>0</v>
+      </c>
+      <c r="J278" s="7">
+        <v>0</v>
+      </c>
+      <c r="K278" s="7">
+        <v>0</v>
+      </c>
+      <c r="L278" s="7">
+        <v>0</v>
+      </c>
+      <c r="M278" s="7">
+        <v>11.5424260715183</v>
+      </c>
+      <c r="N278" s="7">
+        <v>1.17260969756024</v>
+      </c>
+      <c r="O278" s="7">
+        <v>0</v>
+      </c>
+      <c r="P278" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q278" s="7">
+        <v>0</v>
+      </c>
+      <c r="R278" s="7">
+        <v>1.0726785582859499</v>
+      </c>
+      <c r="S278" s="7">
+        <v>0</v>
+      </c>
+      <c r="T278" t="b">
+        <v>1</v>
+      </c>
+      <c r="U278" s="2">
+        <v>21</v>
+      </c>
+      <c r="V278" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="W278" s="12" t="str">
+        <f t="shared" ref="W278:W301" si="16">IF(T278=FALSE, "NA", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="279" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A279" s="10">
+        <v>278</v>
+      </c>
+      <c r="B279" s="7">
+        <v>0</v>
+      </c>
+      <c r="C279" s="7">
+        <v>0</v>
+      </c>
+      <c r="D279" s="7">
+        <v>0</v>
+      </c>
+      <c r="E279" s="7">
+        <v>14.4543180189381</v>
+      </c>
+      <c r="F279" s="7">
+        <v>12.474550519730199</v>
+      </c>
+      <c r="G279" s="7">
+        <v>0</v>
+      </c>
+      <c r="H279" s="7">
+        <v>0</v>
+      </c>
+      <c r="I279" s="7">
+        <v>0</v>
+      </c>
+      <c r="J279" s="7">
+        <v>0</v>
+      </c>
+      <c r="K279" s="7">
+        <v>0</v>
+      </c>
+      <c r="L279" s="7">
+        <v>0</v>
+      </c>
+      <c r="M279" s="7">
+        <v>0</v>
+      </c>
+      <c r="N279" s="7">
+        <v>1.5606383400809201</v>
+      </c>
+      <c r="O279" s="7">
+        <v>0</v>
+      </c>
+      <c r="P279" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q279" s="7">
+        <v>0</v>
+      </c>
+      <c r="R279" s="7">
+        <v>1.14678728141218</v>
+      </c>
+      <c r="S279" s="7">
+        <v>0</v>
+      </c>
+      <c r="T279" t="b">
+        <v>1</v>
+      </c>
+      <c r="U279" s="2">
+        <v>73</v>
+      </c>
+      <c r="V279" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="W279" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="280" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A280" s="10">
+        <v>279</v>
+      </c>
+      <c r="B280" s="7">
+        <v>0</v>
+      </c>
+      <c r="C280" s="7">
+        <v>0</v>
+      </c>
+      <c r="D280" s="7">
+        <v>0</v>
+      </c>
+      <c r="E280" s="7">
+        <v>0</v>
+      </c>
+      <c r="F280" s="7">
+        <v>0</v>
+      </c>
+      <c r="G280" s="7">
+        <v>0</v>
+      </c>
+      <c r="H280" s="7">
+        <v>12.0485909138945</v>
+      </c>
+      <c r="I280" s="7">
+        <v>0</v>
+      </c>
+      <c r="J280" s="7">
+        <v>10.2446028557261</v>
+      </c>
+      <c r="K280" s="7">
+        <v>0</v>
+      </c>
+      <c r="L280" s="7">
+        <v>0</v>
+      </c>
+      <c r="M280" s="7">
+        <v>0</v>
+      </c>
+      <c r="N280" s="7">
+        <v>1.17860224717853</v>
+      </c>
+      <c r="O280" s="7">
+        <v>0</v>
+      </c>
+      <c r="P280" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q280" s="7">
+        <v>0</v>
+      </c>
+      <c r="R280" s="7">
+        <v>1.28574790601293</v>
+      </c>
+      <c r="S280" s="7">
+        <v>0</v>
+      </c>
+      <c r="T280" t="b">
+        <v>1</v>
+      </c>
+      <c r="U280" s="2">
+        <v>29</v>
+      </c>
+      <c r="V280" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="W280" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="281" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A281" s="10">
+        <v>280</v>
+      </c>
+      <c r="B281" s="7">
+        <v>0</v>
+      </c>
+      <c r="C281" s="7">
+        <v>0</v>
+      </c>
+      <c r="D281" s="7">
+        <v>0</v>
+      </c>
+      <c r="E281" s="7">
+        <v>12.4766467767029</v>
+      </c>
+      <c r="F281" s="7">
+        <v>12.6173036721136</v>
+      </c>
+      <c r="G281" s="7">
+        <v>0</v>
+      </c>
+      <c r="H281" s="7">
+        <v>0</v>
+      </c>
+      <c r="I281" s="7">
+        <v>0</v>
+      </c>
+      <c r="J281" s="7">
+        <v>0</v>
+      </c>
+      <c r="K281" s="7">
+        <v>0</v>
+      </c>
+      <c r="L281" s="7">
+        <v>0</v>
+      </c>
+      <c r="M281" s="7">
+        <v>0</v>
+      </c>
+      <c r="N281" s="7">
+        <v>2.7228513875117502</v>
+      </c>
+      <c r="O281" s="7">
+        <v>0</v>
+      </c>
+      <c r="P281" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q281" s="7">
+        <v>0</v>
+      </c>
+      <c r="R281" s="7">
+        <v>1.3733054991114999</v>
+      </c>
+      <c r="S281" s="7">
+        <v>0</v>
+      </c>
+      <c r="T281" t="b">
+        <v>1</v>
+      </c>
+      <c r="U281" s="2">
+        <v>21</v>
+      </c>
+      <c r="V281" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="W281" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="282" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A282" s="10">
+        <v>281</v>
+      </c>
+      <c r="B282" s="7">
+        <v>0</v>
+      </c>
+      <c r="C282" s="7">
+        <v>0</v>
+      </c>
+      <c r="D282" s="7">
+        <v>0</v>
+      </c>
+      <c r="E282" s="7">
+        <v>0</v>
+      </c>
+      <c r="F282" s="7">
+        <v>13.5739044493449</v>
+      </c>
+      <c r="G282" s="7">
+        <v>0</v>
+      </c>
+      <c r="H282" s="7">
+        <v>0</v>
+      </c>
+      <c r="I282" s="7">
+        <v>0</v>
+      </c>
+      <c r="J282" s="7">
+        <v>0</v>
+      </c>
+      <c r="K282" s="7">
+        <v>0</v>
+      </c>
+      <c r="L282" s="7">
+        <v>0</v>
+      </c>
+      <c r="M282" s="7">
+        <v>10.8628400258574</v>
+      </c>
+      <c r="N282" s="7">
+        <v>1.97804033062894</v>
+      </c>
+      <c r="O282" s="7">
+        <v>0</v>
+      </c>
+      <c r="P282" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q282" s="7">
+        <v>0</v>
+      </c>
+      <c r="R282" s="7">
+        <v>1.4279055044343001</v>
+      </c>
+      <c r="S282" s="7">
+        <v>0</v>
+      </c>
+      <c r="T282" t="b">
+        <v>1</v>
+      </c>
+      <c r="U282" s="2">
+        <v>31</v>
+      </c>
+      <c r="V282" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="W282" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="283" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A283" s="10">
+        <v>282</v>
+      </c>
+      <c r="B283" s="7">
+        <v>0</v>
+      </c>
+      <c r="C283" s="7">
+        <v>0</v>
+      </c>
+      <c r="D283" s="7">
+        <v>0</v>
+      </c>
+      <c r="E283" s="7">
+        <v>0</v>
+      </c>
+      <c r="F283" s="7">
+        <v>0</v>
+      </c>
+      <c r="G283" s="7">
+        <v>0</v>
+      </c>
+      <c r="H283" s="7">
+        <v>0</v>
+      </c>
+      <c r="I283" s="7">
+        <v>0</v>
+      </c>
+      <c r="J283" s="7">
+        <v>12.2328145001671</v>
+      </c>
+      <c r="K283" s="7">
+        <v>0</v>
+      </c>
+      <c r="L283" s="7">
+        <v>0</v>
+      </c>
+      <c r="M283" s="7">
+        <v>12.5993817042082</v>
+      </c>
+      <c r="N283" s="7">
+        <v>1.2653522388815199</v>
+      </c>
+      <c r="O283" s="7">
+        <v>0</v>
+      </c>
+      <c r="P283" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q283" s="7">
+        <v>0</v>
+      </c>
+      <c r="R283" s="7">
+        <v>1.70369310279243</v>
+      </c>
+      <c r="S283" s="7">
+        <v>0</v>
+      </c>
+      <c r="T283" t="b">
+        <v>1</v>
+      </c>
+      <c r="U283" s="2">
+        <v>17</v>
+      </c>
+      <c r="V283" s="2" t="str">
+        <f t="shared" si="13"/>
+        <v/>
+      </c>
+      <c r="W283" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="284" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A284" s="10">
+        <v>283</v>
+      </c>
+      <c r="B284" s="7">
+        <v>0</v>
+      </c>
+      <c r="C284" s="7">
+        <v>0</v>
+      </c>
+      <c r="D284" s="7">
+        <v>0</v>
+      </c>
+      <c r="E284" s="7">
+        <v>11.8152367075649</v>
+      </c>
+      <c r="F284" s="7">
+        <v>0</v>
+      </c>
+      <c r="G284" s="7">
+        <v>0</v>
+      </c>
+      <c r="H284" s="7">
+        <v>0</v>
+      </c>
+      <c r="I284" s="7">
+        <v>0</v>
+      </c>
+      <c r="J284" s="7">
+        <v>0</v>
+      </c>
+      <c r="K284" s="7">
+        <v>0</v>
+      </c>
+      <c r="L284" s="7">
+        <v>0</v>
+      </c>
+      <c r="M284" s="7">
+        <v>12.711753002217501</v>
+      </c>
+      <c r="N284" s="7">
+        <v>1.2695599555466699</v>
+      </c>
+      <c r="O284" s="7">
+        <v>0</v>
+      </c>
+      <c r="P284" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q284" s="7">
+        <v>0</v>
+      </c>
+      <c r="R284" s="7">
+        <v>1.7415434777877099</v>
+      </c>
+      <c r="S284" s="7">
+        <v>0</v>
+      </c>
+      <c r="T284" t="b">
+        <v>1</v>
+      </c>
+      <c r="U284" s="2">
+        <v>20</v>
+      </c>
+      <c r="V284" s="2" t="str">
+        <f t="shared" ref="V284:V301" si="17">IF(T284=FALSE, "NA", "")</f>
+        <v/>
+      </c>
+      <c r="W284" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="285" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A285" s="10">
+        <v>284</v>
+      </c>
+      <c r="B285" s="7">
+        <v>0</v>
+      </c>
+      <c r="C285" s="7">
+        <v>0</v>
+      </c>
+      <c r="D285" s="7">
+        <v>0</v>
+      </c>
+      <c r="E285" s="7">
+        <v>0</v>
+      </c>
+      <c r="F285" s="7">
+        <v>0</v>
+      </c>
+      <c r="G285" s="7">
+        <v>0</v>
+      </c>
+      <c r="H285" s="7">
+        <v>12.359174728327099</v>
+      </c>
+      <c r="I285" s="7">
+        <v>0</v>
+      </c>
+      <c r="J285" s="7">
+        <v>12.211030553063599</v>
+      </c>
+      <c r="K285" s="7">
+        <v>0</v>
+      </c>
+      <c r="L285" s="7">
+        <v>0</v>
+      </c>
+      <c r="M285" s="7">
+        <v>0</v>
+      </c>
+      <c r="N285" s="7">
+        <v>1.7468667333169301</v>
+      </c>
+      <c r="O285" s="7">
+        <v>0</v>
+      </c>
+      <c r="P285" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q285" s="7">
+        <v>0</v>
+      </c>
+      <c r="R285" s="7">
+        <v>1.4123078041799499</v>
+      </c>
+      <c r="S285" s="7">
+        <v>0</v>
+      </c>
+      <c r="T285" t="b">
+        <v>1</v>
+      </c>
+      <c r="U285" s="2">
+        <v>19</v>
+      </c>
+      <c r="V285" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W285" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="286" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A286" s="10">
+        <v>285</v>
+      </c>
+      <c r="B286" s="7">
+        <v>0</v>
+      </c>
+      <c r="C286" s="7">
+        <v>0</v>
+      </c>
+      <c r="D286" s="7">
+        <v>0</v>
+      </c>
+      <c r="E286" s="7">
+        <v>0</v>
+      </c>
+      <c r="F286" s="7">
+        <v>0</v>
+      </c>
+      <c r="G286" s="7">
+        <v>0</v>
+      </c>
+      <c r="H286" s="7">
+        <v>13.000542080164299</v>
+      </c>
+      <c r="I286" s="7">
+        <v>0</v>
+      </c>
+      <c r="J286" s="7">
+        <v>0</v>
+      </c>
+      <c r="K286" s="7">
+        <v>0</v>
+      </c>
+      <c r="L286" s="7">
+        <v>0</v>
+      </c>
+      <c r="M286" s="7">
+        <v>12.787321344453099</v>
+      </c>
+      <c r="N286" s="7">
+        <v>1.25242503904397</v>
+      </c>
+      <c r="O286" s="7">
+        <v>0</v>
+      </c>
+      <c r="P286" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q286" s="7">
+        <v>0</v>
+      </c>
+      <c r="R286" s="7">
+        <v>1.1450743214115799</v>
+      </c>
+      <c r="S286" s="7">
+        <v>0</v>
+      </c>
+      <c r="T286" t="b">
+        <v>1</v>
+      </c>
+      <c r="U286" s="2">
+        <v>18</v>
+      </c>
+      <c r="V286" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W286" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="287" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A287" s="10">
+        <v>286</v>
+      </c>
+      <c r="B287" s="7">
+        <v>0</v>
+      </c>
+      <c r="C287" s="7">
+        <v>0</v>
+      </c>
+      <c r="D287" s="7">
+        <v>0</v>
+      </c>
+      <c r="E287" s="7">
+        <v>0</v>
+      </c>
+      <c r="F287" s="7">
+        <v>8.6882036124305007</v>
+      </c>
+      <c r="G287" s="7">
+        <v>0</v>
+      </c>
+      <c r="H287" s="7">
+        <v>0</v>
+      </c>
+      <c r="I287" s="7">
+        <v>0</v>
+      </c>
+      <c r="J287" s="7">
+        <v>0</v>
+      </c>
+      <c r="K287" s="7">
+        <v>0</v>
+      </c>
+      <c r="L287" s="7">
+        <v>0</v>
+      </c>
+      <c r="M287" s="7">
+        <v>12.4060876015544</v>
+      </c>
+      <c r="N287" s="7">
+        <v>1.10940121752673</v>
+      </c>
+      <c r="O287" s="7">
+        <v>0</v>
+      </c>
+      <c r="P287" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q287" s="7">
+        <v>0</v>
+      </c>
+      <c r="R287" s="7">
+        <v>1.2787175764659899</v>
+      </c>
+      <c r="S287" s="7">
+        <v>0</v>
+      </c>
+      <c r="T287" t="b">
+        <v>1</v>
+      </c>
+      <c r="U287" s="2">
+        <v>25</v>
+      </c>
+      <c r="V287" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W287" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="288" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A288" s="10">
+        <v>287</v>
+      </c>
+      <c r="B288" s="7">
+        <v>0</v>
+      </c>
+      <c r="C288" s="7">
+        <v>0</v>
+      </c>
+      <c r="D288" s="7">
+        <v>0</v>
+      </c>
+      <c r="E288" s="7">
+        <v>0</v>
+      </c>
+      <c r="F288" s="7">
+        <v>0</v>
+      </c>
+      <c r="G288" s="7">
+        <v>0</v>
+      </c>
+      <c r="H288" s="7">
+        <v>0</v>
+      </c>
+      <c r="I288" s="7">
+        <v>0</v>
+      </c>
+      <c r="J288" s="7">
+        <v>11.657203983520001</v>
+      </c>
+      <c r="K288" s="7">
+        <v>0</v>
+      </c>
+      <c r="L288" s="7">
+        <v>0</v>
+      </c>
+      <c r="M288" s="7">
+        <v>12.0759839883893</v>
+      </c>
+      <c r="N288" s="7">
+        <v>1.6487597578875399</v>
+      </c>
+      <c r="O288" s="7">
+        <v>0</v>
+      </c>
+      <c r="P288" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q288" s="7">
+        <v>0</v>
+      </c>
+      <c r="R288" s="7">
+        <v>1.18869858864295</v>
+      </c>
+      <c r="S288" s="7">
+        <v>0</v>
+      </c>
+      <c r="T288" t="b">
+        <v>1</v>
+      </c>
+      <c r="U288" s="2">
+        <v>19</v>
+      </c>
+      <c r="V288" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W288" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="289" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A289" s="10">
+        <v>288</v>
+      </c>
+      <c r="B289" s="7">
+        <v>0</v>
+      </c>
+      <c r="C289" s="7">
+        <v>0</v>
+      </c>
+      <c r="D289" s="7">
+        <v>0</v>
+      </c>
+      <c r="E289" s="7">
+        <v>0</v>
+      </c>
+      <c r="F289" s="7">
+        <v>12.7175812001444</v>
+      </c>
+      <c r="G289" s="7">
+        <v>0</v>
+      </c>
+      <c r="H289" s="7">
+        <v>0</v>
+      </c>
+      <c r="I289" s="7">
+        <v>0</v>
+      </c>
+      <c r="J289" s="7">
+        <v>0</v>
+      </c>
+      <c r="K289" s="7">
+        <v>0</v>
+      </c>
+      <c r="L289" s="7">
+        <v>0</v>
+      </c>
+      <c r="M289" s="7">
+        <v>11.6190656723301</v>
+      </c>
+      <c r="N289" s="7">
+        <v>1.20211656661585</v>
+      </c>
+      <c r="O289" s="7">
+        <v>0</v>
+      </c>
+      <c r="P289" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q289" s="7">
+        <v>0</v>
+      </c>
+      <c r="R289" s="7">
+        <v>1.60938430822259</v>
+      </c>
+      <c r="S289" s="7">
+        <v>0</v>
+      </c>
+      <c r="T289" t="b">
+        <v>1</v>
+      </c>
+      <c r="U289" s="2">
+        <v>20</v>
+      </c>
+      <c r="V289" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W289" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="290" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A290" s="10">
+        <v>289</v>
+      </c>
+      <c r="B290" s="7">
+        <v>0</v>
+      </c>
+      <c r="C290" s="7">
+        <v>0</v>
+      </c>
+      <c r="D290" s="7">
+        <v>0</v>
+      </c>
+      <c r="E290" s="7">
+        <v>8.4691884818040393</v>
+      </c>
+      <c r="F290" s="7">
+        <v>0</v>
+      </c>
+      <c r="G290" s="7">
+        <v>0</v>
+      </c>
+      <c r="H290" s="7">
+        <v>0</v>
+      </c>
+      <c r="I290" s="7">
+        <v>0</v>
+      </c>
+      <c r="J290" s="7">
+        <v>0</v>
+      </c>
+      <c r="K290" s="7">
+        <v>0</v>
+      </c>
+      <c r="L290" s="7">
+        <v>0</v>
+      </c>
+      <c r="M290" s="7">
+        <v>13.0557358248839</v>
+      </c>
+      <c r="N290" s="7">
+        <v>2.0665834169671302</v>
+      </c>
+      <c r="O290" s="7">
+        <v>0</v>
+      </c>
+      <c r="P290" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q290" s="7">
+        <v>0</v>
+      </c>
+      <c r="R290" s="7">
+        <v>1.17148655047705</v>
+      </c>
+      <c r="S290" s="7">
+        <v>0</v>
+      </c>
+      <c r="T290" t="b">
+        <v>1</v>
+      </c>
+      <c r="U290" s="2">
+        <v>23</v>
+      </c>
+      <c r="V290" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W290" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="291" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A291" s="10">
+        <v>290</v>
+      </c>
+      <c r="B291" s="7">
+        <v>0</v>
+      </c>
+      <c r="C291" s="7">
+        <v>0</v>
+      </c>
+      <c r="D291" s="7">
+        <v>0</v>
+      </c>
+      <c r="E291" s="7">
+        <v>13.9203689437531</v>
+      </c>
+      <c r="F291" s="7">
+        <v>0</v>
+      </c>
+      <c r="G291" s="7">
+        <v>0</v>
+      </c>
+      <c r="H291" s="7">
+        <v>0</v>
+      </c>
+      <c r="I291" s="7">
+        <v>0</v>
+      </c>
+      <c r="J291" s="7">
+        <v>0</v>
+      </c>
+      <c r="K291" s="7">
+        <v>0</v>
+      </c>
+      <c r="L291" s="7">
+        <v>0</v>
+      </c>
+      <c r="M291" s="7">
+        <v>9.4395134737880504</v>
+      </c>
+      <c r="N291" s="7">
+        <v>1.3316803344579999</v>
+      </c>
+      <c r="O291" s="7">
+        <v>0</v>
+      </c>
+      <c r="P291" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q291" s="7">
+        <v>0</v>
+      </c>
+      <c r="R291" s="7">
+        <v>1.3644564229087099</v>
+      </c>
+      <c r="S291" s="7">
+        <v>0</v>
+      </c>
+      <c r="T291" t="b">
+        <v>1</v>
+      </c>
+      <c r="U291" s="2">
+        <v>36</v>
+      </c>
+      <c r="V291" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W291" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="292" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A292" s="10">
+        <v>291</v>
+      </c>
+      <c r="B292" s="7">
+        <v>0</v>
+      </c>
+      <c r="C292" s="7">
+        <v>0</v>
+      </c>
+      <c r="D292" s="7">
+        <v>0</v>
+      </c>
+      <c r="E292" s="7">
+        <v>13.950043681331</v>
+      </c>
+      <c r="F292" s="7">
+        <v>7.7784070792326396</v>
+      </c>
+      <c r="G292" s="7">
+        <v>0</v>
+      </c>
+      <c r="H292" s="7">
+        <v>0</v>
+      </c>
+      <c r="I292" s="7">
+        <v>0</v>
+      </c>
+      <c r="J292" s="7">
+        <v>0</v>
+      </c>
+      <c r="K292" s="7">
+        <v>0</v>
+      </c>
+      <c r="L292" s="7">
+        <v>0</v>
+      </c>
+      <c r="M292" s="7">
+        <v>0</v>
+      </c>
+      <c r="N292" s="7">
+        <v>2.8091671342490399</v>
+      </c>
+      <c r="O292" s="7">
+        <v>0</v>
+      </c>
+      <c r="P292" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q292" s="7">
+        <v>0</v>
+      </c>
+      <c r="R292" s="7">
+        <v>1.1456039506265701</v>
+      </c>
+      <c r="S292" s="7">
+        <v>0</v>
+      </c>
+      <c r="T292" t="b">
+        <v>1</v>
+      </c>
+      <c r="U292" s="2">
+        <v>24</v>
+      </c>
+      <c r="V292" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W292" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="293" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A293" s="10">
+        <v>292</v>
+      </c>
+      <c r="B293" s="7">
+        <v>0</v>
+      </c>
+      <c r="C293" s="7">
+        <v>0</v>
+      </c>
+      <c r="D293" s="7">
+        <v>0</v>
+      </c>
+      <c r="E293" s="7">
+        <v>0</v>
+      </c>
+      <c r="F293" s="7">
+        <v>12.2689934520308</v>
+      </c>
+      <c r="G293" s="7">
+        <v>0</v>
+      </c>
+      <c r="H293" s="7">
+        <v>0</v>
+      </c>
+      <c r="I293" s="7">
+        <v>0</v>
+      </c>
+      <c r="J293" s="7">
+        <v>0</v>
+      </c>
+      <c r="K293" s="7">
+        <v>0</v>
+      </c>
+      <c r="L293" s="7">
+        <v>0</v>
+      </c>
+      <c r="M293" s="7">
+        <v>10.432107495906701</v>
+      </c>
+      <c r="N293" s="7">
+        <v>1.5486226528663001</v>
+      </c>
+      <c r="O293" s="7">
+        <v>0</v>
+      </c>
+      <c r="P293" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q293" s="7">
+        <v>0</v>
+      </c>
+      <c r="R293" s="7">
+        <v>1.16573484735439</v>
+      </c>
+      <c r="S293" s="7">
+        <v>0</v>
+      </c>
+      <c r="T293" t="b">
+        <v>1</v>
+      </c>
+      <c r="U293" s="2">
+        <v>23</v>
+      </c>
+      <c r="V293" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W293" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="294" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A294" s="10">
+        <v>293</v>
+      </c>
+      <c r="B294" s="7">
+        <v>0</v>
+      </c>
+      <c r="C294" s="7">
+        <v>0</v>
+      </c>
+      <c r="D294" s="7">
+        <v>0</v>
+      </c>
+      <c r="E294" s="7">
+        <v>12.0074387706644</v>
+      </c>
+      <c r="F294" s="7">
+        <v>0</v>
+      </c>
+      <c r="G294" s="7">
+        <v>0</v>
+      </c>
+      <c r="H294" s="7">
+        <v>0</v>
+      </c>
+      <c r="I294" s="7">
+        <v>0</v>
+      </c>
+      <c r="J294" s="7">
+        <v>0</v>
+      </c>
+      <c r="K294" s="7">
+        <v>0</v>
+      </c>
+      <c r="L294" s="7">
+        <v>0</v>
+      </c>
+      <c r="M294" s="7">
+        <v>12.953924764337399</v>
+      </c>
+      <c r="N294" s="7">
+        <v>1.72199703300226</v>
+      </c>
+      <c r="O294" s="7">
+        <v>0</v>
+      </c>
+      <c r="P294" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q294" s="7">
+        <v>0</v>
+      </c>
+      <c r="R294" s="7">
+        <v>1.5872746477745401</v>
+      </c>
+      <c r="S294" s="7">
+        <v>0</v>
+      </c>
+      <c r="T294" t="b">
+        <v>1</v>
+      </c>
+      <c r="U294" s="2">
+        <v>22</v>
+      </c>
+      <c r="V294" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W294" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="295" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A295" s="10">
+        <v>294</v>
+      </c>
+      <c r="B295" s="7">
+        <v>0</v>
+      </c>
+      <c r="C295" s="7">
+        <v>0</v>
+      </c>
+      <c r="D295" s="7">
+        <v>0</v>
+      </c>
+      <c r="E295" s="7">
+        <v>0</v>
+      </c>
+      <c r="F295" s="7">
+        <v>0</v>
+      </c>
+      <c r="G295" s="7">
+        <v>0</v>
+      </c>
+      <c r="H295" s="7">
+        <v>12.719086086645699</v>
+      </c>
+      <c r="I295" s="7">
+        <v>0</v>
+      </c>
+      <c r="J295" s="7">
+        <v>13.0062944401192</v>
+      </c>
+      <c r="K295" s="7">
+        <v>0</v>
+      </c>
+      <c r="L295" s="7">
+        <v>0</v>
+      </c>
+      <c r="M295" s="7">
+        <v>0</v>
+      </c>
+      <c r="N295" s="7">
+        <v>1.10047186983865</v>
+      </c>
+      <c r="O295" s="7">
+        <v>0</v>
+      </c>
+      <c r="P295" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q295" s="7">
+        <v>0</v>
+      </c>
+      <c r="R295" s="7">
+        <v>2.0923770081236199</v>
+      </c>
+      <c r="S295" s="7">
+        <v>0</v>
+      </c>
+      <c r="T295" t="b">
+        <v>1</v>
+      </c>
+      <c r="U295" s="2">
+        <v>19</v>
+      </c>
+      <c r="V295" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W295" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="296" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A296" s="10">
+        <v>295</v>
+      </c>
+      <c r="B296" s="7">
+        <v>0</v>
+      </c>
+      <c r="C296" s="7">
+        <v>0</v>
+      </c>
+      <c r="D296" s="7">
+        <v>0</v>
+      </c>
+      <c r="E296" s="7">
+        <v>0</v>
+      </c>
+      <c r="F296" s="7">
+        <v>0</v>
+      </c>
+      <c r="G296" s="7">
+        <v>0</v>
+      </c>
+      <c r="H296" s="7">
+        <v>0</v>
+      </c>
+      <c r="I296" s="7">
+        <v>0</v>
+      </c>
+      <c r="J296" s="7">
+        <v>12.3943281829035</v>
+      </c>
+      <c r="K296" s="7">
+        <v>0</v>
+      </c>
+      <c r="L296" s="7">
+        <v>0</v>
+      </c>
+      <c r="M296" s="7">
+        <v>9.5819504692567605</v>
+      </c>
+      <c r="N296" s="7">
+        <v>0.84782703104947699</v>
+      </c>
+      <c r="O296" s="7">
+        <v>0</v>
+      </c>
+      <c r="P296" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q296" s="7">
+        <v>0</v>
+      </c>
+      <c r="R296" s="7">
+        <v>1.2591987265881499</v>
+      </c>
+      <c r="S296" s="7">
+        <v>0</v>
+      </c>
+      <c r="T296" t="b">
+        <v>1</v>
+      </c>
+      <c r="U296" s="2">
+        <v>14</v>
+      </c>
+      <c r="V296" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W296" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="297" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A297" s="10">
+        <v>296</v>
+      </c>
+      <c r="B297" s="7">
+        <v>0</v>
+      </c>
+      <c r="C297" s="7">
+        <v>0</v>
+      </c>
+      <c r="D297" s="7">
+        <v>0</v>
+      </c>
+      <c r="E297" s="7">
+        <v>0</v>
+      </c>
+      <c r="F297" s="7">
+        <v>8.3865754680621691</v>
+      </c>
+      <c r="G297" s="7">
+        <v>0</v>
+      </c>
+      <c r="H297" s="7">
+        <v>0</v>
+      </c>
+      <c r="I297" s="7">
+        <v>0</v>
+      </c>
+      <c r="J297" s="7">
+        <v>0</v>
+      </c>
+      <c r="K297" s="7">
+        <v>0</v>
+      </c>
+      <c r="L297" s="7">
+        <v>0</v>
+      </c>
+      <c r="M297" s="7">
+        <v>12.9347651694845</v>
+      </c>
+      <c r="N297" s="7">
+        <v>1.9711174609355699</v>
+      </c>
+      <c r="O297" s="7">
+        <v>0</v>
+      </c>
+      <c r="P297" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q297" s="7">
+        <v>0</v>
+      </c>
+      <c r="R297" s="7">
+        <v>1.1846869650124101</v>
+      </c>
+      <c r="S297" s="7">
+        <v>0</v>
+      </c>
+      <c r="T297" t="b">
+        <v>1</v>
+      </c>
+      <c r="U297" s="2">
+        <v>33</v>
+      </c>
+      <c r="V297" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W297" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="298" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A298" s="10">
+        <v>297</v>
+      </c>
+      <c r="B298" s="7">
+        <v>0</v>
+      </c>
+      <c r="C298" s="7">
+        <v>0</v>
+      </c>
+      <c r="D298" s="7">
+        <v>0</v>
+      </c>
+      <c r="E298" s="7">
+        <v>12.163869868881701</v>
+      </c>
+      <c r="F298" s="7">
+        <v>13.079357048405001</v>
+      </c>
+      <c r="G298" s="7">
+        <v>0</v>
+      </c>
+      <c r="H298" s="7">
+        <v>0</v>
+      </c>
+      <c r="I298" s="7">
+        <v>0</v>
+      </c>
+      <c r="J298" s="7">
+        <v>0</v>
+      </c>
+      <c r="K298" s="7">
+        <v>0</v>
+      </c>
+      <c r="L298" s="7">
+        <v>0</v>
+      </c>
+      <c r="M298" s="7">
+        <v>0</v>
+      </c>
+      <c r="N298" s="7">
+        <v>2.1167613621779</v>
+      </c>
+      <c r="O298" s="7">
+        <v>0</v>
+      </c>
+      <c r="P298" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q298" s="7">
+        <v>0</v>
+      </c>
+      <c r="R298" s="7">
+        <v>1.40955962561507</v>
+      </c>
+      <c r="S298" s="7">
+        <v>0</v>
+      </c>
+      <c r="T298" t="b">
+        <v>1</v>
+      </c>
+      <c r="U298" s="2">
+        <v>24</v>
+      </c>
+      <c r="V298" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W298" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="299" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A299" s="10">
+        <v>298</v>
+      </c>
+      <c r="B299" s="7">
+        <v>0</v>
+      </c>
+      <c r="C299" s="7">
+        <v>0</v>
+      </c>
+      <c r="D299" s="7">
+        <v>0</v>
+      </c>
+      <c r="E299" s="7">
+        <v>10.1703811076931</v>
+      </c>
+      <c r="F299" s="7">
+        <v>12.707374345017699</v>
+      </c>
+      <c r="G299" s="7">
+        <v>0</v>
+      </c>
+      <c r="H299" s="7">
+        <v>0</v>
+      </c>
+      <c r="I299" s="7">
+        <v>0</v>
+      </c>
+      <c r="J299" s="7">
+        <v>0</v>
+      </c>
+      <c r="K299" s="7">
+        <v>0</v>
+      </c>
+      <c r="L299" s="7">
+        <v>0</v>
+      </c>
+      <c r="M299" s="7">
+        <v>0</v>
+      </c>
+      <c r="N299" s="7">
+        <v>2.5318783316043998</v>
+      </c>
+      <c r="O299" s="7">
+        <v>0</v>
+      </c>
+      <c r="P299" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q299" s="7">
+        <v>0</v>
+      </c>
+      <c r="R299" s="7">
+        <v>1.14476461361619</v>
+      </c>
+      <c r="S299" s="7">
+        <v>0</v>
+      </c>
+      <c r="T299" t="b">
+        <v>1</v>
+      </c>
+      <c r="U299" s="2">
+        <v>24</v>
+      </c>
+      <c r="V299" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W299" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="300" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A300" s="10">
+        <v>299</v>
+      </c>
+      <c r="B300" s="7">
+        <v>0</v>
+      </c>
+      <c r="C300" s="7">
+        <v>0</v>
+      </c>
+      <c r="D300" s="7">
+        <v>0</v>
+      </c>
+      <c r="E300" s="7">
+        <v>14.118611991368301</v>
+      </c>
+      <c r="F300" s="7">
+        <v>0</v>
+      </c>
+      <c r="G300" s="7">
+        <v>0</v>
+      </c>
+      <c r="H300" s="7">
+        <v>0</v>
+      </c>
+      <c r="I300" s="7">
+        <v>0</v>
+      </c>
+      <c r="J300" s="7">
+        <v>0</v>
+      </c>
+      <c r="K300" s="7">
+        <v>0</v>
+      </c>
+      <c r="L300" s="7">
+        <v>0</v>
+      </c>
+      <c r="M300" s="7">
+        <v>11.2461075487717</v>
+      </c>
+      <c r="N300" s="7">
+        <v>2.5387069879172102</v>
+      </c>
+      <c r="O300" s="7">
+        <v>0</v>
+      </c>
+      <c r="P300" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q300" s="7">
+        <v>0</v>
+      </c>
+      <c r="R300" s="7">
+        <v>1.20011603065178</v>
+      </c>
+      <c r="S300" s="7">
+        <v>0</v>
+      </c>
+      <c r="T300" t="b">
+        <v>1</v>
+      </c>
+      <c r="U300" s="2">
+        <v>29</v>
+      </c>
+      <c r="V300" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W300" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
+    <row r="301" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A301" s="10">
+        <v>300</v>
+      </c>
+      <c r="B301" s="7">
+        <v>0</v>
+      </c>
+      <c r="C301" s="7">
+        <v>0</v>
+      </c>
+      <c r="D301" s="7">
+        <v>0</v>
+      </c>
+      <c r="E301" s="7">
+        <v>12.0395739012358</v>
+      </c>
+      <c r="F301" s="7">
+        <v>0</v>
+      </c>
+      <c r="G301" s="7">
+        <v>0</v>
+      </c>
+      <c r="H301" s="7">
+        <v>0</v>
+      </c>
+      <c r="I301" s="7">
+        <v>0</v>
+      </c>
+      <c r="J301" s="7">
+        <v>0</v>
+      </c>
+      <c r="K301" s="7">
+        <v>0</v>
+      </c>
+      <c r="L301" s="7">
+        <v>0</v>
+      </c>
+      <c r="M301" s="7">
+        <v>11.5763617422982</v>
+      </c>
+      <c r="N301" s="7">
+        <v>1.2085402338236999</v>
+      </c>
+      <c r="O301" s="7">
+        <v>0</v>
+      </c>
+      <c r="P301" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q301" s="7">
+        <v>0</v>
+      </c>
+      <c r="R301" s="7">
+        <v>1.6606648676803</v>
+      </c>
+      <c r="S301" s="7">
+        <v>0</v>
+      </c>
+      <c r="T301" t="b">
+        <v>1</v>
+      </c>
+      <c r="U301" s="2">
+        <v>18</v>
+      </c>
+      <c r="V301" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W301" s="12" t="str">
+        <f t="shared" si="16"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W277">
+  <conditionalFormatting sqref="A1:W301">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
@@ -31120,7 +32882,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated dataset till S324
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D95519-86AE-3C46-BA4E-CB8993923F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F6062D-9BBE-A448-A90F-0F04D10879CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-5300" windowWidth="38400" windowHeight="21600" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -690,11 +690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W301"/>
+  <dimension ref="A1:W337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="108" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W301" sqref="W301"/>
+    <sheetView tabSelected="1" topLeftCell="A264" zoomScale="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W325" sqref="W325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16788,11 +16788,11 @@
         <v>0</v>
       </c>
       <c r="U220" s="2" t="str">
-        <f t="shared" ref="U220:U277" si="12">IF(T220=FALSE, "NA", "")</f>
+        <f t="shared" ref="U220:U275" si="12">IF(T220=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V220" s="2" t="str">
-        <f t="shared" ref="V220:V283" si="13">IF(T220=FALSE, "NA", "")</f>
+        <f t="shared" ref="V220:V277" si="13">IF(T220=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W220" s="12" t="str">
@@ -20952,7 +20952,7 @@
         <v>0</v>
       </c>
       <c r="U277" s="2" t="str">
-        <f t="shared" si="12"/>
+        <f>IF(T277=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V277" s="2" t="str">
@@ -22668,8 +22668,1802 @@
         <v>0</v>
       </c>
     </row>
+    <row r="302" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A302" s="10">
+        <v>301</v>
+      </c>
+      <c r="B302" s="7">
+        <v>0</v>
+      </c>
+      <c r="C302" s="7">
+        <v>0</v>
+      </c>
+      <c r="D302" s="7">
+        <v>0</v>
+      </c>
+      <c r="E302" s="7">
+        <v>11.8856413645932</v>
+      </c>
+      <c r="F302" s="7">
+        <v>0</v>
+      </c>
+      <c r="G302" s="7">
+        <v>0</v>
+      </c>
+      <c r="H302" s="7">
+        <v>0</v>
+      </c>
+      <c r="I302" s="7">
+        <v>6.6854217089702903</v>
+      </c>
+      <c r="J302" s="7">
+        <v>0</v>
+      </c>
+      <c r="K302" s="7">
+        <v>0</v>
+      </c>
+      <c r="L302" s="7">
+        <v>0</v>
+      </c>
+      <c r="M302" s="7">
+        <v>0</v>
+      </c>
+      <c r="N302" s="7">
+        <v>0</v>
+      </c>
+      <c r="O302" s="7">
+        <v>0</v>
+      </c>
+      <c r="P302" s="7">
+        <v>2.8011051598955898</v>
+      </c>
+      <c r="Q302" s="7">
+        <v>0</v>
+      </c>
+      <c r="R302" s="7">
+        <v>4.9858917170300598</v>
+      </c>
+      <c r="S302" s="7">
+        <v>0</v>
+      </c>
+      <c r="T302" t="b">
+        <v>1</v>
+      </c>
+      <c r="U302" s="2">
+        <v>2447</v>
+      </c>
+      <c r="V302" s="2">
+        <v>41</v>
+      </c>
+      <c r="W302" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="303" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A303" s="10">
+        <v>302</v>
+      </c>
+      <c r="B303" s="7">
+        <v>0</v>
+      </c>
+      <c r="C303" s="7">
+        <v>0</v>
+      </c>
+      <c r="D303" s="7">
+        <v>10.457587722222501</v>
+      </c>
+      <c r="E303" s="7">
+        <v>0</v>
+      </c>
+      <c r="F303" s="7">
+        <v>0</v>
+      </c>
+      <c r="G303" s="7">
+        <v>0</v>
+      </c>
+      <c r="H303" s="7">
+        <v>12.6611119778182</v>
+      </c>
+      <c r="I303" s="7">
+        <v>0</v>
+      </c>
+      <c r="J303" s="7">
+        <v>0</v>
+      </c>
+      <c r="K303" s="7">
+        <v>0</v>
+      </c>
+      <c r="L303" s="7">
+        <v>0</v>
+      </c>
+      <c r="M303" s="7">
+        <v>0</v>
+      </c>
+      <c r="N303" s="7">
+        <v>0</v>
+      </c>
+      <c r="O303" s="7">
+        <v>0</v>
+      </c>
+      <c r="P303" s="7">
+        <v>1.51881891887701</v>
+      </c>
+      <c r="Q303" s="7">
+        <v>0</v>
+      </c>
+      <c r="R303" s="7">
+        <v>2.98816490880048</v>
+      </c>
+      <c r="S303" s="7">
+        <v>0</v>
+      </c>
+      <c r="T303" t="b">
+        <v>1</v>
+      </c>
+      <c r="U303" s="2">
+        <v>15</v>
+      </c>
+      <c r="V303" s="2">
+        <v>5</v>
+      </c>
+      <c r="W303" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="304" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A304" s="10">
+        <v>303</v>
+      </c>
+      <c r="B304" s="7">
+        <v>0</v>
+      </c>
+      <c r="C304" s="7">
+        <v>0</v>
+      </c>
+      <c r="D304" s="7">
+        <v>0</v>
+      </c>
+      <c r="E304" s="7">
+        <v>8.5577504978556203</v>
+      </c>
+      <c r="F304" s="7">
+        <v>0</v>
+      </c>
+      <c r="G304" s="7">
+        <v>0</v>
+      </c>
+      <c r="H304" s="7">
+        <v>0</v>
+      </c>
+      <c r="I304" s="7">
+        <v>0</v>
+      </c>
+      <c r="J304" s="7">
+        <v>0</v>
+      </c>
+      <c r="K304" s="7">
+        <v>0</v>
+      </c>
+      <c r="L304" s="7">
+        <v>0</v>
+      </c>
+      <c r="M304" s="7">
+        <v>11.093490290174</v>
+      </c>
+      <c r="N304" s="7">
+        <v>0</v>
+      </c>
+      <c r="O304" s="7">
+        <v>0</v>
+      </c>
+      <c r="P304" s="7">
+        <v>1.84412938820503</v>
+      </c>
+      <c r="Q304" s="7">
+        <v>0</v>
+      </c>
+      <c r="R304" s="7">
+        <v>3.1238809233754798</v>
+      </c>
+      <c r="S304" s="7">
+        <v>0</v>
+      </c>
+      <c r="T304" t="b">
+        <v>0</v>
+      </c>
+      <c r="U304" s="2" t="str">
+        <f>IF(T304=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V304" s="2" t="str">
+        <f>IF(T304=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W304" s="12" t="str">
+        <f>IF(T304=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="305" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A305" s="10">
+        <v>304</v>
+      </c>
+      <c r="B305" s="7">
+        <v>5.4381784094815497</v>
+      </c>
+      <c r="C305" s="7">
+        <v>8.7037817297442892</v>
+      </c>
+      <c r="D305" s="7">
+        <v>0</v>
+      </c>
+      <c r="E305" s="7">
+        <v>0</v>
+      </c>
+      <c r="F305" s="7">
+        <v>0</v>
+      </c>
+      <c r="G305" s="7">
+        <v>0</v>
+      </c>
+      <c r="H305" s="7">
+        <v>0</v>
+      </c>
+      <c r="I305" s="7">
+        <v>0</v>
+      </c>
+      <c r="J305" s="7">
+        <v>0</v>
+      </c>
+      <c r="K305" s="7">
+        <v>0</v>
+      </c>
+      <c r="L305" s="7">
+        <v>0</v>
+      </c>
+      <c r="M305" s="7">
+        <v>0</v>
+      </c>
+      <c r="N305" s="7">
+        <v>0</v>
+      </c>
+      <c r="O305" s="7">
+        <v>0</v>
+      </c>
+      <c r="P305" s="7">
+        <v>2.3994251134511702</v>
+      </c>
+      <c r="Q305" s="7">
+        <v>0</v>
+      </c>
+      <c r="R305" s="7">
+        <v>4.81181308542988</v>
+      </c>
+      <c r="S305" s="7">
+        <v>0</v>
+      </c>
+      <c r="T305" t="b">
+        <v>1</v>
+      </c>
+      <c r="U305" s="2">
+        <v>730</v>
+      </c>
+      <c r="V305" s="2">
+        <v>10</v>
+      </c>
+      <c r="W305" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A306" s="10">
+        <v>305</v>
+      </c>
+      <c r="B306" s="7">
+        <v>0</v>
+      </c>
+      <c r="C306" s="7">
+        <v>9.1935749098104296</v>
+      </c>
+      <c r="D306" s="7">
+        <v>0</v>
+      </c>
+      <c r="E306" s="7">
+        <v>0</v>
+      </c>
+      <c r="F306" s="7">
+        <v>11.0464982323762</v>
+      </c>
+      <c r="G306" s="7">
+        <v>0</v>
+      </c>
+      <c r="H306" s="7">
+        <v>0</v>
+      </c>
+      <c r="I306" s="7">
+        <v>0</v>
+      </c>
+      <c r="J306" s="7">
+        <v>0</v>
+      </c>
+      <c r="K306" s="7">
+        <v>0</v>
+      </c>
+      <c r="L306" s="7">
+        <v>0</v>
+      </c>
+      <c r="M306" s="7">
+        <v>0</v>
+      </c>
+      <c r="N306" s="7">
+        <v>0</v>
+      </c>
+      <c r="O306" s="7">
+        <v>0</v>
+      </c>
+      <c r="P306" s="7">
+        <v>2.5253865662070201</v>
+      </c>
+      <c r="Q306" s="7">
+        <v>0</v>
+      </c>
+      <c r="R306" s="7">
+        <v>3.5423534107875998</v>
+      </c>
+      <c r="S306" s="7">
+        <v>0</v>
+      </c>
+      <c r="T306" t="b">
+        <v>1</v>
+      </c>
+      <c r="U306" s="2">
+        <v>16</v>
+      </c>
+      <c r="V306" s="2">
+        <v>5</v>
+      </c>
+      <c r="W306" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A307" s="10">
+        <v>306</v>
+      </c>
+      <c r="B307" s="7">
+        <v>0</v>
+      </c>
+      <c r="C307" s="7">
+        <v>0</v>
+      </c>
+      <c r="D307" s="7">
+        <v>0</v>
+      </c>
+      <c r="E307" s="7">
+        <v>0</v>
+      </c>
+      <c r="F307" s="7">
+        <v>0</v>
+      </c>
+      <c r="G307" s="7">
+        <v>11.011100857519001</v>
+      </c>
+      <c r="H307" s="7">
+        <v>0</v>
+      </c>
+      <c r="I307" s="7">
+        <v>0</v>
+      </c>
+      <c r="J307" s="7">
+        <v>8.2529058243888809</v>
+      </c>
+      <c r="K307" s="7">
+        <v>0</v>
+      </c>
+      <c r="L307" s="7">
+        <v>0</v>
+      </c>
+      <c r="M307" s="7">
+        <v>0</v>
+      </c>
+      <c r="N307" s="7">
+        <v>0</v>
+      </c>
+      <c r="O307" s="7">
+        <v>0</v>
+      </c>
+      <c r="P307" s="7">
+        <v>2.9784367587122702</v>
+      </c>
+      <c r="Q307" s="7">
+        <v>0</v>
+      </c>
+      <c r="R307" s="7">
+        <v>2.4142828978808799</v>
+      </c>
+      <c r="S307" s="7">
+        <v>0</v>
+      </c>
+      <c r="T307" t="b">
+        <v>0</v>
+      </c>
+      <c r="U307" s="2" t="str">
+        <f t="shared" ref="U307:U325" si="16">IF(T307=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V307" s="2" t="str">
+        <f t="shared" ref="V305:V325" si="17">IF(T307=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W307" s="12" t="str">
+        <f t="shared" ref="W305:W325" si="18">IF(T307=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="308" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A308" s="10">
+        <v>307</v>
+      </c>
+      <c r="B308" s="7">
+        <v>0</v>
+      </c>
+      <c r="C308" s="7">
+        <v>0</v>
+      </c>
+      <c r="D308" s="7">
+        <v>0</v>
+      </c>
+      <c r="E308" s="7">
+        <v>0</v>
+      </c>
+      <c r="F308" s="7">
+        <v>0</v>
+      </c>
+      <c r="G308" s="7">
+        <v>8.9009972988586306</v>
+      </c>
+      <c r="H308" s="7">
+        <v>0</v>
+      </c>
+      <c r="I308" s="7">
+        <v>0</v>
+      </c>
+      <c r="J308" s="7">
+        <v>0</v>
+      </c>
+      <c r="K308" s="7">
+        <v>10.7534638581492</v>
+      </c>
+      <c r="L308" s="7">
+        <v>0</v>
+      </c>
+      <c r="M308" s="7">
+        <v>0</v>
+      </c>
+      <c r="N308" s="7">
+        <v>0</v>
+      </c>
+      <c r="O308" s="7">
+        <v>0</v>
+      </c>
+      <c r="P308" s="7">
+        <v>1.8228529751213101</v>
+      </c>
+      <c r="Q308" s="7">
+        <v>0</v>
+      </c>
+      <c r="R308" s="7">
+        <v>1.7220672474866601</v>
+      </c>
+      <c r="S308" s="7">
+        <v>0</v>
+      </c>
+      <c r="T308" t="b">
+        <v>1</v>
+      </c>
+      <c r="U308" s="2">
+        <v>19</v>
+      </c>
+      <c r="V308" s="2">
+        <v>2</v>
+      </c>
+      <c r="W308" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A309" s="10">
+        <v>308</v>
+      </c>
+      <c r="B309" s="7">
+        <v>8.1131640642811398</v>
+      </c>
+      <c r="C309" s="7">
+        <v>0</v>
+      </c>
+      <c r="D309" s="7">
+        <v>0</v>
+      </c>
+      <c r="E309" s="7">
+        <v>0</v>
+      </c>
+      <c r="F309" s="7">
+        <v>0</v>
+      </c>
+      <c r="G309" s="7">
+        <v>0</v>
+      </c>
+      <c r="H309" s="7">
+        <v>0</v>
+      </c>
+      <c r="I309" s="7">
+        <v>0</v>
+      </c>
+      <c r="J309" s="7">
+        <v>0</v>
+      </c>
+      <c r="K309" s="7">
+        <v>0</v>
+      </c>
+      <c r="L309" s="7">
+        <v>0</v>
+      </c>
+      <c r="M309" s="7">
+        <v>12.557903269619301</v>
+      </c>
+      <c r="N309" s="7">
+        <v>0</v>
+      </c>
+      <c r="O309" s="7">
+        <v>0</v>
+      </c>
+      <c r="P309" s="7">
+        <v>2.15628362365231</v>
+      </c>
+      <c r="Q309" s="7">
+        <v>0</v>
+      </c>
+      <c r="R309" s="7">
+        <v>2.3404362529285199</v>
+      </c>
+      <c r="S309" s="7">
+        <v>0</v>
+      </c>
+      <c r="T309" t="b">
+        <v>0</v>
+      </c>
+      <c r="U309" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V309" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W309" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="310" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A310" s="10">
+        <v>309</v>
+      </c>
+      <c r="B310" s="7">
+        <v>0</v>
+      </c>
+      <c r="C310" s="7">
+        <v>0</v>
+      </c>
+      <c r="D310" s="7">
+        <v>10.683821208828499</v>
+      </c>
+      <c r="E310" s="7">
+        <v>0</v>
+      </c>
+      <c r="F310" s="7">
+        <v>0</v>
+      </c>
+      <c r="G310" s="7">
+        <v>0</v>
+      </c>
+      <c r="H310" s="7">
+        <v>0</v>
+      </c>
+      <c r="I310" s="7">
+        <v>0</v>
+      </c>
+      <c r="J310" s="7">
+        <v>0</v>
+      </c>
+      <c r="K310" s="7">
+        <v>11.584818497197601</v>
+      </c>
+      <c r="L310" s="7">
+        <v>0</v>
+      </c>
+      <c r="M310" s="7">
+        <v>0</v>
+      </c>
+      <c r="N310" s="7">
+        <v>0</v>
+      </c>
+      <c r="O310" s="7">
+        <v>0</v>
+      </c>
+      <c r="P310" s="7">
+        <v>1.90853477428754</v>
+      </c>
+      <c r="Q310" s="7">
+        <v>0</v>
+      </c>
+      <c r="R310" s="7">
+        <v>1.74338505081304</v>
+      </c>
+      <c r="S310" s="7">
+        <v>0</v>
+      </c>
+      <c r="T310" t="b">
+        <v>1</v>
+      </c>
+      <c r="U310" s="2">
+        <v>14</v>
+      </c>
+      <c r="V310" s="2">
+        <v>5</v>
+      </c>
+      <c r="W310" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="311" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A311" s="10">
+        <v>310</v>
+      </c>
+      <c r="B311" s="7">
+        <v>0</v>
+      </c>
+      <c r="C311" s="7">
+        <v>9.0601343312784106</v>
+      </c>
+      <c r="D311" s="7">
+        <v>0</v>
+      </c>
+      <c r="E311" s="7">
+        <v>0</v>
+      </c>
+      <c r="F311" s="7">
+        <v>0</v>
+      </c>
+      <c r="G311" s="7">
+        <v>0</v>
+      </c>
+      <c r="H311" s="7">
+        <v>0</v>
+      </c>
+      <c r="I311" s="7">
+        <v>0</v>
+      </c>
+      <c r="J311" s="7">
+        <v>10.9937724030792</v>
+      </c>
+      <c r="K311" s="7">
+        <v>0</v>
+      </c>
+      <c r="L311" s="7">
+        <v>0</v>
+      </c>
+      <c r="M311" s="7">
+        <v>0</v>
+      </c>
+      <c r="N311" s="7">
+        <v>0</v>
+      </c>
+      <c r="O311" s="7">
+        <v>0</v>
+      </c>
+      <c r="P311" s="7">
+        <v>2.7678491442078701</v>
+      </c>
+      <c r="Q311" s="7">
+        <v>0</v>
+      </c>
+      <c r="R311" s="7">
+        <v>4.6474986079822296</v>
+      </c>
+      <c r="S311" s="7">
+        <v>0</v>
+      </c>
+      <c r="T311" t="b">
+        <v>1</v>
+      </c>
+      <c r="U311" s="2">
+        <v>58</v>
+      </c>
+      <c r="V311" s="2">
+        <v>471</v>
+      </c>
+      <c r="W311" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="312" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A312" s="10">
+        <v>311</v>
+      </c>
+      <c r="B312" s="7">
+        <v>0</v>
+      </c>
+      <c r="C312" s="7">
+        <v>0</v>
+      </c>
+      <c r="D312" s="7">
+        <v>0</v>
+      </c>
+      <c r="E312" s="7">
+        <v>0</v>
+      </c>
+      <c r="F312" s="7">
+        <v>0</v>
+      </c>
+      <c r="G312" s="7">
+        <v>0</v>
+      </c>
+      <c r="H312" s="7">
+        <v>8.1636229767029995</v>
+      </c>
+      <c r="I312" s="7">
+        <v>0</v>
+      </c>
+      <c r="J312" s="7">
+        <v>0</v>
+      </c>
+      <c r="K312" s="7">
+        <v>0</v>
+      </c>
+      <c r="L312" s="7">
+        <v>11.627821357322301</v>
+      </c>
+      <c r="M312" s="7">
+        <v>0</v>
+      </c>
+      <c r="N312" s="7">
+        <v>0</v>
+      </c>
+      <c r="O312" s="7">
+        <v>0</v>
+      </c>
+      <c r="P312" s="7">
+        <v>2.1278585147736702</v>
+      </c>
+      <c r="Q312" s="7">
+        <v>0</v>
+      </c>
+      <c r="R312" s="7">
+        <v>2.01730427787066</v>
+      </c>
+      <c r="S312" s="7">
+        <v>0</v>
+      </c>
+      <c r="T312" t="b">
+        <v>0</v>
+      </c>
+      <c r="U312" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V312" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W312" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="313" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A313" s="10">
+        <v>312</v>
+      </c>
+      <c r="B313" s="7">
+        <v>0</v>
+      </c>
+      <c r="C313" s="7">
+        <v>0</v>
+      </c>
+      <c r="D313" s="7">
+        <v>0</v>
+      </c>
+      <c r="E313" s="7">
+        <v>0</v>
+      </c>
+      <c r="F313" s="7">
+        <v>0</v>
+      </c>
+      <c r="G313" s="7">
+        <v>0</v>
+      </c>
+      <c r="H313" s="7">
+        <v>0</v>
+      </c>
+      <c r="I313" s="7">
+        <v>0</v>
+      </c>
+      <c r="J313" s="7">
+        <v>0</v>
+      </c>
+      <c r="K313" s="7">
+        <v>0</v>
+      </c>
+      <c r="L313" s="7">
+        <v>12.7975831283454</v>
+      </c>
+      <c r="M313" s="7">
+        <v>11.639237017498999</v>
+      </c>
+      <c r="N313" s="7">
+        <v>0</v>
+      </c>
+      <c r="O313" s="7">
+        <v>0</v>
+      </c>
+      <c r="P313" s="7">
+        <v>1.45664762434465</v>
+      </c>
+      <c r="Q313" s="7">
+        <v>0</v>
+      </c>
+      <c r="R313" s="7">
+        <v>3.1772348182288099</v>
+      </c>
+      <c r="S313" s="7">
+        <v>0</v>
+      </c>
+      <c r="T313" t="b">
+        <v>0</v>
+      </c>
+      <c r="U313" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V313" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W313" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="314" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A314" s="10">
+        <v>313</v>
+      </c>
+      <c r="B314" s="7">
+        <v>0</v>
+      </c>
+      <c r="C314" s="7">
+        <v>0</v>
+      </c>
+      <c r="D314" s="7">
+        <v>0</v>
+      </c>
+      <c r="E314" s="7">
+        <v>0</v>
+      </c>
+      <c r="F314" s="7">
+        <v>12.1792429274826</v>
+      </c>
+      <c r="G314" s="7">
+        <v>0</v>
+      </c>
+      <c r="H314" s="7">
+        <v>0</v>
+      </c>
+      <c r="I314" s="7">
+        <v>0</v>
+      </c>
+      <c r="J314" s="7">
+        <v>8.6214180892636207</v>
+      </c>
+      <c r="K314" s="7">
+        <v>0</v>
+      </c>
+      <c r="L314" s="7">
+        <v>0</v>
+      </c>
+      <c r="M314" s="7">
+        <v>0</v>
+      </c>
+      <c r="N314" s="7">
+        <v>0</v>
+      </c>
+      <c r="O314" s="7">
+        <v>0</v>
+      </c>
+      <c r="P314" s="7">
+        <v>2.3999425643069499</v>
+      </c>
+      <c r="Q314" s="7">
+        <v>0</v>
+      </c>
+      <c r="R314" s="7">
+        <v>1.04787973319973</v>
+      </c>
+      <c r="S314" s="7">
+        <v>0</v>
+      </c>
+      <c r="T314" t="b">
+        <v>1</v>
+      </c>
+      <c r="U314" s="2">
+        <v>23</v>
+      </c>
+      <c r="V314" s="2">
+        <v>8</v>
+      </c>
+      <c r="W314" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A315" s="10">
+        <v>314</v>
+      </c>
+      <c r="B315" s="7">
+        <v>0</v>
+      </c>
+      <c r="C315" s="7">
+        <v>0</v>
+      </c>
+      <c r="D315" s="7">
+        <v>0</v>
+      </c>
+      <c r="E315" s="7">
+        <v>11.9069727723268</v>
+      </c>
+      <c r="F315" s="7">
+        <v>0</v>
+      </c>
+      <c r="G315" s="7">
+        <v>0</v>
+      </c>
+      <c r="H315" s="7">
+        <v>0</v>
+      </c>
+      <c r="I315" s="7">
+        <v>0</v>
+      </c>
+      <c r="J315" s="7">
+        <v>0</v>
+      </c>
+      <c r="K315" s="7">
+        <v>10.317314070825301</v>
+      </c>
+      <c r="L315" s="7">
+        <v>0</v>
+      </c>
+      <c r="M315" s="7">
+        <v>0</v>
+      </c>
+      <c r="N315" s="7">
+        <v>0</v>
+      </c>
+      <c r="O315" s="7">
+        <v>0</v>
+      </c>
+      <c r="P315" s="7">
+        <v>1.4893694990528099</v>
+      </c>
+      <c r="Q315" s="7">
+        <v>0</v>
+      </c>
+      <c r="R315" s="7">
+        <v>4.4755927659979298</v>
+      </c>
+      <c r="S315" s="7">
+        <v>0</v>
+      </c>
+      <c r="T315" t="b">
+        <v>0</v>
+      </c>
+      <c r="U315" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V315" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W315" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="316" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A316" s="10">
+        <v>315</v>
+      </c>
+      <c r="B316" s="7">
+        <v>0</v>
+      </c>
+      <c r="C316" s="7">
+        <v>11.494123371495199</v>
+      </c>
+      <c r="D316" s="7">
+        <v>0</v>
+      </c>
+      <c r="E316" s="7">
+        <v>0</v>
+      </c>
+      <c r="F316" s="7">
+        <v>0</v>
+      </c>
+      <c r="G316" s="7">
+        <v>0</v>
+      </c>
+      <c r="H316" s="7">
+        <v>0</v>
+      </c>
+      <c r="I316" s="7">
+        <v>0</v>
+      </c>
+      <c r="J316" s="7">
+        <v>0</v>
+      </c>
+      <c r="K316" s="7">
+        <v>0</v>
+      </c>
+      <c r="L316" s="7">
+        <v>8.69857669468532</v>
+      </c>
+      <c r="M316" s="7">
+        <v>0</v>
+      </c>
+      <c r="N316" s="7">
+        <v>0</v>
+      </c>
+      <c r="O316" s="7">
+        <v>0</v>
+      </c>
+      <c r="P316" s="7">
+        <v>1.0546430077230999</v>
+      </c>
+      <c r="Q316" s="7">
+        <v>0</v>
+      </c>
+      <c r="R316" s="7">
+        <v>3.35703267247079</v>
+      </c>
+      <c r="S316" s="7">
+        <v>0</v>
+      </c>
+      <c r="T316" t="b">
+        <v>1</v>
+      </c>
+      <c r="U316" s="2">
+        <v>25</v>
+      </c>
+      <c r="V316" s="2">
+        <v>3</v>
+      </c>
+      <c r="W316" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A317" s="10">
+        <v>316</v>
+      </c>
+      <c r="B317" s="7">
+        <v>0</v>
+      </c>
+      <c r="C317" s="7">
+        <v>9.3890798774183892</v>
+      </c>
+      <c r="D317" s="7">
+        <v>0</v>
+      </c>
+      <c r="E317" s="7">
+        <v>0</v>
+      </c>
+      <c r="F317" s="7">
+        <v>0</v>
+      </c>
+      <c r="G317" s="7">
+        <v>9.0807405634291491</v>
+      </c>
+      <c r="H317" s="7">
+        <v>0</v>
+      </c>
+      <c r="I317" s="7">
+        <v>0</v>
+      </c>
+      <c r="J317" s="7">
+        <v>0</v>
+      </c>
+      <c r="K317" s="7">
+        <v>0</v>
+      </c>
+      <c r="L317" s="7">
+        <v>0</v>
+      </c>
+      <c r="M317" s="7">
+        <v>0</v>
+      </c>
+      <c r="N317" s="7">
+        <v>0</v>
+      </c>
+      <c r="O317" s="7">
+        <v>0</v>
+      </c>
+      <c r="P317" s="7">
+        <v>3.0341376584250002</v>
+      </c>
+      <c r="Q317" s="7">
+        <v>0</v>
+      </c>
+      <c r="R317" s="7">
+        <v>3.0292121102781802</v>
+      </c>
+      <c r="S317" s="7">
+        <v>0</v>
+      </c>
+      <c r="T317" t="b">
+        <v>1</v>
+      </c>
+      <c r="U317" s="2">
+        <v>28</v>
+      </c>
+      <c r="V317" s="2">
+        <v>8</v>
+      </c>
+      <c r="W317" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="318" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A318" s="10">
+        <v>317</v>
+      </c>
+      <c r="B318" s="7">
+        <v>5.1468825557761297</v>
+      </c>
+      <c r="C318" s="7">
+        <v>0</v>
+      </c>
+      <c r="D318" s="7">
+        <v>0</v>
+      </c>
+      <c r="E318" s="7">
+        <v>0</v>
+      </c>
+      <c r="F318" s="7">
+        <v>0</v>
+      </c>
+      <c r="G318" s="7">
+        <v>0</v>
+      </c>
+      <c r="H318" s="7">
+        <v>0</v>
+      </c>
+      <c r="I318" s="7">
+        <v>12.0888038455351</v>
+      </c>
+      <c r="J318" s="7">
+        <v>0</v>
+      </c>
+      <c r="K318" s="7">
+        <v>0</v>
+      </c>
+      <c r="L318" s="7">
+        <v>0</v>
+      </c>
+      <c r="M318" s="7">
+        <v>0</v>
+      </c>
+      <c r="N318" s="7">
+        <v>0</v>
+      </c>
+      <c r="O318" s="7">
+        <v>0</v>
+      </c>
+      <c r="P318" s="7">
+        <v>2.4263578963384602</v>
+      </c>
+      <c r="Q318" s="7">
+        <v>0</v>
+      </c>
+      <c r="R318" s="7">
+        <v>1.3051060616378001</v>
+      </c>
+      <c r="S318" s="7">
+        <v>0</v>
+      </c>
+      <c r="T318" t="b">
+        <v>1</v>
+      </c>
+      <c r="U318" s="2">
+        <v>411</v>
+      </c>
+      <c r="V318" s="2">
+        <v>151</v>
+      </c>
+      <c r="W318" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="319" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A319" s="10">
+        <v>318</v>
+      </c>
+      <c r="B319" s="7">
+        <v>0</v>
+      </c>
+      <c r="C319" s="7">
+        <v>0</v>
+      </c>
+      <c r="D319" s="7">
+        <v>0</v>
+      </c>
+      <c r="E319" s="7">
+        <v>0</v>
+      </c>
+      <c r="F319" s="7">
+        <v>0</v>
+      </c>
+      <c r="G319" s="7">
+        <v>0</v>
+      </c>
+      <c r="H319" s="7">
+        <v>0</v>
+      </c>
+      <c r="I319" s="7">
+        <v>8.1465888216476596</v>
+      </c>
+      <c r="J319" s="7">
+        <v>0</v>
+      </c>
+      <c r="K319" s="7">
+        <v>0</v>
+      </c>
+      <c r="L319" s="7">
+        <v>0</v>
+      </c>
+      <c r="M319" s="7">
+        <v>11.3386320677215</v>
+      </c>
+      <c r="N319" s="7">
+        <v>0</v>
+      </c>
+      <c r="O319" s="7">
+        <v>0</v>
+      </c>
+      <c r="P319" s="7">
+        <v>3.4043809135985099</v>
+      </c>
+      <c r="Q319" s="7">
+        <v>0</v>
+      </c>
+      <c r="R319" s="7">
+        <v>4.3564113008565997</v>
+      </c>
+      <c r="S319" s="7">
+        <v>0</v>
+      </c>
+      <c r="T319" t="b">
+        <v>1</v>
+      </c>
+      <c r="U319" s="2">
+        <v>2083</v>
+      </c>
+      <c r="V319" s="2">
+        <v>32</v>
+      </c>
+      <c r="W319" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="320" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A320" s="10">
+        <v>319</v>
+      </c>
+      <c r="B320" s="7">
+        <v>0</v>
+      </c>
+      <c r="C320" s="7">
+        <v>0</v>
+      </c>
+      <c r="D320" s="7">
+        <v>11.3645396507416</v>
+      </c>
+      <c r="E320" s="7">
+        <v>0</v>
+      </c>
+      <c r="F320" s="7">
+        <v>0</v>
+      </c>
+      <c r="G320" s="7">
+        <v>0</v>
+      </c>
+      <c r="H320" s="7">
+        <v>0</v>
+      </c>
+      <c r="I320" s="7">
+        <v>0</v>
+      </c>
+      <c r="J320" s="7">
+        <v>10.7967585695772</v>
+      </c>
+      <c r="K320" s="7">
+        <v>0</v>
+      </c>
+      <c r="L320" s="7">
+        <v>0</v>
+      </c>
+      <c r="M320" s="7">
+        <v>0</v>
+      </c>
+      <c r="N320" s="7">
+        <v>0</v>
+      </c>
+      <c r="O320" s="7">
+        <v>0</v>
+      </c>
+      <c r="P320" s="7">
+        <v>1.89384221880547</v>
+      </c>
+      <c r="Q320" s="7">
+        <v>0</v>
+      </c>
+      <c r="R320" s="7">
+        <v>1.5259735863756001</v>
+      </c>
+      <c r="S320" s="7">
+        <v>0</v>
+      </c>
+      <c r="T320" t="b">
+        <v>0</v>
+      </c>
+      <c r="U320" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V320" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W320" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="321" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A321" s="10">
+        <v>320</v>
+      </c>
+      <c r="B321" s="7">
+        <v>0</v>
+      </c>
+      <c r="C321" s="7">
+        <v>0</v>
+      </c>
+      <c r="D321" s="7">
+        <v>13.126857600898401</v>
+      </c>
+      <c r="E321" s="7">
+        <v>0</v>
+      </c>
+      <c r="F321" s="7">
+        <v>0</v>
+      </c>
+      <c r="G321" s="7">
+        <v>0</v>
+      </c>
+      <c r="H321" s="7">
+        <v>0</v>
+      </c>
+      <c r="I321" s="7">
+        <v>0</v>
+      </c>
+      <c r="J321" s="7">
+        <v>0</v>
+      </c>
+      <c r="K321" s="7">
+        <v>0</v>
+      </c>
+      <c r="L321" s="7">
+        <v>0</v>
+      </c>
+      <c r="M321" s="7">
+        <v>11.724960187210201</v>
+      </c>
+      <c r="N321" s="7">
+        <v>0</v>
+      </c>
+      <c r="O321" s="7">
+        <v>0</v>
+      </c>
+      <c r="P321" s="7">
+        <v>2.2351930791671801</v>
+      </c>
+      <c r="Q321" s="7">
+        <v>0</v>
+      </c>
+      <c r="R321" s="7">
+        <v>2.1273548165757599</v>
+      </c>
+      <c r="S321" s="7">
+        <v>0</v>
+      </c>
+      <c r="T321" t="b">
+        <v>0</v>
+      </c>
+      <c r="U321" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V321" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W321" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="322" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A322" s="10">
+        <v>321</v>
+      </c>
+      <c r="B322" s="7">
+        <v>4.9418895174507798</v>
+      </c>
+      <c r="C322" s="7">
+        <v>0</v>
+      </c>
+      <c r="D322" s="7">
+        <v>0</v>
+      </c>
+      <c r="E322" s="7">
+        <v>0</v>
+      </c>
+      <c r="F322" s="7">
+        <v>0</v>
+      </c>
+      <c r="G322" s="7">
+        <v>9.2427026869199302</v>
+      </c>
+      <c r="H322" s="7">
+        <v>0</v>
+      </c>
+      <c r="I322" s="7">
+        <v>0</v>
+      </c>
+      <c r="J322" s="7">
+        <v>0</v>
+      </c>
+      <c r="K322" s="7">
+        <v>0</v>
+      </c>
+      <c r="L322" s="7">
+        <v>0</v>
+      </c>
+      <c r="M322" s="7">
+        <v>0</v>
+      </c>
+      <c r="N322" s="7">
+        <v>0</v>
+      </c>
+      <c r="O322" s="7">
+        <v>0</v>
+      </c>
+      <c r="P322" s="7">
+        <v>2.50517699089905</v>
+      </c>
+      <c r="Q322" s="7">
+        <v>0</v>
+      </c>
+      <c r="R322" s="7">
+        <v>1.3381690758840099</v>
+      </c>
+      <c r="S322" s="7">
+        <v>0</v>
+      </c>
+      <c r="T322" t="b">
+        <v>1</v>
+      </c>
+      <c r="U322" s="2">
+        <v>502</v>
+      </c>
+      <c r="V322" s="2">
+        <v>182</v>
+      </c>
+      <c r="W322" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="323" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A323" s="10">
+        <v>322</v>
+      </c>
+      <c r="B323" s="7">
+        <v>0</v>
+      </c>
+      <c r="C323" s="7">
+        <v>0</v>
+      </c>
+      <c r="D323" s="7">
+        <v>13.577247953314901</v>
+      </c>
+      <c r="E323" s="7">
+        <v>10.0004932179995</v>
+      </c>
+      <c r="F323" s="7">
+        <v>0</v>
+      </c>
+      <c r="G323" s="7">
+        <v>0</v>
+      </c>
+      <c r="H323" s="7">
+        <v>0</v>
+      </c>
+      <c r="I323" s="7">
+        <v>0</v>
+      </c>
+      <c r="J323" s="7">
+        <v>0</v>
+      </c>
+      <c r="K323" s="7">
+        <v>0</v>
+      </c>
+      <c r="L323" s="7">
+        <v>0</v>
+      </c>
+      <c r="M323" s="7">
+        <v>0</v>
+      </c>
+      <c r="N323" s="7">
+        <v>0</v>
+      </c>
+      <c r="O323" s="7">
+        <v>0</v>
+      </c>
+      <c r="P323" s="7">
+        <v>3.0459900548295802</v>
+      </c>
+      <c r="Q323" s="7">
+        <v>0</v>
+      </c>
+      <c r="R323" s="7">
+        <v>3.4783476995575202</v>
+      </c>
+      <c r="S323" s="7">
+        <v>0</v>
+      </c>
+      <c r="T323" t="b">
+        <v>1</v>
+      </c>
+      <c r="U323" s="2">
+        <v>15</v>
+      </c>
+      <c r="V323" s="2">
+        <v>7</v>
+      </c>
+      <c r="W323" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A324" s="10">
+        <v>323</v>
+      </c>
+      <c r="B324" s="7">
+        <v>0</v>
+      </c>
+      <c r="C324" s="7">
+        <v>0</v>
+      </c>
+      <c r="D324" s="7">
+        <v>0</v>
+      </c>
+      <c r="E324" s="7">
+        <v>0</v>
+      </c>
+      <c r="F324" s="7">
+        <v>0</v>
+      </c>
+      <c r="G324" s="7">
+        <v>0</v>
+      </c>
+      <c r="H324" s="7">
+        <v>12.2756417541112</v>
+      </c>
+      <c r="I324" s="7">
+        <v>8.3735837904553705</v>
+      </c>
+      <c r="J324" s="7">
+        <v>0</v>
+      </c>
+      <c r="K324" s="7">
+        <v>0</v>
+      </c>
+      <c r="L324" s="7">
+        <v>0</v>
+      </c>
+      <c r="M324" s="7">
+        <v>0</v>
+      </c>
+      <c r="N324" s="7">
+        <v>0</v>
+      </c>
+      <c r="O324" s="7">
+        <v>0</v>
+      </c>
+      <c r="P324" s="7">
+        <v>3.21328257284594</v>
+      </c>
+      <c r="Q324" s="7">
+        <v>0</v>
+      </c>
+      <c r="R324" s="7">
+        <v>4.4965904334522104</v>
+      </c>
+      <c r="S324" s="7">
+        <v>0</v>
+      </c>
+      <c r="T324" t="b">
+        <v>0</v>
+      </c>
+      <c r="U324" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V324" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W324" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="325" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A325" s="10">
+        <v>324</v>
+      </c>
+      <c r="B325" s="7">
+        <v>0</v>
+      </c>
+      <c r="C325" s="7">
+        <v>0</v>
+      </c>
+      <c r="D325" s="7">
+        <v>0</v>
+      </c>
+      <c r="E325" s="7">
+        <v>0</v>
+      </c>
+      <c r="F325" s="7">
+        <v>8.7855267535158301</v>
+      </c>
+      <c r="G325" s="7">
+        <v>0</v>
+      </c>
+      <c r="H325" s="7">
+        <v>0</v>
+      </c>
+      <c r="I325" s="7">
+        <v>13.945435681053601</v>
+      </c>
+      <c r="J325" s="7">
+        <v>0</v>
+      </c>
+      <c r="K325" s="7">
+        <v>0</v>
+      </c>
+      <c r="L325" s="7">
+        <v>0</v>
+      </c>
+      <c r="M325" s="7">
+        <v>0</v>
+      </c>
+      <c r="N325" s="7">
+        <v>0</v>
+      </c>
+      <c r="O325" s="7">
+        <v>0</v>
+      </c>
+      <c r="P325" s="7">
+        <v>2.3918327841189999</v>
+      </c>
+      <c r="Q325" s="7">
+        <v>0</v>
+      </c>
+      <c r="R325" s="7">
+        <v>1.95939723479413</v>
+      </c>
+      <c r="S325" s="7">
+        <v>0</v>
+      </c>
+      <c r="T325" t="b">
+        <v>0</v>
+      </c>
+      <c r="U325" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V325" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W325" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="326" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A326" s="10">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="327" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A327" s="10">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="328" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A328" s="10">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="329" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A329" s="10">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="330" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A330" s="10">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="331" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A331" s="10">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="332" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A332" s="10">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="333" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A333" s="10">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="334" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A334" s="10">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="335" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A335" s="10">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="336" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A336" s="10">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A337" s="10">
+        <v>336</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W301">
+  <conditionalFormatting sqref="A1:W337">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated dataset to S336
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F6062D-9BBE-A448-A90F-0F04D10879CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D10E34-6C4A-6942-8F66-0184DDD0C9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5300" windowWidth="38400" windowHeight="21600" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -692,9 +692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
   <dimension ref="A1:W337"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A264" zoomScale="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W325" sqref="W325"/>
+    <sheetView tabSelected="1" topLeftCell="A309" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W337" sqref="W337"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23088,15 +23088,15 @@
         <v>0</v>
       </c>
       <c r="U307" s="2" t="str">
-        <f t="shared" ref="U307:U325" si="16">IF(T307=FALSE, "NA", "")</f>
+        <f t="shared" ref="U307:U337" si="16">IF(T307=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V307" s="2" t="str">
-        <f t="shared" ref="V305:V325" si="17">IF(T307=FALSE, "NA", "")</f>
+        <f t="shared" ref="V307:V337" si="17">IF(T307=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W307" s="12" t="str">
-        <f t="shared" ref="W305:W325" si="18">IF(T307=FALSE, "NA", "")</f>
+        <f t="shared" ref="W307:W337" si="18">IF(T307=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -24406,60 +24406,879 @@
       <c r="A326" s="10">
         <v>325</v>
       </c>
+      <c r="B326" s="7">
+        <v>0</v>
+      </c>
+      <c r="C326" s="7">
+        <v>0</v>
+      </c>
+      <c r="D326" s="7">
+        <v>0</v>
+      </c>
+      <c r="E326" s="7">
+        <v>0</v>
+      </c>
+      <c r="F326" s="7">
+        <v>0</v>
+      </c>
+      <c r="G326" s="7">
+        <v>0</v>
+      </c>
+      <c r="H326" s="7">
+        <v>0</v>
+      </c>
+      <c r="I326" s="7">
+        <v>6.8839056279085096</v>
+      </c>
+      <c r="J326" s="7">
+        <v>0</v>
+      </c>
+      <c r="K326" s="7">
+        <v>0</v>
+      </c>
+      <c r="L326" s="7">
+        <v>12.841675478118701</v>
+      </c>
+      <c r="M326" s="7">
+        <v>0</v>
+      </c>
+      <c r="N326" s="7">
+        <v>0</v>
+      </c>
+      <c r="O326" s="7">
+        <v>0</v>
+      </c>
+      <c r="P326" s="7">
+        <v>3.0967980680127098</v>
+      </c>
+      <c r="Q326" s="7">
+        <v>0</v>
+      </c>
+      <c r="R326" s="7">
+        <v>4.2064945628284596</v>
+      </c>
+      <c r="S326" s="7">
+        <v>0</v>
+      </c>
+      <c r="T326" t="b">
+        <v>0</v>
+      </c>
+      <c r="U326" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V326" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W326" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="327" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A327" s="10">
         <v>326</v>
       </c>
+      <c r="B327" s="7">
+        <v>0</v>
+      </c>
+      <c r="C327" s="7">
+        <v>0</v>
+      </c>
+      <c r="D327" s="7">
+        <v>0</v>
+      </c>
+      <c r="E327" s="7">
+        <v>0</v>
+      </c>
+      <c r="F327" s="7">
+        <v>0</v>
+      </c>
+      <c r="G327" s="7">
+        <v>0</v>
+      </c>
+      <c r="H327" s="7">
+        <v>0</v>
+      </c>
+      <c r="I327" s="7">
+        <v>12.718336918402899</v>
+      </c>
+      <c r="J327" s="7">
+        <v>0</v>
+      </c>
+      <c r="K327" s="7">
+        <v>12.6773949278631</v>
+      </c>
+      <c r="L327" s="7">
+        <v>0</v>
+      </c>
+      <c r="M327" s="7">
+        <v>0</v>
+      </c>
+      <c r="N327" s="7">
+        <v>0</v>
+      </c>
+      <c r="O327" s="7">
+        <v>0</v>
+      </c>
+      <c r="P327" s="7">
+        <v>2.2908018516323101</v>
+      </c>
+      <c r="Q327" s="7">
+        <v>0</v>
+      </c>
+      <c r="R327" s="7">
+        <v>4.9520312367200301</v>
+      </c>
+      <c r="S327" s="7">
+        <v>0</v>
+      </c>
+      <c r="T327" t="b">
+        <v>0</v>
+      </c>
+      <c r="U327" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V327" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W327" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="328" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A328" s="10">
         <v>327</v>
       </c>
+      <c r="B328" s="7">
+        <v>0</v>
+      </c>
+      <c r="C328" s="7">
+        <v>0</v>
+      </c>
+      <c r="D328" s="7">
+        <v>0</v>
+      </c>
+      <c r="E328" s="7">
+        <v>0</v>
+      </c>
+      <c r="F328" s="7">
+        <v>0</v>
+      </c>
+      <c r="G328" s="7">
+        <v>0</v>
+      </c>
+      <c r="H328" s="7">
+        <v>0</v>
+      </c>
+      <c r="I328" s="7">
+        <v>0</v>
+      </c>
+      <c r="J328" s="7">
+        <v>0</v>
+      </c>
+      <c r="K328" s="7">
+        <v>10.9165740351428</v>
+      </c>
+      <c r="L328" s="7">
+        <v>9.5268147456526897</v>
+      </c>
+      <c r="M328" s="7">
+        <v>0</v>
+      </c>
+      <c r="N328" s="7">
+        <v>0</v>
+      </c>
+      <c r="O328" s="7">
+        <v>0</v>
+      </c>
+      <c r="P328" s="7">
+        <v>1.7470765766068701</v>
+      </c>
+      <c r="Q328" s="7">
+        <v>0</v>
+      </c>
+      <c r="R328" s="7">
+        <v>4.0201281508352302</v>
+      </c>
+      <c r="S328" s="7">
+        <v>0</v>
+      </c>
+      <c r="T328" t="b">
+        <v>1</v>
+      </c>
+      <c r="U328" s="2">
+        <v>260</v>
+      </c>
+      <c r="V328" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W328" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
     </row>
     <row r="329" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A329" s="10">
         <v>328</v>
       </c>
+      <c r="B329" s="7">
+        <v>5.71608400516965</v>
+      </c>
+      <c r="C329" s="7">
+        <v>0</v>
+      </c>
+      <c r="D329" s="7">
+        <v>0</v>
+      </c>
+      <c r="E329" s="7">
+        <v>0</v>
+      </c>
+      <c r="F329" s="7">
+        <v>0</v>
+      </c>
+      <c r="G329" s="7">
+        <v>0</v>
+      </c>
+      <c r="H329" s="7">
+        <v>0</v>
+      </c>
+      <c r="I329" s="7">
+        <v>0</v>
+      </c>
+      <c r="J329" s="7">
+        <v>0</v>
+      </c>
+      <c r="K329" s="7">
+        <v>10.4575314325762</v>
+      </c>
+      <c r="L329" s="7">
+        <v>0</v>
+      </c>
+      <c r="M329" s="7">
+        <v>0</v>
+      </c>
+      <c r="N329" s="7">
+        <v>0</v>
+      </c>
+      <c r="O329" s="7">
+        <v>0</v>
+      </c>
+      <c r="P329" s="7">
+        <v>1.6814282037173101</v>
+      </c>
+      <c r="Q329" s="7">
+        <v>0</v>
+      </c>
+      <c r="R329" s="7">
+        <v>1.5900881865298799</v>
+      </c>
+      <c r="S329" s="7">
+        <v>0</v>
+      </c>
+      <c r="T329" t="b">
+        <v>1</v>
+      </c>
+      <c r="U329" s="2">
+        <v>17</v>
+      </c>
+      <c r="V329" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W329" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
     </row>
     <row r="330" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A330" s="10">
         <v>329</v>
       </c>
+      <c r="B330" s="7">
+        <v>0</v>
+      </c>
+      <c r="C330" s="7">
+        <v>0</v>
+      </c>
+      <c r="D330" s="7">
+        <v>6.77839884299238</v>
+      </c>
+      <c r="E330" s="7">
+        <v>0</v>
+      </c>
+      <c r="F330" s="7">
+        <v>8.2691178204643094</v>
+      </c>
+      <c r="G330" s="7">
+        <v>0</v>
+      </c>
+      <c r="H330" s="7">
+        <v>0</v>
+      </c>
+      <c r="I330" s="7">
+        <v>0</v>
+      </c>
+      <c r="J330" s="7">
+        <v>0</v>
+      </c>
+      <c r="K330" s="7">
+        <v>0</v>
+      </c>
+      <c r="L330" s="7">
+        <v>0</v>
+      </c>
+      <c r="M330" s="7">
+        <v>0</v>
+      </c>
+      <c r="N330" s="7">
+        <v>0</v>
+      </c>
+      <c r="O330" s="7">
+        <v>0</v>
+      </c>
+      <c r="P330" s="7">
+        <v>1.3346307352876201</v>
+      </c>
+      <c r="Q330" s="7">
+        <v>0</v>
+      </c>
+      <c r="R330" s="7">
+        <v>2.7251888537683699</v>
+      </c>
+      <c r="S330" s="7">
+        <v>0</v>
+      </c>
+      <c r="T330" t="b">
+        <v>1</v>
+      </c>
+      <c r="U330" s="2">
+        <v>14</v>
+      </c>
+      <c r="V330" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W330" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
     </row>
     <row r="331" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A331" s="10">
         <v>330</v>
       </c>
+      <c r="B331" s="7">
+        <v>0</v>
+      </c>
+      <c r="C331" s="7">
+        <v>0</v>
+      </c>
+      <c r="D331" s="7">
+        <v>11.9443176708183</v>
+      </c>
+      <c r="E331" s="7">
+        <v>0</v>
+      </c>
+      <c r="F331" s="7">
+        <v>0</v>
+      </c>
+      <c r="G331" s="7">
+        <v>0</v>
+      </c>
+      <c r="H331" s="7">
+        <v>0</v>
+      </c>
+      <c r="I331" s="7">
+        <v>11.4604409704804</v>
+      </c>
+      <c r="J331" s="7">
+        <v>0</v>
+      </c>
+      <c r="K331" s="7">
+        <v>0</v>
+      </c>
+      <c r="L331" s="7">
+        <v>0</v>
+      </c>
+      <c r="M331" s="7">
+        <v>0</v>
+      </c>
+      <c r="N331" s="7">
+        <v>0</v>
+      </c>
+      <c r="O331" s="7">
+        <v>0</v>
+      </c>
+      <c r="P331" s="7">
+        <v>1.63586060119261</v>
+      </c>
+      <c r="Q331" s="7">
+        <v>0</v>
+      </c>
+      <c r="R331" s="7">
+        <v>3.7956795056453898</v>
+      </c>
+      <c r="S331" s="7">
+        <v>0</v>
+      </c>
+      <c r="T331" t="b">
+        <v>1</v>
+      </c>
+      <c r="U331" s="2">
+        <v>17</v>
+      </c>
+      <c r="V331" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W331" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
     </row>
     <row r="332" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A332" s="10">
         <v>331</v>
       </c>
+      <c r="B332" s="7">
+        <v>0</v>
+      </c>
+      <c r="C332" s="7">
+        <v>0</v>
+      </c>
+      <c r="D332" s="7">
+        <v>0</v>
+      </c>
+      <c r="E332" s="7">
+        <v>0</v>
+      </c>
+      <c r="F332" s="7">
+        <v>0</v>
+      </c>
+      <c r="G332" s="7">
+        <v>0</v>
+      </c>
+      <c r="H332" s="7">
+        <v>11.322698361209699</v>
+      </c>
+      <c r="I332" s="7">
+        <v>0</v>
+      </c>
+      <c r="J332" s="7">
+        <v>0</v>
+      </c>
+      <c r="K332" s="7">
+        <v>12.1542136733379</v>
+      </c>
+      <c r="L332" s="7">
+        <v>0</v>
+      </c>
+      <c r="M332" s="7">
+        <v>0</v>
+      </c>
+      <c r="N332" s="7">
+        <v>0</v>
+      </c>
+      <c r="O332" s="7">
+        <v>0</v>
+      </c>
+      <c r="P332" s="7">
+        <v>1.7550628977643701</v>
+      </c>
+      <c r="Q332" s="7">
+        <v>0</v>
+      </c>
+      <c r="R332" s="7">
+        <v>1.62730920273282</v>
+      </c>
+      <c r="S332" s="7">
+        <v>0</v>
+      </c>
+      <c r="T332" t="b">
+        <v>1</v>
+      </c>
+      <c r="U332" s="2">
+        <v>14</v>
+      </c>
+      <c r="V332" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W332" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
     </row>
     <row r="333" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A333" s="10">
         <v>332</v>
       </c>
+      <c r="B333" s="7">
+        <v>0</v>
+      </c>
+      <c r="C333" s="7">
+        <v>12.097613164707401</v>
+      </c>
+      <c r="D333" s="7">
+        <v>0</v>
+      </c>
+      <c r="E333" s="7">
+        <v>0</v>
+      </c>
+      <c r="F333" s="7">
+        <v>0</v>
+      </c>
+      <c r="G333" s="7">
+        <v>0</v>
+      </c>
+      <c r="H333" s="7">
+        <v>0</v>
+      </c>
+      <c r="I333" s="7">
+        <v>0</v>
+      </c>
+      <c r="J333" s="7">
+        <v>0</v>
+      </c>
+      <c r="K333" s="7">
+        <v>9.1803815116118699</v>
+      </c>
+      <c r="L333" s="7">
+        <v>0</v>
+      </c>
+      <c r="M333" s="7">
+        <v>0</v>
+      </c>
+      <c r="N333" s="7">
+        <v>0</v>
+      </c>
+      <c r="O333" s="7">
+        <v>0</v>
+      </c>
+      <c r="P333" s="7">
+        <v>2.0832101668337701</v>
+      </c>
+      <c r="Q333" s="7">
+        <v>0</v>
+      </c>
+      <c r="R333" s="7">
+        <v>1.5092519674760301</v>
+      </c>
+      <c r="S333" s="7">
+        <v>0</v>
+      </c>
+      <c r="T333" t="b">
+        <v>1</v>
+      </c>
+      <c r="U333" s="2">
+        <v>19</v>
+      </c>
+      <c r="V333" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W333" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
     </row>
     <row r="334" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A334" s="10">
         <v>333</v>
       </c>
+      <c r="B334" s="7">
+        <v>0</v>
+      </c>
+      <c r="C334" s="7">
+        <v>0</v>
+      </c>
+      <c r="D334" s="7">
+        <v>0</v>
+      </c>
+      <c r="E334" s="7">
+        <v>0</v>
+      </c>
+      <c r="F334" s="7">
+        <v>11.6486896999442</v>
+      </c>
+      <c r="G334" s="7">
+        <v>0</v>
+      </c>
+      <c r="H334" s="7">
+        <v>0</v>
+      </c>
+      <c r="I334" s="7">
+        <v>0</v>
+      </c>
+      <c r="J334" s="7">
+        <v>0</v>
+      </c>
+      <c r="K334" s="7">
+        <v>8.9292710963321493</v>
+      </c>
+      <c r="L334" s="7">
+        <v>0</v>
+      </c>
+      <c r="M334" s="7">
+        <v>0</v>
+      </c>
+      <c r="N334" s="7">
+        <v>0</v>
+      </c>
+      <c r="O334" s="7">
+        <v>0</v>
+      </c>
+      <c r="P334" s="7">
+        <v>1.50526824423536</v>
+      </c>
+      <c r="Q334" s="7">
+        <v>0</v>
+      </c>
+      <c r="R334" s="7">
+        <v>4.8436849443217298</v>
+      </c>
+      <c r="S334" s="7">
+        <v>0</v>
+      </c>
+      <c r="T334" t="b">
+        <v>1</v>
+      </c>
+      <c r="U334" s="2">
+        <v>38</v>
+      </c>
+      <c r="V334" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W334" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
     </row>
     <row r="335" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A335" s="10">
         <v>334</v>
       </c>
+      <c r="B335" s="7">
+        <v>0</v>
+      </c>
+      <c r="C335" s="7">
+        <v>11.977110596305801</v>
+      </c>
+      <c r="D335" s="7">
+        <v>0</v>
+      </c>
+      <c r="E335" s="7">
+        <v>0</v>
+      </c>
+      <c r="F335" s="7">
+        <v>0</v>
+      </c>
+      <c r="G335" s="7">
+        <v>0</v>
+      </c>
+      <c r="H335" s="7">
+        <v>0</v>
+      </c>
+      <c r="I335" s="7">
+        <v>0</v>
+      </c>
+      <c r="J335" s="7">
+        <v>0</v>
+      </c>
+      <c r="K335" s="7">
+        <v>0</v>
+      </c>
+      <c r="L335" s="7">
+        <v>0</v>
+      </c>
+      <c r="M335" s="7">
+        <v>9.5412393327413092</v>
+      </c>
+      <c r="N335" s="7">
+        <v>0</v>
+      </c>
+      <c r="O335" s="7">
+        <v>0</v>
+      </c>
+      <c r="P335" s="7">
+        <v>3.2567509567805102</v>
+      </c>
+      <c r="Q335" s="7">
+        <v>0</v>
+      </c>
+      <c r="R335" s="7">
+        <v>4.1638825018197796</v>
+      </c>
+      <c r="S335" s="7">
+        <v>0</v>
+      </c>
+      <c r="T335" t="b">
+        <v>0</v>
+      </c>
+      <c r="U335" s="2" t="str">
+        <f t="shared" si="16"/>
+        <v>NA</v>
+      </c>
+      <c r="V335" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v>NA</v>
+      </c>
+      <c r="W335" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="336" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A336" s="10">
         <v>335</v>
       </c>
-    </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B336" s="7">
+        <v>4.6823987416364199</v>
+      </c>
+      <c r="C336" s="7">
+        <v>0</v>
+      </c>
+      <c r="D336" s="7">
+        <v>0</v>
+      </c>
+      <c r="E336" s="7">
+        <v>0</v>
+      </c>
+      <c r="F336" s="7">
+        <v>13.2133026529169</v>
+      </c>
+      <c r="G336" s="7">
+        <v>0</v>
+      </c>
+      <c r="H336" s="7">
+        <v>0</v>
+      </c>
+      <c r="I336" s="7">
+        <v>0</v>
+      </c>
+      <c r="J336" s="7">
+        <v>0</v>
+      </c>
+      <c r="K336" s="7">
+        <v>0</v>
+      </c>
+      <c r="L336" s="7">
+        <v>0</v>
+      </c>
+      <c r="M336" s="7">
+        <v>0</v>
+      </c>
+      <c r="N336" s="7">
+        <v>0</v>
+      </c>
+      <c r="O336" s="7">
+        <v>0</v>
+      </c>
+      <c r="P336" s="7">
+        <v>1.38389767580903</v>
+      </c>
+      <c r="Q336" s="7">
+        <v>0</v>
+      </c>
+      <c r="R336" s="7">
+        <v>2.9201510590465101</v>
+      </c>
+      <c r="S336" s="7">
+        <v>0</v>
+      </c>
+      <c r="T336" t="b">
+        <v>1</v>
+      </c>
+      <c r="U336" s="2">
+        <v>86</v>
+      </c>
+      <c r="V336" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W336" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+    </row>
+    <row r="337" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A337" s="10">
         <v>336</v>
+      </c>
+      <c r="B337" s="7">
+        <v>6.9806328179698101</v>
+      </c>
+      <c r="C337" s="7">
+        <v>0</v>
+      </c>
+      <c r="D337" s="7">
+        <v>0</v>
+      </c>
+      <c r="E337" s="7">
+        <v>0</v>
+      </c>
+      <c r="F337" s="7">
+        <v>0</v>
+      </c>
+      <c r="G337" s="7">
+        <v>0</v>
+      </c>
+      <c r="H337" s="7">
+        <v>0</v>
+      </c>
+      <c r="I337" s="7">
+        <v>0</v>
+      </c>
+      <c r="J337" s="7">
+        <v>0</v>
+      </c>
+      <c r="K337" s="7">
+        <v>0</v>
+      </c>
+      <c r="L337" s="7">
+        <v>9.6324195130896104</v>
+      </c>
+      <c r="M337" s="7">
+        <v>0</v>
+      </c>
+      <c r="N337" s="7">
+        <v>0</v>
+      </c>
+      <c r="O337" s="7">
+        <v>0</v>
+      </c>
+      <c r="P337" s="7">
+        <v>1.0367276462331101</v>
+      </c>
+      <c r="Q337" s="7">
+        <v>0</v>
+      </c>
+      <c r="R337" s="7">
+        <v>3.7911707063232098</v>
+      </c>
+      <c r="S337" s="7">
+        <v>0</v>
+      </c>
+      <c r="T337" t="b">
+        <v>1</v>
+      </c>
+      <c r="U337" s="2">
+        <v>941</v>
+      </c>
+      <c r="V337" s="2" t="str">
+        <f t="shared" si="17"/>
+        <v/>
+      </c>
+      <c r="W337" s="12" t="str">
+        <f t="shared" si="18"/>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated dataset till S336
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D10E34-6C4A-6942-8F66-0184DDD0C9E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3074798-2760-B243-A996-6AF756E9108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -359,7 +359,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -690,11 +700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W337"/>
+  <dimension ref="A1:W361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A309" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W337" sqref="W337"/>
+    <sheetView tabSelected="1" topLeftCell="A311" zoomScale="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T349" sqref="T349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23088,15 +23098,15 @@
         <v>0</v>
       </c>
       <c r="U307" s="2" t="str">
-        <f t="shared" ref="U307:U337" si="16">IF(T307=FALSE, "NA", "")</f>
+        <f t="shared" ref="U307:U335" si="16">IF(T307=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V307" s="2" t="str">
-        <f t="shared" ref="V307:V337" si="17">IF(T307=FALSE, "NA", "")</f>
+        <f t="shared" ref="V307:V335" si="17">IF(T307=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W307" s="12" t="str">
-        <f t="shared" ref="W307:W337" si="18">IF(T307=FALSE, "NA", "")</f>
+        <f t="shared" ref="W307:W335" si="18">IF(T307=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -24614,13 +24624,11 @@
       <c r="U328" s="2">
         <v>260</v>
       </c>
-      <c r="V328" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W328" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V328" s="2">
+        <v>4</v>
+      </c>
+      <c r="W328" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="329" spans="1:23" x14ac:dyDescent="0.2">
@@ -24687,13 +24695,11 @@
       <c r="U329" s="2">
         <v>17</v>
       </c>
-      <c r="V329" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W329" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V329" s="2">
+        <v>2</v>
+      </c>
+      <c r="W329" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="330" spans="1:23" x14ac:dyDescent="0.2">
@@ -24760,13 +24766,11 @@
       <c r="U330" s="2">
         <v>14</v>
       </c>
-      <c r="V330" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W330" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V330" s="2">
+        <v>4</v>
+      </c>
+      <c r="W330" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="331" spans="1:23" x14ac:dyDescent="0.2">
@@ -24833,13 +24837,11 @@
       <c r="U331" s="2">
         <v>17</v>
       </c>
-      <c r="V331" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W331" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V331" s="2">
+        <v>8</v>
+      </c>
+      <c r="W331" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="332" spans="1:23" x14ac:dyDescent="0.2">
@@ -24906,13 +24908,11 @@
       <c r="U332" s="2">
         <v>14</v>
       </c>
-      <c r="V332" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W332" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V332" s="2">
+        <v>2</v>
+      </c>
+      <c r="W332" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="333" spans="1:23" x14ac:dyDescent="0.2">
@@ -24979,13 +24979,11 @@
       <c r="U333" s="2">
         <v>19</v>
       </c>
-      <c r="V333" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W333" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V333" s="2">
+        <v>2</v>
+      </c>
+      <c r="W333" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="334" spans="1:23" x14ac:dyDescent="0.2">
@@ -25052,13 +25050,11 @@
       <c r="U334" s="2">
         <v>38</v>
       </c>
-      <c r="V334" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W334" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V334" s="2">
+        <v>19</v>
+      </c>
+      <c r="W334" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="335" spans="1:23" x14ac:dyDescent="0.2">
@@ -25123,7 +25119,7 @@
         <v>0</v>
       </c>
       <c r="U335" s="2" t="str">
-        <f t="shared" si="16"/>
+        <f>IF(T335=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V335" s="2" t="str">
@@ -25199,13 +25195,11 @@
       <c r="U336" s="2">
         <v>86</v>
       </c>
-      <c r="V336" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W336" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V336" s="2">
+        <v>134</v>
+      </c>
+      <c r="W336" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="337" spans="1:23" x14ac:dyDescent="0.2">
@@ -25272,17 +25266,1071 @@
       <c r="U337" s="2">
         <v>941</v>
       </c>
-      <c r="V337" s="2" t="str">
-        <f t="shared" si="17"/>
-        <v/>
-      </c>
-      <c r="W337" s="12" t="str">
-        <f t="shared" si="18"/>
-        <v/>
+      <c r="V337" s="2">
+        <v>12</v>
+      </c>
+      <c r="W337" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A338" s="10">
+        <v>337</v>
+      </c>
+      <c r="B338" s="7">
+        <v>0</v>
+      </c>
+      <c r="C338" s="7">
+        <v>0</v>
+      </c>
+      <c r="D338" s="7">
+        <v>0</v>
+      </c>
+      <c r="E338" s="7">
+        <v>0</v>
+      </c>
+      <c r="F338" s="7">
+        <v>8.3847048533018498</v>
+      </c>
+      <c r="G338" s="7">
+        <v>0</v>
+      </c>
+      <c r="H338" s="7">
+        <v>0</v>
+      </c>
+      <c r="I338" s="7">
+        <v>0</v>
+      </c>
+      <c r="J338" s="7">
+        <v>0</v>
+      </c>
+      <c r="K338" s="7">
+        <v>0</v>
+      </c>
+      <c r="L338" s="7">
+        <v>0</v>
+      </c>
+      <c r="M338" s="7">
+        <v>8.2783661700701803</v>
+      </c>
+      <c r="N338" s="7">
+        <v>0</v>
+      </c>
+      <c r="O338" s="7">
+        <v>0</v>
+      </c>
+      <c r="P338" s="7">
+        <v>2.9819975085475301</v>
+      </c>
+      <c r="Q338" s="7">
+        <v>0</v>
+      </c>
+      <c r="R338" s="7">
+        <v>2.2120452502429702</v>
+      </c>
+      <c r="S338" s="7">
+        <v>0</v>
+      </c>
+      <c r="U338" s="2" t="str">
+        <f>IF(T338=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V338" s="2" t="str">
+        <f>IF(T338=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W338" s="12" t="str">
+        <f>IF(T338=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="339" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A339" s="10">
+        <v>338</v>
+      </c>
+      <c r="B339" s="7">
+        <v>0</v>
+      </c>
+      <c r="C339" s="7">
+        <v>0</v>
+      </c>
+      <c r="D339" s="7">
+        <v>0</v>
+      </c>
+      <c r="E339" s="7">
+        <v>0</v>
+      </c>
+      <c r="F339" s="7">
+        <v>0</v>
+      </c>
+      <c r="G339" s="7">
+        <v>0</v>
+      </c>
+      <c r="H339" s="7">
+        <v>0</v>
+      </c>
+      <c r="I339" s="7">
+        <v>0</v>
+      </c>
+      <c r="J339" s="7">
+        <v>0</v>
+      </c>
+      <c r="K339" s="7">
+        <v>10.3902784059874</v>
+      </c>
+      <c r="L339" s="7">
+        <v>0</v>
+      </c>
+      <c r="M339" s="7">
+        <v>12.404942493478201</v>
+      </c>
+      <c r="N339" s="7">
+        <v>0</v>
+      </c>
+      <c r="O339" s="7">
+        <v>0</v>
+      </c>
+      <c r="P339" s="7">
+        <v>2.7052857861156401</v>
+      </c>
+      <c r="Q339" s="7">
+        <v>0</v>
+      </c>
+      <c r="R339" s="7">
+        <v>2.4762341291676302</v>
+      </c>
+      <c r="S339" s="7">
+        <v>0</v>
+      </c>
+      <c r="U339" s="2" t="str">
+        <f t="shared" ref="U339:U361" si="19">IF(T339=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V339" s="2" t="str">
+        <f t="shared" ref="V339:V361" si="20">IF(T339=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W339" s="12" t="str">
+        <f t="shared" ref="W339:W361" si="21">IF(T339=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="340" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A340" s="10">
+        <v>339</v>
+      </c>
+      <c r="B340" s="7">
+        <v>0</v>
+      </c>
+      <c r="C340" s="7">
+        <v>0</v>
+      </c>
+      <c r="D340" s="7">
+        <v>0</v>
+      </c>
+      <c r="E340" s="7">
+        <v>0</v>
+      </c>
+      <c r="F340" s="7">
+        <v>0</v>
+      </c>
+      <c r="G340" s="7">
+        <v>7.8557818579115803</v>
+      </c>
+      <c r="H340" s="7">
+        <v>0</v>
+      </c>
+      <c r="I340" s="7">
+        <v>6.9630566791938699</v>
+      </c>
+      <c r="J340" s="7">
+        <v>0</v>
+      </c>
+      <c r="K340" s="7">
+        <v>0</v>
+      </c>
+      <c r="L340" s="7">
+        <v>0</v>
+      </c>
+      <c r="M340" s="7">
+        <v>0</v>
+      </c>
+      <c r="N340" s="7">
+        <v>0</v>
+      </c>
+      <c r="O340" s="7">
+        <v>0</v>
+      </c>
+      <c r="P340" s="7">
+        <v>2.1619127650156802</v>
+      </c>
+      <c r="Q340" s="7">
+        <v>0</v>
+      </c>
+      <c r="R340" s="7">
+        <v>2.1419412845074302</v>
+      </c>
+      <c r="S340" s="7">
+        <v>0</v>
+      </c>
+      <c r="U340" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V340" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W340" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="341" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A341" s="10">
+        <v>340</v>
+      </c>
+      <c r="B341" s="7">
+        <v>0</v>
+      </c>
+      <c r="C341" s="7">
+        <v>0</v>
+      </c>
+      <c r="D341" s="7">
+        <v>0</v>
+      </c>
+      <c r="E341" s="7">
+        <v>0</v>
+      </c>
+      <c r="F341" s="7">
+        <v>0</v>
+      </c>
+      <c r="G341" s="7">
+        <v>0</v>
+      </c>
+      <c r="H341" s="7">
+        <v>0</v>
+      </c>
+      <c r="I341" s="7">
+        <v>0</v>
+      </c>
+      <c r="J341" s="7">
+        <v>11.162138574387701</v>
+      </c>
+      <c r="K341" s="7">
+        <v>12.656716678075901</v>
+      </c>
+      <c r="L341" s="7">
+        <v>0</v>
+      </c>
+      <c r="M341" s="7">
+        <v>0</v>
+      </c>
+      <c r="N341" s="7">
+        <v>0</v>
+      </c>
+      <c r="O341" s="7">
+        <v>0</v>
+      </c>
+      <c r="P341" s="7">
+        <v>3.1636875319848801</v>
+      </c>
+      <c r="Q341" s="7">
+        <v>0</v>
+      </c>
+      <c r="R341" s="7">
+        <v>2.5073514239506598</v>
+      </c>
+      <c r="S341" s="7">
+        <v>0</v>
+      </c>
+      <c r="U341" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V341" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W341" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="342" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A342" s="10">
+        <v>341</v>
+      </c>
+      <c r="B342" s="7">
+        <v>0</v>
+      </c>
+      <c r="C342" s="7">
+        <v>12.0016308541126</v>
+      </c>
+      <c r="D342" s="7">
+        <v>0</v>
+      </c>
+      <c r="E342" s="7">
+        <v>0</v>
+      </c>
+      <c r="F342" s="7">
+        <v>0</v>
+      </c>
+      <c r="G342" s="7">
+        <v>0</v>
+      </c>
+      <c r="H342" s="7">
+        <v>0</v>
+      </c>
+      <c r="I342" s="7">
+        <v>9.8453094713407605</v>
+      </c>
+      <c r="J342" s="7">
+        <v>0</v>
+      </c>
+      <c r="K342" s="7">
+        <v>0</v>
+      </c>
+      <c r="L342" s="7">
+        <v>0</v>
+      </c>
+      <c r="M342" s="7">
+        <v>0</v>
+      </c>
+      <c r="N342" s="7">
+        <v>0</v>
+      </c>
+      <c r="O342" s="7">
+        <v>0</v>
+      </c>
+      <c r="P342" s="7">
+        <v>3.3619144063294701</v>
+      </c>
+      <c r="Q342" s="7">
+        <v>0</v>
+      </c>
+      <c r="R342" s="7">
+        <v>4.7646484274500898</v>
+      </c>
+      <c r="S342" s="7">
+        <v>0</v>
+      </c>
+      <c r="U342" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V342" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W342" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="343" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A343" s="10">
+        <v>342</v>
+      </c>
+      <c r="B343" s="7">
+        <v>0</v>
+      </c>
+      <c r="C343" s="7">
+        <v>0</v>
+      </c>
+      <c r="D343" s="7">
+        <v>0</v>
+      </c>
+      <c r="E343" s="7">
+        <v>7.4445799876268097</v>
+      </c>
+      <c r="F343" s="7">
+        <v>0</v>
+      </c>
+      <c r="G343" s="7">
+        <v>0</v>
+      </c>
+      <c r="H343" s="7">
+        <v>8.7662626665894603</v>
+      </c>
+      <c r="I343" s="7">
+        <v>0</v>
+      </c>
+      <c r="J343" s="7">
+        <v>0</v>
+      </c>
+      <c r="K343" s="7">
+        <v>0</v>
+      </c>
+      <c r="L343" s="7">
+        <v>0</v>
+      </c>
+      <c r="M343" s="7">
+        <v>0</v>
+      </c>
+      <c r="N343" s="7">
+        <v>0</v>
+      </c>
+      <c r="O343" s="7">
+        <v>0</v>
+      </c>
+      <c r="P343" s="7">
+        <v>3.0706894440376198</v>
+      </c>
+      <c r="Q343" s="7">
+        <v>0</v>
+      </c>
+      <c r="R343" s="7">
+        <v>3.4765349378611199</v>
+      </c>
+      <c r="S343" s="7">
+        <v>0</v>
+      </c>
+      <c r="U343" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V343" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W343" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="344" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A344" s="10">
+        <v>343</v>
+      </c>
+      <c r="B344" s="7">
+        <v>0</v>
+      </c>
+      <c r="C344" s="7">
+        <v>10.301915466942599</v>
+      </c>
+      <c r="D344" s="7">
+        <v>12.0308594923969</v>
+      </c>
+      <c r="E344" s="7">
+        <v>0</v>
+      </c>
+      <c r="F344" s="7">
+        <v>0</v>
+      </c>
+      <c r="G344" s="7">
+        <v>0</v>
+      </c>
+      <c r="H344" s="7">
+        <v>0</v>
+      </c>
+      <c r="I344" s="7">
+        <v>0</v>
+      </c>
+      <c r="J344" s="7">
+        <v>0</v>
+      </c>
+      <c r="K344" s="7">
+        <v>0</v>
+      </c>
+      <c r="L344" s="7">
+        <v>0</v>
+      </c>
+      <c r="M344" s="7">
+        <v>0</v>
+      </c>
+      <c r="N344" s="7">
+        <v>0</v>
+      </c>
+      <c r="O344" s="7">
+        <v>0</v>
+      </c>
+      <c r="P344" s="7">
+        <v>2.4688523475865698</v>
+      </c>
+      <c r="Q344" s="7">
+        <v>0</v>
+      </c>
+      <c r="R344" s="7">
+        <v>4.7633155283406801</v>
+      </c>
+      <c r="S344" s="7">
+        <v>0</v>
+      </c>
+      <c r="U344" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V344" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W344" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="345" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A345" s="10">
+        <v>344</v>
+      </c>
+      <c r="B345" s="7">
+        <v>0</v>
+      </c>
+      <c r="C345" s="7">
+        <v>0</v>
+      </c>
+      <c r="D345" s="7">
+        <v>9.1188352406104602</v>
+      </c>
+      <c r="E345" s="7">
+        <v>0</v>
+      </c>
+      <c r="F345" s="7">
+        <v>0</v>
+      </c>
+      <c r="G345" s="7">
+        <v>0</v>
+      </c>
+      <c r="H345" s="7">
+        <v>0</v>
+      </c>
+      <c r="I345" s="7">
+        <v>0</v>
+      </c>
+      <c r="J345" s="7">
+        <v>0</v>
+      </c>
+      <c r="K345" s="7">
+        <v>0</v>
+      </c>
+      <c r="L345" s="7">
+        <v>10.3971859414084</v>
+      </c>
+      <c r="M345" s="7">
+        <v>0</v>
+      </c>
+      <c r="N345" s="7">
+        <v>0</v>
+      </c>
+      <c r="O345" s="7">
+        <v>0</v>
+      </c>
+      <c r="P345" s="7">
+        <v>1.55559238629845</v>
+      </c>
+      <c r="Q345" s="7">
+        <v>0</v>
+      </c>
+      <c r="R345" s="7">
+        <v>4.1947439207790698</v>
+      </c>
+      <c r="S345" s="7">
+        <v>0</v>
+      </c>
+      <c r="U345" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V345" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W345" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="346" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A346" s="10">
+        <v>345</v>
+      </c>
+      <c r="B346" s="7">
+        <v>3.9621170145865401</v>
+      </c>
+      <c r="C346" s="7">
+        <v>0</v>
+      </c>
+      <c r="D346" s="7">
+        <v>0</v>
+      </c>
+      <c r="E346" s="7">
+        <v>0</v>
+      </c>
+      <c r="F346" s="7">
+        <v>0</v>
+      </c>
+      <c r="G346" s="7">
+        <v>0</v>
+      </c>
+      <c r="H346" s="7">
+        <v>11.950090341866501</v>
+      </c>
+      <c r="I346" s="7">
+        <v>0</v>
+      </c>
+      <c r="J346" s="7">
+        <v>0</v>
+      </c>
+      <c r="K346" s="7">
+        <v>0</v>
+      </c>
+      <c r="L346" s="7">
+        <v>0</v>
+      </c>
+      <c r="M346" s="7">
+        <v>0</v>
+      </c>
+      <c r="N346" s="7">
+        <v>0</v>
+      </c>
+      <c r="O346" s="7">
+        <v>0</v>
+      </c>
+      <c r="P346" s="7">
+        <v>2.1383506461701698</v>
+      </c>
+      <c r="Q346" s="7">
+        <v>0</v>
+      </c>
+      <c r="R346" s="7">
+        <v>4.9243748053630698</v>
+      </c>
+      <c r="S346" s="7">
+        <v>0</v>
+      </c>
+      <c r="U346" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V346" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W346" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="347" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A347" s="10">
+        <v>346</v>
+      </c>
+      <c r="B347" s="7">
+        <v>0</v>
+      </c>
+      <c r="C347" s="7">
+        <v>0</v>
+      </c>
+      <c r="D347" s="7">
+        <v>0</v>
+      </c>
+      <c r="E347" s="7">
+        <v>0</v>
+      </c>
+      <c r="F347" s="7">
+        <v>0</v>
+      </c>
+      <c r="G347" s="7">
+        <v>9.1876191161456298</v>
+      </c>
+      <c r="H347" s="7">
+        <v>0</v>
+      </c>
+      <c r="I347" s="7">
+        <v>0</v>
+      </c>
+      <c r="J347" s="7">
+        <v>0</v>
+      </c>
+      <c r="K347" s="7">
+        <v>0</v>
+      </c>
+      <c r="L347" s="7">
+        <v>0</v>
+      </c>
+      <c r="M347" s="7">
+        <v>11.501048389995301</v>
+      </c>
+      <c r="N347" s="7">
+        <v>0</v>
+      </c>
+      <c r="O347" s="7">
+        <v>0</v>
+      </c>
+      <c r="P347" s="7">
+        <v>3.2172690659056</v>
+      </c>
+      <c r="Q347" s="7">
+        <v>0</v>
+      </c>
+      <c r="R347" s="7">
+        <v>5.1676601961316297</v>
+      </c>
+      <c r="S347" s="7">
+        <v>0</v>
+      </c>
+      <c r="U347" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V347" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W347" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="348" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A348" s="10">
+        <v>347</v>
+      </c>
+      <c r="B348" s="7">
+        <v>0</v>
+      </c>
+      <c r="C348" s="7">
+        <v>0</v>
+      </c>
+      <c r="D348" s="7">
+        <v>0</v>
+      </c>
+      <c r="E348" s="7">
+        <v>0</v>
+      </c>
+      <c r="F348" s="7">
+        <v>7.9386427287180998</v>
+      </c>
+      <c r="G348" s="7">
+        <v>9.2947203740050206</v>
+      </c>
+      <c r="H348" s="7">
+        <v>0</v>
+      </c>
+      <c r="I348" s="7">
+        <v>0</v>
+      </c>
+      <c r="J348" s="7">
+        <v>0</v>
+      </c>
+      <c r="K348" s="7">
+        <v>0</v>
+      </c>
+      <c r="L348" s="7">
+        <v>0</v>
+      </c>
+      <c r="M348" s="7">
+        <v>0</v>
+      </c>
+      <c r="N348" s="7">
+        <v>0</v>
+      </c>
+      <c r="O348" s="7">
+        <v>0</v>
+      </c>
+      <c r="P348" s="7">
+        <v>3.5843080722890899</v>
+      </c>
+      <c r="Q348" s="7">
+        <v>0</v>
+      </c>
+      <c r="R348" s="7">
+        <v>4.2729798888689796</v>
+      </c>
+      <c r="S348" s="7">
+        <v>0</v>
+      </c>
+      <c r="U348" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V348" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W348" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="349" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A349" s="10">
+        <v>348</v>
+      </c>
+      <c r="B349" s="7">
+        <v>0</v>
+      </c>
+      <c r="C349" s="7">
+        <v>0</v>
+      </c>
+      <c r="D349" s="7">
+        <v>0</v>
+      </c>
+      <c r="E349" s="7">
+        <v>10.412293228514001</v>
+      </c>
+      <c r="F349" s="7">
+        <v>10.6592948187979</v>
+      </c>
+      <c r="G349" s="7">
+        <v>0</v>
+      </c>
+      <c r="H349" s="7">
+        <v>0</v>
+      </c>
+      <c r="I349" s="7">
+        <v>0</v>
+      </c>
+      <c r="J349" s="7">
+        <v>0</v>
+      </c>
+      <c r="K349" s="7">
+        <v>0</v>
+      </c>
+      <c r="L349" s="7">
+        <v>0</v>
+      </c>
+      <c r="M349" s="7">
+        <v>0</v>
+      </c>
+      <c r="N349" s="7">
+        <v>0</v>
+      </c>
+      <c r="O349" s="7">
+        <v>0</v>
+      </c>
+      <c r="P349" s="7">
+        <v>3.02013353199278</v>
+      </c>
+      <c r="Q349" s="7">
+        <v>0</v>
+      </c>
+      <c r="R349" s="7">
+        <v>3.4599825940557301</v>
+      </c>
+      <c r="S349" s="7">
+        <v>0</v>
+      </c>
+      <c r="U349" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V349" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W349" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="350" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A350" s="10">
+        <v>349</v>
+      </c>
+      <c r="U350" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V350" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W350" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="351" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A351" s="10">
+        <v>350</v>
+      </c>
+      <c r="U351" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V351" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W351" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="352" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A352" s="10">
+        <v>351</v>
+      </c>
+      <c r="U352" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V352" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W352" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="353" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A353" s="10">
+        <v>352</v>
+      </c>
+      <c r="U353" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V353" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W353" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="354" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A354" s="10">
+        <v>353</v>
+      </c>
+      <c r="U354" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V354" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W354" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="355" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A355" s="10">
+        <v>354</v>
+      </c>
+      <c r="U355" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V355" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W355" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="356" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A356" s="10">
+        <v>355</v>
+      </c>
+      <c r="U356" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V356" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W356" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="357" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A357" s="10">
+        <v>356</v>
+      </c>
+      <c r="U357" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V357" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W357" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="358" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A358" s="10">
+        <v>357</v>
+      </c>
+      <c r="U358" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V358" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W358" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="359" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A359" s="10">
+        <v>358</v>
+      </c>
+      <c r="U359" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V359" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W359" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="360" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A360" s="10">
+        <v>359</v>
+      </c>
+      <c r="U360" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V360" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W360" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="361" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A361" s="10">
+        <v>360</v>
+      </c>
+      <c r="U361" s="2" t="str">
+        <f t="shared" si="19"/>
+        <v>NA</v>
+      </c>
+      <c r="V361" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>NA</v>
+      </c>
+      <c r="W361" s="12" t="str">
+        <f t="shared" si="21"/>
+        <v>NA</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W337">
+  <conditionalFormatting sqref="A1:W361">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
@@ -35437,7 +36485,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated dataset till S360 (Simon send updated S349-354)
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3074798-2760-B243-A996-6AF756E9108C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2762A7D0-4DF8-DD40-9ED5-7C4196A12A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -359,17 +359,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -702,9 +692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
   <dimension ref="A1:W361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A311" zoomScale="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A320" zoomScale="75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T349" sqref="T349"/>
+      <selection pane="topRight" activeCell="W361" sqref="W361"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23098,7 +23088,7 @@
         <v>0</v>
       </c>
       <c r="U307" s="2" t="str">
-        <f t="shared" ref="U307:U335" si="16">IF(T307=FALSE, "NA", "")</f>
+        <f t="shared" ref="U307:U327" si="16">IF(T307=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V307" s="2" t="str">
@@ -26129,6 +26119,60 @@
       <c r="A350" s="10">
         <v>349</v>
       </c>
+      <c r="B350" s="7">
+        <v>0</v>
+      </c>
+      <c r="C350" s="7">
+        <v>0</v>
+      </c>
+      <c r="D350" s="7">
+        <v>0</v>
+      </c>
+      <c r="E350" s="7">
+        <v>0</v>
+      </c>
+      <c r="F350" s="7">
+        <v>0</v>
+      </c>
+      <c r="G350" s="7">
+        <v>0</v>
+      </c>
+      <c r="H350" s="7">
+        <v>0</v>
+      </c>
+      <c r="I350" s="7">
+        <v>17.0512978210106</v>
+      </c>
+      <c r="J350" s="7">
+        <v>14.5292461779029</v>
+      </c>
+      <c r="K350" s="7">
+        <v>0</v>
+      </c>
+      <c r="L350" s="7">
+        <v>0</v>
+      </c>
+      <c r="M350" s="7">
+        <v>0</v>
+      </c>
+      <c r="N350" s="7">
+        <v>0</v>
+      </c>
+      <c r="O350" s="7">
+        <v>0</v>
+      </c>
+      <c r="P350" s="7">
+        <v>1.6182755019939501</v>
+      </c>
+      <c r="Q350" s="7">
+        <v>0</v>
+      </c>
+      <c r="R350" s="7">
+        <v>3.2201634039678502</v>
+      </c>
+      <c r="S350" s="7">
+        <v>0</v>
+      </c>
       <c r="U350" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26146,6 +26190,60 @@
       <c r="A351" s="10">
         <v>350</v>
       </c>
+      <c r="B351" s="7">
+        <v>0</v>
+      </c>
+      <c r="C351" s="7">
+        <v>0</v>
+      </c>
+      <c r="D351" s="7">
+        <v>0</v>
+      </c>
+      <c r="E351" s="7">
+        <v>0</v>
+      </c>
+      <c r="F351" s="7">
+        <v>0</v>
+      </c>
+      <c r="G351" s="7">
+        <v>18.481327138584799</v>
+      </c>
+      <c r="H351" s="7">
+        <v>0</v>
+      </c>
+      <c r="I351" s="7">
+        <v>0</v>
+      </c>
+      <c r="J351" s="7">
+        <v>0</v>
+      </c>
+      <c r="K351" s="7">
+        <v>0</v>
+      </c>
+      <c r="L351" s="7">
+        <v>17.662032972421301</v>
+      </c>
+      <c r="M351" s="7">
+        <v>0</v>
+      </c>
+      <c r="N351" s="7">
+        <v>0</v>
+      </c>
+      <c r="O351" s="7">
+        <v>0</v>
+      </c>
+      <c r="P351" s="7">
+        <v>3.8985001215208701</v>
+      </c>
+      <c r="Q351" s="7">
+        <v>0</v>
+      </c>
+      <c r="R351" s="7">
+        <v>5.64216521493546</v>
+      </c>
+      <c r="S351" s="7">
+        <v>0</v>
+      </c>
       <c r="U351" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26163,6 +26261,60 @@
       <c r="A352" s="10">
         <v>351</v>
       </c>
+      <c r="B352" s="7">
+        <v>0</v>
+      </c>
+      <c r="C352" s="7">
+        <v>0</v>
+      </c>
+      <c r="D352" s="7">
+        <v>0</v>
+      </c>
+      <c r="E352" s="7">
+        <v>0</v>
+      </c>
+      <c r="F352" s="7">
+        <v>0</v>
+      </c>
+      <c r="G352" s="7">
+        <v>0</v>
+      </c>
+      <c r="H352" s="7">
+        <v>0</v>
+      </c>
+      <c r="I352" s="7">
+        <v>0</v>
+      </c>
+      <c r="J352" s="7">
+        <v>17.072970683774901</v>
+      </c>
+      <c r="K352" s="7">
+        <v>0</v>
+      </c>
+      <c r="L352" s="7">
+        <v>16.139392511553702</v>
+      </c>
+      <c r="M352" s="7">
+        <v>0</v>
+      </c>
+      <c r="N352" s="7">
+        <v>0</v>
+      </c>
+      <c r="O352" s="7">
+        <v>0</v>
+      </c>
+      <c r="P352" s="7">
+        <v>2.8594828006181898</v>
+      </c>
+      <c r="Q352" s="7">
+        <v>0</v>
+      </c>
+      <c r="R352" s="7">
+        <v>2.20605800970135</v>
+      </c>
+      <c r="S352" s="7">
+        <v>0</v>
+      </c>
       <c r="U352" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26180,6 +26332,60 @@
       <c r="A353" s="10">
         <v>352</v>
       </c>
+      <c r="B353" s="7">
+        <v>0</v>
+      </c>
+      <c r="C353" s="7">
+        <v>0</v>
+      </c>
+      <c r="D353" s="7">
+        <v>15.513852594017299</v>
+      </c>
+      <c r="E353" s="7">
+        <v>0</v>
+      </c>
+      <c r="F353" s="7">
+        <v>0</v>
+      </c>
+      <c r="G353" s="7">
+        <v>16.5527763704394</v>
+      </c>
+      <c r="H353" s="7">
+        <v>0</v>
+      </c>
+      <c r="I353" s="7">
+        <v>0</v>
+      </c>
+      <c r="J353" s="7">
+        <v>0</v>
+      </c>
+      <c r="K353" s="7">
+        <v>0</v>
+      </c>
+      <c r="L353" s="7">
+        <v>0</v>
+      </c>
+      <c r="M353" s="7">
+        <v>0</v>
+      </c>
+      <c r="N353" s="7">
+        <v>0</v>
+      </c>
+      <c r="O353" s="7">
+        <v>0</v>
+      </c>
+      <c r="P353" s="7">
+        <v>2.6629382401022599</v>
+      </c>
+      <c r="Q353" s="7">
+        <v>0</v>
+      </c>
+      <c r="R353" s="7">
+        <v>4.9480136978148996</v>
+      </c>
+      <c r="S353" s="7">
+        <v>0</v>
+      </c>
       <c r="U353" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26197,6 +26403,60 @@
       <c r="A354" s="10">
         <v>353</v>
       </c>
+      <c r="B354" s="7">
+        <v>0</v>
+      </c>
+      <c r="C354" s="7">
+        <v>0</v>
+      </c>
+      <c r="D354" s="7">
+        <v>0</v>
+      </c>
+      <c r="E354" s="7">
+        <v>0</v>
+      </c>
+      <c r="F354" s="7">
+        <v>0</v>
+      </c>
+      <c r="G354" s="7">
+        <v>14.743020648004601</v>
+      </c>
+      <c r="H354" s="7">
+        <v>14.5778107047774</v>
+      </c>
+      <c r="I354" s="7">
+        <v>0</v>
+      </c>
+      <c r="J354" s="7">
+        <v>0</v>
+      </c>
+      <c r="K354" s="7">
+        <v>0</v>
+      </c>
+      <c r="L354" s="7">
+        <v>0</v>
+      </c>
+      <c r="M354" s="7">
+        <v>0</v>
+      </c>
+      <c r="N354" s="7">
+        <v>0</v>
+      </c>
+      <c r="O354" s="7">
+        <v>0</v>
+      </c>
+      <c r="P354" s="7">
+        <v>5.9927940120690701</v>
+      </c>
+      <c r="Q354" s="7">
+        <v>0</v>
+      </c>
+      <c r="R354" s="7">
+        <v>3.7683601336148498</v>
+      </c>
+      <c r="S354" s="7">
+        <v>0</v>
+      </c>
       <c r="U354" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26214,6 +26474,60 @@
       <c r="A355" s="10">
         <v>354</v>
       </c>
+      <c r="B355" s="7">
+        <v>7.7860153034526602</v>
+      </c>
+      <c r="C355" s="7">
+        <v>0</v>
+      </c>
+      <c r="D355" s="7">
+        <v>0</v>
+      </c>
+      <c r="E355" s="7">
+        <v>14.0969695707408</v>
+      </c>
+      <c r="F355" s="7">
+        <v>0</v>
+      </c>
+      <c r="G355" s="7">
+        <v>0</v>
+      </c>
+      <c r="H355" s="7">
+        <v>0</v>
+      </c>
+      <c r="I355" s="7">
+        <v>0</v>
+      </c>
+      <c r="J355" s="7">
+        <v>0</v>
+      </c>
+      <c r="K355" s="7">
+        <v>0</v>
+      </c>
+      <c r="L355" s="7">
+        <v>0</v>
+      </c>
+      <c r="M355" s="7">
+        <v>0</v>
+      </c>
+      <c r="N355" s="7">
+        <v>0</v>
+      </c>
+      <c r="O355" s="7">
+        <v>0</v>
+      </c>
+      <c r="P355" s="7">
+        <v>4.7646743481566496</v>
+      </c>
+      <c r="Q355" s="7">
+        <v>0</v>
+      </c>
+      <c r="R355" s="7">
+        <v>5.6975106373188398</v>
+      </c>
+      <c r="S355" s="7">
+        <v>0</v>
+      </c>
       <c r="U355" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26231,6 +26545,60 @@
       <c r="A356" s="10">
         <v>355</v>
       </c>
+      <c r="B356" s="7">
+        <v>0</v>
+      </c>
+      <c r="C356" s="7">
+        <v>0</v>
+      </c>
+      <c r="D356" s="7">
+        <v>0</v>
+      </c>
+      <c r="E356" s="7">
+        <v>6.8847541424966998</v>
+      </c>
+      <c r="F356" s="7">
+        <v>0</v>
+      </c>
+      <c r="G356" s="7">
+        <v>0</v>
+      </c>
+      <c r="H356" s="7">
+        <v>0</v>
+      </c>
+      <c r="I356" s="7">
+        <v>0</v>
+      </c>
+      <c r="J356" s="7">
+        <v>8.4649778179028292</v>
+      </c>
+      <c r="K356" s="7">
+        <v>0</v>
+      </c>
+      <c r="L356" s="7">
+        <v>0</v>
+      </c>
+      <c r="M356" s="7">
+        <v>0</v>
+      </c>
+      <c r="N356" s="7">
+        <v>0</v>
+      </c>
+      <c r="O356" s="7">
+        <v>0</v>
+      </c>
+      <c r="P356" s="7">
+        <v>1.49569537502413</v>
+      </c>
+      <c r="Q356" s="7">
+        <v>0</v>
+      </c>
+      <c r="R356" s="7">
+        <v>3.9783978503180002</v>
+      </c>
+      <c r="S356" s="7">
+        <v>0</v>
+      </c>
       <c r="U356" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26248,6 +26616,60 @@
       <c r="A357" s="10">
         <v>356</v>
       </c>
+      <c r="B357" s="7">
+        <v>0</v>
+      </c>
+      <c r="C357" s="7">
+        <v>0</v>
+      </c>
+      <c r="D357" s="7">
+        <v>0</v>
+      </c>
+      <c r="E357" s="7">
+        <v>0</v>
+      </c>
+      <c r="F357" s="7">
+        <v>8.7947096176898398</v>
+      </c>
+      <c r="G357" s="7">
+        <v>0</v>
+      </c>
+      <c r="H357" s="7">
+        <v>0</v>
+      </c>
+      <c r="I357" s="7">
+        <v>0</v>
+      </c>
+      <c r="J357" s="7">
+        <v>0</v>
+      </c>
+      <c r="K357" s="7">
+        <v>0</v>
+      </c>
+      <c r="L357" s="7">
+        <v>7.9615266012769901</v>
+      </c>
+      <c r="M357" s="7">
+        <v>0</v>
+      </c>
+      <c r="N357" s="7">
+        <v>0</v>
+      </c>
+      <c r="O357" s="7">
+        <v>0</v>
+      </c>
+      <c r="P357" s="7">
+        <v>1.90057297373125</v>
+      </c>
+      <c r="Q357" s="7">
+        <v>0</v>
+      </c>
+      <c r="R357" s="7">
+        <v>1.48423303044529</v>
+      </c>
+      <c r="S357" s="7">
+        <v>0</v>
+      </c>
       <c r="U357" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26265,6 +26687,60 @@
       <c r="A358" s="10">
         <v>357</v>
       </c>
+      <c r="B358" s="7">
+        <v>0</v>
+      </c>
+      <c r="C358" s="7">
+        <v>0</v>
+      </c>
+      <c r="D358" s="7">
+        <v>0</v>
+      </c>
+      <c r="E358" s="7">
+        <v>0</v>
+      </c>
+      <c r="F358" s="7">
+        <v>0</v>
+      </c>
+      <c r="G358" s="7">
+        <v>0</v>
+      </c>
+      <c r="H358" s="7">
+        <v>8.9083150838504501</v>
+      </c>
+      <c r="I358" s="7">
+        <v>0</v>
+      </c>
+      <c r="J358" s="7">
+        <v>12.352916525900801</v>
+      </c>
+      <c r="K358" s="7">
+        <v>0</v>
+      </c>
+      <c r="L358" s="7">
+        <v>0</v>
+      </c>
+      <c r="M358" s="7">
+        <v>0</v>
+      </c>
+      <c r="N358" s="7">
+        <v>0</v>
+      </c>
+      <c r="O358" s="7">
+        <v>0</v>
+      </c>
+      <c r="P358" s="7">
+        <v>1.23588726090864</v>
+      </c>
+      <c r="Q358" s="7">
+        <v>0</v>
+      </c>
+      <c r="R358" s="7">
+        <v>2.72490805718405</v>
+      </c>
+      <c r="S358" s="7">
+        <v>0</v>
+      </c>
       <c r="U358" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26282,6 +26758,60 @@
       <c r="A359" s="10">
         <v>358</v>
       </c>
+      <c r="B359" s="7">
+        <v>0</v>
+      </c>
+      <c r="C359" s="7">
+        <v>8.8330896029060408</v>
+      </c>
+      <c r="D359" s="7">
+        <v>0</v>
+      </c>
+      <c r="E359" s="7">
+        <v>0</v>
+      </c>
+      <c r="F359" s="7">
+        <v>0</v>
+      </c>
+      <c r="G359" s="7">
+        <v>0</v>
+      </c>
+      <c r="H359" s="7">
+        <v>12.8856765808719</v>
+      </c>
+      <c r="I359" s="7">
+        <v>0</v>
+      </c>
+      <c r="J359" s="7">
+        <v>0</v>
+      </c>
+      <c r="K359" s="7">
+        <v>0</v>
+      </c>
+      <c r="L359" s="7">
+        <v>0</v>
+      </c>
+      <c r="M359" s="7">
+        <v>0</v>
+      </c>
+      <c r="N359" s="7">
+        <v>0</v>
+      </c>
+      <c r="O359" s="7">
+        <v>0</v>
+      </c>
+      <c r="P359" s="7">
+        <v>1.2839078207243799</v>
+      </c>
+      <c r="Q359" s="7">
+        <v>0</v>
+      </c>
+      <c r="R359" s="7">
+        <v>2.8547635211524902</v>
+      </c>
+      <c r="S359" s="7">
+        <v>0</v>
+      </c>
       <c r="U359" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26299,6 +26829,60 @@
       <c r="A360" s="10">
         <v>359</v>
       </c>
+      <c r="B360" s="7">
+        <v>4.35585876633548</v>
+      </c>
+      <c r="C360" s="7">
+        <v>0</v>
+      </c>
+      <c r="D360" s="7">
+        <v>7.8787923441815604</v>
+      </c>
+      <c r="E360" s="7">
+        <v>0</v>
+      </c>
+      <c r="F360" s="7">
+        <v>0</v>
+      </c>
+      <c r="G360" s="7">
+        <v>0</v>
+      </c>
+      <c r="H360" s="7">
+        <v>0</v>
+      </c>
+      <c r="I360" s="7">
+        <v>0</v>
+      </c>
+      <c r="J360" s="7">
+        <v>0</v>
+      </c>
+      <c r="K360" s="7">
+        <v>0</v>
+      </c>
+      <c r="L360" s="7">
+        <v>0</v>
+      </c>
+      <c r="M360" s="7">
+        <v>0</v>
+      </c>
+      <c r="N360" s="7">
+        <v>0</v>
+      </c>
+      <c r="O360" s="7">
+        <v>0</v>
+      </c>
+      <c r="P360" s="7">
+        <v>1.3465978015439</v>
+      </c>
+      <c r="Q360" s="7">
+        <v>0</v>
+      </c>
+      <c r="R360" s="7">
+        <v>3.9680810956739299</v>
+      </c>
+      <c r="S360" s="7">
+        <v>0</v>
+      </c>
       <c r="U360" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26315,6 +26899,60 @@
     <row r="361" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A361" s="10">
         <v>360</v>
+      </c>
+      <c r="B361" s="7">
+        <v>0</v>
+      </c>
+      <c r="C361" s="7">
+        <v>11.059690560140099</v>
+      </c>
+      <c r="D361" s="7">
+        <v>0</v>
+      </c>
+      <c r="E361" s="7">
+        <v>8.3288067144775706</v>
+      </c>
+      <c r="F361" s="7">
+        <v>0</v>
+      </c>
+      <c r="G361" s="7">
+        <v>0</v>
+      </c>
+      <c r="H361" s="7">
+        <v>0</v>
+      </c>
+      <c r="I361" s="7">
+        <v>0</v>
+      </c>
+      <c r="J361" s="7">
+        <v>0</v>
+      </c>
+      <c r="K361" s="7">
+        <v>0</v>
+      </c>
+      <c r="L361" s="7">
+        <v>0</v>
+      </c>
+      <c r="M361" s="7">
+        <v>0</v>
+      </c>
+      <c r="N361" s="7">
+        <v>0</v>
+      </c>
+      <c r="O361" s="7">
+        <v>0</v>
+      </c>
+      <c r="P361" s="7">
+        <v>2.4520088660528598</v>
+      </c>
+      <c r="Q361" s="7">
+        <v>0</v>
+      </c>
+      <c r="R361" s="7">
+        <v>3.8950106132044602</v>
+      </c>
+      <c r="S361" s="7">
+        <v>0</v>
       </c>
       <c r="U361" s="2" t="str">
         <f t="shared" si="19"/>
@@ -36485,7 +37123,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Formulations dataset updated to S360
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2762A7D0-4DF8-DD40-9ED5-7C4196A12A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C782001-A234-1349-8CAF-D2E4B56ED1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="-38420" yWindow="-4840" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -692,9 +692,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
   <dimension ref="A1:W361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A320" zoomScale="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W361" sqref="W361"/>
+    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U355" sqref="U355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25321,17 +25321,18 @@
       <c r="S338" s="7">
         <v>0</v>
       </c>
+      <c r="T338" t="b">
+        <v>1</v>
+      </c>
       <c r="U338" s="2" t="str">
         <f>IF(T338=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-      <c r="V338" s="2" t="str">
-        <f>IF(T338=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-      <c r="W338" s="12" t="str">
-        <f>IF(T338=FALSE, "NA", "")</f>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V338" s="2">
+        <v>133</v>
+      </c>
+      <c r="W338" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="339" spans="1:23" x14ac:dyDescent="0.2">
@@ -25392,17 +25393,18 @@
       <c r="S339" s="7">
         <v>0</v>
       </c>
+      <c r="T339" t="b">
+        <v>1</v>
+      </c>
       <c r="U339" s="2" t="str">
         <f t="shared" ref="U339:U361" si="19">IF(T339=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-      <c r="V339" s="2" t="str">
-        <f t="shared" ref="V339:V361" si="20">IF(T339=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-      <c r="W339" s="12" t="str">
-        <f t="shared" ref="W339:W361" si="21">IF(T339=FALSE, "NA", "")</f>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V339" s="2">
+        <v>104</v>
+      </c>
+      <c r="W339" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="340" spans="1:23" x14ac:dyDescent="0.2">
@@ -25463,17 +25465,18 @@
       <c r="S340" s="7">
         <v>0</v>
       </c>
+      <c r="T340" t="b">
+        <v>1</v>
+      </c>
       <c r="U340" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V340" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W340" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V340" s="2">
+        <v>26</v>
+      </c>
+      <c r="W340" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="341" spans="1:23" x14ac:dyDescent="0.2">
@@ -25534,17 +25537,18 @@
       <c r="S341" s="7">
         <v>0</v>
       </c>
+      <c r="T341" t="b">
+        <v>1</v>
+      </c>
       <c r="U341" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V341" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W341" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V341" s="2">
+        <v>4</v>
+      </c>
+      <c r="W341" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="342" spans="1:23" x14ac:dyDescent="0.2">
@@ -25605,17 +25609,18 @@
       <c r="S342" s="7">
         <v>0</v>
       </c>
+      <c r="T342" t="b">
+        <v>1</v>
+      </c>
       <c r="U342" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V342" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W342" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V342" s="2">
+        <v>17</v>
+      </c>
+      <c r="W342" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="343" spans="1:23" x14ac:dyDescent="0.2">
@@ -25676,16 +25681,19 @@
       <c r="S343" s="7">
         <v>0</v>
       </c>
+      <c r="T343" t="b">
+        <v>0</v>
+      </c>
       <c r="U343" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
       </c>
       <c r="V343" s="2" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="V343:V360" si="20">IF(T343=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W343" s="12" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="W343:W360" si="21">IF(T343=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -25747,17 +25755,18 @@
       <c r="S344" s="7">
         <v>0</v>
       </c>
+      <c r="T344" t="b">
+        <v>1</v>
+      </c>
       <c r="U344" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V344" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W344" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V344" s="2">
+        <v>6</v>
+      </c>
+      <c r="W344" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="345" spans="1:23" x14ac:dyDescent="0.2">
@@ -25818,6 +25827,9 @@
       <c r="S345" s="7">
         <v>0</v>
       </c>
+      <c r="T345" t="b">
+        <v>0</v>
+      </c>
       <c r="U345" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -25889,6 +25901,9 @@
       <c r="S346" s="7">
         <v>0</v>
       </c>
+      <c r="T346" t="b">
+        <v>0</v>
+      </c>
       <c r="U346" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -25960,6 +25975,9 @@
       <c r="S347" s="7">
         <v>0</v>
       </c>
+      <c r="T347" t="b">
+        <v>0</v>
+      </c>
       <c r="U347" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26031,6 +26049,9 @@
       <c r="S348" s="7">
         <v>0</v>
       </c>
+      <c r="T348" t="b">
+        <v>0</v>
+      </c>
       <c r="U348" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26102,6 +26123,9 @@
       <c r="S349" s="7">
         <v>0</v>
       </c>
+      <c r="T349" t="b">
+        <v>0</v>
+      </c>
       <c r="U349" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26173,17 +26197,18 @@
       <c r="S350" s="7">
         <v>0</v>
       </c>
+      <c r="T350" t="b">
+        <v>1</v>
+      </c>
       <c r="U350" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V350" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W350" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V350" s="2">
+        <v>108</v>
+      </c>
+      <c r="W350" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="351" spans="1:23" x14ac:dyDescent="0.2">
@@ -26244,6 +26269,9 @@
       <c r="S351" s="7">
         <v>0</v>
       </c>
+      <c r="T351" t="b">
+        <v>0</v>
+      </c>
       <c r="U351" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26315,17 +26343,18 @@
       <c r="S352" s="7">
         <v>0</v>
       </c>
+      <c r="T352" t="b">
+        <v>1</v>
+      </c>
       <c r="U352" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V352" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W352" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V352" s="2">
+        <v>281</v>
+      </c>
+      <c r="W352" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="353" spans="1:23" x14ac:dyDescent="0.2">
@@ -26386,17 +26415,18 @@
       <c r="S353" s="7">
         <v>0</v>
       </c>
+      <c r="T353" t="b">
+        <v>1</v>
+      </c>
       <c r="U353" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V353" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W353" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V353" s="2">
+        <v>7</v>
+      </c>
+      <c r="W353" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="354" spans="1:23" x14ac:dyDescent="0.2">
@@ -26457,6 +26487,9 @@
       <c r="S354" s="7">
         <v>0</v>
       </c>
+      <c r="T354" t="b">
+        <v>0</v>
+      </c>
       <c r="U354" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26528,17 +26561,18 @@
       <c r="S355" s="7">
         <v>0</v>
       </c>
+      <c r="T355" t="b">
+        <v>1</v>
+      </c>
       <c r="U355" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V355" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W355" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V355" s="2">
+        <v>228</v>
+      </c>
+      <c r="W355" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="356" spans="1:23" x14ac:dyDescent="0.2">
@@ -26599,17 +26633,18 @@
       <c r="S356" s="7">
         <v>0</v>
       </c>
+      <c r="T356" t="b">
+        <v>1</v>
+      </c>
       <c r="U356" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V356" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W356" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V356" s="2">
+        <v>40</v>
+      </c>
+      <c r="W356" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="357" spans="1:23" x14ac:dyDescent="0.2">
@@ -26670,17 +26705,18 @@
       <c r="S357" s="7">
         <v>0</v>
       </c>
+      <c r="T357" t="b">
+        <v>1</v>
+      </c>
       <c r="U357" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V357" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W357" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V357" s="2">
+        <v>9</v>
+      </c>
+      <c r="W357" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="358" spans="1:23" x14ac:dyDescent="0.2">
@@ -26741,17 +26777,18 @@
       <c r="S358" s="7">
         <v>0</v>
       </c>
+      <c r="T358" t="b">
+        <v>1</v>
+      </c>
       <c r="U358" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V358" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W358" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V358" s="2">
+        <v>78</v>
+      </c>
+      <c r="W358" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="359" spans="1:23" x14ac:dyDescent="0.2">
@@ -26812,17 +26849,18 @@
       <c r="S359" s="7">
         <v>0</v>
       </c>
+      <c r="T359" t="b">
+        <v>1</v>
+      </c>
       <c r="U359" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V359" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W359" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V359" s="2">
+        <v>10</v>
+      </c>
+      <c r="W359" s="12" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="360" spans="1:23" x14ac:dyDescent="0.2">
@@ -26883,6 +26921,9 @@
       <c r="S360" s="7">
         <v>0</v>
       </c>
+      <c r="T360" t="b">
+        <v>0</v>
+      </c>
       <c r="U360" s="2" t="str">
         <f t="shared" si="19"/>
         <v>NA</v>
@@ -26954,17 +26995,18 @@
       <c r="S361" s="7">
         <v>0</v>
       </c>
+      <c r="T361" t="b">
+        <v>1</v>
+      </c>
       <c r="U361" s="2" t="str">
         <f t="shared" si="19"/>
-        <v>NA</v>
-      </c>
-      <c r="V361" s="2" t="str">
-        <f t="shared" si="20"/>
-        <v>NA</v>
-      </c>
-      <c r="W361" s="12" t="str">
-        <f t="shared" si="21"/>
-        <v>NA</v>
+        <v/>
+      </c>
+      <c r="V361" s="2">
+        <v>5</v>
+      </c>
+      <c r="W361" s="12" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dataset updated till S384 & S385-396
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96475E1C-046E-564F-94A7-5B20177E3C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9C0B91-0A1D-194C-8CAB-84B3D6E66D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="-38400" yWindow="-4120" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -690,11 +690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W361"/>
+  <dimension ref="A1:W385"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A354" zoomScale="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W361" sqref="A1:W361"/>
+      <selection pane="topRight" activeCell="W385" sqref="W385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -25680,7 +25680,7 @@
         <v>0</v>
       </c>
       <c r="U343" s="2" t="str">
-        <f t="shared" ref="U339:U361" si="19">IF(T343=FALSE, "NA", "")</f>
+        <f t="shared" ref="U343:U360" si="19">IF(T343=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V343" s="2" t="str">
@@ -26994,8 +26994,1430 @@
         <v>1</v>
       </c>
     </row>
+    <row r="362" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A362" s="10">
+        <v>361</v>
+      </c>
+      <c r="B362" s="7">
+        <v>0</v>
+      </c>
+      <c r="C362" s="7">
+        <v>0</v>
+      </c>
+      <c r="D362" s="7">
+        <v>0</v>
+      </c>
+      <c r="E362" s="7">
+        <v>0</v>
+      </c>
+      <c r="F362" s="7">
+        <v>0</v>
+      </c>
+      <c r="G362" s="7">
+        <v>0</v>
+      </c>
+      <c r="H362" s="7">
+        <v>0</v>
+      </c>
+      <c r="I362" s="7">
+        <v>0</v>
+      </c>
+      <c r="J362" s="7">
+        <v>10.027028501079499</v>
+      </c>
+      <c r="K362" s="7">
+        <v>0</v>
+      </c>
+      <c r="L362" s="7">
+        <v>0</v>
+      </c>
+      <c r="M362" s="7">
+        <v>9.9106800659364591</v>
+      </c>
+      <c r="N362" s="7">
+        <v>0</v>
+      </c>
+      <c r="O362" s="7">
+        <v>0</v>
+      </c>
+      <c r="P362" s="7">
+        <v>0.95536107304973705</v>
+      </c>
+      <c r="Q362" s="7">
+        <v>0</v>
+      </c>
+      <c r="R362" s="7">
+        <v>1.2637847265540301</v>
+      </c>
+      <c r="S362" s="7">
+        <v>0</v>
+      </c>
+      <c r="T362" t="b">
+        <v>1</v>
+      </c>
+      <c r="U362" s="2">
+        <v>23</v>
+      </c>
+      <c r="V362" s="2">
+        <v>2</v>
+      </c>
+      <c r="W362" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="363" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A363" s="10">
+        <v>362</v>
+      </c>
+      <c r="B363" s="7">
+        <v>0</v>
+      </c>
+      <c r="C363" s="7">
+        <v>0</v>
+      </c>
+      <c r="D363" s="7">
+        <v>0</v>
+      </c>
+      <c r="E363" s="7">
+        <v>0</v>
+      </c>
+      <c r="F363" s="7">
+        <v>0</v>
+      </c>
+      <c r="G363" s="7">
+        <v>12.9322799900494</v>
+      </c>
+      <c r="H363" s="7">
+        <v>0</v>
+      </c>
+      <c r="I363" s="7">
+        <v>11.4070211112476</v>
+      </c>
+      <c r="J363" s="7">
+        <v>0</v>
+      </c>
+      <c r="K363" s="7">
+        <v>0</v>
+      </c>
+      <c r="L363" s="7">
+        <v>0</v>
+      </c>
+      <c r="M363" s="7">
+        <v>0</v>
+      </c>
+      <c r="N363" s="7">
+        <v>0</v>
+      </c>
+      <c r="O363" s="7">
+        <v>0</v>
+      </c>
+      <c r="P363" s="7">
+        <v>2.9939066121672302</v>
+      </c>
+      <c r="Q363" s="7">
+        <v>0</v>
+      </c>
+      <c r="R363" s="7">
+        <v>1.3417090856692999</v>
+      </c>
+      <c r="S363" s="7">
+        <v>0</v>
+      </c>
+      <c r="T363" t="b">
+        <v>1</v>
+      </c>
+      <c r="U363" s="2">
+        <v>160</v>
+      </c>
+      <c r="V363" s="2">
+        <v>244</v>
+      </c>
+      <c r="W363" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="364" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A364" s="10">
+        <v>363</v>
+      </c>
+      <c r="B364" s="7">
+        <v>0</v>
+      </c>
+      <c r="C364" s="7">
+        <v>0</v>
+      </c>
+      <c r="D364" s="7">
+        <v>0</v>
+      </c>
+      <c r="E364" s="7">
+        <v>0</v>
+      </c>
+      <c r="F364" s="7">
+        <v>11.725487070546199</v>
+      </c>
+      <c r="G364" s="7">
+        <v>0</v>
+      </c>
+      <c r="H364" s="7">
+        <v>7.7572132153346702</v>
+      </c>
+      <c r="I364" s="7">
+        <v>0</v>
+      </c>
+      <c r="J364" s="7">
+        <v>0</v>
+      </c>
+      <c r="K364" s="7">
+        <v>0</v>
+      </c>
+      <c r="L364" s="7">
+        <v>0</v>
+      </c>
+      <c r="M364" s="7">
+        <v>0</v>
+      </c>
+      <c r="N364" s="7">
+        <v>0</v>
+      </c>
+      <c r="O364" s="7">
+        <v>0</v>
+      </c>
+      <c r="P364" s="7">
+        <v>1.1519750552569099</v>
+      </c>
+      <c r="Q364" s="7">
+        <v>0</v>
+      </c>
+      <c r="R364" s="7">
+        <v>2.0822727485293102</v>
+      </c>
+      <c r="S364" s="7">
+        <v>0</v>
+      </c>
+      <c r="T364" t="b">
+        <v>0</v>
+      </c>
+      <c r="U364" s="2" t="str">
+        <f>IF(T364=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V364" s="2" t="str">
+        <f>IF(T364=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W364" s="2" t="str">
+        <f>IF(T364=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="365" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A365" s="10">
+        <v>364</v>
+      </c>
+      <c r="B365" s="7">
+        <v>0</v>
+      </c>
+      <c r="C365" s="7">
+        <v>0</v>
+      </c>
+      <c r="D365" s="7">
+        <v>0</v>
+      </c>
+      <c r="E365" s="7">
+        <v>7.8711556575569999</v>
+      </c>
+      <c r="F365" s="7">
+        <v>0</v>
+      </c>
+      <c r="G365" s="7">
+        <v>0</v>
+      </c>
+      <c r="H365" s="7">
+        <v>0</v>
+      </c>
+      <c r="I365" s="7">
+        <v>0</v>
+      </c>
+      <c r="J365" s="7">
+        <v>12.258505129058101</v>
+      </c>
+      <c r="K365" s="7">
+        <v>0</v>
+      </c>
+      <c r="L365" s="7">
+        <v>0</v>
+      </c>
+      <c r="M365" s="7">
+        <v>0</v>
+      </c>
+      <c r="N365" s="7">
+        <v>0</v>
+      </c>
+      <c r="O365" s="7">
+        <v>0</v>
+      </c>
+      <c r="P365" s="7">
+        <v>2.90818593539491</v>
+      </c>
+      <c r="Q365" s="7">
+        <v>0</v>
+      </c>
+      <c r="R365" s="7">
+        <v>1.1482320331128499</v>
+      </c>
+      <c r="S365" s="7">
+        <v>0</v>
+      </c>
+      <c r="T365" t="b">
+        <v>1</v>
+      </c>
+      <c r="U365" s="2">
+        <v>26</v>
+      </c>
+      <c r="V365" s="2">
+        <v>9</v>
+      </c>
+      <c r="W365" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A366" s="10">
+        <v>365</v>
+      </c>
+      <c r="B366" s="7">
+        <v>4.5896847771906799</v>
+      </c>
+      <c r="C366" s="7">
+        <v>0</v>
+      </c>
+      <c r="D366" s="7">
+        <v>0</v>
+      </c>
+      <c r="E366" s="7">
+        <v>0</v>
+      </c>
+      <c r="F366" s="7">
+        <v>0</v>
+      </c>
+      <c r="G366" s="7">
+        <v>0</v>
+      </c>
+      <c r="H366" s="7">
+        <v>0</v>
+      </c>
+      <c r="I366" s="7">
+        <v>0</v>
+      </c>
+      <c r="J366" s="7">
+        <v>0</v>
+      </c>
+      <c r="K366" s="7">
+        <v>0</v>
+      </c>
+      <c r="L366" s="7">
+        <v>0</v>
+      </c>
+      <c r="M366" s="7">
+        <v>8.7981177837518008</v>
+      </c>
+      <c r="N366" s="7">
+        <v>0</v>
+      </c>
+      <c r="O366" s="7">
+        <v>0</v>
+      </c>
+      <c r="P366" s="7">
+        <v>1.08143531091953</v>
+      </c>
+      <c r="Q366" s="7">
+        <v>0</v>
+      </c>
+      <c r="R366" s="7">
+        <v>4.6713815851826199</v>
+      </c>
+      <c r="S366" s="7">
+        <v>0</v>
+      </c>
+      <c r="T366" t="b">
+        <v>0</v>
+      </c>
+      <c r="U366" s="2" t="str">
+        <f t="shared" ref="U366:U385" si="22">IF(T366=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V366" s="2" t="str">
+        <f t="shared" ref="V366:V385" si="23">IF(T366=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W366" s="2" t="str">
+        <f t="shared" ref="W366:W385" si="24">IF(T366=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="367" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A367" s="10">
+        <v>366</v>
+      </c>
+      <c r="B367" s="7">
+        <v>0</v>
+      </c>
+      <c r="C367" s="7">
+        <v>0</v>
+      </c>
+      <c r="D367" s="7">
+        <v>0</v>
+      </c>
+      <c r="E367" s="7">
+        <v>0</v>
+      </c>
+      <c r="F367" s="7">
+        <v>12.098199374902901</v>
+      </c>
+      <c r="G367" s="7">
+        <v>0</v>
+      </c>
+      <c r="H367" s="7">
+        <v>0</v>
+      </c>
+      <c r="I367" s="7">
+        <v>0</v>
+      </c>
+      <c r="J367" s="7">
+        <v>0</v>
+      </c>
+      <c r="K367" s="7">
+        <v>0</v>
+      </c>
+      <c r="L367" s="7">
+        <v>0</v>
+      </c>
+      <c r="M367" s="7">
+        <v>0</v>
+      </c>
+      <c r="N367" s="7">
+        <v>0</v>
+      </c>
+      <c r="O367" s="7">
+        <v>0</v>
+      </c>
+      <c r="P367" s="7">
+        <v>2.5834594307104202</v>
+      </c>
+      <c r="Q367" s="7">
+        <v>0</v>
+      </c>
+      <c r="R367" s="7">
+        <v>2.94551194000233</v>
+      </c>
+      <c r="S367" s="7">
+        <v>0</v>
+      </c>
+      <c r="T367" t="b">
+        <v>0</v>
+      </c>
+      <c r="U367" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V367" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W367" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="368" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A368" s="10">
+        <v>367</v>
+      </c>
+      <c r="T368" t="b">
+        <v>0</v>
+      </c>
+      <c r="U368" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V368" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W368" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="369" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A369" s="10">
+        <v>368</v>
+      </c>
+      <c r="T369" t="b">
+        <v>1</v>
+      </c>
+      <c r="U369" s="2">
+        <v>20</v>
+      </c>
+      <c r="V369" s="2">
+        <v>8</v>
+      </c>
+      <c r="W369" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A370" s="10">
+        <v>369</v>
+      </c>
+      <c r="T370" t="b">
+        <v>0</v>
+      </c>
+      <c r="U370" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V370" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W370" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="371" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A371" s="10">
+        <v>370</v>
+      </c>
+      <c r="T371" t="b">
+        <v>0</v>
+      </c>
+      <c r="U371" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V371" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W371" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="372" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A372" s="10">
+        <v>371</v>
+      </c>
+      <c r="T372" t="b">
+        <v>0</v>
+      </c>
+      <c r="U372" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V372" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W372" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="373" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A373" s="10">
+        <v>372</v>
+      </c>
+      <c r="T373" t="b">
+        <v>1</v>
+      </c>
+      <c r="U373" s="2">
+        <v>16</v>
+      </c>
+      <c r="V373" s="2">
+        <v>2</v>
+      </c>
+      <c r="W373" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A374" s="10">
+        <v>373</v>
+      </c>
+      <c r="B374" s="7">
+        <v>0</v>
+      </c>
+      <c r="C374" s="7">
+        <v>0</v>
+      </c>
+      <c r="D374" s="7">
+        <v>0</v>
+      </c>
+      <c r="E374" s="7">
+        <v>8.3476138461952996</v>
+      </c>
+      <c r="F374" s="7">
+        <v>0</v>
+      </c>
+      <c r="G374" s="7">
+        <v>8.84289624350731</v>
+      </c>
+      <c r="H374" s="7">
+        <v>0</v>
+      </c>
+      <c r="I374" s="7">
+        <v>0</v>
+      </c>
+      <c r="J374" s="7">
+        <v>0</v>
+      </c>
+      <c r="K374" s="7">
+        <v>0</v>
+      </c>
+      <c r="L374" s="7">
+        <v>0</v>
+      </c>
+      <c r="M374" s="7">
+        <v>0</v>
+      </c>
+      <c r="N374" s="7">
+        <v>0</v>
+      </c>
+      <c r="O374" s="7">
+        <v>0</v>
+      </c>
+      <c r="P374" s="7">
+        <v>2.6982363396076599</v>
+      </c>
+      <c r="Q374" s="7">
+        <v>0</v>
+      </c>
+      <c r="R374" s="7">
+        <v>2.72204799332459</v>
+      </c>
+      <c r="S374" s="7">
+        <v>0</v>
+      </c>
+      <c r="T374" t="b">
+        <v>0</v>
+      </c>
+      <c r="U374" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V374" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W374" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="375" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A375" s="10">
+        <v>374</v>
+      </c>
+      <c r="B375" s="7">
+        <v>7.3182769275371999</v>
+      </c>
+      <c r="C375" s="7">
+        <v>0</v>
+      </c>
+      <c r="D375" s="7">
+        <v>0</v>
+      </c>
+      <c r="E375" s="7">
+        <v>0</v>
+      </c>
+      <c r="F375" s="7">
+        <v>0</v>
+      </c>
+      <c r="G375" s="7">
+        <v>0</v>
+      </c>
+      <c r="H375" s="7">
+        <v>0</v>
+      </c>
+      <c r="I375" s="7">
+        <v>0</v>
+      </c>
+      <c r="J375" s="7">
+        <v>12.744411037919299</v>
+      </c>
+      <c r="K375" s="7">
+        <v>0</v>
+      </c>
+      <c r="L375" s="7">
+        <v>0</v>
+      </c>
+      <c r="M375" s="7">
+        <v>0</v>
+      </c>
+      <c r="N375" s="7">
+        <v>0</v>
+      </c>
+      <c r="O375" s="7">
+        <v>0</v>
+      </c>
+      <c r="P375" s="7">
+        <v>4.0235072833486401</v>
+      </c>
+      <c r="Q375" s="7">
+        <v>0</v>
+      </c>
+      <c r="R375" s="7">
+        <v>4.1664222620531701</v>
+      </c>
+      <c r="S375" s="7">
+        <v>0</v>
+      </c>
+      <c r="T375" t="b">
+        <v>0</v>
+      </c>
+      <c r="U375" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V375" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W375" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="376" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A376" s="10">
+        <v>375</v>
+      </c>
+      <c r="B376" s="7">
+        <v>0</v>
+      </c>
+      <c r="C376" s="7">
+        <v>0</v>
+      </c>
+      <c r="D376" s="7">
+        <v>0</v>
+      </c>
+      <c r="E376" s="7">
+        <v>0</v>
+      </c>
+      <c r="F376" s="7">
+        <v>0</v>
+      </c>
+      <c r="G376" s="7">
+        <v>0</v>
+      </c>
+      <c r="H376" s="7">
+        <v>0</v>
+      </c>
+      <c r="I376" s="7">
+        <v>7.7395851784695298</v>
+      </c>
+      <c r="J376" s="7">
+        <v>11.7662746702189</v>
+      </c>
+      <c r="K376" s="7">
+        <v>0</v>
+      </c>
+      <c r="L376" s="7">
+        <v>0</v>
+      </c>
+      <c r="M376" s="7">
+        <v>0</v>
+      </c>
+      <c r="N376" s="7">
+        <v>0</v>
+      </c>
+      <c r="O376" s="7">
+        <v>0</v>
+      </c>
+      <c r="P376" s="7">
+        <v>1.95624618957984</v>
+      </c>
+      <c r="Q376" s="7">
+        <v>0</v>
+      </c>
+      <c r="R376" s="7">
+        <v>2.5570223036385902</v>
+      </c>
+      <c r="S376" s="7">
+        <v>0</v>
+      </c>
+      <c r="T376" t="b">
+        <v>1</v>
+      </c>
+      <c r="U376" s="2">
+        <v>62</v>
+      </c>
+      <c r="V376" s="2">
+        <v>99</v>
+      </c>
+      <c r="W376" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="377" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A377" s="10">
+        <v>376</v>
+      </c>
+      <c r="B377" s="7">
+        <v>7.4873563118831203</v>
+      </c>
+      <c r="C377" s="7">
+        <v>0</v>
+      </c>
+      <c r="D377" s="7">
+        <v>0</v>
+      </c>
+      <c r="E377" s="7">
+        <v>0</v>
+      </c>
+      <c r="F377" s="7">
+        <v>0</v>
+      </c>
+      <c r="G377" s="7">
+        <v>0</v>
+      </c>
+      <c r="H377" s="7">
+        <v>0</v>
+      </c>
+      <c r="I377" s="7">
+        <v>14.3881865612897</v>
+      </c>
+      <c r="J377" s="7">
+        <v>0</v>
+      </c>
+      <c r="K377" s="7">
+        <v>0</v>
+      </c>
+      <c r="L377" s="7">
+        <v>0</v>
+      </c>
+      <c r="M377" s="7">
+        <v>0</v>
+      </c>
+      <c r="N377" s="7">
+        <v>0</v>
+      </c>
+      <c r="O377" s="7">
+        <v>0</v>
+      </c>
+      <c r="P377" s="7">
+        <v>2.02638325547822</v>
+      </c>
+      <c r="Q377" s="7">
+        <v>0</v>
+      </c>
+      <c r="R377" s="7">
+        <v>4.8910141297572398</v>
+      </c>
+      <c r="S377" s="7">
+        <v>0</v>
+      </c>
+      <c r="T377" t="b">
+        <v>0</v>
+      </c>
+      <c r="U377" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V377" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W377" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="378" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A378" s="10">
+        <v>377</v>
+      </c>
+      <c r="B378" s="7">
+        <v>0</v>
+      </c>
+      <c r="C378" s="7">
+        <v>0</v>
+      </c>
+      <c r="D378" s="7">
+        <v>0</v>
+      </c>
+      <c r="E378" s="7">
+        <v>10.196543628128101</v>
+      </c>
+      <c r="F378" s="7">
+        <v>0</v>
+      </c>
+      <c r="G378" s="7">
+        <v>0</v>
+      </c>
+      <c r="H378" s="7">
+        <v>0</v>
+      </c>
+      <c r="I378" s="7">
+        <v>0</v>
+      </c>
+      <c r="J378" s="7">
+        <v>0</v>
+      </c>
+      <c r="K378" s="7">
+        <v>0</v>
+      </c>
+      <c r="L378" s="7">
+        <v>8.2529439482906</v>
+      </c>
+      <c r="M378" s="7">
+        <v>0</v>
+      </c>
+      <c r="N378" s="7">
+        <v>0</v>
+      </c>
+      <c r="O378" s="7">
+        <v>0</v>
+      </c>
+      <c r="P378" s="7">
+        <v>2.3363401802284298</v>
+      </c>
+      <c r="Q378" s="7">
+        <v>0</v>
+      </c>
+      <c r="R378" s="7">
+        <v>2.4221449087782498</v>
+      </c>
+      <c r="S378" s="7">
+        <v>0</v>
+      </c>
+      <c r="T378" t="b">
+        <v>1</v>
+      </c>
+      <c r="U378" s="2">
+        <v>1504</v>
+      </c>
+      <c r="V378" s="2">
+        <v>303</v>
+      </c>
+      <c r="W378" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="379" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A379" s="10">
+        <v>378</v>
+      </c>
+      <c r="B379" s="7">
+        <v>0</v>
+      </c>
+      <c r="C379" s="7">
+        <v>0</v>
+      </c>
+      <c r="D379" s="7">
+        <v>0</v>
+      </c>
+      <c r="E379" s="7">
+        <v>0</v>
+      </c>
+      <c r="F379" s="7">
+        <v>0</v>
+      </c>
+      <c r="G379" s="7">
+        <v>0</v>
+      </c>
+      <c r="H379" s="7">
+        <v>7.6936050225384003</v>
+      </c>
+      <c r="I379" s="7">
+        <v>0</v>
+      </c>
+      <c r="J379" s="7">
+        <v>10.0176220806781</v>
+      </c>
+      <c r="K379" s="7">
+        <v>0</v>
+      </c>
+      <c r="L379" s="7">
+        <v>0</v>
+      </c>
+      <c r="M379" s="7">
+        <v>0</v>
+      </c>
+      <c r="N379" s="7">
+        <v>0</v>
+      </c>
+      <c r="O379" s="7">
+        <v>0</v>
+      </c>
+      <c r="P379" s="7">
+        <v>2.5759175442115301</v>
+      </c>
+      <c r="Q379" s="7">
+        <v>0</v>
+      </c>
+      <c r="R379" s="7">
+        <v>4.6519932594791102</v>
+      </c>
+      <c r="S379" s="7">
+        <v>0</v>
+      </c>
+      <c r="T379" t="b">
+        <v>0</v>
+      </c>
+      <c r="U379" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V379" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W379" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="380" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A380" s="10">
+        <v>379</v>
+      </c>
+      <c r="B380" s="7">
+        <v>0</v>
+      </c>
+      <c r="C380" s="7">
+        <v>0</v>
+      </c>
+      <c r="D380" s="7">
+        <v>7.3982687374564904</v>
+      </c>
+      <c r="E380" s="7">
+        <v>0</v>
+      </c>
+      <c r="F380" s="7">
+        <v>0</v>
+      </c>
+      <c r="G380" s="7">
+        <v>0</v>
+      </c>
+      <c r="H380" s="7">
+        <v>0</v>
+      </c>
+      <c r="I380" s="7">
+        <v>7.4922669039867298</v>
+      </c>
+      <c r="J380" s="7">
+        <v>0</v>
+      </c>
+      <c r="K380" s="7">
+        <v>0</v>
+      </c>
+      <c r="L380" s="7">
+        <v>0</v>
+      </c>
+      <c r="M380" s="7">
+        <v>0</v>
+      </c>
+      <c r="N380" s="7">
+        <v>0</v>
+      </c>
+      <c r="O380" s="7">
+        <v>0</v>
+      </c>
+      <c r="P380" s="7">
+        <v>3.0894234352830301</v>
+      </c>
+      <c r="Q380" s="7">
+        <v>0</v>
+      </c>
+      <c r="R380" s="7">
+        <v>2.30397679919413</v>
+      </c>
+      <c r="S380" s="7">
+        <v>0</v>
+      </c>
+      <c r="T380" t="b">
+        <v>1</v>
+      </c>
+      <c r="U380" s="2">
+        <v>17</v>
+      </c>
+      <c r="V380" s="2">
+        <v>3</v>
+      </c>
+      <c r="W380" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A381" s="10">
+        <v>380</v>
+      </c>
+      <c r="B381" s="7">
+        <v>0</v>
+      </c>
+      <c r="C381" s="7">
+        <v>0</v>
+      </c>
+      <c r="D381" s="7">
+        <v>0</v>
+      </c>
+      <c r="E381" s="7">
+        <v>0</v>
+      </c>
+      <c r="F381" s="7">
+        <v>12.643819500563801</v>
+      </c>
+      <c r="G381" s="7">
+        <v>0</v>
+      </c>
+      <c r="H381" s="7">
+        <v>0</v>
+      </c>
+      <c r="I381" s="7">
+        <v>0</v>
+      </c>
+      <c r="J381" s="7">
+        <v>10.3298343341311</v>
+      </c>
+      <c r="K381" s="7">
+        <v>0</v>
+      </c>
+      <c r="L381" s="7">
+        <v>0</v>
+      </c>
+      <c r="M381" s="7">
+        <v>0</v>
+      </c>
+      <c r="N381" s="7">
+        <v>0</v>
+      </c>
+      <c r="O381" s="7">
+        <v>0</v>
+      </c>
+      <c r="P381" s="7">
+        <v>1.7799885895637499</v>
+      </c>
+      <c r="Q381" s="7">
+        <v>0</v>
+      </c>
+      <c r="R381" s="7">
+        <v>4.2041166963452303</v>
+      </c>
+      <c r="S381" s="7">
+        <v>0</v>
+      </c>
+      <c r="T381" t="b">
+        <v>1</v>
+      </c>
+      <c r="U381" s="2">
+        <v>250</v>
+      </c>
+      <c r="V381" s="2">
+        <v>64</v>
+      </c>
+      <c r="W381" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="382" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A382" s="10">
+        <v>381</v>
+      </c>
+      <c r="B382" s="7">
+        <v>0</v>
+      </c>
+      <c r="C382" s="7">
+        <v>0</v>
+      </c>
+      <c r="D382" s="7">
+        <v>9.3582415553819995</v>
+      </c>
+      <c r="E382" s="7">
+        <v>0</v>
+      </c>
+      <c r="F382" s="7">
+        <v>0</v>
+      </c>
+      <c r="G382" s="7">
+        <v>0</v>
+      </c>
+      <c r="H382" s="7">
+        <v>0</v>
+      </c>
+      <c r="I382" s="7">
+        <v>0</v>
+      </c>
+      <c r="J382" s="7">
+        <v>0</v>
+      </c>
+      <c r="K382" s="7">
+        <v>0</v>
+      </c>
+      <c r="L382" s="7">
+        <v>0</v>
+      </c>
+      <c r="M382" s="7">
+        <v>7.8896744316926899</v>
+      </c>
+      <c r="N382" s="7">
+        <v>0</v>
+      </c>
+      <c r="O382" s="7">
+        <v>0</v>
+      </c>
+      <c r="P382" s="7">
+        <v>3.27903346882304</v>
+      </c>
+      <c r="Q382" s="7">
+        <v>0</v>
+      </c>
+      <c r="R382" s="7">
+        <v>5.0835015820016203</v>
+      </c>
+      <c r="S382" s="7">
+        <v>0</v>
+      </c>
+      <c r="T382" t="b">
+        <v>0</v>
+      </c>
+      <c r="U382" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V382" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W382" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="383" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A383" s="10">
+        <v>382</v>
+      </c>
+      <c r="B383" s="7">
+        <v>7.5068773971176199</v>
+      </c>
+      <c r="C383" s="7">
+        <v>0</v>
+      </c>
+      <c r="D383" s="7">
+        <v>0</v>
+      </c>
+      <c r="E383" s="7">
+        <v>0</v>
+      </c>
+      <c r="F383" s="7">
+        <v>9.9769617987710095</v>
+      </c>
+      <c r="G383" s="7">
+        <v>0</v>
+      </c>
+      <c r="H383" s="7">
+        <v>0</v>
+      </c>
+      <c r="I383" s="7">
+        <v>0</v>
+      </c>
+      <c r="J383" s="7">
+        <v>0</v>
+      </c>
+      <c r="K383" s="7">
+        <v>0</v>
+      </c>
+      <c r="L383" s="7">
+        <v>0</v>
+      </c>
+      <c r="M383" s="7">
+        <v>0</v>
+      </c>
+      <c r="N383" s="7">
+        <v>0</v>
+      </c>
+      <c r="O383" s="7">
+        <v>0</v>
+      </c>
+      <c r="P383" s="7">
+        <v>3.33302067097816</v>
+      </c>
+      <c r="Q383" s="7">
+        <v>0</v>
+      </c>
+      <c r="R383" s="7">
+        <v>5.0110950720181497</v>
+      </c>
+      <c r="S383" s="7">
+        <v>0</v>
+      </c>
+      <c r="T383" t="b">
+        <v>1</v>
+      </c>
+      <c r="U383" s="2">
+        <v>2368</v>
+      </c>
+      <c r="V383" s="2">
+        <v>247</v>
+      </c>
+      <c r="W383" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="384" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A384" s="10">
+        <v>383</v>
+      </c>
+      <c r="B384" s="7">
+        <v>0</v>
+      </c>
+      <c r="C384" s="7">
+        <v>0</v>
+      </c>
+      <c r="D384" s="7">
+        <v>0</v>
+      </c>
+      <c r="E384" s="7">
+        <v>0</v>
+      </c>
+      <c r="F384" s="7">
+        <v>0</v>
+      </c>
+      <c r="G384" s="7">
+        <v>0</v>
+      </c>
+      <c r="H384" s="7">
+        <v>8.8046479244904496</v>
+      </c>
+      <c r="I384" s="7">
+        <v>13.420922979332399</v>
+      </c>
+      <c r="J384" s="7">
+        <v>0</v>
+      </c>
+      <c r="K384" s="7">
+        <v>0</v>
+      </c>
+      <c r="L384" s="7">
+        <v>0</v>
+      </c>
+      <c r="M384" s="7">
+        <v>0</v>
+      </c>
+      <c r="N384" s="7">
+        <v>0</v>
+      </c>
+      <c r="O384" s="7">
+        <v>0</v>
+      </c>
+      <c r="P384" s="7">
+        <v>2.1967757400444001</v>
+      </c>
+      <c r="Q384" s="7">
+        <v>0</v>
+      </c>
+      <c r="R384" s="7">
+        <v>5.00031482925238</v>
+      </c>
+      <c r="S384" s="7">
+        <v>0</v>
+      </c>
+      <c r="T384" t="b">
+        <v>0</v>
+      </c>
+      <c r="U384" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V384" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W384" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="385" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A385" s="10">
+        <v>384</v>
+      </c>
+      <c r="B385" s="7">
+        <v>0</v>
+      </c>
+      <c r="C385" s="7">
+        <v>0</v>
+      </c>
+      <c r="D385" s="7">
+        <v>0</v>
+      </c>
+      <c r="E385" s="7">
+        <v>6.6401475952103901</v>
+      </c>
+      <c r="F385" s="7">
+        <v>0</v>
+      </c>
+      <c r="G385" s="7">
+        <v>0</v>
+      </c>
+      <c r="H385" s="7">
+        <v>0</v>
+      </c>
+      <c r="I385" s="7">
+        <v>0</v>
+      </c>
+      <c r="J385" s="7">
+        <v>0</v>
+      </c>
+      <c r="K385" s="7">
+        <v>0</v>
+      </c>
+      <c r="L385" s="7">
+        <v>10.6339966812752</v>
+      </c>
+      <c r="M385" s="7">
+        <v>0</v>
+      </c>
+      <c r="N385" s="7">
+        <v>0</v>
+      </c>
+      <c r="O385" s="7">
+        <v>0</v>
+      </c>
+      <c r="P385" s="7">
+        <v>3.4074703704985398</v>
+      </c>
+      <c r="Q385" s="7">
+        <v>0</v>
+      </c>
+      <c r="R385" s="7">
+        <v>3.1771517667197999</v>
+      </c>
+      <c r="S385" s="7">
+        <v>0</v>
+      </c>
+      <c r="T385" t="b">
+        <v>0</v>
+      </c>
+      <c r="U385" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V385" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W385" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W361">
+  <conditionalFormatting sqref="A1:W385">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Dataset updated till S408
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9C0B91-0A1D-194C-8CAB-84B3D6E66D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E29BC25-7E3A-FF4E-B8E2-74EA9EDC3771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4120" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="-38400" yWindow="-5300" windowWidth="38400" windowHeight="21600" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -359,7 +359,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -690,11 +700,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W385"/>
+  <dimension ref="A1:W409"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A354" zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W385" sqref="W385"/>
+    <sheetView tabSelected="1" topLeftCell="A366" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W409" sqref="W409"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27343,15 +27353,15 @@
         <v>0</v>
       </c>
       <c r="U366" s="2" t="str">
-        <f t="shared" ref="U366:U385" si="22">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="U366:U409" si="22">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V366" s="2" t="str">
-        <f t="shared" ref="V366:V385" si="23">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="V366:V409" si="23">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W366" s="2" t="str">
-        <f t="shared" ref="W366:W385" si="24">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="W366:W409" si="24">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -28416,8 +28426,1784 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="386" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A386" s="10">
+        <v>385</v>
+      </c>
+      <c r="B386" s="7">
+        <v>0</v>
+      </c>
+      <c r="C386" s="7">
+        <v>11.623131470932099</v>
+      </c>
+      <c r="D386" s="7">
+        <v>0</v>
+      </c>
+      <c r="E386" s="7">
+        <v>7.3493237705262304</v>
+      </c>
+      <c r="F386" s="7">
+        <v>0</v>
+      </c>
+      <c r="G386" s="7">
+        <v>0</v>
+      </c>
+      <c r="H386" s="7">
+        <v>0</v>
+      </c>
+      <c r="I386" s="7">
+        <v>0</v>
+      </c>
+      <c r="J386" s="7">
+        <v>0</v>
+      </c>
+      <c r="K386" s="7">
+        <v>0</v>
+      </c>
+      <c r="L386" s="7">
+        <v>0</v>
+      </c>
+      <c r="M386" s="7">
+        <v>0</v>
+      </c>
+      <c r="N386" s="7">
+        <v>0</v>
+      </c>
+      <c r="O386" s="7">
+        <v>2.9028094393700301</v>
+      </c>
+      <c r="P386" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q386" s="7">
+        <v>0</v>
+      </c>
+      <c r="R386" s="7">
+        <v>0</v>
+      </c>
+      <c r="S386" s="7">
+        <v>2.9734283629910898</v>
+      </c>
+      <c r="T386" t="b">
+        <v>0</v>
+      </c>
+      <c r="U386" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V386" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W386" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="387" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A387" s="10">
+        <v>386</v>
+      </c>
+      <c r="B387" s="7">
+        <v>0</v>
+      </c>
+      <c r="C387" s="7">
+        <v>0</v>
+      </c>
+      <c r="D387" s="7">
+        <v>0</v>
+      </c>
+      <c r="E387" s="7">
+        <v>0</v>
+      </c>
+      <c r="F387" s="7">
+        <v>0</v>
+      </c>
+      <c r="G387" s="7">
+        <v>0</v>
+      </c>
+      <c r="H387" s="7">
+        <v>8.5680732545096099</v>
+      </c>
+      <c r="I387" s="7">
+        <v>0</v>
+      </c>
+      <c r="J387" s="7">
+        <v>11.8749627944847</v>
+      </c>
+      <c r="K387" s="7">
+        <v>0</v>
+      </c>
+      <c r="L387" s="7">
+        <v>0</v>
+      </c>
+      <c r="M387" s="7">
+        <v>0</v>
+      </c>
+      <c r="N387" s="7">
+        <v>0</v>
+      </c>
+      <c r="O387" s="7">
+        <v>3.1324165166059199</v>
+      </c>
+      <c r="P387" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q387" s="7">
+        <v>0</v>
+      </c>
+      <c r="R387" s="7">
+        <v>0</v>
+      </c>
+      <c r="S387" s="7">
+        <v>4.5593653645546102</v>
+      </c>
+      <c r="T387" t="b">
+        <v>0</v>
+      </c>
+      <c r="U387" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V387" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W387" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="388" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A388" s="10">
+        <v>387</v>
+      </c>
+      <c r="B388" s="7">
+        <v>0</v>
+      </c>
+      <c r="C388" s="7">
+        <v>0</v>
+      </c>
+      <c r="D388" s="7">
+        <v>0</v>
+      </c>
+      <c r="E388" s="7">
+        <v>0</v>
+      </c>
+      <c r="F388" s="7">
+        <v>0</v>
+      </c>
+      <c r="G388" s="7">
+        <v>0</v>
+      </c>
+      <c r="H388" s="7">
+        <v>8.3932986406025307</v>
+      </c>
+      <c r="I388" s="7">
+        <v>0</v>
+      </c>
+      <c r="J388" s="7">
+        <v>0</v>
+      </c>
+      <c r="K388" s="7">
+        <v>8.0077924821096307</v>
+      </c>
+      <c r="L388" s="7">
+        <v>0</v>
+      </c>
+      <c r="M388" s="7">
+        <v>0</v>
+      </c>
+      <c r="N388" s="7">
+        <v>0</v>
+      </c>
+      <c r="O388" s="7">
+        <v>3.0803893993490599</v>
+      </c>
+      <c r="P388" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q388" s="7">
+        <v>0</v>
+      </c>
+      <c r="R388" s="7">
+        <v>0</v>
+      </c>
+      <c r="S388" s="7">
+        <v>3.0059720712855298</v>
+      </c>
+      <c r="T388" t="b">
+        <v>0</v>
+      </c>
+      <c r="U388" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V388" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W388" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="389" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A389" s="10">
+        <v>388</v>
+      </c>
+      <c r="B389" s="7">
+        <v>0</v>
+      </c>
+      <c r="C389" s="7">
+        <v>9.4591888065552308</v>
+      </c>
+      <c r="D389" s="7">
+        <v>0</v>
+      </c>
+      <c r="E389" s="7">
+        <v>0</v>
+      </c>
+      <c r="F389" s="7">
+        <v>0</v>
+      </c>
+      <c r="G389" s="7">
+        <v>0</v>
+      </c>
+      <c r="H389" s="7">
+        <v>0</v>
+      </c>
+      <c r="I389" s="7">
+        <v>0</v>
+      </c>
+      <c r="J389" s="7">
+        <v>0</v>
+      </c>
+      <c r="K389" s="7">
+        <v>9.7466815486291907</v>
+      </c>
+      <c r="L389" s="7">
+        <v>0</v>
+      </c>
+      <c r="M389" s="7">
+        <v>0</v>
+      </c>
+      <c r="N389" s="7">
+        <v>0</v>
+      </c>
+      <c r="O389" s="7">
+        <v>3.0467454736628001</v>
+      </c>
+      <c r="P389" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q389" s="7">
+        <v>0</v>
+      </c>
+      <c r="R389" s="7">
+        <v>0</v>
+      </c>
+      <c r="S389" s="7">
+        <v>3.3782817166268901</v>
+      </c>
+      <c r="T389" t="b">
+        <v>0</v>
+      </c>
+      <c r="U389" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V389" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W389" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="390" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A390" s="10">
+        <v>389</v>
+      </c>
+      <c r="B390" s="7">
+        <v>0</v>
+      </c>
+      <c r="C390" s="7">
+        <v>0</v>
+      </c>
+      <c r="D390" s="7">
+        <v>0</v>
+      </c>
+      <c r="E390" s="7">
+        <v>8.6945264536113207</v>
+      </c>
+      <c r="F390" s="7">
+        <v>0</v>
+      </c>
+      <c r="G390" s="7">
+        <v>7.84089256061743</v>
+      </c>
+      <c r="H390" s="7">
+        <v>0</v>
+      </c>
+      <c r="I390" s="7">
+        <v>0</v>
+      </c>
+      <c r="J390" s="7">
+        <v>0</v>
+      </c>
+      <c r="K390" s="7">
+        <v>0</v>
+      </c>
+      <c r="L390" s="7">
+        <v>0</v>
+      </c>
+      <c r="M390" s="7">
+        <v>0</v>
+      </c>
+      <c r="N390" s="7">
+        <v>0</v>
+      </c>
+      <c r="O390" s="7">
+        <v>2.9611932785208399</v>
+      </c>
+      <c r="P390" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q390" s="7">
+        <v>0</v>
+      </c>
+      <c r="R390" s="7">
+        <v>0</v>
+      </c>
+      <c r="S390" s="7">
+        <v>2.0062807880531799</v>
+      </c>
+      <c r="T390" t="b">
+        <v>0</v>
+      </c>
+      <c r="U390" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V390" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W390" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="391" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A391" s="10">
+        <v>390</v>
+      </c>
+      <c r="B391" s="7">
+        <v>0</v>
+      </c>
+      <c r="C391" s="7">
+        <v>12.332220096913099</v>
+      </c>
+      <c r="D391" s="7">
+        <v>0</v>
+      </c>
+      <c r="E391" s="7">
+        <v>0</v>
+      </c>
+      <c r="F391" s="7">
+        <v>0</v>
+      </c>
+      <c r="G391" s="7">
+        <v>0</v>
+      </c>
+      <c r="H391" s="7">
+        <v>8.1764985523495106</v>
+      </c>
+      <c r="I391" s="7">
+        <v>0</v>
+      </c>
+      <c r="J391" s="7">
+        <v>0</v>
+      </c>
+      <c r="K391" s="7">
+        <v>0</v>
+      </c>
+      <c r="L391" s="7">
+        <v>0</v>
+      </c>
+      <c r="M391" s="7">
+        <v>0</v>
+      </c>
+      <c r="N391" s="7">
+        <v>0</v>
+      </c>
+      <c r="O391" s="7">
+        <v>3.72285368187225</v>
+      </c>
+      <c r="P391" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q391" s="7">
+        <v>0</v>
+      </c>
+      <c r="R391" s="7">
+        <v>0</v>
+      </c>
+      <c r="S391" s="7">
+        <v>3.7679935797380399</v>
+      </c>
+      <c r="T391" t="b">
+        <v>1</v>
+      </c>
+      <c r="U391" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v/>
+      </c>
+      <c r="V391" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v/>
+      </c>
+      <c r="W391" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v/>
+      </c>
+    </row>
+    <row r="392" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A392" s="10">
+        <v>391</v>
+      </c>
+      <c r="B392" s="7">
+        <v>0</v>
+      </c>
+      <c r="C392" s="7">
+        <v>0</v>
+      </c>
+      <c r="D392" s="7">
+        <v>0</v>
+      </c>
+      <c r="E392" s="7">
+        <v>0</v>
+      </c>
+      <c r="F392" s="7">
+        <v>0</v>
+      </c>
+      <c r="G392" s="7">
+        <v>0</v>
+      </c>
+      <c r="H392" s="7">
+        <v>0</v>
+      </c>
+      <c r="I392" s="7">
+        <v>0</v>
+      </c>
+      <c r="J392" s="7">
+        <v>0</v>
+      </c>
+      <c r="K392" s="7">
+        <v>12.8454725097597</v>
+      </c>
+      <c r="L392" s="7">
+        <v>9.7625195189359406</v>
+      </c>
+      <c r="M392" s="7">
+        <v>0</v>
+      </c>
+      <c r="N392" s="7">
+        <v>0</v>
+      </c>
+      <c r="O392" s="7">
+        <v>1.27054282567254</v>
+      </c>
+      <c r="P392" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q392" s="7">
+        <v>0</v>
+      </c>
+      <c r="R392" s="7">
+        <v>0</v>
+      </c>
+      <c r="S392" s="7">
+        <v>1.7715845436836599</v>
+      </c>
+      <c r="T392" t="b">
+        <v>0</v>
+      </c>
+      <c r="U392" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V392" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W392" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="393" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A393" s="10">
+        <v>392</v>
+      </c>
+      <c r="B393" s="7">
+        <v>0</v>
+      </c>
+      <c r="C393" s="7">
+        <v>0</v>
+      </c>
+      <c r="D393" s="7">
+        <v>10.1666492142179</v>
+      </c>
+      <c r="E393" s="7">
+        <v>0</v>
+      </c>
+      <c r="F393" s="7">
+        <v>0</v>
+      </c>
+      <c r="G393" s="7">
+        <v>0</v>
+      </c>
+      <c r="H393" s="7">
+        <v>0</v>
+      </c>
+      <c r="I393" s="7">
+        <v>0</v>
+      </c>
+      <c r="J393" s="7">
+        <v>0</v>
+      </c>
+      <c r="K393" s="7">
+        <v>0</v>
+      </c>
+      <c r="L393" s="7">
+        <v>10.5428626321099</v>
+      </c>
+      <c r="M393" s="7">
+        <v>0</v>
+      </c>
+      <c r="N393" s="7">
+        <v>0</v>
+      </c>
+      <c r="O393" s="7">
+        <v>1.67370536306318</v>
+      </c>
+      <c r="P393" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q393" s="7">
+        <v>0</v>
+      </c>
+      <c r="R393" s="7">
+        <v>0</v>
+      </c>
+      <c r="S393" s="7">
+        <v>3.3424735421646998</v>
+      </c>
+      <c r="T393" t="b">
+        <v>0</v>
+      </c>
+      <c r="U393" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V393" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W393" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="394" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A394" s="10">
+        <v>393</v>
+      </c>
+      <c r="B394" s="7">
+        <v>0</v>
+      </c>
+      <c r="C394" s="7">
+        <v>9.0057191532473198</v>
+      </c>
+      <c r="D394" s="7">
+        <v>0</v>
+      </c>
+      <c r="E394" s="7">
+        <v>0</v>
+      </c>
+      <c r="F394" s="7">
+        <v>0</v>
+      </c>
+      <c r="G394" s="7">
+        <v>0</v>
+      </c>
+      <c r="H394" s="7">
+        <v>0</v>
+      </c>
+      <c r="I394" s="7">
+        <v>9.9810821408384403</v>
+      </c>
+      <c r="J394" s="7">
+        <v>0</v>
+      </c>
+      <c r="K394" s="7">
+        <v>0</v>
+      </c>
+      <c r="L394" s="7">
+        <v>0</v>
+      </c>
+      <c r="M394" s="7">
+        <v>0</v>
+      </c>
+      <c r="N394" s="7">
+        <v>0</v>
+      </c>
+      <c r="O394" s="7">
+        <v>2.6060169436783802</v>
+      </c>
+      <c r="P394" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q394" s="7">
+        <v>0</v>
+      </c>
+      <c r="R394" s="7">
+        <v>0</v>
+      </c>
+      <c r="S394" s="7">
+        <v>4.1865122125220697</v>
+      </c>
+      <c r="T394" t="b">
+        <v>0</v>
+      </c>
+      <c r="U394" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V394" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W394" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="395" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A395" s="10">
+        <v>394</v>
+      </c>
+      <c r="B395" s="7">
+        <v>0</v>
+      </c>
+      <c r="C395" s="7">
+        <v>0</v>
+      </c>
+      <c r="D395" s="7">
+        <v>0</v>
+      </c>
+      <c r="E395" s="7">
+        <v>0</v>
+      </c>
+      <c r="F395" s="7">
+        <v>7.82862582440697</v>
+      </c>
+      <c r="G395" s="7">
+        <v>0</v>
+      </c>
+      <c r="H395" s="7">
+        <v>0</v>
+      </c>
+      <c r="I395" s="7">
+        <v>0</v>
+      </c>
+      <c r="J395" s="7">
+        <v>0</v>
+      </c>
+      <c r="K395" s="7">
+        <v>0</v>
+      </c>
+      <c r="L395" s="7">
+        <v>9.3605940738757099</v>
+      </c>
+      <c r="M395" s="7">
+        <v>0</v>
+      </c>
+      <c r="N395" s="7">
+        <v>0</v>
+      </c>
+      <c r="O395" s="7">
+        <v>1.95095114076859</v>
+      </c>
+      <c r="P395" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q395" s="7">
+        <v>0</v>
+      </c>
+      <c r="R395" s="7">
+        <v>0</v>
+      </c>
+      <c r="S395" s="7">
+        <v>5.2124648799158599</v>
+      </c>
+      <c r="T395" t="b">
+        <v>0</v>
+      </c>
+      <c r="U395" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V395" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W395" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="396" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A396" s="10">
+        <v>395</v>
+      </c>
+      <c r="B396" s="7">
+        <v>7.90295179539185</v>
+      </c>
+      <c r="C396" s="7">
+        <v>0</v>
+      </c>
+      <c r="D396" s="7">
+        <v>0</v>
+      </c>
+      <c r="E396" s="7">
+        <v>0</v>
+      </c>
+      <c r="F396" s="7">
+        <v>0</v>
+      </c>
+      <c r="G396" s="7">
+        <v>0</v>
+      </c>
+      <c r="H396" s="7">
+        <v>0</v>
+      </c>
+      <c r="I396" s="7">
+        <v>0</v>
+      </c>
+      <c r="J396" s="7">
+        <v>0</v>
+      </c>
+      <c r="K396" s="7">
+        <v>12.3907719794593</v>
+      </c>
+      <c r="L396" s="7">
+        <v>0</v>
+      </c>
+      <c r="M396" s="7">
+        <v>0</v>
+      </c>
+      <c r="N396" s="7">
+        <v>0</v>
+      </c>
+      <c r="O396" s="7">
+        <v>2.5877596013832198</v>
+      </c>
+      <c r="P396" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q396" s="7">
+        <v>0</v>
+      </c>
+      <c r="R396" s="7">
+        <v>0</v>
+      </c>
+      <c r="S396" s="7">
+        <v>2.6969584854454598</v>
+      </c>
+      <c r="T396" t="b">
+        <v>0</v>
+      </c>
+      <c r="U396" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V396" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W396" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="397" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A397" s="10">
+        <v>396</v>
+      </c>
+      <c r="B397" s="7">
+        <v>0</v>
+      </c>
+      <c r="C397" s="7">
+        <v>9.8467399952795098</v>
+      </c>
+      <c r="D397" s="7">
+        <v>0</v>
+      </c>
+      <c r="E397" s="7">
+        <v>0</v>
+      </c>
+      <c r="F397" s="7">
+        <v>0</v>
+      </c>
+      <c r="G397" s="7">
+        <v>0</v>
+      </c>
+      <c r="H397" s="7">
+        <v>0</v>
+      </c>
+      <c r="I397" s="7">
+        <v>0</v>
+      </c>
+      <c r="J397" s="7">
+        <v>0</v>
+      </c>
+      <c r="K397" s="7">
+        <v>0</v>
+      </c>
+      <c r="L397" s="7">
+        <v>0</v>
+      </c>
+      <c r="M397" s="7">
+        <v>12.0442957023806</v>
+      </c>
+      <c r="N397" s="7">
+        <v>0</v>
+      </c>
+      <c r="O397" s="7">
+        <v>1.7764230503510801</v>
+      </c>
+      <c r="P397" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q397" s="7">
+        <v>0</v>
+      </c>
+      <c r="R397" s="7">
+        <v>0</v>
+      </c>
+      <c r="S397" s="7">
+        <v>1.72482570034092</v>
+      </c>
+      <c r="T397" t="b">
+        <v>0</v>
+      </c>
+      <c r="U397" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V397" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W397" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="398" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A398" s="10">
+        <v>397</v>
+      </c>
+      <c r="B398" s="7">
+        <v>0</v>
+      </c>
+      <c r="C398" s="7">
+        <v>0</v>
+      </c>
+      <c r="D398" s="7">
+        <v>0</v>
+      </c>
+      <c r="E398" s="7">
+        <v>0</v>
+      </c>
+      <c r="F398" s="7">
+        <v>12.226008839382899</v>
+      </c>
+      <c r="G398" s="7">
+        <v>0</v>
+      </c>
+      <c r="H398" s="7">
+        <v>0</v>
+      </c>
+      <c r="I398" s="7">
+        <v>0</v>
+      </c>
+      <c r="J398" s="7">
+        <v>0</v>
+      </c>
+      <c r="K398" s="7">
+        <v>8.6659373891436395</v>
+      </c>
+      <c r="L398" s="7">
+        <v>0</v>
+      </c>
+      <c r="M398" s="7">
+        <v>0</v>
+      </c>
+      <c r="N398" s="7">
+        <v>0</v>
+      </c>
+      <c r="O398" s="7">
+        <v>2.2670499414174601</v>
+      </c>
+      <c r="P398" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q398" s="7">
+        <v>0</v>
+      </c>
+      <c r="R398" s="7">
+        <v>0</v>
+      </c>
+      <c r="S398" s="7">
+        <v>3.07874030191405</v>
+      </c>
+      <c r="T398" t="b">
+        <v>0</v>
+      </c>
+      <c r="U398" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V398" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W398" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="399" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A399" s="10">
+        <v>398</v>
+      </c>
+      <c r="B399" s="7">
+        <v>0</v>
+      </c>
+      <c r="C399" s="7">
+        <v>0</v>
+      </c>
+      <c r="D399" s="7">
+        <v>0</v>
+      </c>
+      <c r="E399" s="7">
+        <v>0</v>
+      </c>
+      <c r="F399" s="7">
+        <v>0</v>
+      </c>
+      <c r="G399" s="7">
+        <v>10.0802890497432</v>
+      </c>
+      <c r="H399" s="7">
+        <v>0</v>
+      </c>
+      <c r="I399" s="7">
+        <v>0</v>
+      </c>
+      <c r="J399" s="7">
+        <v>10.4373054508787</v>
+      </c>
+      <c r="K399" s="7">
+        <v>0</v>
+      </c>
+      <c r="L399" s="7">
+        <v>0</v>
+      </c>
+      <c r="M399" s="7">
+        <v>0</v>
+      </c>
+      <c r="N399" s="7">
+        <v>0</v>
+      </c>
+      <c r="O399" s="7">
+        <v>1.79494433720112</v>
+      </c>
+      <c r="P399" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q399" s="7">
+        <v>0</v>
+      </c>
+      <c r="R399" s="7">
+        <v>0</v>
+      </c>
+      <c r="S399" s="7">
+        <v>2.8009021525555502</v>
+      </c>
+      <c r="T399" t="b">
+        <v>0</v>
+      </c>
+      <c r="U399" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V399" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W399" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="400" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A400" s="10">
+        <v>399</v>
+      </c>
+      <c r="B400" s="7">
+        <v>7.8385966870765902</v>
+      </c>
+      <c r="C400" s="7">
+        <v>0</v>
+      </c>
+      <c r="D400" s="7">
+        <v>0</v>
+      </c>
+      <c r="E400" s="7">
+        <v>0</v>
+      </c>
+      <c r="F400" s="7">
+        <v>0</v>
+      </c>
+      <c r="G400" s="7">
+        <v>0</v>
+      </c>
+      <c r="H400" s="7">
+        <v>0</v>
+      </c>
+      <c r="I400" s="7">
+        <v>0</v>
+      </c>
+      <c r="J400" s="7">
+        <v>11.920632318821699</v>
+      </c>
+      <c r="K400" s="7">
+        <v>0</v>
+      </c>
+      <c r="L400" s="7">
+        <v>0</v>
+      </c>
+      <c r="M400" s="7">
+        <v>0</v>
+      </c>
+      <c r="N400" s="7">
+        <v>0</v>
+      </c>
+      <c r="O400" s="7">
+        <v>2.8353067782827401</v>
+      </c>
+      <c r="P400" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q400" s="7">
+        <v>0</v>
+      </c>
+      <c r="R400" s="7">
+        <v>0</v>
+      </c>
+      <c r="S400" s="7">
+        <v>1.7432539232089701</v>
+      </c>
+      <c r="T400" t="b">
+        <v>0</v>
+      </c>
+      <c r="U400" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V400" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W400" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="401" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A401" s="10">
+        <v>400</v>
+      </c>
+      <c r="B401" s="7">
+        <v>0</v>
+      </c>
+      <c r="C401" s="7">
+        <v>0</v>
+      </c>
+      <c r="D401" s="7">
+        <v>0</v>
+      </c>
+      <c r="E401" s="7">
+        <v>0</v>
+      </c>
+      <c r="F401" s="7">
+        <v>0</v>
+      </c>
+      <c r="G401" s="7">
+        <v>0</v>
+      </c>
+      <c r="H401" s="7">
+        <v>0</v>
+      </c>
+      <c r="I401" s="7">
+        <v>6.7102235897462101</v>
+      </c>
+      <c r="J401" s="7">
+        <v>0</v>
+      </c>
+      <c r="K401" s="7">
+        <v>0</v>
+      </c>
+      <c r="L401" s="7">
+        <v>12.7906139164501</v>
+      </c>
+      <c r="M401" s="7">
+        <v>0</v>
+      </c>
+      <c r="N401" s="7">
+        <v>0</v>
+      </c>
+      <c r="O401" s="7">
+        <v>1.69330172901264</v>
+      </c>
+      <c r="P401" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q401" s="7">
+        <v>0</v>
+      </c>
+      <c r="R401" s="7">
+        <v>0</v>
+      </c>
+      <c r="S401" s="7">
+        <v>3.7340114880366699</v>
+      </c>
+      <c r="T401" t="b">
+        <v>0</v>
+      </c>
+      <c r="U401" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V401" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W401" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="402" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A402" s="10">
+        <v>401</v>
+      </c>
+      <c r="B402" s="7">
+        <v>0</v>
+      </c>
+      <c r="C402" s="7">
+        <v>0</v>
+      </c>
+      <c r="D402" s="7">
+        <v>0</v>
+      </c>
+      <c r="E402" s="7">
+        <v>10.5637424729575</v>
+      </c>
+      <c r="F402" s="7">
+        <v>0</v>
+      </c>
+      <c r="G402" s="7">
+        <v>0</v>
+      </c>
+      <c r="H402" s="7">
+        <v>0</v>
+      </c>
+      <c r="I402" s="7">
+        <v>0</v>
+      </c>
+      <c r="J402" s="7">
+        <v>0</v>
+      </c>
+      <c r="K402" s="7">
+        <v>0</v>
+      </c>
+      <c r="L402" s="7">
+        <v>0</v>
+      </c>
+      <c r="M402" s="7">
+        <v>12.902615170474901</v>
+      </c>
+      <c r="N402" s="7">
+        <v>0</v>
+      </c>
+      <c r="O402" s="7">
+        <v>2.9211027094525899</v>
+      </c>
+      <c r="P402" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q402" s="7">
+        <v>0</v>
+      </c>
+      <c r="R402" s="7">
+        <v>0</v>
+      </c>
+      <c r="S402" s="7">
+        <v>4.4388818003947996</v>
+      </c>
+      <c r="T402" t="b">
+        <v>0</v>
+      </c>
+      <c r="U402" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V402" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W402" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="403" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A403" s="10">
+        <v>402</v>
+      </c>
+      <c r="B403" s="7">
+        <v>6.2787110046145997</v>
+      </c>
+      <c r="C403" s="7">
+        <v>11.1355281434939</v>
+      </c>
+      <c r="D403" s="7">
+        <v>0</v>
+      </c>
+      <c r="E403" s="7">
+        <v>0</v>
+      </c>
+      <c r="F403" s="7">
+        <v>0</v>
+      </c>
+      <c r="G403" s="7">
+        <v>0</v>
+      </c>
+      <c r="H403" s="7">
+        <v>0</v>
+      </c>
+      <c r="I403" s="7">
+        <v>0</v>
+      </c>
+      <c r="J403" s="7">
+        <v>0</v>
+      </c>
+      <c r="K403" s="7">
+        <v>0</v>
+      </c>
+      <c r="L403" s="7">
+        <v>0</v>
+      </c>
+      <c r="M403" s="7">
+        <v>0</v>
+      </c>
+      <c r="N403" s="7">
+        <v>0</v>
+      </c>
+      <c r="O403" s="7">
+        <v>1.6870137003803201</v>
+      </c>
+      <c r="P403" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q403" s="7">
+        <v>0</v>
+      </c>
+      <c r="R403" s="7">
+        <v>0</v>
+      </c>
+      <c r="S403" s="7">
+        <v>4.3815322812520998</v>
+      </c>
+      <c r="T403" t="b">
+        <v>0</v>
+      </c>
+      <c r="U403" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V403" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W403" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="404" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A404" s="10">
+        <v>403</v>
+      </c>
+      <c r="B404" s="7">
+        <v>0</v>
+      </c>
+      <c r="C404" s="7">
+        <v>0</v>
+      </c>
+      <c r="D404" s="7">
+        <v>0</v>
+      </c>
+      <c r="E404" s="7">
+        <v>0</v>
+      </c>
+      <c r="F404" s="7">
+        <v>0</v>
+      </c>
+      <c r="G404" s="7">
+        <v>0</v>
+      </c>
+      <c r="H404" s="7">
+        <v>0</v>
+      </c>
+      <c r="I404" s="7">
+        <v>0</v>
+      </c>
+      <c r="J404" s="7">
+        <v>0</v>
+      </c>
+      <c r="K404" s="7">
+        <v>0</v>
+      </c>
+      <c r="L404" s="7">
+        <v>12.471244476744101</v>
+      </c>
+      <c r="M404" s="7">
+        <v>10.373680477163401</v>
+      </c>
+      <c r="N404" s="7">
+        <v>0</v>
+      </c>
+      <c r="O404" s="7">
+        <v>2.4592561212270101</v>
+      </c>
+      <c r="P404" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q404" s="7">
+        <v>0</v>
+      </c>
+      <c r="R404" s="7">
+        <v>0</v>
+      </c>
+      <c r="S404" s="7">
+        <v>4.0849933738854203</v>
+      </c>
+      <c r="T404" t="b">
+        <v>0</v>
+      </c>
+      <c r="U404" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V404" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W404" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="405" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A405" s="10">
+        <v>404</v>
+      </c>
+      <c r="B405" s="7">
+        <v>0</v>
+      </c>
+      <c r="C405" s="7">
+        <v>8.3556737799734098</v>
+      </c>
+      <c r="D405" s="7">
+        <v>0</v>
+      </c>
+      <c r="E405" s="7">
+        <v>0</v>
+      </c>
+      <c r="F405" s="7">
+        <v>7.8488493545088298</v>
+      </c>
+      <c r="G405" s="7">
+        <v>0</v>
+      </c>
+      <c r="H405" s="7">
+        <v>0</v>
+      </c>
+      <c r="I405" s="7">
+        <v>0</v>
+      </c>
+      <c r="J405" s="7">
+        <v>0</v>
+      </c>
+      <c r="K405" s="7">
+        <v>0</v>
+      </c>
+      <c r="L405" s="7">
+        <v>0</v>
+      </c>
+      <c r="M405" s="7">
+        <v>0</v>
+      </c>
+      <c r="N405" s="7">
+        <v>0</v>
+      </c>
+      <c r="O405" s="7">
+        <v>1.86099593725273</v>
+      </c>
+      <c r="P405" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q405" s="7">
+        <v>0</v>
+      </c>
+      <c r="R405" s="7">
+        <v>0</v>
+      </c>
+      <c r="S405" s="7">
+        <v>2.25695251964691</v>
+      </c>
+      <c r="T405" t="b">
+        <v>0</v>
+      </c>
+      <c r="U405" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V405" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W405" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="406" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A406" s="10">
+        <v>405</v>
+      </c>
+      <c r="B406" s="7">
+        <v>6.9158064983111904</v>
+      </c>
+      <c r="C406" s="7">
+        <v>0</v>
+      </c>
+      <c r="D406" s="7">
+        <v>0</v>
+      </c>
+      <c r="E406" s="7">
+        <v>0</v>
+      </c>
+      <c r="F406" s="7">
+        <v>0</v>
+      </c>
+      <c r="G406" s="7">
+        <v>9.3523902492170805</v>
+      </c>
+      <c r="H406" s="7">
+        <v>0</v>
+      </c>
+      <c r="I406" s="7">
+        <v>0</v>
+      </c>
+      <c r="J406" s="7">
+        <v>0</v>
+      </c>
+      <c r="K406" s="7">
+        <v>0</v>
+      </c>
+      <c r="L406" s="7">
+        <v>0</v>
+      </c>
+      <c r="M406" s="7">
+        <v>0</v>
+      </c>
+      <c r="N406" s="7">
+        <v>0</v>
+      </c>
+      <c r="O406" s="7">
+        <v>3.4849932804675499</v>
+      </c>
+      <c r="P406" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q406" s="7">
+        <v>0</v>
+      </c>
+      <c r="R406" s="7">
+        <v>0</v>
+      </c>
+      <c r="S406" s="7">
+        <v>2.96724455118646</v>
+      </c>
+      <c r="T406" t="b">
+        <v>0</v>
+      </c>
+      <c r="U406" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V406" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W406" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="407" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A407" s="10">
+        <v>406</v>
+      </c>
+      <c r="B407" s="7">
+        <v>0</v>
+      </c>
+      <c r="C407" s="7">
+        <v>0</v>
+      </c>
+      <c r="D407" s="7">
+        <v>0</v>
+      </c>
+      <c r="E407" s="7">
+        <v>0</v>
+      </c>
+      <c r="F407" s="7">
+        <v>0</v>
+      </c>
+      <c r="G407" s="7">
+        <v>0</v>
+      </c>
+      <c r="H407" s="7">
+        <v>9.90563141609044</v>
+      </c>
+      <c r="I407" s="7">
+        <v>0</v>
+      </c>
+      <c r="J407" s="7">
+        <v>0</v>
+      </c>
+      <c r="K407" s="7">
+        <v>0</v>
+      </c>
+      <c r="L407" s="7">
+        <v>0</v>
+      </c>
+      <c r="M407" s="7">
+        <v>10.8640173442038</v>
+      </c>
+      <c r="N407" s="7">
+        <v>0</v>
+      </c>
+      <c r="O407" s="7">
+        <v>2.96030364159023</v>
+      </c>
+      <c r="P407" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q407" s="7">
+        <v>0</v>
+      </c>
+      <c r="R407" s="7">
+        <v>0</v>
+      </c>
+      <c r="S407" s="7">
+        <v>4.82163168379408</v>
+      </c>
+      <c r="T407" t="b">
+        <v>0</v>
+      </c>
+      <c r="U407" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V407" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W407" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="408" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A408" s="10">
+        <v>407</v>
+      </c>
+      <c r="B408" s="7">
+        <v>0</v>
+      </c>
+      <c r="C408" s="7">
+        <v>0</v>
+      </c>
+      <c r="D408" s="7">
+        <v>0</v>
+      </c>
+      <c r="E408" s="7">
+        <v>0</v>
+      </c>
+      <c r="F408" s="7">
+        <v>0</v>
+      </c>
+      <c r="G408" s="7">
+        <v>0</v>
+      </c>
+      <c r="H408" s="7">
+        <v>0</v>
+      </c>
+      <c r="I408" s="7">
+        <v>0</v>
+      </c>
+      <c r="J408" s="7">
+        <v>9.9102575645907702</v>
+      </c>
+      <c r="K408" s="7">
+        <v>11.4788643071459</v>
+      </c>
+      <c r="L408" s="7">
+        <v>0</v>
+      </c>
+      <c r="M408" s="7">
+        <v>0</v>
+      </c>
+      <c r="N408" s="7">
+        <v>0</v>
+      </c>
+      <c r="O408" s="7">
+        <v>3.3697882943419302</v>
+      </c>
+      <c r="P408" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q408" s="7">
+        <v>0</v>
+      </c>
+      <c r="R408" s="7">
+        <v>0</v>
+      </c>
+      <c r="S408" s="7">
+        <v>4.9425178437342998</v>
+      </c>
+      <c r="T408" t="b">
+        <v>0</v>
+      </c>
+      <c r="U408" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V408" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W408" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="409" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A409" s="10">
+        <v>408</v>
+      </c>
+      <c r="B409" s="7">
+        <v>0</v>
+      </c>
+      <c r="C409" s="7">
+        <v>0</v>
+      </c>
+      <c r="D409" s="7">
+        <v>9.3672186683497003</v>
+      </c>
+      <c r="E409" s="7">
+        <v>0</v>
+      </c>
+      <c r="F409" s="7">
+        <v>0</v>
+      </c>
+      <c r="G409" s="7">
+        <v>0</v>
+      </c>
+      <c r="H409" s="7">
+        <v>0</v>
+      </c>
+      <c r="I409" s="7">
+        <v>11.1679263913735</v>
+      </c>
+      <c r="J409" s="7">
+        <v>0</v>
+      </c>
+      <c r="K409" s="7">
+        <v>0</v>
+      </c>
+      <c r="L409" s="7">
+        <v>0</v>
+      </c>
+      <c r="M409" s="7">
+        <v>0</v>
+      </c>
+      <c r="N409" s="7">
+        <v>0</v>
+      </c>
+      <c r="O409" s="7">
+        <v>4.8629920631332899</v>
+      </c>
+      <c r="P409" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q409" s="7">
+        <v>0</v>
+      </c>
+      <c r="R409" s="7">
+        <v>0</v>
+      </c>
+      <c r="S409" s="7">
+        <v>2.6833690414054798</v>
+      </c>
+      <c r="T409" t="b">
+        <v>0</v>
+      </c>
+      <c r="U409" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V409" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W409" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W385">
+  <conditionalFormatting sqref="A1:W409">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
@@ -38572,7 +40358,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
AC: fixed an issue I created - overwrote Simon's git commit somehow
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45870AE-5944-1A49-85FF-111199287A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ECC814-9E0C-3744-96E3-E8BF045158B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -723,9 +723,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
   <dimension ref="A1:W421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A386" zoomScale="67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W409" sqref="W409"/>
+      <selection pane="topRight" activeCell="B368" sqref="B368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
dataset fully updated till S420
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ECC814-9E0C-3744-96E3-E8BF045158B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9455394-2F73-F64F-8CF9-61E3B2F7F20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -35,28 +35,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -390,7 +368,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -723,9 +711,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
   <dimension ref="A1:W421"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A354" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A367" zoomScale="75" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B368" sqref="B368"/>
+      <selection activeCell="A390" sqref="A390"/>
+      <selection pane="topRight" activeCell="W421" sqref="W421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27374,15 +27363,15 @@
         <v>0</v>
       </c>
       <c r="U366" s="2" t="str">
-        <f t="shared" ref="U366:U409" si="22">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="U366:U421" si="22">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V366" s="2" t="str">
-        <f t="shared" ref="V366:V409" si="23">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="V366:V421" si="23">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W366" s="2" t="str">
-        <f t="shared" ref="W366:W409" si="24">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="W366:W421" si="24">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -29202,17 +29191,14 @@
       <c r="T391" t="b">
         <v>1</v>
       </c>
-      <c r="U391" s="2" t="str">
-        <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="V391" s="2" t="str">
-        <f t="shared" si="23"/>
-        <v/>
-      </c>
-      <c r="W391" s="2" t="str">
-        <f t="shared" si="24"/>
-        <v/>
+      <c r="U391" s="2">
+        <v>40</v>
+      </c>
+      <c r="V391" s="2">
+        <v>89</v>
+      </c>
+      <c r="W391" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="392" spans="1:23" x14ac:dyDescent="0.2">
@@ -30548,212 +30534,889 @@
       </c>
     </row>
     <row r="410" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A410" s="10"/>
+      <c r="A410" s="10">
+        <v>409</v>
+      </c>
+      <c r="B410" s="7">
+        <v>5.4836737793905002</v>
+      </c>
+      <c r="C410" s="7">
+        <v>0</v>
+      </c>
+      <c r="D410" s="7">
+        <v>0</v>
+      </c>
+      <c r="E410" s="7">
+        <v>7.4399663098640501</v>
+      </c>
+      <c r="F410" s="7">
+        <v>0</v>
+      </c>
+      <c r="G410" s="7">
+        <v>0</v>
+      </c>
+      <c r="H410" s="7">
+        <v>0</v>
+      </c>
+      <c r="I410" s="7">
+        <v>0</v>
+      </c>
+      <c r="J410" s="7">
+        <v>0</v>
+      </c>
+      <c r="K410" s="7">
+        <v>0</v>
+      </c>
+      <c r="L410" s="7">
+        <v>0</v>
+      </c>
+      <c r="M410" s="7">
+        <v>0</v>
+      </c>
+      <c r="N410" s="7">
+        <v>0</v>
+      </c>
+      <c r="O410" s="7">
+        <v>1.7446392164109401</v>
+      </c>
+      <c r="P410" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q410" s="7">
+        <v>0</v>
+      </c>
+      <c r="R410" s="7">
+        <v>0</v>
+      </c>
+      <c r="S410" s="7">
+        <v>1.41450180298392</v>
+      </c>
+      <c r="T410" t="b">
+        <v>0</v>
+      </c>
+      <c r="U410" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V410" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W410" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="411" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A411" s="10"/>
+      <c r="A411" s="10">
+        <v>410</v>
+      </c>
+      <c r="B411" s="7">
+        <v>0</v>
+      </c>
+      <c r="C411" s="7">
+        <v>0</v>
+      </c>
+      <c r="D411" s="7">
+        <v>0</v>
+      </c>
+      <c r="E411" s="7">
+        <v>0</v>
+      </c>
+      <c r="F411" s="7">
+        <v>0</v>
+      </c>
+      <c r="G411" s="7">
+        <v>0</v>
+      </c>
+      <c r="H411" s="7">
+        <v>0</v>
+      </c>
+      <c r="I411" s="7">
+        <v>10.918539070636299</v>
+      </c>
+      <c r="J411" s="7">
+        <v>0</v>
+      </c>
+      <c r="K411" s="7">
+        <v>12.2626509448958</v>
+      </c>
+      <c r="L411" s="7">
+        <v>0</v>
+      </c>
+      <c r="M411" s="7">
+        <v>0</v>
+      </c>
+      <c r="N411" s="7">
+        <v>0</v>
+      </c>
+      <c r="O411" s="7">
+        <v>1.3234063646893</v>
+      </c>
+      <c r="P411" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q411" s="7">
+        <v>0</v>
+      </c>
+      <c r="R411" s="7">
+        <v>0</v>
+      </c>
+      <c r="S411" s="7">
+        <v>4.57516922307319</v>
+      </c>
+      <c r="T411" t="b">
+        <v>0</v>
+      </c>
+      <c r="U411" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V411" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W411" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="412" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A412" s="10"/>
-      <c r="B412" s="7" cm="1">
-        <f t="array" ref="B412">MIN(IF(B2:B409&gt;0,B2:B409))</f>
-        <v>3.9621170145865401</v>
-      </c>
-      <c r="C412" s="7" cm="1">
-        <f t="array" ref="C412">MIN(IF(C2:C409&gt;0,C2:C409))</f>
-        <v>8.2485917419671395</v>
-      </c>
-      <c r="D412" s="7" cm="1">
-        <f t="array" ref="D412">MIN(IF(D2:D409&gt;0,D2:D409))</f>
-        <v>6.0617436123523101</v>
-      </c>
-      <c r="E412" s="7" cm="1">
-        <f t="array" ref="E412">MIN(IF(E2:E409&gt;0,E2:E409))</f>
-        <v>6.5840255421615099</v>
-      </c>
-      <c r="F412" s="7" cm="1">
-        <f t="array" ref="F412">MIN(IF(F2:F409&gt;0,F2:F409))</f>
-        <v>6.7216799284721196</v>
-      </c>
-      <c r="G412" s="7" cm="1">
-        <f t="array" ref="G412">MIN(IF(G2:G409&gt;0,G2:G409))</f>
-        <v>7.5859787297801304</v>
-      </c>
-      <c r="H412" s="7" cm="1">
-        <f t="array" ref="H412">MIN(IF(H2:H409&gt;0,H2:H409))</f>
-        <v>7.6936050225384003</v>
-      </c>
-      <c r="I412" s="7" cm="1">
-        <f t="array" ref="I412">MIN(IF(I2:I409&gt;0,I2:I409))</f>
-        <v>6.3013595158887803</v>
-      </c>
-      <c r="J412" s="7" cm="1">
-        <f t="array" ref="J412">MIN(IF(J2:J409&gt;0,J2:J409))</f>
-        <v>7.9649584843580401</v>
-      </c>
-      <c r="K412" s="7" cm="1">
-        <f t="array" ref="K412">MIN(IF(K2:K409&gt;0,K2:K409))</f>
-        <v>7.8022593571000396</v>
-      </c>
-      <c r="L412" s="7" cm="1">
-        <f t="array" ref="L412">MIN(IF(L2:L409&gt;0,L2:L409))</f>
-        <v>7.7308087686644997</v>
-      </c>
-      <c r="M412" s="7" cm="1">
-        <f t="array" ref="M412">MIN(IF(M2:M409&gt;0,M2:M409))</f>
-        <v>7.8896744316926899</v>
-      </c>
-      <c r="N412" s="7" cm="1">
-        <f t="array" ref="N412">MIN(IF(N2:N409&gt;0,N2:N409))</f>
-        <v>0.295416728640995</v>
-      </c>
-      <c r="O412" s="7" cm="1">
-        <f t="array" ref="O412">MIN(IF(O2:O409&gt;0,O2:O409))</f>
-        <v>1.27054282567254</v>
-      </c>
-      <c r="P412" s="7" cm="1">
-        <f t="array" ref="P412">MIN(IF(P2:P409&gt;0,P2:P409))</f>
-        <v>0.95536107304973705</v>
-      </c>
-      <c r="Q412" s="7" cm="1">
-        <f t="array" ref="Q412">MIN(IF(Q2:Q409&gt;0,Q2:Q409))</f>
-        <v>0</v>
-      </c>
-      <c r="R412" s="7" cm="1">
-        <f t="array" ref="R412">MIN(IF(R2:R409&gt;0,R2:R409))</f>
-        <v>1.0352734146981399</v>
-      </c>
-      <c r="S412" s="7" cm="1">
-        <f t="array" ref="S412">MIN(IF(S2:S409&gt;0,S2:S409))</f>
-        <v>0.91866605487075703</v>
-      </c>
-      <c r="T412" s="7" cm="1">
-        <f t="array" ref="T412">MIN(IF(T2:T409&gt;0,T2:T409))</f>
-        <v>0</v>
-      </c>
-      <c r="U412" s="7" cm="1">
-        <f t="array" ref="U412">MIN(IF(U2:U409&gt;0,U2:U409))</f>
-        <v>14</v>
-      </c>
-      <c r="V412" s="7" cm="1">
-        <f t="array" ref="V412">MIN(IF(V2:V409&gt;0,V2:V409))</f>
-        <v>2</v>
-      </c>
-      <c r="W412" s="7"/>
+      <c r="A412" s="10">
+        <v>411</v>
+      </c>
+      <c r="B412" s="7">
+        <v>0</v>
+      </c>
+      <c r="C412" s="7">
+        <v>0</v>
+      </c>
+      <c r="D412" s="7">
+        <v>0</v>
+      </c>
+      <c r="E412" s="7">
+        <v>13.018558622918899</v>
+      </c>
+      <c r="F412" s="7">
+        <v>0</v>
+      </c>
+      <c r="G412" s="7">
+        <v>0</v>
+      </c>
+      <c r="H412" s="7">
+        <v>0</v>
+      </c>
+      <c r="I412" s="7">
+        <v>0</v>
+      </c>
+      <c r="J412" s="7">
+        <v>12.2476474981246</v>
+      </c>
+      <c r="K412" s="7">
+        <v>0</v>
+      </c>
+      <c r="L412" s="7">
+        <v>0</v>
+      </c>
+      <c r="M412" s="7">
+        <v>0</v>
+      </c>
+      <c r="N412" s="7">
+        <v>0</v>
+      </c>
+      <c r="O412" s="7">
+        <v>2.5088046362959</v>
+      </c>
+      <c r="P412" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q412" s="7">
+        <v>0</v>
+      </c>
+      <c r="R412" s="7">
+        <v>0</v>
+      </c>
+      <c r="S412" s="7">
+        <v>1.94399521555911</v>
+      </c>
+      <c r="T412" t="b">
+        <v>0</v>
+      </c>
+      <c r="U412" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V412" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W412" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="413" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A413" s="10"/>
+      <c r="A413" s="10">
+        <v>412</v>
+      </c>
       <c r="B413" s="7">
-        <f>MAX(B2:B409)</f>
-        <v>12.244958900697901</v>
+        <v>0</v>
       </c>
       <c r="C413" s="7">
-        <f t="shared" ref="C413:V413" si="25">MAX(C2:C409)</f>
-        <v>13.488219238295001</v>
+        <v>0</v>
       </c>
       <c r="D413" s="7">
-        <f t="shared" si="25"/>
-        <v>13.577247953314901</v>
+        <v>0</v>
       </c>
       <c r="E413" s="7">
-        <f>MAX(E2:E409)</f>
-        <v>14.4543180189381</v>
+        <v>0</v>
       </c>
       <c r="F413" s="7">
-        <f t="shared" si="25"/>
-        <v>13.909598487475201</v>
+        <v>0</v>
       </c>
       <c r="G413" s="7">
-        <f t="shared" si="25"/>
-        <v>13.7389913042143</v>
+        <v>0</v>
       </c>
       <c r="H413" s="7">
-        <f t="shared" si="25"/>
-        <v>13.304211345061701</v>
+        <v>7.7620811955363997</v>
       </c>
       <c r="I413" s="7">
-        <f t="shared" si="25"/>
-        <v>14.3881865612897</v>
+        <v>11.4344844689845</v>
       </c>
       <c r="J413" s="7">
-        <f t="shared" si="25"/>
-        <v>13.515049563038</v>
+        <v>0</v>
       </c>
       <c r="K413" s="7">
-        <f t="shared" si="25"/>
-        <v>13.195638329590601</v>
+        <v>0</v>
       </c>
       <c r="L413" s="7">
-        <f t="shared" si="25"/>
-        <v>13.182329962527101</v>
+        <v>0</v>
       </c>
       <c r="M413" s="7">
-        <f t="shared" si="25"/>
-        <v>13.303807174445399</v>
+        <v>0</v>
       </c>
       <c r="N413" s="7">
-        <f t="shared" si="25"/>
-        <v>3.08375949176355</v>
+        <v>0</v>
       </c>
       <c r="O413" s="7">
-        <f t="shared" si="25"/>
-        <v>4.8629920631332899</v>
+        <v>1.7941843977985701</v>
       </c>
       <c r="P413" s="7">
-        <f t="shared" si="25"/>
-        <v>4.0235072833486401</v>
+        <v>0</v>
       </c>
       <c r="Q413" s="7">
-        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="R413" s="7">
-        <f t="shared" si="25"/>
-        <v>5.1676601961316297</v>
+        <v>0</v>
       </c>
       <c r="S413" s="7">
-        <f t="shared" si="25"/>
-        <v>5.52361716601445</v>
-      </c>
-      <c r="T413" s="7">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="U413" s="7">
-        <f t="shared" si="25"/>
-        <v>2910</v>
-      </c>
-      <c r="V413" s="7">
-        <f t="shared" si="25"/>
-        <v>2100</v>
+        <v>1.96563405088563</v>
+      </c>
+      <c r="T413" t="b">
+        <v>0</v>
+      </c>
+      <c r="U413" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V413" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W413" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
       </c>
     </row>
     <row r="414" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A414" s="10"/>
+      <c r="A414" s="10">
+        <v>413</v>
+      </c>
+      <c r="B414" s="7">
+        <v>0</v>
+      </c>
+      <c r="C414" s="7">
+        <v>0</v>
+      </c>
+      <c r="D414" s="7">
+        <v>8.0193771230817301</v>
+      </c>
+      <c r="E414" s="7">
+        <v>0</v>
+      </c>
+      <c r="F414" s="7">
+        <v>0</v>
+      </c>
+      <c r="G414" s="7">
+        <v>0</v>
+      </c>
+      <c r="H414" s="7">
+        <v>0</v>
+      </c>
+      <c r="I414" s="7">
+        <v>0</v>
+      </c>
+      <c r="J414" s="7">
+        <v>0</v>
+      </c>
+      <c r="K414" s="7">
+        <v>9.5260844784134502</v>
+      </c>
+      <c r="L414" s="7">
+        <v>0</v>
+      </c>
+      <c r="M414" s="7">
+        <v>0</v>
+      </c>
+      <c r="N414" s="7">
+        <v>0</v>
+      </c>
+      <c r="O414" s="7">
+        <v>2.6500382532150701</v>
+      </c>
+      <c r="P414" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q414" s="7">
+        <v>0</v>
+      </c>
+      <c r="R414" s="7">
+        <v>0</v>
+      </c>
+      <c r="S414" s="7">
+        <v>1.92228153594957</v>
+      </c>
+      <c r="T414" t="b">
+        <v>0</v>
+      </c>
+      <c r="U414" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V414" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W414" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="415" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A415" s="10"/>
+      <c r="A415" s="10">
+        <v>414</v>
+      </c>
+      <c r="B415" s="7">
+        <v>0</v>
+      </c>
+      <c r="C415" s="7">
+        <v>0</v>
+      </c>
+      <c r="D415" s="7">
+        <v>0</v>
+      </c>
+      <c r="E415" s="7">
+        <v>0</v>
+      </c>
+      <c r="F415" s="7">
+        <v>12.4898159581693</v>
+      </c>
+      <c r="G415" s="7">
+        <v>0</v>
+      </c>
+      <c r="H415" s="7">
+        <v>0</v>
+      </c>
+      <c r="I415" s="7">
+        <v>0</v>
+      </c>
+      <c r="J415" s="7">
+        <v>0</v>
+      </c>
+      <c r="K415" s="7">
+        <v>0</v>
+      </c>
+      <c r="L415" s="7">
+        <v>0</v>
+      </c>
+      <c r="M415" s="7">
+        <v>7.8363427637498697</v>
+      </c>
+      <c r="N415" s="7">
+        <v>0</v>
+      </c>
+      <c r="O415" s="7">
+        <v>3.0318306198600702</v>
+      </c>
+      <c r="P415" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q415" s="7">
+        <v>0</v>
+      </c>
+      <c r="R415" s="7">
+        <v>0</v>
+      </c>
+      <c r="S415" s="7">
+        <v>4.9314830981602604</v>
+      </c>
+      <c r="T415" t="b">
+        <v>0</v>
+      </c>
+      <c r="U415" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V415" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W415" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
     </row>
     <row r="416" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A416" s="10"/>
-    </row>
-    <row r="417" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A417" s="10"/>
-    </row>
-    <row r="418" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A418" s="10"/>
-    </row>
-    <row r="419" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A419" s="10"/>
-    </row>
-    <row r="420" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A420" s="10"/>
-    </row>
-    <row r="421" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A421" s="10"/>
+      <c r="A416" s="10">
+        <v>415</v>
+      </c>
+      <c r="B416" s="7">
+        <v>0</v>
+      </c>
+      <c r="C416" s="7">
+        <v>0</v>
+      </c>
+      <c r="D416" s="7">
+        <v>0</v>
+      </c>
+      <c r="E416" s="7">
+        <v>0</v>
+      </c>
+      <c r="F416" s="7">
+        <v>8.1990641689913506</v>
+      </c>
+      <c r="G416" s="7">
+        <v>8.1749404053459696</v>
+      </c>
+      <c r="H416" s="7">
+        <v>0</v>
+      </c>
+      <c r="I416" s="7">
+        <v>0</v>
+      </c>
+      <c r="J416" s="7">
+        <v>0</v>
+      </c>
+      <c r="K416" s="7">
+        <v>0</v>
+      </c>
+      <c r="L416" s="7">
+        <v>0</v>
+      </c>
+      <c r="M416" s="7">
+        <v>0</v>
+      </c>
+      <c r="N416" s="7">
+        <v>0</v>
+      </c>
+      <c r="O416" s="7">
+        <v>1.6622780886931401</v>
+      </c>
+      <c r="P416" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q416" s="7">
+        <v>0</v>
+      </c>
+      <c r="R416" s="7">
+        <v>0</v>
+      </c>
+      <c r="S416" s="7">
+        <v>4.1211429560947801</v>
+      </c>
+      <c r="T416" t="b">
+        <v>0</v>
+      </c>
+      <c r="U416" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V416" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W416" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="417" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A417" s="10">
+        <v>416</v>
+      </c>
+      <c r="B417" s="7">
+        <v>6.9934728585953199</v>
+      </c>
+      <c r="C417" s="7">
+        <v>0</v>
+      </c>
+      <c r="D417" s="7">
+        <v>0</v>
+      </c>
+      <c r="E417" s="7">
+        <v>0</v>
+      </c>
+      <c r="F417" s="7">
+        <v>0</v>
+      </c>
+      <c r="G417" s="7">
+        <v>0</v>
+      </c>
+      <c r="H417" s="7">
+        <v>0</v>
+      </c>
+      <c r="I417" s="7">
+        <v>0</v>
+      </c>
+      <c r="J417" s="7">
+        <v>0</v>
+      </c>
+      <c r="K417" s="7">
+        <v>0</v>
+      </c>
+      <c r="L417" s="7">
+        <v>13.709208147101901</v>
+      </c>
+      <c r="M417" s="7">
+        <v>0</v>
+      </c>
+      <c r="N417" s="7">
+        <v>0</v>
+      </c>
+      <c r="O417" s="7">
+        <v>1.50866639634616</v>
+      </c>
+      <c r="P417" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q417" s="7">
+        <v>0</v>
+      </c>
+      <c r="R417" s="7">
+        <v>0</v>
+      </c>
+      <c r="S417" s="7">
+        <v>3.0581765529994702</v>
+      </c>
+      <c r="T417" t="b">
+        <v>0</v>
+      </c>
+      <c r="U417" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V417" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W417" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="418" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A418" s="10">
+        <v>417</v>
+      </c>
+      <c r="B418" s="7">
+        <v>0</v>
+      </c>
+      <c r="C418" s="7">
+        <v>0</v>
+      </c>
+      <c r="D418" s="7">
+        <v>9.93536527368828</v>
+      </c>
+      <c r="E418" s="7">
+        <v>0</v>
+      </c>
+      <c r="F418" s="7">
+        <v>0</v>
+      </c>
+      <c r="G418" s="7">
+        <v>0</v>
+      </c>
+      <c r="H418" s="7">
+        <v>0</v>
+      </c>
+      <c r="I418" s="7">
+        <v>0</v>
+      </c>
+      <c r="J418" s="7">
+        <v>0</v>
+      </c>
+      <c r="K418" s="7">
+        <v>0</v>
+      </c>
+      <c r="L418" s="7">
+        <v>0</v>
+      </c>
+      <c r="M418" s="7">
+        <v>11.323548013141099</v>
+      </c>
+      <c r="N418" s="7">
+        <v>0</v>
+      </c>
+      <c r="O418" s="7">
+        <v>2.89536679695789</v>
+      </c>
+      <c r="P418" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q418" s="7">
+        <v>0</v>
+      </c>
+      <c r="R418" s="7">
+        <v>0</v>
+      </c>
+      <c r="S418" s="7">
+        <v>2.5542960736704399</v>
+      </c>
+      <c r="T418" t="b">
+        <v>0</v>
+      </c>
+      <c r="U418" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V418" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W418" s="2" t="str">
+        <f t="shared" si="24"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="419" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A419" s="10">
+        <v>418</v>
+      </c>
+      <c r="B419" s="7">
+        <v>0</v>
+      </c>
+      <c r="C419" s="7">
+        <v>0</v>
+      </c>
+      <c r="D419" s="7">
+        <v>8.3780332188699997</v>
+      </c>
+      <c r="E419" s="7">
+        <v>0</v>
+      </c>
+      <c r="F419" s="7">
+        <v>0</v>
+      </c>
+      <c r="G419" s="7">
+        <v>0</v>
+      </c>
+      <c r="H419" s="7">
+        <v>0</v>
+      </c>
+      <c r="I419" s="7">
+        <v>0</v>
+      </c>
+      <c r="J419" s="7">
+        <v>11.7555856724296</v>
+      </c>
+      <c r="K419" s="7">
+        <v>0</v>
+      </c>
+      <c r="L419" s="7">
+        <v>0</v>
+      </c>
+      <c r="M419" s="7">
+        <v>0</v>
+      </c>
+      <c r="N419" s="7">
+        <v>0</v>
+      </c>
+      <c r="O419" s="7">
+        <v>1.44197031969977</v>
+      </c>
+      <c r="P419" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q419" s="7">
+        <v>0</v>
+      </c>
+      <c r="R419" s="7">
+        <v>0</v>
+      </c>
+      <c r="S419" s="7">
+        <v>4.0895020912342703</v>
+      </c>
+      <c r="T419" t="b">
+        <v>1</v>
+      </c>
+      <c r="U419" s="2">
+        <v>541</v>
+      </c>
+      <c r="V419" s="2">
+        <v>143</v>
+      </c>
+      <c r="W419" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A420" s="10">
+        <v>419</v>
+      </c>
+      <c r="B420" s="7">
+        <v>0</v>
+      </c>
+      <c r="C420" s="7">
+        <v>0</v>
+      </c>
+      <c r="D420" s="7">
+        <v>0</v>
+      </c>
+      <c r="E420" s="7">
+        <v>0</v>
+      </c>
+      <c r="F420" s="7">
+        <v>0</v>
+      </c>
+      <c r="G420" s="7">
+        <v>0</v>
+      </c>
+      <c r="H420" s="7">
+        <v>0</v>
+      </c>
+      <c r="I420" s="7">
+        <v>0</v>
+      </c>
+      <c r="J420" s="7">
+        <v>12.6874302522129</v>
+      </c>
+      <c r="K420" s="7">
+        <v>0</v>
+      </c>
+      <c r="L420" s="7">
+        <v>0</v>
+      </c>
+      <c r="M420" s="7">
+        <v>11.761476631917599</v>
+      </c>
+      <c r="N420" s="7">
+        <v>0</v>
+      </c>
+      <c r="O420" s="7">
+        <v>3.4158654895043798</v>
+      </c>
+      <c r="P420" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q420" s="7">
+        <v>0</v>
+      </c>
+      <c r="R420" s="7">
+        <v>0</v>
+      </c>
+      <c r="S420" s="7">
+        <v>1.6005348898001399</v>
+      </c>
+      <c r="T420" t="b">
+        <v>1</v>
+      </c>
+      <c r="U420" s="2">
+        <v>24</v>
+      </c>
+      <c r="V420" s="2">
+        <v>10</v>
+      </c>
+      <c r="W420" s="2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="421" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A421" s="10">
+        <v>420</v>
+      </c>
+      <c r="B421" s="7">
+        <v>0</v>
+      </c>
+      <c r="C421" s="7">
+        <v>11.3863539533486</v>
+      </c>
+      <c r="D421" s="7">
+        <v>0</v>
+      </c>
+      <c r="E421" s="7">
+        <v>0</v>
+      </c>
+      <c r="F421" s="7">
+        <v>0</v>
+      </c>
+      <c r="G421" s="7">
+        <v>0</v>
+      </c>
+      <c r="H421" s="7">
+        <v>0</v>
+      </c>
+      <c r="I421" s="7">
+        <v>0</v>
+      </c>
+      <c r="J421" s="7">
+        <v>0</v>
+      </c>
+      <c r="K421" s="7">
+        <v>0</v>
+      </c>
+      <c r="L421" s="7">
+        <v>9.2726204126961793</v>
+      </c>
+      <c r="M421" s="7">
+        <v>0</v>
+      </c>
+      <c r="N421" s="7">
+        <v>0</v>
+      </c>
+      <c r="O421" s="7">
+        <v>2.03449283984129</v>
+      </c>
+      <c r="P421" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q421" s="7">
+        <v>0</v>
+      </c>
+      <c r="R421" s="7">
+        <v>0</v>
+      </c>
+      <c r="S421" s="7">
+        <v>4.1419065699994801</v>
+      </c>
+      <c r="T421" t="b">
+        <v>0</v>
+      </c>
+      <c r="U421" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V421" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W421" s="2" t="str">
+        <f>IF(T421=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W409">
+  <conditionalFormatting sqref="A1:W421">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
@@ -40908,7 +41571,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
dataset updated till S450
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9455394-2F73-F64F-8CF9-61E3B2F7F20C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAE6D1B-D547-4C48-83FF-2F8B111E1D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -301,7 +301,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,21 +364,16 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -709,12 +704,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W421"/>
+  <dimension ref="A1:X451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A367" zoomScale="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A366" zoomScale="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
       <selection activeCell="A390" sqref="A390"/>
-      <selection pane="topRight" activeCell="W421" sqref="W421"/>
+      <selection pane="topRight" activeCell="E412" sqref="E412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27363,15 +27358,15 @@
         <v>0</v>
       </c>
       <c r="U366" s="2" t="str">
-        <f t="shared" ref="U366:U421" si="22">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="U366:U429" si="22">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V366" s="2" t="str">
-        <f t="shared" ref="V366:V421" si="23">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="V366:V429" si="23">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W366" s="2" t="str">
-        <f t="shared" ref="W366:W421" si="24">IF(T366=FALSE, "NA", "")</f>
+        <f t="shared" ref="W366:W418" si="24">IF(T366=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -28686,7 +28681,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="385" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A385" s="10">
         <v>384</v>
       </c>
@@ -28760,7 +28755,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="386" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A386" s="10">
         <v>385</v>
       </c>
@@ -28833,8 +28828,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="387" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X386" t="str">
+        <f>IF(COUNTIF(B386:M386,"&lt;&gt;0")&gt;=2, "At least two non-zero values", "Less than two non-zero values")</f>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="387" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A387" s="10">
         <v>386</v>
       </c>
@@ -28907,8 +28906,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="388" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X387" t="str">
+        <f t="shared" ref="X387:X450" si="25">IF(COUNTIF(B387:M387,"&lt;&gt;0")&gt;=2, "At least two non-zero values", "Less than two non-zero values")</f>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="388" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A388" s="10">
         <v>387</v>
       </c>
@@ -28981,8 +28984,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="389" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X388" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="389" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A389" s="10">
         <v>388</v>
       </c>
@@ -29055,82 +29062,90 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="390" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A390" s="10">
+      <c r="X389" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="390" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A390" s="24">
         <v>389</v>
       </c>
-      <c r="B390" s="7">
-        <v>0</v>
-      </c>
-      <c r="C390" s="7">
-        <v>0</v>
-      </c>
-      <c r="D390" s="7">
-        <v>0</v>
-      </c>
-      <c r="E390" s="7">
+      <c r="B390" s="23">
+        <v>0</v>
+      </c>
+      <c r="C390" s="23">
+        <v>0</v>
+      </c>
+      <c r="D390" s="23">
+        <v>0</v>
+      </c>
+      <c r="E390" s="23">
         <v>8.6945264536113207</v>
       </c>
-      <c r="F390" s="7">
-        <v>0</v>
-      </c>
-      <c r="G390" s="7">
-        <v>0</v>
-      </c>
-      <c r="H390" s="7">
-        <v>0</v>
-      </c>
-      <c r="I390" s="7">
-        <v>0</v>
-      </c>
-      <c r="J390" s="7">
-        <v>0</v>
-      </c>
-      <c r="K390" s="7">
-        <v>0</v>
-      </c>
-      <c r="L390" s="7">
-        <v>0</v>
-      </c>
-      <c r="M390" s="7">
-        <v>0</v>
-      </c>
-      <c r="N390" s="7">
-        <v>0</v>
-      </c>
-      <c r="O390" s="7">
+      <c r="F390" s="23">
+        <v>0</v>
+      </c>
+      <c r="G390" s="23">
+        <v>0</v>
+      </c>
+      <c r="H390" s="23">
+        <v>0</v>
+      </c>
+      <c r="I390" s="23">
+        <v>0</v>
+      </c>
+      <c r="J390" s="23">
+        <v>0</v>
+      </c>
+      <c r="K390" s="23">
+        <v>0</v>
+      </c>
+      <c r="L390" s="23">
+        <v>0</v>
+      </c>
+      <c r="M390" s="23">
+        <v>0</v>
+      </c>
+      <c r="N390" s="23">
+        <v>0</v>
+      </c>
+      <c r="O390" s="23">
         <v>2.9611932785208399</v>
       </c>
-      <c r="P390" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q390" s="7">
-        <v>0</v>
-      </c>
-      <c r="R390" s="7">
-        <v>0</v>
-      </c>
-      <c r="S390" s="7">
+      <c r="P390" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q390" s="23">
+        <v>0</v>
+      </c>
+      <c r="R390" s="23">
+        <v>0</v>
+      </c>
+      <c r="S390" s="23">
         <v>2.0062807880531799</v>
       </c>
-      <c r="T390" t="b">
-        <v>0</v>
-      </c>
-      <c r="U390" s="2" t="str">
+      <c r="T390" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="U390" s="26" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="V390" s="2" t="str">
+      <c r="V390" s="26" t="str">
         <f t="shared" si="23"/>
         <v>NA</v>
       </c>
-      <c r="W390" s="2" t="str">
+      <c r="W390" s="26" t="str">
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="391" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X390" s="25" t="str">
+        <f t="shared" si="25"/>
+        <v>Less than two non-zero values</v>
+      </c>
+    </row>
+    <row r="391" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A391" s="10">
         <v>390</v>
       </c>
@@ -29200,8 +29215,12 @@
       <c r="W391" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="392" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X391" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="392" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A392" s="10">
         <v>391</v>
       </c>
@@ -29274,8 +29293,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="393" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X392" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="393" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A393" s="10">
         <v>392</v>
       </c>
@@ -29348,8 +29371,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="394" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X393" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="394" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A394" s="10">
         <v>393</v>
       </c>
@@ -29422,8 +29449,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="395" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X394" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="395" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A395" s="10">
         <v>394</v>
       </c>
@@ -29496,8 +29527,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="396" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X395" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="396" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A396" s="10">
         <v>395</v>
       </c>
@@ -29570,8 +29605,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="397" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X396" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="397" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A397" s="10">
         <v>396</v>
       </c>
@@ -29644,8 +29683,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="398" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X397" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="398" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A398" s="10">
         <v>397</v>
       </c>
@@ -29718,82 +29761,90 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="399" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A399" s="10">
+      <c r="X398" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="399" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A399" s="24">
         <v>398</v>
       </c>
-      <c r="B399" s="7">
-        <v>0</v>
-      </c>
-      <c r="C399" s="7">
-        <v>0</v>
-      </c>
-      <c r="D399" s="7">
-        <v>0</v>
-      </c>
-      <c r="E399" s="7">
-        <v>0</v>
-      </c>
-      <c r="F399" s="7">
-        <v>0</v>
-      </c>
-      <c r="G399" s="7">
-        <v>0</v>
-      </c>
-      <c r="H399" s="7">
-        <v>0</v>
-      </c>
-      <c r="I399" s="7">
-        <v>0</v>
-      </c>
-      <c r="J399" s="7">
+      <c r="B399" s="23">
+        <v>0</v>
+      </c>
+      <c r="C399" s="23">
+        <v>0</v>
+      </c>
+      <c r="D399" s="23">
+        <v>0</v>
+      </c>
+      <c r="E399" s="23">
+        <v>0</v>
+      </c>
+      <c r="F399" s="23">
+        <v>0</v>
+      </c>
+      <c r="G399" s="23">
+        <v>0</v>
+      </c>
+      <c r="H399" s="23">
+        <v>0</v>
+      </c>
+      <c r="I399" s="23">
+        <v>0</v>
+      </c>
+      <c r="J399" s="23">
         <v>10.4373054508787</v>
       </c>
-      <c r="K399" s="7">
-        <v>0</v>
-      </c>
-      <c r="L399" s="7">
-        <v>0</v>
-      </c>
-      <c r="M399" s="7">
-        <v>0</v>
-      </c>
-      <c r="N399" s="7">
-        <v>0</v>
-      </c>
-      <c r="O399" s="7">
+      <c r="K399" s="23">
+        <v>0</v>
+      </c>
+      <c r="L399" s="23">
+        <v>0</v>
+      </c>
+      <c r="M399" s="23">
+        <v>0</v>
+      </c>
+      <c r="N399" s="23">
+        <v>0</v>
+      </c>
+      <c r="O399" s="23">
         <v>1.79494433720112</v>
       </c>
-      <c r="P399" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q399" s="7">
-        <v>0</v>
-      </c>
-      <c r="R399" s="7">
-        <v>0</v>
-      </c>
-      <c r="S399" s="7">
+      <c r="P399" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q399" s="23">
+        <v>0</v>
+      </c>
+      <c r="R399" s="23">
+        <v>0</v>
+      </c>
+      <c r="S399" s="23">
         <v>2.8009021525555502</v>
       </c>
-      <c r="T399" t="b">
-        <v>0</v>
-      </c>
-      <c r="U399" s="2" t="str">
+      <c r="T399" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="U399" s="26" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="V399" s="2" t="str">
+      <c r="V399" s="26" t="str">
         <f t="shared" si="23"/>
         <v>NA</v>
       </c>
-      <c r="W399" s="2" t="str">
+      <c r="W399" s="26" t="str">
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="400" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X399" s="25" t="str">
+        <f t="shared" si="25"/>
+        <v>Less than two non-zero values</v>
+      </c>
+    </row>
+    <row r="400" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A400" s="10">
         <v>399</v>
       </c>
@@ -29866,8 +29917,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="401" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X400" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="401" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A401" s="10">
         <v>400</v>
       </c>
@@ -29940,8 +29995,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="402" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X401" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="402" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A402" s="10">
         <v>401</v>
       </c>
@@ -30014,8 +30073,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="403" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X402" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="403" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A403" s="10">
         <v>402</v>
       </c>
@@ -30088,8 +30151,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="404" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X403" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="404" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A404" s="10">
         <v>403</v>
       </c>
@@ -30162,8 +30229,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="405" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X404" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="405" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A405" s="10">
         <v>404</v>
       </c>
@@ -30236,82 +30307,90 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="406" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A406" s="10">
+      <c r="X405" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="406" spans="1:24" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A406" s="24">
         <v>405</v>
       </c>
-      <c r="B406" s="7">
+      <c r="B406" s="23">
         <v>6.9158064983111904</v>
       </c>
-      <c r="C406" s="7">
-        <v>0</v>
-      </c>
-      <c r="D406" s="7">
-        <v>0</v>
-      </c>
-      <c r="E406" s="7">
-        <v>0</v>
-      </c>
-      <c r="F406" s="7">
-        <v>0</v>
-      </c>
-      <c r="G406" s="7">
-        <v>0</v>
-      </c>
-      <c r="H406" s="7">
-        <v>0</v>
-      </c>
-      <c r="I406" s="7">
-        <v>0</v>
-      </c>
-      <c r="J406" s="7">
-        <v>0</v>
-      </c>
-      <c r="K406" s="7">
-        <v>0</v>
-      </c>
-      <c r="L406" s="7">
-        <v>0</v>
-      </c>
-      <c r="M406" s="7">
-        <v>0</v>
-      </c>
-      <c r="N406" s="7">
-        <v>0</v>
-      </c>
-      <c r="O406" s="7">
+      <c r="C406" s="23">
+        <v>0</v>
+      </c>
+      <c r="D406" s="23">
+        <v>0</v>
+      </c>
+      <c r="E406" s="23">
+        <v>0</v>
+      </c>
+      <c r="F406" s="23">
+        <v>0</v>
+      </c>
+      <c r="G406" s="23">
+        <v>0</v>
+      </c>
+      <c r="H406" s="23">
+        <v>0</v>
+      </c>
+      <c r="I406" s="23">
+        <v>0</v>
+      </c>
+      <c r="J406" s="23">
+        <v>0</v>
+      </c>
+      <c r="K406" s="23">
+        <v>0</v>
+      </c>
+      <c r="L406" s="23">
+        <v>0</v>
+      </c>
+      <c r="M406" s="23">
+        <v>0</v>
+      </c>
+      <c r="N406" s="23">
+        <v>0</v>
+      </c>
+      <c r="O406" s="23">
         <v>3.4849932804675499</v>
       </c>
-      <c r="P406" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q406" s="7">
-        <v>0</v>
-      </c>
-      <c r="R406" s="7">
-        <v>0</v>
-      </c>
-      <c r="S406" s="7">
+      <c r="P406" s="23">
+        <v>0</v>
+      </c>
+      <c r="Q406" s="23">
+        <v>0</v>
+      </c>
+      <c r="R406" s="23">
+        <v>0</v>
+      </c>
+      <c r="S406" s="23">
         <v>2.96724455118646</v>
       </c>
-      <c r="T406" t="b">
-        <v>0</v>
-      </c>
-      <c r="U406" s="2" t="str">
+      <c r="T406" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="U406" s="26" t="str">
         <f t="shared" si="22"/>
         <v>NA</v>
       </c>
-      <c r="V406" s="2" t="str">
+      <c r="V406" s="26" t="str">
         <f t="shared" si="23"/>
         <v>NA</v>
       </c>
-      <c r="W406" s="2" t="str">
+      <c r="W406" s="26" t="str">
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="407" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X406" s="25" t="str">
+        <f t="shared" si="25"/>
+        <v>Less than two non-zero values</v>
+      </c>
+    </row>
+    <row r="407" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A407" s="10">
         <v>406</v>
       </c>
@@ -30384,8 +30463,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="408" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X407" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="408" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A408" s="10">
         <v>407</v>
       </c>
@@ -30458,8 +30541,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="409" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X408" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="409" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A409" s="10">
         <v>408</v>
       </c>
@@ -30532,8 +30619,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="410" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X409" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="410" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A410" s="10">
         <v>409</v>
       </c>
@@ -30606,8 +30697,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="411" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X410" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="411" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A411" s="10">
         <v>410</v>
       </c>
@@ -30680,8 +30775,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="412" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X411" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="412" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A412" s="10">
         <v>411</v>
       </c>
@@ -30754,8 +30853,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="413" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X412" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="413" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A413" s="10">
         <v>412</v>
       </c>
@@ -30828,8 +30931,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="414" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X413" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="414" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A414" s="10">
         <v>413</v>
       </c>
@@ -30902,8 +31009,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="415" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X414" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="415" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A415" s="10">
         <v>414</v>
       </c>
@@ -30976,8 +31087,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="416" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X415" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="416" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A416" s="10">
         <v>415</v>
       </c>
@@ -31050,8 +31165,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="417" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X416" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="417" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A417" s="10">
         <v>416</v>
       </c>
@@ -31124,8 +31243,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="418" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X417" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="418" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A418" s="10">
         <v>417</v>
       </c>
@@ -31198,8 +31321,12 @@
         <f t="shared" si="24"/>
         <v>NA</v>
       </c>
-    </row>
-    <row r="419" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X418" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="419" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A419" s="10">
         <v>418</v>
       </c>
@@ -31269,8 +31396,12 @@
       <c r="W419" s="2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="420" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X419" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="420" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A420" s="10">
         <v>419</v>
       </c>
@@ -31340,8 +31471,12 @@
       <c r="W420" s="2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="421" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X420" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="421" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A421" s="10">
         <v>420</v>
       </c>
@@ -31414,9 +31549,2350 @@
         <f>IF(T421=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
+      <c r="X421" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="422" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A422" s="10">
+        <v>421</v>
+      </c>
+      <c r="B422" s="7">
+        <v>0</v>
+      </c>
+      <c r="C422" s="7">
+        <v>0</v>
+      </c>
+      <c r="D422" s="7">
+        <v>12.392116082873001</v>
+      </c>
+      <c r="E422" s="7">
+        <v>0</v>
+      </c>
+      <c r="F422" s="7">
+        <v>0</v>
+      </c>
+      <c r="G422" s="7">
+        <v>0</v>
+      </c>
+      <c r="H422" s="7">
+        <v>12.628857423997101</v>
+      </c>
+      <c r="I422" s="7">
+        <v>0</v>
+      </c>
+      <c r="J422" s="7">
+        <v>0</v>
+      </c>
+      <c r="K422" s="7">
+        <v>0</v>
+      </c>
+      <c r="L422" s="7">
+        <v>0</v>
+      </c>
+      <c r="M422" s="7">
+        <v>0</v>
+      </c>
+      <c r="N422" s="7">
+        <v>0</v>
+      </c>
+      <c r="O422" s="7">
+        <v>2.5029428554767801</v>
+      </c>
+      <c r="P422" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q422" s="7">
+        <v>0</v>
+      </c>
+      <c r="R422" s="7">
+        <v>0</v>
+      </c>
+      <c r="S422" s="7">
+        <v>3.1084734916502001</v>
+      </c>
+      <c r="T422" t="b">
+        <v>1</v>
+      </c>
+      <c r="U422" s="2">
+        <v>69</v>
+      </c>
+      <c r="V422" s="2">
+        <v>12</v>
+      </c>
+      <c r="W422" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="X422" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="423" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A423" s="10">
+        <v>422</v>
+      </c>
+      <c r="B423" s="7">
+        <v>4.0981543022480098</v>
+      </c>
+      <c r="C423" s="7">
+        <v>0</v>
+      </c>
+      <c r="D423" s="7">
+        <v>9.3524889231086998</v>
+      </c>
+      <c r="E423" s="7">
+        <v>0</v>
+      </c>
+      <c r="F423" s="7">
+        <v>0</v>
+      </c>
+      <c r="G423" s="7">
+        <v>0</v>
+      </c>
+      <c r="H423" s="7">
+        <v>0</v>
+      </c>
+      <c r="I423" s="7">
+        <v>0</v>
+      </c>
+      <c r="J423" s="7">
+        <v>0</v>
+      </c>
+      <c r="K423" s="7">
+        <v>0</v>
+      </c>
+      <c r="L423" s="7">
+        <v>0</v>
+      </c>
+      <c r="M423" s="7">
+        <v>0</v>
+      </c>
+      <c r="N423" s="7">
+        <v>0</v>
+      </c>
+      <c r="O423" s="7">
+        <v>1.3550598208337801</v>
+      </c>
+      <c r="P423" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q423" s="7">
+        <v>0</v>
+      </c>
+      <c r="R423" s="7">
+        <v>0</v>
+      </c>
+      <c r="S423" s="7">
+        <v>3.3490071617566399</v>
+      </c>
+      <c r="T423" t="b">
+        <v>0</v>
+      </c>
+      <c r="U423" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V423" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W423" s="2" t="str">
+        <f t="shared" ref="W423:W451" si="26">IF(T423=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="X423" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="424" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A424" s="10">
+        <v>423</v>
+      </c>
+      <c r="B424" s="7">
+        <v>0</v>
+      </c>
+      <c r="C424" s="7">
+        <v>0</v>
+      </c>
+      <c r="D424" s="7">
+        <v>0</v>
+      </c>
+      <c r="E424" s="7">
+        <v>0</v>
+      </c>
+      <c r="F424" s="7">
+        <v>0</v>
+      </c>
+      <c r="G424" s="7">
+        <v>10.9949313257051</v>
+      </c>
+      <c r="H424" s="7">
+        <v>0</v>
+      </c>
+      <c r="I424" s="7">
+        <v>0</v>
+      </c>
+      <c r="J424" s="7">
+        <v>0</v>
+      </c>
+      <c r="K424" s="7">
+        <v>0</v>
+      </c>
+      <c r="L424" s="7">
+        <v>0</v>
+      </c>
+      <c r="M424" s="7">
+        <v>9.5601667446377192</v>
+      </c>
+      <c r="N424" s="7">
+        <v>0</v>
+      </c>
+      <c r="O424" s="7">
+        <v>2.9644405648341099</v>
+      </c>
+      <c r="P424" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q424" s="7">
+        <v>0</v>
+      </c>
+      <c r="R424" s="7">
+        <v>0</v>
+      </c>
+      <c r="S424" s="7">
+        <v>4.7973399909914702</v>
+      </c>
+      <c r="T424" t="b">
+        <v>0</v>
+      </c>
+      <c r="U424" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V424" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W424" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X424" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="425" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A425" s="10">
+        <v>424</v>
+      </c>
+      <c r="B425" s="7">
+        <v>0</v>
+      </c>
+      <c r="C425" s="7">
+        <v>0</v>
+      </c>
+      <c r="D425" s="7">
+        <v>0</v>
+      </c>
+      <c r="E425" s="7">
+        <v>7.5643458526164702</v>
+      </c>
+      <c r="F425" s="7">
+        <v>0</v>
+      </c>
+      <c r="G425" s="7">
+        <v>0</v>
+      </c>
+      <c r="H425" s="7">
+        <v>0</v>
+      </c>
+      <c r="I425" s="7">
+        <v>0</v>
+      </c>
+      <c r="J425" s="7">
+        <v>0</v>
+      </c>
+      <c r="K425" s="7">
+        <v>0</v>
+      </c>
+      <c r="L425" s="7">
+        <v>0</v>
+      </c>
+      <c r="M425" s="7">
+        <v>8.3458319065284101</v>
+      </c>
+      <c r="N425" s="7">
+        <v>0</v>
+      </c>
+      <c r="O425" s="7">
+        <v>2.4078353832217099</v>
+      </c>
+      <c r="P425" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q425" s="7">
+        <v>0</v>
+      </c>
+      <c r="R425" s="7">
+        <v>0</v>
+      </c>
+      <c r="S425" s="7">
+        <v>2.3304852310145701</v>
+      </c>
+      <c r="T425" t="b">
+        <v>0</v>
+      </c>
+      <c r="U425" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V425" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W425" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X425" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="426" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A426" s="10">
+        <v>425</v>
+      </c>
+      <c r="B426" s="7">
+        <v>5.8500451582053001</v>
+      </c>
+      <c r="C426" s="7">
+        <v>0</v>
+      </c>
+      <c r="D426" s="7">
+        <v>0</v>
+      </c>
+      <c r="E426" s="7">
+        <v>0</v>
+      </c>
+      <c r="F426" s="7">
+        <v>0</v>
+      </c>
+      <c r="G426" s="7">
+        <v>0</v>
+      </c>
+      <c r="H426" s="7">
+        <v>0</v>
+      </c>
+      <c r="I426" s="7">
+        <v>7.4726486161525099</v>
+      </c>
+      <c r="J426" s="7">
+        <v>0</v>
+      </c>
+      <c r="K426" s="7">
+        <v>0</v>
+      </c>
+      <c r="L426" s="7">
+        <v>0</v>
+      </c>
+      <c r="M426" s="7">
+        <v>0</v>
+      </c>
+      <c r="N426" s="7">
+        <v>0</v>
+      </c>
+      <c r="O426" s="7">
+        <v>3.6594296445160501</v>
+      </c>
+      <c r="P426" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q426" s="7">
+        <v>0</v>
+      </c>
+      <c r="R426" s="7">
+        <v>0</v>
+      </c>
+      <c r="S426" s="7">
+        <v>4.0287761432563904</v>
+      </c>
+      <c r="T426" t="b">
+        <v>0</v>
+      </c>
+      <c r="U426" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V426" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W426" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X426" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="427" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A427" s="10">
+        <v>426</v>
+      </c>
+      <c r="B427" s="7">
+        <v>0</v>
+      </c>
+      <c r="C427" s="7">
+        <v>0</v>
+      </c>
+      <c r="D427" s="7">
+        <v>0</v>
+      </c>
+      <c r="E427" s="7">
+        <v>0</v>
+      </c>
+      <c r="F427" s="7">
+        <v>0</v>
+      </c>
+      <c r="G427" s="7">
+        <v>0</v>
+      </c>
+      <c r="H427" s="7">
+        <v>0</v>
+      </c>
+      <c r="I427" s="7">
+        <v>0</v>
+      </c>
+      <c r="J427" s="7">
+        <v>12.6788868470005</v>
+      </c>
+      <c r="K427" s="7">
+        <v>0</v>
+      </c>
+      <c r="L427" s="7">
+        <v>11.2280444808776</v>
+      </c>
+      <c r="M427" s="7">
+        <v>0</v>
+      </c>
+      <c r="N427" s="7">
+        <v>0</v>
+      </c>
+      <c r="O427" s="7">
+        <v>2.2623304692087598</v>
+      </c>
+      <c r="P427" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q427" s="7">
+        <v>0</v>
+      </c>
+      <c r="R427" s="7">
+        <v>0</v>
+      </c>
+      <c r="S427" s="7">
+        <v>3.9197334433900002</v>
+      </c>
+      <c r="T427" t="b">
+        <v>0</v>
+      </c>
+      <c r="U427" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V427" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W427" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X427" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="428" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A428" s="10">
+        <v>427</v>
+      </c>
+      <c r="B428" s="7">
+        <v>0</v>
+      </c>
+      <c r="C428" s="7">
+        <v>0</v>
+      </c>
+      <c r="D428" s="7">
+        <v>6.5121357566335396</v>
+      </c>
+      <c r="E428" s="7">
+        <v>0</v>
+      </c>
+      <c r="F428" s="7">
+        <v>0</v>
+      </c>
+      <c r="G428" s="7">
+        <v>0</v>
+      </c>
+      <c r="H428" s="7">
+        <v>0</v>
+      </c>
+      <c r="I428" s="7">
+        <v>0</v>
+      </c>
+      <c r="J428" s="7">
+        <v>0</v>
+      </c>
+      <c r="K428" s="7">
+        <v>0</v>
+      </c>
+      <c r="L428" s="7">
+        <v>0</v>
+      </c>
+      <c r="M428" s="7">
+        <v>12.8204471949955</v>
+      </c>
+      <c r="N428" s="7">
+        <v>0</v>
+      </c>
+      <c r="O428" s="7">
+        <v>1.61830363250724</v>
+      </c>
+      <c r="P428" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q428" s="7">
+        <v>0</v>
+      </c>
+      <c r="R428" s="7">
+        <v>0</v>
+      </c>
+      <c r="S428" s="7">
+        <v>4.4554562034218099</v>
+      </c>
+      <c r="T428" t="b">
+        <v>0</v>
+      </c>
+      <c r="U428" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V428" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W428" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X428" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="429" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A429" s="10">
+        <v>428</v>
+      </c>
+      <c r="B429" s="7">
+        <v>0</v>
+      </c>
+      <c r="C429" s="7">
+        <v>0</v>
+      </c>
+      <c r="D429" s="7">
+        <v>0</v>
+      </c>
+      <c r="E429" s="7">
+        <v>11.298898295402401</v>
+      </c>
+      <c r="F429" s="7">
+        <v>10.3934905406973</v>
+      </c>
+      <c r="G429" s="7">
+        <v>0</v>
+      </c>
+      <c r="H429" s="7">
+        <v>0</v>
+      </c>
+      <c r="I429" s="7">
+        <v>0</v>
+      </c>
+      <c r="J429" s="7">
+        <v>0</v>
+      </c>
+      <c r="K429" s="7">
+        <v>0</v>
+      </c>
+      <c r="L429" s="7">
+        <v>0</v>
+      </c>
+      <c r="M429" s="7">
+        <v>0</v>
+      </c>
+      <c r="N429" s="7">
+        <v>0</v>
+      </c>
+      <c r="O429" s="7">
+        <v>1.4540651712791399</v>
+      </c>
+      <c r="P429" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q429" s="7">
+        <v>0</v>
+      </c>
+      <c r="R429" s="7">
+        <v>0</v>
+      </c>
+      <c r="S429" s="7">
+        <v>2.1306606401486001</v>
+      </c>
+      <c r="T429" t="b">
+        <v>0</v>
+      </c>
+      <c r="U429" s="2" t="str">
+        <f t="shared" si="22"/>
+        <v>NA</v>
+      </c>
+      <c r="V429" s="2" t="str">
+        <f t="shared" si="23"/>
+        <v>NA</v>
+      </c>
+      <c r="W429" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X429" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="430" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A430" s="10">
+        <v>429</v>
+      </c>
+      <c r="B430" s="7">
+        <v>0</v>
+      </c>
+      <c r="C430" s="7">
+        <v>0</v>
+      </c>
+      <c r="D430" s="7">
+        <v>0</v>
+      </c>
+      <c r="E430" s="7">
+        <v>0</v>
+      </c>
+      <c r="F430" s="7">
+        <v>8.2904254805641795</v>
+      </c>
+      <c r="G430" s="7">
+        <v>0</v>
+      </c>
+      <c r="H430" s="7">
+        <v>0</v>
+      </c>
+      <c r="I430" s="7">
+        <v>0</v>
+      </c>
+      <c r="J430" s="7">
+        <v>0</v>
+      </c>
+      <c r="K430" s="7">
+        <v>0</v>
+      </c>
+      <c r="L430" s="7">
+        <v>0</v>
+      </c>
+      <c r="M430" s="7">
+        <v>12.8277196162684</v>
+      </c>
+      <c r="N430" s="7">
+        <v>0</v>
+      </c>
+      <c r="O430" s="7">
+        <v>3.0491109776077798</v>
+      </c>
+      <c r="P430" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q430" s="7">
+        <v>0</v>
+      </c>
+      <c r="R430" s="7">
+        <v>0</v>
+      </c>
+      <c r="S430" s="7">
+        <v>3.3437885043560098</v>
+      </c>
+      <c r="T430" t="b">
+        <v>0</v>
+      </c>
+      <c r="U430" s="2" t="str">
+        <f t="shared" ref="U430:U451" si="27">IF(T430=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V430" s="2" t="str">
+        <f t="shared" ref="V430:V451" si="28">IF(T430=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W430" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X430" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="431" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A431" s="10">
+        <v>430</v>
+      </c>
+      <c r="B431" s="7">
+        <v>0</v>
+      </c>
+      <c r="C431" s="7">
+        <v>0</v>
+      </c>
+      <c r="D431" s="7">
+        <v>0</v>
+      </c>
+      <c r="E431" s="7">
+        <v>13.0313145634201</v>
+      </c>
+      <c r="F431" s="7">
+        <v>0</v>
+      </c>
+      <c r="G431" s="7">
+        <v>0</v>
+      </c>
+      <c r="H431" s="7">
+        <v>0</v>
+      </c>
+      <c r="I431" s="7">
+        <v>7.4016208314917602</v>
+      </c>
+      <c r="J431" s="7">
+        <v>0</v>
+      </c>
+      <c r="K431" s="7">
+        <v>0</v>
+      </c>
+      <c r="L431" s="7">
+        <v>0</v>
+      </c>
+      <c r="M431" s="7">
+        <v>0</v>
+      </c>
+      <c r="N431" s="7">
+        <v>0</v>
+      </c>
+      <c r="O431" s="7">
+        <v>2.8861681656541398</v>
+      </c>
+      <c r="P431" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q431" s="7">
+        <v>0</v>
+      </c>
+      <c r="R431" s="7">
+        <v>0</v>
+      </c>
+      <c r="S431" s="7">
+        <v>2.7689445761982299</v>
+      </c>
+      <c r="T431" t="b">
+        <v>0</v>
+      </c>
+      <c r="U431" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V431" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W431" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X431" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="432" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A432" s="10">
+        <v>431</v>
+      </c>
+      <c r="B432" s="7">
+        <v>0</v>
+      </c>
+      <c r="C432" s="7">
+        <v>0</v>
+      </c>
+      <c r="D432" s="7">
+        <v>0</v>
+      </c>
+      <c r="E432" s="7">
+        <v>8.94153544916316</v>
+      </c>
+      <c r="F432" s="7">
+        <v>0</v>
+      </c>
+      <c r="G432" s="7">
+        <v>0</v>
+      </c>
+      <c r="H432" s="7">
+        <v>0</v>
+      </c>
+      <c r="I432" s="7">
+        <v>0</v>
+      </c>
+      <c r="J432" s="7">
+        <v>0</v>
+      </c>
+      <c r="K432" s="7">
+        <v>10.314908541028</v>
+      </c>
+      <c r="L432" s="7">
+        <v>0</v>
+      </c>
+      <c r="M432" s="7">
+        <v>0</v>
+      </c>
+      <c r="N432" s="7">
+        <v>0</v>
+      </c>
+      <c r="O432" s="7">
+        <v>3.8181720000784898</v>
+      </c>
+      <c r="P432" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q432" s="7">
+        <v>0</v>
+      </c>
+      <c r="R432" s="7">
+        <v>0</v>
+      </c>
+      <c r="S432" s="7">
+        <v>1.4659053214587501</v>
+      </c>
+      <c r="T432" t="b">
+        <v>0</v>
+      </c>
+      <c r="U432" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V432" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W432" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X432" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="433" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A433" s="10">
+        <v>432</v>
+      </c>
+      <c r="B433" s="7">
+        <v>0</v>
+      </c>
+      <c r="C433" s="7">
+        <v>0</v>
+      </c>
+      <c r="D433" s="7">
+        <v>0</v>
+      </c>
+      <c r="E433" s="7">
+        <v>0</v>
+      </c>
+      <c r="F433" s="7">
+        <v>0</v>
+      </c>
+      <c r="G433" s="7">
+        <v>9.6658541420956592</v>
+      </c>
+      <c r="H433" s="7">
+        <v>7.7691396442838503</v>
+      </c>
+      <c r="I433" s="7">
+        <v>0</v>
+      </c>
+      <c r="J433" s="7">
+        <v>0</v>
+      </c>
+      <c r="K433" s="7">
+        <v>0</v>
+      </c>
+      <c r="L433" s="7">
+        <v>0</v>
+      </c>
+      <c r="M433" s="7">
+        <v>0</v>
+      </c>
+      <c r="N433" s="7">
+        <v>0</v>
+      </c>
+      <c r="O433" s="7">
+        <v>2.1184084001534602</v>
+      </c>
+      <c r="P433" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q433" s="7">
+        <v>0</v>
+      </c>
+      <c r="R433" s="7">
+        <v>0</v>
+      </c>
+      <c r="S433" s="7">
+        <v>3.4830575323453599</v>
+      </c>
+      <c r="T433" t="b">
+        <v>0</v>
+      </c>
+      <c r="U433" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V433" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W433" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X433" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="434" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A434" s="10">
+        <v>433</v>
+      </c>
+      <c r="B434" s="7">
+        <v>0</v>
+      </c>
+      <c r="C434" s="7">
+        <v>0</v>
+      </c>
+      <c r="D434" s="7">
+        <v>0</v>
+      </c>
+      <c r="E434" s="7">
+        <v>0</v>
+      </c>
+      <c r="F434" s="7">
+        <v>0</v>
+      </c>
+      <c r="G434" s="7">
+        <v>9.9594829110003893</v>
+      </c>
+      <c r="H434" s="7">
+        <v>0</v>
+      </c>
+      <c r="I434" s="7">
+        <v>11.395120078255699</v>
+      </c>
+      <c r="J434" s="7">
+        <v>0</v>
+      </c>
+      <c r="K434" s="7">
+        <v>0</v>
+      </c>
+      <c r="L434" s="7">
+        <v>0</v>
+      </c>
+      <c r="M434" s="7">
+        <v>0</v>
+      </c>
+      <c r="N434" s="7">
+        <v>0</v>
+      </c>
+      <c r="O434" s="7">
+        <v>1.99949466191534</v>
+      </c>
+      <c r="P434" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q434" s="7">
+        <v>0</v>
+      </c>
+      <c r="R434" s="7">
+        <v>0</v>
+      </c>
+      <c r="S434" s="7">
+        <v>3.9040133273897402</v>
+      </c>
+      <c r="T434" t="b">
+        <v>0</v>
+      </c>
+      <c r="U434" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V434" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W434" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X434" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="435" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A435" s="10">
+        <v>434</v>
+      </c>
+      <c r="B435" s="7">
+        <v>0</v>
+      </c>
+      <c r="C435" s="7">
+        <v>0</v>
+      </c>
+      <c r="D435" s="7">
+        <v>0</v>
+      </c>
+      <c r="E435" s="7">
+        <v>6.6434002756897499</v>
+      </c>
+      <c r="F435" s="7">
+        <v>0</v>
+      </c>
+      <c r="G435" s="7">
+        <v>0</v>
+      </c>
+      <c r="H435" s="7">
+        <v>0</v>
+      </c>
+      <c r="I435" s="7">
+        <v>0</v>
+      </c>
+      <c r="J435" s="7">
+        <v>0</v>
+      </c>
+      <c r="K435" s="7">
+        <v>0</v>
+      </c>
+      <c r="L435" s="7">
+        <v>10.150469818166799</v>
+      </c>
+      <c r="M435" s="7">
+        <v>0</v>
+      </c>
+      <c r="N435" s="7">
+        <v>0</v>
+      </c>
+      <c r="O435" s="7">
+        <v>1.49740607774134</v>
+      </c>
+      <c r="P435" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q435" s="7">
+        <v>0</v>
+      </c>
+      <c r="R435" s="7">
+        <v>0</v>
+      </c>
+      <c r="S435" s="7">
+        <v>3.68247285008606</v>
+      </c>
+      <c r="T435" t="b">
+        <v>0</v>
+      </c>
+      <c r="U435" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V435" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W435" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X435" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="436" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A436" s="10">
+        <v>435</v>
+      </c>
+      <c r="B436" s="7">
+        <v>5.1535313802283804</v>
+      </c>
+      <c r="C436" s="7">
+        <v>0</v>
+      </c>
+      <c r="D436" s="7">
+        <v>0</v>
+      </c>
+      <c r="E436" s="7">
+        <v>0</v>
+      </c>
+      <c r="F436" s="7">
+        <v>0</v>
+      </c>
+      <c r="G436" s="7">
+        <v>0</v>
+      </c>
+      <c r="H436" s="7">
+        <v>0</v>
+      </c>
+      <c r="I436" s="7">
+        <v>0</v>
+      </c>
+      <c r="J436" s="7">
+        <v>0</v>
+      </c>
+      <c r="K436" s="7">
+        <v>0</v>
+      </c>
+      <c r="L436" s="7">
+        <v>0</v>
+      </c>
+      <c r="M436" s="7">
+        <v>8.8612138219107806</v>
+      </c>
+      <c r="N436" s="7">
+        <v>0</v>
+      </c>
+      <c r="O436" s="7">
+        <v>2.3790787079712601</v>
+      </c>
+      <c r="P436" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q436" s="7">
+        <v>0</v>
+      </c>
+      <c r="R436" s="7">
+        <v>0</v>
+      </c>
+      <c r="S436" s="7">
+        <v>5.5152564964901201</v>
+      </c>
+      <c r="T436" t="b">
+        <v>0</v>
+      </c>
+      <c r="U436" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V436" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W436" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X436" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="437" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A437" s="10">
+        <v>436</v>
+      </c>
+      <c r="B437" s="7">
+        <v>0</v>
+      </c>
+      <c r="C437" s="7">
+        <v>0</v>
+      </c>
+      <c r="D437" s="7">
+        <v>0</v>
+      </c>
+      <c r="E437" s="7">
+        <v>0</v>
+      </c>
+      <c r="F437" s="7">
+        <v>0</v>
+      </c>
+      <c r="G437" s="7">
+        <v>0</v>
+      </c>
+      <c r="H437" s="7">
+        <v>0</v>
+      </c>
+      <c r="I437" s="7">
+        <v>0</v>
+      </c>
+      <c r="J437" s="7">
+        <v>8.3317733771323397</v>
+      </c>
+      <c r="K437" s="7">
+        <v>0</v>
+      </c>
+      <c r="L437" s="7">
+        <v>8.8250765094847203</v>
+      </c>
+      <c r="M437" s="7">
+        <v>0</v>
+      </c>
+      <c r="N437" s="7">
+        <v>0</v>
+      </c>
+      <c r="O437" s="7">
+        <v>2.5648364140269102</v>
+      </c>
+      <c r="P437" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q437" s="7">
+        <v>0</v>
+      </c>
+      <c r="R437" s="7">
+        <v>0</v>
+      </c>
+      <c r="S437" s="7">
+        <v>2.0441005779561001</v>
+      </c>
+      <c r="T437" t="b">
+        <v>0</v>
+      </c>
+      <c r="U437" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V437" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W437" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X437" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="438" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A438" s="10">
+        <v>437</v>
+      </c>
+      <c r="B438" s="7">
+        <v>10.565402482619699</v>
+      </c>
+      <c r="C438" s="7">
+        <v>0</v>
+      </c>
+      <c r="D438" s="7">
+        <v>0</v>
+      </c>
+      <c r="E438" s="7">
+        <v>0</v>
+      </c>
+      <c r="F438" s="7">
+        <v>0</v>
+      </c>
+      <c r="G438" s="7">
+        <v>0</v>
+      </c>
+      <c r="H438" s="7">
+        <v>0</v>
+      </c>
+      <c r="I438" s="7">
+        <v>0</v>
+      </c>
+      <c r="J438" s="7">
+        <v>0</v>
+      </c>
+      <c r="K438" s="7">
+        <v>0</v>
+      </c>
+      <c r="L438" s="7">
+        <v>0</v>
+      </c>
+      <c r="M438" s="7">
+        <v>13.065159511204699</v>
+      </c>
+      <c r="N438" s="7">
+        <v>0</v>
+      </c>
+      <c r="O438" s="7">
+        <v>1.99417153229356</v>
+      </c>
+      <c r="P438" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q438" s="7">
+        <v>0</v>
+      </c>
+      <c r="R438" s="7">
+        <v>0</v>
+      </c>
+      <c r="S438" s="7">
+        <v>2.4612079878120898</v>
+      </c>
+      <c r="T438" t="b">
+        <v>0</v>
+      </c>
+      <c r="U438" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V438" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W438" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X438" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="439" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A439" s="10">
+        <v>438</v>
+      </c>
+      <c r="B439" s="7">
+        <v>7.9687514967353401</v>
+      </c>
+      <c r="C439" s="7">
+        <v>0</v>
+      </c>
+      <c r="D439" s="7">
+        <v>0</v>
+      </c>
+      <c r="E439" s="7">
+        <v>0</v>
+      </c>
+      <c r="F439" s="7">
+        <v>0</v>
+      </c>
+      <c r="G439" s="7">
+        <v>0</v>
+      </c>
+      <c r="H439" s="7">
+        <v>0</v>
+      </c>
+      <c r="I439" s="7">
+        <v>0</v>
+      </c>
+      <c r="J439" s="7">
+        <v>11.272357074052399</v>
+      </c>
+      <c r="K439" s="7">
+        <v>0</v>
+      </c>
+      <c r="L439" s="7">
+        <v>0</v>
+      </c>
+      <c r="M439" s="7">
+        <v>0</v>
+      </c>
+      <c r="N439" s="7">
+        <v>0</v>
+      </c>
+      <c r="O439" s="7">
+        <v>2.3328223260721099</v>
+      </c>
+      <c r="P439" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q439" s="7">
+        <v>0</v>
+      </c>
+      <c r="R439" s="7">
+        <v>0</v>
+      </c>
+      <c r="S439" s="7">
+        <v>4.43373393453352</v>
+      </c>
+      <c r="T439" t="b">
+        <v>0</v>
+      </c>
+      <c r="U439" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V439" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W439" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X439" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="440" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A440" s="10">
+        <v>439</v>
+      </c>
+      <c r="B440" s="7">
+        <v>0</v>
+      </c>
+      <c r="C440" s="7">
+        <v>0</v>
+      </c>
+      <c r="D440" s="7">
+        <v>0</v>
+      </c>
+      <c r="E440" s="7">
+        <v>0</v>
+      </c>
+      <c r="F440" s="7">
+        <v>0</v>
+      </c>
+      <c r="G440" s="7">
+        <v>0</v>
+      </c>
+      <c r="H440" s="7">
+        <v>0</v>
+      </c>
+      <c r="I440" s="7">
+        <v>0</v>
+      </c>
+      <c r="J440" s="7">
+        <v>0</v>
+      </c>
+      <c r="K440" s="7">
+        <v>12.7035364529074</v>
+      </c>
+      <c r="L440" s="7">
+        <v>0</v>
+      </c>
+      <c r="M440" s="7">
+        <v>8.8199470232901405</v>
+      </c>
+      <c r="N440" s="7">
+        <v>0</v>
+      </c>
+      <c r="O440" s="7">
+        <v>2.6545227800734099</v>
+      </c>
+      <c r="P440" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q440" s="7">
+        <v>0</v>
+      </c>
+      <c r="R440" s="7">
+        <v>0</v>
+      </c>
+      <c r="S440" s="7">
+        <v>4.1789270634267304</v>
+      </c>
+      <c r="T440" t="b">
+        <v>0</v>
+      </c>
+      <c r="U440" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V440" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W440" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X440" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="441" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A441" s="10">
+        <v>440</v>
+      </c>
+      <c r="B441" s="7">
+        <v>0</v>
+      </c>
+      <c r="C441" s="7">
+        <v>0</v>
+      </c>
+      <c r="D441" s="7">
+        <v>0</v>
+      </c>
+      <c r="E441" s="7">
+        <v>0</v>
+      </c>
+      <c r="F441" s="7">
+        <v>0</v>
+      </c>
+      <c r="G441" s="7">
+        <v>11.0574376477068</v>
+      </c>
+      <c r="H441" s="7">
+        <v>0</v>
+      </c>
+      <c r="I441" s="7">
+        <v>0</v>
+      </c>
+      <c r="J441" s="7">
+        <v>0</v>
+      </c>
+      <c r="K441" s="7">
+        <v>12.120935551063001</v>
+      </c>
+      <c r="L441" s="7">
+        <v>0</v>
+      </c>
+      <c r="M441" s="7">
+        <v>0</v>
+      </c>
+      <c r="N441" s="7">
+        <v>0</v>
+      </c>
+      <c r="O441" s="7">
+        <v>2.3340593385870498</v>
+      </c>
+      <c r="P441" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q441" s="7">
+        <v>0</v>
+      </c>
+      <c r="R441" s="7">
+        <v>0</v>
+      </c>
+      <c r="S441" s="7">
+        <v>3.9452341576118402</v>
+      </c>
+      <c r="T441" t="b">
+        <v>0</v>
+      </c>
+      <c r="U441" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V441" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W441" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X441" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="442" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A442" s="10">
+        <v>441</v>
+      </c>
+      <c r="B442" s="7">
+        <v>0</v>
+      </c>
+      <c r="C442" s="7">
+        <v>0</v>
+      </c>
+      <c r="D442" s="7">
+        <v>0</v>
+      </c>
+      <c r="E442" s="7">
+        <v>0</v>
+      </c>
+      <c r="F442" s="7">
+        <v>0</v>
+      </c>
+      <c r="G442" s="7">
+        <v>0</v>
+      </c>
+      <c r="H442" s="7">
+        <v>0</v>
+      </c>
+      <c r="I442" s="7">
+        <v>0</v>
+      </c>
+      <c r="J442" s="7">
+        <v>12.3867514238604</v>
+      </c>
+      <c r="K442" s="7">
+        <v>8.2750151421549401</v>
+      </c>
+      <c r="L442" s="7">
+        <v>0</v>
+      </c>
+      <c r="M442" s="7">
+        <v>0</v>
+      </c>
+      <c r="N442" s="7">
+        <v>0</v>
+      </c>
+      <c r="O442" s="7">
+        <v>2.6415571606391199</v>
+      </c>
+      <c r="P442" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q442" s="7">
+        <v>0</v>
+      </c>
+      <c r="R442" s="7">
+        <v>0</v>
+      </c>
+      <c r="S442" s="7">
+        <v>2.6111664892098001</v>
+      </c>
+      <c r="T442" t="b">
+        <v>0</v>
+      </c>
+      <c r="U442" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V442" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W442" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X442" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="443" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A443" s="10">
+        <v>442</v>
+      </c>
+      <c r="B443" s="7">
+        <v>0</v>
+      </c>
+      <c r="C443" s="7">
+        <v>0</v>
+      </c>
+      <c r="D443" s="7">
+        <v>0</v>
+      </c>
+      <c r="E443" s="7">
+        <v>0</v>
+      </c>
+      <c r="F443" s="7">
+        <v>0</v>
+      </c>
+      <c r="G443" s="7">
+        <v>10.069386040153599</v>
+      </c>
+      <c r="H443" s="7">
+        <v>0</v>
+      </c>
+      <c r="I443" s="7">
+        <v>0</v>
+      </c>
+      <c r="J443" s="7">
+        <v>0</v>
+      </c>
+      <c r="K443" s="7">
+        <v>0</v>
+      </c>
+      <c r="L443" s="7">
+        <v>8.1128537912319398</v>
+      </c>
+      <c r="M443" s="7">
+        <v>0</v>
+      </c>
+      <c r="N443" s="7">
+        <v>0</v>
+      </c>
+      <c r="O443" s="7">
+        <v>3.4722858714718301</v>
+      </c>
+      <c r="P443" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q443" s="7">
+        <v>0</v>
+      </c>
+      <c r="R443" s="7">
+        <v>0</v>
+      </c>
+      <c r="S443" s="7">
+        <v>2.8526687285570498</v>
+      </c>
+      <c r="T443" t="b">
+        <v>0</v>
+      </c>
+      <c r="U443" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V443" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W443" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X443" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="444" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A444" s="10">
+        <v>443</v>
+      </c>
+      <c r="B444" s="7">
+        <v>0</v>
+      </c>
+      <c r="C444" s="7">
+        <v>10.3899008526777</v>
+      </c>
+      <c r="D444" s="7">
+        <v>0</v>
+      </c>
+      <c r="E444" s="7">
+        <v>0</v>
+      </c>
+      <c r="F444" s="7">
+        <v>0</v>
+      </c>
+      <c r="G444" s="7">
+        <v>10.4716804321029</v>
+      </c>
+      <c r="H444" s="7">
+        <v>0</v>
+      </c>
+      <c r="I444" s="7">
+        <v>0</v>
+      </c>
+      <c r="J444" s="7">
+        <v>0</v>
+      </c>
+      <c r="K444" s="7">
+        <v>0</v>
+      </c>
+      <c r="L444" s="7">
+        <v>0</v>
+      </c>
+      <c r="M444" s="7">
+        <v>0</v>
+      </c>
+      <c r="N444" s="7">
+        <v>0</v>
+      </c>
+      <c r="O444" s="7">
+        <v>3.04604594198037</v>
+      </c>
+      <c r="P444" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q444" s="7">
+        <v>0</v>
+      </c>
+      <c r="R444" s="7">
+        <v>0</v>
+      </c>
+      <c r="S444" s="7">
+        <v>2.00067899665031</v>
+      </c>
+      <c r="T444" t="b">
+        <v>0</v>
+      </c>
+      <c r="U444" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V444" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W444" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X444" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="445" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A445" s="10">
+        <v>444</v>
+      </c>
+      <c r="B445" s="7">
+        <v>0</v>
+      </c>
+      <c r="C445" s="7">
+        <v>0</v>
+      </c>
+      <c r="D445" s="7">
+        <v>10.6043776968722</v>
+      </c>
+      <c r="E445" s="7">
+        <v>0</v>
+      </c>
+      <c r="F445" s="7">
+        <v>0</v>
+      </c>
+      <c r="G445" s="7">
+        <v>0</v>
+      </c>
+      <c r="H445" s="7">
+        <v>0</v>
+      </c>
+      <c r="I445" s="7">
+        <v>7.0252111304242204</v>
+      </c>
+      <c r="J445" s="7">
+        <v>0</v>
+      </c>
+      <c r="K445" s="7">
+        <v>0</v>
+      </c>
+      <c r="L445" s="7">
+        <v>0</v>
+      </c>
+      <c r="M445" s="7">
+        <v>0</v>
+      </c>
+      <c r="N445" s="7">
+        <v>0</v>
+      </c>
+      <c r="O445" s="7">
+        <v>2.6107544234691402</v>
+      </c>
+      <c r="P445" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q445" s="7">
+        <v>0</v>
+      </c>
+      <c r="R445" s="7">
+        <v>0</v>
+      </c>
+      <c r="S445" s="7">
+        <v>2.18844504062892</v>
+      </c>
+      <c r="T445" t="b">
+        <v>0</v>
+      </c>
+      <c r="U445" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V445" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W445" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X445" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="446" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A446" s="10">
+        <v>445</v>
+      </c>
+      <c r="B446" s="7">
+        <v>0</v>
+      </c>
+      <c r="C446" s="7">
+        <v>0</v>
+      </c>
+      <c r="D446" s="7">
+        <v>0</v>
+      </c>
+      <c r="E446" s="7">
+        <v>0</v>
+      </c>
+      <c r="F446" s="7">
+        <v>0</v>
+      </c>
+      <c r="G446" s="7">
+        <v>0</v>
+      </c>
+      <c r="H446" s="7">
+        <v>0</v>
+      </c>
+      <c r="I446" s="7">
+        <v>6.6118999889689603</v>
+      </c>
+      <c r="J446" s="7">
+        <v>10.766913594123</v>
+      </c>
+      <c r="K446" s="7">
+        <v>0</v>
+      </c>
+      <c r="L446" s="7">
+        <v>0</v>
+      </c>
+      <c r="M446" s="7">
+        <v>0</v>
+      </c>
+      <c r="N446" s="7">
+        <v>0</v>
+      </c>
+      <c r="O446" s="7">
+        <v>2.3761673239771</v>
+      </c>
+      <c r="P446" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q446" s="7">
+        <v>0</v>
+      </c>
+      <c r="R446" s="7">
+        <v>0</v>
+      </c>
+      <c r="S446" s="7">
+        <v>4.9692671212684196</v>
+      </c>
+      <c r="T446" t="b">
+        <v>0</v>
+      </c>
+      <c r="U446" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V446" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W446" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X446" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="447" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A447" s="10">
+        <v>446</v>
+      </c>
+      <c r="B447" s="7">
+        <v>0</v>
+      </c>
+      <c r="C447" s="7">
+        <v>11.3533226891987</v>
+      </c>
+      <c r="D447" s="7">
+        <v>0</v>
+      </c>
+      <c r="E447" s="7">
+        <v>0</v>
+      </c>
+      <c r="F447" s="7">
+        <v>0</v>
+      </c>
+      <c r="G447" s="7">
+        <v>0</v>
+      </c>
+      <c r="H447" s="7">
+        <v>0</v>
+      </c>
+      <c r="I447" s="7">
+        <v>0</v>
+      </c>
+      <c r="J447" s="7">
+        <v>0</v>
+      </c>
+      <c r="K447" s="7">
+        <v>0</v>
+      </c>
+      <c r="L447" s="7">
+        <v>0</v>
+      </c>
+      <c r="M447" s="7">
+        <v>9.6691881484576907</v>
+      </c>
+      <c r="N447" s="7">
+        <v>0</v>
+      </c>
+      <c r="O447" s="7">
+        <v>1.93500446655571</v>
+      </c>
+      <c r="P447" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q447" s="7">
+        <v>0</v>
+      </c>
+      <c r="R447" s="7">
+        <v>0</v>
+      </c>
+      <c r="S447" s="7">
+        <v>3.8019434493633799</v>
+      </c>
+      <c r="T447" t="b">
+        <v>0</v>
+      </c>
+      <c r="U447" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V447" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W447" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X447" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="448" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A448" s="10">
+        <v>447</v>
+      </c>
+      <c r="B448" s="7">
+        <v>0</v>
+      </c>
+      <c r="C448" s="7">
+        <v>8.8777395841943907</v>
+      </c>
+      <c r="D448" s="7">
+        <v>0</v>
+      </c>
+      <c r="E448" s="7">
+        <v>0</v>
+      </c>
+      <c r="F448" s="7">
+        <v>0</v>
+      </c>
+      <c r="G448" s="7">
+        <v>0</v>
+      </c>
+      <c r="H448" s="7">
+        <v>0</v>
+      </c>
+      <c r="I448" s="7">
+        <v>0</v>
+      </c>
+      <c r="J448" s="7">
+        <v>0</v>
+      </c>
+      <c r="K448" s="7">
+        <v>11.9440863289579</v>
+      </c>
+      <c r="L448" s="7">
+        <v>0</v>
+      </c>
+      <c r="M448" s="7">
+        <v>0</v>
+      </c>
+      <c r="N448" s="7">
+        <v>0</v>
+      </c>
+      <c r="O448" s="7">
+        <v>1.8525442888439501</v>
+      </c>
+      <c r="P448" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q448" s="7">
+        <v>0</v>
+      </c>
+      <c r="R448" s="7">
+        <v>0</v>
+      </c>
+      <c r="S448" s="7">
+        <v>2.4218157109365901</v>
+      </c>
+      <c r="T448" t="b">
+        <v>0</v>
+      </c>
+      <c r="U448" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V448" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W448" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X448" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="449" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A449" s="10">
+        <v>448</v>
+      </c>
+      <c r="B449" s="7">
+        <v>0</v>
+      </c>
+      <c r="C449" s="7">
+        <v>0</v>
+      </c>
+      <c r="D449" s="7">
+        <v>9.4707456900534002</v>
+      </c>
+      <c r="E449" s="7">
+        <v>11.5041907246361</v>
+      </c>
+      <c r="F449" s="7">
+        <v>0</v>
+      </c>
+      <c r="G449" s="7">
+        <v>0</v>
+      </c>
+      <c r="H449" s="7">
+        <v>0</v>
+      </c>
+      <c r="I449" s="7">
+        <v>0</v>
+      </c>
+      <c r="J449" s="7">
+        <v>0</v>
+      </c>
+      <c r="K449" s="7">
+        <v>0</v>
+      </c>
+      <c r="L449" s="7">
+        <v>0</v>
+      </c>
+      <c r="M449" s="7">
+        <v>0</v>
+      </c>
+      <c r="N449" s="7">
+        <v>0</v>
+      </c>
+      <c r="O449" s="7">
+        <v>2.51724777831777</v>
+      </c>
+      <c r="P449" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q449" s="7">
+        <v>0</v>
+      </c>
+      <c r="R449" s="7">
+        <v>0</v>
+      </c>
+      <c r="S449" s="7">
+        <v>3.7034240484910299</v>
+      </c>
+      <c r="T449" t="b">
+        <v>0</v>
+      </c>
+      <c r="U449" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V449" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W449" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X449" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="450" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A450" s="10">
+        <v>449</v>
+      </c>
+      <c r="B450" s="7">
+        <v>0</v>
+      </c>
+      <c r="C450" s="7">
+        <v>0</v>
+      </c>
+      <c r="D450" s="7">
+        <v>0</v>
+      </c>
+      <c r="E450" s="7">
+        <v>0</v>
+      </c>
+      <c r="F450" s="7">
+        <v>0</v>
+      </c>
+      <c r="G450" s="7">
+        <v>11.965625772753</v>
+      </c>
+      <c r="H450" s="7">
+        <v>11.470872566456601</v>
+      </c>
+      <c r="I450" s="7">
+        <v>0</v>
+      </c>
+      <c r="J450" s="7">
+        <v>0</v>
+      </c>
+      <c r="K450" s="7">
+        <v>0</v>
+      </c>
+      <c r="L450" s="7">
+        <v>0</v>
+      </c>
+      <c r="M450" s="7">
+        <v>0</v>
+      </c>
+      <c r="N450" s="7">
+        <v>0</v>
+      </c>
+      <c r="O450" s="7">
+        <v>3.0045544122531802</v>
+      </c>
+      <c r="P450" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q450" s="7">
+        <v>0</v>
+      </c>
+      <c r="R450" s="7">
+        <v>0</v>
+      </c>
+      <c r="S450" s="7">
+        <v>4.7283992452153898</v>
+      </c>
+      <c r="T450" t="b">
+        <v>0</v>
+      </c>
+      <c r="U450" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V450" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W450" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X450" t="str">
+        <f t="shared" si="25"/>
+        <v>At least two non-zero values</v>
+      </c>
+    </row>
+    <row r="451" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A451" s="10">
+        <v>450</v>
+      </c>
+      <c r="B451" s="7">
+        <v>0</v>
+      </c>
+      <c r="C451" s="7">
+        <v>0</v>
+      </c>
+      <c r="D451" s="7">
+        <v>0</v>
+      </c>
+      <c r="E451" s="7">
+        <v>0</v>
+      </c>
+      <c r="F451" s="7">
+        <v>0</v>
+      </c>
+      <c r="G451" s="7">
+        <v>0</v>
+      </c>
+      <c r="H451" s="7">
+        <v>0</v>
+      </c>
+      <c r="I451" s="7">
+        <v>0</v>
+      </c>
+      <c r="J451" s="7">
+        <v>0</v>
+      </c>
+      <c r="K451" s="7">
+        <v>0</v>
+      </c>
+      <c r="L451" s="7">
+        <v>8.0670043974870609</v>
+      </c>
+      <c r="M451" s="7">
+        <v>11.551170405537601</v>
+      </c>
+      <c r="N451" s="7">
+        <v>0</v>
+      </c>
+      <c r="O451" s="7">
+        <v>2.9757741297073701</v>
+      </c>
+      <c r="P451" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q451" s="7">
+        <v>0</v>
+      </c>
+      <c r="R451" s="7">
+        <v>0</v>
+      </c>
+      <c r="S451" s="7">
+        <v>3.00258290565074</v>
+      </c>
+      <c r="T451" t="b">
+        <v>0</v>
+      </c>
+      <c r="U451" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="V451" s="2" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+      <c r="W451" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="X451" t="str">
+        <f t="shared" ref="X451" si="29">IF(COUNTIF(B451:M451,"&lt;&gt;0")&gt;=2, "At least two non-zero values", "Less than two non-zero values")</f>
+        <v>At least two non-zero values</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W421">
+  <conditionalFormatting sqref="A1:W451">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
@@ -41571,7 +44047,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S468
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AD7B9C-4443-4646-AE6E-96C06E512DB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5883E7FE-ABFF-AC40-AE93-2220E1CAA521}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="-38400" yWindow="-5300" windowWidth="38400" windowHeight="21600" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -699,11 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W451"/>
+  <dimension ref="A1:W469"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A406" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W451" sqref="W451"/>
+    <sheetView tabSelected="1" topLeftCell="A435" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="S1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W453" sqref="W453"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31545,7 +31545,7 @@
         <v>NA</v>
       </c>
       <c r="W423" s="2" t="str">
-        <f t="shared" ref="W423:W451" si="25">IF(T423=FALSE, "NA", "")</f>
+        <f t="shared" ref="W423:W469" si="25">IF(T423=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -32055,11 +32055,11 @@
         <v>0</v>
       </c>
       <c r="U430" s="2" t="str">
-        <f t="shared" ref="U430:U451" si="26">IF(T430=FALSE, "NA", "")</f>
+        <f t="shared" ref="U430:U469" si="26">IF(T430=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V430" s="2" t="str">
-        <f t="shared" ref="V430:V451" si="27">IF(T430=FALSE, "NA", "")</f>
+        <f t="shared" ref="V430:V469" si="27">IF(T430=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W430" s="2" t="str">
@@ -33088,19 +33088,16 @@
         <v>2.00067899665031</v>
       </c>
       <c r="T444" t="b">
-        <v>0</v>
-      </c>
-      <c r="U444" s="2" t="str">
-        <f t="shared" si="26"/>
-        <v>NA</v>
-      </c>
-      <c r="V444" s="2" t="str">
-        <f t="shared" si="27"/>
-        <v>NA</v>
-      </c>
-      <c r="W444" s="2" t="str">
-        <f t="shared" si="25"/>
-        <v>NA</v>
+        <v>1</v>
+      </c>
+      <c r="U444" s="2">
+        <v>144</v>
+      </c>
+      <c r="V444" s="2">
+        <v>6</v>
+      </c>
+      <c r="W444" s="2" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="445" spans="1:23" x14ac:dyDescent="0.2">
@@ -33621,8 +33618,1339 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="452" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A452" s="10">
+        <v>451</v>
+      </c>
+      <c r="B452" s="7">
+        <v>0</v>
+      </c>
+      <c r="C452" s="7">
+        <v>0</v>
+      </c>
+      <c r="D452" s="7">
+        <v>0</v>
+      </c>
+      <c r="E452" s="7">
+        <v>0</v>
+      </c>
+      <c r="F452" s="7">
+        <v>0</v>
+      </c>
+      <c r="G452" s="7">
+        <v>8.7862879550550907</v>
+      </c>
+      <c r="H452" s="7">
+        <v>0</v>
+      </c>
+      <c r="I452" s="7">
+        <v>0</v>
+      </c>
+      <c r="J452" s="7">
+        <v>0</v>
+      </c>
+      <c r="K452" s="7">
+        <v>8.3553149699179698</v>
+      </c>
+      <c r="L452" s="7">
+        <v>0</v>
+      </c>
+      <c r="M452" s="7">
+        <v>0</v>
+      </c>
+      <c r="N452" s="7">
+        <v>0</v>
+      </c>
+      <c r="O452" s="7">
+        <v>0.61691697469230999</v>
+      </c>
+      <c r="P452" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q452" s="7">
+        <v>0</v>
+      </c>
+      <c r="R452" s="7">
+        <v>0</v>
+      </c>
+      <c r="S452" s="7">
+        <v>1.49946822017785</v>
+      </c>
+      <c r="T452" t="b">
+        <v>0</v>
+      </c>
+      <c r="U452" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V452" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W452" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="453" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A453" s="10">
+        <v>452</v>
+      </c>
+      <c r="B453" s="7">
+        <v>0</v>
+      </c>
+      <c r="C453" s="7">
+        <v>0</v>
+      </c>
+      <c r="D453" s="7">
+        <v>11.056568414900401</v>
+      </c>
+      <c r="E453" s="7">
+        <v>0</v>
+      </c>
+      <c r="F453" s="7">
+        <v>0</v>
+      </c>
+      <c r="G453" s="7">
+        <v>13.297140426555099</v>
+      </c>
+      <c r="H453" s="7">
+        <v>0</v>
+      </c>
+      <c r="I453" s="7">
+        <v>0</v>
+      </c>
+      <c r="J453" s="7">
+        <v>0</v>
+      </c>
+      <c r="K453" s="7">
+        <v>0</v>
+      </c>
+      <c r="L453" s="7">
+        <v>0</v>
+      </c>
+      <c r="M453" s="7">
+        <v>0</v>
+      </c>
+      <c r="N453" s="7">
+        <v>0</v>
+      </c>
+      <c r="O453" s="7">
+        <v>1.65660849444181</v>
+      </c>
+      <c r="P453" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q453" s="7">
+        <v>0</v>
+      </c>
+      <c r="R453" s="7">
+        <v>0</v>
+      </c>
+      <c r="S453" s="7">
+        <v>1.92489004437684</v>
+      </c>
+      <c r="T453" t="b">
+        <v>1</v>
+      </c>
+      <c r="U453" s="2">
+        <v>28</v>
+      </c>
+      <c r="V453" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="W453" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+    </row>
+    <row r="454" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A454" s="10">
+        <v>453</v>
+      </c>
+      <c r="B454" s="7">
+        <v>0</v>
+      </c>
+      <c r="C454" s="7">
+        <v>12.7260988185909</v>
+      </c>
+      <c r="D454" s="7">
+        <v>0</v>
+      </c>
+      <c r="E454" s="7">
+        <v>0</v>
+      </c>
+      <c r="F454" s="7">
+        <v>0</v>
+      </c>
+      <c r="G454" s="7">
+        <v>13.564166033197999</v>
+      </c>
+      <c r="H454" s="7">
+        <v>0</v>
+      </c>
+      <c r="I454" s="7">
+        <v>0</v>
+      </c>
+      <c r="J454" s="7">
+        <v>0</v>
+      </c>
+      <c r="K454" s="7">
+        <v>0</v>
+      </c>
+      <c r="L454" s="7">
+        <v>0</v>
+      </c>
+      <c r="M454" s="7">
+        <v>0</v>
+      </c>
+      <c r="N454" s="7">
+        <v>0</v>
+      </c>
+      <c r="O454" s="7">
+        <v>1.16438361569696</v>
+      </c>
+      <c r="P454" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q454" s="7">
+        <v>0</v>
+      </c>
+      <c r="R454" s="7">
+        <v>0</v>
+      </c>
+      <c r="S454" s="7">
+        <v>4.9417066792347804</v>
+      </c>
+      <c r="T454" t="b">
+        <v>0</v>
+      </c>
+      <c r="U454" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V454" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W454" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="455" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A455" s="10">
+        <v>454</v>
+      </c>
+      <c r="B455" s="7">
+        <v>4.9689529290191397</v>
+      </c>
+      <c r="C455" s="7">
+        <v>0</v>
+      </c>
+      <c r="D455" s="7">
+        <v>0</v>
+      </c>
+      <c r="E455" s="7">
+        <v>0</v>
+      </c>
+      <c r="F455" s="7">
+        <v>0</v>
+      </c>
+      <c r="G455" s="7">
+        <v>0</v>
+      </c>
+      <c r="H455" s="7">
+        <v>0</v>
+      </c>
+      <c r="I455" s="7">
+        <v>0</v>
+      </c>
+      <c r="J455" s="7">
+        <v>0</v>
+      </c>
+      <c r="K455" s="7">
+        <v>0</v>
+      </c>
+      <c r="L455" s="7">
+        <v>8.4717592967772699</v>
+      </c>
+      <c r="M455" s="7">
+        <v>0</v>
+      </c>
+      <c r="N455" s="7">
+        <v>0</v>
+      </c>
+      <c r="O455" s="7">
+        <v>1.1298957874123901</v>
+      </c>
+      <c r="P455" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q455" s="7">
+        <v>0</v>
+      </c>
+      <c r="R455" s="7">
+        <v>0</v>
+      </c>
+      <c r="S455" s="7">
+        <v>5.6430075980734298</v>
+      </c>
+      <c r="T455" t="b">
+        <v>0</v>
+      </c>
+      <c r="U455" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V455" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W455" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="456" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A456" s="10">
+        <v>455</v>
+      </c>
+      <c r="B456" s="7">
+        <v>0</v>
+      </c>
+      <c r="C456" s="7">
+        <v>0</v>
+      </c>
+      <c r="D456" s="7">
+        <v>0</v>
+      </c>
+      <c r="E456" s="7">
+        <v>0</v>
+      </c>
+      <c r="F456" s="7">
+        <v>0</v>
+      </c>
+      <c r="G456" s="7">
+        <v>0</v>
+      </c>
+      <c r="H456" s="7">
+        <v>0</v>
+      </c>
+      <c r="I456" s="7">
+        <v>6.7615234700401698</v>
+      </c>
+      <c r="J456" s="7">
+        <v>0</v>
+      </c>
+      <c r="K456" s="7">
+        <v>0</v>
+      </c>
+      <c r="L456" s="7">
+        <v>0</v>
+      </c>
+      <c r="M456" s="7">
+        <v>11.0306348347032</v>
+      </c>
+      <c r="N456" s="7">
+        <v>0</v>
+      </c>
+      <c r="O456" s="7">
+        <v>0.87576677369884803</v>
+      </c>
+      <c r="P456" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q456" s="7">
+        <v>0</v>
+      </c>
+      <c r="R456" s="7">
+        <v>0</v>
+      </c>
+      <c r="S456" s="7">
+        <v>3.8453207764706399</v>
+      </c>
+      <c r="T456" t="b">
+        <v>0</v>
+      </c>
+      <c r="U456" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V456" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W456" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="457" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A457" s="10">
+        <v>456</v>
+      </c>
+      <c r="B457" s="7">
+        <v>0</v>
+      </c>
+      <c r="C457" s="7">
+        <v>0</v>
+      </c>
+      <c r="D457" s="7">
+        <v>0</v>
+      </c>
+      <c r="E457" s="7">
+        <v>0</v>
+      </c>
+      <c r="F457" s="7">
+        <v>0</v>
+      </c>
+      <c r="G457" s="7">
+        <v>0</v>
+      </c>
+      <c r="H457" s="7">
+        <v>11.8211424070065</v>
+      </c>
+      <c r="I457" s="7">
+        <v>0</v>
+      </c>
+      <c r="J457" s="7">
+        <v>0</v>
+      </c>
+      <c r="K457" s="7">
+        <v>0</v>
+      </c>
+      <c r="L457" s="7">
+        <v>9.3288969456214605</v>
+      </c>
+      <c r="M457" s="7">
+        <v>0</v>
+      </c>
+      <c r="N457" s="7">
+        <v>0</v>
+      </c>
+      <c r="O457" s="7">
+        <v>1.9431148747527001</v>
+      </c>
+      <c r="P457" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q457" s="7">
+        <v>0</v>
+      </c>
+      <c r="R457" s="7">
+        <v>0</v>
+      </c>
+      <c r="S457" s="7">
+        <v>1.89690813805651</v>
+      </c>
+      <c r="T457" t="b">
+        <v>0</v>
+      </c>
+      <c r="U457" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V457" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W457" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="458" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A458" s="10">
+        <v>457</v>
+      </c>
+      <c r="B458" s="7">
+        <v>0</v>
+      </c>
+      <c r="C458" s="7">
+        <v>0</v>
+      </c>
+      <c r="D458" s="7">
+        <v>0</v>
+      </c>
+      <c r="E458" s="7">
+        <v>8.8696997743585406</v>
+      </c>
+      <c r="F458" s="7">
+        <v>0</v>
+      </c>
+      <c r="G458" s="7">
+        <v>8.4691846268438304</v>
+      </c>
+      <c r="H458" s="7">
+        <v>0</v>
+      </c>
+      <c r="I458" s="7">
+        <v>0</v>
+      </c>
+      <c r="J458" s="7">
+        <v>0</v>
+      </c>
+      <c r="K458" s="7">
+        <v>0</v>
+      </c>
+      <c r="L458" s="7">
+        <v>0</v>
+      </c>
+      <c r="M458" s="7">
+        <v>0</v>
+      </c>
+      <c r="N458" s="7">
+        <v>0</v>
+      </c>
+      <c r="O458" s="7">
+        <v>1.26293092997726</v>
+      </c>
+      <c r="P458" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q458" s="7">
+        <v>0</v>
+      </c>
+      <c r="R458" s="7">
+        <v>0</v>
+      </c>
+      <c r="S458" s="7">
+        <v>2.7472521425004</v>
+      </c>
+      <c r="T458" t="b">
+        <v>0</v>
+      </c>
+      <c r="U458" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V458" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W458" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="459" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A459" s="10">
+        <v>458</v>
+      </c>
+      <c r="B459" s="7">
+        <v>0</v>
+      </c>
+      <c r="C459" s="7">
+        <v>0</v>
+      </c>
+      <c r="D459" s="7">
+        <v>0</v>
+      </c>
+      <c r="E459" s="7">
+        <v>0</v>
+      </c>
+      <c r="F459" s="7">
+        <v>11.617754122333601</v>
+      </c>
+      <c r="G459" s="7">
+        <v>0</v>
+      </c>
+      <c r="H459" s="7">
+        <v>11.857810608795001</v>
+      </c>
+      <c r="I459" s="7">
+        <v>0</v>
+      </c>
+      <c r="J459" s="7">
+        <v>0</v>
+      </c>
+      <c r="K459" s="7">
+        <v>0</v>
+      </c>
+      <c r="L459" s="7">
+        <v>0</v>
+      </c>
+      <c r="M459" s="7">
+        <v>0</v>
+      </c>
+      <c r="N459" s="7">
+        <v>0</v>
+      </c>
+      <c r="O459" s="7">
+        <v>1.10474974891893</v>
+      </c>
+      <c r="P459" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q459" s="7">
+        <v>0</v>
+      </c>
+      <c r="R459" s="7">
+        <v>0</v>
+      </c>
+      <c r="S459" s="7">
+        <v>3.8017108876322099</v>
+      </c>
+      <c r="T459" t="b">
+        <v>0</v>
+      </c>
+      <c r="U459" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V459" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W459" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="460" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A460" s="10">
+        <v>459</v>
+      </c>
+      <c r="B460" s="7">
+        <v>0</v>
+      </c>
+      <c r="C460" s="7">
+        <v>7.4695665348034597</v>
+      </c>
+      <c r="D460" s="7">
+        <v>0</v>
+      </c>
+      <c r="E460" s="7">
+        <v>0</v>
+      </c>
+      <c r="F460" s="7">
+        <v>0</v>
+      </c>
+      <c r="G460" s="7">
+        <v>0</v>
+      </c>
+      <c r="H460" s="7">
+        <v>0</v>
+      </c>
+      <c r="I460" s="7">
+        <v>0</v>
+      </c>
+      <c r="J460" s="7">
+        <v>0</v>
+      </c>
+      <c r="K460" s="7">
+        <v>0</v>
+      </c>
+      <c r="L460" s="7">
+        <v>10.478740362995699</v>
+      </c>
+      <c r="M460" s="7">
+        <v>0</v>
+      </c>
+      <c r="N460" s="7">
+        <v>0</v>
+      </c>
+      <c r="O460" s="7">
+        <v>1.58635262013391</v>
+      </c>
+      <c r="P460" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q460" s="7">
+        <v>0</v>
+      </c>
+      <c r="R460" s="7">
+        <v>0</v>
+      </c>
+      <c r="S460" s="7">
+        <v>2.0416945759131</v>
+      </c>
+      <c r="T460" t="b">
+        <v>0</v>
+      </c>
+      <c r="U460" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V460" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W460" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="461" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A461" s="10">
+        <v>460</v>
+      </c>
+      <c r="B461" s="7">
+        <v>0</v>
+      </c>
+      <c r="C461" s="7">
+        <v>0</v>
+      </c>
+      <c r="D461" s="7">
+        <v>0</v>
+      </c>
+      <c r="E461" s="7">
+        <v>10.8582440325451</v>
+      </c>
+      <c r="F461" s="7">
+        <v>0</v>
+      </c>
+      <c r="G461" s="7">
+        <v>0</v>
+      </c>
+      <c r="H461" s="7">
+        <v>0</v>
+      </c>
+      <c r="I461" s="7">
+        <v>9.9614211238618804</v>
+      </c>
+      <c r="J461" s="7">
+        <v>0</v>
+      </c>
+      <c r="K461" s="7">
+        <v>0</v>
+      </c>
+      <c r="L461" s="7">
+        <v>0</v>
+      </c>
+      <c r="M461" s="7">
+        <v>0</v>
+      </c>
+      <c r="N461" s="7">
+        <v>0</v>
+      </c>
+      <c r="O461" s="7">
+        <v>1.79708757195039</v>
+      </c>
+      <c r="P461" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q461" s="7">
+        <v>0</v>
+      </c>
+      <c r="R461" s="7">
+        <v>0</v>
+      </c>
+      <c r="S461" s="7">
+        <v>1.7307108764064301</v>
+      </c>
+      <c r="T461" t="b">
+        <v>0</v>
+      </c>
+      <c r="U461" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V461" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W461" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="462" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A462" s="10">
+        <v>461</v>
+      </c>
+      <c r="B462" s="7">
+        <v>0</v>
+      </c>
+      <c r="C462" s="7">
+        <v>0</v>
+      </c>
+      <c r="D462" s="7">
+        <v>0</v>
+      </c>
+      <c r="E462" s="7">
+        <v>0</v>
+      </c>
+      <c r="F462" s="7">
+        <v>9.3729236712160109</v>
+      </c>
+      <c r="G462" s="7">
+        <v>0</v>
+      </c>
+      <c r="H462" s="7">
+        <v>0</v>
+      </c>
+      <c r="I462" s="7">
+        <v>0</v>
+      </c>
+      <c r="J462" s="7">
+        <v>0</v>
+      </c>
+      <c r="K462" s="7">
+        <v>12.5254661919803</v>
+      </c>
+      <c r="L462" s="7">
+        <v>0</v>
+      </c>
+      <c r="M462" s="7">
+        <v>0</v>
+      </c>
+      <c r="N462" s="7">
+        <v>0</v>
+      </c>
+      <c r="O462" s="7">
+        <v>1.66243556337397</v>
+      </c>
+      <c r="P462" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q462" s="7">
+        <v>0</v>
+      </c>
+      <c r="R462" s="7">
+        <v>0</v>
+      </c>
+      <c r="S462" s="7">
+        <v>2.03484060172859</v>
+      </c>
+      <c r="T462" t="b">
+        <v>0</v>
+      </c>
+      <c r="U462" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V462" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W462" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="463" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A463" s="10">
+        <v>462</v>
+      </c>
+      <c r="B463" s="7">
+        <v>7.1702593395934304</v>
+      </c>
+      <c r="C463" s="7">
+        <v>0</v>
+      </c>
+      <c r="D463" s="7">
+        <v>0</v>
+      </c>
+      <c r="E463" s="7">
+        <v>0</v>
+      </c>
+      <c r="F463" s="7">
+        <v>0</v>
+      </c>
+      <c r="G463" s="7">
+        <v>8.8951657666798791</v>
+      </c>
+      <c r="H463" s="7">
+        <v>0</v>
+      </c>
+      <c r="I463" s="7">
+        <v>0</v>
+      </c>
+      <c r="J463" s="7">
+        <v>0</v>
+      </c>
+      <c r="K463" s="7">
+        <v>0</v>
+      </c>
+      <c r="L463" s="7">
+        <v>0</v>
+      </c>
+      <c r="M463" s="7">
+        <v>0</v>
+      </c>
+      <c r="N463" s="7">
+        <v>0</v>
+      </c>
+      <c r="O463" s="7">
+        <v>1.33146640279092</v>
+      </c>
+      <c r="P463" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q463" s="7">
+        <v>0</v>
+      </c>
+      <c r="R463" s="7">
+        <v>0</v>
+      </c>
+      <c r="S463" s="7">
+        <v>4.5446024869948802</v>
+      </c>
+      <c r="T463" t="b">
+        <v>0</v>
+      </c>
+      <c r="U463" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V463" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W463" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="464" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A464" s="10">
+        <v>463</v>
+      </c>
+      <c r="B464" s="7">
+        <v>0</v>
+      </c>
+      <c r="C464" s="7">
+        <v>0</v>
+      </c>
+      <c r="D464" s="7">
+        <v>0</v>
+      </c>
+      <c r="E464" s="7">
+        <v>0</v>
+      </c>
+      <c r="F464" s="7">
+        <v>0</v>
+      </c>
+      <c r="G464" s="7">
+        <v>8.5182127644925298</v>
+      </c>
+      <c r="H464" s="7">
+        <v>0</v>
+      </c>
+      <c r="I464" s="7">
+        <v>0</v>
+      </c>
+      <c r="J464" s="7">
+        <v>8.9418308811445808</v>
+      </c>
+      <c r="K464" s="7">
+        <v>0</v>
+      </c>
+      <c r="L464" s="7">
+        <v>0</v>
+      </c>
+      <c r="M464" s="7">
+        <v>0</v>
+      </c>
+      <c r="N464" s="7">
+        <v>0</v>
+      </c>
+      <c r="O464" s="7">
+        <v>1.8950681041998001</v>
+      </c>
+      <c r="P464" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q464" s="7">
+        <v>0</v>
+      </c>
+      <c r="R464" s="7">
+        <v>0</v>
+      </c>
+      <c r="S464" s="7">
+        <v>4.3458235025962102</v>
+      </c>
+      <c r="T464" t="b">
+        <v>0</v>
+      </c>
+      <c r="U464" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V464" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W464" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="465" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A465" s="10">
+        <v>464</v>
+      </c>
+      <c r="B465" s="7">
+        <v>0</v>
+      </c>
+      <c r="C465" s="7">
+        <v>0</v>
+      </c>
+      <c r="D465" s="7">
+        <v>0</v>
+      </c>
+      <c r="E465" s="7">
+        <v>0</v>
+      </c>
+      <c r="F465" s="7">
+        <v>0</v>
+      </c>
+      <c r="G465" s="7">
+        <v>0</v>
+      </c>
+      <c r="H465" s="7">
+        <v>0</v>
+      </c>
+      <c r="I465" s="7">
+        <v>0</v>
+      </c>
+      <c r="J465" s="7">
+        <v>12.377885235959599</v>
+      </c>
+      <c r="K465" s="7">
+        <v>0</v>
+      </c>
+      <c r="L465" s="7">
+        <v>0</v>
+      </c>
+      <c r="M465" s="7">
+        <v>9.9365860226203093</v>
+      </c>
+      <c r="N465" s="7">
+        <v>0</v>
+      </c>
+      <c r="O465" s="7">
+        <v>0.78968556186590799</v>
+      </c>
+      <c r="P465" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q465" s="7">
+        <v>0</v>
+      </c>
+      <c r="R465" s="7">
+        <v>0</v>
+      </c>
+      <c r="S465" s="7">
+        <v>5.14665732118275</v>
+      </c>
+      <c r="T465" t="b">
+        <v>0</v>
+      </c>
+      <c r="U465" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V465" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W465" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="466" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A466" s="10">
+        <v>465</v>
+      </c>
+      <c r="B466" s="7">
+        <v>0</v>
+      </c>
+      <c r="C466" s="7">
+        <v>0</v>
+      </c>
+      <c r="D466" s="7">
+        <v>0</v>
+      </c>
+      <c r="E466" s="7">
+        <v>0</v>
+      </c>
+      <c r="F466" s="7">
+        <v>0</v>
+      </c>
+      <c r="G466" s="7">
+        <v>0</v>
+      </c>
+      <c r="H466" s="7">
+        <v>9.4788693879642505</v>
+      </c>
+      <c r="I466" s="7">
+        <v>0</v>
+      </c>
+      <c r="J466" s="7">
+        <v>12.7075055096014</v>
+      </c>
+      <c r="K466" s="7">
+        <v>0</v>
+      </c>
+      <c r="L466" s="7">
+        <v>0</v>
+      </c>
+      <c r="M466" s="7">
+        <v>0</v>
+      </c>
+      <c r="N466" s="7">
+        <v>0</v>
+      </c>
+      <c r="O466" s="7">
+        <v>1.59307703370247</v>
+      </c>
+      <c r="P466" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q466" s="7">
+        <v>0</v>
+      </c>
+      <c r="R466" s="7">
+        <v>0</v>
+      </c>
+      <c r="S466" s="7">
+        <v>2.9053818698942599</v>
+      </c>
+      <c r="T466" t="b">
+        <v>0</v>
+      </c>
+      <c r="U466" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V466" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W466" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="467" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A467" s="10">
+        <v>466</v>
+      </c>
+      <c r="B467" s="7">
+        <v>0</v>
+      </c>
+      <c r="C467" s="7">
+        <v>0</v>
+      </c>
+      <c r="D467" s="7">
+        <v>0</v>
+      </c>
+      <c r="E467" s="7">
+        <v>0</v>
+      </c>
+      <c r="F467" s="7">
+        <v>12.0476849101059</v>
+      </c>
+      <c r="G467" s="7">
+        <v>0</v>
+      </c>
+      <c r="H467" s="7">
+        <v>0</v>
+      </c>
+      <c r="I467" s="7">
+        <v>0</v>
+      </c>
+      <c r="J467" s="7">
+        <v>8.5750533782792999</v>
+      </c>
+      <c r="K467" s="7">
+        <v>0</v>
+      </c>
+      <c r="L467" s="7">
+        <v>0</v>
+      </c>
+      <c r="M467" s="7">
+        <v>0</v>
+      </c>
+      <c r="N467" s="7">
+        <v>0</v>
+      </c>
+      <c r="O467" s="7">
+        <v>2.3280965563595899</v>
+      </c>
+      <c r="P467" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q467" s="7">
+        <v>0</v>
+      </c>
+      <c r="R467" s="7">
+        <v>0</v>
+      </c>
+      <c r="S467" s="7">
+        <v>1.9636027887060701</v>
+      </c>
+      <c r="T467" t="b">
+        <v>0</v>
+      </c>
+      <c r="U467" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V467" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W467" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="468" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A468" s="10">
+        <v>467</v>
+      </c>
+      <c r="B468" s="7">
+        <v>4.1790936276505599</v>
+      </c>
+      <c r="C468" s="7">
+        <v>0</v>
+      </c>
+      <c r="D468" s="7">
+        <v>0</v>
+      </c>
+      <c r="E468" s="7">
+        <v>0</v>
+      </c>
+      <c r="F468" s="7">
+        <v>0</v>
+      </c>
+      <c r="G468" s="7">
+        <v>0</v>
+      </c>
+      <c r="H468" s="7">
+        <v>10.2395466631956</v>
+      </c>
+      <c r="I468" s="7">
+        <v>0</v>
+      </c>
+      <c r="J468" s="7">
+        <v>0</v>
+      </c>
+      <c r="K468" s="7">
+        <v>0</v>
+      </c>
+      <c r="L468" s="7">
+        <v>0</v>
+      </c>
+      <c r="M468" s="7">
+        <v>0</v>
+      </c>
+      <c r="N468" s="7">
+        <v>0</v>
+      </c>
+      <c r="O468" s="7">
+        <v>1.26088932584558</v>
+      </c>
+      <c r="P468" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q468" s="7">
+        <v>0</v>
+      </c>
+      <c r="R468" s="7">
+        <v>0</v>
+      </c>
+      <c r="S468" s="7">
+        <v>4.0921357431094298</v>
+      </c>
+      <c r="T468" t="b">
+        <v>0</v>
+      </c>
+      <c r="U468" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V468" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W468" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="469" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A469" s="10">
+        <v>468</v>
+      </c>
+      <c r="B469" s="7">
+        <v>0</v>
+      </c>
+      <c r="C469" s="7">
+        <v>0</v>
+      </c>
+      <c r="D469" s="7">
+        <v>11.445720657839701</v>
+      </c>
+      <c r="E469" s="7">
+        <v>0</v>
+      </c>
+      <c r="F469" s="7">
+        <v>0</v>
+      </c>
+      <c r="G469" s="7">
+        <v>0</v>
+      </c>
+      <c r="H469" s="7">
+        <v>0</v>
+      </c>
+      <c r="I469" s="7">
+        <v>0</v>
+      </c>
+      <c r="J469" s="7">
+        <v>0</v>
+      </c>
+      <c r="K469" s="7">
+        <v>11.429753134034099</v>
+      </c>
+      <c r="L469" s="7">
+        <v>0</v>
+      </c>
+      <c r="M469" s="7">
+        <v>0</v>
+      </c>
+      <c r="N469" s="7">
+        <v>0</v>
+      </c>
+      <c r="O469" s="7">
+        <v>1.9223401706480701</v>
+      </c>
+      <c r="P469" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q469" s="7">
+        <v>0</v>
+      </c>
+      <c r="R469" s="7">
+        <v>0</v>
+      </c>
+      <c r="S469" s="7">
+        <v>2.8941136897493802</v>
+      </c>
+      <c r="T469" t="b">
+        <v>0</v>
+      </c>
+      <c r="U469" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V469" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W469" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W451">
+  <conditionalFormatting sqref="A1:W469">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Dataset updated till S486
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E32707-40B8-2247-AA64-1868F1F2D02C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0893FAE-81B1-1647-ADB3-4D0B86EF8AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-5300" windowWidth="38400" windowHeight="21600" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -368,7 +368,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -699,11 +709,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W469"/>
+  <dimension ref="A1:W487"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A416" zoomScale="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A421" zoomScale="59" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W454" sqref="W454"/>
+      <selection pane="topRight" activeCell="W487" sqref="W487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -31545,7 +31555,7 @@
         <v>NA</v>
       </c>
       <c r="W423" s="2" t="str">
-        <f t="shared" ref="W423:W469" si="25">IF(T423=FALSE, "NA", "")</f>
+        <f t="shared" ref="W423:W486" si="25">IF(T423=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -32055,11 +32065,11 @@
         <v>0</v>
       </c>
       <c r="U430" s="2" t="str">
-        <f t="shared" ref="U430:U469" si="26">IF(T430=FALSE, "NA", "")</f>
+        <f t="shared" ref="U430:U487" si="26">IF(T430=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V430" s="2" t="str">
-        <f t="shared" ref="V430:V469" si="27">IF(T430=FALSE, "NA", "")</f>
+        <f t="shared" ref="V430:V487" si="27">IF(T430=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W430" s="2" t="str">
@@ -34947,8 +34957,1339 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="470" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A470" s="10">
+        <v>469</v>
+      </c>
+      <c r="B470" s="7">
+        <v>0</v>
+      </c>
+      <c r="C470" s="7">
+        <v>0</v>
+      </c>
+      <c r="D470" s="7">
+        <v>11.7303788332629</v>
+      </c>
+      <c r="E470" s="7">
+        <v>0</v>
+      </c>
+      <c r="F470" s="7">
+        <v>0</v>
+      </c>
+      <c r="G470" s="7">
+        <v>0</v>
+      </c>
+      <c r="H470" s="7">
+        <v>0</v>
+      </c>
+      <c r="I470" s="7">
+        <v>0</v>
+      </c>
+      <c r="J470" s="7">
+        <v>0</v>
+      </c>
+      <c r="K470" s="7">
+        <v>12.8041045510343</v>
+      </c>
+      <c r="L470" s="7">
+        <v>0</v>
+      </c>
+      <c r="M470" s="7">
+        <v>0</v>
+      </c>
+      <c r="N470" s="7">
+        <v>0</v>
+      </c>
+      <c r="O470" s="7">
+        <v>2.6532170482004598</v>
+      </c>
+      <c r="P470" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q470" s="7">
+        <v>0</v>
+      </c>
+      <c r="R470" s="7">
+        <v>2.0350037931814602</v>
+      </c>
+      <c r="S470" s="7">
+        <v>0</v>
+      </c>
+      <c r="T470" t="b">
+        <v>0</v>
+      </c>
+      <c r="U470" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V470" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W470" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="471" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A471" s="10">
+        <v>470</v>
+      </c>
+      <c r="B471" s="7">
+        <v>0</v>
+      </c>
+      <c r="C471" s="7">
+        <v>0</v>
+      </c>
+      <c r="D471" s="7">
+        <v>0</v>
+      </c>
+      <c r="E471" s="7">
+        <v>0</v>
+      </c>
+      <c r="F471" s="7">
+        <v>0</v>
+      </c>
+      <c r="G471" s="7">
+        <v>0</v>
+      </c>
+      <c r="H471" s="7">
+        <v>0</v>
+      </c>
+      <c r="I471" s="7">
+        <v>10.029003479209701</v>
+      </c>
+      <c r="J471" s="7">
+        <v>8.0811392576501895</v>
+      </c>
+      <c r="K471" s="7">
+        <v>0</v>
+      </c>
+      <c r="L471" s="7">
+        <v>0</v>
+      </c>
+      <c r="M471" s="7">
+        <v>0</v>
+      </c>
+      <c r="N471" s="7">
+        <v>0</v>
+      </c>
+      <c r="O471" s="7">
+        <v>2.1189266564018001</v>
+      </c>
+      <c r="P471" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q471" s="7">
+        <v>0</v>
+      </c>
+      <c r="R471" s="7">
+        <v>5.0844250706352296</v>
+      </c>
+      <c r="S471" s="7">
+        <v>0</v>
+      </c>
+      <c r="T471" t="b">
+        <v>0</v>
+      </c>
+      <c r="U471" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V471" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W471" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="472" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A472" s="10">
+        <v>471</v>
+      </c>
+      <c r="B472" s="7">
+        <v>0</v>
+      </c>
+      <c r="C472" s="7">
+        <v>7.5713286399087796</v>
+      </c>
+      <c r="D472" s="7">
+        <v>0</v>
+      </c>
+      <c r="E472" s="7">
+        <v>0</v>
+      </c>
+      <c r="F472" s="7">
+        <v>0</v>
+      </c>
+      <c r="G472" s="7">
+        <v>0</v>
+      </c>
+      <c r="H472" s="7">
+        <v>0</v>
+      </c>
+      <c r="I472" s="7">
+        <v>0</v>
+      </c>
+      <c r="J472" s="7">
+        <v>0</v>
+      </c>
+      <c r="K472" s="7">
+        <v>0</v>
+      </c>
+      <c r="L472" s="7">
+        <v>9.7032161926805607</v>
+      </c>
+      <c r="M472" s="7">
+        <v>0</v>
+      </c>
+      <c r="N472" s="7">
+        <v>0</v>
+      </c>
+      <c r="O472" s="7">
+        <v>2.0157111001987098</v>
+      </c>
+      <c r="P472" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q472" s="7">
+        <v>0</v>
+      </c>
+      <c r="R472" s="7">
+        <v>3.3065605732323</v>
+      </c>
+      <c r="S472" s="7">
+        <v>0</v>
+      </c>
+      <c r="T472" t="b">
+        <v>0</v>
+      </c>
+      <c r="U472" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V472" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W472" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="473" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A473" s="10">
+        <v>472</v>
+      </c>
+      <c r="B473" s="7">
+        <v>0</v>
+      </c>
+      <c r="C473" s="7">
+        <v>0</v>
+      </c>
+      <c r="D473" s="7">
+        <v>9.4627024388682592</v>
+      </c>
+      <c r="E473" s="7">
+        <v>0</v>
+      </c>
+      <c r="F473" s="7">
+        <v>0</v>
+      </c>
+      <c r="G473" s="7">
+        <v>0</v>
+      </c>
+      <c r="H473" s="7">
+        <v>7.9855587188466703</v>
+      </c>
+      <c r="I473" s="7">
+        <v>0</v>
+      </c>
+      <c r="J473" s="7">
+        <v>0</v>
+      </c>
+      <c r="K473" s="7">
+        <v>0</v>
+      </c>
+      <c r="L473" s="7">
+        <v>0</v>
+      </c>
+      <c r="M473" s="7">
+        <v>0</v>
+      </c>
+      <c r="N473" s="7">
+        <v>0</v>
+      </c>
+      <c r="O473" s="7">
+        <v>2.42281512185974</v>
+      </c>
+      <c r="P473" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q473" s="7">
+        <v>0</v>
+      </c>
+      <c r="R473" s="7">
+        <v>3.6379654455938102</v>
+      </c>
+      <c r="S473" s="7">
+        <v>0</v>
+      </c>
+      <c r="T473" t="b">
+        <v>0</v>
+      </c>
+      <c r="U473" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V473" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W473" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="474" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A474" s="10">
+        <v>473</v>
+      </c>
+      <c r="B474" s="7">
+        <v>0</v>
+      </c>
+      <c r="C474" s="7">
+        <v>9.0544874983586006</v>
+      </c>
+      <c r="D474" s="7">
+        <v>0</v>
+      </c>
+      <c r="E474" s="7">
+        <v>0</v>
+      </c>
+      <c r="F474" s="7">
+        <v>0</v>
+      </c>
+      <c r="G474" s="7">
+        <v>0</v>
+      </c>
+      <c r="H474" s="7">
+        <v>11.559125330634499</v>
+      </c>
+      <c r="I474" s="7">
+        <v>0</v>
+      </c>
+      <c r="J474" s="7">
+        <v>0</v>
+      </c>
+      <c r="K474" s="7">
+        <v>0</v>
+      </c>
+      <c r="L474" s="7">
+        <v>0</v>
+      </c>
+      <c r="M474" s="7">
+        <v>0</v>
+      </c>
+      <c r="N474" s="7">
+        <v>0</v>
+      </c>
+      <c r="O474" s="7">
+        <v>2.1426318638310899</v>
+      </c>
+      <c r="P474" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q474" s="7">
+        <v>0</v>
+      </c>
+      <c r="R474" s="7">
+        <v>3.7984114931359398</v>
+      </c>
+      <c r="S474" s="7">
+        <v>0</v>
+      </c>
+      <c r="T474" t="b">
+        <v>0</v>
+      </c>
+      <c r="U474" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V474" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W474" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="475" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A475" s="10">
+        <v>474</v>
+      </c>
+      <c r="B475" s="7">
+        <v>0</v>
+      </c>
+      <c r="C475" s="7">
+        <v>0</v>
+      </c>
+      <c r="D475" s="7">
+        <v>0</v>
+      </c>
+      <c r="E475" s="7">
+        <v>0</v>
+      </c>
+      <c r="F475" s="7">
+        <v>0</v>
+      </c>
+      <c r="G475" s="7">
+        <v>0</v>
+      </c>
+      <c r="H475" s="7">
+        <v>11.4071976571191</v>
+      </c>
+      <c r="I475" s="7">
+        <v>0</v>
+      </c>
+      <c r="J475" s="7">
+        <v>0</v>
+      </c>
+      <c r="K475" s="7">
+        <v>9.0167259459227207</v>
+      </c>
+      <c r="L475" s="7">
+        <v>0</v>
+      </c>
+      <c r="M475" s="7">
+        <v>0</v>
+      </c>
+      <c r="N475" s="7">
+        <v>0</v>
+      </c>
+      <c r="O475" s="7">
+        <v>1.80535522487283</v>
+      </c>
+      <c r="P475" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q475" s="7">
+        <v>0</v>
+      </c>
+      <c r="R475" s="7">
+        <v>3.6965046559514301</v>
+      </c>
+      <c r="S475" s="7">
+        <v>0</v>
+      </c>
+      <c r="T475" t="b">
+        <v>0</v>
+      </c>
+      <c r="U475" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V475" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W475" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="476" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A476" s="10">
+        <v>475</v>
+      </c>
+      <c r="B476" s="7">
+        <v>0</v>
+      </c>
+      <c r="C476" s="7">
+        <v>0</v>
+      </c>
+      <c r="D476" s="7">
+        <v>7.4256041713668903</v>
+      </c>
+      <c r="E476" s="7">
+        <v>0</v>
+      </c>
+      <c r="F476" s="7">
+        <v>0</v>
+      </c>
+      <c r="G476" s="7">
+        <v>11.730697409846099</v>
+      </c>
+      <c r="H476" s="7">
+        <v>0</v>
+      </c>
+      <c r="I476" s="7">
+        <v>0</v>
+      </c>
+      <c r="J476" s="7">
+        <v>0</v>
+      </c>
+      <c r="K476" s="7">
+        <v>0</v>
+      </c>
+      <c r="L476" s="7">
+        <v>0</v>
+      </c>
+      <c r="M476" s="7">
+        <v>0</v>
+      </c>
+      <c r="N476" s="7">
+        <v>0</v>
+      </c>
+      <c r="O476" s="7">
+        <v>1.5855023186517401</v>
+      </c>
+      <c r="P476" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q476" s="7">
+        <v>0</v>
+      </c>
+      <c r="R476" s="7">
+        <v>2.9488323378745198</v>
+      </c>
+      <c r="S476" s="7">
+        <v>0</v>
+      </c>
+      <c r="T476" t="b">
+        <v>0</v>
+      </c>
+      <c r="U476" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V476" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W476" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="477" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A477" s="10">
+        <v>476</v>
+      </c>
+      <c r="B477" s="7">
+        <v>0</v>
+      </c>
+      <c r="C477" s="7">
+        <v>0</v>
+      </c>
+      <c r="D477" s="7">
+        <v>0</v>
+      </c>
+      <c r="E477" s="7">
+        <v>11.927716792758799</v>
+      </c>
+      <c r="F477" s="7">
+        <v>0</v>
+      </c>
+      <c r="G477" s="7">
+        <v>0</v>
+      </c>
+      <c r="H477" s="7">
+        <v>8.1209776189564202</v>
+      </c>
+      <c r="I477" s="7">
+        <v>0</v>
+      </c>
+      <c r="J477" s="7">
+        <v>0</v>
+      </c>
+      <c r="K477" s="7">
+        <v>0</v>
+      </c>
+      <c r="L477" s="7">
+        <v>0</v>
+      </c>
+      <c r="M477" s="7">
+        <v>0</v>
+      </c>
+      <c r="N477" s="7">
+        <v>0</v>
+      </c>
+      <c r="O477" s="7">
+        <v>1.3516001549396901</v>
+      </c>
+      <c r="P477" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q477" s="7">
+        <v>0</v>
+      </c>
+      <c r="R477" s="7">
+        <v>3.3932212489975302</v>
+      </c>
+      <c r="S477" s="7">
+        <v>0</v>
+      </c>
+      <c r="T477" t="b">
+        <v>0</v>
+      </c>
+      <c r="U477" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V477" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W477" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="478" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A478" s="10">
+        <v>477</v>
+      </c>
+      <c r="B478" s="7">
+        <v>0</v>
+      </c>
+      <c r="C478" s="7">
+        <v>0</v>
+      </c>
+      <c r="D478" s="7">
+        <v>0</v>
+      </c>
+      <c r="E478" s="7">
+        <v>9.7452857418265708</v>
+      </c>
+      <c r="F478" s="7">
+        <v>0</v>
+      </c>
+      <c r="G478" s="7">
+        <v>0</v>
+      </c>
+      <c r="H478" s="7">
+        <v>0</v>
+      </c>
+      <c r="I478" s="7">
+        <v>0</v>
+      </c>
+      <c r="J478" s="7">
+        <v>0</v>
+      </c>
+      <c r="K478" s="7">
+        <v>0</v>
+      </c>
+      <c r="L478" s="7">
+        <v>0</v>
+      </c>
+      <c r="M478" s="7">
+        <v>10.9092589237934</v>
+      </c>
+      <c r="N478" s="7">
+        <v>0</v>
+      </c>
+      <c r="O478" s="7">
+        <v>1.7564235729593001</v>
+      </c>
+      <c r="P478" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q478" s="7">
+        <v>0</v>
+      </c>
+      <c r="R478" s="7">
+        <v>4.4745201943758302</v>
+      </c>
+      <c r="S478" s="7">
+        <v>0</v>
+      </c>
+      <c r="T478" t="b">
+        <v>1</v>
+      </c>
+      <c r="U478" s="2">
+        <v>1077</v>
+      </c>
+      <c r="V478" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="W478" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v/>
+      </c>
+    </row>
+    <row r="479" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A479" s="10">
+        <v>478</v>
+      </c>
+      <c r="B479" s="7">
+        <v>0</v>
+      </c>
+      <c r="C479" s="7">
+        <v>0</v>
+      </c>
+      <c r="D479" s="7">
+        <v>0</v>
+      </c>
+      <c r="E479" s="7">
+        <v>0</v>
+      </c>
+      <c r="F479" s="7">
+        <v>7.2060916901213998</v>
+      </c>
+      <c r="G479" s="7">
+        <v>0</v>
+      </c>
+      <c r="H479" s="7">
+        <v>0</v>
+      </c>
+      <c r="I479" s="7">
+        <v>0</v>
+      </c>
+      <c r="J479" s="7">
+        <v>0</v>
+      </c>
+      <c r="K479" s="7">
+        <v>11.668864307656101</v>
+      </c>
+      <c r="L479" s="7">
+        <v>0</v>
+      </c>
+      <c r="M479" s="7">
+        <v>0</v>
+      </c>
+      <c r="N479" s="7">
+        <v>0</v>
+      </c>
+      <c r="O479" s="7">
+        <v>1.61636639993692</v>
+      </c>
+      <c r="P479" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q479" s="7">
+        <v>0</v>
+      </c>
+      <c r="R479" s="7">
+        <v>4.4387523119010996</v>
+      </c>
+      <c r="S479" s="7">
+        <v>0</v>
+      </c>
+      <c r="T479" t="b">
+        <v>0</v>
+      </c>
+      <c r="U479" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V479" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W479" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="480" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A480" s="10">
+        <v>479</v>
+      </c>
+      <c r="B480" s="7">
+        <v>0</v>
+      </c>
+      <c r="C480" s="7">
+        <v>0</v>
+      </c>
+      <c r="D480" s="7">
+        <v>0</v>
+      </c>
+      <c r="E480" s="7">
+        <v>0</v>
+      </c>
+      <c r="F480" s="7">
+        <v>13.9916256523163</v>
+      </c>
+      <c r="G480" s="7">
+        <v>0</v>
+      </c>
+      <c r="H480" s="7">
+        <v>0</v>
+      </c>
+      <c r="I480" s="7">
+        <v>9.6145163989736098</v>
+      </c>
+      <c r="J480" s="7">
+        <v>0</v>
+      </c>
+      <c r="K480" s="7">
+        <v>0</v>
+      </c>
+      <c r="L480" s="7">
+        <v>0</v>
+      </c>
+      <c r="M480" s="7">
+        <v>0</v>
+      </c>
+      <c r="N480" s="7">
+        <v>0</v>
+      </c>
+      <c r="O480" s="7">
+        <v>2.19493811559816</v>
+      </c>
+      <c r="P480" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q480" s="7">
+        <v>0</v>
+      </c>
+      <c r="R480" s="7">
+        <v>3.5354707902252001</v>
+      </c>
+      <c r="S480" s="7">
+        <v>0</v>
+      </c>
+      <c r="T480" t="b">
+        <v>0</v>
+      </c>
+      <c r="U480" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V480" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W480" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="481" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A481" s="10">
+        <v>480</v>
+      </c>
+      <c r="B481" s="7">
+        <v>0</v>
+      </c>
+      <c r="C481" s="7">
+        <v>0</v>
+      </c>
+      <c r="D481" s="7">
+        <v>13.004183469568</v>
+      </c>
+      <c r="E481" s="7">
+        <v>13.322080481414099</v>
+      </c>
+      <c r="F481" s="7">
+        <v>0</v>
+      </c>
+      <c r="G481" s="7">
+        <v>0</v>
+      </c>
+      <c r="H481" s="7">
+        <v>0</v>
+      </c>
+      <c r="I481" s="7">
+        <v>0</v>
+      </c>
+      <c r="J481" s="7">
+        <v>0</v>
+      </c>
+      <c r="K481" s="7">
+        <v>0</v>
+      </c>
+      <c r="L481" s="7">
+        <v>0</v>
+      </c>
+      <c r="M481" s="7">
+        <v>0</v>
+      </c>
+      <c r="N481" s="7">
+        <v>0</v>
+      </c>
+      <c r="O481" s="7">
+        <v>2.4498594794288602</v>
+      </c>
+      <c r="P481" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q481" s="7">
+        <v>0</v>
+      </c>
+      <c r="R481" s="7">
+        <v>2.3102425485504599</v>
+      </c>
+      <c r="S481" s="7">
+        <v>0</v>
+      </c>
+      <c r="T481" t="b">
+        <v>0</v>
+      </c>
+      <c r="U481" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V481" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W481" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="482" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A482" s="10">
+        <v>481</v>
+      </c>
+      <c r="B482" s="7">
+        <v>0</v>
+      </c>
+      <c r="C482" s="7">
+        <v>0</v>
+      </c>
+      <c r="D482" s="7">
+        <v>11.1969045523419</v>
+      </c>
+      <c r="E482" s="7">
+        <v>0</v>
+      </c>
+      <c r="F482" s="7">
+        <v>0</v>
+      </c>
+      <c r="G482" s="7">
+        <v>0</v>
+      </c>
+      <c r="H482" s="7">
+        <v>0</v>
+      </c>
+      <c r="I482" s="7">
+        <v>6.7266338640536896</v>
+      </c>
+      <c r="J482" s="7">
+        <v>0</v>
+      </c>
+      <c r="K482" s="7">
+        <v>0</v>
+      </c>
+      <c r="L482" s="7">
+        <v>0</v>
+      </c>
+      <c r="M482" s="7">
+        <v>0</v>
+      </c>
+      <c r="N482" s="7">
+        <v>0</v>
+      </c>
+      <c r="O482" s="7">
+        <v>2.3790703975775398</v>
+      </c>
+      <c r="P482" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q482" s="7">
+        <v>0</v>
+      </c>
+      <c r="R482" s="7">
+        <v>3.0702693052523902</v>
+      </c>
+      <c r="S482" s="7">
+        <v>0</v>
+      </c>
+      <c r="T482" t="b">
+        <v>0</v>
+      </c>
+      <c r="U482" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V482" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W482" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="483" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A483" s="10">
+        <v>482</v>
+      </c>
+      <c r="B483" s="7">
+        <v>0</v>
+      </c>
+      <c r="C483" s="7">
+        <v>0</v>
+      </c>
+      <c r="D483" s="7">
+        <v>0</v>
+      </c>
+      <c r="E483" s="7">
+        <v>0</v>
+      </c>
+      <c r="F483" s="7">
+        <v>0</v>
+      </c>
+      <c r="G483" s="7">
+        <v>0</v>
+      </c>
+      <c r="H483" s="7">
+        <v>0</v>
+      </c>
+      <c r="I483" s="7">
+        <v>0</v>
+      </c>
+      <c r="J483" s="7">
+        <v>0</v>
+      </c>
+      <c r="K483" s="7">
+        <v>9.6419487598037996</v>
+      </c>
+      <c r="L483" s="7">
+        <v>10.493851848533</v>
+      </c>
+      <c r="M483" s="7">
+        <v>0</v>
+      </c>
+      <c r="N483" s="7">
+        <v>0</v>
+      </c>
+      <c r="O483" s="7">
+        <v>2.02887446131556</v>
+      </c>
+      <c r="P483" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q483" s="7">
+        <v>0</v>
+      </c>
+      <c r="R483" s="7">
+        <v>3.3876847972856501</v>
+      </c>
+      <c r="S483" s="7">
+        <v>0</v>
+      </c>
+      <c r="T483" t="b">
+        <v>0</v>
+      </c>
+      <c r="U483" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V483" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W483" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="484" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A484" s="10">
+        <v>483</v>
+      </c>
+      <c r="B484" s="7">
+        <v>0</v>
+      </c>
+      <c r="C484" s="7">
+        <v>0</v>
+      </c>
+      <c r="D484" s="7">
+        <v>0</v>
+      </c>
+      <c r="E484" s="7">
+        <v>0</v>
+      </c>
+      <c r="F484" s="7">
+        <v>8.4702662767220698</v>
+      </c>
+      <c r="G484" s="7">
+        <v>0</v>
+      </c>
+      <c r="H484" s="7">
+        <v>0</v>
+      </c>
+      <c r="I484" s="7">
+        <v>0</v>
+      </c>
+      <c r="J484" s="7">
+        <v>0</v>
+      </c>
+      <c r="K484" s="7">
+        <v>0</v>
+      </c>
+      <c r="L484" s="7">
+        <v>0</v>
+      </c>
+      <c r="M484" s="7">
+        <v>9.0813254198134299</v>
+      </c>
+      <c r="N484" s="7">
+        <v>0</v>
+      </c>
+      <c r="O484" s="7">
+        <v>3.6895086646288102</v>
+      </c>
+      <c r="P484" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q484" s="7">
+        <v>0</v>
+      </c>
+      <c r="R484" s="7">
+        <v>3.8405117477650599</v>
+      </c>
+      <c r="S484" s="7">
+        <v>0</v>
+      </c>
+      <c r="T484" t="b">
+        <v>0</v>
+      </c>
+      <c r="U484" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V484" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W484" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="485" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A485" s="10">
+        <v>484</v>
+      </c>
+      <c r="B485" s="7">
+        <v>0</v>
+      </c>
+      <c r="C485" s="7">
+        <v>0</v>
+      </c>
+      <c r="D485" s="7">
+        <v>0</v>
+      </c>
+      <c r="E485" s="7">
+        <v>6.7030395248416301</v>
+      </c>
+      <c r="F485" s="7">
+        <v>0</v>
+      </c>
+      <c r="G485" s="7">
+        <v>0</v>
+      </c>
+      <c r="H485" s="7">
+        <v>0</v>
+      </c>
+      <c r="I485" s="7">
+        <v>0</v>
+      </c>
+      <c r="J485" s="7">
+        <v>0</v>
+      </c>
+      <c r="K485" s="7">
+        <v>0</v>
+      </c>
+      <c r="L485" s="7">
+        <v>10.1128335943219</v>
+      </c>
+      <c r="M485" s="7">
+        <v>0</v>
+      </c>
+      <c r="N485" s="7">
+        <v>0</v>
+      </c>
+      <c r="O485" s="7">
+        <v>2.3695727849185002</v>
+      </c>
+      <c r="P485" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q485" s="7">
+        <v>0</v>
+      </c>
+      <c r="R485" s="7">
+        <v>2.64973772270455</v>
+      </c>
+      <c r="S485" s="7">
+        <v>0</v>
+      </c>
+      <c r="T485" t="b">
+        <v>0</v>
+      </c>
+      <c r="U485" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V485" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W485" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="486" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A486" s="10">
+        <v>485</v>
+      </c>
+      <c r="B486" s="7">
+        <v>0</v>
+      </c>
+      <c r="C486" s="7">
+        <v>0</v>
+      </c>
+      <c r="D486" s="7">
+        <v>0</v>
+      </c>
+      <c r="E486" s="7">
+        <v>0</v>
+      </c>
+      <c r="F486" s="7">
+        <v>0</v>
+      </c>
+      <c r="G486" s="7">
+        <v>0</v>
+      </c>
+      <c r="H486" s="7">
+        <v>0</v>
+      </c>
+      <c r="I486" s="7">
+        <v>0</v>
+      </c>
+      <c r="J486" s="7">
+        <v>0</v>
+      </c>
+      <c r="K486" s="7">
+        <v>12.0341663478151</v>
+      </c>
+      <c r="L486" s="7">
+        <v>0</v>
+      </c>
+      <c r="M486" s="7">
+        <v>12.036147606680499</v>
+      </c>
+      <c r="N486" s="7">
+        <v>0</v>
+      </c>
+      <c r="O486" s="7">
+        <v>2.4134209552901602</v>
+      </c>
+      <c r="P486" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q486" s="7">
+        <v>0</v>
+      </c>
+      <c r="R486" s="7">
+        <v>1.89210221635878</v>
+      </c>
+      <c r="S486" s="7">
+        <v>0</v>
+      </c>
+      <c r="T486" t="b">
+        <v>0</v>
+      </c>
+      <c r="U486" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V486" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W486" s="2" t="str">
+        <f t="shared" si="25"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="487" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A487" s="10">
+        <v>486</v>
+      </c>
+      <c r="B487" s="7">
+        <v>0</v>
+      </c>
+      <c r="C487" s="7">
+        <v>9.5967887195515207</v>
+      </c>
+      <c r="D487" s="7">
+        <v>0</v>
+      </c>
+      <c r="E487" s="7">
+        <v>0</v>
+      </c>
+      <c r="F487" s="7">
+        <v>0</v>
+      </c>
+      <c r="G487" s="7">
+        <v>10.874844936914799</v>
+      </c>
+      <c r="H487" s="7">
+        <v>0</v>
+      </c>
+      <c r="I487" s="7">
+        <v>0</v>
+      </c>
+      <c r="J487" s="7">
+        <v>0</v>
+      </c>
+      <c r="K487" s="7">
+        <v>0</v>
+      </c>
+      <c r="L487" s="7">
+        <v>0</v>
+      </c>
+      <c r="M487" s="7">
+        <v>0</v>
+      </c>
+      <c r="N487" s="7">
+        <v>0</v>
+      </c>
+      <c r="O487" s="7">
+        <v>1.9126363345691799</v>
+      </c>
+      <c r="P487" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q487" s="7">
+        <v>0</v>
+      </c>
+      <c r="R487" s="7">
+        <v>4.5221246670046096</v>
+      </c>
+      <c r="S487" s="7">
+        <v>0</v>
+      </c>
+      <c r="T487" t="b">
+        <v>0</v>
+      </c>
+      <c r="U487" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V487" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W487" s="2" t="str">
+        <f t="shared" ref="W487" si="28">IF(T487=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W469">
+  <conditionalFormatting sqref="A1:W487">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
@@ -45103,7 +46444,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S522 & P4_T2 init DoE
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0893FAE-81B1-1647-ADB3-4D0B86EF8AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D47193D-7828-8F4A-95C7-C324F5FBAD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="-38400" yWindow="-4840" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -368,17 +368,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -709,11 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W487"/>
+  <dimension ref="A1:W523"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A421" zoomScale="59" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W487" sqref="W487"/>
+    <sheetView tabSelected="1" topLeftCell="A487" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W523" sqref="W523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32065,11 +32055,11 @@
         <v>0</v>
       </c>
       <c r="U430" s="2" t="str">
-        <f t="shared" ref="U430:U487" si="26">IF(T430=FALSE, "NA", "")</f>
+        <f t="shared" ref="U430:U493" si="26">IF(T430=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V430" s="2" t="str">
-        <f t="shared" ref="V430:V487" si="27">IF(T430=FALSE, "NA", "")</f>
+        <f t="shared" ref="V430:V493" si="27">IF(T430=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W430" s="2" t="str">
@@ -35613,13 +35603,11 @@
       <c r="U478" s="2">
         <v>1077</v>
       </c>
-      <c r="V478" s="2" t="str">
-        <f t="shared" si="27"/>
-        <v/>
-      </c>
-      <c r="W478" s="2" t="str">
-        <f t="shared" si="25"/>
-        <v/>
+      <c r="V478" s="2">
+        <v>80</v>
+      </c>
+      <c r="W478" s="2" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="479" spans="1:23" x14ac:dyDescent="0.2">
@@ -36284,12 +36272,2658 @@
         <v>NA</v>
       </c>
       <c r="W487" s="2" t="str">
-        <f t="shared" ref="W487" si="28">IF(T487=FALSE, "NA", "")</f>
+        <f t="shared" ref="W487:W523" si="28">IF(T487=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="488" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A488" s="10">
+        <v>487</v>
+      </c>
+      <c r="B488" s="7">
+        <v>0</v>
+      </c>
+      <c r="C488" s="7">
+        <v>12.259920991583</v>
+      </c>
+      <c r="D488" s="7">
+        <v>0</v>
+      </c>
+      <c r="E488" s="7">
+        <v>0</v>
+      </c>
+      <c r="F488" s="7">
+        <v>0</v>
+      </c>
+      <c r="G488" s="7">
+        <v>0</v>
+      </c>
+      <c r="H488" s="7">
+        <v>0</v>
+      </c>
+      <c r="I488" s="7">
+        <v>0</v>
+      </c>
+      <c r="J488" s="7">
+        <v>0</v>
+      </c>
+      <c r="K488" s="7">
+        <v>0</v>
+      </c>
+      <c r="L488" s="7">
+        <v>0</v>
+      </c>
+      <c r="M488" s="7">
+        <v>11.7416899737094</v>
+      </c>
+      <c r="N488" s="7">
+        <v>0</v>
+      </c>
+      <c r="O488" s="7">
+        <v>3.6024863365850699</v>
+      </c>
+      <c r="P488" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q488" s="7">
+        <v>0</v>
+      </c>
+      <c r="R488" s="7">
+        <v>1.64448072526802</v>
+      </c>
+      <c r="S488" s="7">
+        <v>0</v>
+      </c>
+      <c r="T488" t="b">
+        <v>0</v>
+      </c>
+      <c r="U488" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V488" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W488" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="489" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A489" s="10">
+        <v>488</v>
+      </c>
+      <c r="B489" s="7">
+        <v>0</v>
+      </c>
+      <c r="C489" s="7">
+        <v>0</v>
+      </c>
+      <c r="D489" s="7">
+        <v>0</v>
+      </c>
+      <c r="E489" s="7">
+        <v>9.2772736759851906</v>
+      </c>
+      <c r="F489" s="7">
+        <v>0</v>
+      </c>
+      <c r="G489" s="7">
+        <v>0</v>
+      </c>
+      <c r="H489" s="7">
+        <v>0</v>
+      </c>
+      <c r="I489" s="7">
+        <v>7.3132854274145602</v>
+      </c>
+      <c r="J489" s="7">
+        <v>0</v>
+      </c>
+      <c r="K489" s="7">
+        <v>0</v>
+      </c>
+      <c r="L489" s="7">
+        <v>0</v>
+      </c>
+      <c r="M489" s="7">
+        <v>0</v>
+      </c>
+      <c r="N489" s="7">
+        <v>0</v>
+      </c>
+      <c r="O489" s="7">
+        <v>2.1126364000954299</v>
+      </c>
+      <c r="P489" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q489" s="7">
+        <v>0</v>
+      </c>
+      <c r="R489" s="7">
+        <v>4.9583321775733102</v>
+      </c>
+      <c r="S489" s="7">
+        <v>0</v>
+      </c>
+      <c r="T489" t="b">
+        <v>0</v>
+      </c>
+      <c r="U489" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V489" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W489" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="490" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A490" s="10">
+        <v>489</v>
+      </c>
+      <c r="B490" s="7">
+        <v>0</v>
+      </c>
+      <c r="C490" s="7">
+        <v>0</v>
+      </c>
+      <c r="D490" s="7">
+        <v>0</v>
+      </c>
+      <c r="E490" s="7">
+        <v>0</v>
+      </c>
+      <c r="F490" s="7">
+        <v>0</v>
+      </c>
+      <c r="G490" s="7">
+        <v>0</v>
+      </c>
+      <c r="H490" s="7">
+        <v>0</v>
+      </c>
+      <c r="I490" s="7">
+        <v>0</v>
+      </c>
+      <c r="J490" s="7">
+        <v>8.3227774226712903</v>
+      </c>
+      <c r="K490" s="7">
+        <v>0</v>
+      </c>
+      <c r="L490" s="7">
+        <v>0</v>
+      </c>
+      <c r="M490" s="7">
+        <v>10.7687883090629</v>
+      </c>
+      <c r="N490" s="7">
+        <v>0</v>
+      </c>
+      <c r="O490" s="7">
+        <v>3.0674204969582899</v>
+      </c>
+      <c r="P490" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q490" s="7">
+        <v>0</v>
+      </c>
+      <c r="R490" s="7">
+        <v>2.1597017951938899</v>
+      </c>
+      <c r="S490" s="7">
+        <v>0</v>
+      </c>
+      <c r="T490" t="b">
+        <v>1</v>
+      </c>
+      <c r="U490" s="2">
+        <v>39</v>
+      </c>
+      <c r="V490" s="2">
+        <v>17</v>
+      </c>
+      <c r="W490" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="491" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A491" s="10">
+        <v>490</v>
+      </c>
+      <c r="B491" s="7">
+        <v>0</v>
+      </c>
+      <c r="C491" s="7">
+        <v>0</v>
+      </c>
+      <c r="D491" s="7">
+        <v>0</v>
+      </c>
+      <c r="E491" s="7">
+        <v>0</v>
+      </c>
+      <c r="F491" s="7">
+        <v>0</v>
+      </c>
+      <c r="G491" s="7">
+        <v>0</v>
+      </c>
+      <c r="H491" s="7">
+        <v>0</v>
+      </c>
+      <c r="I491" s="7">
+        <v>12.7517169209626</v>
+      </c>
+      <c r="J491" s="7">
+        <v>0</v>
+      </c>
+      <c r="K491" s="7">
+        <v>11.9075232747311</v>
+      </c>
+      <c r="L491" s="7">
+        <v>0</v>
+      </c>
+      <c r="M491" s="7">
+        <v>0</v>
+      </c>
+      <c r="N491" s="7">
+        <v>0</v>
+      </c>
+      <c r="O491" s="7">
+        <v>3.73035229705008</v>
+      </c>
+      <c r="P491" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q491" s="7">
+        <v>0</v>
+      </c>
+      <c r="R491" s="7">
+        <v>4.4692604800498099</v>
+      </c>
+      <c r="S491" s="7">
+        <v>0</v>
+      </c>
+      <c r="T491" t="b">
+        <v>0</v>
+      </c>
+      <c r="U491" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V491" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W491" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="492" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A492" s="10">
+        <v>491</v>
+      </c>
+      <c r="B492" s="7">
+        <v>4.0558370137006099</v>
+      </c>
+      <c r="C492" s="7">
+        <v>11.2330927635085</v>
+      </c>
+      <c r="D492" s="7">
+        <v>0</v>
+      </c>
+      <c r="E492" s="7">
+        <v>0</v>
+      </c>
+      <c r="F492" s="7">
+        <v>0</v>
+      </c>
+      <c r="G492" s="7">
+        <v>0</v>
+      </c>
+      <c r="H492" s="7">
+        <v>0</v>
+      </c>
+      <c r="I492" s="7">
+        <v>0</v>
+      </c>
+      <c r="J492" s="7">
+        <v>0</v>
+      </c>
+      <c r="K492" s="7">
+        <v>0</v>
+      </c>
+      <c r="L492" s="7">
+        <v>0</v>
+      </c>
+      <c r="M492" s="7">
+        <v>0</v>
+      </c>
+      <c r="N492" s="7">
+        <v>0</v>
+      </c>
+      <c r="O492" s="7">
+        <v>2.72747762552128</v>
+      </c>
+      <c r="P492" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q492" s="7">
+        <v>0</v>
+      </c>
+      <c r="R492" s="7">
+        <v>4.34087975358955</v>
+      </c>
+      <c r="S492" s="7">
+        <v>0</v>
+      </c>
+      <c r="T492" t="b">
+        <v>0</v>
+      </c>
+      <c r="U492" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V492" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W492" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="493" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A493" s="10">
+        <v>492</v>
+      </c>
+      <c r="B493" s="7">
+        <v>0</v>
+      </c>
+      <c r="C493" s="7">
+        <v>11.4237093547803</v>
+      </c>
+      <c r="D493" s="7">
+        <v>0</v>
+      </c>
+      <c r="E493" s="7">
+        <v>0</v>
+      </c>
+      <c r="F493" s="7">
+        <v>8.1963659988628095</v>
+      </c>
+      <c r="G493" s="7">
+        <v>0</v>
+      </c>
+      <c r="H493" s="7">
+        <v>0</v>
+      </c>
+      <c r="I493" s="7">
+        <v>0</v>
+      </c>
+      <c r="J493" s="7">
+        <v>0</v>
+      </c>
+      <c r="K493" s="7">
+        <v>0</v>
+      </c>
+      <c r="L493" s="7">
+        <v>0</v>
+      </c>
+      <c r="M493" s="7">
+        <v>0</v>
+      </c>
+      <c r="N493" s="7">
+        <v>0</v>
+      </c>
+      <c r="O493" s="7">
+        <v>3.58566768584895</v>
+      </c>
+      <c r="P493" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q493" s="7">
+        <v>0</v>
+      </c>
+      <c r="R493" s="7">
+        <v>4.9554460783469398</v>
+      </c>
+      <c r="S493" s="7">
+        <v>0</v>
+      </c>
+      <c r="T493" t="b">
+        <v>0</v>
+      </c>
+      <c r="U493" s="2" t="str">
+        <f t="shared" si="26"/>
+        <v>NA</v>
+      </c>
+      <c r="V493" s="2" t="str">
+        <f t="shared" si="27"/>
+        <v>NA</v>
+      </c>
+      <c r="W493" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="494" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A494" s="10">
+        <v>493</v>
+      </c>
+      <c r="B494" s="7">
+        <v>4.6203510504972201</v>
+      </c>
+      <c r="C494" s="7">
+        <v>0</v>
+      </c>
+      <c r="D494" s="7">
+        <v>0</v>
+      </c>
+      <c r="E494" s="7">
+        <v>0</v>
+      </c>
+      <c r="F494" s="7">
+        <v>0</v>
+      </c>
+      <c r="G494" s="7">
+        <v>0</v>
+      </c>
+      <c r="H494" s="7">
+        <v>0</v>
+      </c>
+      <c r="I494" s="7">
+        <v>0</v>
+      </c>
+      <c r="J494" s="7">
+        <v>0</v>
+      </c>
+      <c r="K494" s="7">
+        <v>0</v>
+      </c>
+      <c r="L494" s="7">
+        <v>0</v>
+      </c>
+      <c r="M494" s="7">
+        <v>13.360428206968299</v>
+      </c>
+      <c r="N494" s="7">
+        <v>0</v>
+      </c>
+      <c r="O494" s="7">
+        <v>2.2671530690786801</v>
+      </c>
+      <c r="P494" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q494" s="7">
+        <v>0</v>
+      </c>
+      <c r="R494" s="7">
+        <v>4.7559369729722896</v>
+      </c>
+      <c r="S494" s="7">
+        <v>0</v>
+      </c>
+      <c r="T494" t="b">
+        <v>0</v>
+      </c>
+      <c r="U494" s="2" t="str">
+        <f t="shared" ref="U494:U523" si="29">IF(T494=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V494" s="2" t="str">
+        <f t="shared" ref="V494:V523" si="30">IF(T494=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W494" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="495" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A495" s="10">
+        <v>494</v>
+      </c>
+      <c r="B495" s="7">
+        <v>0</v>
+      </c>
+      <c r="C495" s="7">
+        <v>0</v>
+      </c>
+      <c r="D495" s="7">
+        <v>0</v>
+      </c>
+      <c r="E495" s="7">
+        <v>0</v>
+      </c>
+      <c r="F495" s="7">
+        <v>0</v>
+      </c>
+      <c r="G495" s="7">
+        <v>0</v>
+      </c>
+      <c r="H495" s="7">
+        <v>0</v>
+      </c>
+      <c r="I495" s="7">
+        <v>0</v>
+      </c>
+      <c r="J495" s="7">
+        <v>0</v>
+      </c>
+      <c r="K495" s="7">
+        <v>0</v>
+      </c>
+      <c r="L495" s="7">
+        <v>11.1600194519777</v>
+      </c>
+      <c r="M495" s="7">
+        <v>9.56544903337495</v>
+      </c>
+      <c r="N495" s="7">
+        <v>0</v>
+      </c>
+      <c r="O495" s="7">
+        <v>3.16496572875488</v>
+      </c>
+      <c r="P495" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q495" s="7">
+        <v>0</v>
+      </c>
+      <c r="R495" s="7">
+        <v>3.2611727929961098</v>
+      </c>
+      <c r="S495" s="7">
+        <v>0</v>
+      </c>
+      <c r="T495" t="b">
+        <v>0</v>
+      </c>
+      <c r="U495" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V495" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W495" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="496" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A496" s="10">
+        <v>495</v>
+      </c>
+      <c r="B496" s="7">
+        <v>0</v>
+      </c>
+      <c r="C496" s="7">
+        <v>11.562809706261699</v>
+      </c>
+      <c r="D496" s="7">
+        <v>0</v>
+      </c>
+      <c r="E496" s="7">
+        <v>0</v>
+      </c>
+      <c r="F496" s="7">
+        <v>0</v>
+      </c>
+      <c r="G496" s="7">
+        <v>0</v>
+      </c>
+      <c r="H496" s="7">
+        <v>0</v>
+      </c>
+      <c r="I496" s="7">
+        <v>0</v>
+      </c>
+      <c r="J496" s="7">
+        <v>10.037344670122</v>
+      </c>
+      <c r="K496" s="7">
+        <v>0</v>
+      </c>
+      <c r="L496" s="7">
+        <v>0</v>
+      </c>
+      <c r="M496" s="7">
+        <v>0</v>
+      </c>
+      <c r="N496" s="7">
+        <v>0</v>
+      </c>
+      <c r="O496" s="7">
+        <v>2.90489052343781</v>
+      </c>
+      <c r="P496" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q496" s="7">
+        <v>0</v>
+      </c>
+      <c r="R496" s="7">
+        <v>3.97266712426357</v>
+      </c>
+      <c r="S496" s="7">
+        <v>0</v>
+      </c>
+      <c r="T496" t="b">
+        <v>1</v>
+      </c>
+      <c r="U496" s="2">
+        <v>364</v>
+      </c>
+      <c r="V496" s="2">
+        <v>16</v>
+      </c>
+      <c r="W496" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="497" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A497" s="10">
+        <v>496</v>
+      </c>
+      <c r="B497" s="7">
+        <v>0</v>
+      </c>
+      <c r="C497" s="7">
+        <v>0</v>
+      </c>
+      <c r="D497" s="7">
+        <v>0</v>
+      </c>
+      <c r="E497" s="7">
+        <v>0</v>
+      </c>
+      <c r="F497" s="7">
+        <v>0</v>
+      </c>
+      <c r="G497" s="7">
+        <v>12.948840688641001</v>
+      </c>
+      <c r="H497" s="7">
+        <v>0</v>
+      </c>
+      <c r="I497" s="7">
+        <v>7.0242012906500104</v>
+      </c>
+      <c r="J497" s="7">
+        <v>0</v>
+      </c>
+      <c r="K497" s="7">
+        <v>0</v>
+      </c>
+      <c r="L497" s="7">
+        <v>0</v>
+      </c>
+      <c r="M497" s="7">
+        <v>0</v>
+      </c>
+      <c r="N497" s="7">
+        <v>0</v>
+      </c>
+      <c r="O497" s="7">
+        <v>2.60271298000999</v>
+      </c>
+      <c r="P497" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q497" s="7">
+        <v>0</v>
+      </c>
+      <c r="R497" s="7">
+        <v>1.20951808192496</v>
+      </c>
+      <c r="S497" s="7">
+        <v>0</v>
+      </c>
+      <c r="T497" t="b">
+        <v>1</v>
+      </c>
+      <c r="U497" s="2">
+        <v>57</v>
+      </c>
+      <c r="V497" s="2">
+        <v>248</v>
+      </c>
+      <c r="W497" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A498" s="10">
+        <v>497</v>
+      </c>
+      <c r="B498" s="7">
+        <v>0</v>
+      </c>
+      <c r="C498" s="7">
+        <v>0</v>
+      </c>
+      <c r="D498" s="7">
+        <v>0</v>
+      </c>
+      <c r="E498" s="7">
+        <v>11.620893929030499</v>
+      </c>
+      <c r="F498" s="7">
+        <v>0</v>
+      </c>
+      <c r="G498" s="7">
+        <v>0</v>
+      </c>
+      <c r="H498" s="7">
+        <v>0</v>
+      </c>
+      <c r="I498" s="7">
+        <v>0</v>
+      </c>
+      <c r="J498" s="7">
+        <v>0</v>
+      </c>
+      <c r="K498" s="7">
+        <v>11.916885690235</v>
+      </c>
+      <c r="L498" s="7">
+        <v>0</v>
+      </c>
+      <c r="M498" s="7">
+        <v>0</v>
+      </c>
+      <c r="N498" s="7">
+        <v>0</v>
+      </c>
+      <c r="O498" s="7">
+        <v>2.21622593778141</v>
+      </c>
+      <c r="P498" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q498" s="7">
+        <v>0</v>
+      </c>
+      <c r="R498" s="7">
+        <v>4.3804800780270901</v>
+      </c>
+      <c r="S498" s="7">
+        <v>0</v>
+      </c>
+      <c r="T498" t="b">
+        <v>0</v>
+      </c>
+      <c r="U498" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V498" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W498" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="499" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A499" s="10">
+        <v>498</v>
+      </c>
+      <c r="B499" s="7">
+        <v>0</v>
+      </c>
+      <c r="C499" s="7">
+        <v>0</v>
+      </c>
+      <c r="D499" s="7">
+        <v>0</v>
+      </c>
+      <c r="E499" s="7">
+        <v>0</v>
+      </c>
+      <c r="F499" s="7">
+        <v>0</v>
+      </c>
+      <c r="G499" s="7">
+        <v>0</v>
+      </c>
+      <c r="H499" s="7">
+        <v>12.1668155256462</v>
+      </c>
+      <c r="I499" s="7">
+        <v>0</v>
+      </c>
+      <c r="J499" s="7">
+        <v>12.5641033018203</v>
+      </c>
+      <c r="K499" s="7">
+        <v>0</v>
+      </c>
+      <c r="L499" s="7">
+        <v>0</v>
+      </c>
+      <c r="M499" s="7">
+        <v>0</v>
+      </c>
+      <c r="N499" s="7">
+        <v>0</v>
+      </c>
+      <c r="O499" s="7">
+        <v>1.76449725282249</v>
+      </c>
+      <c r="P499" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q499" s="7">
+        <v>0</v>
+      </c>
+      <c r="R499" s="7">
+        <v>4.2328314918296099</v>
+      </c>
+      <c r="S499" s="7">
+        <v>0</v>
+      </c>
+      <c r="T499" t="b">
+        <v>1</v>
+      </c>
+      <c r="U499" s="2">
+        <v>18</v>
+      </c>
+      <c r="V499" s="2">
+        <v>395</v>
+      </c>
+      <c r="W499" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A500" s="10">
+        <v>499</v>
+      </c>
+      <c r="B500" s="7">
+        <v>0</v>
+      </c>
+      <c r="C500" s="7">
+        <v>0</v>
+      </c>
+      <c r="D500" s="7">
+        <v>0</v>
+      </c>
+      <c r="E500" s="7">
+        <v>0</v>
+      </c>
+      <c r="F500" s="7">
+        <v>0</v>
+      </c>
+      <c r="G500" s="7">
+        <v>8.4697499835780992</v>
+      </c>
+      <c r="H500" s="7">
+        <v>0</v>
+      </c>
+      <c r="I500" s="7">
+        <v>0</v>
+      </c>
+      <c r="J500" s="7">
+        <v>0</v>
+      </c>
+      <c r="K500" s="7">
+        <v>9.1195114485939204</v>
+      </c>
+      <c r="L500" s="7">
+        <v>0</v>
+      </c>
+      <c r="M500" s="7">
+        <v>0</v>
+      </c>
+      <c r="N500" s="7">
+        <v>0</v>
+      </c>
+      <c r="O500" s="7">
+        <v>2.7793695693912399</v>
+      </c>
+      <c r="P500" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q500" s="7">
+        <v>0</v>
+      </c>
+      <c r="R500" s="7">
+        <v>1.1425469186057899</v>
+      </c>
+      <c r="S500" s="7">
+        <v>0</v>
+      </c>
+      <c r="T500" t="b">
+        <v>0</v>
+      </c>
+      <c r="U500" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V500" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W500" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="501" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A501" s="10">
+        <v>500</v>
+      </c>
+      <c r="B501" s="7">
+        <v>4.69706913845903</v>
+      </c>
+      <c r="C501" s="7">
+        <v>0</v>
+      </c>
+      <c r="D501" s="7">
+        <v>0</v>
+      </c>
+      <c r="E501" s="7">
+        <v>0</v>
+      </c>
+      <c r="F501" s="7">
+        <v>0</v>
+      </c>
+      <c r="G501" s="7">
+        <v>0</v>
+      </c>
+      <c r="H501" s="7">
+        <v>0</v>
+      </c>
+      <c r="I501" s="7">
+        <v>6.7643639536752103</v>
+      </c>
+      <c r="J501" s="7">
+        <v>0</v>
+      </c>
+      <c r="K501" s="7">
+        <v>0</v>
+      </c>
+      <c r="L501" s="7">
+        <v>0</v>
+      </c>
+      <c r="M501" s="7">
+        <v>0</v>
+      </c>
+      <c r="N501" s="7">
+        <v>0</v>
+      </c>
+      <c r="O501" s="7">
+        <v>2.7067369646474702</v>
+      </c>
+      <c r="P501" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q501" s="7">
+        <v>0</v>
+      </c>
+      <c r="R501" s="7">
+        <v>1.7688363007527601</v>
+      </c>
+      <c r="S501" s="7">
+        <v>0</v>
+      </c>
+      <c r="T501" t="b">
+        <v>0</v>
+      </c>
+      <c r="U501" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V501" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W501" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="502" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A502" s="10">
+        <v>501</v>
+      </c>
+      <c r="B502" s="7">
+        <v>0</v>
+      </c>
+      <c r="C502" s="7">
+        <v>0</v>
+      </c>
+      <c r="D502" s="7">
+        <v>7.8509862854644199</v>
+      </c>
+      <c r="E502" s="7">
+        <v>0</v>
+      </c>
+      <c r="F502" s="7">
+        <v>0</v>
+      </c>
+      <c r="G502" s="7">
+        <v>0</v>
+      </c>
+      <c r="H502" s="7">
+        <v>0</v>
+      </c>
+      <c r="I502" s="7">
+        <v>0</v>
+      </c>
+      <c r="J502" s="7">
+        <v>10.0935551761537</v>
+      </c>
+      <c r="K502" s="7">
+        <v>0</v>
+      </c>
+      <c r="L502" s="7">
+        <v>0</v>
+      </c>
+      <c r="M502" s="7">
+        <v>0</v>
+      </c>
+      <c r="N502" s="7">
+        <v>0</v>
+      </c>
+      <c r="O502" s="7">
+        <v>2.79822319323103</v>
+      </c>
+      <c r="P502" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q502" s="7">
+        <v>0</v>
+      </c>
+      <c r="R502" s="7">
+        <v>2.30940702043846</v>
+      </c>
+      <c r="S502" s="7">
+        <v>0</v>
+      </c>
+      <c r="T502" t="b">
+        <v>0</v>
+      </c>
+      <c r="U502" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V502" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W502" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="503" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A503" s="10">
+        <v>502</v>
+      </c>
+      <c r="B503" s="7">
+        <v>0</v>
+      </c>
+      <c r="C503" s="7">
+        <v>0</v>
+      </c>
+      <c r="D503" s="7">
+        <v>12.2397601090211</v>
+      </c>
+      <c r="E503" s="7">
+        <v>0</v>
+      </c>
+      <c r="F503" s="7">
+        <v>0</v>
+      </c>
+      <c r="G503" s="7">
+        <v>0</v>
+      </c>
+      <c r="H503" s="7">
+        <v>0</v>
+      </c>
+      <c r="I503" s="7">
+        <v>0</v>
+      </c>
+      <c r="J503" s="7">
+        <v>0</v>
+      </c>
+      <c r="K503" s="7">
+        <v>0</v>
+      </c>
+      <c r="L503" s="7">
+        <v>0</v>
+      </c>
+      <c r="M503" s="7">
+        <v>12.5486743163629</v>
+      </c>
+      <c r="N503" s="7">
+        <v>0</v>
+      </c>
+      <c r="O503" s="7">
+        <v>3.7130039687137999</v>
+      </c>
+      <c r="P503" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q503" s="7">
+        <v>0</v>
+      </c>
+      <c r="R503" s="7">
+        <v>1.3128853812026999</v>
+      </c>
+      <c r="S503" s="7">
+        <v>0</v>
+      </c>
+      <c r="T503" t="b">
+        <v>0</v>
+      </c>
+      <c r="U503" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V503" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W503" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="504" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A504" s="10">
+        <v>503</v>
+      </c>
+      <c r="B504" s="7">
+        <v>6.2411199261248198</v>
+      </c>
+      <c r="C504" s="7">
+        <v>0</v>
+      </c>
+      <c r="D504" s="7">
+        <v>0</v>
+      </c>
+      <c r="E504" s="7">
+        <v>0</v>
+      </c>
+      <c r="F504" s="7">
+        <v>0</v>
+      </c>
+      <c r="G504" s="7">
+        <v>8.8524339152757694</v>
+      </c>
+      <c r="H504" s="7">
+        <v>0</v>
+      </c>
+      <c r="I504" s="7">
+        <v>0</v>
+      </c>
+      <c r="J504" s="7">
+        <v>0</v>
+      </c>
+      <c r="K504" s="7">
+        <v>0</v>
+      </c>
+      <c r="L504" s="7">
+        <v>0</v>
+      </c>
+      <c r="M504" s="7">
+        <v>0</v>
+      </c>
+      <c r="N504" s="7">
+        <v>0</v>
+      </c>
+      <c r="O504" s="7">
+        <v>3.22563852255738</v>
+      </c>
+      <c r="P504" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q504" s="7">
+        <v>0</v>
+      </c>
+      <c r="R504" s="7">
+        <v>1.4407934871646799</v>
+      </c>
+      <c r="S504" s="7">
+        <v>0</v>
+      </c>
+      <c r="T504" t="b">
+        <v>0</v>
+      </c>
+      <c r="U504" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V504" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W504" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="505" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A505" s="10">
+        <v>504</v>
+      </c>
+      <c r="B505" s="7">
+        <v>0</v>
+      </c>
+      <c r="C505" s="7">
+        <v>0</v>
+      </c>
+      <c r="D505" s="7">
+        <v>0</v>
+      </c>
+      <c r="E505" s="7">
+        <v>0</v>
+      </c>
+      <c r="F505" s="7">
+        <v>0</v>
+      </c>
+      <c r="G505" s="7">
+        <v>0</v>
+      </c>
+      <c r="H505" s="7">
+        <v>10.870708496168501</v>
+      </c>
+      <c r="I505" s="7">
+        <v>0</v>
+      </c>
+      <c r="J505" s="7">
+        <v>0</v>
+      </c>
+      <c r="K505" s="7">
+        <v>0</v>
+      </c>
+      <c r="L505" s="7">
+        <v>11.972780864680599</v>
+      </c>
+      <c r="M505" s="7">
+        <v>0</v>
+      </c>
+      <c r="N505" s="7">
+        <v>0</v>
+      </c>
+      <c r="O505" s="7">
+        <v>2.8544556786751598</v>
+      </c>
+      <c r="P505" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q505" s="7">
+        <v>0</v>
+      </c>
+      <c r="R505" s="7">
+        <v>3.5395740661286301</v>
+      </c>
+      <c r="S505" s="7">
+        <v>0</v>
+      </c>
+      <c r="T505" t="b">
+        <v>0</v>
+      </c>
+      <c r="U505" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V505" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W505" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="506" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A506" s="10">
+        <v>505</v>
+      </c>
+      <c r="B506" s="7">
+        <v>0</v>
+      </c>
+      <c r="C506" s="7">
+        <v>0</v>
+      </c>
+      <c r="D506" s="7">
+        <v>0</v>
+      </c>
+      <c r="E506" s="7">
+        <v>0</v>
+      </c>
+      <c r="F506" s="7">
+        <v>0</v>
+      </c>
+      <c r="G506" s="7">
+        <v>12.217580411573699</v>
+      </c>
+      <c r="H506" s="7">
+        <v>0</v>
+      </c>
+      <c r="I506" s="7">
+        <v>0</v>
+      </c>
+      <c r="J506" s="7">
+        <v>0</v>
+      </c>
+      <c r="K506" s="7">
+        <v>0</v>
+      </c>
+      <c r="L506" s="7">
+        <v>0</v>
+      </c>
+      <c r="M506" s="7">
+        <v>8.5378017610232604</v>
+      </c>
+      <c r="N506" s="7">
+        <v>0</v>
+      </c>
+      <c r="O506" s="7">
+        <v>1.8093404069424599</v>
+      </c>
+      <c r="P506" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q506" s="7">
+        <v>0</v>
+      </c>
+      <c r="R506" s="7">
+        <v>1.85777161893336</v>
+      </c>
+      <c r="S506" s="7">
+        <v>0</v>
+      </c>
+      <c r="T506" t="b">
+        <v>0</v>
+      </c>
+      <c r="U506" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V506" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W506" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="507" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A507" s="10">
+        <v>506</v>
+      </c>
+      <c r="B507" s="7">
+        <v>0</v>
+      </c>
+      <c r="C507" s="7">
+        <v>0</v>
+      </c>
+      <c r="D507" s="7">
+        <v>0</v>
+      </c>
+      <c r="E507" s="7">
+        <v>0</v>
+      </c>
+      <c r="F507" s="7">
+        <v>7.7298899690667904</v>
+      </c>
+      <c r="G507" s="7">
+        <v>0</v>
+      </c>
+      <c r="H507" s="7">
+        <v>12.3750024888504</v>
+      </c>
+      <c r="I507" s="7">
+        <v>0</v>
+      </c>
+      <c r="J507" s="7">
+        <v>0</v>
+      </c>
+      <c r="K507" s="7">
+        <v>0</v>
+      </c>
+      <c r="L507" s="7">
+        <v>0</v>
+      </c>
+      <c r="M507" s="7">
+        <v>0</v>
+      </c>
+      <c r="N507" s="7">
+        <v>0</v>
+      </c>
+      <c r="O507" s="7">
+        <v>1.82329888829234</v>
+      </c>
+      <c r="P507" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q507" s="7">
+        <v>0</v>
+      </c>
+      <c r="R507" s="7">
+        <v>2.9711172588441301</v>
+      </c>
+      <c r="S507" s="7">
+        <v>0</v>
+      </c>
+      <c r="T507" t="b">
+        <v>0</v>
+      </c>
+      <c r="U507" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V507" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W507" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="508" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A508" s="10">
+        <v>507</v>
+      </c>
+      <c r="B508" s="7">
+        <v>0</v>
+      </c>
+      <c r="C508" s="7">
+        <v>0</v>
+      </c>
+      <c r="D508" s="7">
+        <v>0</v>
+      </c>
+      <c r="E508" s="7">
+        <v>0</v>
+      </c>
+      <c r="F508" s="7">
+        <v>0</v>
+      </c>
+      <c r="G508" s="7">
+        <v>0</v>
+      </c>
+      <c r="H508" s="7">
+        <v>0</v>
+      </c>
+      <c r="I508" s="7">
+        <v>0</v>
+      </c>
+      <c r="J508" s="7">
+        <v>8.9704923154654406</v>
+      </c>
+      <c r="K508" s="7">
+        <v>10.653890662535799</v>
+      </c>
+      <c r="L508" s="7">
+        <v>0</v>
+      </c>
+      <c r="M508" s="7">
+        <v>0</v>
+      </c>
+      <c r="N508" s="7">
+        <v>0</v>
+      </c>
+      <c r="O508" s="7">
+        <v>2.6891069101266099</v>
+      </c>
+      <c r="P508" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q508" s="7">
+        <v>0</v>
+      </c>
+      <c r="R508" s="7">
+        <v>5.0571635736948597</v>
+      </c>
+      <c r="S508" s="7">
+        <v>0</v>
+      </c>
+      <c r="T508" t="b">
+        <v>0</v>
+      </c>
+      <c r="U508" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V508" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W508" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="509" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A509" s="10">
+        <v>508</v>
+      </c>
+      <c r="B509" s="7">
+        <v>5.07394298842783</v>
+      </c>
+      <c r="C509" s="7">
+        <v>0</v>
+      </c>
+      <c r="D509" s="7">
+        <v>0</v>
+      </c>
+      <c r="E509" s="7">
+        <v>0</v>
+      </c>
+      <c r="F509" s="7">
+        <v>0</v>
+      </c>
+      <c r="G509" s="7">
+        <v>0</v>
+      </c>
+      <c r="H509" s="7">
+        <v>0</v>
+      </c>
+      <c r="I509" s="7">
+        <v>0</v>
+      </c>
+      <c r="J509" s="7">
+        <v>0</v>
+      </c>
+      <c r="K509" s="7">
+        <v>9.4427395979203403</v>
+      </c>
+      <c r="L509" s="7">
+        <v>0</v>
+      </c>
+      <c r="M509" s="7">
+        <v>0</v>
+      </c>
+      <c r="N509" s="7">
+        <v>0</v>
+      </c>
+      <c r="O509" s="7">
+        <v>3.3416679501756499</v>
+      </c>
+      <c r="P509" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q509" s="7">
+        <v>0</v>
+      </c>
+      <c r="R509" s="7">
+        <v>2.8672496143476498</v>
+      </c>
+      <c r="S509" s="7">
+        <v>0</v>
+      </c>
+      <c r="T509" t="b">
+        <v>0</v>
+      </c>
+      <c r="U509" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V509" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W509" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="510" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A510" s="10">
+        <v>509</v>
+      </c>
+      <c r="B510" s="7">
+        <v>0</v>
+      </c>
+      <c r="C510" s="7">
+        <v>0</v>
+      </c>
+      <c r="D510" s="7">
+        <v>0</v>
+      </c>
+      <c r="E510" s="7">
+        <v>0</v>
+      </c>
+      <c r="F510" s="7">
+        <v>9.6804989095489091</v>
+      </c>
+      <c r="G510" s="7">
+        <v>0</v>
+      </c>
+      <c r="H510" s="7">
+        <v>0</v>
+      </c>
+      <c r="I510" s="7">
+        <v>0</v>
+      </c>
+      <c r="J510" s="7">
+        <v>9.3863805920183498</v>
+      </c>
+      <c r="K510" s="7">
+        <v>0</v>
+      </c>
+      <c r="L510" s="7">
+        <v>0</v>
+      </c>
+      <c r="M510" s="7">
+        <v>0</v>
+      </c>
+      <c r="N510" s="7">
+        <v>0</v>
+      </c>
+      <c r="O510" s="7">
+        <v>2.8752264097453</v>
+      </c>
+      <c r="P510" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q510" s="7">
+        <v>0</v>
+      </c>
+      <c r="R510" s="7">
+        <v>2.4330717961821202</v>
+      </c>
+      <c r="S510" s="7">
+        <v>0</v>
+      </c>
+      <c r="T510" t="b">
+        <v>1</v>
+      </c>
+      <c r="U510" s="2">
+        <v>33</v>
+      </c>
+      <c r="V510" s="2">
+        <v>78</v>
+      </c>
+      <c r="W510" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="511" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A511" s="10">
+        <v>510</v>
+      </c>
+      <c r="B511" s="7">
+        <v>8.1055975057435496</v>
+      </c>
+      <c r="C511" s="7">
+        <v>0</v>
+      </c>
+      <c r="D511" s="7">
+        <v>0</v>
+      </c>
+      <c r="E511" s="7">
+        <v>0</v>
+      </c>
+      <c r="F511" s="7">
+        <v>0</v>
+      </c>
+      <c r="G511" s="7">
+        <v>0</v>
+      </c>
+      <c r="H511" s="7">
+        <v>10.501991196185401</v>
+      </c>
+      <c r="I511" s="7">
+        <v>0</v>
+      </c>
+      <c r="J511" s="7">
+        <v>0</v>
+      </c>
+      <c r="K511" s="7">
+        <v>0</v>
+      </c>
+      <c r="L511" s="7">
+        <v>0</v>
+      </c>
+      <c r="M511" s="7">
+        <v>0</v>
+      </c>
+      <c r="N511" s="7">
+        <v>0</v>
+      </c>
+      <c r="O511" s="7">
+        <v>2.20282718284205</v>
+      </c>
+      <c r="P511" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q511" s="7">
+        <v>0</v>
+      </c>
+      <c r="R511" s="7">
+        <v>5.0004681129959598</v>
+      </c>
+      <c r="S511" s="7">
+        <v>0</v>
+      </c>
+      <c r="T511" t="b">
+        <v>0</v>
+      </c>
+      <c r="U511" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V511" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W511" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="512" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A512" s="10">
+        <v>511</v>
+      </c>
+      <c r="B512" s="7">
+        <v>5.0613126179396799</v>
+      </c>
+      <c r="C512" s="7">
+        <v>0</v>
+      </c>
+      <c r="D512" s="7">
+        <v>0</v>
+      </c>
+      <c r="E512" s="7">
+        <v>0</v>
+      </c>
+      <c r="F512" s="7">
+        <v>0</v>
+      </c>
+      <c r="G512" s="7">
+        <v>0</v>
+      </c>
+      <c r="H512" s="7">
+        <v>0</v>
+      </c>
+      <c r="I512" s="7">
+        <v>0</v>
+      </c>
+      <c r="J512" s="7">
+        <v>0</v>
+      </c>
+      <c r="K512" s="7">
+        <v>0</v>
+      </c>
+      <c r="L512" s="7">
+        <v>8.77642043646863</v>
+      </c>
+      <c r="M512" s="7">
+        <v>0</v>
+      </c>
+      <c r="N512" s="7">
+        <v>0</v>
+      </c>
+      <c r="O512" s="7">
+        <v>2.4158636516558598</v>
+      </c>
+      <c r="P512" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q512" s="7">
+        <v>0</v>
+      </c>
+      <c r="R512" s="7">
+        <v>2.8124201041953598</v>
+      </c>
+      <c r="S512" s="7">
+        <v>0</v>
+      </c>
+      <c r="T512" t="b">
+        <v>0</v>
+      </c>
+      <c r="U512" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V512" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W512" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="513" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A513" s="10">
+        <v>512</v>
+      </c>
+      <c r="B513" s="7">
+        <v>0</v>
+      </c>
+      <c r="C513" s="7">
+        <v>0</v>
+      </c>
+      <c r="D513" s="7">
+        <v>0</v>
+      </c>
+      <c r="E513" s="7">
+        <v>0</v>
+      </c>
+      <c r="F513" s="7">
+        <v>8.0137790070154793</v>
+      </c>
+      <c r="G513" s="7">
+        <v>12.840996230905199</v>
+      </c>
+      <c r="H513" s="7">
+        <v>0</v>
+      </c>
+      <c r="I513" s="7">
+        <v>0</v>
+      </c>
+      <c r="J513" s="7">
+        <v>0</v>
+      </c>
+      <c r="K513" s="7">
+        <v>0</v>
+      </c>
+      <c r="L513" s="7">
+        <v>0</v>
+      </c>
+      <c r="M513" s="7">
+        <v>0</v>
+      </c>
+      <c r="N513" s="7">
+        <v>0</v>
+      </c>
+      <c r="O513" s="7">
+        <v>2.1754891672747201</v>
+      </c>
+      <c r="P513" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q513" s="7">
+        <v>0</v>
+      </c>
+      <c r="R513" s="7">
+        <v>1.5209723690974699</v>
+      </c>
+      <c r="S513" s="7">
+        <v>0</v>
+      </c>
+      <c r="T513" t="b">
+        <v>0</v>
+      </c>
+      <c r="U513" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V513" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W513" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="514" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A514" s="10">
+        <v>513</v>
+      </c>
+      <c r="B514" s="7">
+        <v>0</v>
+      </c>
+      <c r="C514" s="7">
+        <v>9.8689974900252704</v>
+      </c>
+      <c r="D514" s="7">
+        <v>0</v>
+      </c>
+      <c r="E514" s="7">
+        <v>0</v>
+      </c>
+      <c r="F514" s="7">
+        <v>0</v>
+      </c>
+      <c r="G514" s="7">
+        <v>0</v>
+      </c>
+      <c r="H514" s="7">
+        <v>0</v>
+      </c>
+      <c r="I514" s="7">
+        <v>0</v>
+      </c>
+      <c r="J514" s="7">
+        <v>0</v>
+      </c>
+      <c r="K514" s="7">
+        <v>12.3185181245255</v>
+      </c>
+      <c r="L514" s="7">
+        <v>0</v>
+      </c>
+      <c r="M514" s="7">
+        <v>0</v>
+      </c>
+      <c r="N514" s="7">
+        <v>0</v>
+      </c>
+      <c r="O514" s="7">
+        <v>2.1225239112779399</v>
+      </c>
+      <c r="P514" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q514" s="7">
+        <v>0</v>
+      </c>
+      <c r="R514" s="7">
+        <v>1.56603852386627</v>
+      </c>
+      <c r="S514" s="7">
+        <v>0</v>
+      </c>
+      <c r="T514" t="b">
+        <v>0</v>
+      </c>
+      <c r="U514" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V514" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W514" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="515" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A515" s="10">
+        <v>514</v>
+      </c>
+      <c r="B515" s="7">
+        <v>0</v>
+      </c>
+      <c r="C515" s="7">
+        <v>0</v>
+      </c>
+      <c r="D515" s="7">
+        <v>7.1090622049983301</v>
+      </c>
+      <c r="E515" s="7">
+        <v>0</v>
+      </c>
+      <c r="F515" s="7">
+        <v>8.83596396436843</v>
+      </c>
+      <c r="G515" s="7">
+        <v>0</v>
+      </c>
+      <c r="H515" s="7">
+        <v>0</v>
+      </c>
+      <c r="I515" s="7">
+        <v>0</v>
+      </c>
+      <c r="J515" s="7">
+        <v>0</v>
+      </c>
+      <c r="K515" s="7">
+        <v>0</v>
+      </c>
+      <c r="L515" s="7">
+        <v>0</v>
+      </c>
+      <c r="M515" s="7">
+        <v>0</v>
+      </c>
+      <c r="N515" s="7">
+        <v>0</v>
+      </c>
+      <c r="O515" s="7">
+        <v>1.78027234479462</v>
+      </c>
+      <c r="P515" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q515" s="7">
+        <v>0</v>
+      </c>
+      <c r="R515" s="7">
+        <v>1.8391553850517599</v>
+      </c>
+      <c r="S515" s="7">
+        <v>0</v>
+      </c>
+      <c r="T515" t="b">
+        <v>0</v>
+      </c>
+      <c r="U515" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V515" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W515" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="516" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A516" s="10">
+        <v>515</v>
+      </c>
+      <c r="B516" s="7">
+        <v>0</v>
+      </c>
+      <c r="C516" s="7">
+        <v>0</v>
+      </c>
+      <c r="D516" s="7">
+        <v>0</v>
+      </c>
+      <c r="E516" s="7">
+        <v>0</v>
+      </c>
+      <c r="F516" s="7">
+        <v>0</v>
+      </c>
+      <c r="G516" s="7">
+        <v>0</v>
+      </c>
+      <c r="H516" s="7">
+        <v>11.868717698931</v>
+      </c>
+      <c r="I516" s="7">
+        <v>0</v>
+      </c>
+      <c r="J516" s="7">
+        <v>0</v>
+      </c>
+      <c r="K516" s="7">
+        <v>0</v>
+      </c>
+      <c r="L516" s="7">
+        <v>0</v>
+      </c>
+      <c r="M516" s="7">
+        <v>9.6545968266792208</v>
+      </c>
+      <c r="N516" s="7">
+        <v>0</v>
+      </c>
+      <c r="O516" s="7">
+        <v>2.0472696347856298</v>
+      </c>
+      <c r="P516" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q516" s="7">
+        <v>0</v>
+      </c>
+      <c r="R516" s="7">
+        <v>3.9806645377692802</v>
+      </c>
+      <c r="S516" s="7">
+        <v>0</v>
+      </c>
+      <c r="T516" t="b">
+        <v>0</v>
+      </c>
+      <c r="U516" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V516" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W516" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="517" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A517" s="10">
+        <v>516</v>
+      </c>
+      <c r="B517" s="7">
+        <v>0</v>
+      </c>
+      <c r="C517" s="7">
+        <v>0</v>
+      </c>
+      <c r="D517" s="7">
+        <v>0</v>
+      </c>
+      <c r="E517" s="7">
+        <v>10.9484235533304</v>
+      </c>
+      <c r="F517" s="7">
+        <v>13.652915873368601</v>
+      </c>
+      <c r="G517" s="7">
+        <v>0</v>
+      </c>
+      <c r="H517" s="7">
+        <v>0</v>
+      </c>
+      <c r="I517" s="7">
+        <v>0</v>
+      </c>
+      <c r="J517" s="7">
+        <v>0</v>
+      </c>
+      <c r="K517" s="7">
+        <v>0</v>
+      </c>
+      <c r="L517" s="7">
+        <v>0</v>
+      </c>
+      <c r="M517" s="7">
+        <v>0</v>
+      </c>
+      <c r="N517" s="7">
+        <v>0</v>
+      </c>
+      <c r="O517" s="7">
+        <v>2.0602526538089201</v>
+      </c>
+      <c r="P517" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q517" s="7">
+        <v>0</v>
+      </c>
+      <c r="R517" s="7">
+        <v>4.6486504061134797</v>
+      </c>
+      <c r="S517" s="7">
+        <v>0</v>
+      </c>
+      <c r="T517" t="b">
+        <v>0</v>
+      </c>
+      <c r="U517" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V517" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W517" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="518" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A518" s="10">
+        <v>517</v>
+      </c>
+      <c r="B518" s="7">
+        <v>5.6105325830519002</v>
+      </c>
+      <c r="C518" s="7">
+        <v>0</v>
+      </c>
+      <c r="D518" s="7">
+        <v>0</v>
+      </c>
+      <c r="E518" s="7">
+        <v>0</v>
+      </c>
+      <c r="F518" s="7">
+        <v>8.9955644206812408</v>
+      </c>
+      <c r="G518" s="7">
+        <v>0</v>
+      </c>
+      <c r="H518" s="7">
+        <v>0</v>
+      </c>
+      <c r="I518" s="7">
+        <v>0</v>
+      </c>
+      <c r="J518" s="7">
+        <v>0</v>
+      </c>
+      <c r="K518" s="7">
+        <v>0</v>
+      </c>
+      <c r="L518" s="7">
+        <v>0</v>
+      </c>
+      <c r="M518" s="7">
+        <v>0</v>
+      </c>
+      <c r="N518" s="7">
+        <v>0</v>
+      </c>
+      <c r="O518" s="7">
+        <v>2.80027284393937</v>
+      </c>
+      <c r="P518" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q518" s="7">
+        <v>0</v>
+      </c>
+      <c r="R518" s="7">
+        <v>2.7858181272414599</v>
+      </c>
+      <c r="S518" s="7">
+        <v>0</v>
+      </c>
+      <c r="T518" t="b">
+        <v>0</v>
+      </c>
+      <c r="U518" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V518" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W518" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="519" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A519" s="10">
+        <v>518</v>
+      </c>
+      <c r="B519" s="7">
+        <v>0</v>
+      </c>
+      <c r="C519" s="7">
+        <v>0</v>
+      </c>
+      <c r="D519" s="7">
+        <v>0</v>
+      </c>
+      <c r="E519" s="7">
+        <v>0</v>
+      </c>
+      <c r="F519" s="7">
+        <v>0</v>
+      </c>
+      <c r="G519" s="7">
+        <v>0</v>
+      </c>
+      <c r="H519" s="7">
+        <v>0</v>
+      </c>
+      <c r="I519" s="7">
+        <v>9.9016606700940706</v>
+      </c>
+      <c r="J519" s="7">
+        <v>0</v>
+      </c>
+      <c r="K519" s="7">
+        <v>0</v>
+      </c>
+      <c r="L519" s="7">
+        <v>0</v>
+      </c>
+      <c r="M519" s="7">
+        <v>10.885601803403</v>
+      </c>
+      <c r="N519" s="7">
+        <v>0</v>
+      </c>
+      <c r="O519" s="7">
+        <v>3.25553992321835</v>
+      </c>
+      <c r="P519" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q519" s="7">
+        <v>0</v>
+      </c>
+      <c r="R519" s="7">
+        <v>3.9759253958195799</v>
+      </c>
+      <c r="S519" s="7">
+        <v>0</v>
+      </c>
+      <c r="T519" t="b">
+        <v>0</v>
+      </c>
+      <c r="U519" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V519" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W519" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="520" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A520" s="10">
+        <v>519</v>
+      </c>
+      <c r="B520" s="7">
+        <v>0</v>
+      </c>
+      <c r="C520" s="7">
+        <v>0</v>
+      </c>
+      <c r="D520" s="7">
+        <v>0</v>
+      </c>
+      <c r="E520" s="7">
+        <v>0</v>
+      </c>
+      <c r="F520" s="7">
+        <v>0</v>
+      </c>
+      <c r="G520" s="7">
+        <v>7.8120144452400497</v>
+      </c>
+      <c r="H520" s="7">
+        <v>11.3199540878869</v>
+      </c>
+      <c r="I520" s="7">
+        <v>0</v>
+      </c>
+      <c r="J520" s="7">
+        <v>0</v>
+      </c>
+      <c r="K520" s="7">
+        <v>0</v>
+      </c>
+      <c r="L520" s="7">
+        <v>0</v>
+      </c>
+      <c r="M520" s="7">
+        <v>0</v>
+      </c>
+      <c r="N520" s="7">
+        <v>0</v>
+      </c>
+      <c r="O520" s="7">
+        <v>2.82108763198478</v>
+      </c>
+      <c r="P520" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q520" s="7">
+        <v>0</v>
+      </c>
+      <c r="R520" s="7">
+        <v>2.26478200779842</v>
+      </c>
+      <c r="S520" s="7">
+        <v>0</v>
+      </c>
+      <c r="T520" t="b">
+        <v>1</v>
+      </c>
+      <c r="U520" s="2">
+        <v>40</v>
+      </c>
+      <c r="V520" s="2">
+        <v>1397</v>
+      </c>
+      <c r="W520" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="521" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A521" s="10">
+        <v>520</v>
+      </c>
+      <c r="B521" s="7">
+        <v>0</v>
+      </c>
+      <c r="C521" s="7">
+        <v>0</v>
+      </c>
+      <c r="D521" s="7">
+        <v>0</v>
+      </c>
+      <c r="E521" s="7">
+        <v>0</v>
+      </c>
+      <c r="F521" s="7">
+        <v>0</v>
+      </c>
+      <c r="G521" s="7">
+        <v>9.4886060249117907</v>
+      </c>
+      <c r="H521" s="7">
+        <v>0</v>
+      </c>
+      <c r="I521" s="7">
+        <v>0</v>
+      </c>
+      <c r="J521" s="7">
+        <v>9.1866514150561809</v>
+      </c>
+      <c r="K521" s="7">
+        <v>0</v>
+      </c>
+      <c r="L521" s="7">
+        <v>0</v>
+      </c>
+      <c r="M521" s="7">
+        <v>0</v>
+      </c>
+      <c r="N521" s="7">
+        <v>0</v>
+      </c>
+      <c r="O521" s="7">
+        <v>3.5802142454963501</v>
+      </c>
+      <c r="P521" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q521" s="7">
+        <v>0</v>
+      </c>
+      <c r="R521" s="7">
+        <v>2.8583082000893199</v>
+      </c>
+      <c r="S521" s="7">
+        <v>0</v>
+      </c>
+      <c r="T521" t="b">
+        <v>0</v>
+      </c>
+      <c r="U521" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V521" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W521" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="522" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A522" s="10">
+        <v>521</v>
+      </c>
+      <c r="B522" s="7">
+        <v>0</v>
+      </c>
+      <c r="C522" s="7">
+        <v>0</v>
+      </c>
+      <c r="D522" s="7">
+        <v>0</v>
+      </c>
+      <c r="E522" s="7">
+        <v>0</v>
+      </c>
+      <c r="F522" s="7">
+        <v>0</v>
+      </c>
+      <c r="G522" s="7">
+        <v>0</v>
+      </c>
+      <c r="H522" s="7">
+        <v>0</v>
+      </c>
+      <c r="I522" s="7">
+        <v>0</v>
+      </c>
+      <c r="J522" s="7">
+        <v>11.423066020641899</v>
+      </c>
+      <c r="K522" s="7">
+        <v>0</v>
+      </c>
+      <c r="L522" s="7">
+        <v>10.242148728407299</v>
+      </c>
+      <c r="M522" s="7">
+        <v>0</v>
+      </c>
+      <c r="N522" s="7">
+        <v>0</v>
+      </c>
+      <c r="O522" s="7">
+        <v>1.7721127835841901</v>
+      </c>
+      <c r="P522" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q522" s="7">
+        <v>0</v>
+      </c>
+      <c r="R522" s="7">
+        <v>2.5052737896823198</v>
+      </c>
+      <c r="S522" s="7">
+        <v>0</v>
+      </c>
+      <c r="T522" t="b">
+        <v>0</v>
+      </c>
+      <c r="U522" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V522" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W522" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="523" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A523" s="10">
+        <v>522</v>
+      </c>
+      <c r="B523" s="7">
+        <v>0</v>
+      </c>
+      <c r="C523" s="7">
+        <v>0</v>
+      </c>
+      <c r="D523" s="7">
+        <v>0</v>
+      </c>
+      <c r="E523" s="7">
+        <v>0</v>
+      </c>
+      <c r="F523" s="7">
+        <v>0</v>
+      </c>
+      <c r="G523" s="7">
+        <v>0</v>
+      </c>
+      <c r="H523" s="7">
+        <v>0</v>
+      </c>
+      <c r="I523" s="7">
+        <v>8.0602120809860907</v>
+      </c>
+      <c r="J523" s="7">
+        <v>0</v>
+      </c>
+      <c r="K523" s="7">
+        <v>0</v>
+      </c>
+      <c r="L523" s="7">
+        <v>11.2775652206575</v>
+      </c>
+      <c r="M523" s="7">
+        <v>0</v>
+      </c>
+      <c r="N523" s="7">
+        <v>0</v>
+      </c>
+      <c r="O523" s="7">
+        <v>1.29436591696018</v>
+      </c>
+      <c r="P523" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q523" s="7">
+        <v>0</v>
+      </c>
+      <c r="R523" s="7">
+        <v>1.3760371889672001</v>
+      </c>
+      <c r="S523" s="7">
+        <v>0</v>
+      </c>
+      <c r="T523" t="b">
+        <v>0</v>
+      </c>
+      <c r="U523" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V523" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W523" s="12" t="str">
+        <f t="shared" si="28"/>
         <v>NA</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W487">
+  <conditionalFormatting sqref="A1:W523">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
@@ -46444,7 +49078,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S558
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D47193D-7828-8F4A-95C7-C324F5FBAD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AAACCB-B5AB-8247-A275-B18B75F5CCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4840" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
   <si>
     <t>Sample</t>
   </si>
@@ -699,11 +699,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W523"/>
+  <dimension ref="A1:W559"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A487" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W523" sqref="W523"/>
+    <sheetView tabSelected="1" topLeftCell="A524" zoomScale="116" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W559" sqref="W559"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36272,7 +36272,7 @@
         <v>NA</v>
       </c>
       <c r="W487" s="2" t="str">
-        <f t="shared" ref="W487:W523" si="28">IF(T487=FALSE, "NA", "")</f>
+        <f t="shared" ref="W487:W532" si="28">IF(T487=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -36779,11 +36779,11 @@
         <v>0</v>
       </c>
       <c r="U494" s="2" t="str">
-        <f t="shared" ref="U494:U523" si="29">IF(T494=FALSE, "NA", "")</f>
+        <f t="shared" ref="U494:U531" si="29">IF(T494=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V494" s="2" t="str">
-        <f t="shared" ref="V494:V523" si="30">IF(T494=FALSE, "NA", "")</f>
+        <f t="shared" ref="V494:V532" si="30">IF(T494=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W494" s="12" t="str">
@@ -38922,8 +38922,2614 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="524" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A524" s="10">
+        <v>523</v>
+      </c>
+      <c r="B524" s="7">
+        <v>7.6290374090131197</v>
+      </c>
+      <c r="C524" s="7">
+        <v>0</v>
+      </c>
+      <c r="D524" s="7">
+        <v>0</v>
+      </c>
+      <c r="E524" s="7">
+        <v>0</v>
+      </c>
+      <c r="F524" s="7">
+        <v>0</v>
+      </c>
+      <c r="G524" s="7">
+        <v>0</v>
+      </c>
+      <c r="H524" s="7">
+        <v>0</v>
+      </c>
+      <c r="I524" s="7">
+        <v>0</v>
+      </c>
+      <c r="J524" s="7">
+        <v>0</v>
+      </c>
+      <c r="K524" s="7">
+        <v>12.486136063124601</v>
+      </c>
+      <c r="L524" s="7">
+        <v>0</v>
+      </c>
+      <c r="M524" s="7">
+        <v>0</v>
+      </c>
+      <c r="N524" s="7">
+        <v>0</v>
+      </c>
+      <c r="O524" s="7">
+        <v>0</v>
+      </c>
+      <c r="P524" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q524" s="7">
+        <v>2.3297731512745599</v>
+      </c>
+      <c r="R524" s="7">
+        <v>1.6186881162020299</v>
+      </c>
+      <c r="S524" s="7">
+        <v>0</v>
+      </c>
+      <c r="T524" t="b">
+        <v>1</v>
+      </c>
+      <c r="U524" s="2">
+        <v>26</v>
+      </c>
+      <c r="V524" s="2">
+        <v>2</v>
+      </c>
+      <c r="W524" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="525" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A525" s="10">
+        <v>524</v>
+      </c>
+      <c r="B525" s="7">
+        <v>0</v>
+      </c>
+      <c r="C525" s="7">
+        <v>0</v>
+      </c>
+      <c r="D525" s="7">
+        <v>0</v>
+      </c>
+      <c r="E525" s="7">
+        <v>0</v>
+      </c>
+      <c r="F525" s="7">
+        <v>10.554423539254699</v>
+      </c>
+      <c r="G525" s="7">
+        <v>0</v>
+      </c>
+      <c r="H525" s="7">
+        <v>12.5938026398326</v>
+      </c>
+      <c r="I525" s="7">
+        <v>0</v>
+      </c>
+      <c r="J525" s="7">
+        <v>0</v>
+      </c>
+      <c r="K525" s="7">
+        <v>0</v>
+      </c>
+      <c r="L525" s="7">
+        <v>0</v>
+      </c>
+      <c r="M525" s="7">
+        <v>0</v>
+      </c>
+      <c r="N525" s="7">
+        <v>0</v>
+      </c>
+      <c r="O525" s="7">
+        <v>0</v>
+      </c>
+      <c r="P525" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q525" s="7">
+        <v>2.4831056772167801</v>
+      </c>
+      <c r="R525" s="7">
+        <v>2.62023971856211</v>
+      </c>
+      <c r="S525" s="7">
+        <v>0</v>
+      </c>
+      <c r="T525" t="b">
+        <v>1</v>
+      </c>
+      <c r="U525" s="2">
+        <v>43</v>
+      </c>
+      <c r="V525" s="2">
+        <v>242</v>
+      </c>
+      <c r="W525" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="526" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A526" s="10">
+        <v>525</v>
+      </c>
+      <c r="B526" s="7">
+        <v>0</v>
+      </c>
+      <c r="C526" s="7">
+        <v>0</v>
+      </c>
+      <c r="D526" s="7">
+        <v>12.2433475070425</v>
+      </c>
+      <c r="E526" s="7">
+        <v>0</v>
+      </c>
+      <c r="F526" s="7">
+        <v>12.8882940231693</v>
+      </c>
+      <c r="G526" s="7">
+        <v>0</v>
+      </c>
+      <c r="H526" s="7">
+        <v>0</v>
+      </c>
+      <c r="I526" s="7">
+        <v>0</v>
+      </c>
+      <c r="J526" s="7">
+        <v>0</v>
+      </c>
+      <c r="K526" s="7">
+        <v>0</v>
+      </c>
+      <c r="L526" s="7">
+        <v>0</v>
+      </c>
+      <c r="M526" s="7">
+        <v>0</v>
+      </c>
+      <c r="N526" s="7">
+        <v>0</v>
+      </c>
+      <c r="O526" s="7">
+        <v>0</v>
+      </c>
+      <c r="P526" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q526" s="7">
+        <v>2.1731893478186</v>
+      </c>
+      <c r="R526" s="7">
+        <v>1.1893316564257601</v>
+      </c>
+      <c r="S526" s="7">
+        <v>0</v>
+      </c>
+      <c r="T526" t="b">
+        <v>1</v>
+      </c>
+      <c r="U526" s="2">
+        <v>66</v>
+      </c>
+      <c r="V526" s="2">
+        <v>3</v>
+      </c>
+      <c r="W526" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="527" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A527" s="10">
+        <v>526</v>
+      </c>
+      <c r="B527" s="7">
+        <v>0</v>
+      </c>
+      <c r="C527" s="7">
+        <v>0</v>
+      </c>
+      <c r="D527" s="7">
+        <v>0</v>
+      </c>
+      <c r="E527" s="7">
+        <v>0</v>
+      </c>
+      <c r="F527" s="7">
+        <v>0</v>
+      </c>
+      <c r="G527" s="7">
+        <v>8.1590194198893293</v>
+      </c>
+      <c r="H527" s="7">
+        <v>0</v>
+      </c>
+      <c r="I527" s="7">
+        <v>0</v>
+      </c>
+      <c r="J527" s="7">
+        <v>12.477510717451</v>
+      </c>
+      <c r="K527" s="7">
+        <v>0</v>
+      </c>
+      <c r="L527" s="7">
+        <v>0</v>
+      </c>
+      <c r="M527" s="7">
+        <v>0</v>
+      </c>
+      <c r="N527" s="7">
+        <v>0</v>
+      </c>
+      <c r="O527" s="7">
+        <v>0</v>
+      </c>
+      <c r="P527" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q527" s="7">
+        <v>2.1387120341098398</v>
+      </c>
+      <c r="R527" s="7">
+        <v>2.1671622231119101</v>
+      </c>
+      <c r="S527" s="7">
+        <v>0</v>
+      </c>
+      <c r="T527" t="b">
+        <v>0</v>
+      </c>
+      <c r="U527" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="V527" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W527" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="528" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A528" s="10">
+        <v>527</v>
+      </c>
+      <c r="B528" s="7">
+        <v>0</v>
+      </c>
+      <c r="C528" s="7">
+        <v>0</v>
+      </c>
+      <c r="D528" s="7">
+        <v>9.5210886251747198</v>
+      </c>
+      <c r="E528" s="7">
+        <v>0</v>
+      </c>
+      <c r="F528" s="7">
+        <v>0</v>
+      </c>
+      <c r="G528" s="7">
+        <v>0</v>
+      </c>
+      <c r="H528" s="7">
+        <v>0</v>
+      </c>
+      <c r="I528" s="7">
+        <v>7.08464113912627</v>
+      </c>
+      <c r="J528" s="7">
+        <v>0</v>
+      </c>
+      <c r="K528" s="7">
+        <v>0</v>
+      </c>
+      <c r="L528" s="7">
+        <v>0</v>
+      </c>
+      <c r="M528" s="7">
+        <v>0</v>
+      </c>
+      <c r="N528" s="7">
+        <v>0</v>
+      </c>
+      <c r="O528" s="7">
+        <v>0</v>
+      </c>
+      <c r="P528" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q528" s="7">
+        <v>2.3389593577296401</v>
+      </c>
+      <c r="R528" s="7">
+        <v>2.9825825304812601</v>
+      </c>
+      <c r="S528" s="7">
+        <v>0</v>
+      </c>
+      <c r="T528" t="b">
+        <v>1</v>
+      </c>
+      <c r="U528" s="2">
+        <v>80</v>
+      </c>
+      <c r="V528" s="2">
+        <v>4</v>
+      </c>
+      <c r="W528" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="529" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A529" s="10">
+        <v>528</v>
+      </c>
+      <c r="B529" s="7">
+        <v>0</v>
+      </c>
+      <c r="C529" s="7">
+        <v>8.2566730572777196</v>
+      </c>
+      <c r="D529" s="7">
+        <v>12.835049769463</v>
+      </c>
+      <c r="E529" s="7">
+        <v>0</v>
+      </c>
+      <c r="F529" s="7">
+        <v>0</v>
+      </c>
+      <c r="G529" s="7">
+        <v>0</v>
+      </c>
+      <c r="H529" s="7">
+        <v>0</v>
+      </c>
+      <c r="I529" s="7">
+        <v>0</v>
+      </c>
+      <c r="J529" s="7">
+        <v>0</v>
+      </c>
+      <c r="K529" s="7">
+        <v>0</v>
+      </c>
+      <c r="L529" s="7">
+        <v>0</v>
+      </c>
+      <c r="M529" s="7">
+        <v>0</v>
+      </c>
+      <c r="N529" s="7">
+        <v>0</v>
+      </c>
+      <c r="O529" s="7">
+        <v>0</v>
+      </c>
+      <c r="P529" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q529" s="7">
+        <v>2.0071310859770102</v>
+      </c>
+      <c r="R529" s="7">
+        <v>2.4162585255645399</v>
+      </c>
+      <c r="S529" s="7">
+        <v>0</v>
+      </c>
+      <c r="T529" t="b">
+        <v>1</v>
+      </c>
+      <c r="U529" s="2">
+        <v>17</v>
+      </c>
+      <c r="V529" s="2">
+        <v>3</v>
+      </c>
+      <c r="W529" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="530" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A530" s="10">
+        <v>529</v>
+      </c>
+      <c r="B530" s="7">
+        <v>4.7080025546081901</v>
+      </c>
+      <c r="C530" s="7">
+        <v>0</v>
+      </c>
+      <c r="D530" s="7">
+        <v>0</v>
+      </c>
+      <c r="E530" s="7">
+        <v>0</v>
+      </c>
+      <c r="F530" s="7">
+        <v>0</v>
+      </c>
+      <c r="G530" s="7">
+        <v>0</v>
+      </c>
+      <c r="H530" s="7">
+        <v>0</v>
+      </c>
+      <c r="I530" s="7">
+        <v>0</v>
+      </c>
+      <c r="J530" s="7">
+        <v>0</v>
+      </c>
+      <c r="K530" s="7">
+        <v>0</v>
+      </c>
+      <c r="L530" s="7">
+        <v>9.9514578813962995</v>
+      </c>
+      <c r="M530" s="7">
+        <v>0</v>
+      </c>
+      <c r="N530" s="7">
+        <v>0</v>
+      </c>
+      <c r="O530" s="7">
+        <v>0</v>
+      </c>
+      <c r="P530" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q530" s="7">
+        <v>2.2803896192891902</v>
+      </c>
+      <c r="R530" s="7">
+        <v>3.6098528378867898</v>
+      </c>
+      <c r="S530" s="7">
+        <v>0</v>
+      </c>
+      <c r="T530" t="b">
+        <v>0</v>
+      </c>
+      <c r="U530" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V530" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W530" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="531" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A531" s="10">
+        <v>530</v>
+      </c>
+      <c r="B531" s="7">
+        <v>0</v>
+      </c>
+      <c r="C531" s="7">
+        <v>0</v>
+      </c>
+      <c r="D531" s="7">
+        <v>0</v>
+      </c>
+      <c r="E531" s="7">
+        <v>0</v>
+      </c>
+      <c r="F531" s="7">
+        <v>0</v>
+      </c>
+      <c r="G531" s="7">
+        <v>11.0671803158101</v>
+      </c>
+      <c r="H531" s="7">
+        <v>12.6409040644211</v>
+      </c>
+      <c r="I531" s="7">
+        <v>0</v>
+      </c>
+      <c r="J531" s="7">
+        <v>0</v>
+      </c>
+      <c r="K531" s="7">
+        <v>0</v>
+      </c>
+      <c r="L531" s="7">
+        <v>0</v>
+      </c>
+      <c r="M531" s="7">
+        <v>0</v>
+      </c>
+      <c r="N531" s="7">
+        <v>0</v>
+      </c>
+      <c r="O531" s="7">
+        <v>0</v>
+      </c>
+      <c r="P531" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q531" s="7">
+        <v>1.6833241221089601</v>
+      </c>
+      <c r="R531" s="7">
+        <v>4.87549643542211</v>
+      </c>
+      <c r="S531" s="7">
+        <v>0</v>
+      </c>
+      <c r="T531" t="b">
+        <v>0</v>
+      </c>
+      <c r="U531" s="2" t="str">
+        <f t="shared" si="29"/>
+        <v>NA</v>
+      </c>
+      <c r="V531" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W531" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="532" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A532" s="10">
+        <v>531</v>
+      </c>
+      <c r="B532" s="7">
+        <v>0</v>
+      </c>
+      <c r="C532" s="7">
+        <v>0</v>
+      </c>
+      <c r="D532" s="7">
+        <v>0</v>
+      </c>
+      <c r="E532" s="7">
+        <v>0</v>
+      </c>
+      <c r="F532" s="7">
+        <v>0</v>
+      </c>
+      <c r="G532" s="7">
+        <v>0</v>
+      </c>
+      <c r="H532" s="7">
+        <v>10.639869592181601</v>
+      </c>
+      <c r="I532" s="7">
+        <v>0</v>
+      </c>
+      <c r="J532" s="7">
+        <v>0</v>
+      </c>
+      <c r="K532" s="7">
+        <v>0</v>
+      </c>
+      <c r="L532" s="7">
+        <v>9.1380932686858891</v>
+      </c>
+      <c r="M532" s="7">
+        <v>0</v>
+      </c>
+      <c r="N532" s="7">
+        <v>0</v>
+      </c>
+      <c r="O532" s="7">
+        <v>0</v>
+      </c>
+      <c r="P532" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q532" s="7">
+        <v>1.41036598265629</v>
+      </c>
+      <c r="R532" s="7">
+        <v>2.3575535626678001</v>
+      </c>
+      <c r="S532" s="7">
+        <v>0</v>
+      </c>
+      <c r="T532" t="b">
+        <v>0</v>
+      </c>
+      <c r="U532" s="2" t="str">
+        <f>IF(T532=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V532" s="2" t="str">
+        <f t="shared" si="30"/>
+        <v>NA</v>
+      </c>
+      <c r="W532" s="12" t="str">
+        <f t="shared" si="28"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="533" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A533" s="10">
+        <v>532</v>
+      </c>
+      <c r="B533" s="7">
+        <v>0</v>
+      </c>
+      <c r="C533" s="7">
+        <v>0</v>
+      </c>
+      <c r="D533" s="7">
+        <v>0</v>
+      </c>
+      <c r="E533" s="7">
+        <v>0</v>
+      </c>
+      <c r="F533" s="7">
+        <v>10.5211848742232</v>
+      </c>
+      <c r="G533" s="7">
+        <v>0</v>
+      </c>
+      <c r="H533" s="7">
+        <v>0</v>
+      </c>
+      <c r="I533" s="7">
+        <v>0</v>
+      </c>
+      <c r="J533" s="7">
+        <v>0</v>
+      </c>
+      <c r="K533" s="7">
+        <v>11.994984983091101</v>
+      </c>
+      <c r="L533" s="7">
+        <v>0</v>
+      </c>
+      <c r="M533" s="7">
+        <v>0</v>
+      </c>
+      <c r="N533" s="7">
+        <v>0</v>
+      </c>
+      <c r="O533" s="7">
+        <v>0</v>
+      </c>
+      <c r="P533" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q533" s="7">
+        <v>1.53438084110578</v>
+      </c>
+      <c r="R533" s="7">
+        <v>3.9278163278792699</v>
+      </c>
+      <c r="S533" s="7">
+        <v>0</v>
+      </c>
+      <c r="T533" t="b">
+        <v>1</v>
+      </c>
+      <c r="U533" s="2">
+        <v>39</v>
+      </c>
+      <c r="V533" s="2">
+        <v>5</v>
+      </c>
+      <c r="W533" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="534" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A534" s="10">
+        <v>533</v>
+      </c>
+      <c r="B534" s="7">
+        <v>0</v>
+      </c>
+      <c r="C534" s="7">
+        <v>0</v>
+      </c>
+      <c r="D534" s="7">
+        <v>0</v>
+      </c>
+      <c r="E534" s="7">
+        <v>0</v>
+      </c>
+      <c r="F534" s="7">
+        <v>0</v>
+      </c>
+      <c r="G534" s="7">
+        <v>0</v>
+      </c>
+      <c r="H534" s="7">
+        <v>0</v>
+      </c>
+      <c r="I534" s="7">
+        <v>0</v>
+      </c>
+      <c r="J534" s="7">
+        <v>0</v>
+      </c>
+      <c r="K534" s="7">
+        <v>9.0272340115540892</v>
+      </c>
+      <c r="L534" s="7">
+        <v>8.8626904533867101</v>
+      </c>
+      <c r="M534" s="7">
+        <v>0</v>
+      </c>
+      <c r="N534" s="7">
+        <v>0</v>
+      </c>
+      <c r="O534" s="7">
+        <v>0</v>
+      </c>
+      <c r="P534" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q534" s="7">
+        <v>2.6689063663826</v>
+      </c>
+      <c r="R534" s="7">
+        <v>1.50749487422807</v>
+      </c>
+      <c r="S534" s="7">
+        <v>0</v>
+      </c>
+      <c r="T534" t="b">
+        <v>1</v>
+      </c>
+      <c r="U534" s="2">
+        <v>34</v>
+      </c>
+      <c r="V534" s="2">
+        <v>3</v>
+      </c>
+      <c r="W534" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="535" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A535" s="10">
+        <v>534</v>
+      </c>
+      <c r="B535" s="7">
+        <v>0</v>
+      </c>
+      <c r="C535" s="7">
+        <v>0</v>
+      </c>
+      <c r="D535" s="7">
+        <v>0</v>
+      </c>
+      <c r="E535" s="7">
+        <v>0</v>
+      </c>
+      <c r="F535" s="7">
+        <v>0</v>
+      </c>
+      <c r="G535" s="7">
+        <v>0</v>
+      </c>
+      <c r="H535" s="7">
+        <v>10.0872511629813</v>
+      </c>
+      <c r="I535" s="7">
+        <v>0</v>
+      </c>
+      <c r="J535" s="7">
+        <v>0</v>
+      </c>
+      <c r="K535" s="7">
+        <v>10.5952351871991</v>
+      </c>
+      <c r="L535" s="7">
+        <v>0</v>
+      </c>
+      <c r="M535" s="7">
+        <v>0</v>
+      </c>
+      <c r="N535" s="7">
+        <v>0</v>
+      </c>
+      <c r="O535" s="7">
+        <v>0</v>
+      </c>
+      <c r="P535" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q535" s="7">
+        <v>2.75158013117903</v>
+      </c>
+      <c r="R535" s="7">
+        <v>1.41432931598178</v>
+      </c>
+      <c r="S535" s="7">
+        <v>0</v>
+      </c>
+      <c r="T535" t="b">
+        <v>1</v>
+      </c>
+      <c r="U535" s="2">
+        <v>17</v>
+      </c>
+      <c r="V535" s="2">
+        <v>3</v>
+      </c>
+      <c r="W535" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="536" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A536" s="10">
+        <v>535</v>
+      </c>
+      <c r="B536" s="7">
+        <v>0</v>
+      </c>
+      <c r="C536" s="7">
+        <v>0</v>
+      </c>
+      <c r="D536" s="7">
+        <v>7.4304386668871203</v>
+      </c>
+      <c r="E536" s="7">
+        <v>0</v>
+      </c>
+      <c r="F536" s="7">
+        <v>0</v>
+      </c>
+      <c r="G536" s="7">
+        <v>0</v>
+      </c>
+      <c r="H536" s="7">
+        <v>0</v>
+      </c>
+      <c r="I536" s="7">
+        <v>0</v>
+      </c>
+      <c r="J536" s="7">
+        <v>13.404227130634499</v>
+      </c>
+      <c r="K536" s="7">
+        <v>0</v>
+      </c>
+      <c r="L536" s="7">
+        <v>0</v>
+      </c>
+      <c r="M536" s="7">
+        <v>0</v>
+      </c>
+      <c r="N536" s="7">
+        <v>0</v>
+      </c>
+      <c r="O536" s="7">
+        <v>0</v>
+      </c>
+      <c r="P536" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q536" s="7">
+        <v>2.0454008078930701</v>
+      </c>
+      <c r="R536" s="7">
+        <v>3.3903914135796098</v>
+      </c>
+      <c r="S536" s="7">
+        <v>0</v>
+      </c>
+      <c r="T536" t="b">
+        <v>0</v>
+      </c>
+      <c r="U536" s="2" t="str">
+        <f>IF(T536=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V536" s="2" t="str">
+        <f>IF(T536=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W536" s="12" t="str">
+        <f>IF(T536=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="537" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A537" s="10">
+        <v>536</v>
+      </c>
+      <c r="B537" s="7">
+        <v>0</v>
+      </c>
+      <c r="C537" s="7">
+        <v>0</v>
+      </c>
+      <c r="D537" s="7">
+        <v>0</v>
+      </c>
+      <c r="E537" s="7">
+        <v>12.1472718377111</v>
+      </c>
+      <c r="F537" s="7">
+        <v>0</v>
+      </c>
+      <c r="G537" s="7">
+        <v>0</v>
+      </c>
+      <c r="H537" s="7">
+        <v>0</v>
+      </c>
+      <c r="I537" s="7">
+        <v>7.8496883529146499</v>
+      </c>
+      <c r="J537" s="7">
+        <v>0</v>
+      </c>
+      <c r="K537" s="7">
+        <v>0</v>
+      </c>
+      <c r="L537" s="7">
+        <v>0</v>
+      </c>
+      <c r="M537" s="7">
+        <v>0</v>
+      </c>
+      <c r="N537" s="7">
+        <v>0</v>
+      </c>
+      <c r="O537" s="7">
+        <v>0</v>
+      </c>
+      <c r="P537" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q537" s="7">
+        <v>2.4719164265867701</v>
+      </c>
+      <c r="R537" s="7">
+        <v>1.85362250633507</v>
+      </c>
+      <c r="S537" s="7">
+        <v>0</v>
+      </c>
+      <c r="T537" t="b">
+        <v>0</v>
+      </c>
+      <c r="U537" s="2" t="str">
+        <f t="shared" ref="U537:U557" si="31">IF(T537=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V537" s="2" t="str">
+        <f t="shared" ref="V537:V559" si="32">IF(T537=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W537" s="12" t="str">
+        <f t="shared" ref="W537:W559" si="33">IF(T537=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="538" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A538" s="10">
+        <v>537</v>
+      </c>
+      <c r="B538" s="7">
+        <v>0</v>
+      </c>
+      <c r="C538" s="7">
+        <v>9.6116659659997108</v>
+      </c>
+      <c r="D538" s="7">
+        <v>0</v>
+      </c>
+      <c r="E538" s="7">
+        <v>0</v>
+      </c>
+      <c r="F538" s="7">
+        <v>0</v>
+      </c>
+      <c r="G538" s="7">
+        <v>0</v>
+      </c>
+      <c r="H538" s="7">
+        <v>12.3727781288798</v>
+      </c>
+      <c r="I538" s="7">
+        <v>0</v>
+      </c>
+      <c r="J538" s="7">
+        <v>0</v>
+      </c>
+      <c r="K538" s="7">
+        <v>0</v>
+      </c>
+      <c r="L538" s="7">
+        <v>0</v>
+      </c>
+      <c r="M538" s="7">
+        <v>0</v>
+      </c>
+      <c r="N538" s="7">
+        <v>0</v>
+      </c>
+      <c r="O538" s="7">
+        <v>0</v>
+      </c>
+      <c r="P538" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q538" s="7">
+        <v>2.1999225209241899</v>
+      </c>
+      <c r="R538" s="7">
+        <v>5.1142655693601302</v>
+      </c>
+      <c r="S538" s="7">
+        <v>0</v>
+      </c>
+      <c r="T538" t="b">
+        <v>0</v>
+      </c>
+      <c r="U538" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V538" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W538" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="539" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A539" s="10">
+        <v>538</v>
+      </c>
+      <c r="B539" s="7">
+        <v>0</v>
+      </c>
+      <c r="C539" s="7">
+        <v>0</v>
+      </c>
+      <c r="D539" s="7">
+        <v>0</v>
+      </c>
+      <c r="E539" s="7">
+        <v>0</v>
+      </c>
+      <c r="F539" s="7">
+        <v>0</v>
+      </c>
+      <c r="G539" s="7">
+        <v>0</v>
+      </c>
+      <c r="H539" s="7">
+        <v>0</v>
+      </c>
+      <c r="I539" s="7">
+        <v>14.265931444563201</v>
+      </c>
+      <c r="J539" s="7">
+        <v>0</v>
+      </c>
+      <c r="K539" s="7">
+        <v>0</v>
+      </c>
+      <c r="L539" s="7">
+        <v>7.8641286938141404</v>
+      </c>
+      <c r="M539" s="7">
+        <v>0</v>
+      </c>
+      <c r="N539" s="7">
+        <v>0</v>
+      </c>
+      <c r="O539" s="7">
+        <v>0</v>
+      </c>
+      <c r="P539" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q539" s="7">
+        <v>1.3084224490572101</v>
+      </c>
+      <c r="R539" s="7">
+        <v>4.7918848134303804</v>
+      </c>
+      <c r="S539" s="7">
+        <v>0</v>
+      </c>
+      <c r="T539" t="b">
+        <v>1</v>
+      </c>
+      <c r="U539" s="2">
+        <v>3047</v>
+      </c>
+      <c r="V539" s="2">
+        <v>6</v>
+      </c>
+      <c r="W539" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="540" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A540" s="10">
+        <v>539</v>
+      </c>
+      <c r="B540" s="7">
+        <v>0</v>
+      </c>
+      <c r="C540" s="7">
+        <v>0</v>
+      </c>
+      <c r="D540" s="7">
+        <v>8.1872208621113494</v>
+      </c>
+      <c r="E540" s="7">
+        <v>0</v>
+      </c>
+      <c r="F540" s="7">
+        <v>0</v>
+      </c>
+      <c r="G540" s="7">
+        <v>0</v>
+      </c>
+      <c r="H540" s="7">
+        <v>8.5953496323598504</v>
+      </c>
+      <c r="I540" s="7">
+        <v>0</v>
+      </c>
+      <c r="J540" s="7">
+        <v>0</v>
+      </c>
+      <c r="K540" s="7">
+        <v>0</v>
+      </c>
+      <c r="L540" s="7">
+        <v>0</v>
+      </c>
+      <c r="M540" s="7">
+        <v>0</v>
+      </c>
+      <c r="N540" s="7">
+        <v>0</v>
+      </c>
+      <c r="O540" s="7">
+        <v>0</v>
+      </c>
+      <c r="P540" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q540" s="7">
+        <v>1.4713337912945601</v>
+      </c>
+      <c r="R540" s="7">
+        <v>3.3961439939763798</v>
+      </c>
+      <c r="S540" s="7">
+        <v>0</v>
+      </c>
+      <c r="T540" t="b">
+        <v>0</v>
+      </c>
+      <c r="U540" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V540" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W540" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="541" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A541" s="10">
+        <v>540</v>
+      </c>
+      <c r="B541" s="7">
+        <v>0</v>
+      </c>
+      <c r="C541" s="7">
+        <v>0</v>
+      </c>
+      <c r="D541" s="7">
+        <v>8.2043879094610705</v>
+      </c>
+      <c r="E541" s="7">
+        <v>0</v>
+      </c>
+      <c r="F541" s="7">
+        <v>0</v>
+      </c>
+      <c r="G541" s="7">
+        <v>0</v>
+      </c>
+      <c r="H541" s="7">
+        <v>0</v>
+      </c>
+      <c r="I541" s="7">
+        <v>0</v>
+      </c>
+      <c r="J541" s="7">
+        <v>0</v>
+      </c>
+      <c r="K541" s="7">
+        <v>7.9472927906749904</v>
+      </c>
+      <c r="L541" s="7">
+        <v>0</v>
+      </c>
+      <c r="M541" s="7">
+        <v>0</v>
+      </c>
+      <c r="N541" s="7">
+        <v>0</v>
+      </c>
+      <c r="O541" s="7">
+        <v>0</v>
+      </c>
+      <c r="P541" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q541" s="7">
+        <v>1.60930708933624</v>
+      </c>
+      <c r="R541" s="7">
+        <v>1.32487714470229</v>
+      </c>
+      <c r="S541" s="7">
+        <v>0</v>
+      </c>
+      <c r="T541" t="b">
+        <v>1</v>
+      </c>
+      <c r="U541" s="2">
+        <v>18</v>
+      </c>
+      <c r="V541" s="2">
+        <v>2</v>
+      </c>
+      <c r="W541" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="542" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A542" s="10">
+        <v>541</v>
+      </c>
+      <c r="B542" s="7">
+        <v>0</v>
+      </c>
+      <c r="C542" s="7">
+        <v>7.59190859540508</v>
+      </c>
+      <c r="D542" s="7">
+        <v>0</v>
+      </c>
+      <c r="E542" s="7">
+        <v>0</v>
+      </c>
+      <c r="F542" s="7">
+        <v>0</v>
+      </c>
+      <c r="G542" s="7">
+        <v>9.4458166178449297</v>
+      </c>
+      <c r="H542" s="7">
+        <v>0</v>
+      </c>
+      <c r="I542" s="7">
+        <v>0</v>
+      </c>
+      <c r="J542" s="7">
+        <v>0</v>
+      </c>
+      <c r="K542" s="7">
+        <v>0</v>
+      </c>
+      <c r="L542" s="7">
+        <v>0</v>
+      </c>
+      <c r="M542" s="7">
+        <v>0</v>
+      </c>
+      <c r="N542" s="7">
+        <v>0</v>
+      </c>
+      <c r="O542" s="7">
+        <v>0</v>
+      </c>
+      <c r="P542" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q542" s="7">
+        <v>0.80125684384227602</v>
+      </c>
+      <c r="R542" s="7">
+        <v>3.8360171398945901</v>
+      </c>
+      <c r="S542" s="7">
+        <v>0</v>
+      </c>
+      <c r="T542" t="b">
+        <v>0</v>
+      </c>
+      <c r="U542" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V542" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W542" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="543" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A543" s="10">
+        <v>542</v>
+      </c>
+      <c r="B543" s="7">
+        <v>0</v>
+      </c>
+      <c r="C543" s="7">
+        <v>0</v>
+      </c>
+      <c r="D543" s="7">
+        <v>0</v>
+      </c>
+      <c r="E543" s="7">
+        <v>9.0725091546166805</v>
+      </c>
+      <c r="F543" s="7">
+        <v>0</v>
+      </c>
+      <c r="G543" s="7">
+        <v>0</v>
+      </c>
+      <c r="H543" s="7">
+        <v>0</v>
+      </c>
+      <c r="I543" s="7">
+        <v>0</v>
+      </c>
+      <c r="J543" s="7">
+        <v>0</v>
+      </c>
+      <c r="K543" s="7">
+        <v>0</v>
+      </c>
+      <c r="L543" s="7">
+        <v>0</v>
+      </c>
+      <c r="M543" s="7">
+        <v>9.5711772386776204</v>
+      </c>
+      <c r="N543" s="7">
+        <v>0</v>
+      </c>
+      <c r="O543" s="7">
+        <v>0</v>
+      </c>
+      <c r="P543" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q543" s="7">
+        <v>2.3384587852351202</v>
+      </c>
+      <c r="R543" s="7">
+        <v>2.21404566853957</v>
+      </c>
+      <c r="S543" s="7">
+        <v>0</v>
+      </c>
+      <c r="T543" t="b">
+        <v>1</v>
+      </c>
+      <c r="U543" s="2">
+        <v>38</v>
+      </c>
+      <c r="V543" s="2">
+        <v>451</v>
+      </c>
+      <c r="W543" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="544" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A544" s="10">
+        <v>543</v>
+      </c>
+      <c r="B544" s="7">
+        <v>0</v>
+      </c>
+      <c r="C544" s="7">
+        <v>0</v>
+      </c>
+      <c r="D544" s="7">
+        <v>0</v>
+      </c>
+      <c r="E544" s="7">
+        <v>0</v>
+      </c>
+      <c r="F544" s="7">
+        <v>0</v>
+      </c>
+      <c r="G544" s="7">
+        <v>0</v>
+      </c>
+      <c r="H544" s="7">
+        <v>9.1479627717048295</v>
+      </c>
+      <c r="I544" s="7">
+        <v>0</v>
+      </c>
+      <c r="J544" s="7">
+        <v>0</v>
+      </c>
+      <c r="K544" s="7">
+        <v>0</v>
+      </c>
+      <c r="L544" s="7">
+        <v>0</v>
+      </c>
+      <c r="M544" s="7">
+        <v>9.3753900437525601</v>
+      </c>
+      <c r="N544" s="7">
+        <v>0</v>
+      </c>
+      <c r="O544" s="7">
+        <v>0</v>
+      </c>
+      <c r="P544" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q544" s="7">
+        <v>2.2431012193730702</v>
+      </c>
+      <c r="R544" s="7">
+        <v>4.1445627866572696</v>
+      </c>
+      <c r="S544" s="7">
+        <v>0</v>
+      </c>
+      <c r="T544" t="b">
+        <v>0</v>
+      </c>
+      <c r="U544" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V544" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W544" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="545" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A545" s="10">
+        <v>544</v>
+      </c>
+      <c r="B545" s="7">
+        <v>0</v>
+      </c>
+      <c r="C545" s="7">
+        <v>11.6414518125175</v>
+      </c>
+      <c r="D545" s="7">
+        <v>0</v>
+      </c>
+      <c r="E545" s="7">
+        <v>0</v>
+      </c>
+      <c r="F545" s="7">
+        <v>0</v>
+      </c>
+      <c r="G545" s="7">
+        <v>0</v>
+      </c>
+      <c r="H545" s="7">
+        <v>0</v>
+      </c>
+      <c r="I545" s="7">
+        <v>0</v>
+      </c>
+      <c r="J545" s="7">
+        <v>0</v>
+      </c>
+      <c r="K545" s="7">
+        <v>12.726597601082799</v>
+      </c>
+      <c r="L545" s="7">
+        <v>0</v>
+      </c>
+      <c r="M545" s="7">
+        <v>0</v>
+      </c>
+      <c r="N545" s="7">
+        <v>0</v>
+      </c>
+      <c r="O545" s="7">
+        <v>0</v>
+      </c>
+      <c r="P545" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q545" s="7">
+        <v>1.5549048159761401</v>
+      </c>
+      <c r="R545" s="7">
+        <v>4.9240681877897803</v>
+      </c>
+      <c r="S545" s="7">
+        <v>0</v>
+      </c>
+      <c r="T545" t="b">
+        <v>1</v>
+      </c>
+      <c r="U545" s="2">
+        <v>14</v>
+      </c>
+      <c r="V545" s="2">
+        <v>3</v>
+      </c>
+      <c r="W545" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="546" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A546" s="10">
+        <v>545</v>
+      </c>
+      <c r="B546" s="7">
+        <v>0</v>
+      </c>
+      <c r="C546" s="7">
+        <v>0</v>
+      </c>
+      <c r="D546" s="7">
+        <v>0</v>
+      </c>
+      <c r="E546" s="7">
+        <v>0</v>
+      </c>
+      <c r="F546" s="7">
+        <v>0</v>
+      </c>
+      <c r="G546" s="7">
+        <v>0</v>
+      </c>
+      <c r="H546" s="7">
+        <v>0</v>
+      </c>
+      <c r="I546" s="7">
+        <v>7.7697695867324397</v>
+      </c>
+      <c r="J546" s="7">
+        <v>0</v>
+      </c>
+      <c r="K546" s="7">
+        <v>0</v>
+      </c>
+      <c r="L546" s="7">
+        <v>0</v>
+      </c>
+      <c r="M546" s="7">
+        <v>9.7289615520306807</v>
+      </c>
+      <c r="N546" s="7">
+        <v>0</v>
+      </c>
+      <c r="O546" s="7">
+        <v>0</v>
+      </c>
+      <c r="P546" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q546" s="7">
+        <v>1.42752005243557</v>
+      </c>
+      <c r="R546" s="7">
+        <v>2.8321997840323498</v>
+      </c>
+      <c r="S546" s="7">
+        <v>0</v>
+      </c>
+      <c r="T546" t="b">
+        <v>0</v>
+      </c>
+      <c r="U546" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V546" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W546" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="547" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A547" s="10">
+        <v>546</v>
+      </c>
+      <c r="B547" s="7">
+        <v>0</v>
+      </c>
+      <c r="C547" s="7">
+        <v>8.4481940958498392</v>
+      </c>
+      <c r="D547" s="7">
+        <v>0</v>
+      </c>
+      <c r="E547" s="7">
+        <v>12.128260327642501</v>
+      </c>
+      <c r="F547" s="7">
+        <v>0</v>
+      </c>
+      <c r="G547" s="7">
+        <v>0</v>
+      </c>
+      <c r="H547" s="7">
+        <v>0</v>
+      </c>
+      <c r="I547" s="7">
+        <v>0</v>
+      </c>
+      <c r="J547" s="7">
+        <v>0</v>
+      </c>
+      <c r="K547" s="7">
+        <v>0</v>
+      </c>
+      <c r="L547" s="7">
+        <v>0</v>
+      </c>
+      <c r="M547" s="7">
+        <v>0</v>
+      </c>
+      <c r="N547" s="7">
+        <v>0</v>
+      </c>
+      <c r="O547" s="7">
+        <v>0</v>
+      </c>
+      <c r="P547" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q547" s="7">
+        <v>1.6139580878590301</v>
+      </c>
+      <c r="R547" s="7">
+        <v>4.0669325899311204</v>
+      </c>
+      <c r="S547" s="7">
+        <v>0</v>
+      </c>
+      <c r="T547" t="b">
+        <v>0</v>
+      </c>
+      <c r="U547" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V547" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W547" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="548" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A548" s="10">
+        <v>547</v>
+      </c>
+      <c r="B548" s="7">
+        <v>0</v>
+      </c>
+      <c r="C548" s="7">
+        <v>0</v>
+      </c>
+      <c r="D548" s="7">
+        <v>0</v>
+      </c>
+      <c r="E548" s="7">
+        <v>0</v>
+      </c>
+      <c r="F548" s="7">
+        <v>0</v>
+      </c>
+      <c r="G548" s="7">
+        <v>8.6383012505471601</v>
+      </c>
+      <c r="H548" s="7">
+        <v>0</v>
+      </c>
+      <c r="I548" s="7">
+        <v>8.5413219762854897</v>
+      </c>
+      <c r="J548" s="7">
+        <v>0</v>
+      </c>
+      <c r="K548" s="7">
+        <v>0</v>
+      </c>
+      <c r="L548" s="7">
+        <v>0</v>
+      </c>
+      <c r="M548" s="7">
+        <v>0</v>
+      </c>
+      <c r="N548" s="7">
+        <v>0</v>
+      </c>
+      <c r="O548" s="7">
+        <v>0</v>
+      </c>
+      <c r="P548" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q548" s="7">
+        <v>2.1628930246509901</v>
+      </c>
+      <c r="R548" s="7">
+        <v>3.15437849966797</v>
+      </c>
+      <c r="S548" s="7">
+        <v>0</v>
+      </c>
+      <c r="T548" t="b">
+        <v>0</v>
+      </c>
+      <c r="U548" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V548" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W548" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="549" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A549" s="10">
+        <v>548</v>
+      </c>
+      <c r="B549" s="7">
+        <v>5.4451295984320698</v>
+      </c>
+      <c r="C549" s="7">
+        <v>10.5162776537539</v>
+      </c>
+      <c r="D549" s="7">
+        <v>0</v>
+      </c>
+      <c r="E549" s="7">
+        <v>0</v>
+      </c>
+      <c r="F549" s="7">
+        <v>0</v>
+      </c>
+      <c r="G549" s="7">
+        <v>0</v>
+      </c>
+      <c r="H549" s="7">
+        <v>0</v>
+      </c>
+      <c r="I549" s="7">
+        <v>0</v>
+      </c>
+      <c r="J549" s="7">
+        <v>0</v>
+      </c>
+      <c r="K549" s="7">
+        <v>0</v>
+      </c>
+      <c r="L549" s="7">
+        <v>0</v>
+      </c>
+      <c r="M549" s="7">
+        <v>0</v>
+      </c>
+      <c r="N549" s="7">
+        <v>0</v>
+      </c>
+      <c r="O549" s="7">
+        <v>0</v>
+      </c>
+      <c r="P549" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q549" s="7">
+        <v>1.9415267436535599</v>
+      </c>
+      <c r="R549" s="7">
+        <v>4.0106655737446104</v>
+      </c>
+      <c r="S549" s="7">
+        <v>0</v>
+      </c>
+      <c r="T549" t="b">
+        <v>1</v>
+      </c>
+      <c r="U549" s="2">
+        <v>21</v>
+      </c>
+      <c r="V549" s="2">
+        <v>4</v>
+      </c>
+      <c r="W549" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="550" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A550" s="10">
+        <v>549</v>
+      </c>
+      <c r="B550" s="7">
+        <v>11.033054871085</v>
+      </c>
+      <c r="C550" s="7">
+        <v>0</v>
+      </c>
+      <c r="D550" s="7">
+        <v>0</v>
+      </c>
+      <c r="E550" s="7">
+        <v>0</v>
+      </c>
+      <c r="F550" s="7">
+        <v>0</v>
+      </c>
+      <c r="G550" s="7">
+        <v>0</v>
+      </c>
+      <c r="H550" s="7">
+        <v>0</v>
+      </c>
+      <c r="I550" s="7">
+        <v>0</v>
+      </c>
+      <c r="J550" s="7">
+        <v>0</v>
+      </c>
+      <c r="K550" s="7">
+        <v>0</v>
+      </c>
+      <c r="L550" s="7">
+        <v>0</v>
+      </c>
+      <c r="M550" s="7">
+        <v>10.117796923076099</v>
+      </c>
+      <c r="N550" s="7">
+        <v>0</v>
+      </c>
+      <c r="O550" s="7">
+        <v>0</v>
+      </c>
+      <c r="P550" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q550" s="7">
+        <v>1.71860662726552</v>
+      </c>
+      <c r="R550" s="7">
+        <v>4.3864436591254501</v>
+      </c>
+      <c r="S550" s="7">
+        <v>0</v>
+      </c>
+      <c r="T550" t="b">
+        <v>1</v>
+      </c>
+      <c r="U550" s="2">
+        <v>3275</v>
+      </c>
+      <c r="V550" s="2">
+        <v>31</v>
+      </c>
+      <c r="W550" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A551" s="10">
+        <v>550</v>
+      </c>
+      <c r="B551" s="7">
+        <v>0</v>
+      </c>
+      <c r="C551" s="7">
+        <v>0</v>
+      </c>
+      <c r="D551" s="7">
+        <v>0</v>
+      </c>
+      <c r="E551" s="7">
+        <v>0</v>
+      </c>
+      <c r="F551" s="7">
+        <v>0</v>
+      </c>
+      <c r="G551" s="7">
+        <v>0</v>
+      </c>
+      <c r="H551" s="7">
+        <v>0</v>
+      </c>
+      <c r="I551" s="7">
+        <v>0</v>
+      </c>
+      <c r="J551" s="7">
+        <v>12.6243933562998</v>
+      </c>
+      <c r="K551" s="7">
+        <v>0</v>
+      </c>
+      <c r="L551" s="7">
+        <v>9.6767516812601002</v>
+      </c>
+      <c r="M551" s="7">
+        <v>0</v>
+      </c>
+      <c r="N551" s="7">
+        <v>0</v>
+      </c>
+      <c r="O551" s="7">
+        <v>0</v>
+      </c>
+      <c r="P551" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q551" s="7">
+        <v>2.1874317004898298</v>
+      </c>
+      <c r="R551" s="7">
+        <v>1.9978129751781599</v>
+      </c>
+      <c r="S551" s="7">
+        <v>0</v>
+      </c>
+      <c r="T551" t="b">
+        <v>0</v>
+      </c>
+      <c r="U551" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V551" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W551" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="552" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A552" s="10">
+        <v>551</v>
+      </c>
+      <c r="B552" s="7">
+        <v>0</v>
+      </c>
+      <c r="C552" s="7">
+        <v>0</v>
+      </c>
+      <c r="D552" s="7">
+        <v>0</v>
+      </c>
+      <c r="E552" s="7">
+        <v>0</v>
+      </c>
+      <c r="F552" s="7">
+        <v>8.1668731633608402</v>
+      </c>
+      <c r="G552" s="7">
+        <v>0</v>
+      </c>
+      <c r="H552" s="7">
+        <v>0</v>
+      </c>
+      <c r="I552" s="7">
+        <v>0</v>
+      </c>
+      <c r="J552" s="7">
+        <v>0</v>
+      </c>
+      <c r="K552" s="7">
+        <v>0</v>
+      </c>
+      <c r="L552" s="7">
+        <v>12.298572611913601</v>
+      </c>
+      <c r="M552" s="7">
+        <v>0</v>
+      </c>
+      <c r="N552" s="7">
+        <v>0</v>
+      </c>
+      <c r="O552" s="7">
+        <v>0</v>
+      </c>
+      <c r="P552" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q552" s="7">
+        <v>2.4790694246645502</v>
+      </c>
+      <c r="R552" s="7">
+        <v>1.8857346953294001</v>
+      </c>
+      <c r="S552" s="7">
+        <v>0</v>
+      </c>
+      <c r="T552" t="b">
+        <v>1</v>
+      </c>
+      <c r="U552" s="2">
+        <v>60</v>
+      </c>
+      <c r="V552" s="2">
+        <v>46</v>
+      </c>
+      <c r="W552" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="553" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A553" s="10">
+        <v>552</v>
+      </c>
+      <c r="B553" s="7">
+        <v>0</v>
+      </c>
+      <c r="C553" s="7">
+        <v>0</v>
+      </c>
+      <c r="D553" s="7">
+        <v>0</v>
+      </c>
+      <c r="E553" s="7">
+        <v>0</v>
+      </c>
+      <c r="F553" s="7">
+        <v>0</v>
+      </c>
+      <c r="G553" s="7">
+        <v>0</v>
+      </c>
+      <c r="H553" s="7">
+        <v>0</v>
+      </c>
+      <c r="I553" s="7">
+        <v>0</v>
+      </c>
+      <c r="J553" s="7">
+        <v>12.6367462634164</v>
+      </c>
+      <c r="K553" s="7">
+        <v>0</v>
+      </c>
+      <c r="L553" s="7">
+        <v>0</v>
+      </c>
+      <c r="M553" s="7">
+        <v>11.154239457098299</v>
+      </c>
+      <c r="N553" s="7">
+        <v>0</v>
+      </c>
+      <c r="O553" s="7">
+        <v>0</v>
+      </c>
+      <c r="P553" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q553" s="7">
+        <v>3.1070133515546998</v>
+      </c>
+      <c r="R553" s="7">
+        <v>3.0762508431235598</v>
+      </c>
+      <c r="S553" s="7">
+        <v>0</v>
+      </c>
+      <c r="T553" t="b">
+        <v>1</v>
+      </c>
+      <c r="U553" s="2">
+        <v>30</v>
+      </c>
+      <c r="V553" s="2">
+        <v>37</v>
+      </c>
+      <c r="W553" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="554" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A554" s="10">
+        <v>553</v>
+      </c>
+      <c r="B554" s="7">
+        <v>0</v>
+      </c>
+      <c r="C554" s="7">
+        <v>11.6201888463712</v>
+      </c>
+      <c r="D554" s="7">
+        <v>0</v>
+      </c>
+      <c r="E554" s="7">
+        <v>0</v>
+      </c>
+      <c r="F554" s="7">
+        <v>0</v>
+      </c>
+      <c r="G554" s="7">
+        <v>0</v>
+      </c>
+      <c r="H554" s="7">
+        <v>0</v>
+      </c>
+      <c r="I554" s="7">
+        <v>10.5633552816532</v>
+      </c>
+      <c r="J554" s="7">
+        <v>0</v>
+      </c>
+      <c r="K554" s="7">
+        <v>0</v>
+      </c>
+      <c r="L554" s="7">
+        <v>0</v>
+      </c>
+      <c r="M554" s="7">
+        <v>0</v>
+      </c>
+      <c r="N554" s="7">
+        <v>0</v>
+      </c>
+      <c r="O554" s="7">
+        <v>0</v>
+      </c>
+      <c r="P554" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q554" s="7">
+        <v>1.57504059774766</v>
+      </c>
+      <c r="R554" s="7">
+        <v>4.3528394701390098</v>
+      </c>
+      <c r="S554" s="7">
+        <v>0</v>
+      </c>
+      <c r="T554" t="b">
+        <v>0</v>
+      </c>
+      <c r="U554" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V554" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W554" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="555" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A555" s="10">
+        <v>554</v>
+      </c>
+      <c r="B555" s="7">
+        <v>7.7215461321252299</v>
+      </c>
+      <c r="C555" s="7">
+        <v>0</v>
+      </c>
+      <c r="D555" s="7">
+        <v>0</v>
+      </c>
+      <c r="E555" s="7">
+        <v>0</v>
+      </c>
+      <c r="F555" s="7">
+        <v>0</v>
+      </c>
+      <c r="G555" s="7">
+        <v>0</v>
+      </c>
+      <c r="H555" s="7">
+        <v>0</v>
+      </c>
+      <c r="I555" s="7">
+        <v>0</v>
+      </c>
+      <c r="J555" s="7">
+        <v>9.3725515860074609</v>
+      </c>
+      <c r="K555" s="7">
+        <v>0</v>
+      </c>
+      <c r="L555" s="7">
+        <v>0</v>
+      </c>
+      <c r="M555" s="7">
+        <v>0</v>
+      </c>
+      <c r="N555" s="7">
+        <v>0</v>
+      </c>
+      <c r="O555" s="7">
+        <v>0</v>
+      </c>
+      <c r="P555" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q555" s="7">
+        <v>2.68159401454766</v>
+      </c>
+      <c r="R555" s="7">
+        <v>3.86438464049299</v>
+      </c>
+      <c r="S555" s="7">
+        <v>0</v>
+      </c>
+      <c r="T555" t="b">
+        <v>0</v>
+      </c>
+      <c r="U555" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V555" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W555" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="556" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A556" s="10">
+        <v>555</v>
+      </c>
+      <c r="B556" s="7">
+        <v>6.8492004984801298</v>
+      </c>
+      <c r="C556" s="7">
+        <v>0</v>
+      </c>
+      <c r="D556" s="7">
+        <v>0</v>
+      </c>
+      <c r="E556" s="7">
+        <v>0</v>
+      </c>
+      <c r="F556" s="7">
+        <v>0</v>
+      </c>
+      <c r="G556" s="7">
+        <v>0</v>
+      </c>
+      <c r="H556" s="7">
+        <v>10.333180961309299</v>
+      </c>
+      <c r="I556" s="7">
+        <v>0</v>
+      </c>
+      <c r="J556" s="7">
+        <v>0</v>
+      </c>
+      <c r="K556" s="7">
+        <v>0</v>
+      </c>
+      <c r="L556" s="7">
+        <v>0</v>
+      </c>
+      <c r="M556" s="7">
+        <v>0</v>
+      </c>
+      <c r="N556" s="7">
+        <v>0</v>
+      </c>
+      <c r="O556" s="7">
+        <v>0</v>
+      </c>
+      <c r="P556" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q556" s="7">
+        <v>2.26003140514125</v>
+      </c>
+      <c r="R556" s="7">
+        <v>4.6992272478361397</v>
+      </c>
+      <c r="S556" s="7">
+        <v>0</v>
+      </c>
+      <c r="T556" t="b">
+        <v>1</v>
+      </c>
+      <c r="U556" s="2">
+        <v>2289</v>
+      </c>
+      <c r="V556" s="2">
+        <v>341</v>
+      </c>
+      <c r="W556" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A557" s="10">
+        <v>556</v>
+      </c>
+      <c r="B557" s="7">
+        <v>0</v>
+      </c>
+      <c r="C557" s="7">
+        <v>0</v>
+      </c>
+      <c r="D557" s="7">
+        <v>0</v>
+      </c>
+      <c r="E557" s="7">
+        <v>0</v>
+      </c>
+      <c r="F557" s="7">
+        <v>6.9465430102700498</v>
+      </c>
+      <c r="G557" s="7">
+        <v>0</v>
+      </c>
+      <c r="H557" s="7">
+        <v>0</v>
+      </c>
+      <c r="I557" s="7">
+        <v>0</v>
+      </c>
+      <c r="J557" s="7">
+        <v>10.8841768952785</v>
+      </c>
+      <c r="K557" s="7">
+        <v>0</v>
+      </c>
+      <c r="L557" s="7">
+        <v>0</v>
+      </c>
+      <c r="M557" s="7">
+        <v>0</v>
+      </c>
+      <c r="N557" s="7">
+        <v>0</v>
+      </c>
+      <c r="O557" s="7">
+        <v>0</v>
+      </c>
+      <c r="P557" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q557" s="7">
+        <v>1.54746028624861</v>
+      </c>
+      <c r="R557" s="7">
+        <v>2.9681406936238099</v>
+      </c>
+      <c r="S557" s="7">
+        <v>0</v>
+      </c>
+      <c r="T557" t="b">
+        <v>0</v>
+      </c>
+      <c r="U557" s="2" t="str">
+        <f t="shared" si="31"/>
+        <v>NA</v>
+      </c>
+      <c r="V557" s="2" t="str">
+        <f t="shared" si="32"/>
+        <v>NA</v>
+      </c>
+      <c r="W557" s="12" t="str">
+        <f t="shared" si="33"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="558" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A558" s="10">
+        <v>557</v>
+      </c>
+      <c r="B558" s="7">
+        <v>0</v>
+      </c>
+      <c r="C558" s="7">
+        <v>0</v>
+      </c>
+      <c r="D558" s="7">
+        <v>0</v>
+      </c>
+      <c r="E558" s="7">
+        <v>0</v>
+      </c>
+      <c r="F558" s="7">
+        <v>0</v>
+      </c>
+      <c r="G558" s="7">
+        <v>11.369264346751599</v>
+      </c>
+      <c r="H558" s="7">
+        <v>0</v>
+      </c>
+      <c r="I558" s="7">
+        <v>0</v>
+      </c>
+      <c r="J558" s="7">
+        <v>0</v>
+      </c>
+      <c r="K558" s="7">
+        <v>8.29972104423533</v>
+      </c>
+      <c r="L558" s="7">
+        <v>0</v>
+      </c>
+      <c r="M558" s="7">
+        <v>0</v>
+      </c>
+      <c r="N558" s="7">
+        <v>0</v>
+      </c>
+      <c r="O558" s="7">
+        <v>0</v>
+      </c>
+      <c r="P558" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q558" s="7">
+        <v>1.70420411871269</v>
+      </c>
+      <c r="R558" s="7">
+        <v>4.6828565348977298</v>
+      </c>
+      <c r="S558" s="7">
+        <v>0</v>
+      </c>
+      <c r="T558" t="b">
+        <v>1</v>
+      </c>
+      <c r="U558" s="2">
+        <v>1332</v>
+      </c>
+      <c r="V558" s="2">
+        <v>309</v>
+      </c>
+      <c r="W558" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A559" s="10">
+        <v>558</v>
+      </c>
+      <c r="B559" s="7">
+        <v>0</v>
+      </c>
+      <c r="C559" s="7">
+        <v>0</v>
+      </c>
+      <c r="D559" s="7">
+        <v>0</v>
+      </c>
+      <c r="E559" s="7">
+        <v>0</v>
+      </c>
+      <c r="F559" s="7">
+        <v>0</v>
+      </c>
+      <c r="G559" s="7">
+        <v>0</v>
+      </c>
+      <c r="H559" s="7">
+        <v>0</v>
+      </c>
+      <c r="I559" s="7">
+        <v>12.7876427790354</v>
+      </c>
+      <c r="J559" s="7">
+        <v>0</v>
+      </c>
+      <c r="K559" s="7">
+        <v>11.5397109070387</v>
+      </c>
+      <c r="L559" s="7">
+        <v>0</v>
+      </c>
+      <c r="M559" s="7">
+        <v>0</v>
+      </c>
+      <c r="N559" s="7">
+        <v>0</v>
+      </c>
+      <c r="O559" s="7">
+        <v>0</v>
+      </c>
+      <c r="P559" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q559" s="7">
+        <v>2.3441409870771102</v>
+      </c>
+      <c r="R559" s="7">
+        <v>2.5368435239959899</v>
+      </c>
+      <c r="S559" s="7">
+        <v>0</v>
+      </c>
+      <c r="T559" t="b">
+        <v>1</v>
+      </c>
+      <c r="U559" s="2">
+        <v>23</v>
+      </c>
+      <c r="V559" s="2">
+        <v>9</v>
+      </c>
+      <c r="W559" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W523">
+  <conditionalFormatting sqref="A1:W559">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>

</xml_diff>

<commit_message>
Dataset updated till S582
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AAACCB-B5AB-8247-A275-B18B75F5CCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F7A9B2-0358-724A-BF0F-A1C3466E18A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="8020" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -231,7 +231,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -274,6 +274,13 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -301,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,11 +371,14 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -376,6 +386,36 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -699,11 +739,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W559"/>
+  <dimension ref="A1:W583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A524" zoomScale="116" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W559" sqref="W559"/>
+    <sheetView tabSelected="1" topLeftCell="A536" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W583" sqref="W583"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -39921,15 +39961,15 @@
         <v>0</v>
       </c>
       <c r="U537" s="2" t="str">
-        <f t="shared" ref="U537:U557" si="31">IF(T537=FALSE, "NA", "")</f>
+        <f t="shared" ref="U537:U555" si="31">IF(T537=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V537" s="2" t="str">
-        <f t="shared" ref="V537:V559" si="32">IF(T537=FALSE, "NA", "")</f>
+        <f t="shared" ref="V537:V557" si="32">IF(T537=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W537" s="12" t="str">
-        <f t="shared" ref="W537:W559" si="33">IF(T537=FALSE, "NA", "")</f>
+        <f t="shared" ref="W537:W557" si="33">IF(T537=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -41374,7 +41414,7 @@
         <v>0</v>
       </c>
       <c r="U557" s="2" t="str">
-        <f t="shared" si="31"/>
+        <f>IF(T557=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V557" s="2" t="str">
@@ -41528,10 +41568,1754 @@
         <v>1</v>
       </c>
     </row>
+    <row r="560" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A560" s="10">
+        <v>559</v>
+      </c>
+      <c r="B560" s="7">
+        <v>0</v>
+      </c>
+      <c r="C560" s="7">
+        <v>0</v>
+      </c>
+      <c r="D560" s="7">
+        <v>0</v>
+      </c>
+      <c r="E560" s="7">
+        <v>0</v>
+      </c>
+      <c r="F560" s="7">
+        <v>8.1052634369671193</v>
+      </c>
+      <c r="G560" s="7">
+        <v>0</v>
+      </c>
+      <c r="H560" s="7">
+        <v>0</v>
+      </c>
+      <c r="I560" s="7">
+        <v>10.6482898403156</v>
+      </c>
+      <c r="J560" s="7">
+        <v>0</v>
+      </c>
+      <c r="K560" s="7">
+        <v>0</v>
+      </c>
+      <c r="L560" s="7">
+        <v>0</v>
+      </c>
+      <c r="M560" s="7">
+        <v>0</v>
+      </c>
+      <c r="N560" s="7">
+        <v>0</v>
+      </c>
+      <c r="O560" s="7">
+        <v>0</v>
+      </c>
+      <c r="P560" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q560" s="7">
+        <v>0.66235199648968501</v>
+      </c>
+      <c r="R560" s="7">
+        <v>1.1600658294158399</v>
+      </c>
+      <c r="S560" s="7">
+        <v>0</v>
+      </c>
+      <c r="T560" t="b">
+        <v>1</v>
+      </c>
+      <c r="U560" s="2">
+        <v>33</v>
+      </c>
+      <c r="V560" s="2">
+        <v>80</v>
+      </c>
+      <c r="W560" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A561" s="10">
+        <v>560</v>
+      </c>
+      <c r="B561" s="7">
+        <v>0</v>
+      </c>
+      <c r="C561" s="7">
+        <v>0</v>
+      </c>
+      <c r="D561" s="7">
+        <v>0</v>
+      </c>
+      <c r="E561" s="7">
+        <v>0</v>
+      </c>
+      <c r="F561" s="7">
+        <v>13.958508472939901</v>
+      </c>
+      <c r="G561" s="7">
+        <v>8.3471565755412005</v>
+      </c>
+      <c r="H561" s="7">
+        <v>0</v>
+      </c>
+      <c r="I561" s="7">
+        <v>0</v>
+      </c>
+      <c r="J561" s="7">
+        <v>0</v>
+      </c>
+      <c r="K561" s="7">
+        <v>0</v>
+      </c>
+      <c r="L561" s="7">
+        <v>0</v>
+      </c>
+      <c r="M561" s="7">
+        <v>0</v>
+      </c>
+      <c r="N561" s="7">
+        <v>0</v>
+      </c>
+      <c r="O561" s="7">
+        <v>0</v>
+      </c>
+      <c r="P561" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q561" s="7">
+        <v>2.2708162930984899</v>
+      </c>
+      <c r="R561" s="7">
+        <v>5.0878094194232899</v>
+      </c>
+      <c r="S561" s="7">
+        <v>0</v>
+      </c>
+      <c r="T561" t="b">
+        <v>0</v>
+      </c>
+      <c r="U561" s="2" t="str">
+        <f>IF(T561=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V561" s="2" t="str">
+        <f>IF(T561=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W561" s="2" t="str">
+        <f>IF(T561=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="562" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A562" s="10">
+        <v>561</v>
+      </c>
+      <c r="B562" s="7">
+        <v>0</v>
+      </c>
+      <c r="C562" s="7">
+        <v>12.767662633607999</v>
+      </c>
+      <c r="D562" s="7">
+        <v>0</v>
+      </c>
+      <c r="E562" s="7">
+        <v>0</v>
+      </c>
+      <c r="F562" s="7">
+        <v>0</v>
+      </c>
+      <c r="G562" s="7">
+        <v>0</v>
+      </c>
+      <c r="H562" s="7">
+        <v>0</v>
+      </c>
+      <c r="I562" s="7">
+        <v>0</v>
+      </c>
+      <c r="J562" s="7">
+        <v>0</v>
+      </c>
+      <c r="K562" s="7">
+        <v>0</v>
+      </c>
+      <c r="L562" s="7">
+        <v>0</v>
+      </c>
+      <c r="M562" s="7">
+        <v>8.03959286594338</v>
+      </c>
+      <c r="N562" s="7">
+        <v>0</v>
+      </c>
+      <c r="O562" s="7">
+        <v>0</v>
+      </c>
+      <c r="P562" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q562" s="7">
+        <v>1.2416978552154301</v>
+      </c>
+      <c r="R562" s="7">
+        <v>3.7731831548752801</v>
+      </c>
+      <c r="S562" s="7">
+        <v>0</v>
+      </c>
+      <c r="T562" t="b">
+        <v>1</v>
+      </c>
+      <c r="U562" s="2">
+        <v>1301</v>
+      </c>
+      <c r="V562" s="2">
+        <v>325</v>
+      </c>
+      <c r="W562" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A563" s="10">
+        <v>562</v>
+      </c>
+      <c r="B563" s="7">
+        <v>0</v>
+      </c>
+      <c r="C563" s="7">
+        <v>0</v>
+      </c>
+      <c r="D563" s="7">
+        <v>6.7678149852970497</v>
+      </c>
+      <c r="E563" s="7">
+        <v>0</v>
+      </c>
+      <c r="F563" s="7">
+        <v>0</v>
+      </c>
+      <c r="G563" s="7">
+        <v>0</v>
+      </c>
+      <c r="H563" s="7">
+        <v>0</v>
+      </c>
+      <c r="I563" s="7">
+        <v>0</v>
+      </c>
+      <c r="J563" s="7">
+        <v>0</v>
+      </c>
+      <c r="K563" s="7">
+        <v>13.438222138722001</v>
+      </c>
+      <c r="L563" s="7">
+        <v>0</v>
+      </c>
+      <c r="M563" s="7">
+        <v>0</v>
+      </c>
+      <c r="N563" s="7">
+        <v>0</v>
+      </c>
+      <c r="O563" s="7">
+        <v>0</v>
+      </c>
+      <c r="P563" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q563" s="7">
+        <v>2.7332536156888998</v>
+      </c>
+      <c r="R563" s="7">
+        <v>3.9876331172739801</v>
+      </c>
+      <c r="S563" s="7">
+        <v>0</v>
+      </c>
+      <c r="T563" t="b">
+        <v>1</v>
+      </c>
+      <c r="U563" s="2">
+        <v>20</v>
+      </c>
+      <c r="V563" s="2">
+        <v>4</v>
+      </c>
+      <c r="W563" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="564" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A564" s="10">
+        <v>563</v>
+      </c>
+      <c r="B564" s="7">
+        <v>0</v>
+      </c>
+      <c r="C564" s="7">
+        <v>0</v>
+      </c>
+      <c r="D564" s="7">
+        <v>11.973119467075</v>
+      </c>
+      <c r="E564" s="7">
+        <v>9.9337688335878909</v>
+      </c>
+      <c r="F564" s="7">
+        <v>0</v>
+      </c>
+      <c r="G564" s="7">
+        <v>0</v>
+      </c>
+      <c r="H564" s="7">
+        <v>0</v>
+      </c>
+      <c r="I564" s="7">
+        <v>0</v>
+      </c>
+      <c r="J564" s="7">
+        <v>0</v>
+      </c>
+      <c r="K564" s="7">
+        <v>0</v>
+      </c>
+      <c r="L564" s="7">
+        <v>0</v>
+      </c>
+      <c r="M564" s="7">
+        <v>0</v>
+      </c>
+      <c r="N564" s="7">
+        <v>0</v>
+      </c>
+      <c r="O564" s="7">
+        <v>0</v>
+      </c>
+      <c r="P564" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q564" s="7">
+        <v>1.6045466094012899</v>
+      </c>
+      <c r="R564" s="7">
+        <v>1.9406093036779899</v>
+      </c>
+      <c r="S564" s="7">
+        <v>0</v>
+      </c>
+      <c r="T564" t="b">
+        <v>1</v>
+      </c>
+      <c r="U564" s="2">
+        <v>15</v>
+      </c>
+      <c r="V564" s="2">
+        <v>3</v>
+      </c>
+      <c r="W564" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="565" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A565" s="10">
+        <v>564</v>
+      </c>
+      <c r="B565" s="7">
+        <v>0</v>
+      </c>
+      <c r="C565" s="7">
+        <v>12.0540739844303</v>
+      </c>
+      <c r="D565" s="7">
+        <v>0</v>
+      </c>
+      <c r="E565" s="7">
+        <v>0</v>
+      </c>
+      <c r="F565" s="7">
+        <v>0</v>
+      </c>
+      <c r="G565" s="7">
+        <v>8.6294230436503998</v>
+      </c>
+      <c r="H565" s="7">
+        <v>0</v>
+      </c>
+      <c r="I565" s="7">
+        <v>0</v>
+      </c>
+      <c r="J565" s="7">
+        <v>0</v>
+      </c>
+      <c r="K565" s="7">
+        <v>0</v>
+      </c>
+      <c r="L565" s="7">
+        <v>0</v>
+      </c>
+      <c r="M565" s="7">
+        <v>0</v>
+      </c>
+      <c r="N565" s="7">
+        <v>0</v>
+      </c>
+      <c r="O565" s="7">
+        <v>0</v>
+      </c>
+      <c r="P565" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q565" s="7">
+        <v>2.65492771250354</v>
+      </c>
+      <c r="R565" s="7">
+        <v>1.1331565612874701</v>
+      </c>
+      <c r="S565" s="7">
+        <v>0</v>
+      </c>
+      <c r="T565" t="b">
+        <v>1</v>
+      </c>
+      <c r="U565" s="2">
+        <v>18</v>
+      </c>
+      <c r="V565" s="2">
+        <v>2</v>
+      </c>
+      <c r="W565" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="566" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A566" s="10">
+        <v>565</v>
+      </c>
+      <c r="B566" s="7">
+        <v>0</v>
+      </c>
+      <c r="C566" s="7">
+        <v>0</v>
+      </c>
+      <c r="D566" s="7">
+        <v>0</v>
+      </c>
+      <c r="E566" s="7">
+        <v>0</v>
+      </c>
+      <c r="F566" s="7">
+        <v>11.3047558437597</v>
+      </c>
+      <c r="G566" s="7">
+        <v>0</v>
+      </c>
+      <c r="H566" s="7">
+        <v>0</v>
+      </c>
+      <c r="I566" s="7">
+        <v>0</v>
+      </c>
+      <c r="J566" s="7">
+        <v>0</v>
+      </c>
+      <c r="K566" s="7">
+        <v>0</v>
+      </c>
+      <c r="L566" s="7">
+        <v>0</v>
+      </c>
+      <c r="M566" s="7">
+        <v>11.825215783693601</v>
+      </c>
+      <c r="N566" s="7">
+        <v>0</v>
+      </c>
+      <c r="O566" s="7">
+        <v>0</v>
+      </c>
+      <c r="P566" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q566" s="7">
+        <v>1.8704029091374399</v>
+      </c>
+      <c r="R566" s="7">
+        <v>4.6658420396417997</v>
+      </c>
+      <c r="S566" s="7">
+        <v>0</v>
+      </c>
+      <c r="T566" t="b">
+        <v>0</v>
+      </c>
+      <c r="U566" s="2" t="str">
+        <f>IF(T566=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V566" s="2" t="str">
+        <f>IF(T566=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W566" s="2" t="str">
+        <f>IF(T566=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="567" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A567" s="10">
+        <v>566</v>
+      </c>
+      <c r="B567" s="7">
+        <v>5.9725293876531804</v>
+      </c>
+      <c r="C567" s="7">
+        <v>0</v>
+      </c>
+      <c r="D567" s="7">
+        <v>0</v>
+      </c>
+      <c r="E567" s="7">
+        <v>0</v>
+      </c>
+      <c r="F567" s="7">
+        <v>0</v>
+      </c>
+      <c r="G567" s="7">
+        <v>9.9072063632262601</v>
+      </c>
+      <c r="H567" s="7">
+        <v>0</v>
+      </c>
+      <c r="I567" s="7">
+        <v>0</v>
+      </c>
+      <c r="J567" s="7">
+        <v>0</v>
+      </c>
+      <c r="K567" s="7">
+        <v>0</v>
+      </c>
+      <c r="L567" s="7">
+        <v>0</v>
+      </c>
+      <c r="M567" s="7">
+        <v>0</v>
+      </c>
+      <c r="N567" s="7">
+        <v>0</v>
+      </c>
+      <c r="O567" s="7">
+        <v>0</v>
+      </c>
+      <c r="P567" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q567" s="7">
+        <v>1.81321519611673</v>
+      </c>
+      <c r="R567" s="7">
+        <v>5.2683974864945702</v>
+      </c>
+      <c r="S567" s="7">
+        <v>0</v>
+      </c>
+      <c r="T567" t="b">
+        <v>1</v>
+      </c>
+      <c r="U567" s="2">
+        <v>1216</v>
+      </c>
+      <c r="V567" s="2">
+        <v>21</v>
+      </c>
+      <c r="W567" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A568" s="10">
+        <v>567</v>
+      </c>
+      <c r="B568" s="7">
+        <v>0</v>
+      </c>
+      <c r="C568" s="7">
+        <v>0</v>
+      </c>
+      <c r="D568" s="7">
+        <v>0</v>
+      </c>
+      <c r="E568" s="7">
+        <v>0</v>
+      </c>
+      <c r="F568" s="7">
+        <v>0</v>
+      </c>
+      <c r="G568" s="7">
+        <v>0</v>
+      </c>
+      <c r="H568" s="7">
+        <v>12.6755926259864</v>
+      </c>
+      <c r="I568" s="7">
+        <v>0</v>
+      </c>
+      <c r="J568" s="7">
+        <v>0</v>
+      </c>
+      <c r="K568" s="7">
+        <v>0</v>
+      </c>
+      <c r="L568" s="7">
+        <v>0</v>
+      </c>
+      <c r="M568" s="7">
+        <v>12.338012410002101</v>
+      </c>
+      <c r="N568" s="7">
+        <v>0</v>
+      </c>
+      <c r="O568" s="7">
+        <v>0</v>
+      </c>
+      <c r="P568" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q568" s="7">
+        <v>1.75101175079761</v>
+      </c>
+      <c r="R568" s="7">
+        <v>1.68295122338151</v>
+      </c>
+      <c r="S568" s="7">
+        <v>0</v>
+      </c>
+      <c r="T568" t="b">
+        <v>1</v>
+      </c>
+      <c r="U568" s="2">
+        <v>34</v>
+      </c>
+      <c r="V568" s="2">
+        <v>52</v>
+      </c>
+      <c r="W568" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="569" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A569" s="10">
+        <v>568</v>
+      </c>
+      <c r="B569" s="7">
+        <v>0</v>
+      </c>
+      <c r="C569" s="7">
+        <v>0</v>
+      </c>
+      <c r="D569" s="7">
+        <v>0</v>
+      </c>
+      <c r="E569" s="7">
+        <v>0</v>
+      </c>
+      <c r="F569" s="7">
+        <v>0</v>
+      </c>
+      <c r="G569" s="7">
+        <v>0</v>
+      </c>
+      <c r="H569" s="7">
+        <v>8.1746463355648409</v>
+      </c>
+      <c r="I569" s="7">
+        <v>0</v>
+      </c>
+      <c r="J569" s="7">
+        <v>0</v>
+      </c>
+      <c r="K569" s="7">
+        <v>0</v>
+      </c>
+      <c r="L569" s="7">
+        <v>7.8369415941857703</v>
+      </c>
+      <c r="M569" s="7">
+        <v>0</v>
+      </c>
+      <c r="N569" s="7">
+        <v>0</v>
+      </c>
+      <c r="O569" s="7">
+        <v>0</v>
+      </c>
+      <c r="P569" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q569" s="7">
+        <v>2.6411200459623099</v>
+      </c>
+      <c r="R569" s="7">
+        <v>4.5923860110838204</v>
+      </c>
+      <c r="S569" s="7">
+        <v>0</v>
+      </c>
+      <c r="T569" t="b">
+        <v>1</v>
+      </c>
+      <c r="U569" s="24">
+        <v>4265</v>
+      </c>
+      <c r="V569" s="2">
+        <v>16</v>
+      </c>
+      <c r="W569" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A570" s="10">
+        <v>569</v>
+      </c>
+      <c r="B570" s="7">
+        <v>0</v>
+      </c>
+      <c r="C570" s="7">
+        <v>0</v>
+      </c>
+      <c r="D570" s="7">
+        <v>0</v>
+      </c>
+      <c r="E570" s="7">
+        <v>8.0211847729726706</v>
+      </c>
+      <c r="F570" s="7">
+        <v>0</v>
+      </c>
+      <c r="G570" s="7">
+        <v>0</v>
+      </c>
+      <c r="H570" s="7">
+        <v>0</v>
+      </c>
+      <c r="I570" s="7">
+        <v>0</v>
+      </c>
+      <c r="J570" s="7">
+        <v>0</v>
+      </c>
+      <c r="K570" s="7">
+        <v>0</v>
+      </c>
+      <c r="L570" s="7">
+        <v>9.3727433863551006</v>
+      </c>
+      <c r="M570" s="7">
+        <v>0</v>
+      </c>
+      <c r="N570" s="7">
+        <v>0</v>
+      </c>
+      <c r="O570" s="7">
+        <v>0</v>
+      </c>
+      <c r="P570" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q570" s="7">
+        <v>1.57172540751946</v>
+      </c>
+      <c r="R570" s="7">
+        <v>4.75900920205099</v>
+      </c>
+      <c r="S570" s="7">
+        <v>0</v>
+      </c>
+      <c r="T570" t="b">
+        <v>0</v>
+      </c>
+      <c r="U570" s="2" t="str">
+        <f>IF(T570=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V570" s="2" t="str">
+        <f>IF(T570=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W570" s="12" t="str">
+        <f>IF(T570=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="571" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A571" s="10">
+        <v>570</v>
+      </c>
+      <c r="B571" s="7">
+        <v>0</v>
+      </c>
+      <c r="C571" s="7">
+        <v>0</v>
+      </c>
+      <c r="D571" s="7">
+        <v>0</v>
+      </c>
+      <c r="E571" s="7">
+        <v>12.759272753152</v>
+      </c>
+      <c r="F571" s="7">
+        <v>0</v>
+      </c>
+      <c r="G571" s="7">
+        <v>10.5043387835206</v>
+      </c>
+      <c r="H571" s="7">
+        <v>0</v>
+      </c>
+      <c r="I571" s="7">
+        <v>0</v>
+      </c>
+      <c r="J571" s="7">
+        <v>0</v>
+      </c>
+      <c r="K571" s="7">
+        <v>0</v>
+      </c>
+      <c r="L571" s="7">
+        <v>0</v>
+      </c>
+      <c r="M571" s="7">
+        <v>0</v>
+      </c>
+      <c r="N571" s="7">
+        <v>0</v>
+      </c>
+      <c r="O571" s="7">
+        <v>0</v>
+      </c>
+      <c r="P571" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q571" s="7">
+        <v>1.35919455413371</v>
+      </c>
+      <c r="R571" s="7">
+        <v>3.4698726750863602</v>
+      </c>
+      <c r="S571" s="7">
+        <v>0</v>
+      </c>
+      <c r="T571" t="b">
+        <v>0</v>
+      </c>
+      <c r="U571" s="2" t="str">
+        <f t="shared" ref="U571:U583" si="34">IF(T571=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V571" s="2" t="str">
+        <f t="shared" ref="V571:V583" si="35">IF(T571=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W571" s="12" t="str">
+        <f t="shared" ref="W571:W583" si="36">IF(T571=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="572" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A572" s="10">
+        <v>571</v>
+      </c>
+      <c r="B572" s="7">
+        <v>9.8281067790602297</v>
+      </c>
+      <c r="C572" s="7">
+        <v>0</v>
+      </c>
+      <c r="D572" s="7">
+        <v>0</v>
+      </c>
+      <c r="E572" s="7">
+        <v>0</v>
+      </c>
+      <c r="F572" s="7">
+        <v>0</v>
+      </c>
+      <c r="G572" s="7">
+        <v>0</v>
+      </c>
+      <c r="H572" s="7">
+        <v>0</v>
+      </c>
+      <c r="I572" s="7">
+        <v>6.7588951025894204</v>
+      </c>
+      <c r="J572" s="7">
+        <v>0</v>
+      </c>
+      <c r="K572" s="7">
+        <v>0</v>
+      </c>
+      <c r="L572" s="7">
+        <v>0</v>
+      </c>
+      <c r="M572" s="7">
+        <v>0</v>
+      </c>
+      <c r="N572" s="7">
+        <v>0</v>
+      </c>
+      <c r="O572" s="7">
+        <v>0</v>
+      </c>
+      <c r="P572" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q572" s="7">
+        <v>1.37508555535426</v>
+      </c>
+      <c r="R572" s="7">
+        <v>2.8485764800185698</v>
+      </c>
+      <c r="S572" s="7">
+        <v>0</v>
+      </c>
+      <c r="T572" t="b">
+        <v>1</v>
+      </c>
+      <c r="U572" s="2">
+        <v>826</v>
+      </c>
+      <c r="V572" s="2">
+        <v>72</v>
+      </c>
+      <c r="W572" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="573" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A573" s="10">
+        <v>572</v>
+      </c>
+      <c r="B573" s="7">
+        <v>0</v>
+      </c>
+      <c r="C573" s="7">
+        <v>0</v>
+      </c>
+      <c r="D573" s="7">
+        <v>0</v>
+      </c>
+      <c r="E573" s="7">
+        <v>0</v>
+      </c>
+      <c r="F573" s="7">
+        <v>0</v>
+      </c>
+      <c r="G573" s="7">
+        <v>8.9485491467923506</v>
+      </c>
+      <c r="H573" s="7">
+        <v>0</v>
+      </c>
+      <c r="I573" s="7">
+        <v>0</v>
+      </c>
+      <c r="J573" s="7">
+        <v>0</v>
+      </c>
+      <c r="K573" s="7">
+        <v>0</v>
+      </c>
+      <c r="L573" s="7">
+        <v>0</v>
+      </c>
+      <c r="M573" s="7">
+        <v>11.304271436412099</v>
+      </c>
+      <c r="N573" s="7">
+        <v>0</v>
+      </c>
+      <c r="O573" s="7">
+        <v>0</v>
+      </c>
+      <c r="P573" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q573" s="7">
+        <v>2.2481220027581101</v>
+      </c>
+      <c r="R573" s="7">
+        <v>2.22690152855114</v>
+      </c>
+      <c r="S573" s="7">
+        <v>0</v>
+      </c>
+      <c r="T573" t="b">
+        <v>0</v>
+      </c>
+      <c r="U573" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V573" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W573" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="574" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A574" s="10">
+        <v>573</v>
+      </c>
+      <c r="B574" s="7">
+        <v>9.3991964455964805</v>
+      </c>
+      <c r="C574" s="7">
+        <v>0</v>
+      </c>
+      <c r="D574" s="7">
+        <v>0</v>
+      </c>
+      <c r="E574" s="7">
+        <v>0</v>
+      </c>
+      <c r="F574" s="7">
+        <v>0</v>
+      </c>
+      <c r="G574" s="7">
+        <v>12.927326191915</v>
+      </c>
+      <c r="H574" s="7">
+        <v>0</v>
+      </c>
+      <c r="I574" s="7">
+        <v>0</v>
+      </c>
+      <c r="J574" s="7">
+        <v>0</v>
+      </c>
+      <c r="K574" s="7">
+        <v>0</v>
+      </c>
+      <c r="L574" s="7">
+        <v>0</v>
+      </c>
+      <c r="M574" s="7">
+        <v>0</v>
+      </c>
+      <c r="N574" s="7">
+        <v>0</v>
+      </c>
+      <c r="O574" s="7">
+        <v>0</v>
+      </c>
+      <c r="P574" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q574" s="7">
+        <v>2.97646122318955</v>
+      </c>
+      <c r="R574" s="7">
+        <v>1.41654556360941</v>
+      </c>
+      <c r="S574" s="7">
+        <v>0</v>
+      </c>
+      <c r="T574" t="b">
+        <v>0</v>
+      </c>
+      <c r="U574" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V574" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W574" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="575" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A575" s="10">
+        <v>574</v>
+      </c>
+      <c r="B575" s="7">
+        <v>0</v>
+      </c>
+      <c r="C575" s="7">
+        <v>0</v>
+      </c>
+      <c r="D575" s="7">
+        <v>0</v>
+      </c>
+      <c r="E575" s="7">
+        <v>8.6747168125536493</v>
+      </c>
+      <c r="F575" s="7">
+        <v>0</v>
+      </c>
+      <c r="G575" s="7">
+        <v>0</v>
+      </c>
+      <c r="H575" s="7">
+        <v>9.7654592530345408</v>
+      </c>
+      <c r="I575" s="7">
+        <v>0</v>
+      </c>
+      <c r="J575" s="7">
+        <v>0</v>
+      </c>
+      <c r="K575" s="7">
+        <v>0</v>
+      </c>
+      <c r="L575" s="7">
+        <v>0</v>
+      </c>
+      <c r="M575" s="7">
+        <v>0</v>
+      </c>
+      <c r="N575" s="7">
+        <v>0</v>
+      </c>
+      <c r="O575" s="7">
+        <v>0</v>
+      </c>
+      <c r="P575" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q575" s="7">
+        <v>2.80846091086064</v>
+      </c>
+      <c r="R575" s="7">
+        <v>5.0519654471627602</v>
+      </c>
+      <c r="S575" s="7">
+        <v>0</v>
+      </c>
+      <c r="T575" t="b">
+        <v>0</v>
+      </c>
+      <c r="U575" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V575" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W575" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="576" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A576" s="10">
+        <v>575</v>
+      </c>
+      <c r="B576" s="7">
+        <v>0</v>
+      </c>
+      <c r="C576" s="7">
+        <v>0</v>
+      </c>
+      <c r="D576" s="7">
+        <v>0</v>
+      </c>
+      <c r="E576" s="7">
+        <v>10.7969889797274</v>
+      </c>
+      <c r="F576" s="7">
+        <v>0</v>
+      </c>
+      <c r="G576" s="7">
+        <v>0</v>
+      </c>
+      <c r="H576" s="7">
+        <v>0</v>
+      </c>
+      <c r="I576" s="7">
+        <v>0</v>
+      </c>
+      <c r="J576" s="7">
+        <v>0</v>
+      </c>
+      <c r="K576" s="7">
+        <v>7.9058684210345804</v>
+      </c>
+      <c r="L576" s="7">
+        <v>0</v>
+      </c>
+      <c r="M576" s="7">
+        <v>0</v>
+      </c>
+      <c r="N576" s="7">
+        <v>0</v>
+      </c>
+      <c r="O576" s="7">
+        <v>0</v>
+      </c>
+      <c r="P576" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q576" s="7">
+        <v>2.85230367831607</v>
+      </c>
+      <c r="R576" s="7">
+        <v>3.0365610218765098</v>
+      </c>
+      <c r="S576" s="7">
+        <v>0</v>
+      </c>
+      <c r="T576" t="b">
+        <v>1</v>
+      </c>
+      <c r="U576" s="2">
+        <v>44</v>
+      </c>
+      <c r="V576" s="2">
+        <v>13</v>
+      </c>
+      <c r="W576" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="577" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A577" s="10">
+        <v>576</v>
+      </c>
+      <c r="B577" s="7">
+        <v>0</v>
+      </c>
+      <c r="C577" s="7">
+        <v>0</v>
+      </c>
+      <c r="D577" s="7">
+        <v>0</v>
+      </c>
+      <c r="E577" s="7">
+        <v>0</v>
+      </c>
+      <c r="F577" s="7">
+        <v>7.79711246526103</v>
+      </c>
+      <c r="G577" s="7">
+        <v>0</v>
+      </c>
+      <c r="H577" s="7">
+        <v>0</v>
+      </c>
+      <c r="I577" s="7">
+        <v>0</v>
+      </c>
+      <c r="J577" s="7">
+        <v>0</v>
+      </c>
+      <c r="K577" s="7">
+        <v>0</v>
+      </c>
+      <c r="L577" s="7">
+        <v>0</v>
+      </c>
+      <c r="M577" s="7">
+        <v>8.3559088633622505</v>
+      </c>
+      <c r="N577" s="7">
+        <v>0</v>
+      </c>
+      <c r="O577" s="7">
+        <v>0</v>
+      </c>
+      <c r="P577" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q577" s="7">
+        <v>1.77628156116833</v>
+      </c>
+      <c r="R577" s="7">
+        <v>2.1280328780734199</v>
+      </c>
+      <c r="S577" s="7">
+        <v>0</v>
+      </c>
+      <c r="T577" t="b">
+        <v>1</v>
+      </c>
+      <c r="U577" s="2">
+        <v>22</v>
+      </c>
+      <c r="V577" s="2">
+        <v>50</v>
+      </c>
+      <c r="W577" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="578" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A578" s="10">
+        <v>577</v>
+      </c>
+      <c r="B578" s="7">
+        <v>0</v>
+      </c>
+      <c r="C578" s="7">
+        <v>0</v>
+      </c>
+      <c r="D578" s="7">
+        <v>0</v>
+      </c>
+      <c r="E578" s="7">
+        <v>0</v>
+      </c>
+      <c r="F578" s="7">
+        <v>0</v>
+      </c>
+      <c r="G578" s="7">
+        <v>8.20722154130749</v>
+      </c>
+      <c r="H578" s="7">
+        <v>0</v>
+      </c>
+      <c r="I578" s="7">
+        <v>0</v>
+      </c>
+      <c r="J578" s="7">
+        <v>0</v>
+      </c>
+      <c r="K578" s="7">
+        <v>12.5414171059337</v>
+      </c>
+      <c r="L578" s="7">
+        <v>0</v>
+      </c>
+      <c r="M578" s="7">
+        <v>0</v>
+      </c>
+      <c r="N578" s="7">
+        <v>0</v>
+      </c>
+      <c r="O578" s="7">
+        <v>0</v>
+      </c>
+      <c r="P578" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q578" s="7">
+        <v>0.76861597990844499</v>
+      </c>
+      <c r="R578" s="7">
+        <v>3.2741044338954501</v>
+      </c>
+      <c r="S578" s="7">
+        <v>0</v>
+      </c>
+      <c r="T578" t="b">
+        <v>1</v>
+      </c>
+      <c r="U578" s="2">
+        <v>25</v>
+      </c>
+      <c r="V578" s="2">
+        <v>5</v>
+      </c>
+      <c r="W578" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="579" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A579" s="10">
+        <v>578</v>
+      </c>
+      <c r="B579" s="7">
+        <v>0</v>
+      </c>
+      <c r="C579" s="7">
+        <v>0</v>
+      </c>
+      <c r="D579" s="7">
+        <v>0</v>
+      </c>
+      <c r="E579" s="7">
+        <v>0</v>
+      </c>
+      <c r="F579" s="7">
+        <v>0</v>
+      </c>
+      <c r="G579" s="7">
+        <v>0</v>
+      </c>
+      <c r="H579" s="7">
+        <v>0</v>
+      </c>
+      <c r="I579" s="7">
+        <v>6.22518450996699</v>
+      </c>
+      <c r="J579" s="7">
+        <v>0</v>
+      </c>
+      <c r="K579" s="7">
+        <v>10.4211652293922</v>
+      </c>
+      <c r="L579" s="7">
+        <v>0</v>
+      </c>
+      <c r="M579" s="7">
+        <v>0</v>
+      </c>
+      <c r="N579" s="7">
+        <v>0</v>
+      </c>
+      <c r="O579" s="7">
+        <v>0</v>
+      </c>
+      <c r="P579" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q579" s="7">
+        <v>1.6513834436985599</v>
+      </c>
+      <c r="R579" s="7">
+        <v>1.35550003954432</v>
+      </c>
+      <c r="S579" s="7">
+        <v>0</v>
+      </c>
+      <c r="T579" t="b">
+        <v>1</v>
+      </c>
+      <c r="U579" s="2">
+        <v>27</v>
+      </c>
+      <c r="V579" s="2">
+        <v>2</v>
+      </c>
+      <c r="W579" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="580" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A580" s="10">
+        <v>579</v>
+      </c>
+      <c r="B580" s="7">
+        <v>0</v>
+      </c>
+      <c r="C580" s="7">
+        <v>0</v>
+      </c>
+      <c r="D580" s="7">
+        <v>0</v>
+      </c>
+      <c r="E580" s="7">
+        <v>0</v>
+      </c>
+      <c r="F580" s="7">
+        <v>0</v>
+      </c>
+      <c r="G580" s="7">
+        <v>0</v>
+      </c>
+      <c r="H580" s="7">
+        <v>0</v>
+      </c>
+      <c r="I580" s="7">
+        <v>0</v>
+      </c>
+      <c r="J580" s="7">
+        <v>0</v>
+      </c>
+      <c r="K580" s="7">
+        <v>0</v>
+      </c>
+      <c r="L580" s="7">
+        <v>11.386005225637399</v>
+      </c>
+      <c r="M580" s="7">
+        <v>11.221339894332001</v>
+      </c>
+      <c r="N580" s="7">
+        <v>0</v>
+      </c>
+      <c r="O580" s="7">
+        <v>0</v>
+      </c>
+      <c r="P580" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q580" s="7">
+        <v>2.5641103037893802</v>
+      </c>
+      <c r="R580" s="7">
+        <v>3.5995439800626001</v>
+      </c>
+      <c r="S580" s="7">
+        <v>0</v>
+      </c>
+      <c r="T580" t="b">
+        <v>1</v>
+      </c>
+      <c r="U580" s="2">
+        <v>4940</v>
+      </c>
+      <c r="V580" s="2">
+        <v>124</v>
+      </c>
+      <c r="W580" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A581" s="10">
+        <v>580</v>
+      </c>
+      <c r="B581" s="7">
+        <v>0</v>
+      </c>
+      <c r="C581" s="7">
+        <v>0</v>
+      </c>
+      <c r="D581" s="7">
+        <v>0</v>
+      </c>
+      <c r="E581" s="7">
+        <v>0</v>
+      </c>
+      <c r="F581" s="7">
+        <v>0</v>
+      </c>
+      <c r="G581" s="7">
+        <v>12.677412420723201</v>
+      </c>
+      <c r="H581" s="7">
+        <v>0</v>
+      </c>
+      <c r="I581" s="7">
+        <v>0</v>
+      </c>
+      <c r="J581" s="7">
+        <v>0</v>
+      </c>
+      <c r="K581" s="7">
+        <v>0</v>
+      </c>
+      <c r="L581" s="7">
+        <v>9.2171102718637901</v>
+      </c>
+      <c r="M581" s="7">
+        <v>0</v>
+      </c>
+      <c r="N581" s="7">
+        <v>0</v>
+      </c>
+      <c r="O581" s="7">
+        <v>0</v>
+      </c>
+      <c r="P581" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q581" s="7">
+        <v>1.3345283764726701</v>
+      </c>
+      <c r="R581" s="7">
+        <v>1.4426021030478</v>
+      </c>
+      <c r="S581" s="7">
+        <v>0</v>
+      </c>
+      <c r="T581" t="b">
+        <v>1</v>
+      </c>
+      <c r="U581" s="2">
+        <v>1642</v>
+      </c>
+      <c r="V581" s="2">
+        <v>103</v>
+      </c>
+      <c r="W581" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="582" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A582" s="10">
+        <v>581</v>
+      </c>
+      <c r="B582" s="7">
+        <v>0</v>
+      </c>
+      <c r="C582" s="7">
+        <v>0</v>
+      </c>
+      <c r="D582" s="7">
+        <v>0</v>
+      </c>
+      <c r="E582" s="7">
+        <v>11.7152424554234</v>
+      </c>
+      <c r="F582" s="7">
+        <v>0</v>
+      </c>
+      <c r="G582" s="7">
+        <v>0</v>
+      </c>
+      <c r="H582" s="7">
+        <v>12.929149218363699</v>
+      </c>
+      <c r="I582" s="7">
+        <v>0</v>
+      </c>
+      <c r="J582" s="7">
+        <v>0</v>
+      </c>
+      <c r="K582" s="7">
+        <v>0</v>
+      </c>
+      <c r="L582" s="7">
+        <v>0</v>
+      </c>
+      <c r="M582" s="7">
+        <v>0</v>
+      </c>
+      <c r="N582" s="7">
+        <v>0</v>
+      </c>
+      <c r="O582" s="7">
+        <v>0</v>
+      </c>
+      <c r="P582" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q582" s="7">
+        <v>1.12532035362503</v>
+      </c>
+      <c r="R582" s="7">
+        <v>4.4268390537311602</v>
+      </c>
+      <c r="S582" s="7">
+        <v>0</v>
+      </c>
+      <c r="T582" t="b">
+        <v>0</v>
+      </c>
+      <c r="U582" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V582" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W582" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="583" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A583" s="10">
+        <v>582</v>
+      </c>
+      <c r="B583" s="7">
+        <v>6.5312392910791903</v>
+      </c>
+      <c r="C583" s="7">
+        <v>0</v>
+      </c>
+      <c r="D583" s="7">
+        <v>0</v>
+      </c>
+      <c r="E583" s="7">
+        <v>8.3710971893037591</v>
+      </c>
+      <c r="F583" s="7">
+        <v>0</v>
+      </c>
+      <c r="G583" s="7">
+        <v>0</v>
+      </c>
+      <c r="H583" s="7">
+        <v>0</v>
+      </c>
+      <c r="I583" s="7">
+        <v>0</v>
+      </c>
+      <c r="J583" s="7">
+        <v>0</v>
+      </c>
+      <c r="K583" s="7">
+        <v>0</v>
+      </c>
+      <c r="L583" s="7">
+        <v>0</v>
+      </c>
+      <c r="M583" s="7">
+        <v>0</v>
+      </c>
+      <c r="N583" s="7">
+        <v>0</v>
+      </c>
+      <c r="O583" s="7">
+        <v>0</v>
+      </c>
+      <c r="P583" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q583" s="7">
+        <v>2.25497903960667</v>
+      </c>
+      <c r="R583" s="7">
+        <v>4.1922110327235202</v>
+      </c>
+      <c r="S583" s="7">
+        <v>0</v>
+      </c>
+      <c r="T583" t="b">
+        <v>0</v>
+      </c>
+      <c r="U583" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V583" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W583" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W559">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A1:W583">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$T1=TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U580">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+      <formula>4000</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>4000</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U569">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dataset updated till S618
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F7A9B2-0358-724A-BF0F-A1C3466E18A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6B9256-ACB1-9440-82E6-9FC896D9E309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="-21140" windowWidth="38400" windowHeight="21140" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -378,7 +378,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -401,6 +431,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -411,11 +451,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -739,11 +779,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W583"/>
+  <dimension ref="A1:W619"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A536" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W583" sqref="W583"/>
+    <sheetView tabSelected="1" topLeftCell="A582" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W619" sqref="W619"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42420,15 +42460,15 @@
         <v>0</v>
       </c>
       <c r="U571" s="2" t="str">
-        <f t="shared" ref="U571:U583" si="34">IF(T571=FALSE, "NA", "")</f>
+        <f t="shared" ref="U571:U619" si="34">IF(T571=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V571" s="2" t="str">
-        <f t="shared" ref="V571:V583" si="35">IF(T571=FALSE, "NA", "")</f>
+        <f t="shared" ref="V571:V619" si="35">IF(T571=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W571" s="12" t="str">
-        <f t="shared" ref="W571:W583" si="36">IF(T571=FALSE, "NA", "")</f>
+        <f t="shared" ref="W571:W619" si="36">IF(T571=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -43299,22 +43339,2674 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="584" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A584" s="10">
+        <v>583</v>
+      </c>
+      <c r="B584" s="7">
+        <v>0</v>
+      </c>
+      <c r="C584" s="7">
+        <v>0</v>
+      </c>
+      <c r="D584" s="7">
+        <v>0</v>
+      </c>
+      <c r="E584" s="7">
+        <v>8.8936023438133596</v>
+      </c>
+      <c r="F584" s="7">
+        <v>0</v>
+      </c>
+      <c r="G584" s="7">
+        <v>9.3289255146874801</v>
+      </c>
+      <c r="H584" s="7">
+        <v>0</v>
+      </c>
+      <c r="I584" s="7">
+        <v>0</v>
+      </c>
+      <c r="J584" s="7">
+        <v>0</v>
+      </c>
+      <c r="K584" s="7">
+        <v>0</v>
+      </c>
+      <c r="L584" s="7">
+        <v>0</v>
+      </c>
+      <c r="M584" s="7">
+        <v>0</v>
+      </c>
+      <c r="N584" s="7">
+        <v>0</v>
+      </c>
+      <c r="O584" s="7">
+        <v>1.54364595649059</v>
+      </c>
+      <c r="P584" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q584" s="7">
+        <v>0</v>
+      </c>
+      <c r="R584" s="7">
+        <v>1.0908097844893301</v>
+      </c>
+      <c r="S584" s="7">
+        <v>0</v>
+      </c>
+      <c r="T584" t="b">
+        <v>0</v>
+      </c>
+      <c r="U584" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V584" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W584" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="585" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A585" s="10">
+        <v>584</v>
+      </c>
+      <c r="B585" s="7">
+        <v>0</v>
+      </c>
+      <c r="C585" s="7">
+        <v>0</v>
+      </c>
+      <c r="D585" s="7">
+        <v>0</v>
+      </c>
+      <c r="E585" s="7">
+        <v>0</v>
+      </c>
+      <c r="F585" s="7">
+        <v>0</v>
+      </c>
+      <c r="G585" s="7">
+        <v>0</v>
+      </c>
+      <c r="H585" s="7">
+        <v>0</v>
+      </c>
+      <c r="I585" s="7">
+        <v>0</v>
+      </c>
+      <c r="J585" s="7">
+        <v>12.819365569421301</v>
+      </c>
+      <c r="K585" s="7">
+        <v>0</v>
+      </c>
+      <c r="L585" s="7">
+        <v>0</v>
+      </c>
+      <c r="M585" s="7">
+        <v>9.2825745062127591</v>
+      </c>
+      <c r="N585" s="7">
+        <v>0</v>
+      </c>
+      <c r="O585" s="7">
+        <v>1.2479405046783001</v>
+      </c>
+      <c r="P585" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q585" s="7">
+        <v>0</v>
+      </c>
+      <c r="R585" s="7">
+        <v>4.9667281068840197</v>
+      </c>
+      <c r="S585" s="7">
+        <v>0</v>
+      </c>
+      <c r="T585" t="b">
+        <v>0</v>
+      </c>
+      <c r="U585" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V585" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W585" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="586" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A586" s="10">
+        <v>585</v>
+      </c>
+      <c r="B586" s="7">
+        <v>8.11811687486904</v>
+      </c>
+      <c r="C586" s="7">
+        <v>0</v>
+      </c>
+      <c r="D586" s="7">
+        <v>0</v>
+      </c>
+      <c r="E586" s="7">
+        <v>0</v>
+      </c>
+      <c r="F586" s="7">
+        <v>0</v>
+      </c>
+      <c r="G586" s="7">
+        <v>0</v>
+      </c>
+      <c r="H586" s="7">
+        <v>0</v>
+      </c>
+      <c r="I586" s="7">
+        <v>0</v>
+      </c>
+      <c r="J586" s="7">
+        <v>8.4355960136893806</v>
+      </c>
+      <c r="K586" s="7">
+        <v>0</v>
+      </c>
+      <c r="L586" s="7">
+        <v>0</v>
+      </c>
+      <c r="M586" s="7">
+        <v>0</v>
+      </c>
+      <c r="N586" s="7">
+        <v>0</v>
+      </c>
+      <c r="O586" s="7">
+        <v>2.5612580831221101</v>
+      </c>
+      <c r="P586" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q586" s="7">
+        <v>0</v>
+      </c>
+      <c r="R586" s="7">
+        <v>2.7852464325966202</v>
+      </c>
+      <c r="S586" s="7">
+        <v>0</v>
+      </c>
+      <c r="T586" t="b">
+        <v>0</v>
+      </c>
+      <c r="U586" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V586" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W586" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="587" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A587" s="10">
+        <v>586</v>
+      </c>
+      <c r="B587" s="7">
+        <v>0</v>
+      </c>
+      <c r="C587" s="7">
+        <v>0</v>
+      </c>
+      <c r="D587" s="7">
+        <v>0</v>
+      </c>
+      <c r="E587" s="7">
+        <v>0</v>
+      </c>
+      <c r="F587" s="7">
+        <v>0</v>
+      </c>
+      <c r="G587" s="7">
+        <v>0</v>
+      </c>
+      <c r="H587" s="7">
+        <v>0</v>
+      </c>
+      <c r="I587" s="7">
+        <v>0</v>
+      </c>
+      <c r="J587" s="7">
+        <v>0</v>
+      </c>
+      <c r="K587" s="7">
+        <v>0</v>
+      </c>
+      <c r="L587" s="7">
+        <v>8.2392537406377198</v>
+      </c>
+      <c r="M587" s="7">
+        <v>13.1114376608213</v>
+      </c>
+      <c r="N587" s="7">
+        <v>0</v>
+      </c>
+      <c r="O587" s="7">
+        <v>1.9611337690183199</v>
+      </c>
+      <c r="P587" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q587" s="7">
+        <v>0</v>
+      </c>
+      <c r="R587" s="7">
+        <v>4.97385387923807</v>
+      </c>
+      <c r="S587" s="7">
+        <v>0</v>
+      </c>
+      <c r="T587" t="b">
+        <v>0</v>
+      </c>
+      <c r="U587" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V587" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W587" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="588" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A588" s="10">
+        <v>587</v>
+      </c>
+      <c r="B588" s="7">
+        <v>15.1162535118051</v>
+      </c>
+      <c r="C588" s="7">
+        <v>0</v>
+      </c>
+      <c r="D588" s="7">
+        <v>0</v>
+      </c>
+      <c r="E588" s="7">
+        <v>0</v>
+      </c>
+      <c r="F588" s="7">
+        <v>0</v>
+      </c>
+      <c r="G588" s="7">
+        <v>0</v>
+      </c>
+      <c r="H588" s="7">
+        <v>0</v>
+      </c>
+      <c r="I588" s="7">
+        <v>0</v>
+      </c>
+      <c r="J588" s="7">
+        <v>0</v>
+      </c>
+      <c r="K588" s="7">
+        <v>0</v>
+      </c>
+      <c r="L588" s="7">
+        <v>0</v>
+      </c>
+      <c r="M588" s="7">
+        <v>10.7452196198746</v>
+      </c>
+      <c r="N588" s="7">
+        <v>0</v>
+      </c>
+      <c r="O588" s="7">
+        <v>1.4381541720664499</v>
+      </c>
+      <c r="P588" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q588" s="7">
+        <v>0</v>
+      </c>
+      <c r="R588" s="7">
+        <v>2.8691474104960202</v>
+      </c>
+      <c r="S588" s="7">
+        <v>0</v>
+      </c>
+      <c r="T588" t="b">
+        <v>0</v>
+      </c>
+      <c r="U588" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V588" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W588" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="589" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A589" s="10">
+        <v>588</v>
+      </c>
+      <c r="B589" s="7">
+        <v>0</v>
+      </c>
+      <c r="C589" s="7">
+        <v>0</v>
+      </c>
+      <c r="D589" s="7">
+        <v>0</v>
+      </c>
+      <c r="E589" s="7">
+        <v>0</v>
+      </c>
+      <c r="F589" s="7">
+        <v>11.997773773586999</v>
+      </c>
+      <c r="G589" s="7">
+        <v>0</v>
+      </c>
+      <c r="H589" s="7">
+        <v>0</v>
+      </c>
+      <c r="I589" s="7">
+        <v>0</v>
+      </c>
+      <c r="J589" s="7">
+        <v>0</v>
+      </c>
+      <c r="K589" s="7">
+        <v>0</v>
+      </c>
+      <c r="L589" s="7">
+        <v>0</v>
+      </c>
+      <c r="M589" s="7">
+        <v>10.800375333526601</v>
+      </c>
+      <c r="N589" s="7">
+        <v>0</v>
+      </c>
+      <c r="O589" s="7">
+        <v>1.8498715552674201</v>
+      </c>
+      <c r="P589" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q589" s="7">
+        <v>0</v>
+      </c>
+      <c r="R589" s="7">
+        <v>1.6850805861779099</v>
+      </c>
+      <c r="S589" s="7">
+        <v>0</v>
+      </c>
+      <c r="T589" t="b">
+        <v>1</v>
+      </c>
+      <c r="U589" s="2">
+        <v>39</v>
+      </c>
+      <c r="V589" s="2">
+        <v>13</v>
+      </c>
+      <c r="W589" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="590" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A590" s="10">
+        <v>589</v>
+      </c>
+      <c r="B590" s="7">
+        <v>8.0707090092444904</v>
+      </c>
+      <c r="C590" s="7">
+        <v>0</v>
+      </c>
+      <c r="D590" s="7">
+        <v>0</v>
+      </c>
+      <c r="E590" s="7">
+        <v>0</v>
+      </c>
+      <c r="F590" s="7">
+        <v>0</v>
+      </c>
+      <c r="G590" s="7">
+        <v>0</v>
+      </c>
+      <c r="H590" s="7">
+        <v>0</v>
+      </c>
+      <c r="I590" s="7">
+        <v>0</v>
+      </c>
+      <c r="J590" s="7">
+        <v>0</v>
+      </c>
+      <c r="K590" s="7">
+        <v>12.969203334451899</v>
+      </c>
+      <c r="L590" s="7">
+        <v>0</v>
+      </c>
+      <c r="M590" s="7">
+        <v>0</v>
+      </c>
+      <c r="N590" s="7">
+        <v>0</v>
+      </c>
+      <c r="O590" s="7">
+        <v>1.96316580264091</v>
+      </c>
+      <c r="P590" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q590" s="7">
+        <v>0</v>
+      </c>
+      <c r="R590" s="7">
+        <v>3.2606387867278799</v>
+      </c>
+      <c r="S590" s="7">
+        <v>0</v>
+      </c>
+      <c r="T590" t="b">
+        <v>0</v>
+      </c>
+      <c r="U590" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V590" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W590" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="591" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A591" s="10">
+        <v>590</v>
+      </c>
+      <c r="B591" s="7">
+        <v>0</v>
+      </c>
+      <c r="C591" s="7">
+        <v>0</v>
+      </c>
+      <c r="D591" s="7">
+        <v>0</v>
+      </c>
+      <c r="E591" s="7">
+        <v>0</v>
+      </c>
+      <c r="F591" s="7">
+        <v>0</v>
+      </c>
+      <c r="G591" s="7">
+        <v>11.939583221716299</v>
+      </c>
+      <c r="H591" s="7">
+        <v>0</v>
+      </c>
+      <c r="I591" s="7">
+        <v>0</v>
+      </c>
+      <c r="J591" s="7">
+        <v>0</v>
+      </c>
+      <c r="K591" s="7">
+        <v>0</v>
+      </c>
+      <c r="L591" s="7">
+        <v>8.4140112852899502</v>
+      </c>
+      <c r="M591" s="7">
+        <v>0</v>
+      </c>
+      <c r="N591" s="7">
+        <v>0</v>
+      </c>
+      <c r="O591" s="7">
+        <v>3.8530236777347899</v>
+      </c>
+      <c r="P591" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q591" s="7">
+        <v>0</v>
+      </c>
+      <c r="R591" s="7">
+        <v>4.87861334012194</v>
+      </c>
+      <c r="S591" s="7">
+        <v>0</v>
+      </c>
+      <c r="T591" t="b">
+        <v>0</v>
+      </c>
+      <c r="U591" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V591" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W591" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="592" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A592" s="10">
+        <v>591</v>
+      </c>
+      <c r="B592" s="7">
+        <v>0</v>
+      </c>
+      <c r="C592" s="7">
+        <v>0</v>
+      </c>
+      <c r="D592" s="7">
+        <v>7.09680836717635</v>
+      </c>
+      <c r="E592" s="7">
+        <v>7.1420365751530497</v>
+      </c>
+      <c r="F592" s="7">
+        <v>0</v>
+      </c>
+      <c r="G592" s="7">
+        <v>0</v>
+      </c>
+      <c r="H592" s="7">
+        <v>0</v>
+      </c>
+      <c r="I592" s="7">
+        <v>0</v>
+      </c>
+      <c r="J592" s="7">
+        <v>0</v>
+      </c>
+      <c r="K592" s="7">
+        <v>0</v>
+      </c>
+      <c r="L592" s="7">
+        <v>0</v>
+      </c>
+      <c r="M592" s="7">
+        <v>0</v>
+      </c>
+      <c r="N592" s="7">
+        <v>0</v>
+      </c>
+      <c r="O592" s="7">
+        <v>2.5013711689293601</v>
+      </c>
+      <c r="P592" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q592" s="7">
+        <v>0</v>
+      </c>
+      <c r="R592" s="7">
+        <v>4.4323643817091396</v>
+      </c>
+      <c r="S592" s="7">
+        <v>0</v>
+      </c>
+      <c r="T592" t="b">
+        <v>0</v>
+      </c>
+      <c r="U592" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V592" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W592" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="593" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A593" s="10">
+        <v>592</v>
+      </c>
+      <c r="B593" s="7">
+        <v>0</v>
+      </c>
+      <c r="C593" s="7">
+        <v>0</v>
+      </c>
+      <c r="D593" s="7">
+        <v>8.9717977149311299</v>
+      </c>
+      <c r="E593" s="7">
+        <v>0</v>
+      </c>
+      <c r="F593" s="7">
+        <v>11.236944795806499</v>
+      </c>
+      <c r="G593" s="7">
+        <v>0</v>
+      </c>
+      <c r="H593" s="7">
+        <v>0</v>
+      </c>
+      <c r="I593" s="7">
+        <v>0</v>
+      </c>
+      <c r="J593" s="7">
+        <v>0</v>
+      </c>
+      <c r="K593" s="7">
+        <v>0</v>
+      </c>
+      <c r="L593" s="7">
+        <v>0</v>
+      </c>
+      <c r="M593" s="7">
+        <v>0</v>
+      </c>
+      <c r="N593" s="7">
+        <v>0</v>
+      </c>
+      <c r="O593" s="7">
+        <v>3.2605884591870802</v>
+      </c>
+      <c r="P593" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q593" s="7">
+        <v>0</v>
+      </c>
+      <c r="R593" s="7">
+        <v>1.18387478094536</v>
+      </c>
+      <c r="S593" s="7">
+        <v>0</v>
+      </c>
+      <c r="T593" t="b">
+        <v>0</v>
+      </c>
+      <c r="U593" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V593" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W593" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="594" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A594" s="10">
+        <v>593</v>
+      </c>
+      <c r="B594" s="7">
+        <v>8.40453495030917</v>
+      </c>
+      <c r="C594" s="7">
+        <v>12.4135107805053</v>
+      </c>
+      <c r="D594" s="7">
+        <v>0</v>
+      </c>
+      <c r="E594" s="7">
+        <v>0</v>
+      </c>
+      <c r="F594" s="7">
+        <v>0</v>
+      </c>
+      <c r="G594" s="7">
+        <v>0</v>
+      </c>
+      <c r="H594" s="7">
+        <v>0</v>
+      </c>
+      <c r="I594" s="7">
+        <v>0</v>
+      </c>
+      <c r="J594" s="7">
+        <v>0</v>
+      </c>
+      <c r="K594" s="7">
+        <v>0</v>
+      </c>
+      <c r="L594" s="7">
+        <v>0</v>
+      </c>
+      <c r="M594" s="7">
+        <v>0</v>
+      </c>
+      <c r="N594" s="7">
+        <v>0</v>
+      </c>
+      <c r="O594" s="7">
+        <v>2.0716774541516298</v>
+      </c>
+      <c r="P594" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q594" s="7">
+        <v>0</v>
+      </c>
+      <c r="R594" s="7">
+        <v>2.32242102380807</v>
+      </c>
+      <c r="S594" s="7">
+        <v>0</v>
+      </c>
+      <c r="T594" t="b">
+        <v>0</v>
+      </c>
+      <c r="U594" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V594" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W594" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="595" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A595" s="10">
+        <v>594</v>
+      </c>
+      <c r="B595" s="7">
+        <v>9.7186490885808396</v>
+      </c>
+      <c r="C595" s="7">
+        <v>0</v>
+      </c>
+      <c r="D595" s="7">
+        <v>0</v>
+      </c>
+      <c r="E595" s="7">
+        <v>8.0548349482292299</v>
+      </c>
+      <c r="F595" s="7">
+        <v>0</v>
+      </c>
+      <c r="G595" s="7">
+        <v>0</v>
+      </c>
+      <c r="H595" s="7">
+        <v>0</v>
+      </c>
+      <c r="I595" s="7">
+        <v>0</v>
+      </c>
+      <c r="J595" s="7">
+        <v>0</v>
+      </c>
+      <c r="K595" s="7">
+        <v>0</v>
+      </c>
+      <c r="L595" s="7">
+        <v>0</v>
+      </c>
+      <c r="M595" s="7">
+        <v>0</v>
+      </c>
+      <c r="N595" s="7">
+        <v>0</v>
+      </c>
+      <c r="O595" s="7">
+        <v>2.0773479341068</v>
+      </c>
+      <c r="P595" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q595" s="7">
+        <v>0</v>
+      </c>
+      <c r="R595" s="7">
+        <v>1.44216583427794</v>
+      </c>
+      <c r="S595" s="7">
+        <v>0</v>
+      </c>
+      <c r="T595" t="b">
+        <v>0</v>
+      </c>
+      <c r="U595" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V595" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W595" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="596" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A596" s="10">
+        <v>595</v>
+      </c>
+      <c r="B596" s="7">
+        <v>8.9873587845216605</v>
+      </c>
+      <c r="C596" s="7">
+        <v>0</v>
+      </c>
+      <c r="D596" s="7">
+        <v>0</v>
+      </c>
+      <c r="E596" s="7">
+        <v>0</v>
+      </c>
+      <c r="F596" s="7">
+        <v>10.9649802863788</v>
+      </c>
+      <c r="G596" s="7">
+        <v>0</v>
+      </c>
+      <c r="H596" s="7">
+        <v>0</v>
+      </c>
+      <c r="I596" s="7">
+        <v>0</v>
+      </c>
+      <c r="J596" s="7">
+        <v>0</v>
+      </c>
+      <c r="K596" s="7">
+        <v>0</v>
+      </c>
+      <c r="L596" s="7">
+        <v>0</v>
+      </c>
+      <c r="M596" s="7">
+        <v>0</v>
+      </c>
+      <c r="N596" s="7">
+        <v>0</v>
+      </c>
+      <c r="O596" s="7">
+        <v>1.4303789106943601</v>
+      </c>
+      <c r="P596" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q596" s="7">
+        <v>0</v>
+      </c>
+      <c r="R596" s="7">
+        <v>4.1514955191659197</v>
+      </c>
+      <c r="S596" s="7">
+        <v>0</v>
+      </c>
+      <c r="T596" t="b">
+        <v>0</v>
+      </c>
+      <c r="U596" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V596" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W596" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="597" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A597" s="10">
+        <v>596</v>
+      </c>
+      <c r="B597" s="7">
+        <v>0</v>
+      </c>
+      <c r="C597" s="7">
+        <v>0</v>
+      </c>
+      <c r="D597" s="7">
+        <v>11.691180646705</v>
+      </c>
+      <c r="E597" s="7">
+        <v>0</v>
+      </c>
+      <c r="F597" s="7">
+        <v>0</v>
+      </c>
+      <c r="G597" s="7">
+        <v>0</v>
+      </c>
+      <c r="H597" s="7">
+        <v>0</v>
+      </c>
+      <c r="I597" s="7">
+        <v>0</v>
+      </c>
+      <c r="J597" s="7">
+        <v>13.123763330671</v>
+      </c>
+      <c r="K597" s="7">
+        <v>0</v>
+      </c>
+      <c r="L597" s="7">
+        <v>0</v>
+      </c>
+      <c r="M597" s="7">
+        <v>0</v>
+      </c>
+      <c r="N597" s="7">
+        <v>0</v>
+      </c>
+      <c r="O597" s="7">
+        <v>2.2371737528443001</v>
+      </c>
+      <c r="P597" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q597" s="7">
+        <v>0</v>
+      </c>
+      <c r="R597" s="7">
+        <v>1.22185056263693</v>
+      </c>
+      <c r="S597" s="7">
+        <v>0</v>
+      </c>
+      <c r="T597" t="b">
+        <v>0</v>
+      </c>
+      <c r="U597" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V597" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W597" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="598" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A598" s="10">
+        <v>597</v>
+      </c>
+      <c r="B598" s="7">
+        <v>7.9971780009376001</v>
+      </c>
+      <c r="C598" s="7">
+        <v>0</v>
+      </c>
+      <c r="D598" s="7">
+        <v>8.1511440553158305</v>
+      </c>
+      <c r="E598" s="7">
+        <v>0</v>
+      </c>
+      <c r="F598" s="7">
+        <v>0</v>
+      </c>
+      <c r="G598" s="7">
+        <v>0</v>
+      </c>
+      <c r="H598" s="7">
+        <v>0</v>
+      </c>
+      <c r="I598" s="7">
+        <v>0</v>
+      </c>
+      <c r="J598" s="7">
+        <v>0</v>
+      </c>
+      <c r="K598" s="7">
+        <v>0</v>
+      </c>
+      <c r="L598" s="7">
+        <v>0</v>
+      </c>
+      <c r="M598" s="7">
+        <v>0</v>
+      </c>
+      <c r="N598" s="7">
+        <v>0</v>
+      </c>
+      <c r="O598" s="7">
+        <v>3.33467328559294</v>
+      </c>
+      <c r="P598" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q598" s="7">
+        <v>0</v>
+      </c>
+      <c r="R598" s="7">
+        <v>1.8063337752211901</v>
+      </c>
+      <c r="S598" s="7">
+        <v>0</v>
+      </c>
+      <c r="T598" t="b">
+        <v>0</v>
+      </c>
+      <c r="U598" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V598" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W598" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="599" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A599" s="10">
+        <v>598</v>
+      </c>
+      <c r="B599" s="7">
+        <v>0</v>
+      </c>
+      <c r="C599" s="7">
+        <v>9.8752937539976102</v>
+      </c>
+      <c r="D599" s="7">
+        <v>0</v>
+      </c>
+      <c r="E599" s="7">
+        <v>7.4930739319457498</v>
+      </c>
+      <c r="F599" s="7">
+        <v>0</v>
+      </c>
+      <c r="G599" s="7">
+        <v>0</v>
+      </c>
+      <c r="H599" s="7">
+        <v>0</v>
+      </c>
+      <c r="I599" s="7">
+        <v>0</v>
+      </c>
+      <c r="J599" s="7">
+        <v>0</v>
+      </c>
+      <c r="K599" s="7">
+        <v>0</v>
+      </c>
+      <c r="L599" s="7">
+        <v>0</v>
+      </c>
+      <c r="M599" s="7">
+        <v>0</v>
+      </c>
+      <c r="N599" s="7">
+        <v>0</v>
+      </c>
+      <c r="O599" s="7">
+        <v>3.85621833694645</v>
+      </c>
+      <c r="P599" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q599" s="7">
+        <v>0</v>
+      </c>
+      <c r="R599" s="7">
+        <v>4.4964399141229299</v>
+      </c>
+      <c r="S599" s="7">
+        <v>0</v>
+      </c>
+      <c r="T599" t="b">
+        <v>0</v>
+      </c>
+      <c r="U599" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V599" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W599" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="600" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A600" s="10">
+        <v>599</v>
+      </c>
+      <c r="B600" s="7">
+        <v>0</v>
+      </c>
+      <c r="C600" s="7">
+        <v>10.722811478451399</v>
+      </c>
+      <c r="D600" s="7">
+        <v>8.5655765073636498</v>
+      </c>
+      <c r="E600" s="7">
+        <v>0</v>
+      </c>
+      <c r="F600" s="7">
+        <v>0</v>
+      </c>
+      <c r="G600" s="7">
+        <v>0</v>
+      </c>
+      <c r="H600" s="7">
+        <v>0</v>
+      </c>
+      <c r="I600" s="7">
+        <v>0</v>
+      </c>
+      <c r="J600" s="7">
+        <v>0</v>
+      </c>
+      <c r="K600" s="7">
+        <v>0</v>
+      </c>
+      <c r="L600" s="7">
+        <v>0</v>
+      </c>
+      <c r="M600" s="7">
+        <v>0</v>
+      </c>
+      <c r="N600" s="7">
+        <v>0</v>
+      </c>
+      <c r="O600" s="7">
+        <v>3.3625792106076302</v>
+      </c>
+      <c r="P600" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q600" s="7">
+        <v>0</v>
+      </c>
+      <c r="R600" s="7">
+        <v>2.2657207529005299</v>
+      </c>
+      <c r="S600" s="7">
+        <v>0</v>
+      </c>
+      <c r="T600" t="b">
+        <v>0</v>
+      </c>
+      <c r="U600" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V600" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W600" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="601" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A601" s="10">
+        <v>600</v>
+      </c>
+      <c r="B601" s="7">
+        <v>0</v>
+      </c>
+      <c r="C601" s="7">
+        <v>0</v>
+      </c>
+      <c r="D601" s="7">
+        <v>0</v>
+      </c>
+      <c r="E601" s="7">
+        <v>0</v>
+      </c>
+      <c r="F601" s="7">
+        <v>0</v>
+      </c>
+      <c r="G601" s="7">
+        <v>9.3600023415264406</v>
+      </c>
+      <c r="H601" s="7">
+        <v>0</v>
+      </c>
+      <c r="I601" s="7">
+        <v>11.0178551908761</v>
+      </c>
+      <c r="J601" s="7">
+        <v>0</v>
+      </c>
+      <c r="K601" s="7">
+        <v>0</v>
+      </c>
+      <c r="L601" s="7">
+        <v>0</v>
+      </c>
+      <c r="M601" s="7">
+        <v>0</v>
+      </c>
+      <c r="N601" s="7">
+        <v>0</v>
+      </c>
+      <c r="O601" s="7">
+        <v>3.72792991409138</v>
+      </c>
+      <c r="P601" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q601" s="7">
+        <v>0</v>
+      </c>
+      <c r="R601" s="7">
+        <v>5.0899863892098001</v>
+      </c>
+      <c r="S601" s="7">
+        <v>0</v>
+      </c>
+      <c r="T601" t="b">
+        <v>0</v>
+      </c>
+      <c r="U601" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V601" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W601" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="602" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A602" s="10">
+        <v>601</v>
+      </c>
+      <c r="B602" s="7">
+        <v>0</v>
+      </c>
+      <c r="C602" s="7">
+        <v>0</v>
+      </c>
+      <c r="D602" s="7">
+        <v>0</v>
+      </c>
+      <c r="E602" s="7">
+        <v>0</v>
+      </c>
+      <c r="F602" s="7">
+        <v>0</v>
+      </c>
+      <c r="G602" s="7">
+        <v>8.3637424335302502</v>
+      </c>
+      <c r="H602" s="7">
+        <v>0</v>
+      </c>
+      <c r="I602" s="7">
+        <v>0</v>
+      </c>
+      <c r="J602" s="7">
+        <v>0</v>
+      </c>
+      <c r="K602" s="7">
+        <v>0</v>
+      </c>
+      <c r="L602" s="7">
+        <v>9.3047254293120893</v>
+      </c>
+      <c r="M602" s="7">
+        <v>0</v>
+      </c>
+      <c r="N602" s="7">
+        <v>0</v>
+      </c>
+      <c r="O602" s="7">
+        <v>1.8194982057531801</v>
+      </c>
+      <c r="P602" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q602" s="7">
+        <v>0</v>
+      </c>
+      <c r="R602" s="7">
+        <v>1.7500895548525399</v>
+      </c>
+      <c r="S602" s="7">
+        <v>0</v>
+      </c>
+      <c r="T602" t="b">
+        <v>0</v>
+      </c>
+      <c r="U602" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V602" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W602" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="603" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A603" s="10">
+        <v>602</v>
+      </c>
+      <c r="B603" s="7">
+        <v>0</v>
+      </c>
+      <c r="C603" s="7">
+        <v>0</v>
+      </c>
+      <c r="D603" s="7">
+        <v>10.1245443701557</v>
+      </c>
+      <c r="E603" s="7">
+        <v>0</v>
+      </c>
+      <c r="F603" s="7">
+        <v>0</v>
+      </c>
+      <c r="G603" s="7">
+        <v>0</v>
+      </c>
+      <c r="H603" s="7">
+        <v>0</v>
+      </c>
+      <c r="I603" s="7">
+        <v>0</v>
+      </c>
+      <c r="J603" s="7">
+        <v>0</v>
+      </c>
+      <c r="K603" s="7">
+        <v>0</v>
+      </c>
+      <c r="L603" s="7">
+        <v>0</v>
+      </c>
+      <c r="M603" s="7">
+        <v>10.206015470293201</v>
+      </c>
+      <c r="N603" s="7">
+        <v>0</v>
+      </c>
+      <c r="O603" s="7">
+        <v>1.46094781419145</v>
+      </c>
+      <c r="P603" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q603" s="7">
+        <v>0</v>
+      </c>
+      <c r="R603" s="7">
+        <v>4.86312060696432</v>
+      </c>
+      <c r="S603" s="7">
+        <v>0</v>
+      </c>
+      <c r="T603" t="b">
+        <v>1</v>
+      </c>
+      <c r="U603" s="2">
+        <v>1523</v>
+      </c>
+      <c r="V603" s="2">
+        <v>365</v>
+      </c>
+      <c r="W603" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A604" s="10">
+        <v>603</v>
+      </c>
+      <c r="B604" s="7">
+        <v>0</v>
+      </c>
+      <c r="C604" s="7">
+        <v>0</v>
+      </c>
+      <c r="D604" s="7">
+        <v>0</v>
+      </c>
+      <c r="E604" s="7">
+        <v>0</v>
+      </c>
+      <c r="F604" s="7">
+        <v>12.507027176482101</v>
+      </c>
+      <c r="G604" s="7">
+        <v>0</v>
+      </c>
+      <c r="H604" s="7">
+        <v>0</v>
+      </c>
+      <c r="I604" s="7">
+        <v>0</v>
+      </c>
+      <c r="J604" s="7">
+        <v>0</v>
+      </c>
+      <c r="K604" s="7">
+        <v>8.3180000483389307</v>
+      </c>
+      <c r="L604" s="7">
+        <v>0</v>
+      </c>
+      <c r="M604" s="7">
+        <v>0</v>
+      </c>
+      <c r="N604" s="7">
+        <v>0</v>
+      </c>
+      <c r="O604" s="7">
+        <v>3.1430009651227699</v>
+      </c>
+      <c r="P604" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q604" s="7">
+        <v>0</v>
+      </c>
+      <c r="R604" s="7">
+        <v>3.3079039131753598</v>
+      </c>
+      <c r="S604" s="7">
+        <v>0</v>
+      </c>
+      <c r="T604" t="b">
+        <v>0</v>
+      </c>
+      <c r="U604" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V604" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W604" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="605" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A605" s="10">
+        <v>604</v>
+      </c>
+      <c r="B605" s="7">
+        <v>0</v>
+      </c>
+      <c r="C605" s="7">
+        <v>0</v>
+      </c>
+      <c r="D605" s="7">
+        <v>0</v>
+      </c>
+      <c r="E605" s="7">
+        <v>7.0848659881894998</v>
+      </c>
+      <c r="F605" s="7">
+        <v>13.5013665897993</v>
+      </c>
+      <c r="G605" s="7">
+        <v>0</v>
+      </c>
+      <c r="H605" s="7">
+        <v>0</v>
+      </c>
+      <c r="I605" s="7">
+        <v>0</v>
+      </c>
+      <c r="J605" s="7">
+        <v>0</v>
+      </c>
+      <c r="K605" s="7">
+        <v>0</v>
+      </c>
+      <c r="L605" s="7">
+        <v>0</v>
+      </c>
+      <c r="M605" s="7">
+        <v>0</v>
+      </c>
+      <c r="N605" s="7">
+        <v>0</v>
+      </c>
+      <c r="O605" s="7">
+        <v>3.9952433101109399</v>
+      </c>
+      <c r="P605" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q605" s="7">
+        <v>0</v>
+      </c>
+      <c r="R605" s="7">
+        <v>2.8692453464285199</v>
+      </c>
+      <c r="S605" s="7">
+        <v>0</v>
+      </c>
+      <c r="T605" t="b">
+        <v>1</v>
+      </c>
+      <c r="U605" s="2">
+        <v>38</v>
+      </c>
+      <c r="V605" s="2">
+        <v>66</v>
+      </c>
+      <c r="W605" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="606" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A606" s="10">
+        <v>605</v>
+      </c>
+      <c r="B606" s="7">
+        <v>0</v>
+      </c>
+      <c r="C606" s="7">
+        <v>0</v>
+      </c>
+      <c r="D606" s="7">
+        <v>0</v>
+      </c>
+      <c r="E606" s="7">
+        <v>9.1064873674224192</v>
+      </c>
+      <c r="F606" s="7">
+        <v>0</v>
+      </c>
+      <c r="G606" s="7">
+        <v>13.1563840026328</v>
+      </c>
+      <c r="H606" s="7">
+        <v>0</v>
+      </c>
+      <c r="I606" s="7">
+        <v>0</v>
+      </c>
+      <c r="J606" s="7">
+        <v>0</v>
+      </c>
+      <c r="K606" s="7">
+        <v>0</v>
+      </c>
+      <c r="L606" s="7">
+        <v>0</v>
+      </c>
+      <c r="M606" s="7">
+        <v>0</v>
+      </c>
+      <c r="N606" s="7">
+        <v>0</v>
+      </c>
+      <c r="O606" s="7">
+        <v>3.7281398616232599</v>
+      </c>
+      <c r="P606" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q606" s="7">
+        <v>0</v>
+      </c>
+      <c r="R606" s="7">
+        <v>4.4747311775813401</v>
+      </c>
+      <c r="S606" s="7">
+        <v>0</v>
+      </c>
+      <c r="T606" t="b">
+        <v>0</v>
+      </c>
+      <c r="U606" s="2" t="str">
+        <f>IF(T606=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V606" s="2" t="str">
+        <f>IF(T606=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W606" s="12" t="str">
+        <f>IF(T606=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="607" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A607" s="10">
+        <v>606</v>
+      </c>
+      <c r="B607" s="7">
+        <v>0</v>
+      </c>
+      <c r="C607" s="7">
+        <v>0</v>
+      </c>
+      <c r="D607" s="7">
+        <v>0</v>
+      </c>
+      <c r="E607" s="7">
+        <v>0</v>
+      </c>
+      <c r="F607" s="7">
+        <v>0</v>
+      </c>
+      <c r="G607" s="7">
+        <v>0</v>
+      </c>
+      <c r="H607" s="7">
+        <v>0</v>
+      </c>
+      <c r="I607" s="7">
+        <v>10.871145244019299</v>
+      </c>
+      <c r="J607" s="7">
+        <v>0</v>
+      </c>
+      <c r="K607" s="7">
+        <v>8.7521682986455591</v>
+      </c>
+      <c r="L607" s="7">
+        <v>0</v>
+      </c>
+      <c r="M607" s="7">
+        <v>0</v>
+      </c>
+      <c r="N607" s="7">
+        <v>0</v>
+      </c>
+      <c r="O607" s="7">
+        <v>2.1944097816169399</v>
+      </c>
+      <c r="P607" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q607" s="7">
+        <v>0</v>
+      </c>
+      <c r="R607" s="7">
+        <v>1.3372184606729001</v>
+      </c>
+      <c r="S607" s="7">
+        <v>0</v>
+      </c>
+      <c r="T607" t="b">
+        <v>0</v>
+      </c>
+      <c r="U607" s="2" t="str">
+        <f>IF(T607=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V607" s="2" t="str">
+        <f>IF(T607=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W607" s="12" t="str">
+        <f>IF(T607=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="608" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A608" s="10">
+        <v>607</v>
+      </c>
+      <c r="B608" s="7">
+        <v>0</v>
+      </c>
+      <c r="C608" s="7">
+        <v>0</v>
+      </c>
+      <c r="D608" s="7">
+        <v>0</v>
+      </c>
+      <c r="E608" s="7">
+        <v>0</v>
+      </c>
+      <c r="F608" s="7">
+        <v>12.416008049506299</v>
+      </c>
+      <c r="G608" s="7">
+        <v>0</v>
+      </c>
+      <c r="H608" s="7">
+        <v>0</v>
+      </c>
+      <c r="I608" s="7">
+        <v>0</v>
+      </c>
+      <c r="J608" s="7">
+        <v>0</v>
+      </c>
+      <c r="K608" s="7">
+        <v>0</v>
+      </c>
+      <c r="L608" s="7">
+        <v>12.385404865159099</v>
+      </c>
+      <c r="M608" s="7">
+        <v>0</v>
+      </c>
+      <c r="N608" s="7">
+        <v>0</v>
+      </c>
+      <c r="O608" s="7">
+        <v>1.7362371119559401</v>
+      </c>
+      <c r="P608" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q608" s="7">
+        <v>0</v>
+      </c>
+      <c r="R608" s="7">
+        <v>3.88463001310391</v>
+      </c>
+      <c r="S608" s="7">
+        <v>0</v>
+      </c>
+      <c r="T608" t="b">
+        <v>0</v>
+      </c>
+      <c r="U608" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V608" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W608" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="609" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A609" s="10">
+        <v>608</v>
+      </c>
+      <c r="B609" s="7">
+        <v>0</v>
+      </c>
+      <c r="C609" s="7">
+        <v>11.4498465575334</v>
+      </c>
+      <c r="D609" s="7">
+        <v>0</v>
+      </c>
+      <c r="E609" s="7">
+        <v>0</v>
+      </c>
+      <c r="F609" s="7">
+        <v>0</v>
+      </c>
+      <c r="G609" s="7">
+        <v>0</v>
+      </c>
+      <c r="H609" s="7">
+        <v>0</v>
+      </c>
+      <c r="I609" s="7">
+        <v>10.0885935699934</v>
+      </c>
+      <c r="J609" s="7">
+        <v>0</v>
+      </c>
+      <c r="K609" s="7">
+        <v>0</v>
+      </c>
+      <c r="L609" s="7">
+        <v>0</v>
+      </c>
+      <c r="M609" s="7">
+        <v>0</v>
+      </c>
+      <c r="N609" s="7">
+        <v>0</v>
+      </c>
+      <c r="O609" s="7">
+        <v>2.50569746353638</v>
+      </c>
+      <c r="P609" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q609" s="7">
+        <v>0</v>
+      </c>
+      <c r="R609" s="7">
+        <v>1.3062528668312701</v>
+      </c>
+      <c r="S609" s="7">
+        <v>0</v>
+      </c>
+      <c r="T609" t="b">
+        <v>0</v>
+      </c>
+      <c r="U609" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V609" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W609" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="610" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A610" s="10">
+        <v>609</v>
+      </c>
+      <c r="B610" s="7">
+        <v>0</v>
+      </c>
+      <c r="C610" s="7">
+        <v>0</v>
+      </c>
+      <c r="D610" s="7">
+        <v>0</v>
+      </c>
+      <c r="E610" s="7">
+        <v>0</v>
+      </c>
+      <c r="F610" s="7">
+        <v>10.002634094803</v>
+      </c>
+      <c r="G610" s="7">
+        <v>0</v>
+      </c>
+      <c r="H610" s="7">
+        <v>0</v>
+      </c>
+      <c r="I610" s="7">
+        <v>8.1179663911646607</v>
+      </c>
+      <c r="J610" s="7">
+        <v>0</v>
+      </c>
+      <c r="K610" s="7">
+        <v>0</v>
+      </c>
+      <c r="L610" s="7">
+        <v>0</v>
+      </c>
+      <c r="M610" s="7">
+        <v>0</v>
+      </c>
+      <c r="N610" s="7">
+        <v>0</v>
+      </c>
+      <c r="O610" s="7">
+        <v>2.5344181476755701</v>
+      </c>
+      <c r="P610" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q610" s="7">
+        <v>0</v>
+      </c>
+      <c r="R610" s="7">
+        <v>4.63827877219392</v>
+      </c>
+      <c r="S610" s="7">
+        <v>0</v>
+      </c>
+      <c r="T610" t="b">
+        <v>0</v>
+      </c>
+      <c r="U610" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V610" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W610" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="611" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A611" s="10">
+        <v>610</v>
+      </c>
+      <c r="B611" s="7">
+        <v>0</v>
+      </c>
+      <c r="C611" s="7">
+        <v>0</v>
+      </c>
+      <c r="D611" s="7">
+        <v>6.3374786926166804</v>
+      </c>
+      <c r="E611" s="7">
+        <v>0</v>
+      </c>
+      <c r="F611" s="7">
+        <v>0</v>
+      </c>
+      <c r="G611" s="7">
+        <v>0</v>
+      </c>
+      <c r="H611" s="7">
+        <v>0</v>
+      </c>
+      <c r="I611" s="7">
+        <v>13.3528883259184</v>
+      </c>
+      <c r="J611" s="7">
+        <v>0</v>
+      </c>
+      <c r="K611" s="7">
+        <v>0</v>
+      </c>
+      <c r="L611" s="7">
+        <v>0</v>
+      </c>
+      <c r="M611" s="7">
+        <v>0</v>
+      </c>
+      <c r="N611" s="7">
+        <v>0</v>
+      </c>
+      <c r="O611" s="7">
+        <v>2.02179187693421</v>
+      </c>
+      <c r="P611" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q611" s="7">
+        <v>0</v>
+      </c>
+      <c r="R611" s="7">
+        <v>3.6835554002533901</v>
+      </c>
+      <c r="S611" s="7">
+        <v>0</v>
+      </c>
+      <c r="T611" t="b">
+        <v>0</v>
+      </c>
+      <c r="U611" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V611" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W611" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="612" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A612" s="10">
+        <v>611</v>
+      </c>
+      <c r="B612" s="7">
+        <v>0</v>
+      </c>
+      <c r="C612" s="7">
+        <v>0</v>
+      </c>
+      <c r="D612" s="7">
+        <v>0</v>
+      </c>
+      <c r="E612" s="7">
+        <v>8.24978498767274</v>
+      </c>
+      <c r="F612" s="7">
+        <v>0</v>
+      </c>
+      <c r="G612" s="7">
+        <v>0</v>
+      </c>
+      <c r="H612" s="7">
+        <v>0</v>
+      </c>
+      <c r="I612" s="7">
+        <v>0</v>
+      </c>
+      <c r="J612" s="7">
+        <v>0</v>
+      </c>
+      <c r="K612" s="7">
+        <v>10.226545062013701</v>
+      </c>
+      <c r="L612" s="7">
+        <v>0</v>
+      </c>
+      <c r="M612" s="7">
+        <v>0</v>
+      </c>
+      <c r="N612" s="7">
+        <v>0</v>
+      </c>
+      <c r="O612" s="7">
+        <v>3.3714021681204902</v>
+      </c>
+      <c r="P612" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q612" s="7">
+        <v>0</v>
+      </c>
+      <c r="R612" s="7">
+        <v>1.6190701213729199</v>
+      </c>
+      <c r="S612" s="7">
+        <v>0</v>
+      </c>
+      <c r="T612" t="b">
+        <v>0</v>
+      </c>
+      <c r="U612" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V612" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W612" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="613" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A613" s="10">
+        <v>612</v>
+      </c>
+      <c r="B613" s="7">
+        <v>6.1607849714564802</v>
+      </c>
+      <c r="C613" s="7">
+        <v>8.7511034502862692</v>
+      </c>
+      <c r="D613" s="7">
+        <v>0</v>
+      </c>
+      <c r="E613" s="7">
+        <v>0</v>
+      </c>
+      <c r="F613" s="7">
+        <v>0</v>
+      </c>
+      <c r="G613" s="7">
+        <v>0</v>
+      </c>
+      <c r="H613" s="7">
+        <v>0</v>
+      </c>
+      <c r="I613" s="7">
+        <v>0</v>
+      </c>
+      <c r="J613" s="7">
+        <v>0</v>
+      </c>
+      <c r="K613" s="7">
+        <v>0</v>
+      </c>
+      <c r="L613" s="7">
+        <v>0</v>
+      </c>
+      <c r="M613" s="7">
+        <v>0</v>
+      </c>
+      <c r="N613" s="7">
+        <v>0</v>
+      </c>
+      <c r="O613" s="7">
+        <v>2.7404449918463798</v>
+      </c>
+      <c r="P613" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q613" s="7">
+        <v>0</v>
+      </c>
+      <c r="R613" s="7">
+        <v>3.0279754320308898</v>
+      </c>
+      <c r="S613" s="7">
+        <v>0</v>
+      </c>
+      <c r="T613" t="b">
+        <v>0</v>
+      </c>
+      <c r="U613" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V613" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W613" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="614" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A614" s="10">
+        <v>613</v>
+      </c>
+      <c r="B614" s="7">
+        <v>0</v>
+      </c>
+      <c r="C614" s="7">
+        <v>0</v>
+      </c>
+      <c r="D614" s="7">
+        <v>0</v>
+      </c>
+      <c r="E614" s="7">
+        <v>0</v>
+      </c>
+      <c r="F614" s="7">
+        <v>0</v>
+      </c>
+      <c r="G614" s="7">
+        <v>12.297149168609399</v>
+      </c>
+      <c r="H614" s="7">
+        <v>0</v>
+      </c>
+      <c r="I614" s="7">
+        <v>0</v>
+      </c>
+      <c r="J614" s="7">
+        <v>0</v>
+      </c>
+      <c r="K614" s="7">
+        <v>7.8515383276690196</v>
+      </c>
+      <c r="L614" s="7">
+        <v>0</v>
+      </c>
+      <c r="M614" s="7">
+        <v>0</v>
+      </c>
+      <c r="N614" s="7">
+        <v>0</v>
+      </c>
+      <c r="O614" s="7">
+        <v>1.2958945709016501</v>
+      </c>
+      <c r="P614" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q614" s="7">
+        <v>0</v>
+      </c>
+      <c r="R614" s="7">
+        <v>1.9784649937429399</v>
+      </c>
+      <c r="S614" s="7">
+        <v>0</v>
+      </c>
+      <c r="T614" t="b">
+        <v>0</v>
+      </c>
+      <c r="U614" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V614" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W614" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="615" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A615" s="10">
+        <v>614</v>
+      </c>
+      <c r="B615" s="7">
+        <v>0</v>
+      </c>
+      <c r="C615" s="7">
+        <v>0</v>
+      </c>
+      <c r="D615" s="7">
+        <v>0</v>
+      </c>
+      <c r="E615" s="7">
+        <v>0</v>
+      </c>
+      <c r="F615" s="7">
+        <v>11.4112438678363</v>
+      </c>
+      <c r="G615" s="7">
+        <v>0</v>
+      </c>
+      <c r="H615" s="7">
+        <v>0</v>
+      </c>
+      <c r="I615" s="7">
+        <v>10.059301243607599</v>
+      </c>
+      <c r="J615" s="7">
+        <v>0</v>
+      </c>
+      <c r="K615" s="7">
+        <v>0</v>
+      </c>
+      <c r="L615" s="7">
+        <v>0</v>
+      </c>
+      <c r="M615" s="7">
+        <v>0</v>
+      </c>
+      <c r="N615" s="7">
+        <v>0</v>
+      </c>
+      <c r="O615" s="7">
+        <v>2.7690086982429198</v>
+      </c>
+      <c r="P615" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q615" s="7">
+        <v>0</v>
+      </c>
+      <c r="R615" s="7">
+        <v>5.08366774681972</v>
+      </c>
+      <c r="S615" s="7">
+        <v>0</v>
+      </c>
+      <c r="T615" t="b">
+        <v>0</v>
+      </c>
+      <c r="U615" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V615" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W615" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="616" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A616" s="10">
+        <v>615</v>
+      </c>
+      <c r="B616" s="7">
+        <v>0</v>
+      </c>
+      <c r="C616" s="7">
+        <v>0</v>
+      </c>
+      <c r="D616" s="7">
+        <v>0</v>
+      </c>
+      <c r="E616" s="7">
+        <v>0</v>
+      </c>
+      <c r="F616" s="7">
+        <v>0</v>
+      </c>
+      <c r="G616" s="7">
+        <v>0</v>
+      </c>
+      <c r="H616" s="7">
+        <v>0</v>
+      </c>
+      <c r="I616" s="7">
+        <v>0</v>
+      </c>
+      <c r="J616" s="7">
+        <v>0</v>
+      </c>
+      <c r="K616" s="7">
+        <v>8.26938868102439</v>
+      </c>
+      <c r="L616" s="7">
+        <v>0</v>
+      </c>
+      <c r="M616" s="7">
+        <v>7.9694677451000704</v>
+      </c>
+      <c r="N616" s="7">
+        <v>0</v>
+      </c>
+      <c r="O616" s="7">
+        <v>4.1582175511729398</v>
+      </c>
+      <c r="P616" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q616" s="7">
+        <v>0</v>
+      </c>
+      <c r="R616" s="7">
+        <v>3.3716601947047602</v>
+      </c>
+      <c r="S616" s="7">
+        <v>0</v>
+      </c>
+      <c r="T616" t="b">
+        <v>0</v>
+      </c>
+      <c r="U616" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V616" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W616" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="617" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A617" s="10">
+        <v>616</v>
+      </c>
+      <c r="B617" s="7">
+        <v>0</v>
+      </c>
+      <c r="C617" s="7">
+        <v>0</v>
+      </c>
+      <c r="D617" s="7">
+        <v>9.3965906611375392</v>
+      </c>
+      <c r="E617" s="7">
+        <v>0</v>
+      </c>
+      <c r="F617" s="7">
+        <v>0</v>
+      </c>
+      <c r="G617" s="7">
+        <v>0</v>
+      </c>
+      <c r="H617" s="7">
+        <v>11.535241223797801</v>
+      </c>
+      <c r="I617" s="7">
+        <v>0</v>
+      </c>
+      <c r="J617" s="7">
+        <v>0</v>
+      </c>
+      <c r="K617" s="7">
+        <v>0</v>
+      </c>
+      <c r="L617" s="7">
+        <v>0</v>
+      </c>
+      <c r="M617" s="7">
+        <v>0</v>
+      </c>
+      <c r="N617" s="7">
+        <v>0</v>
+      </c>
+      <c r="O617" s="7">
+        <v>2.3711879501473798</v>
+      </c>
+      <c r="P617" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q617" s="7">
+        <v>0</v>
+      </c>
+      <c r="R617" s="7">
+        <v>2.2486043433251601</v>
+      </c>
+      <c r="S617" s="7">
+        <v>0</v>
+      </c>
+      <c r="T617" t="b">
+        <v>0</v>
+      </c>
+      <c r="U617" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V617" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W617" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="618" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A618" s="10">
+        <v>617</v>
+      </c>
+      <c r="B618" s="7">
+        <v>0</v>
+      </c>
+      <c r="C618" s="7">
+        <v>12.0802866735865</v>
+      </c>
+      <c r="D618" s="7">
+        <v>0</v>
+      </c>
+      <c r="E618" s="7">
+        <v>0</v>
+      </c>
+      <c r="F618" s="7">
+        <v>0</v>
+      </c>
+      <c r="G618" s="7">
+        <v>0</v>
+      </c>
+      <c r="H618" s="7">
+        <v>0</v>
+      </c>
+      <c r="I618" s="7">
+        <v>0</v>
+      </c>
+      <c r="J618" s="7">
+        <v>0</v>
+      </c>
+      <c r="K618" s="7">
+        <v>10.0260222461227</v>
+      </c>
+      <c r="L618" s="7">
+        <v>0</v>
+      </c>
+      <c r="M618" s="7">
+        <v>0</v>
+      </c>
+      <c r="N618" s="7">
+        <v>0</v>
+      </c>
+      <c r="O618" s="7">
+        <v>2.67411086567432</v>
+      </c>
+      <c r="P618" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q618" s="7">
+        <v>0</v>
+      </c>
+      <c r="R618" s="7">
+        <v>3.1175563861128501</v>
+      </c>
+      <c r="S618" s="7">
+        <v>0</v>
+      </c>
+      <c r="T618" t="b">
+        <v>0</v>
+      </c>
+      <c r="U618" s="2" t="str">
+        <f t="shared" si="34"/>
+        <v>NA</v>
+      </c>
+      <c r="V618" s="2" t="str">
+        <f t="shared" si="35"/>
+        <v>NA</v>
+      </c>
+      <c r="W618" s="12" t="str">
+        <f t="shared" si="36"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="619" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A619" s="10">
+        <v>618</v>
+      </c>
+      <c r="B619" s="7">
+        <v>0</v>
+      </c>
+      <c r="C619" s="7">
+        <v>0</v>
+      </c>
+      <c r="D619" s="7">
+        <v>0</v>
+      </c>
+      <c r="E619" s="7">
+        <v>0</v>
+      </c>
+      <c r="F619" s="7">
+        <v>0</v>
+      </c>
+      <c r="G619" s="7">
+        <v>0</v>
+      </c>
+      <c r="H619" s="7">
+        <v>9.9375046468569703</v>
+      </c>
+      <c r="I619" s="7">
+        <v>0</v>
+      </c>
+      <c r="J619" s="7">
+        <v>10.570156754639299</v>
+      </c>
+      <c r="K619" s="7">
+        <v>0</v>
+      </c>
+      <c r="L619" s="7">
+        <v>0</v>
+      </c>
+      <c r="M619" s="7">
+        <v>0</v>
+      </c>
+      <c r="N619" s="7">
+        <v>0</v>
+      </c>
+      <c r="O619" s="7">
+        <v>2.3906949842156799</v>
+      </c>
+      <c r="P619" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q619" s="7">
+        <v>0</v>
+      </c>
+      <c r="R619" s="7">
+        <v>1.9125559873725699</v>
+      </c>
+      <c r="S619" s="7">
+        <v>0</v>
+      </c>
+      <c r="T619" t="b">
+        <v>1</v>
+      </c>
+      <c r="U619" s="2">
+        <v>18</v>
+      </c>
+      <c r="V619" s="2">
+        <v>16</v>
+      </c>
+      <c r="W619" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W583">
-    <cfRule type="expression" dxfId="4" priority="5">
+  <conditionalFormatting sqref="A1:W619">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U580">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U569">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53468,7 +56160,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S642
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6B9256-ACB1-9440-82E6-9FC896D9E309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867CF682-8BC8-2A46-9F31-F883BBDA796E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
   <si>
     <t>Sample</t>
   </si>
@@ -222,6 +222,15 @@
   <si>
     <t>Newtonian</t>
   </si>
+  <si>
+    <t xml:space="preserve">HIGH TURBIDITY - REMOVE SAMPLE </t>
+  </si>
+  <si>
+    <t>HIGH TURBIDITY - REMOVE SAMPLE (NOTE: DEHYQUART A-CA + PLANTAPON AMINO KG-L IS FORMING THESE HIGHLY TURBID SYSTEMS</t>
+  </si>
+  <si>
+    <t>HIGH TURBIDITY - REMOVE SAMPLE (NOTE: MORE DIFFICULT TO DETERMINE THE PHASE STABILITY FOR THESE SAMPLES TOO)</t>
+  </si>
 </sst>
 </file>
 
@@ -276,13 +285,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -295,6 +304,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -305,10 +319,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -371,14 +386,32 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -386,16 +419,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -446,16 +469,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -779,16 +792,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:W619"/>
+  <dimension ref="A1:X643"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A582" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W619" sqref="W619"/>
+    <sheetView tabSelected="1" topLeftCell="A606" zoomScale="75" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W643" sqref="W643"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" style="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
@@ -806,7 +819,7 @@
     <col min="17" max="17" width="14" style="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="8.83203125" style="7" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12.83203125" style="12" customWidth="1"/>
@@ -41679,7 +41692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="561" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="561" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A561" s="10">
         <v>560</v>
       </c>
@@ -41753,7 +41766,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="562" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A562" s="10">
         <v>561</v>
       </c>
@@ -41824,7 +41837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="563" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A563" s="10">
         <v>562</v>
       </c>
@@ -41895,7 +41908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="564" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A564" s="10">
         <v>563</v>
       </c>
@@ -41966,7 +41979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="565" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="565" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A565" s="10">
         <v>564</v>
       </c>
@@ -42037,7 +42050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="566" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A566" s="10">
         <v>565</v>
       </c>
@@ -42111,7 +42124,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="567" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="567" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A567" s="10">
         <v>566</v>
       </c>
@@ -42182,7 +42195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="568" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="568" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A568" s="10">
         <v>567</v>
       </c>
@@ -42253,78 +42266,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="569" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="569" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A569" s="10">
         <v>568</v>
       </c>
-      <c r="B569" s="7">
-        <v>0</v>
-      </c>
-      <c r="C569" s="7">
-        <v>0</v>
-      </c>
-      <c r="D569" s="7">
-        <v>0</v>
-      </c>
-      <c r="E569" s="7">
-        <v>0</v>
-      </c>
-      <c r="F569" s="7">
-        <v>0</v>
-      </c>
-      <c r="G569" s="7">
-        <v>0</v>
-      </c>
-      <c r="H569" s="7">
+      <c r="B569" s="25">
+        <v>0</v>
+      </c>
+      <c r="C569" s="25">
+        <v>0</v>
+      </c>
+      <c r="D569" s="25">
+        <v>0</v>
+      </c>
+      <c r="E569" s="25">
+        <v>0</v>
+      </c>
+      <c r="F569" s="25">
+        <v>0</v>
+      </c>
+      <c r="G569" s="25">
+        <v>0</v>
+      </c>
+      <c r="H569" s="25">
         <v>8.1746463355648409</v>
       </c>
-      <c r="I569" s="7">
-        <v>0</v>
-      </c>
-      <c r="J569" s="7">
-        <v>0</v>
-      </c>
-      <c r="K569" s="7">
-        <v>0</v>
-      </c>
-      <c r="L569" s="7">
+      <c r="I569" s="25">
+        <v>0</v>
+      </c>
+      <c r="J569" s="25">
+        <v>0</v>
+      </c>
+      <c r="K569" s="25">
+        <v>0</v>
+      </c>
+      <c r="L569" s="25">
         <v>7.8369415941857703</v>
       </c>
-      <c r="M569" s="7">
-        <v>0</v>
-      </c>
-      <c r="N569" s="7">
-        <v>0</v>
-      </c>
-      <c r="O569" s="7">
-        <v>0</v>
-      </c>
-      <c r="P569" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q569" s="7">
+      <c r="M569" s="25">
+        <v>0</v>
+      </c>
+      <c r="N569" s="25">
+        <v>0</v>
+      </c>
+      <c r="O569" s="25">
+        <v>0</v>
+      </c>
+      <c r="P569" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q569" s="25">
         <v>2.6411200459623099</v>
       </c>
-      <c r="R569" s="7">
+      <c r="R569" s="25">
         <v>4.5923860110838204</v>
       </c>
-      <c r="S569" s="7">
-        <v>0</v>
-      </c>
-      <c r="T569" t="b">
+      <c r="S569" s="25">
+        <v>0</v>
+      </c>
+      <c r="T569" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="U569" s="24">
+      <c r="U569" s="26">
         <v>4265</v>
       </c>
-      <c r="V569" s="2">
+      <c r="V569" s="26">
         <v>16</v>
       </c>
-      <c r="W569" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="570" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W569" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="X569" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="570" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A570" s="10">
         <v>569</v>
       </c>
@@ -42398,7 +42414,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="571" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A571" s="10">
         <v>570</v>
       </c>
@@ -42460,19 +42476,19 @@
         <v>0</v>
       </c>
       <c r="U571" s="2" t="str">
-        <f t="shared" ref="U571:U619" si="34">IF(T571=FALSE, "NA", "")</f>
+        <f t="shared" ref="U571:U617" si="34">IF(T571=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V571" s="2" t="str">
-        <f t="shared" ref="V571:V619" si="35">IF(T571=FALSE, "NA", "")</f>
+        <f t="shared" ref="V571:V618" si="35">IF(T571=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W571" s="12" t="str">
-        <f t="shared" ref="W571:W619" si="36">IF(T571=FALSE, "NA", "")</f>
-        <v>NA</v>
-      </c>
-    </row>
-    <row r="572" spans="1:23" x14ac:dyDescent="0.2">
+        <f t="shared" ref="W571:W618" si="36">IF(T571=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="572" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A572" s="10">
         <v>571</v>
       </c>
@@ -42543,7 +42559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="573" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="573" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A573" s="10">
         <v>572</v>
       </c>
@@ -42617,7 +42633,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="574" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A574" s="10">
         <v>573</v>
       </c>
@@ -42691,7 +42707,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="575" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A575" s="10">
         <v>574</v>
       </c>
@@ -42765,7 +42781,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="576" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A576" s="10">
         <v>575</v>
       </c>
@@ -42836,7 +42852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="577" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="577" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A577" s="10">
         <v>576</v>
       </c>
@@ -42907,7 +42923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="578" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="578" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A578" s="10">
         <v>577</v>
       </c>
@@ -42978,7 +42994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="579" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="579" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A579" s="10">
         <v>578</v>
       </c>
@@ -43049,78 +43065,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="580" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="580" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A580" s="10">
         <v>579</v>
       </c>
-      <c r="B580" s="7">
-        <v>0</v>
-      </c>
-      <c r="C580" s="7">
-        <v>0</v>
-      </c>
-      <c r="D580" s="7">
-        <v>0</v>
-      </c>
-      <c r="E580" s="7">
-        <v>0</v>
-      </c>
-      <c r="F580" s="7">
-        <v>0</v>
-      </c>
-      <c r="G580" s="7">
-        <v>0</v>
-      </c>
-      <c r="H580" s="7">
-        <v>0</v>
-      </c>
-      <c r="I580" s="7">
-        <v>0</v>
-      </c>
-      <c r="J580" s="7">
-        <v>0</v>
-      </c>
-      <c r="K580" s="7">
-        <v>0</v>
-      </c>
-      <c r="L580" s="7">
+      <c r="B580" s="25">
+        <v>0</v>
+      </c>
+      <c r="C580" s="25">
+        <v>0</v>
+      </c>
+      <c r="D580" s="25">
+        <v>0</v>
+      </c>
+      <c r="E580" s="25">
+        <v>0</v>
+      </c>
+      <c r="F580" s="25">
+        <v>0</v>
+      </c>
+      <c r="G580" s="25">
+        <v>0</v>
+      </c>
+      <c r="H580" s="25">
+        <v>0</v>
+      </c>
+      <c r="I580" s="25">
+        <v>0</v>
+      </c>
+      <c r="J580" s="25">
+        <v>0</v>
+      </c>
+      <c r="K580" s="25">
+        <v>0</v>
+      </c>
+      <c r="L580" s="25">
         <v>11.386005225637399</v>
       </c>
-      <c r="M580" s="7">
+      <c r="M580" s="25">
         <v>11.221339894332001</v>
       </c>
-      <c r="N580" s="7">
-        <v>0</v>
-      </c>
-      <c r="O580" s="7">
-        <v>0</v>
-      </c>
-      <c r="P580" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q580" s="7">
+      <c r="N580" s="25">
+        <v>0</v>
+      </c>
+      <c r="O580" s="25">
+        <v>0</v>
+      </c>
+      <c r="P580" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q580" s="25">
         <v>2.5641103037893802</v>
       </c>
-      <c r="R580" s="7">
+      <c r="R580" s="25">
         <v>3.5995439800626001</v>
       </c>
-      <c r="S580" s="7">
-        <v>0</v>
-      </c>
-      <c r="T580" t="b">
+      <c r="S580" s="25">
+        <v>0</v>
+      </c>
+      <c r="T580" s="24" t="b">
         <v>1</v>
       </c>
-      <c r="U580" s="2">
+      <c r="U580" s="26">
         <v>4940</v>
       </c>
-      <c r="V580" s="2">
+      <c r="V580" s="26">
         <v>124</v>
       </c>
-      <c r="W580" s="12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="581" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="W580" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="X580" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="581" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A581" s="10">
         <v>580</v>
       </c>
@@ -43191,7 +43210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="582" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="582" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A582" s="10">
         <v>581</v>
       </c>
@@ -43265,7 +43284,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="583" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="583" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A583" s="10">
         <v>582</v>
       </c>
@@ -43339,7 +43358,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="584" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="584" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A584" s="10">
         <v>583</v>
       </c>
@@ -43413,7 +43432,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="585" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="585" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A585" s="10">
         <v>584</v>
       </c>
@@ -43487,7 +43506,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="586" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="586" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A586" s="10">
         <v>585</v>
       </c>
@@ -43561,7 +43580,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="587" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="587" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A587" s="10">
         <v>586</v>
       </c>
@@ -43635,7 +43654,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="588" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="588" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A588" s="10">
         <v>587</v>
       </c>
@@ -43709,7 +43728,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="589" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="589" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A589" s="10">
         <v>588</v>
       </c>
@@ -43780,7 +43799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="590" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="590" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A590" s="10">
         <v>589</v>
       </c>
@@ -43854,7 +43873,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="591" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="591" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A591" s="10">
         <v>590</v>
       </c>
@@ -43928,7 +43947,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="592" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="592" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A592" s="10">
         <v>591</v>
       </c>
@@ -45180,7 +45199,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="609" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="609" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A609" s="10">
         <v>608</v>
       </c>
@@ -45254,7 +45273,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="610" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="610" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A610" s="10">
         <v>609</v>
       </c>
@@ -45328,7 +45347,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="611" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="611" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A611" s="10">
         <v>610</v>
       </c>
@@ -45402,7 +45421,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="612" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="612" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A612" s="10">
         <v>611</v>
       </c>
@@ -45476,7 +45495,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="613" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A613" s="10">
         <v>612</v>
       </c>
@@ -45550,7 +45569,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="614" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="614" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A614" s="10">
         <v>613</v>
       </c>
@@ -45624,7 +45643,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="615" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="615" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A615" s="10">
         <v>614</v>
       </c>
@@ -45698,7 +45717,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="616" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="616" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A616" s="10">
         <v>615</v>
       </c>
@@ -45772,7 +45791,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="617" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="617" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A617" s="10">
         <v>616</v>
       </c>
@@ -45846,7 +45865,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="618" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="618" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A618" s="10">
         <v>617</v>
       </c>
@@ -45908,7 +45927,7 @@
         <v>0</v>
       </c>
       <c r="U618" s="2" t="str">
-        <f t="shared" si="34"/>
+        <f>IF(T618=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V618" s="2" t="str">
@@ -45920,7 +45939,7 @@
         <v>NA</v>
       </c>
     </row>
-    <row r="619" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="619" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A619" s="10">
         <v>618</v>
       </c>
@@ -45991,22 +46010,1765 @@
         <v>1</v>
       </c>
     </row>
+    <row r="620" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A620" s="10">
+        <v>619</v>
+      </c>
+      <c r="B620" s="25">
+        <v>0</v>
+      </c>
+      <c r="C620" s="25">
+        <v>0</v>
+      </c>
+      <c r="D620" s="25">
+        <v>0</v>
+      </c>
+      <c r="E620" s="25">
+        <v>0</v>
+      </c>
+      <c r="F620" s="25">
+        <v>0</v>
+      </c>
+      <c r="G620" s="25">
+        <v>0</v>
+      </c>
+      <c r="H620" s="25">
+        <v>0</v>
+      </c>
+      <c r="I620" s="25">
+        <v>0</v>
+      </c>
+      <c r="J620" s="25">
+        <v>0</v>
+      </c>
+      <c r="K620" s="25">
+        <v>0</v>
+      </c>
+      <c r="L620" s="25">
+        <v>12.818365943629599</v>
+      </c>
+      <c r="M620" s="25">
+        <v>13.1382503000175</v>
+      </c>
+      <c r="N620" s="25">
+        <v>0</v>
+      </c>
+      <c r="O620" s="25">
+        <v>0</v>
+      </c>
+      <c r="P620" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q620" s="25">
+        <v>0.87343423873077397</v>
+      </c>
+      <c r="R620" s="25">
+        <v>1.07461150974047</v>
+      </c>
+      <c r="S620" s="25">
+        <v>0</v>
+      </c>
+      <c r="T620" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="U620" s="26">
+        <v>5309</v>
+      </c>
+      <c r="V620" s="26"/>
+      <c r="W620" s="27"/>
+      <c r="X620" s="24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="621" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A621" s="10">
+        <v>620</v>
+      </c>
+      <c r="B621" s="7">
+        <v>0</v>
+      </c>
+      <c r="C621" s="7">
+        <v>7.3718273327324697</v>
+      </c>
+      <c r="D621" s="7">
+        <v>0</v>
+      </c>
+      <c r="E621" s="7">
+        <v>0</v>
+      </c>
+      <c r="F621" s="7">
+        <v>0</v>
+      </c>
+      <c r="G621" s="7">
+        <v>0</v>
+      </c>
+      <c r="H621" s="7">
+        <v>0</v>
+      </c>
+      <c r="I621" s="7">
+        <v>0</v>
+      </c>
+      <c r="J621" s="7">
+        <v>0</v>
+      </c>
+      <c r="K621" s="7">
+        <v>0</v>
+      </c>
+      <c r="L621" s="7">
+        <v>0</v>
+      </c>
+      <c r="M621" s="7">
+        <v>11.850632262481399</v>
+      </c>
+      <c r="N621" s="7">
+        <v>0</v>
+      </c>
+      <c r="O621" s="7">
+        <v>0</v>
+      </c>
+      <c r="P621" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q621" s="7">
+        <v>2.3693722756446798</v>
+      </c>
+      <c r="R621" s="7">
+        <v>4.3842814310070599</v>
+      </c>
+      <c r="S621" s="7">
+        <v>0</v>
+      </c>
+      <c r="T621" t="b">
+        <v>0</v>
+      </c>
+      <c r="U621" s="2" t="str">
+        <f>IF(T621=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V621" s="2" t="str">
+        <f>IF(T621=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W621" s="12" t="str">
+        <f>IF(T621=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="622" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A622" s="10">
+        <v>621</v>
+      </c>
+      <c r="B622" s="7">
+        <v>0</v>
+      </c>
+      <c r="C622" s="7">
+        <v>0</v>
+      </c>
+      <c r="D622" s="7">
+        <v>0</v>
+      </c>
+      <c r="E622" s="7">
+        <v>0</v>
+      </c>
+      <c r="F622" s="7">
+        <v>0</v>
+      </c>
+      <c r="G622" s="7">
+        <v>0</v>
+      </c>
+      <c r="H622" s="7">
+        <v>0</v>
+      </c>
+      <c r="I622" s="7">
+        <v>0</v>
+      </c>
+      <c r="J622" s="7">
+        <v>0</v>
+      </c>
+      <c r="K622" s="7">
+        <v>8.1287306935555304</v>
+      </c>
+      <c r="L622" s="7">
+        <v>0</v>
+      </c>
+      <c r="M622" s="7">
+        <v>11.612189671071601</v>
+      </c>
+      <c r="N622" s="7">
+        <v>0</v>
+      </c>
+      <c r="O622" s="7">
+        <v>0</v>
+      </c>
+      <c r="P622" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q622" s="7">
+        <v>3.3919192174533901</v>
+      </c>
+      <c r="R622" s="7">
+        <v>1.9149128186061299</v>
+      </c>
+      <c r="S622" s="7">
+        <v>0</v>
+      </c>
+      <c r="T622" t="b">
+        <v>0</v>
+      </c>
+      <c r="U622" s="2" t="str">
+        <f t="shared" ref="U622:U643" si="37">IF(T622=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V622" s="2" t="str">
+        <f t="shared" ref="V622:V643" si="38">IF(T622=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W622" s="12" t="str">
+        <f t="shared" ref="W622:W643" si="39">IF(T622=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="623" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A623" s="10">
+        <v>622</v>
+      </c>
+      <c r="B623" s="7">
+        <v>0</v>
+      </c>
+      <c r="C623" s="7">
+        <v>8.5897315185972101</v>
+      </c>
+      <c r="D623" s="7">
+        <v>0</v>
+      </c>
+      <c r="E623" s="7">
+        <v>0</v>
+      </c>
+      <c r="F623" s="7">
+        <v>0</v>
+      </c>
+      <c r="G623" s="7">
+        <v>0</v>
+      </c>
+      <c r="H623" s="7">
+        <v>0</v>
+      </c>
+      <c r="I623" s="7">
+        <v>0</v>
+      </c>
+      <c r="J623" s="7">
+        <v>0</v>
+      </c>
+      <c r="K623" s="7">
+        <v>0</v>
+      </c>
+      <c r="L623" s="7">
+        <v>0</v>
+      </c>
+      <c r="M623" s="7">
+        <v>12.618134681565699</v>
+      </c>
+      <c r="N623" s="7">
+        <v>0</v>
+      </c>
+      <c r="O623" s="7">
+        <v>0</v>
+      </c>
+      <c r="P623" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q623" s="7">
+        <v>2.5404897906564701</v>
+      </c>
+      <c r="R623" s="7">
+        <v>4.4738184992693499</v>
+      </c>
+      <c r="S623" s="7">
+        <v>0</v>
+      </c>
+      <c r="T623" t="b">
+        <v>0</v>
+      </c>
+      <c r="U623" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V623" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W623" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="624" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A624" s="10">
+        <v>623</v>
+      </c>
+      <c r="B624" s="25">
+        <v>0</v>
+      </c>
+      <c r="C624" s="25">
+        <v>0</v>
+      </c>
+      <c r="D624" s="25">
+        <v>0</v>
+      </c>
+      <c r="E624" s="25">
+        <v>0</v>
+      </c>
+      <c r="F624" s="25">
+        <v>0</v>
+      </c>
+      <c r="G624" s="25">
+        <v>0</v>
+      </c>
+      <c r="H624" s="25">
+        <v>0</v>
+      </c>
+      <c r="I624" s="25">
+        <v>0</v>
+      </c>
+      <c r="J624" s="25">
+        <v>0</v>
+      </c>
+      <c r="K624" s="25">
+        <v>0</v>
+      </c>
+      <c r="L624" s="25">
+        <v>10.0720407836437</v>
+      </c>
+      <c r="M624" s="25">
+        <v>9.9212410733102399</v>
+      </c>
+      <c r="N624" s="25">
+        <v>0</v>
+      </c>
+      <c r="O624" s="25">
+        <v>0</v>
+      </c>
+      <c r="P624" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q624" s="25">
+        <v>3.0665071815354898</v>
+      </c>
+      <c r="R624" s="25">
+        <v>2.2521394647837898</v>
+      </c>
+      <c r="S624" s="25">
+        <v>0</v>
+      </c>
+      <c r="T624" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="U624" s="26">
+        <v>5164</v>
+      </c>
+      <c r="V624" s="26" t="str">
+        <f t="shared" si="38"/>
+        <v/>
+      </c>
+      <c r="W624" s="27" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="X624" s="24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="625" spans="1:24" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A625" s="10">
+        <v>624</v>
+      </c>
+      <c r="B625" s="25">
+        <v>0</v>
+      </c>
+      <c r="C625" s="25">
+        <v>0</v>
+      </c>
+      <c r="D625" s="25">
+        <v>0</v>
+      </c>
+      <c r="E625" s="25">
+        <v>0</v>
+      </c>
+      <c r="F625" s="25">
+        <v>0</v>
+      </c>
+      <c r="G625" s="25">
+        <v>0</v>
+      </c>
+      <c r="H625" s="25">
+        <v>0</v>
+      </c>
+      <c r="I625" s="25">
+        <v>0</v>
+      </c>
+      <c r="J625" s="25">
+        <v>0</v>
+      </c>
+      <c r="K625" s="25">
+        <v>0</v>
+      </c>
+      <c r="L625" s="25">
+        <v>12.350524283540601</v>
+      </c>
+      <c r="M625" s="25">
+        <v>12.177197413761199</v>
+      </c>
+      <c r="N625" s="25">
+        <v>0</v>
+      </c>
+      <c r="O625" s="25">
+        <v>0</v>
+      </c>
+      <c r="P625" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q625" s="25">
+        <v>1.70249333029035</v>
+      </c>
+      <c r="R625" s="25">
+        <v>1.45259734616238</v>
+      </c>
+      <c r="S625" s="25">
+        <v>0</v>
+      </c>
+      <c r="T625" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="U625" s="26">
+        <v>5182</v>
+      </c>
+      <c r="V625" s="26" t="str">
+        <f t="shared" si="38"/>
+        <v/>
+      </c>
+      <c r="W625" s="27" t="str">
+        <f t="shared" si="39"/>
+        <v/>
+      </c>
+      <c r="X625" s="24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="626" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A626" s="10">
+        <v>625</v>
+      </c>
+      <c r="B626" s="7">
+        <v>0</v>
+      </c>
+      <c r="C626" s="7">
+        <v>0</v>
+      </c>
+      <c r="D626" s="7">
+        <v>0</v>
+      </c>
+      <c r="E626" s="7">
+        <v>0</v>
+      </c>
+      <c r="F626" s="7">
+        <v>0</v>
+      </c>
+      <c r="G626" s="7">
+        <v>0</v>
+      </c>
+      <c r="H626" s="7">
+        <v>8.3896868459786909</v>
+      </c>
+      <c r="I626" s="7">
+        <v>0</v>
+      </c>
+      <c r="J626" s="7">
+        <v>8.0140292260094199</v>
+      </c>
+      <c r="K626" s="7">
+        <v>0</v>
+      </c>
+      <c r="L626" s="7">
+        <v>0</v>
+      </c>
+      <c r="M626" s="7">
+        <v>0</v>
+      </c>
+      <c r="N626" s="7">
+        <v>0</v>
+      </c>
+      <c r="O626" s="7">
+        <v>0</v>
+      </c>
+      <c r="P626" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q626" s="7">
+        <v>0.83020334013185904</v>
+      </c>
+      <c r="R626" s="7">
+        <v>2.6095682667192599</v>
+      </c>
+      <c r="S626" s="7">
+        <v>0</v>
+      </c>
+      <c r="T626" t="b">
+        <v>1</v>
+      </c>
+      <c r="U626" s="2">
+        <v>22</v>
+      </c>
+      <c r="V626" s="2">
+        <v>260</v>
+      </c>
+      <c r="W626" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="627" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A627" s="10">
+        <v>626</v>
+      </c>
+      <c r="B627" s="7">
+        <v>0</v>
+      </c>
+      <c r="C627" s="7">
+        <v>12.0972374648561</v>
+      </c>
+      <c r="D627" s="7">
+        <v>0</v>
+      </c>
+      <c r="E627" s="7">
+        <v>0</v>
+      </c>
+      <c r="F627" s="7">
+        <v>11.7464508933011</v>
+      </c>
+      <c r="G627" s="7">
+        <v>0</v>
+      </c>
+      <c r="H627" s="7">
+        <v>0</v>
+      </c>
+      <c r="I627" s="7">
+        <v>0</v>
+      </c>
+      <c r="J627" s="7">
+        <v>0</v>
+      </c>
+      <c r="K627" s="7">
+        <v>0</v>
+      </c>
+      <c r="L627" s="7">
+        <v>0</v>
+      </c>
+      <c r="M627" s="7">
+        <v>0</v>
+      </c>
+      <c r="N627" s="7">
+        <v>0</v>
+      </c>
+      <c r="O627" s="7">
+        <v>0</v>
+      </c>
+      <c r="P627" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q627" s="7">
+        <v>1.03864180404558</v>
+      </c>
+      <c r="R627" s="7">
+        <v>2.90035824525958</v>
+      </c>
+      <c r="S627" s="7">
+        <v>0</v>
+      </c>
+      <c r="T627" t="b">
+        <v>1</v>
+      </c>
+      <c r="U627" s="2">
+        <v>17</v>
+      </c>
+      <c r="V627" s="2">
+        <v>3</v>
+      </c>
+      <c r="W627" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="628" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A628" s="10">
+        <v>627</v>
+      </c>
+      <c r="B628" s="7">
+        <v>0</v>
+      </c>
+      <c r="C628" s="7">
+        <v>0</v>
+      </c>
+      <c r="D628" s="7">
+        <v>0</v>
+      </c>
+      <c r="E628" s="7">
+        <v>8.5323482370374109</v>
+      </c>
+      <c r="F628" s="7">
+        <v>0</v>
+      </c>
+      <c r="G628" s="7">
+        <v>0</v>
+      </c>
+      <c r="H628" s="7">
+        <v>0</v>
+      </c>
+      <c r="I628" s="7">
+        <v>10.0871271444342</v>
+      </c>
+      <c r="J628" s="7">
+        <v>0</v>
+      </c>
+      <c r="K628" s="7">
+        <v>0</v>
+      </c>
+      <c r="L628" s="7">
+        <v>0</v>
+      </c>
+      <c r="M628" s="7">
+        <v>0</v>
+      </c>
+      <c r="N628" s="7">
+        <v>0</v>
+      </c>
+      <c r="O628" s="7">
+        <v>0</v>
+      </c>
+      <c r="P628" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q628" s="7">
+        <v>2.7354487360223301</v>
+      </c>
+      <c r="R628" s="7">
+        <v>4.8925893201821902</v>
+      </c>
+      <c r="S628" s="7">
+        <v>0</v>
+      </c>
+      <c r="T628" t="b">
+        <v>0</v>
+      </c>
+      <c r="U628" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V628" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W628" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="629" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A629" s="10">
+        <v>628</v>
+      </c>
+      <c r="B629" s="7">
+        <v>0</v>
+      </c>
+      <c r="C629" s="7">
+        <v>0</v>
+      </c>
+      <c r="D629" s="7">
+        <v>10.538243487867</v>
+      </c>
+      <c r="E629" s="7">
+        <v>0</v>
+      </c>
+      <c r="F629" s="7">
+        <v>0</v>
+      </c>
+      <c r="G629" s="7">
+        <v>0</v>
+      </c>
+      <c r="H629" s="7">
+        <v>0</v>
+      </c>
+      <c r="I629" s="7">
+        <v>0</v>
+      </c>
+      <c r="J629" s="7">
+        <v>0</v>
+      </c>
+      <c r="K629" s="7">
+        <v>0</v>
+      </c>
+      <c r="L629" s="7">
+        <v>8.6840424057401595</v>
+      </c>
+      <c r="M629" s="7">
+        <v>0</v>
+      </c>
+      <c r="N629" s="7">
+        <v>0</v>
+      </c>
+      <c r="O629" s="7">
+        <v>0</v>
+      </c>
+      <c r="P629" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q629" s="7">
+        <v>2.1659938236154801</v>
+      </c>
+      <c r="R629" s="7">
+        <v>3.52177802936429</v>
+      </c>
+      <c r="S629" s="7">
+        <v>0</v>
+      </c>
+      <c r="T629" t="b">
+        <v>0</v>
+      </c>
+      <c r="U629" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V629" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W629" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="630" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A630" s="10">
+        <v>629</v>
+      </c>
+      <c r="B630" s="7">
+        <v>0</v>
+      </c>
+      <c r="C630" s="7">
+        <v>0</v>
+      </c>
+      <c r="D630" s="7">
+        <v>0</v>
+      </c>
+      <c r="E630" s="7">
+        <v>0</v>
+      </c>
+      <c r="F630" s="7">
+        <v>0</v>
+      </c>
+      <c r="G630" s="7">
+        <v>12.237726178246101</v>
+      </c>
+      <c r="H630" s="7">
+        <v>0</v>
+      </c>
+      <c r="I630" s="7">
+        <v>9.4375684933931705</v>
+      </c>
+      <c r="J630" s="7">
+        <v>0</v>
+      </c>
+      <c r="K630" s="7">
+        <v>0</v>
+      </c>
+      <c r="L630" s="7">
+        <v>0</v>
+      </c>
+      <c r="M630" s="7">
+        <v>0</v>
+      </c>
+      <c r="N630" s="7">
+        <v>0</v>
+      </c>
+      <c r="O630" s="7">
+        <v>0</v>
+      </c>
+      <c r="P630" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q630" s="7">
+        <v>2.5815200166179002</v>
+      </c>
+      <c r="R630" s="7">
+        <v>5.1555609795902502</v>
+      </c>
+      <c r="S630" s="7">
+        <v>0</v>
+      </c>
+      <c r="T630" t="b">
+        <v>0</v>
+      </c>
+      <c r="U630" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V630" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W630" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="631" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A631" s="10">
+        <v>630</v>
+      </c>
+      <c r="B631" s="7">
+        <v>0</v>
+      </c>
+      <c r="C631" s="7">
+        <v>10.136977359982501</v>
+      </c>
+      <c r="D631" s="7">
+        <v>0</v>
+      </c>
+      <c r="E631" s="7">
+        <v>10.024052230456199</v>
+      </c>
+      <c r="F631" s="7">
+        <v>0</v>
+      </c>
+      <c r="G631" s="7">
+        <v>0</v>
+      </c>
+      <c r="H631" s="7">
+        <v>0</v>
+      </c>
+      <c r="I631" s="7">
+        <v>0</v>
+      </c>
+      <c r="J631" s="7">
+        <v>0</v>
+      </c>
+      <c r="K631" s="7">
+        <v>0</v>
+      </c>
+      <c r="L631" s="7">
+        <v>0</v>
+      </c>
+      <c r="M631" s="7">
+        <v>0</v>
+      </c>
+      <c r="N631" s="7">
+        <v>0</v>
+      </c>
+      <c r="O631" s="7">
+        <v>0</v>
+      </c>
+      <c r="P631" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q631" s="7">
+        <v>2.2816230373052</v>
+      </c>
+      <c r="R631" s="7">
+        <v>1.2022632324574201</v>
+      </c>
+      <c r="S631" s="7">
+        <v>0</v>
+      </c>
+      <c r="T631" t="b">
+        <v>1</v>
+      </c>
+      <c r="U631" s="2">
+        <v>27</v>
+      </c>
+      <c r="V631" s="2">
+        <v>3</v>
+      </c>
+      <c r="W631" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="632" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A632" s="10">
+        <v>631</v>
+      </c>
+      <c r="B632" s="7">
+        <v>4.72916670328088</v>
+      </c>
+      <c r="C632" s="7">
+        <v>0</v>
+      </c>
+      <c r="D632" s="7">
+        <v>0</v>
+      </c>
+      <c r="E632" s="7">
+        <v>0</v>
+      </c>
+      <c r="F632" s="7">
+        <v>0</v>
+      </c>
+      <c r="G632" s="7">
+        <v>0</v>
+      </c>
+      <c r="H632" s="7">
+        <v>0</v>
+      </c>
+      <c r="I632" s="7">
+        <v>0</v>
+      </c>
+      <c r="J632" s="7">
+        <v>0</v>
+      </c>
+      <c r="K632" s="7">
+        <v>0</v>
+      </c>
+      <c r="L632" s="7">
+        <v>13.595962352040001</v>
+      </c>
+      <c r="M632" s="7">
+        <v>0</v>
+      </c>
+      <c r="N632" s="7">
+        <v>0</v>
+      </c>
+      <c r="O632" s="7">
+        <v>0</v>
+      </c>
+      <c r="P632" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q632" s="7">
+        <v>1.0124597223873799</v>
+      </c>
+      <c r="R632" s="7">
+        <v>1.8916666813123999</v>
+      </c>
+      <c r="S632" s="7">
+        <v>0</v>
+      </c>
+      <c r="T632" t="b">
+        <v>0</v>
+      </c>
+      <c r="U632" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V632" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W632" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="633" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A633" s="10">
+        <v>632</v>
+      </c>
+      <c r="B633" s="7">
+        <v>0</v>
+      </c>
+      <c r="C633" s="7">
+        <v>8.4154009347002301</v>
+      </c>
+      <c r="D633" s="7">
+        <v>0</v>
+      </c>
+      <c r="E633" s="7">
+        <v>0</v>
+      </c>
+      <c r="F633" s="7">
+        <v>0</v>
+      </c>
+      <c r="G633" s="7">
+        <v>0</v>
+      </c>
+      <c r="H633" s="7">
+        <v>0</v>
+      </c>
+      <c r="I633" s="7">
+        <v>0</v>
+      </c>
+      <c r="J633" s="7">
+        <v>0</v>
+      </c>
+      <c r="K633" s="7">
+        <v>0</v>
+      </c>
+      <c r="L633" s="7">
+        <v>12.1453474367613</v>
+      </c>
+      <c r="M633" s="7">
+        <v>0</v>
+      </c>
+      <c r="N633" s="7">
+        <v>0</v>
+      </c>
+      <c r="O633" s="7">
+        <v>0</v>
+      </c>
+      <c r="P633" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q633" s="7">
+        <v>2.6041304221981001</v>
+      </c>
+      <c r="R633" s="7">
+        <v>3.42101544056827</v>
+      </c>
+      <c r="S633" s="7">
+        <v>0</v>
+      </c>
+      <c r="T633" t="b">
+        <v>1</v>
+      </c>
+      <c r="U633" s="2">
+        <v>19</v>
+      </c>
+      <c r="V633" s="2">
+        <v>6</v>
+      </c>
+      <c r="W633" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="634" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A634" s="10">
+        <v>633</v>
+      </c>
+      <c r="B634" s="7">
+        <v>0</v>
+      </c>
+      <c r="C634" s="7">
+        <v>0</v>
+      </c>
+      <c r="D634" s="7">
+        <v>0</v>
+      </c>
+      <c r="E634" s="7">
+        <v>0</v>
+      </c>
+      <c r="F634" s="7">
+        <v>0</v>
+      </c>
+      <c r="G634" s="7">
+        <v>0</v>
+      </c>
+      <c r="H634" s="7">
+        <v>0</v>
+      </c>
+      <c r="I634" s="7">
+        <v>6.5489824272141002</v>
+      </c>
+      <c r="J634" s="7">
+        <v>10.5812154613023</v>
+      </c>
+      <c r="K634" s="7">
+        <v>0</v>
+      </c>
+      <c r="L634" s="7">
+        <v>0</v>
+      </c>
+      <c r="M634" s="7">
+        <v>0</v>
+      </c>
+      <c r="N634" s="7">
+        <v>0</v>
+      </c>
+      <c r="O634" s="7">
+        <v>0</v>
+      </c>
+      <c r="P634" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q634" s="7">
+        <v>2.9446772937361998</v>
+      </c>
+      <c r="R634" s="7">
+        <v>2.8629156431198699</v>
+      </c>
+      <c r="S634" s="7">
+        <v>0</v>
+      </c>
+      <c r="T634" t="b">
+        <v>0</v>
+      </c>
+      <c r="U634" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V634" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W634" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="635" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A635" s="10">
+        <v>634</v>
+      </c>
+      <c r="B635" s="7">
+        <v>7.98834768079006</v>
+      </c>
+      <c r="C635" s="7">
+        <v>0</v>
+      </c>
+      <c r="D635" s="7">
+        <v>11.069553223124</v>
+      </c>
+      <c r="E635" s="7">
+        <v>0</v>
+      </c>
+      <c r="F635" s="7">
+        <v>0</v>
+      </c>
+      <c r="G635" s="7">
+        <v>0</v>
+      </c>
+      <c r="H635" s="7">
+        <v>0</v>
+      </c>
+      <c r="I635" s="7">
+        <v>0</v>
+      </c>
+      <c r="J635" s="7">
+        <v>0</v>
+      </c>
+      <c r="K635" s="7">
+        <v>0</v>
+      </c>
+      <c r="L635" s="7">
+        <v>0</v>
+      </c>
+      <c r="M635" s="7">
+        <v>0</v>
+      </c>
+      <c r="N635" s="7">
+        <v>0</v>
+      </c>
+      <c r="O635" s="7">
+        <v>0</v>
+      </c>
+      <c r="P635" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q635" s="7">
+        <v>2.9670220414543498</v>
+      </c>
+      <c r="R635" s="7">
+        <v>3.0582189294654198</v>
+      </c>
+      <c r="S635" s="7">
+        <v>0</v>
+      </c>
+      <c r="T635" t="b">
+        <v>1</v>
+      </c>
+      <c r="U635" s="2">
+        <v>19</v>
+      </c>
+      <c r="V635" s="2">
+        <v>3</v>
+      </c>
+      <c r="W635" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="636" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A636" s="10">
+        <v>635</v>
+      </c>
+      <c r="B636" s="7">
+        <v>0</v>
+      </c>
+      <c r="C636" s="7">
+        <v>0</v>
+      </c>
+      <c r="D636" s="7">
+        <v>0</v>
+      </c>
+      <c r="E636" s="7">
+        <v>0</v>
+      </c>
+      <c r="F636" s="7">
+        <v>0</v>
+      </c>
+      <c r="G636" s="7">
+        <v>8.9115614059713799</v>
+      </c>
+      <c r="H636" s="7">
+        <v>8.0449000086139897</v>
+      </c>
+      <c r="I636" s="7">
+        <v>0</v>
+      </c>
+      <c r="J636" s="7">
+        <v>0</v>
+      </c>
+      <c r="K636" s="7">
+        <v>0</v>
+      </c>
+      <c r="L636" s="7">
+        <v>0</v>
+      </c>
+      <c r="M636" s="7">
+        <v>0</v>
+      </c>
+      <c r="N636" s="7">
+        <v>0</v>
+      </c>
+      <c r="O636" s="7">
+        <v>0</v>
+      </c>
+      <c r="P636" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q636" s="7">
+        <v>2.9942118367839199</v>
+      </c>
+      <c r="R636" s="7">
+        <v>1.72151809917759</v>
+      </c>
+      <c r="S636" s="7">
+        <v>0</v>
+      </c>
+      <c r="T636" t="b">
+        <v>1</v>
+      </c>
+      <c r="U636" s="2">
+        <v>35</v>
+      </c>
+      <c r="V636" s="2">
+        <v>672</v>
+      </c>
+      <c r="W636" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="637" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A637" s="10">
+        <v>636</v>
+      </c>
+      <c r="B637" s="7">
+        <v>13.559374944065899</v>
+      </c>
+      <c r="C637" s="7">
+        <v>0</v>
+      </c>
+      <c r="D637" s="7">
+        <v>0</v>
+      </c>
+      <c r="E637" s="7">
+        <v>0</v>
+      </c>
+      <c r="F637" s="7">
+        <v>0</v>
+      </c>
+      <c r="G637" s="7">
+        <v>0</v>
+      </c>
+      <c r="H637" s="7">
+        <v>0</v>
+      </c>
+      <c r="I637" s="7">
+        <v>13.209936046056599</v>
+      </c>
+      <c r="J637" s="7">
+        <v>0</v>
+      </c>
+      <c r="K637" s="7">
+        <v>0</v>
+      </c>
+      <c r="L637" s="7">
+        <v>0</v>
+      </c>
+      <c r="M637" s="7">
+        <v>0</v>
+      </c>
+      <c r="N637" s="7">
+        <v>0</v>
+      </c>
+      <c r="O637" s="7">
+        <v>0</v>
+      </c>
+      <c r="P637" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q637" s="7">
+        <v>2.8141288302798801</v>
+      </c>
+      <c r="R637" s="7">
+        <v>3.73785050739456</v>
+      </c>
+      <c r="S637" s="7">
+        <v>0</v>
+      </c>
+      <c r="T637" t="b">
+        <v>1</v>
+      </c>
+      <c r="U637" s="2">
+        <v>2531</v>
+      </c>
+      <c r="V637" s="2">
+        <v>540</v>
+      </c>
+      <c r="W637" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="638" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A638" s="10">
+        <v>637</v>
+      </c>
+      <c r="B638" s="7">
+        <v>0</v>
+      </c>
+      <c r="C638" s="7">
+        <v>0</v>
+      </c>
+      <c r="D638" s="7">
+        <v>0</v>
+      </c>
+      <c r="E638" s="7">
+        <v>0</v>
+      </c>
+      <c r="F638" s="7">
+        <v>10.687707423664101</v>
+      </c>
+      <c r="G638" s="7">
+        <v>0</v>
+      </c>
+      <c r="H638" s="7">
+        <v>0</v>
+      </c>
+      <c r="I638" s="7">
+        <v>0</v>
+      </c>
+      <c r="J638" s="7">
+        <v>0</v>
+      </c>
+      <c r="K638" s="7">
+        <v>0</v>
+      </c>
+      <c r="L638" s="7">
+        <v>9.5425244740014605</v>
+      </c>
+      <c r="M638" s="7">
+        <v>0</v>
+      </c>
+      <c r="N638" s="7">
+        <v>0</v>
+      </c>
+      <c r="O638" s="7">
+        <v>0</v>
+      </c>
+      <c r="P638" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q638" s="7">
+        <v>0.71511424367582499</v>
+      </c>
+      <c r="R638" s="7">
+        <v>3.2055120992741601</v>
+      </c>
+      <c r="S638" s="7">
+        <v>0</v>
+      </c>
+      <c r="T638" t="b">
+        <v>1</v>
+      </c>
+      <c r="U638" s="2">
+        <v>486</v>
+      </c>
+      <c r="V638" s="2">
+        <v>278</v>
+      </c>
+      <c r="W638" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="639" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A639" s="10">
+        <v>638</v>
+      </c>
+      <c r="B639" s="7">
+        <v>0</v>
+      </c>
+      <c r="C639" s="7">
+        <v>0</v>
+      </c>
+      <c r="D639" s="7">
+        <v>12.140425219019701</v>
+      </c>
+      <c r="E639" s="7">
+        <v>0</v>
+      </c>
+      <c r="F639" s="7">
+        <v>0</v>
+      </c>
+      <c r="G639" s="7">
+        <v>0</v>
+      </c>
+      <c r="H639" s="7">
+        <v>0</v>
+      </c>
+      <c r="I639" s="7">
+        <v>0</v>
+      </c>
+      <c r="J639" s="7">
+        <v>0</v>
+      </c>
+      <c r="K639" s="7">
+        <v>0</v>
+      </c>
+      <c r="L639" s="7">
+        <v>12.5588554250334</v>
+      </c>
+      <c r="M639" s="7">
+        <v>0</v>
+      </c>
+      <c r="N639" s="7">
+        <v>0</v>
+      </c>
+      <c r="O639" s="7">
+        <v>0</v>
+      </c>
+      <c r="P639" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q639" s="7">
+        <v>2.1714742918697798</v>
+      </c>
+      <c r="R639" s="7">
+        <v>1.2047220386400499</v>
+      </c>
+      <c r="S639" s="7">
+        <v>0</v>
+      </c>
+      <c r="T639" t="b">
+        <v>0</v>
+      </c>
+      <c r="U639" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V639" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W639" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="640" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A640" s="10">
+        <v>639</v>
+      </c>
+      <c r="B640" s="7">
+        <v>0</v>
+      </c>
+      <c r="C640" s="7">
+        <v>0</v>
+      </c>
+      <c r="D640" s="7">
+        <v>0</v>
+      </c>
+      <c r="E640" s="7">
+        <v>0</v>
+      </c>
+      <c r="F640" s="7">
+        <v>0</v>
+      </c>
+      <c r="G640" s="7">
+        <v>0</v>
+      </c>
+      <c r="H640" s="7">
+        <v>13.2061042896988</v>
+      </c>
+      <c r="I640" s="7">
+        <v>11.242926999425</v>
+      </c>
+      <c r="J640" s="7">
+        <v>0</v>
+      </c>
+      <c r="K640" s="7">
+        <v>0</v>
+      </c>
+      <c r="L640" s="7">
+        <v>0</v>
+      </c>
+      <c r="M640" s="7">
+        <v>0</v>
+      </c>
+      <c r="N640" s="7">
+        <v>0</v>
+      </c>
+      <c r="O640" s="7">
+        <v>0</v>
+      </c>
+      <c r="P640" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q640" s="7">
+        <v>1.65923359812466</v>
+      </c>
+      <c r="R640" s="7">
+        <v>2.3916880693689202</v>
+      </c>
+      <c r="S640" s="7">
+        <v>0</v>
+      </c>
+      <c r="T640" t="b">
+        <v>1</v>
+      </c>
+      <c r="U640" s="2">
+        <v>37</v>
+      </c>
+      <c r="V640" s="2">
+        <v>1368</v>
+      </c>
+      <c r="W640" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="641" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A641" s="10">
+        <v>640</v>
+      </c>
+      <c r="B641" s="7">
+        <v>0</v>
+      </c>
+      <c r="C641" s="7">
+        <v>0</v>
+      </c>
+      <c r="D641" s="7">
+        <v>0</v>
+      </c>
+      <c r="E641" s="7">
+        <v>0</v>
+      </c>
+      <c r="F641" s="7">
+        <v>0</v>
+      </c>
+      <c r="G641" s="7">
+        <v>0</v>
+      </c>
+      <c r="H641" s="7">
+        <v>0</v>
+      </c>
+      <c r="I641" s="7">
+        <v>12.0758121226234</v>
+      </c>
+      <c r="J641" s="7">
+        <v>10.8314364290692</v>
+      </c>
+      <c r="K641" s="7">
+        <v>0</v>
+      </c>
+      <c r="L641" s="7">
+        <v>0</v>
+      </c>
+      <c r="M641" s="7">
+        <v>0</v>
+      </c>
+      <c r="N641" s="7">
+        <v>0</v>
+      </c>
+      <c r="O641" s="7">
+        <v>0</v>
+      </c>
+      <c r="P641" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q641" s="7">
+        <v>1.03331981611793</v>
+      </c>
+      <c r="R641" s="7">
+        <v>1.6640474960860201</v>
+      </c>
+      <c r="S641" s="7">
+        <v>0</v>
+      </c>
+      <c r="T641" t="b">
+        <v>1</v>
+      </c>
+      <c r="U641" s="2">
+        <v>24</v>
+      </c>
+      <c r="V641" s="2">
+        <v>43</v>
+      </c>
+      <c r="W641" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="642" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A642" s="10">
+        <v>641</v>
+      </c>
+      <c r="B642" s="7">
+        <v>0</v>
+      </c>
+      <c r="C642" s="7">
+        <v>0</v>
+      </c>
+      <c r="D642" s="7">
+        <v>0</v>
+      </c>
+      <c r="E642" s="7">
+        <v>0</v>
+      </c>
+      <c r="F642" s="7">
+        <v>0</v>
+      </c>
+      <c r="G642" s="7">
+        <v>0</v>
+      </c>
+      <c r="H642" s="7">
+        <v>0</v>
+      </c>
+      <c r="I642" s="7">
+        <v>0</v>
+      </c>
+      <c r="J642" s="7">
+        <v>8.6757475145646801</v>
+      </c>
+      <c r="K642" s="7">
+        <v>0</v>
+      </c>
+      <c r="L642" s="7">
+        <v>13.324459327480501</v>
+      </c>
+      <c r="M642" s="7">
+        <v>0</v>
+      </c>
+      <c r="N642" s="7">
+        <v>0</v>
+      </c>
+      <c r="O642" s="7">
+        <v>0</v>
+      </c>
+      <c r="P642" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q642" s="7">
+        <v>2.22239310476925</v>
+      </c>
+      <c r="R642" s="7">
+        <v>4.7665134964204503</v>
+      </c>
+      <c r="S642" s="7">
+        <v>0</v>
+      </c>
+      <c r="T642" t="b">
+        <v>0</v>
+      </c>
+      <c r="U642" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V642" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W642" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="643" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A643" s="10">
+        <v>642</v>
+      </c>
+      <c r="B643" s="7">
+        <v>0</v>
+      </c>
+      <c r="C643" s="7">
+        <v>0</v>
+      </c>
+      <c r="D643" s="7">
+        <v>9.3290429249952904</v>
+      </c>
+      <c r="E643" s="7">
+        <v>0</v>
+      </c>
+      <c r="F643" s="7">
+        <v>0</v>
+      </c>
+      <c r="G643" s="7">
+        <v>0</v>
+      </c>
+      <c r="H643" s="7">
+        <v>0</v>
+      </c>
+      <c r="I643" s="7">
+        <v>0</v>
+      </c>
+      <c r="J643" s="7">
+        <v>8.9911421479100699</v>
+      </c>
+      <c r="K643" s="7">
+        <v>0</v>
+      </c>
+      <c r="L643" s="7">
+        <v>0</v>
+      </c>
+      <c r="M643" s="7">
+        <v>0</v>
+      </c>
+      <c r="N643" s="7">
+        <v>0</v>
+      </c>
+      <c r="O643" s="7">
+        <v>0</v>
+      </c>
+      <c r="P643" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q643" s="7">
+        <v>1.3118500757424301</v>
+      </c>
+      <c r="R643" s="7">
+        <v>4.6908578465939099</v>
+      </c>
+      <c r="S643" s="7">
+        <v>0</v>
+      </c>
+      <c r="T643" t="b">
+        <v>0</v>
+      </c>
+      <c r="U643" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V643" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W643" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W619">
-    <cfRule type="expression" dxfId="7" priority="5">
+  <conditionalFormatting sqref="A1:W643">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U580">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
-      <formula>4000</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U569">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56160,7 +57922,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated dataset till S666
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867CF682-8BC8-2A46-9F31-F883BBDA796E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA6860B-1BE2-8149-9098-2998BFFB0456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -401,17 +401,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF9C5700"/>
@@ -454,21 +444,21 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -792,11 +782,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:X643"/>
+  <dimension ref="A1:X667"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A606" zoomScale="75" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W643" sqref="W643"/>
+    <sheetView tabSelected="1" topLeftCell="A634" zoomScale="114" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W667" sqref="W667"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46216,15 +46206,15 @@
         <v>0</v>
       </c>
       <c r="U622" s="2" t="str">
-        <f t="shared" ref="U622:U643" si="37">IF(T622=FALSE, "NA", "")</f>
+        <f t="shared" ref="U622:U667" si="37">IF(T622=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V622" s="2" t="str">
-        <f t="shared" ref="V622:V643" si="38">IF(T622=FALSE, "NA", "")</f>
+        <f t="shared" ref="V622:V667" si="38">IF(T622=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W622" s="12" t="str">
-        <f t="shared" ref="W622:W643" si="39">IF(T622=FALSE, "NA", "")</f>
+        <f t="shared" ref="W622:W667" si="39">IF(T622=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -47756,19 +47746,1762 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="644" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A644" s="10">
+        <v>643</v>
+      </c>
+      <c r="B644" s="7">
+        <v>0</v>
+      </c>
+      <c r="C644" s="7">
+        <v>0</v>
+      </c>
+      <c r="D644" s="7">
+        <v>8.1873080716320601</v>
+      </c>
+      <c r="E644" s="7">
+        <v>0</v>
+      </c>
+      <c r="F644" s="7">
+        <v>0</v>
+      </c>
+      <c r="G644" s="7">
+        <v>0</v>
+      </c>
+      <c r="H644" s="7">
+        <v>0</v>
+      </c>
+      <c r="I644" s="7">
+        <v>0</v>
+      </c>
+      <c r="J644" s="7">
+        <v>0</v>
+      </c>
+      <c r="K644" s="7">
+        <v>0</v>
+      </c>
+      <c r="L644" s="7">
+        <v>0</v>
+      </c>
+      <c r="M644" s="7">
+        <v>8.5176784678879809</v>
+      </c>
+      <c r="N644" s="7">
+        <v>0</v>
+      </c>
+      <c r="O644" s="7">
+        <v>0</v>
+      </c>
+      <c r="P644" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q644" s="7">
+        <v>0.94500121014935801</v>
+      </c>
+      <c r="R644" s="7">
+        <v>1.0640764296588601</v>
+      </c>
+      <c r="S644" s="7">
+        <v>0</v>
+      </c>
+      <c r="T644" t="b">
+        <v>1</v>
+      </c>
+      <c r="U644" s="2">
+        <v>17</v>
+      </c>
+      <c r="V644" s="2">
+        <v>5</v>
+      </c>
+      <c r="W644" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="645" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A645" s="10">
+        <v>644</v>
+      </c>
+      <c r="B645" s="7">
+        <v>0</v>
+      </c>
+      <c r="C645" s="7">
+        <v>0</v>
+      </c>
+      <c r="D645" s="7">
+        <v>14.944241757424001</v>
+      </c>
+      <c r="E645" s="7">
+        <v>0</v>
+      </c>
+      <c r="F645" s="7">
+        <v>0</v>
+      </c>
+      <c r="G645" s="7">
+        <v>0</v>
+      </c>
+      <c r="H645" s="7">
+        <v>0</v>
+      </c>
+      <c r="I645" s="7">
+        <v>0</v>
+      </c>
+      <c r="J645" s="7">
+        <v>0</v>
+      </c>
+      <c r="K645" s="7">
+        <v>0</v>
+      </c>
+      <c r="L645" s="7">
+        <v>0</v>
+      </c>
+      <c r="M645" s="7">
+        <v>8.9320008685857406</v>
+      </c>
+      <c r="N645" s="7">
+        <v>0</v>
+      </c>
+      <c r="O645" s="7">
+        <v>0</v>
+      </c>
+      <c r="P645" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q645" s="7">
+        <v>2.83461244295012</v>
+      </c>
+      <c r="R645" s="7">
+        <v>4.2452475611149403</v>
+      </c>
+      <c r="S645" s="7">
+        <v>0</v>
+      </c>
+      <c r="T645" t="b">
+        <v>0</v>
+      </c>
+      <c r="U645" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V645" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W645" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="646" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A646" s="10">
+        <v>645</v>
+      </c>
+      <c r="B646" s="7">
+        <v>8.9925148235165704</v>
+      </c>
+      <c r="C646" s="7">
+        <v>0</v>
+      </c>
+      <c r="D646" s="7">
+        <v>0</v>
+      </c>
+      <c r="E646" s="7">
+        <v>0</v>
+      </c>
+      <c r="F646" s="7">
+        <v>0</v>
+      </c>
+      <c r="G646" s="7">
+        <v>0</v>
+      </c>
+      <c r="H646" s="7">
+        <v>0</v>
+      </c>
+      <c r="I646" s="7">
+        <v>0</v>
+      </c>
+      <c r="J646" s="7">
+        <v>0</v>
+      </c>
+      <c r="K646" s="7">
+        <v>11.4628004457877</v>
+      </c>
+      <c r="L646" s="7">
+        <v>0</v>
+      </c>
+      <c r="M646" s="7">
+        <v>0</v>
+      </c>
+      <c r="N646" s="7">
+        <v>0</v>
+      </c>
+      <c r="O646" s="7">
+        <v>0</v>
+      </c>
+      <c r="P646" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q646" s="7">
+        <v>1.45456930732599</v>
+      </c>
+      <c r="R646" s="7">
+        <v>5.24240678681325</v>
+      </c>
+      <c r="S646" s="7">
+        <v>0</v>
+      </c>
+      <c r="T646" t="b">
+        <v>1</v>
+      </c>
+      <c r="U646" s="2">
+        <v>29</v>
+      </c>
+      <c r="V646" s="2">
+        <v>6</v>
+      </c>
+      <c r="W646" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="647" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A647" s="10">
+        <v>646</v>
+      </c>
+      <c r="B647" s="7">
+        <v>0</v>
+      </c>
+      <c r="C647" s="7">
+        <v>11.885209989554101</v>
+      </c>
+      <c r="D647" s="7">
+        <v>0</v>
+      </c>
+      <c r="E647" s="7">
+        <v>0</v>
+      </c>
+      <c r="F647" s="7">
+        <v>0</v>
+      </c>
+      <c r="G647" s="7">
+        <v>0</v>
+      </c>
+      <c r="H647" s="7">
+        <v>0</v>
+      </c>
+      <c r="I647" s="7">
+        <v>0</v>
+      </c>
+      <c r="J647" s="7">
+        <v>8.8956188021939298</v>
+      </c>
+      <c r="K647" s="7">
+        <v>0</v>
+      </c>
+      <c r="L647" s="7">
+        <v>0</v>
+      </c>
+      <c r="M647" s="7">
+        <v>0</v>
+      </c>
+      <c r="N647" s="7">
+        <v>0</v>
+      </c>
+      <c r="O647" s="7">
+        <v>0</v>
+      </c>
+      <c r="P647" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q647" s="7">
+        <v>2.1336804966885099</v>
+      </c>
+      <c r="R647" s="7">
+        <v>2.9456983314282499</v>
+      </c>
+      <c r="S647" s="7">
+        <v>0</v>
+      </c>
+      <c r="T647" t="b">
+        <v>1</v>
+      </c>
+      <c r="U647" s="2">
+        <v>18</v>
+      </c>
+      <c r="V647" s="2">
+        <v>3</v>
+      </c>
+      <c r="W647" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="648" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A648" s="10">
+        <v>647</v>
+      </c>
+      <c r="B648" s="7">
+        <v>0</v>
+      </c>
+      <c r="C648" s="7">
+        <v>0</v>
+      </c>
+      <c r="D648" s="7">
+        <v>0</v>
+      </c>
+      <c r="E648" s="7">
+        <v>0</v>
+      </c>
+      <c r="F648" s="7">
+        <v>0</v>
+      </c>
+      <c r="G648" s="7">
+        <v>0</v>
+      </c>
+      <c r="H648" s="7">
+        <v>0</v>
+      </c>
+      <c r="I648" s="7">
+        <v>6.8686537445742601</v>
+      </c>
+      <c r="J648" s="7">
+        <v>0</v>
+      </c>
+      <c r="K648" s="7">
+        <v>0</v>
+      </c>
+      <c r="L648" s="7">
+        <v>11.925053549216299</v>
+      </c>
+      <c r="M648" s="7">
+        <v>0</v>
+      </c>
+      <c r="N648" s="7">
+        <v>0</v>
+      </c>
+      <c r="O648" s="7">
+        <v>0</v>
+      </c>
+      <c r="P648" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q648" s="7">
+        <v>1.65653695092375</v>
+      </c>
+      <c r="R648" s="7">
+        <v>1.45906064014547</v>
+      </c>
+      <c r="S648" s="7">
+        <v>0</v>
+      </c>
+      <c r="T648" t="b">
+        <v>0</v>
+      </c>
+      <c r="U648" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V648" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W648" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="649" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A649" s="10">
+        <v>648</v>
+      </c>
+      <c r="B649" s="7">
+        <v>0</v>
+      </c>
+      <c r="C649" s="7">
+        <v>0</v>
+      </c>
+      <c r="D649" s="7">
+        <v>0</v>
+      </c>
+      <c r="E649" s="7">
+        <v>0</v>
+      </c>
+      <c r="F649" s="7">
+        <v>0</v>
+      </c>
+      <c r="G649" s="7">
+        <v>0</v>
+      </c>
+      <c r="H649" s="7">
+        <v>10.933164705244501</v>
+      </c>
+      <c r="I649" s="7">
+        <v>0</v>
+      </c>
+      <c r="J649" s="7">
+        <v>11.5691904462444</v>
+      </c>
+      <c r="K649" s="7">
+        <v>0</v>
+      </c>
+      <c r="L649" s="7">
+        <v>0</v>
+      </c>
+      <c r="M649" s="7">
+        <v>0</v>
+      </c>
+      <c r="N649" s="7">
+        <v>0</v>
+      </c>
+      <c r="O649" s="7">
+        <v>0</v>
+      </c>
+      <c r="P649" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q649" s="7">
+        <v>2.8832185404125998</v>
+      </c>
+      <c r="R649" s="7">
+        <v>1.18764065834869</v>
+      </c>
+      <c r="S649" s="7">
+        <v>0</v>
+      </c>
+      <c r="T649" t="b">
+        <v>1</v>
+      </c>
+      <c r="U649" s="2">
+        <v>27</v>
+      </c>
+      <c r="V649" s="2">
+        <v>4</v>
+      </c>
+      <c r="W649" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="650" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A650" s="10">
+        <v>649</v>
+      </c>
+      <c r="B650" s="7">
+        <v>0</v>
+      </c>
+      <c r="C650" s="7">
+        <v>7.9468813899144903</v>
+      </c>
+      <c r="D650" s="7">
+        <v>0</v>
+      </c>
+      <c r="E650" s="7">
+        <v>0</v>
+      </c>
+      <c r="F650" s="7">
+        <v>0</v>
+      </c>
+      <c r="G650" s="7">
+        <v>0</v>
+      </c>
+      <c r="H650" s="7">
+        <v>0</v>
+      </c>
+      <c r="I650" s="7">
+        <v>0</v>
+      </c>
+      <c r="J650" s="7">
+        <v>0</v>
+      </c>
+      <c r="K650" s="7">
+        <v>10.1653567359525</v>
+      </c>
+      <c r="L650" s="7">
+        <v>0</v>
+      </c>
+      <c r="M650" s="7">
+        <v>0</v>
+      </c>
+      <c r="N650" s="7">
+        <v>0</v>
+      </c>
+      <c r="O650" s="7">
+        <v>0</v>
+      </c>
+      <c r="P650" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q650" s="7">
+        <v>0.88868458094207303</v>
+      </c>
+      <c r="R650" s="7">
+        <v>1.8470699133306301</v>
+      </c>
+      <c r="S650" s="7">
+        <v>0</v>
+      </c>
+      <c r="T650" t="b">
+        <v>1</v>
+      </c>
+      <c r="U650" s="2">
+        <v>18</v>
+      </c>
+      <c r="V650" s="2">
+        <v>2</v>
+      </c>
+      <c r="W650" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="651" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A651" s="10">
+        <v>650</v>
+      </c>
+      <c r="B651" s="7">
+        <v>0</v>
+      </c>
+      <c r="C651" s="7">
+        <v>0</v>
+      </c>
+      <c r="D651" s="7">
+        <v>0</v>
+      </c>
+      <c r="E651" s="7">
+        <v>7.5790890010537604</v>
+      </c>
+      <c r="F651" s="7">
+        <v>0</v>
+      </c>
+      <c r="G651" s="7">
+        <v>0</v>
+      </c>
+      <c r="H651" s="7">
+        <v>0</v>
+      </c>
+      <c r="I651" s="7">
+        <v>0</v>
+      </c>
+      <c r="J651" s="7">
+        <v>13.110102138132</v>
+      </c>
+      <c r="K651" s="7">
+        <v>0</v>
+      </c>
+      <c r="L651" s="7">
+        <v>0</v>
+      </c>
+      <c r="M651" s="7">
+        <v>0</v>
+      </c>
+      <c r="N651" s="7">
+        <v>0</v>
+      </c>
+      <c r="O651" s="7">
+        <v>0</v>
+      </c>
+      <c r="P651" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q651" s="7">
+        <v>1.0258000424901601</v>
+      </c>
+      <c r="R651" s="7">
+        <v>3.99243893837893</v>
+      </c>
+      <c r="S651" s="7">
+        <v>0</v>
+      </c>
+      <c r="T651" t="b">
+        <v>0</v>
+      </c>
+      <c r="U651" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V651" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W651" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="652" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A652" s="10">
+        <v>651</v>
+      </c>
+      <c r="B652" s="7">
+        <v>0</v>
+      </c>
+      <c r="C652" s="7">
+        <v>0</v>
+      </c>
+      <c r="D652" s="7">
+        <v>11.642678669983599</v>
+      </c>
+      <c r="E652" s="7">
+        <v>0</v>
+      </c>
+      <c r="F652" s="7">
+        <v>0</v>
+      </c>
+      <c r="G652" s="7">
+        <v>0</v>
+      </c>
+      <c r="H652" s="7">
+        <v>12.4199215086087</v>
+      </c>
+      <c r="I652" s="7">
+        <v>0</v>
+      </c>
+      <c r="J652" s="7">
+        <v>0</v>
+      </c>
+      <c r="K652" s="7">
+        <v>0</v>
+      </c>
+      <c r="L652" s="7">
+        <v>0</v>
+      </c>
+      <c r="M652" s="7">
+        <v>0</v>
+      </c>
+      <c r="N652" s="7">
+        <v>0</v>
+      </c>
+      <c r="O652" s="7">
+        <v>0</v>
+      </c>
+      <c r="P652" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q652" s="7">
+        <v>2.6215732458121099</v>
+      </c>
+      <c r="R652" s="7">
+        <v>4.9587893555419003</v>
+      </c>
+      <c r="S652" s="7">
+        <v>0</v>
+      </c>
+      <c r="T652" t="b">
+        <v>0</v>
+      </c>
+      <c r="U652" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V652" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W652" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="653" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A653" s="10">
+        <v>652</v>
+      </c>
+      <c r="B653" s="7">
+        <v>0</v>
+      </c>
+      <c r="C653" s="7">
+        <v>0</v>
+      </c>
+      <c r="D653" s="7">
+        <v>0</v>
+      </c>
+      <c r="E653" s="7">
+        <v>0</v>
+      </c>
+      <c r="F653" s="7">
+        <v>11.524866229748699</v>
+      </c>
+      <c r="G653" s="7">
+        <v>0</v>
+      </c>
+      <c r="H653" s="7">
+        <v>0</v>
+      </c>
+      <c r="I653" s="7">
+        <v>10.158644996576999</v>
+      </c>
+      <c r="J653" s="7">
+        <v>0</v>
+      </c>
+      <c r="K653" s="7">
+        <v>0</v>
+      </c>
+      <c r="L653" s="7">
+        <v>0</v>
+      </c>
+      <c r="M653" s="7">
+        <v>0</v>
+      </c>
+      <c r="N653" s="7">
+        <v>0</v>
+      </c>
+      <c r="O653" s="7">
+        <v>0</v>
+      </c>
+      <c r="P653" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q653" s="7">
+        <v>2.7054380935061499</v>
+      </c>
+      <c r="R653" s="7">
+        <v>2.54041137061192</v>
+      </c>
+      <c r="S653" s="7">
+        <v>0</v>
+      </c>
+      <c r="T653" t="b">
+        <v>0</v>
+      </c>
+      <c r="U653" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V653" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W653" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="654" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A654" s="10">
+        <v>653</v>
+      </c>
+      <c r="B654" s="7">
+        <v>0</v>
+      </c>
+      <c r="C654" s="7">
+        <v>13.6787818824958</v>
+      </c>
+      <c r="D654" s="7">
+        <v>8.7891787656123395</v>
+      </c>
+      <c r="E654" s="7">
+        <v>0</v>
+      </c>
+      <c r="F654" s="7">
+        <v>0</v>
+      </c>
+      <c r="G654" s="7">
+        <v>0</v>
+      </c>
+      <c r="H654" s="7">
+        <v>0</v>
+      </c>
+      <c r="I654" s="7">
+        <v>0</v>
+      </c>
+      <c r="J654" s="7">
+        <v>0</v>
+      </c>
+      <c r="K654" s="7">
+        <v>0</v>
+      </c>
+      <c r="L654" s="7">
+        <v>0</v>
+      </c>
+      <c r="M654" s="7">
+        <v>0</v>
+      </c>
+      <c r="N654" s="7">
+        <v>0</v>
+      </c>
+      <c r="O654" s="7">
+        <v>0</v>
+      </c>
+      <c r="P654" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q654" s="7">
+        <v>1.34737466080264</v>
+      </c>
+      <c r="R654" s="7">
+        <v>4.95013734077469</v>
+      </c>
+      <c r="S654" s="7">
+        <v>0</v>
+      </c>
+      <c r="T654" t="b">
+        <v>1</v>
+      </c>
+      <c r="U654" s="2">
+        <v>15</v>
+      </c>
+      <c r="V654" s="2">
+        <v>4</v>
+      </c>
+      <c r="W654" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="655" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A655" s="10">
+        <v>654</v>
+      </c>
+      <c r="B655" s="7">
+        <v>0</v>
+      </c>
+      <c r="C655" s="7">
+        <v>0</v>
+      </c>
+      <c r="D655" s="7">
+        <v>9.3627476299457104</v>
+      </c>
+      <c r="E655" s="7">
+        <v>0</v>
+      </c>
+      <c r="F655" s="7">
+        <v>10.0849375887222</v>
+      </c>
+      <c r="G655" s="7">
+        <v>0</v>
+      </c>
+      <c r="H655" s="7">
+        <v>0</v>
+      </c>
+      <c r="I655" s="7">
+        <v>0</v>
+      </c>
+      <c r="J655" s="7">
+        <v>0</v>
+      </c>
+      <c r="K655" s="7">
+        <v>0</v>
+      </c>
+      <c r="L655" s="7">
+        <v>0</v>
+      </c>
+      <c r="M655" s="7">
+        <v>0</v>
+      </c>
+      <c r="N655" s="7">
+        <v>0</v>
+      </c>
+      <c r="O655" s="7">
+        <v>0</v>
+      </c>
+      <c r="P655" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q655" s="7">
+        <v>1.93779394760739</v>
+      </c>
+      <c r="R655" s="7">
+        <v>2.7650971709318402</v>
+      </c>
+      <c r="S655" s="7">
+        <v>0</v>
+      </c>
+      <c r="T655" t="b">
+        <v>1</v>
+      </c>
+      <c r="U655" s="2">
+        <v>15</v>
+      </c>
+      <c r="V655" s="2">
+        <v>3</v>
+      </c>
+      <c r="W655" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="656" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A656" s="10">
+        <v>655</v>
+      </c>
+      <c r="B656" s="7">
+        <v>0</v>
+      </c>
+      <c r="C656" s="7">
+        <v>0</v>
+      </c>
+      <c r="D656" s="7">
+        <v>0</v>
+      </c>
+      <c r="E656" s="7">
+        <v>0</v>
+      </c>
+      <c r="F656" s="7">
+        <v>0</v>
+      </c>
+      <c r="G656" s="7">
+        <v>0</v>
+      </c>
+      <c r="H656" s="7">
+        <v>0</v>
+      </c>
+      <c r="I656" s="7">
+        <v>7.5105542703727997</v>
+      </c>
+      <c r="J656" s="7">
+        <v>0</v>
+      </c>
+      <c r="K656" s="7">
+        <v>0</v>
+      </c>
+      <c r="L656" s="7">
+        <v>0</v>
+      </c>
+      <c r="M656" s="7">
+        <v>8.2451482085982004</v>
+      </c>
+      <c r="N656" s="7">
+        <v>0</v>
+      </c>
+      <c r="O656" s="7">
+        <v>0</v>
+      </c>
+      <c r="P656" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q656" s="7">
+        <v>2.0834071777404</v>
+      </c>
+      <c r="R656" s="7">
+        <v>5.1030615316504804</v>
+      </c>
+      <c r="S656" s="7">
+        <v>0</v>
+      </c>
+      <c r="T656" t="b">
+        <v>0</v>
+      </c>
+      <c r="U656" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V656" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W656" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="657" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A657" s="10">
+        <v>656</v>
+      </c>
+      <c r="B657" s="7">
+        <v>0</v>
+      </c>
+      <c r="C657" s="7">
+        <v>0</v>
+      </c>
+      <c r="D657" s="7">
+        <v>11.1666488906233</v>
+      </c>
+      <c r="E657" s="7">
+        <v>0</v>
+      </c>
+      <c r="F657" s="7">
+        <v>0</v>
+      </c>
+      <c r="G657" s="7">
+        <v>13.1808294487714</v>
+      </c>
+      <c r="H657" s="7">
+        <v>0</v>
+      </c>
+      <c r="I657" s="7">
+        <v>0</v>
+      </c>
+      <c r="J657" s="7">
+        <v>0</v>
+      </c>
+      <c r="K657" s="7">
+        <v>0</v>
+      </c>
+      <c r="L657" s="7">
+        <v>0</v>
+      </c>
+      <c r="M657" s="7">
+        <v>0</v>
+      </c>
+      <c r="N657" s="7">
+        <v>0</v>
+      </c>
+      <c r="O657" s="7">
+        <v>0</v>
+      </c>
+      <c r="P657" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q657" s="7">
+        <v>2.0582594353479</v>
+      </c>
+      <c r="R657" s="7">
+        <v>3.3569675969134898</v>
+      </c>
+      <c r="S657" s="7">
+        <v>0</v>
+      </c>
+      <c r="T657" t="b">
+        <v>1</v>
+      </c>
+      <c r="U657" s="2">
+        <v>19</v>
+      </c>
+      <c r="V657" s="2">
+        <v>7</v>
+      </c>
+      <c r="W657" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="658" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A658" s="10">
+        <v>657</v>
+      </c>
+      <c r="B658" s="7">
+        <v>0</v>
+      </c>
+      <c r="C658" s="7">
+        <v>0</v>
+      </c>
+      <c r="D658" s="7">
+        <v>0</v>
+      </c>
+      <c r="E658" s="7">
+        <v>0</v>
+      </c>
+      <c r="F658" s="7">
+        <v>9.0393555924901907</v>
+      </c>
+      <c r="G658" s="7">
+        <v>11.7793022630702</v>
+      </c>
+      <c r="H658" s="7">
+        <v>0</v>
+      </c>
+      <c r="I658" s="7">
+        <v>0</v>
+      </c>
+      <c r="J658" s="7">
+        <v>0</v>
+      </c>
+      <c r="K658" s="7">
+        <v>0</v>
+      </c>
+      <c r="L658" s="7">
+        <v>0</v>
+      </c>
+      <c r="M658" s="7">
+        <v>0</v>
+      </c>
+      <c r="N658" s="7">
+        <v>0</v>
+      </c>
+      <c r="O658" s="7">
+        <v>0</v>
+      </c>
+      <c r="P658" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q658" s="7">
+        <v>2.0142310659399101</v>
+      </c>
+      <c r="R658" s="7">
+        <v>2.0734731561146198</v>
+      </c>
+      <c r="S658" s="7">
+        <v>0</v>
+      </c>
+      <c r="T658" t="b">
+        <v>0</v>
+      </c>
+      <c r="U658" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V658" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W658" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="659" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A659" s="10">
+        <v>658</v>
+      </c>
+      <c r="B659" s="7">
+        <v>0</v>
+      </c>
+      <c r="C659" s="7">
+        <v>0</v>
+      </c>
+      <c r="D659" s="7">
+        <v>0</v>
+      </c>
+      <c r="E659" s="7">
+        <v>0</v>
+      </c>
+      <c r="F659" s="7">
+        <v>0</v>
+      </c>
+      <c r="G659" s="7">
+        <v>0</v>
+      </c>
+      <c r="H659" s="7">
+        <v>0</v>
+      </c>
+      <c r="I659" s="7">
+        <v>0</v>
+      </c>
+      <c r="J659" s="7">
+        <v>0</v>
+      </c>
+      <c r="K659" s="7">
+        <v>0</v>
+      </c>
+      <c r="L659" s="7">
+        <v>8.4563071792161608</v>
+      </c>
+      <c r="M659" s="7">
+        <v>8.1035029676261203</v>
+      </c>
+      <c r="N659" s="7">
+        <v>0</v>
+      </c>
+      <c r="O659" s="7">
+        <v>0</v>
+      </c>
+      <c r="P659" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q659" s="7">
+        <v>1.5966139603827001</v>
+      </c>
+      <c r="R659" s="7">
+        <v>4.3725734439275099</v>
+      </c>
+      <c r="S659" s="7">
+        <v>0</v>
+      </c>
+      <c r="T659" t="b">
+        <v>0</v>
+      </c>
+      <c r="U659" s="2" t="str">
+        <f>IF(T659=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V659" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W659" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="660" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A660" s="10">
+        <v>659</v>
+      </c>
+      <c r="B660" s="7">
+        <v>7.2668671119287698</v>
+      </c>
+      <c r="C660" s="7">
+        <v>0</v>
+      </c>
+      <c r="D660" s="7">
+        <v>0</v>
+      </c>
+      <c r="E660" s="7">
+        <v>0</v>
+      </c>
+      <c r="F660" s="7">
+        <v>9.6366688461547998</v>
+      </c>
+      <c r="G660" s="7">
+        <v>0</v>
+      </c>
+      <c r="H660" s="7">
+        <v>0</v>
+      </c>
+      <c r="I660" s="7">
+        <v>0</v>
+      </c>
+      <c r="J660" s="7">
+        <v>0</v>
+      </c>
+      <c r="K660" s="7">
+        <v>0</v>
+      </c>
+      <c r="L660" s="7">
+        <v>0</v>
+      </c>
+      <c r="M660" s="7">
+        <v>0</v>
+      </c>
+      <c r="N660" s="7">
+        <v>0</v>
+      </c>
+      <c r="O660" s="7">
+        <v>0</v>
+      </c>
+      <c r="P660" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q660" s="7">
+        <v>1.89569376684084</v>
+      </c>
+      <c r="R660" s="7">
+        <v>1.2400125353507701</v>
+      </c>
+      <c r="S660" s="7">
+        <v>0</v>
+      </c>
+      <c r="T660" t="b">
+        <v>1</v>
+      </c>
+      <c r="U660" s="2">
+        <v>35</v>
+      </c>
+      <c r="V660" s="2">
+        <v>4</v>
+      </c>
+      <c r="W660" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="661" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A661" s="10">
+        <v>660</v>
+      </c>
+      <c r="B661" s="7">
+        <v>0</v>
+      </c>
+      <c r="C661" s="7">
+        <v>0</v>
+      </c>
+      <c r="D661" s="7">
+        <v>0</v>
+      </c>
+      <c r="E661" s="7">
+        <v>0</v>
+      </c>
+      <c r="F661" s="7">
+        <v>0</v>
+      </c>
+      <c r="G661" s="7">
+        <v>0</v>
+      </c>
+      <c r="H661" s="7">
+        <v>0</v>
+      </c>
+      <c r="I661" s="7">
+        <v>0</v>
+      </c>
+      <c r="J661" s="7">
+        <v>0</v>
+      </c>
+      <c r="K661" s="7">
+        <v>10.123668314403901</v>
+      </c>
+      <c r="L661" s="7">
+        <v>0</v>
+      </c>
+      <c r="M661" s="7">
+        <v>8.3253196886974106</v>
+      </c>
+      <c r="N661" s="7">
+        <v>0</v>
+      </c>
+      <c r="O661" s="7">
+        <v>0</v>
+      </c>
+      <c r="P661" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q661" s="7">
+        <v>2.1484695970832099</v>
+      </c>
+      <c r="R661" s="7">
+        <v>1.7058450736100499</v>
+      </c>
+      <c r="S661" s="7">
+        <v>0</v>
+      </c>
+      <c r="T661" t="b">
+        <v>0</v>
+      </c>
+      <c r="U661" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V661" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W661" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="662" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A662" s="10">
+        <v>661</v>
+      </c>
+      <c r="B662" s="7">
+        <v>0</v>
+      </c>
+      <c r="C662" s="7">
+        <v>0</v>
+      </c>
+      <c r="D662" s="7">
+        <v>0</v>
+      </c>
+      <c r="E662" s="7">
+        <v>11.119233204176901</v>
+      </c>
+      <c r="F662" s="7">
+        <v>0</v>
+      </c>
+      <c r="G662" s="7">
+        <v>0</v>
+      </c>
+      <c r="H662" s="7">
+        <v>0</v>
+      </c>
+      <c r="I662" s="7">
+        <v>0</v>
+      </c>
+      <c r="J662" s="7">
+        <v>0</v>
+      </c>
+      <c r="K662" s="7">
+        <v>0</v>
+      </c>
+      <c r="L662" s="7">
+        <v>11.0285462093085</v>
+      </c>
+      <c r="M662" s="7">
+        <v>0</v>
+      </c>
+      <c r="N662" s="7">
+        <v>0</v>
+      </c>
+      <c r="O662" s="7">
+        <v>0</v>
+      </c>
+      <c r="P662" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q662" s="7">
+        <v>1.9056864338377599</v>
+      </c>
+      <c r="R662" s="7">
+        <v>4.1967925958674801</v>
+      </c>
+      <c r="S662" s="7">
+        <v>0</v>
+      </c>
+      <c r="T662" t="b">
+        <v>1</v>
+      </c>
+      <c r="U662" s="2">
+        <v>4308</v>
+      </c>
+      <c r="V662" s="2">
+        <v>347</v>
+      </c>
+      <c r="W662" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="663" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A663" s="10">
+        <v>662</v>
+      </c>
+      <c r="B663" s="7">
+        <v>0</v>
+      </c>
+      <c r="C663" s="7">
+        <v>0</v>
+      </c>
+      <c r="D663" s="7">
+        <v>0</v>
+      </c>
+      <c r="E663" s="7">
+        <v>0</v>
+      </c>
+      <c r="F663" s="7">
+        <v>0</v>
+      </c>
+      <c r="G663" s="7">
+        <v>0</v>
+      </c>
+      <c r="H663" s="7">
+        <v>10.8962601840487</v>
+      </c>
+      <c r="I663" s="7">
+        <v>0</v>
+      </c>
+      <c r="J663" s="7">
+        <v>0</v>
+      </c>
+      <c r="K663" s="7">
+        <v>12.5871273321446</v>
+      </c>
+      <c r="L663" s="7">
+        <v>0</v>
+      </c>
+      <c r="M663" s="7">
+        <v>0</v>
+      </c>
+      <c r="N663" s="7">
+        <v>0</v>
+      </c>
+      <c r="O663" s="7">
+        <v>0</v>
+      </c>
+      <c r="P663" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q663" s="7">
+        <v>1.4959381329224499</v>
+      </c>
+      <c r="R663" s="7">
+        <v>2.2729365520870801</v>
+      </c>
+      <c r="S663" s="7">
+        <v>0</v>
+      </c>
+      <c r="T663" t="b">
+        <v>1</v>
+      </c>
+      <c r="U663" s="2">
+        <v>16</v>
+      </c>
+      <c r="V663" s="2">
+        <v>5</v>
+      </c>
+      <c r="W663" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="664" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A664" s="10">
+        <v>663</v>
+      </c>
+      <c r="B664" s="7">
+        <v>0</v>
+      </c>
+      <c r="C664" s="7">
+        <v>0</v>
+      </c>
+      <c r="D664" s="7">
+        <v>0</v>
+      </c>
+      <c r="E664" s="7">
+        <v>0</v>
+      </c>
+      <c r="F664" s="7">
+        <v>8.4473918186538306</v>
+      </c>
+      <c r="G664" s="7">
+        <v>0</v>
+      </c>
+      <c r="H664" s="7">
+        <v>0</v>
+      </c>
+      <c r="I664" s="7">
+        <v>7.5067411449797898</v>
+      </c>
+      <c r="J664" s="7">
+        <v>0</v>
+      </c>
+      <c r="K664" s="7">
+        <v>0</v>
+      </c>
+      <c r="L664" s="7">
+        <v>0</v>
+      </c>
+      <c r="M664" s="7">
+        <v>0</v>
+      </c>
+      <c r="N664" s="7">
+        <v>0</v>
+      </c>
+      <c r="O664" s="7">
+        <v>0</v>
+      </c>
+      <c r="P664" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q664" s="7">
+        <v>1.53868703436322</v>
+      </c>
+      <c r="R664" s="7">
+        <v>3.85697549947036</v>
+      </c>
+      <c r="S664" s="7">
+        <v>0</v>
+      </c>
+      <c r="T664" t="b">
+        <v>0</v>
+      </c>
+      <c r="U664" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V664" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W664" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="665" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A665" s="10">
+        <v>664</v>
+      </c>
+      <c r="B665" s="7">
+        <v>11.793054035448099</v>
+      </c>
+      <c r="C665" s="7">
+        <v>0</v>
+      </c>
+      <c r="D665" s="7">
+        <v>0</v>
+      </c>
+      <c r="E665" s="7">
+        <v>0</v>
+      </c>
+      <c r="F665" s="7">
+        <v>0</v>
+      </c>
+      <c r="G665" s="7">
+        <v>0</v>
+      </c>
+      <c r="H665" s="7">
+        <v>0</v>
+      </c>
+      <c r="I665" s="7">
+        <v>0</v>
+      </c>
+      <c r="J665" s="7">
+        <v>0</v>
+      </c>
+      <c r="K665" s="7">
+        <v>0</v>
+      </c>
+      <c r="L665" s="7">
+        <v>8.5013946595407806</v>
+      </c>
+      <c r="M665" s="7">
+        <v>0</v>
+      </c>
+      <c r="N665" s="7">
+        <v>0</v>
+      </c>
+      <c r="O665" s="7">
+        <v>0</v>
+      </c>
+      <c r="P665" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q665" s="7">
+        <v>2.6322899017030799</v>
+      </c>
+      <c r="R665" s="7">
+        <v>3.5179547818162802</v>
+      </c>
+      <c r="S665" s="7">
+        <v>0</v>
+      </c>
+      <c r="T665" t="b">
+        <v>0</v>
+      </c>
+      <c r="U665" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V665" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W665" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="666" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A666" s="10">
+        <v>665</v>
+      </c>
+      <c r="B666" s="7">
+        <v>0</v>
+      </c>
+      <c r="C666" s="7">
+        <v>8.7284141465519092</v>
+      </c>
+      <c r="D666" s="7">
+        <v>0</v>
+      </c>
+      <c r="E666" s="7">
+        <v>0</v>
+      </c>
+      <c r="F666" s="7">
+        <v>0</v>
+      </c>
+      <c r="G666" s="7">
+        <v>11.702686643748899</v>
+      </c>
+      <c r="H666" s="7">
+        <v>0</v>
+      </c>
+      <c r="I666" s="7">
+        <v>0</v>
+      </c>
+      <c r="J666" s="7">
+        <v>0</v>
+      </c>
+      <c r="K666" s="7">
+        <v>0</v>
+      </c>
+      <c r="L666" s="7">
+        <v>0</v>
+      </c>
+      <c r="M666" s="7">
+        <v>0</v>
+      </c>
+      <c r="N666" s="7">
+        <v>0</v>
+      </c>
+      <c r="O666" s="7">
+        <v>0</v>
+      </c>
+      <c r="P666" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q666" s="7">
+        <v>3.0159656003843001</v>
+      </c>
+      <c r="R666" s="7">
+        <v>3.3847892055029098</v>
+      </c>
+      <c r="S666" s="7">
+        <v>0</v>
+      </c>
+      <c r="T666" t="b">
+        <v>0</v>
+      </c>
+      <c r="U666" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V666" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W666" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="667" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A667" s="10">
+        <v>666</v>
+      </c>
+      <c r="B667" s="7">
+        <v>0</v>
+      </c>
+      <c r="C667" s="7">
+        <v>0</v>
+      </c>
+      <c r="D667" s="7">
+        <v>0</v>
+      </c>
+      <c r="E667" s="7">
+        <v>0</v>
+      </c>
+      <c r="F667" s="7">
+        <v>0</v>
+      </c>
+      <c r="G667" s="7">
+        <v>0</v>
+      </c>
+      <c r="H667" s="7">
+        <v>0</v>
+      </c>
+      <c r="I667" s="7">
+        <v>0</v>
+      </c>
+      <c r="J667" s="7">
+        <v>0</v>
+      </c>
+      <c r="K667" s="7">
+        <v>11.9757545980767</v>
+      </c>
+      <c r="L667" s="7">
+        <v>10.4392874019515</v>
+      </c>
+      <c r="M667" s="7">
+        <v>0</v>
+      </c>
+      <c r="N667" s="7">
+        <v>0</v>
+      </c>
+      <c r="O667" s="7">
+        <v>0</v>
+      </c>
+      <c r="P667" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q667" s="7">
+        <v>2.9425914167437899</v>
+      </c>
+      <c r="R667" s="7">
+        <v>4.6311254176268797</v>
+      </c>
+      <c r="S667" s="7">
+        <v>0</v>
+      </c>
+      <c r="T667" t="b">
+        <v>0</v>
+      </c>
+      <c r="U667" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V667" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W667" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W643">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="A1:W667">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U580">
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U569">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -57922,7 +59655,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S690
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA6860B-1BE2-8149-9098-2998BFFB0456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2920553D-46D8-6042-88FA-63B6275BCE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="65">
   <si>
     <t>Sample</t>
   </si>
@@ -231,6 +231,9 @@
   <si>
     <t>HIGH TURBIDITY - REMOVE SAMPLE (NOTE: MORE DIFFICULT TO DETERMINE THE PHASE STABILITY FOR THESE SAMPLES TOO)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Shear thickening - interesting! </t>
+  </si>
 </sst>
 </file>
 
@@ -404,6 +407,16 @@
   <dxfs count="7">
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -449,16 +462,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -782,11 +785,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:X667"/>
+  <dimension ref="A1:X691"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A634" zoomScale="114" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W667" sqref="W667"/>
+    <sheetView tabSelected="1" topLeftCell="A657" zoomScale="125" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D696" sqref="D696"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -46206,15 +46209,15 @@
         <v>0</v>
       </c>
       <c r="U622" s="2" t="str">
-        <f t="shared" ref="U622:U667" si="37">IF(T622=FALSE, "NA", "")</f>
+        <f t="shared" ref="U622:U685" si="37">IF(T622=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V622" s="2" t="str">
-        <f t="shared" ref="V622:V667" si="38">IF(T622=FALSE, "NA", "")</f>
+        <f t="shared" ref="V622:V685" si="38">IF(T622=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W622" s="12" t="str">
-        <f t="shared" ref="W622:W667" si="39">IF(T622=FALSE, "NA", "")</f>
+        <f t="shared" ref="W622:W685" si="39">IF(T622=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -49489,19 +49492,1786 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="668" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A668" s="10">
+        <v>667</v>
+      </c>
+      <c r="B668" s="7">
+        <v>0</v>
+      </c>
+      <c r="C668" s="7">
+        <v>0</v>
+      </c>
+      <c r="D668" s="7">
+        <v>0</v>
+      </c>
+      <c r="E668" s="7">
+        <v>0</v>
+      </c>
+      <c r="F668" s="7">
+        <v>0</v>
+      </c>
+      <c r="G668" s="7">
+        <v>0</v>
+      </c>
+      <c r="H668" s="7">
+        <v>0</v>
+      </c>
+      <c r="I668" s="7">
+        <v>10.730365142979</v>
+      </c>
+      <c r="J668" s="7">
+        <v>0</v>
+      </c>
+      <c r="K668" s="7">
+        <v>0</v>
+      </c>
+      <c r="L668" s="7">
+        <v>0</v>
+      </c>
+      <c r="M668" s="7">
+        <v>8.29229010388738</v>
+      </c>
+      <c r="N668" s="7">
+        <v>0</v>
+      </c>
+      <c r="O668" s="7">
+        <v>0</v>
+      </c>
+      <c r="P668" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q668" s="7">
+        <v>2.0161199840495598</v>
+      </c>
+      <c r="R668" s="7">
+        <v>0</v>
+      </c>
+      <c r="S668" s="7">
+        <v>2.2021649543290698</v>
+      </c>
+      <c r="T668" t="b">
+        <v>0</v>
+      </c>
+      <c r="U668" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V668" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W668" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="669" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A669" s="10">
+        <v>668</v>
+      </c>
+      <c r="B669" s="7">
+        <v>0</v>
+      </c>
+      <c r="C669" s="7">
+        <v>0</v>
+      </c>
+      <c r="D669" s="7">
+        <v>0</v>
+      </c>
+      <c r="E669" s="7">
+        <v>6.4905317762475798</v>
+      </c>
+      <c r="F669" s="7">
+        <v>0</v>
+      </c>
+      <c r="G669" s="7">
+        <v>0</v>
+      </c>
+      <c r="H669" s="7">
+        <v>0</v>
+      </c>
+      <c r="I669" s="7">
+        <v>0</v>
+      </c>
+      <c r="J669" s="7">
+        <v>0</v>
+      </c>
+      <c r="K669" s="7">
+        <v>0</v>
+      </c>
+      <c r="L669" s="7">
+        <v>10.009735696825301</v>
+      </c>
+      <c r="M669" s="7">
+        <v>0</v>
+      </c>
+      <c r="N669" s="7">
+        <v>0</v>
+      </c>
+      <c r="O669" s="7">
+        <v>0</v>
+      </c>
+      <c r="P669" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q669" s="7">
+        <v>1.82708669456136</v>
+      </c>
+      <c r="R669" s="7">
+        <v>0</v>
+      </c>
+      <c r="S669" s="7">
+        <v>3.9691021490608098</v>
+      </c>
+      <c r="T669" t="b">
+        <v>0</v>
+      </c>
+      <c r="U669" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V669" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W669" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="670" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A670" s="10">
+        <v>669</v>
+      </c>
+      <c r="B670" s="7">
+        <v>0</v>
+      </c>
+      <c r="C670" s="7">
+        <v>0</v>
+      </c>
+      <c r="D670" s="7">
+        <v>0</v>
+      </c>
+      <c r="E670" s="7">
+        <v>0</v>
+      </c>
+      <c r="F670" s="7">
+        <v>0</v>
+      </c>
+      <c r="G670" s="7">
+        <v>9.6540649258841391</v>
+      </c>
+      <c r="H670" s="7">
+        <v>0</v>
+      </c>
+      <c r="I670" s="7">
+        <v>7.9545790602702899</v>
+      </c>
+      <c r="J670" s="7">
+        <v>0</v>
+      </c>
+      <c r="K670" s="7">
+        <v>0</v>
+      </c>
+      <c r="L670" s="7">
+        <v>0</v>
+      </c>
+      <c r="M670" s="7">
+        <v>0</v>
+      </c>
+      <c r="N670" s="7">
+        <v>0</v>
+      </c>
+      <c r="O670" s="7">
+        <v>0</v>
+      </c>
+      <c r="P670" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q670" s="7">
+        <v>2.08741198711266</v>
+      </c>
+      <c r="R670" s="7">
+        <v>0</v>
+      </c>
+      <c r="S670" s="7">
+        <v>1.9063797970798899</v>
+      </c>
+      <c r="T670" t="b">
+        <v>0</v>
+      </c>
+      <c r="U670" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V670" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W670" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="671" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A671" s="10">
+        <v>670</v>
+      </c>
+      <c r="B671" s="7">
+        <v>0</v>
+      </c>
+      <c r="C671" s="7">
+        <v>0</v>
+      </c>
+      <c r="D671" s="7">
+        <v>0</v>
+      </c>
+      <c r="E671" s="7">
+        <v>0</v>
+      </c>
+      <c r="F671" s="7">
+        <v>0</v>
+      </c>
+      <c r="G671" s="7">
+        <v>0</v>
+      </c>
+      <c r="H671" s="7">
+        <v>8.5853479922509202</v>
+      </c>
+      <c r="I671" s="7">
+        <v>0</v>
+      </c>
+      <c r="J671" s="7">
+        <v>0</v>
+      </c>
+      <c r="K671" s="7">
+        <v>0</v>
+      </c>
+      <c r="L671" s="7">
+        <v>0</v>
+      </c>
+      <c r="M671" s="7">
+        <v>11.9609121056319</v>
+      </c>
+      <c r="N671" s="7">
+        <v>0</v>
+      </c>
+      <c r="O671" s="7">
+        <v>0</v>
+      </c>
+      <c r="P671" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q671" s="7">
+        <v>2.4202204943808101</v>
+      </c>
+      <c r="R671" s="7">
+        <v>0</v>
+      </c>
+      <c r="S671" s="7">
+        <v>3.78339063344621</v>
+      </c>
+      <c r="T671" t="b">
+        <v>0</v>
+      </c>
+      <c r="U671" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V671" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W671" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="672" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A672" s="10">
+        <v>671</v>
+      </c>
+      <c r="B672" s="7">
+        <v>8.8338836301705808</v>
+      </c>
+      <c r="C672" s="7">
+        <v>0</v>
+      </c>
+      <c r="D672" s="7">
+        <v>0</v>
+      </c>
+      <c r="E672" s="7">
+        <v>0</v>
+      </c>
+      <c r="F672" s="7">
+        <v>0</v>
+      </c>
+      <c r="G672" s="7">
+        <v>0</v>
+      </c>
+      <c r="H672" s="7">
+        <v>9.4643044140020791</v>
+      </c>
+      <c r="I672" s="7">
+        <v>0</v>
+      </c>
+      <c r="J672" s="7">
+        <v>0</v>
+      </c>
+      <c r="K672" s="7">
+        <v>0</v>
+      </c>
+      <c r="L672" s="7">
+        <v>0</v>
+      </c>
+      <c r="M672" s="7">
+        <v>0</v>
+      </c>
+      <c r="N672" s="7">
+        <v>0</v>
+      </c>
+      <c r="O672" s="7">
+        <v>0</v>
+      </c>
+      <c r="P672" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q672" s="7">
+        <v>1.3387699688339001</v>
+      </c>
+      <c r="R672" s="7">
+        <v>0</v>
+      </c>
+      <c r="S672" s="7">
+        <v>4.1661722164455703</v>
+      </c>
+      <c r="T672" t="b">
+        <v>0</v>
+      </c>
+      <c r="U672" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V672" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W672" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="673" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A673" s="10">
+        <v>672</v>
+      </c>
+      <c r="B673" s="7">
+        <v>0</v>
+      </c>
+      <c r="C673" s="7">
+        <v>0</v>
+      </c>
+      <c r="D673" s="7">
+        <v>0</v>
+      </c>
+      <c r="E673" s="7">
+        <v>0</v>
+      </c>
+      <c r="F673" s="7">
+        <v>0</v>
+      </c>
+      <c r="G673" s="7">
+        <v>0</v>
+      </c>
+      <c r="H673" s="7">
+        <v>9.8037246913882896</v>
+      </c>
+      <c r="I673" s="7">
+        <v>0</v>
+      </c>
+      <c r="J673" s="7">
+        <v>0</v>
+      </c>
+      <c r="K673" s="7">
+        <v>0</v>
+      </c>
+      <c r="L673" s="7">
+        <v>12.1599090493426</v>
+      </c>
+      <c r="M673" s="7">
+        <v>0</v>
+      </c>
+      <c r="N673" s="7">
+        <v>0</v>
+      </c>
+      <c r="O673" s="7">
+        <v>0</v>
+      </c>
+      <c r="P673" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q673" s="7">
+        <v>1.54483824799364</v>
+      </c>
+      <c r="R673" s="7">
+        <v>0</v>
+      </c>
+      <c r="S673" s="7">
+        <v>3.7849761194901101</v>
+      </c>
+      <c r="T673" t="b">
+        <v>1</v>
+      </c>
+      <c r="U673" s="2">
+        <v>44</v>
+      </c>
+      <c r="V673" s="2">
+        <v>4179</v>
+      </c>
+      <c r="W673" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="674" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A674" s="10">
+        <v>673</v>
+      </c>
+      <c r="B674" s="7">
+        <v>0</v>
+      </c>
+      <c r="C674" s="7">
+        <v>9.6153621555513098</v>
+      </c>
+      <c r="D674" s="7">
+        <v>0</v>
+      </c>
+      <c r="E674" s="7">
+        <v>0</v>
+      </c>
+      <c r="F674" s="7">
+        <v>0</v>
+      </c>
+      <c r="G674" s="7">
+        <v>0</v>
+      </c>
+      <c r="H674" s="7">
+        <v>8.2350376941512398</v>
+      </c>
+      <c r="I674" s="7">
+        <v>0</v>
+      </c>
+      <c r="J674" s="7">
+        <v>0</v>
+      </c>
+      <c r="K674" s="7">
+        <v>0</v>
+      </c>
+      <c r="L674" s="7">
+        <v>0</v>
+      </c>
+      <c r="M674" s="7">
+        <v>0</v>
+      </c>
+      <c r="N674" s="7">
+        <v>0</v>
+      </c>
+      <c r="O674" s="7">
+        <v>0</v>
+      </c>
+      <c r="P674" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q674" s="7">
+        <v>1.0766630605460099</v>
+      </c>
+      <c r="R674" s="7">
+        <v>0</v>
+      </c>
+      <c r="S674" s="7">
+        <v>1.7615854478459401</v>
+      </c>
+      <c r="T674" t="b">
+        <v>1</v>
+      </c>
+      <c r="U674" s="2">
+        <v>15</v>
+      </c>
+      <c r="V674" s="2">
+        <v>3</v>
+      </c>
+      <c r="W674" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="675" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A675" s="10">
+        <v>674</v>
+      </c>
+      <c r="B675" s="7">
+        <v>5.3410633666371199</v>
+      </c>
+      <c r="C675" s="7">
+        <v>0</v>
+      </c>
+      <c r="D675" s="7">
+        <v>0</v>
+      </c>
+      <c r="E675" s="7">
+        <v>0</v>
+      </c>
+      <c r="F675" s="7">
+        <v>0</v>
+      </c>
+      <c r="G675" s="7">
+        <v>0</v>
+      </c>
+      <c r="H675" s="7">
+        <v>0</v>
+      </c>
+      <c r="I675" s="7">
+        <v>0</v>
+      </c>
+      <c r="J675" s="7">
+        <v>0</v>
+      </c>
+      <c r="K675" s="7">
+        <v>0</v>
+      </c>
+      <c r="L675" s="7">
+        <v>11.608783839779999</v>
+      </c>
+      <c r="M675" s="7">
+        <v>0</v>
+      </c>
+      <c r="N675" s="7">
+        <v>0</v>
+      </c>
+      <c r="O675" s="7">
+        <v>0</v>
+      </c>
+      <c r="P675" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q675" s="7">
+        <v>1.2056258987788999</v>
+      </c>
+      <c r="R675" s="7">
+        <v>0</v>
+      </c>
+      <c r="S675" s="7">
+        <v>3.44683714009332</v>
+      </c>
+      <c r="T675" t="b">
+        <v>0</v>
+      </c>
+      <c r="U675" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V675" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W675" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="676" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A676" s="10">
+        <v>675</v>
+      </c>
+      <c r="B676" s="7">
+        <v>11.763462216072201</v>
+      </c>
+      <c r="C676" s="7">
+        <v>0</v>
+      </c>
+      <c r="D676" s="7">
+        <v>0</v>
+      </c>
+      <c r="E676" s="7">
+        <v>0</v>
+      </c>
+      <c r="F676" s="7">
+        <v>0</v>
+      </c>
+      <c r="G676" s="7">
+        <v>0</v>
+      </c>
+      <c r="H676" s="7">
+        <v>0</v>
+      </c>
+      <c r="I676" s="7">
+        <v>10.5664503178229</v>
+      </c>
+      <c r="J676" s="7">
+        <v>0</v>
+      </c>
+      <c r="K676" s="7">
+        <v>0</v>
+      </c>
+      <c r="L676" s="7">
+        <v>0</v>
+      </c>
+      <c r="M676" s="7">
+        <v>0</v>
+      </c>
+      <c r="N676" s="7">
+        <v>0</v>
+      </c>
+      <c r="O676" s="7">
+        <v>0</v>
+      </c>
+      <c r="P676" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q676" s="7">
+        <v>1.54368611148282</v>
+      </c>
+      <c r="R676" s="7">
+        <v>0</v>
+      </c>
+      <c r="S676" s="7">
+        <v>4.2878783177484401</v>
+      </c>
+      <c r="T676" t="b">
+        <v>0</v>
+      </c>
+      <c r="U676" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V676" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W676" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="677" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A677" s="10">
+        <v>676</v>
+      </c>
+      <c r="B677" s="7">
+        <v>12.989624797195701</v>
+      </c>
+      <c r="C677" s="7">
+        <v>0</v>
+      </c>
+      <c r="D677" s="7">
+        <v>0</v>
+      </c>
+      <c r="E677" s="7">
+        <v>0</v>
+      </c>
+      <c r="F677" s="7">
+        <v>0</v>
+      </c>
+      <c r="G677" s="7">
+        <v>0</v>
+      </c>
+      <c r="H677" s="7">
+        <v>0</v>
+      </c>
+      <c r="I677" s="7">
+        <v>0</v>
+      </c>
+      <c r="J677" s="7">
+        <v>0</v>
+      </c>
+      <c r="K677" s="7">
+        <v>11.436252505180599</v>
+      </c>
+      <c r="L677" s="7">
+        <v>0</v>
+      </c>
+      <c r="M677" s="7">
+        <v>0</v>
+      </c>
+      <c r="N677" s="7">
+        <v>0</v>
+      </c>
+      <c r="O677" s="7">
+        <v>0</v>
+      </c>
+      <c r="P677" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q677" s="7">
+        <v>1.63089463803838</v>
+      </c>
+      <c r="R677" s="7">
+        <v>0</v>
+      </c>
+      <c r="S677" s="7">
+        <v>4.6220870459206003</v>
+      </c>
+      <c r="T677" t="b">
+        <v>0</v>
+      </c>
+      <c r="U677" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V677" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W677" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="678" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A678" s="10">
+        <v>677</v>
+      </c>
+      <c r="B678" s="7">
+        <v>0</v>
+      </c>
+      <c r="C678" s="7">
+        <v>0</v>
+      </c>
+      <c r="D678" s="7">
+        <v>0</v>
+      </c>
+      <c r="E678" s="7">
+        <v>0</v>
+      </c>
+      <c r="F678" s="7">
+        <v>12.023831996190401</v>
+      </c>
+      <c r="G678" s="7">
+        <v>0</v>
+      </c>
+      <c r="H678" s="7">
+        <v>0</v>
+      </c>
+      <c r="I678" s="7">
+        <v>8.4146115331331401</v>
+      </c>
+      <c r="J678" s="7">
+        <v>0</v>
+      </c>
+      <c r="K678" s="7">
+        <v>0</v>
+      </c>
+      <c r="L678" s="7">
+        <v>0</v>
+      </c>
+      <c r="M678" s="7">
+        <v>0</v>
+      </c>
+      <c r="N678" s="7">
+        <v>0</v>
+      </c>
+      <c r="O678" s="7">
+        <v>0</v>
+      </c>
+      <c r="P678" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q678" s="7">
+        <v>2.1115418897599501</v>
+      </c>
+      <c r="R678" s="7">
+        <v>0</v>
+      </c>
+      <c r="S678" s="7">
+        <v>2.0166272805880201</v>
+      </c>
+      <c r="T678" t="b">
+        <v>0</v>
+      </c>
+      <c r="U678" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V678" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W678" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="679" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A679" s="10">
+        <v>678</v>
+      </c>
+      <c r="B679" s="7">
+        <v>0</v>
+      </c>
+      <c r="C679" s="7">
+        <v>0</v>
+      </c>
+      <c r="D679" s="7">
+        <v>7.4687093894207202</v>
+      </c>
+      <c r="E679" s="7">
+        <v>0</v>
+      </c>
+      <c r="F679" s="7">
+        <v>0</v>
+      </c>
+      <c r="G679" s="7">
+        <v>0</v>
+      </c>
+      <c r="H679" s="7">
+        <v>11.441126674069301</v>
+      </c>
+      <c r="I679" s="7">
+        <v>0</v>
+      </c>
+      <c r="J679" s="7">
+        <v>0</v>
+      </c>
+      <c r="K679" s="7">
+        <v>0</v>
+      </c>
+      <c r="L679" s="7">
+        <v>0</v>
+      </c>
+      <c r="M679" s="7">
+        <v>0</v>
+      </c>
+      <c r="N679" s="7">
+        <v>0</v>
+      </c>
+      <c r="O679" s="7">
+        <v>0</v>
+      </c>
+      <c r="P679" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q679" s="7">
+        <v>2.2898393184743702</v>
+      </c>
+      <c r="R679" s="7">
+        <v>0</v>
+      </c>
+      <c r="S679" s="7">
+        <v>4.14087682922366</v>
+      </c>
+      <c r="T679" t="b">
+        <v>0</v>
+      </c>
+      <c r="U679" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V679" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W679" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="680" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A680" s="10">
+        <v>679</v>
+      </c>
+      <c r="B680" s="7">
+        <v>5.0897344542242102</v>
+      </c>
+      <c r="C680" s="7">
+        <v>0</v>
+      </c>
+      <c r="D680" s="7">
+        <v>0</v>
+      </c>
+      <c r="E680" s="7">
+        <v>8.0544619309272107</v>
+      </c>
+      <c r="F680" s="7">
+        <v>0</v>
+      </c>
+      <c r="G680" s="7">
+        <v>0</v>
+      </c>
+      <c r="H680" s="7">
+        <v>0</v>
+      </c>
+      <c r="I680" s="7">
+        <v>0</v>
+      </c>
+      <c r="J680" s="7">
+        <v>0</v>
+      </c>
+      <c r="K680" s="7">
+        <v>0</v>
+      </c>
+      <c r="L680" s="7">
+        <v>0</v>
+      </c>
+      <c r="M680" s="7">
+        <v>0</v>
+      </c>
+      <c r="N680" s="7">
+        <v>0</v>
+      </c>
+      <c r="O680" s="7">
+        <v>0</v>
+      </c>
+      <c r="P680" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q680" s="7">
+        <v>2.3590362237854499</v>
+      </c>
+      <c r="R680" s="7">
+        <v>0</v>
+      </c>
+      <c r="S680" s="7">
+        <v>5.1090137513992602</v>
+      </c>
+      <c r="T680" t="b">
+        <v>0</v>
+      </c>
+      <c r="U680" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V680" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W680" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="681" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A681" s="10">
+        <v>680</v>
+      </c>
+      <c r="B681" s="7">
+        <v>0</v>
+      </c>
+      <c r="C681" s="7">
+        <v>7.4165843567781096</v>
+      </c>
+      <c r="D681" s="7">
+        <v>0</v>
+      </c>
+      <c r="E681" s="7">
+        <v>0</v>
+      </c>
+      <c r="F681" s="7">
+        <v>0</v>
+      </c>
+      <c r="G681" s="7">
+        <v>0</v>
+      </c>
+      <c r="H681" s="7">
+        <v>0</v>
+      </c>
+      <c r="I681" s="7">
+        <v>0</v>
+      </c>
+      <c r="J681" s="7">
+        <v>9.9181002159206599</v>
+      </c>
+      <c r="K681" s="7">
+        <v>0</v>
+      </c>
+      <c r="L681" s="7">
+        <v>0</v>
+      </c>
+      <c r="M681" s="7">
+        <v>0</v>
+      </c>
+      <c r="N681" s="7">
+        <v>0</v>
+      </c>
+      <c r="O681" s="7">
+        <v>0</v>
+      </c>
+      <c r="P681" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q681" s="7">
+        <v>2.1459566610679901</v>
+      </c>
+      <c r="R681" s="7">
+        <v>0</v>
+      </c>
+      <c r="S681" s="7">
+        <v>4.3783940165948101</v>
+      </c>
+      <c r="T681" t="b">
+        <v>0</v>
+      </c>
+      <c r="U681" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V681" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W681" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="682" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A682" s="10">
+        <v>681</v>
+      </c>
+      <c r="B682" s="7">
+        <v>0</v>
+      </c>
+      <c r="C682" s="7">
+        <v>0</v>
+      </c>
+      <c r="D682" s="7">
+        <v>0</v>
+      </c>
+      <c r="E682" s="7">
+        <v>0</v>
+      </c>
+      <c r="F682" s="7">
+        <v>0</v>
+      </c>
+      <c r="G682" s="7">
+        <v>0</v>
+      </c>
+      <c r="H682" s="7">
+        <v>0</v>
+      </c>
+      <c r="I682" s="7">
+        <v>0</v>
+      </c>
+      <c r="J682" s="7">
+        <v>0</v>
+      </c>
+      <c r="K682" s="7">
+        <v>11.9028015445906</v>
+      </c>
+      <c r="L682" s="7">
+        <v>12.3331775395423</v>
+      </c>
+      <c r="M682" s="7">
+        <v>0</v>
+      </c>
+      <c r="N682" s="7">
+        <v>0</v>
+      </c>
+      <c r="O682" s="7">
+        <v>0</v>
+      </c>
+      <c r="P682" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q682" s="7">
+        <v>2.3648520775234201</v>
+      </c>
+      <c r="R682" s="7">
+        <v>0</v>
+      </c>
+      <c r="S682" s="7">
+        <v>4.8897409952748703</v>
+      </c>
+      <c r="T682" t="b">
+        <v>0</v>
+      </c>
+      <c r="U682" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V682" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W682" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="683" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A683" s="10">
+        <v>682</v>
+      </c>
+      <c r="B683" s="7">
+        <v>0</v>
+      </c>
+      <c r="C683" s="7">
+        <v>0</v>
+      </c>
+      <c r="D683" s="7">
+        <v>10.2786730579992</v>
+      </c>
+      <c r="E683" s="7">
+        <v>0</v>
+      </c>
+      <c r="F683" s="7">
+        <v>0</v>
+      </c>
+      <c r="G683" s="7">
+        <v>0</v>
+      </c>
+      <c r="H683" s="7">
+        <v>0</v>
+      </c>
+      <c r="I683" s="7">
+        <v>0</v>
+      </c>
+      <c r="J683" s="7">
+        <v>0</v>
+      </c>
+      <c r="K683" s="7">
+        <v>11.7694430593593</v>
+      </c>
+      <c r="L683" s="7">
+        <v>0</v>
+      </c>
+      <c r="M683" s="7">
+        <v>0</v>
+      </c>
+      <c r="N683" s="7">
+        <v>0</v>
+      </c>
+      <c r="O683" s="7">
+        <v>0</v>
+      </c>
+      <c r="P683" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q683" s="7">
+        <v>1.8487702874951399</v>
+      </c>
+      <c r="R683" s="7">
+        <v>0</v>
+      </c>
+      <c r="S683" s="7">
+        <v>4.3978694521075496</v>
+      </c>
+      <c r="T683" t="b">
+        <v>0</v>
+      </c>
+      <c r="U683" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V683" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W683" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="684" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A684" s="10">
+        <v>683</v>
+      </c>
+      <c r="B684" s="7">
+        <v>0</v>
+      </c>
+      <c r="C684" s="7">
+        <v>8.79446228044403</v>
+      </c>
+      <c r="D684" s="7">
+        <v>0</v>
+      </c>
+      <c r="E684" s="7">
+        <v>0</v>
+      </c>
+      <c r="F684" s="7">
+        <v>0</v>
+      </c>
+      <c r="G684" s="7">
+        <v>8.8228378262978193</v>
+      </c>
+      <c r="H684" s="7">
+        <v>0</v>
+      </c>
+      <c r="I684" s="7">
+        <v>0</v>
+      </c>
+      <c r="J684" s="7">
+        <v>0</v>
+      </c>
+      <c r="K684" s="7">
+        <v>0</v>
+      </c>
+      <c r="L684" s="7">
+        <v>0</v>
+      </c>
+      <c r="M684" s="7">
+        <v>0</v>
+      </c>
+      <c r="N684" s="7">
+        <v>0</v>
+      </c>
+      <c r="O684" s="7">
+        <v>0</v>
+      </c>
+      <c r="P684" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q684" s="7">
+        <v>2.6149533204813702</v>
+      </c>
+      <c r="R684" s="7">
+        <v>0</v>
+      </c>
+      <c r="S684" s="7">
+        <v>4.4520252977325798</v>
+      </c>
+      <c r="T684" t="b">
+        <v>0</v>
+      </c>
+      <c r="U684" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V684" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W684" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="685" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A685" s="10">
+        <v>684</v>
+      </c>
+      <c r="B685" s="7">
+        <v>0</v>
+      </c>
+      <c r="C685" s="7">
+        <v>0</v>
+      </c>
+      <c r="D685" s="7">
+        <v>7.9752286295160504</v>
+      </c>
+      <c r="E685" s="7">
+        <v>0</v>
+      </c>
+      <c r="F685" s="7">
+        <v>0</v>
+      </c>
+      <c r="G685" s="7">
+        <v>0</v>
+      </c>
+      <c r="H685" s="7">
+        <v>0</v>
+      </c>
+      <c r="I685" s="7">
+        <v>0</v>
+      </c>
+      <c r="J685" s="7">
+        <v>0</v>
+      </c>
+      <c r="K685" s="7">
+        <v>0</v>
+      </c>
+      <c r="L685" s="7">
+        <v>12.415248096867099</v>
+      </c>
+      <c r="M685" s="7">
+        <v>0</v>
+      </c>
+      <c r="N685" s="7">
+        <v>0</v>
+      </c>
+      <c r="O685" s="7">
+        <v>0</v>
+      </c>
+      <c r="P685" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q685" s="7">
+        <v>2.9215797111312698</v>
+      </c>
+      <c r="R685" s="7">
+        <v>0</v>
+      </c>
+      <c r="S685" s="7">
+        <v>1.8027807916512</v>
+      </c>
+      <c r="T685" t="b">
+        <v>0</v>
+      </c>
+      <c r="U685" s="2" t="str">
+        <f t="shared" si="37"/>
+        <v>NA</v>
+      </c>
+      <c r="V685" s="2" t="str">
+        <f t="shared" si="38"/>
+        <v>NA</v>
+      </c>
+      <c r="W685" s="12" t="str">
+        <f t="shared" si="39"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="686" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A686" s="10">
+        <v>685</v>
+      </c>
+      <c r="B686" s="7">
+        <v>0</v>
+      </c>
+      <c r="C686" s="7">
+        <v>8.3762109618108003</v>
+      </c>
+      <c r="D686" s="7">
+        <v>0</v>
+      </c>
+      <c r="E686" s="7">
+        <v>0</v>
+      </c>
+      <c r="F686" s="7">
+        <v>0</v>
+      </c>
+      <c r="G686" s="7">
+        <v>0</v>
+      </c>
+      <c r="H686" s="7">
+        <v>0</v>
+      </c>
+      <c r="I686" s="7">
+        <v>0</v>
+      </c>
+      <c r="J686" s="7">
+        <v>0</v>
+      </c>
+      <c r="K686" s="7">
+        <v>0</v>
+      </c>
+      <c r="L686" s="7">
+        <v>10.904802812978099</v>
+      </c>
+      <c r="M686" s="7">
+        <v>0</v>
+      </c>
+      <c r="N686" s="7">
+        <v>0</v>
+      </c>
+      <c r="O686" s="7">
+        <v>0</v>
+      </c>
+      <c r="P686" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q686" s="7">
+        <v>1.0882261879281501</v>
+      </c>
+      <c r="R686" s="7">
+        <v>0</v>
+      </c>
+      <c r="S686" s="7">
+        <v>2.6448028871164602</v>
+      </c>
+      <c r="T686" t="b">
+        <v>1</v>
+      </c>
+      <c r="U686" s="2">
+        <v>3881</v>
+      </c>
+      <c r="V686" s="2">
+        <v>5</v>
+      </c>
+      <c r="W686" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="687" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A687" s="10">
+        <v>686</v>
+      </c>
+      <c r="B687" s="7">
+        <v>0</v>
+      </c>
+      <c r="C687" s="7">
+        <v>0</v>
+      </c>
+      <c r="D687" s="7">
+        <v>0</v>
+      </c>
+      <c r="E687" s="7">
+        <v>0</v>
+      </c>
+      <c r="F687" s="7">
+        <v>0</v>
+      </c>
+      <c r="G687" s="7">
+        <v>0</v>
+      </c>
+      <c r="H687" s="7">
+        <v>0</v>
+      </c>
+      <c r="I687" s="7">
+        <v>0</v>
+      </c>
+      <c r="J687" s="7">
+        <v>11.073506907632</v>
+      </c>
+      <c r="K687" s="7">
+        <v>10.3390295257028</v>
+      </c>
+      <c r="L687" s="7">
+        <v>0</v>
+      </c>
+      <c r="M687" s="7">
+        <v>0</v>
+      </c>
+      <c r="N687" s="7">
+        <v>0</v>
+      </c>
+      <c r="O687" s="7">
+        <v>0</v>
+      </c>
+      <c r="P687" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q687" s="7">
+        <v>1.2752029915056</v>
+      </c>
+      <c r="R687" s="7">
+        <v>0</v>
+      </c>
+      <c r="S687" s="7">
+        <v>3.3066310128573999</v>
+      </c>
+      <c r="T687" t="b">
+        <v>0</v>
+      </c>
+      <c r="U687" s="2" t="str">
+        <f t="shared" ref="U686:U691" si="40">IF(T687=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V687" s="2" t="str">
+        <f t="shared" ref="V686:V691" si="41">IF(T687=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W687" s="12" t="str">
+        <f t="shared" ref="W686:W691" si="42">IF(T687=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="688" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A688" s="10">
+        <v>687</v>
+      </c>
+      <c r="B688" s="7">
+        <v>0</v>
+      </c>
+      <c r="C688" s="7">
+        <v>0</v>
+      </c>
+      <c r="D688" s="7">
+        <v>0</v>
+      </c>
+      <c r="E688" s="7">
+        <v>0</v>
+      </c>
+      <c r="F688" s="7">
+        <v>0</v>
+      </c>
+      <c r="G688" s="7">
+        <v>0</v>
+      </c>
+      <c r="H688" s="7">
+        <v>0</v>
+      </c>
+      <c r="I688" s="7">
+        <v>0</v>
+      </c>
+      <c r="J688" s="7">
+        <v>0</v>
+      </c>
+      <c r="K688" s="7">
+        <v>0</v>
+      </c>
+      <c r="L688" s="7">
+        <v>12.050983878986001</v>
+      </c>
+      <c r="M688" s="7">
+        <v>9.2313021251975798</v>
+      </c>
+      <c r="N688" s="7">
+        <v>0</v>
+      </c>
+      <c r="O688" s="7">
+        <v>0</v>
+      </c>
+      <c r="P688" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q688" s="7">
+        <v>1.85361525231415</v>
+      </c>
+      <c r="R688" s="7">
+        <v>0</v>
+      </c>
+      <c r="S688" s="7">
+        <v>2.4499525989030899</v>
+      </c>
+      <c r="T688" t="b">
+        <v>0</v>
+      </c>
+      <c r="U688" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V688" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W688" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="689" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A689" s="10">
+        <v>688</v>
+      </c>
+      <c r="B689" s="7">
+        <v>0</v>
+      </c>
+      <c r="C689" s="7">
+        <v>0</v>
+      </c>
+      <c r="D689" s="7">
+        <v>6.2537276929599397</v>
+      </c>
+      <c r="E689" s="7">
+        <v>0</v>
+      </c>
+      <c r="F689" s="7">
+        <v>0</v>
+      </c>
+      <c r="G689" s="7">
+        <v>11.307728148456</v>
+      </c>
+      <c r="H689" s="7">
+        <v>0</v>
+      </c>
+      <c r="I689" s="7">
+        <v>0</v>
+      </c>
+      <c r="J689" s="7">
+        <v>0</v>
+      </c>
+      <c r="K689" s="7">
+        <v>0</v>
+      </c>
+      <c r="L689" s="7">
+        <v>0</v>
+      </c>
+      <c r="M689" s="7">
+        <v>0</v>
+      </c>
+      <c r="N689" s="7">
+        <v>0</v>
+      </c>
+      <c r="O689" s="7">
+        <v>0</v>
+      </c>
+      <c r="P689" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q689" s="7">
+        <v>2.3204857178107798</v>
+      </c>
+      <c r="R689" s="7">
+        <v>0</v>
+      </c>
+      <c r="S689" s="7">
+        <v>2.3267135377726902</v>
+      </c>
+      <c r="T689" t="b">
+        <v>1</v>
+      </c>
+      <c r="U689" s="2">
+        <v>20</v>
+      </c>
+      <c r="V689" s="2">
+        <v>57</v>
+      </c>
+      <c r="W689" s="12" t="b">
+        <v>0</v>
+      </c>
+      <c r="X689" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="690" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A690" s="10">
+        <v>689</v>
+      </c>
+      <c r="B690" s="7">
+        <v>0</v>
+      </c>
+      <c r="C690" s="7">
+        <v>0</v>
+      </c>
+      <c r="D690" s="7">
+        <v>0</v>
+      </c>
+      <c r="E690" s="7">
+        <v>6.9039696390489702</v>
+      </c>
+      <c r="F690" s="7">
+        <v>0</v>
+      </c>
+      <c r="G690" s="7">
+        <v>0</v>
+      </c>
+      <c r="H690" s="7">
+        <v>9.9853118633255509</v>
+      </c>
+      <c r="I690" s="7">
+        <v>0</v>
+      </c>
+      <c r="J690" s="7">
+        <v>0</v>
+      </c>
+      <c r="K690" s="7">
+        <v>0</v>
+      </c>
+      <c r="L690" s="7">
+        <v>0</v>
+      </c>
+      <c r="M690" s="7">
+        <v>0</v>
+      </c>
+      <c r="N690" s="7">
+        <v>0</v>
+      </c>
+      <c r="O690" s="7">
+        <v>0</v>
+      </c>
+      <c r="P690" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q690" s="7">
+        <v>1.86323034367833</v>
+      </c>
+      <c r="R690" s="7">
+        <v>0</v>
+      </c>
+      <c r="S690" s="7">
+        <v>2.8299063015544501</v>
+      </c>
+      <c r="T690" t="b">
+        <v>0</v>
+      </c>
+      <c r="U690" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V690" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W690" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="691" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A691" s="10">
+        <v>690</v>
+      </c>
+      <c r="B691" s="7">
+        <v>0</v>
+      </c>
+      <c r="C691" s="7">
+        <v>0</v>
+      </c>
+      <c r="D691" s="7">
+        <v>0</v>
+      </c>
+      <c r="E691" s="7">
+        <v>12.3659948326028</v>
+      </c>
+      <c r="F691" s="7">
+        <v>0</v>
+      </c>
+      <c r="G691" s="7">
+        <v>0</v>
+      </c>
+      <c r="H691" s="7">
+        <v>0</v>
+      </c>
+      <c r="I691" s="7">
+        <v>0</v>
+      </c>
+      <c r="J691" s="7">
+        <v>0</v>
+      </c>
+      <c r="K691" s="7">
+        <v>0</v>
+      </c>
+      <c r="L691" s="7">
+        <v>0</v>
+      </c>
+      <c r="M691" s="7">
+        <v>12.93154862471</v>
+      </c>
+      <c r="N691" s="7">
+        <v>0</v>
+      </c>
+      <c r="O691" s="7">
+        <v>0</v>
+      </c>
+      <c r="P691" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q691" s="7">
+        <v>2.4822341523185099</v>
+      </c>
+      <c r="R691" s="7">
+        <v>0</v>
+      </c>
+      <c r="S691" s="7">
+        <v>2.5884586339966602</v>
+      </c>
+      <c r="T691" t="b">
+        <v>0</v>
+      </c>
+      <c r="U691" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V691" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W691" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W667">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="A1:W691">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U580">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U569">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -59655,7 +61425,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S714
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2920553D-46D8-6042-88FA-63B6275BCE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0742FC6-8DA7-D44F-B593-EE4CCC01853F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -407,16 +407,6 @@
   <dxfs count="7">
     <dxf>
       <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
@@ -462,6 +452,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -785,11 +785,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:X691"/>
+  <dimension ref="A1:X715"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A657" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D696" sqref="D696"/>
+    <sheetView tabSelected="1" topLeftCell="A660" zoomScale="119" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA26" sqref="AA26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50951,15 +50951,15 @@
         <v>0</v>
       </c>
       <c r="U687" s="2" t="str">
-        <f t="shared" ref="U686:U691" si="40">IF(T687=FALSE, "NA", "")</f>
+        <f t="shared" ref="U687:U715" si="40">IF(T687=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V687" s="2" t="str">
-        <f t="shared" ref="V686:V691" si="41">IF(T687=FALSE, "NA", "")</f>
+        <f t="shared" ref="V687:V715" si="41">IF(T687=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W687" s="12" t="str">
-        <f t="shared" ref="W686:W691" si="42">IF(T687=FALSE, "NA", "")</f>
+        <f t="shared" ref="W687:W715" si="42">IF(T687=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -51259,19 +51259,1768 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="692" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A692" s="10">
+        <v>691</v>
+      </c>
+      <c r="B692" s="7">
+        <v>0</v>
+      </c>
+      <c r="C692" s="7">
+        <v>0</v>
+      </c>
+      <c r="D692" s="7">
+        <v>0</v>
+      </c>
+      <c r="E692" s="7">
+        <v>0</v>
+      </c>
+      <c r="F692" s="7">
+        <v>0</v>
+      </c>
+      <c r="G692" s="7">
+        <v>0</v>
+      </c>
+      <c r="H692" s="7">
+        <v>0</v>
+      </c>
+      <c r="I692" s="7">
+        <v>0</v>
+      </c>
+      <c r="J692" s="7">
+        <v>12.995367738626999</v>
+      </c>
+      <c r="K692" s="7">
+        <v>0</v>
+      </c>
+      <c r="L692" s="7">
+        <v>0</v>
+      </c>
+      <c r="M692" s="7">
+        <v>9.8223246109465006</v>
+      </c>
+      <c r="N692" s="7">
+        <v>0</v>
+      </c>
+      <c r="O692" s="7">
+        <v>0</v>
+      </c>
+      <c r="P692" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q692" s="7">
+        <v>2.21892877187996</v>
+      </c>
+      <c r="R692" s="7">
+        <v>0</v>
+      </c>
+      <c r="S692" s="7">
+        <v>3.3021262445113102</v>
+      </c>
+      <c r="T692" t="b">
+        <v>0</v>
+      </c>
+      <c r="U692" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V692" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W692" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="693" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A693" s="10">
+        <v>692</v>
+      </c>
+      <c r="B693" s="7">
+        <v>0</v>
+      </c>
+      <c r="C693" s="7">
+        <v>0</v>
+      </c>
+      <c r="D693" s="7">
+        <v>12.1675061320603</v>
+      </c>
+      <c r="E693" s="7">
+        <v>8.2278070100054794</v>
+      </c>
+      <c r="F693" s="7">
+        <v>0</v>
+      </c>
+      <c r="G693" s="7">
+        <v>0</v>
+      </c>
+      <c r="H693" s="7">
+        <v>0</v>
+      </c>
+      <c r="I693" s="7">
+        <v>0</v>
+      </c>
+      <c r="J693" s="7">
+        <v>0</v>
+      </c>
+      <c r="K693" s="7">
+        <v>0</v>
+      </c>
+      <c r="L693" s="7">
+        <v>0</v>
+      </c>
+      <c r="M693" s="7">
+        <v>0</v>
+      </c>
+      <c r="N693" s="7">
+        <v>0</v>
+      </c>
+      <c r="O693" s="7">
+        <v>0</v>
+      </c>
+      <c r="P693" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q693" s="7">
+        <v>2.61678806009499</v>
+      </c>
+      <c r="R693" s="7">
+        <v>0</v>
+      </c>
+      <c r="S693" s="7">
+        <v>2.03982909947658</v>
+      </c>
+      <c r="T693" t="b">
+        <v>1</v>
+      </c>
+      <c r="U693" s="2">
+        <v>14</v>
+      </c>
+      <c r="V693" s="2">
+        <v>6</v>
+      </c>
+      <c r="W693" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="694" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A694" s="10">
+        <v>693</v>
+      </c>
+      <c r="B694" s="7">
+        <v>0</v>
+      </c>
+      <c r="C694" s="7">
+        <v>0</v>
+      </c>
+      <c r="D694" s="7">
+        <v>8.7997539859158103</v>
+      </c>
+      <c r="E694" s="7">
+        <v>0</v>
+      </c>
+      <c r="F694" s="7">
+        <v>0</v>
+      </c>
+      <c r="G694" s="7">
+        <v>0</v>
+      </c>
+      <c r="H694" s="7">
+        <v>0</v>
+      </c>
+      <c r="I694" s="7">
+        <v>11.0264123831617</v>
+      </c>
+      <c r="J694" s="7">
+        <v>0</v>
+      </c>
+      <c r="K694" s="7">
+        <v>0</v>
+      </c>
+      <c r="L694" s="7">
+        <v>0</v>
+      </c>
+      <c r="M694" s="7">
+        <v>0</v>
+      </c>
+      <c r="N694" s="7">
+        <v>0</v>
+      </c>
+      <c r="O694" s="7">
+        <v>0</v>
+      </c>
+      <c r="P694" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q694" s="7">
+        <v>2.40355403658265</v>
+      </c>
+      <c r="R694" s="7">
+        <v>0</v>
+      </c>
+      <c r="S694" s="7">
+        <v>3.2905062981523301</v>
+      </c>
+      <c r="T694" t="b">
+        <v>1</v>
+      </c>
+      <c r="U694" s="2">
+        <v>20</v>
+      </c>
+      <c r="V694" s="2">
+        <v>324</v>
+      </c>
+      <c r="W694" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="695" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A695" s="10">
+        <v>694</v>
+      </c>
+      <c r="B695" s="7">
+        <v>0</v>
+      </c>
+      <c r="C695" s="7">
+        <v>0</v>
+      </c>
+      <c r="D695" s="7">
+        <v>0</v>
+      </c>
+      <c r="E695" s="7">
+        <v>0</v>
+      </c>
+      <c r="F695" s="7">
+        <v>0</v>
+      </c>
+      <c r="G695" s="7">
+        <v>8.8475239364473808</v>
+      </c>
+      <c r="H695" s="7">
+        <v>0</v>
+      </c>
+      <c r="I695" s="7">
+        <v>0</v>
+      </c>
+      <c r="J695" s="7">
+        <v>11.0677664897675</v>
+      </c>
+      <c r="K695" s="7">
+        <v>0</v>
+      </c>
+      <c r="L695" s="7">
+        <v>0</v>
+      </c>
+      <c r="M695" s="7">
+        <v>0</v>
+      </c>
+      <c r="N695" s="7">
+        <v>0</v>
+      </c>
+      <c r="O695" s="7">
+        <v>0</v>
+      </c>
+      <c r="P695" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q695" s="7">
+        <v>2.1580226412699601</v>
+      </c>
+      <c r="R695" s="7">
+        <v>0</v>
+      </c>
+      <c r="S695" s="7">
+        <v>4.7857687292434798</v>
+      </c>
+      <c r="T695" t="b">
+        <v>0</v>
+      </c>
+      <c r="U695" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V695" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W695" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="696" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A696" s="10">
+        <v>695</v>
+      </c>
+      <c r="B696" s="7">
+        <v>0</v>
+      </c>
+      <c r="C696" s="7">
+        <v>0</v>
+      </c>
+      <c r="D696" s="7">
+        <v>0</v>
+      </c>
+      <c r="E696" s="7">
+        <v>0</v>
+      </c>
+      <c r="F696" s="7">
+        <v>0</v>
+      </c>
+      <c r="G696" s="7">
+        <v>0</v>
+      </c>
+      <c r="H696" s="7">
+        <v>0</v>
+      </c>
+      <c r="I696" s="7">
+        <v>0</v>
+      </c>
+      <c r="J696" s="7">
+        <v>0</v>
+      </c>
+      <c r="K696" s="7">
+        <v>11.9165993069251</v>
+      </c>
+      <c r="L696" s="7">
+        <v>0</v>
+      </c>
+      <c r="M696" s="7">
+        <v>11.072667065117299</v>
+      </c>
+      <c r="N696" s="7">
+        <v>0</v>
+      </c>
+      <c r="O696" s="7">
+        <v>0</v>
+      </c>
+      <c r="P696" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q696" s="7">
+        <v>2.13694291368913</v>
+      </c>
+      <c r="R696" s="7">
+        <v>0</v>
+      </c>
+      <c r="S696" s="7">
+        <v>3.54431823516133</v>
+      </c>
+      <c r="T696" t="b">
+        <v>0</v>
+      </c>
+      <c r="U696" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V696" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W696" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="697" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A697" s="10">
+        <v>696</v>
+      </c>
+      <c r="B697" s="7">
+        <v>0</v>
+      </c>
+      <c r="C697" s="7">
+        <v>0</v>
+      </c>
+      <c r="D697" s="7">
+        <v>0</v>
+      </c>
+      <c r="E697" s="7">
+        <v>0</v>
+      </c>
+      <c r="F697" s="7">
+        <v>0</v>
+      </c>
+      <c r="G697" s="7">
+        <v>11.737378910374099</v>
+      </c>
+      <c r="H697" s="7">
+        <v>0</v>
+      </c>
+      <c r="I697" s="7">
+        <v>0</v>
+      </c>
+      <c r="J697" s="7">
+        <v>0</v>
+      </c>
+      <c r="K697" s="7">
+        <v>0</v>
+      </c>
+      <c r="L697" s="7">
+        <v>8.3589066595692199</v>
+      </c>
+      <c r="M697" s="7">
+        <v>0</v>
+      </c>
+      <c r="N697" s="7">
+        <v>0</v>
+      </c>
+      <c r="O697" s="7">
+        <v>0</v>
+      </c>
+      <c r="P697" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q697" s="7">
+        <v>1.50183952308679</v>
+      </c>
+      <c r="R697" s="7">
+        <v>0</v>
+      </c>
+      <c r="S697" s="7">
+        <v>2.4000341046907101</v>
+      </c>
+      <c r="T697" t="b">
+        <v>0</v>
+      </c>
+      <c r="U697" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V697" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W697" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="698" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A698" s="10">
+        <v>697</v>
+      </c>
+      <c r="B698" s="7">
+        <v>0</v>
+      </c>
+      <c r="C698" s="7">
+        <v>9.4617642846171908</v>
+      </c>
+      <c r="D698" s="7">
+        <v>0</v>
+      </c>
+      <c r="E698" s="7">
+        <v>0</v>
+      </c>
+      <c r="F698" s="7">
+        <v>0</v>
+      </c>
+      <c r="G698" s="7">
+        <v>0</v>
+      </c>
+      <c r="H698" s="7">
+        <v>0</v>
+      </c>
+      <c r="I698" s="7">
+        <v>0</v>
+      </c>
+      <c r="J698" s="7">
+        <v>0</v>
+      </c>
+      <c r="K698" s="7">
+        <v>0</v>
+      </c>
+      <c r="L698" s="7">
+        <v>0</v>
+      </c>
+      <c r="M698" s="7">
+        <v>10.009313123981499</v>
+      </c>
+      <c r="N698" s="7">
+        <v>0</v>
+      </c>
+      <c r="O698" s="7">
+        <v>0</v>
+      </c>
+      <c r="P698" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q698" s="7">
+        <v>1.9505173856470399</v>
+      </c>
+      <c r="R698" s="7">
+        <v>0</v>
+      </c>
+      <c r="S698" s="7">
+        <v>3.2542050984189999</v>
+      </c>
+      <c r="T698" t="b">
+        <v>0</v>
+      </c>
+      <c r="U698" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V698" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W698" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="699" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A699" s="10">
+        <v>698</v>
+      </c>
+      <c r="B699" s="7">
+        <v>0</v>
+      </c>
+      <c r="C699" s="7">
+        <v>0</v>
+      </c>
+      <c r="D699" s="7">
+        <v>0</v>
+      </c>
+      <c r="E699" s="7">
+        <v>11.0136200342757</v>
+      </c>
+      <c r="F699" s="7">
+        <v>0</v>
+      </c>
+      <c r="G699" s="7">
+        <v>0</v>
+      </c>
+      <c r="H699" s="7">
+        <v>0</v>
+      </c>
+      <c r="I699" s="7">
+        <v>6.1901220946670303</v>
+      </c>
+      <c r="J699" s="7">
+        <v>0</v>
+      </c>
+      <c r="K699" s="7">
+        <v>0</v>
+      </c>
+      <c r="L699" s="7">
+        <v>0</v>
+      </c>
+      <c r="M699" s="7">
+        <v>0</v>
+      </c>
+      <c r="N699" s="7">
+        <v>0</v>
+      </c>
+      <c r="O699" s="7">
+        <v>0</v>
+      </c>
+      <c r="P699" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q699" s="7">
+        <v>1.8544162576013099</v>
+      </c>
+      <c r="R699" s="7">
+        <v>0</v>
+      </c>
+      <c r="S699" s="7">
+        <v>4.9787045176905398</v>
+      </c>
+      <c r="T699" t="b">
+        <v>0</v>
+      </c>
+      <c r="U699" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V699" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W699" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="700" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A700" s="10">
+        <v>699</v>
+      </c>
+      <c r="B700" s="7">
+        <v>0</v>
+      </c>
+      <c r="C700" s="7">
+        <v>0</v>
+      </c>
+      <c r="D700" s="7">
+        <v>0</v>
+      </c>
+      <c r="E700" s="7">
+        <v>0</v>
+      </c>
+      <c r="F700" s="7">
+        <v>0</v>
+      </c>
+      <c r="G700" s="7">
+        <v>0</v>
+      </c>
+      <c r="H700" s="7">
+        <v>8.7840578530551792</v>
+      </c>
+      <c r="I700" s="7">
+        <v>11.503865333637901</v>
+      </c>
+      <c r="J700" s="7">
+        <v>0</v>
+      </c>
+      <c r="K700" s="7">
+        <v>0</v>
+      </c>
+      <c r="L700" s="7">
+        <v>0</v>
+      </c>
+      <c r="M700" s="7">
+        <v>0</v>
+      </c>
+      <c r="N700" s="7">
+        <v>0</v>
+      </c>
+      <c r="O700" s="7">
+        <v>0</v>
+      </c>
+      <c r="P700" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q700" s="7">
+        <v>2.0902768074311799</v>
+      </c>
+      <c r="R700" s="7">
+        <v>0</v>
+      </c>
+      <c r="S700" s="7">
+        <v>2.8245660840464599</v>
+      </c>
+      <c r="T700" t="b">
+        <v>0</v>
+      </c>
+      <c r="U700" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V700" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W700" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="701" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A701" s="10">
+        <v>700</v>
+      </c>
+      <c r="B701" s="7">
+        <v>10.511963338805501</v>
+      </c>
+      <c r="C701" s="7">
+        <v>10.697107427543401</v>
+      </c>
+      <c r="D701" s="7">
+        <v>0</v>
+      </c>
+      <c r="E701" s="7">
+        <v>0</v>
+      </c>
+      <c r="F701" s="7">
+        <v>0</v>
+      </c>
+      <c r="G701" s="7">
+        <v>0</v>
+      </c>
+      <c r="H701" s="7">
+        <v>0</v>
+      </c>
+      <c r="I701" s="7">
+        <v>0</v>
+      </c>
+      <c r="J701" s="7">
+        <v>0</v>
+      </c>
+      <c r="K701" s="7">
+        <v>0</v>
+      </c>
+      <c r="L701" s="7">
+        <v>0</v>
+      </c>
+      <c r="M701" s="7">
+        <v>0</v>
+      </c>
+      <c r="N701" s="7">
+        <v>0</v>
+      </c>
+      <c r="O701" s="7">
+        <v>0</v>
+      </c>
+      <c r="P701" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q701" s="7">
+        <v>2.5373373819255698</v>
+      </c>
+      <c r="R701" s="7">
+        <v>0</v>
+      </c>
+      <c r="S701" s="7">
+        <v>4.6190092604807704</v>
+      </c>
+      <c r="T701" t="b">
+        <v>1</v>
+      </c>
+      <c r="U701" s="2">
+        <v>28</v>
+      </c>
+      <c r="V701" s="2">
+        <v>491</v>
+      </c>
+      <c r="W701" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="702" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A702" s="10">
+        <v>701</v>
+      </c>
+      <c r="B702" s="7">
+        <v>0</v>
+      </c>
+      <c r="C702" s="7">
+        <v>13.1719285734106</v>
+      </c>
+      <c r="D702" s="7">
+        <v>0</v>
+      </c>
+      <c r="E702" s="7">
+        <v>0</v>
+      </c>
+      <c r="F702" s="7">
+        <v>7.46014772661644</v>
+      </c>
+      <c r="G702" s="7">
+        <v>0</v>
+      </c>
+      <c r="H702" s="7">
+        <v>0</v>
+      </c>
+      <c r="I702" s="7">
+        <v>0</v>
+      </c>
+      <c r="J702" s="7">
+        <v>0</v>
+      </c>
+      <c r="K702" s="7">
+        <v>0</v>
+      </c>
+      <c r="L702" s="7">
+        <v>0</v>
+      </c>
+      <c r="M702" s="7">
+        <v>0</v>
+      </c>
+      <c r="N702" s="7">
+        <v>0</v>
+      </c>
+      <c r="O702" s="7">
+        <v>0</v>
+      </c>
+      <c r="P702" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q702" s="7">
+        <v>2.0940470127754902</v>
+      </c>
+      <c r="R702" s="7">
+        <v>0</v>
+      </c>
+      <c r="S702" s="7">
+        <v>2.3285899004787902</v>
+      </c>
+      <c r="T702" t="b">
+        <v>1</v>
+      </c>
+      <c r="U702" s="2">
+        <v>19</v>
+      </c>
+      <c r="V702" s="2">
+        <v>5</v>
+      </c>
+      <c r="W702" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="703" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A703" s="10">
+        <v>702</v>
+      </c>
+      <c r="B703" s="7">
+        <v>0</v>
+      </c>
+      <c r="C703" s="7">
+        <v>0</v>
+      </c>
+      <c r="D703" s="7">
+        <v>0</v>
+      </c>
+      <c r="E703" s="7">
+        <v>0</v>
+      </c>
+      <c r="F703" s="7">
+        <v>0</v>
+      </c>
+      <c r="G703" s="7">
+        <v>10.9653727384666</v>
+      </c>
+      <c r="H703" s="7">
+        <v>12.973034921883199</v>
+      </c>
+      <c r="I703" s="7">
+        <v>0</v>
+      </c>
+      <c r="J703" s="7">
+        <v>0</v>
+      </c>
+      <c r="K703" s="7">
+        <v>0</v>
+      </c>
+      <c r="L703" s="7">
+        <v>0</v>
+      </c>
+      <c r="M703" s="7">
+        <v>0</v>
+      </c>
+      <c r="N703" s="7">
+        <v>0</v>
+      </c>
+      <c r="O703" s="7">
+        <v>0</v>
+      </c>
+      <c r="P703" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q703" s="7">
+        <v>1.6422793271896701</v>
+      </c>
+      <c r="R703" s="7">
+        <v>0</v>
+      </c>
+      <c r="S703" s="7">
+        <v>1.3944797837379601</v>
+      </c>
+      <c r="T703" t="b">
+        <v>1</v>
+      </c>
+      <c r="U703" s="2">
+        <v>26</v>
+      </c>
+      <c r="V703" s="2">
+        <v>9</v>
+      </c>
+      <c r="W703" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="704" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A704" s="10">
+        <v>703</v>
+      </c>
+      <c r="B704" s="7">
+        <v>0</v>
+      </c>
+      <c r="C704" s="7">
+        <v>10.1340102405754</v>
+      </c>
+      <c r="D704" s="7">
+        <v>0</v>
+      </c>
+      <c r="E704" s="7">
+        <v>0</v>
+      </c>
+      <c r="F704" s="7">
+        <v>0</v>
+      </c>
+      <c r="G704" s="7">
+        <v>0</v>
+      </c>
+      <c r="H704" s="7">
+        <v>0</v>
+      </c>
+      <c r="I704" s="7">
+        <v>8.1243550725129001</v>
+      </c>
+      <c r="J704" s="7">
+        <v>0</v>
+      </c>
+      <c r="K704" s="7">
+        <v>0</v>
+      </c>
+      <c r="L704" s="7">
+        <v>0</v>
+      </c>
+      <c r="M704" s="7">
+        <v>0</v>
+      </c>
+      <c r="N704" s="7">
+        <v>0</v>
+      </c>
+      <c r="O704" s="7">
+        <v>0</v>
+      </c>
+      <c r="P704" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q704" s="7">
+        <v>1.3574613374928299</v>
+      </c>
+      <c r="R704" s="7">
+        <v>0</v>
+      </c>
+      <c r="S704" s="7">
+        <v>2.9394651518639301</v>
+      </c>
+      <c r="T704" t="b">
+        <v>1</v>
+      </c>
+      <c r="U704" s="2">
+        <v>21</v>
+      </c>
+      <c r="V704" s="2">
+        <v>26</v>
+      </c>
+      <c r="W704" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="705" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A705" s="10">
+        <v>704</v>
+      </c>
+      <c r="B705" s="7">
+        <v>6.0857664071815698</v>
+      </c>
+      <c r="C705" s="7">
+        <v>0</v>
+      </c>
+      <c r="D705" s="7">
+        <v>0</v>
+      </c>
+      <c r="E705" s="7">
+        <v>0</v>
+      </c>
+      <c r="F705" s="7">
+        <v>0</v>
+      </c>
+      <c r="G705" s="7">
+        <v>0</v>
+      </c>
+      <c r="H705" s="7">
+        <v>0</v>
+      </c>
+      <c r="I705" s="7">
+        <v>0</v>
+      </c>
+      <c r="J705" s="7">
+        <v>0</v>
+      </c>
+      <c r="K705" s="7">
+        <v>0</v>
+      </c>
+      <c r="L705" s="7">
+        <v>0</v>
+      </c>
+      <c r="M705" s="7">
+        <v>9.3177727204445695</v>
+      </c>
+      <c r="N705" s="7">
+        <v>0</v>
+      </c>
+      <c r="O705" s="7">
+        <v>0</v>
+      </c>
+      <c r="P705" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q705" s="7">
+        <v>1.44917504769288</v>
+      </c>
+      <c r="R705" s="7">
+        <v>0</v>
+      </c>
+      <c r="S705" s="7">
+        <v>3.0854230900482502</v>
+      </c>
+      <c r="T705" t="b">
+        <v>0</v>
+      </c>
+      <c r="U705" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V705" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W705" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="706" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A706" s="10">
+        <v>705</v>
+      </c>
+      <c r="B706" s="7">
+        <v>0</v>
+      </c>
+      <c r="C706" s="7">
+        <v>0</v>
+      </c>
+      <c r="D706" s="7">
+        <v>0</v>
+      </c>
+      <c r="E706" s="7">
+        <v>0</v>
+      </c>
+      <c r="F706" s="7">
+        <v>0</v>
+      </c>
+      <c r="G706" s="7">
+        <v>11.0784018987423</v>
+      </c>
+      <c r="H706" s="7">
+        <v>0</v>
+      </c>
+      <c r="I706" s="7">
+        <v>0</v>
+      </c>
+      <c r="J706" s="7">
+        <v>0</v>
+      </c>
+      <c r="K706" s="7">
+        <v>0</v>
+      </c>
+      <c r="L706" s="7">
+        <v>0</v>
+      </c>
+      <c r="M706" s="7">
+        <v>12.885629165162101</v>
+      </c>
+      <c r="N706" s="7">
+        <v>0</v>
+      </c>
+      <c r="O706" s="7">
+        <v>0</v>
+      </c>
+      <c r="P706" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q706" s="7">
+        <v>1.55540051618103</v>
+      </c>
+      <c r="R706" s="7">
+        <v>0</v>
+      </c>
+      <c r="S706" s="7">
+        <v>3.1700543853594398</v>
+      </c>
+      <c r="T706" t="b">
+        <v>0</v>
+      </c>
+      <c r="U706" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V706" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W706" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="707" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A707" s="10">
+        <v>706</v>
+      </c>
+      <c r="B707" s="7">
+        <v>0</v>
+      </c>
+      <c r="C707" s="7">
+        <v>0</v>
+      </c>
+      <c r="D707" s="7">
+        <v>0</v>
+      </c>
+      <c r="E707" s="7">
+        <v>0</v>
+      </c>
+      <c r="F707" s="7">
+        <v>0</v>
+      </c>
+      <c r="G707" s="7">
+        <v>0</v>
+      </c>
+      <c r="H707" s="7">
+        <v>9.2379124105616999</v>
+      </c>
+      <c r="I707" s="7">
+        <v>0</v>
+      </c>
+      <c r="J707" s="7">
+        <v>8.4607988665578802</v>
+      </c>
+      <c r="K707" s="7">
+        <v>0</v>
+      </c>
+      <c r="L707" s="7">
+        <v>0</v>
+      </c>
+      <c r="M707" s="7">
+        <v>0</v>
+      </c>
+      <c r="N707" s="7">
+        <v>0</v>
+      </c>
+      <c r="O707" s="7">
+        <v>0</v>
+      </c>
+      <c r="P707" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q707" s="7">
+        <v>2.3725813124156998</v>
+      </c>
+      <c r="R707" s="7">
+        <v>0</v>
+      </c>
+      <c r="S707" s="7">
+        <v>4.5165998177714197</v>
+      </c>
+      <c r="T707" t="b">
+        <v>0</v>
+      </c>
+      <c r="U707" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V707" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W707" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="708" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A708" s="10">
+        <v>707</v>
+      </c>
+      <c r="B708" s="7">
+        <v>0</v>
+      </c>
+      <c r="C708" s="7">
+        <v>0</v>
+      </c>
+      <c r="D708" s="7">
+        <v>10.6840139491086</v>
+      </c>
+      <c r="E708" s="7">
+        <v>0</v>
+      </c>
+      <c r="F708" s="7">
+        <v>12.598010901722001</v>
+      </c>
+      <c r="G708" s="7">
+        <v>0</v>
+      </c>
+      <c r="H708" s="7">
+        <v>0</v>
+      </c>
+      <c r="I708" s="7">
+        <v>0</v>
+      </c>
+      <c r="J708" s="7">
+        <v>0</v>
+      </c>
+      <c r="K708" s="7">
+        <v>0</v>
+      </c>
+      <c r="L708" s="7">
+        <v>0</v>
+      </c>
+      <c r="M708" s="7">
+        <v>0</v>
+      </c>
+      <c r="N708" s="7">
+        <v>0</v>
+      </c>
+      <c r="O708" s="7">
+        <v>0</v>
+      </c>
+      <c r="P708" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q708" s="7">
+        <v>3.1825878120727298</v>
+      </c>
+      <c r="R708" s="7">
+        <v>0</v>
+      </c>
+      <c r="S708" s="7">
+        <v>2.9085247809322099</v>
+      </c>
+      <c r="T708" t="b">
+        <v>1</v>
+      </c>
+      <c r="U708" s="2">
+        <v>14</v>
+      </c>
+      <c r="V708" s="2">
+        <v>24</v>
+      </c>
+      <c r="W708" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="709" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A709" s="10">
+        <v>708</v>
+      </c>
+      <c r="B709" s="7">
+        <v>12.008331059866601</v>
+      </c>
+      <c r="C709" s="7">
+        <v>0</v>
+      </c>
+      <c r="D709" s="7">
+        <v>11.593312252698301</v>
+      </c>
+      <c r="E709" s="7">
+        <v>0</v>
+      </c>
+      <c r="F709" s="7">
+        <v>0</v>
+      </c>
+      <c r="G709" s="7">
+        <v>0</v>
+      </c>
+      <c r="H709" s="7">
+        <v>0</v>
+      </c>
+      <c r="I709" s="7">
+        <v>0</v>
+      </c>
+      <c r="J709" s="7">
+        <v>0</v>
+      </c>
+      <c r="K709" s="7">
+        <v>0</v>
+      </c>
+      <c r="L709" s="7">
+        <v>0</v>
+      </c>
+      <c r="M709" s="7">
+        <v>0</v>
+      </c>
+      <c r="N709" s="7">
+        <v>0</v>
+      </c>
+      <c r="O709" s="7">
+        <v>0</v>
+      </c>
+      <c r="P709" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q709" s="7">
+        <v>3.02152158497455</v>
+      </c>
+      <c r="R709" s="7">
+        <v>0</v>
+      </c>
+      <c r="S709" s="7">
+        <v>4.91802146199311</v>
+      </c>
+      <c r="T709" t="b">
+        <v>0</v>
+      </c>
+      <c r="U709" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V709" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W709" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="710" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A710" s="10">
+        <v>709</v>
+      </c>
+      <c r="B710" s="7">
+        <v>0</v>
+      </c>
+      <c r="C710" s="7">
+        <v>0</v>
+      </c>
+      <c r="D710" s="7">
+        <v>0</v>
+      </c>
+      <c r="E710" s="7">
+        <v>0</v>
+      </c>
+      <c r="F710" s="7">
+        <v>0</v>
+      </c>
+      <c r="G710" s="7">
+        <v>0</v>
+      </c>
+      <c r="H710" s="7">
+        <v>0</v>
+      </c>
+      <c r="I710" s="7">
+        <v>7.7235419089506401</v>
+      </c>
+      <c r="J710" s="7">
+        <v>0</v>
+      </c>
+      <c r="K710" s="7">
+        <v>0</v>
+      </c>
+      <c r="L710" s="7">
+        <v>9.6053939404953397</v>
+      </c>
+      <c r="M710" s="7">
+        <v>0</v>
+      </c>
+      <c r="N710" s="7">
+        <v>0</v>
+      </c>
+      <c r="O710" s="7">
+        <v>0</v>
+      </c>
+      <c r="P710" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q710" s="7">
+        <v>2.09553462645952</v>
+      </c>
+      <c r="R710" s="7">
+        <v>0</v>
+      </c>
+      <c r="S710" s="7">
+        <v>4.3252660516577199</v>
+      </c>
+      <c r="T710" t="b">
+        <v>0</v>
+      </c>
+      <c r="U710" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V710" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W710" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="711" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A711" s="10">
+        <v>710</v>
+      </c>
+      <c r="B711" s="7">
+        <v>5.7880419327931003</v>
+      </c>
+      <c r="C711" s="7">
+        <v>0</v>
+      </c>
+      <c r="D711" s="7">
+        <v>0</v>
+      </c>
+      <c r="E711" s="7">
+        <v>0</v>
+      </c>
+      <c r="F711" s="7">
+        <v>8.2690777225919199</v>
+      </c>
+      <c r="G711" s="7">
+        <v>0</v>
+      </c>
+      <c r="H711" s="7">
+        <v>0</v>
+      </c>
+      <c r="I711" s="7">
+        <v>0</v>
+      </c>
+      <c r="J711" s="7">
+        <v>0</v>
+      </c>
+      <c r="K711" s="7">
+        <v>0</v>
+      </c>
+      <c r="L711" s="7">
+        <v>0</v>
+      </c>
+      <c r="M711" s="7">
+        <v>0</v>
+      </c>
+      <c r="N711" s="7">
+        <v>0</v>
+      </c>
+      <c r="O711" s="7">
+        <v>0</v>
+      </c>
+      <c r="P711" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q711" s="7">
+        <v>3.0114587436004498</v>
+      </c>
+      <c r="R711" s="7">
+        <v>0</v>
+      </c>
+      <c r="S711" s="7">
+        <v>5.0933102485797503</v>
+      </c>
+      <c r="T711" t="b">
+        <v>0</v>
+      </c>
+      <c r="U711" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V711" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W711" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="712" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A712" s="10">
+        <v>711</v>
+      </c>
+      <c r="B712" s="7">
+        <v>0</v>
+      </c>
+      <c r="C712" s="7">
+        <v>0</v>
+      </c>
+      <c r="D712" s="7">
+        <v>0</v>
+      </c>
+      <c r="E712" s="7">
+        <v>0</v>
+      </c>
+      <c r="F712" s="7">
+        <v>8.9981912837505806</v>
+      </c>
+      <c r="G712" s="7">
+        <v>7.1568738980794198</v>
+      </c>
+      <c r="H712" s="7">
+        <v>0</v>
+      </c>
+      <c r="I712" s="7">
+        <v>0</v>
+      </c>
+      <c r="J712" s="7">
+        <v>0</v>
+      </c>
+      <c r="K712" s="7">
+        <v>0</v>
+      </c>
+      <c r="L712" s="7">
+        <v>0</v>
+      </c>
+      <c r="M712" s="7">
+        <v>0</v>
+      </c>
+      <c r="N712" s="7">
+        <v>0</v>
+      </c>
+      <c r="O712" s="7">
+        <v>0</v>
+      </c>
+      <c r="P712" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q712" s="7">
+        <v>2.4985463728257402</v>
+      </c>
+      <c r="R712" s="7">
+        <v>0</v>
+      </c>
+      <c r="S712" s="7">
+        <v>2.9742852563447002</v>
+      </c>
+      <c r="T712" t="b">
+        <v>0</v>
+      </c>
+      <c r="U712" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V712" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W712" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="713" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A713" s="10">
+        <v>712</v>
+      </c>
+      <c r="B713" s="7">
+        <v>0</v>
+      </c>
+      <c r="C713" s="7">
+        <v>0</v>
+      </c>
+      <c r="D713" s="7">
+        <v>0</v>
+      </c>
+      <c r="E713" s="7">
+        <v>0</v>
+      </c>
+      <c r="F713" s="7">
+        <v>9.5606274256969801</v>
+      </c>
+      <c r="G713" s="7">
+        <v>0</v>
+      </c>
+      <c r="H713" s="7">
+        <v>0</v>
+      </c>
+      <c r="I713" s="7">
+        <v>0</v>
+      </c>
+      <c r="J713" s="7">
+        <v>0</v>
+      </c>
+      <c r="K713" s="7">
+        <v>11.3822103835271</v>
+      </c>
+      <c r="L713" s="7">
+        <v>0</v>
+      </c>
+      <c r="M713" s="7">
+        <v>0</v>
+      </c>
+      <c r="N713" s="7">
+        <v>0</v>
+      </c>
+      <c r="O713" s="7">
+        <v>0</v>
+      </c>
+      <c r="P713" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q713" s="7">
+        <v>1.21837263984482</v>
+      </c>
+      <c r="R713" s="7">
+        <v>0</v>
+      </c>
+      <c r="S713" s="7">
+        <v>2.0879419013155802</v>
+      </c>
+      <c r="T713" t="b">
+        <v>1</v>
+      </c>
+      <c r="U713" s="2">
+        <v>21</v>
+      </c>
+      <c r="V713" s="2">
+        <v>5</v>
+      </c>
+      <c r="W713" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="714" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A714" s="10">
+        <v>713</v>
+      </c>
+      <c r="B714" s="7">
+        <v>0</v>
+      </c>
+      <c r="C714" s="7">
+        <v>0</v>
+      </c>
+      <c r="D714" s="7">
+        <v>0</v>
+      </c>
+      <c r="E714" s="7">
+        <v>0</v>
+      </c>
+      <c r="F714" s="7">
+        <v>0</v>
+      </c>
+      <c r="G714" s="7">
+        <v>0</v>
+      </c>
+      <c r="H714" s="7">
+        <v>0</v>
+      </c>
+      <c r="I714" s="7">
+        <v>9.6577171763728895</v>
+      </c>
+      <c r="J714" s="7">
+        <v>0</v>
+      </c>
+      <c r="K714" s="7">
+        <v>10.775253021067501</v>
+      </c>
+      <c r="L714" s="7">
+        <v>0</v>
+      </c>
+      <c r="M714" s="7">
+        <v>0</v>
+      </c>
+      <c r="N714" s="7">
+        <v>0</v>
+      </c>
+      <c r="O714" s="7">
+        <v>0</v>
+      </c>
+      <c r="P714" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q714" s="7">
+        <v>2.4944996533361099</v>
+      </c>
+      <c r="R714" s="7">
+        <v>0</v>
+      </c>
+      <c r="S714" s="7">
+        <v>1.8034308604859799</v>
+      </c>
+      <c r="T714" t="b">
+        <v>1</v>
+      </c>
+      <c r="U714" s="2">
+        <v>28</v>
+      </c>
+      <c r="V714" s="2">
+        <v>7</v>
+      </c>
+      <c r="W714" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="715" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A715" s="10">
+        <v>714</v>
+      </c>
+      <c r="B715" s="7">
+        <v>0</v>
+      </c>
+      <c r="C715" s="7">
+        <v>0</v>
+      </c>
+      <c r="D715" s="7">
+        <v>6.4677898171981498</v>
+      </c>
+      <c r="E715" s="7">
+        <v>0</v>
+      </c>
+      <c r="F715" s="7">
+        <v>0</v>
+      </c>
+      <c r="G715" s="7">
+        <v>0</v>
+      </c>
+      <c r="H715" s="7">
+        <v>0</v>
+      </c>
+      <c r="I715" s="7">
+        <v>0</v>
+      </c>
+      <c r="J715" s="7">
+        <v>0</v>
+      </c>
+      <c r="K715" s="7">
+        <v>0</v>
+      </c>
+      <c r="L715" s="7">
+        <v>0</v>
+      </c>
+      <c r="M715" s="7">
+        <v>12.5528399813349</v>
+      </c>
+      <c r="N715" s="7">
+        <v>0</v>
+      </c>
+      <c r="O715" s="7">
+        <v>0</v>
+      </c>
+      <c r="P715" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q715" s="7">
+        <v>2.31302330333369</v>
+      </c>
+      <c r="R715" s="7">
+        <v>0</v>
+      </c>
+      <c r="S715" s="7">
+        <v>1.7146736457145</v>
+      </c>
+      <c r="T715" t="b">
+        <v>0</v>
+      </c>
+      <c r="U715" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V715" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W715" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W691">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="A1:W715">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U580">
-    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U569">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -61425,7 +63174,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S720
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0742FC6-8DA7-D44F-B593-EE4CCC01853F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C848CF-924C-FC43-8EF0-363C95DF2D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -404,27 +404,7 @@
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -452,16 +432,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -785,11 +755,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:X715"/>
+  <dimension ref="A1:X727"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A660" zoomScale="119" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA26" sqref="AA26"/>
+    <sheetView tabSelected="1" topLeftCell="A674" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W727" sqref="W727"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50951,15 +50921,15 @@
         <v>0</v>
       </c>
       <c r="U687" s="2" t="str">
-        <f t="shared" ref="U687:U715" si="40">IF(T687=FALSE, "NA", "")</f>
+        <f t="shared" ref="U687:U727" si="40">IF(T687=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V687" s="2" t="str">
-        <f t="shared" ref="V687:V715" si="41">IF(T687=FALSE, "NA", "")</f>
+        <f t="shared" ref="V687:V727" si="41">IF(T687=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="W687" s="12" t="str">
-        <f t="shared" ref="W687:W715" si="42">IF(T687=FALSE, "NA", "")</f>
+        <f t="shared" ref="W687:W727" si="42">IF(T687=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -53008,19 +52978,886 @@
         <v>NA</v>
       </c>
     </row>
+    <row r="716" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A716" s="10">
+        <v>715</v>
+      </c>
+      <c r="B716" s="7">
+        <v>0</v>
+      </c>
+      <c r="C716" s="7">
+        <v>11.988734417536101</v>
+      </c>
+      <c r="D716" s="7">
+        <v>0</v>
+      </c>
+      <c r="E716" s="7">
+        <v>0</v>
+      </c>
+      <c r="F716" s="7">
+        <v>0</v>
+      </c>
+      <c r="G716" s="7">
+        <v>0</v>
+      </c>
+      <c r="H716" s="7">
+        <v>0</v>
+      </c>
+      <c r="I716" s="7">
+        <v>0</v>
+      </c>
+      <c r="J716" s="7">
+        <v>0</v>
+      </c>
+      <c r="K716" s="7">
+        <v>10.505267485424399</v>
+      </c>
+      <c r="L716" s="7">
+        <v>0</v>
+      </c>
+      <c r="M716" s="7">
+        <v>0</v>
+      </c>
+      <c r="N716" s="7">
+        <v>0</v>
+      </c>
+      <c r="O716" s="7">
+        <v>0</v>
+      </c>
+      <c r="P716" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q716" s="7">
+        <v>2.4212088770952298</v>
+      </c>
+      <c r="R716" s="7">
+        <v>0</v>
+      </c>
+      <c r="S716" s="7">
+        <v>1.3968985700254899</v>
+      </c>
+      <c r="T716" t="b">
+        <v>1</v>
+      </c>
+      <c r="U716" s="2">
+        <v>17</v>
+      </c>
+      <c r="V716" s="2">
+        <v>3</v>
+      </c>
+      <c r="W716" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="717" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A717" s="10">
+        <v>716</v>
+      </c>
+      <c r="B717" s="7">
+        <v>0</v>
+      </c>
+      <c r="C717" s="7">
+        <v>0</v>
+      </c>
+      <c r="D717" s="7">
+        <v>0</v>
+      </c>
+      <c r="E717" s="7">
+        <v>0</v>
+      </c>
+      <c r="F717" s="7">
+        <v>0</v>
+      </c>
+      <c r="G717" s="7">
+        <v>0</v>
+      </c>
+      <c r="H717" s="7">
+        <v>12.3529043207174</v>
+      </c>
+      <c r="I717" s="7">
+        <v>0</v>
+      </c>
+      <c r="J717" s="7">
+        <v>0</v>
+      </c>
+      <c r="K717" s="7">
+        <v>12.1910332978852</v>
+      </c>
+      <c r="L717" s="7">
+        <v>0</v>
+      </c>
+      <c r="M717" s="7">
+        <v>0</v>
+      </c>
+      <c r="N717" s="7">
+        <v>0</v>
+      </c>
+      <c r="O717" s="7">
+        <v>0</v>
+      </c>
+      <c r="P717" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q717" s="7">
+        <v>1.3030129774674799</v>
+      </c>
+      <c r="R717" s="7">
+        <v>0</v>
+      </c>
+      <c r="S717" s="7">
+        <v>2.0380146850568202</v>
+      </c>
+      <c r="T717" t="b">
+        <v>1</v>
+      </c>
+      <c r="U717" s="2">
+        <v>16</v>
+      </c>
+      <c r="V717" s="2">
+        <v>5</v>
+      </c>
+      <c r="W717" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="718" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A718" s="10">
+        <v>717</v>
+      </c>
+      <c r="B718" s="7">
+        <v>0</v>
+      </c>
+      <c r="C718" s="7">
+        <v>0</v>
+      </c>
+      <c r="D718" s="7">
+        <v>0</v>
+      </c>
+      <c r="E718" s="7">
+        <v>0</v>
+      </c>
+      <c r="F718" s="7">
+        <v>0</v>
+      </c>
+      <c r="G718" s="7">
+        <v>7.5410515393852</v>
+      </c>
+      <c r="H718" s="7">
+        <v>0</v>
+      </c>
+      <c r="I718" s="7">
+        <v>0</v>
+      </c>
+      <c r="J718" s="7">
+        <v>0</v>
+      </c>
+      <c r="K718" s="7">
+        <v>9.1459269124967495</v>
+      </c>
+      <c r="L718" s="7">
+        <v>0</v>
+      </c>
+      <c r="M718" s="7">
+        <v>0</v>
+      </c>
+      <c r="N718" s="7">
+        <v>0</v>
+      </c>
+      <c r="O718" s="7">
+        <v>0</v>
+      </c>
+      <c r="P718" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q718" s="7">
+        <v>1.9570754206315799</v>
+      </c>
+      <c r="R718" s="7">
+        <v>0</v>
+      </c>
+      <c r="S718" s="7">
+        <v>1.8038916838882799</v>
+      </c>
+      <c r="T718" t="b">
+        <v>0</v>
+      </c>
+      <c r="U718" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V718" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W718" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="719" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A719" s="10">
+        <v>718</v>
+      </c>
+      <c r="B719" s="7">
+        <v>0</v>
+      </c>
+      <c r="C719" s="7">
+        <v>0</v>
+      </c>
+      <c r="D719" s="7">
+        <v>8.4342111999525198</v>
+      </c>
+      <c r="E719" s="7">
+        <v>0</v>
+      </c>
+      <c r="F719" s="7">
+        <v>0</v>
+      </c>
+      <c r="G719" s="7">
+        <v>0</v>
+      </c>
+      <c r="H719" s="7">
+        <v>0</v>
+      </c>
+      <c r="I719" s="7">
+        <v>0</v>
+      </c>
+      <c r="J719" s="7">
+        <v>9.4370197771175306</v>
+      </c>
+      <c r="K719" s="7">
+        <v>0</v>
+      </c>
+      <c r="L719" s="7">
+        <v>0</v>
+      </c>
+      <c r="M719" s="7">
+        <v>0</v>
+      </c>
+      <c r="N719" s="7">
+        <v>0</v>
+      </c>
+      <c r="O719" s="7">
+        <v>0</v>
+      </c>
+      <c r="P719" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q719" s="7">
+        <v>3.22707005913374</v>
+      </c>
+      <c r="R719" s="7">
+        <v>0</v>
+      </c>
+      <c r="S719" s="7">
+        <v>2.00862257464131</v>
+      </c>
+      <c r="T719" t="b">
+        <v>0</v>
+      </c>
+      <c r="U719" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V719" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W719" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="720" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A720" s="10">
+        <v>719</v>
+      </c>
+      <c r="B720" s="7">
+        <v>8.8268371494030902</v>
+      </c>
+      <c r="C720" s="7">
+        <v>13.1642278416809</v>
+      </c>
+      <c r="D720" s="7">
+        <v>0</v>
+      </c>
+      <c r="E720" s="7">
+        <v>0</v>
+      </c>
+      <c r="F720" s="7">
+        <v>0</v>
+      </c>
+      <c r="G720" s="7">
+        <v>0</v>
+      </c>
+      <c r="H720" s="7">
+        <v>0</v>
+      </c>
+      <c r="I720" s="7">
+        <v>0</v>
+      </c>
+      <c r="J720" s="7">
+        <v>0</v>
+      </c>
+      <c r="K720" s="7">
+        <v>0</v>
+      </c>
+      <c r="L720" s="7">
+        <v>0</v>
+      </c>
+      <c r="M720" s="7">
+        <v>0</v>
+      </c>
+      <c r="N720" s="7">
+        <v>0</v>
+      </c>
+      <c r="O720" s="7">
+        <v>0</v>
+      </c>
+      <c r="P720" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q720" s="7">
+        <v>1.79378285093643</v>
+      </c>
+      <c r="R720" s="7">
+        <v>0</v>
+      </c>
+      <c r="S720" s="7">
+        <v>1.53006113377897</v>
+      </c>
+      <c r="T720" t="b">
+        <v>1</v>
+      </c>
+      <c r="U720" s="2">
+        <v>23</v>
+      </c>
+      <c r="V720" s="2">
+        <v>3</v>
+      </c>
+      <c r="W720" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="721" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A721" s="10">
+        <v>720</v>
+      </c>
+      <c r="B721" s="7">
+        <v>16.2397534817128</v>
+      </c>
+      <c r="C721" s="7">
+        <v>0</v>
+      </c>
+      <c r="D721" s="7">
+        <v>0</v>
+      </c>
+      <c r="E721" s="7">
+        <v>0</v>
+      </c>
+      <c r="F721" s="7">
+        <v>0</v>
+      </c>
+      <c r="G721" s="7">
+        <v>0</v>
+      </c>
+      <c r="H721" s="7">
+        <v>0</v>
+      </c>
+      <c r="I721" s="7">
+        <v>0</v>
+      </c>
+      <c r="J721" s="7">
+        <v>11.5216257890627</v>
+      </c>
+      <c r="K721" s="7">
+        <v>0</v>
+      </c>
+      <c r="L721" s="7">
+        <v>0</v>
+      </c>
+      <c r="M721" s="7">
+        <v>0</v>
+      </c>
+      <c r="N721" s="7">
+        <v>0</v>
+      </c>
+      <c r="O721" s="7">
+        <v>0</v>
+      </c>
+      <c r="P721" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q721" s="7">
+        <v>2.6923849921499499</v>
+      </c>
+      <c r="R721" s="7">
+        <v>0</v>
+      </c>
+      <c r="S721" s="7">
+        <v>1.7225780942562701</v>
+      </c>
+      <c r="T721" t="b">
+        <v>1</v>
+      </c>
+      <c r="U721" s="2">
+        <v>29</v>
+      </c>
+      <c r="V721" s="2">
+        <v>261</v>
+      </c>
+      <c r="W721" s="12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="722" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A722" s="10">
+        <v>721</v>
+      </c>
+      <c r="B722" s="7">
+        <v>0</v>
+      </c>
+      <c r="C722" s="7">
+        <v>0</v>
+      </c>
+      <c r="D722" s="7">
+        <v>12.1859002389146</v>
+      </c>
+      <c r="E722" s="7">
+        <v>0</v>
+      </c>
+      <c r="F722" s="7">
+        <v>0</v>
+      </c>
+      <c r="G722" s="7">
+        <v>8.8927369484373102</v>
+      </c>
+      <c r="H722" s="7">
+        <v>0</v>
+      </c>
+      <c r="I722" s="7">
+        <v>0</v>
+      </c>
+      <c r="J722" s="7">
+        <v>0</v>
+      </c>
+      <c r="K722" s="7">
+        <v>0</v>
+      </c>
+      <c r="L722" s="7">
+        <v>0</v>
+      </c>
+      <c r="M722" s="7">
+        <v>0</v>
+      </c>
+      <c r="N722" s="7">
+        <v>0</v>
+      </c>
+      <c r="O722" s="7">
+        <v>0</v>
+      </c>
+      <c r="P722" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q722" s="7">
+        <v>0.92072021476336396</v>
+      </c>
+      <c r="R722" s="7">
+        <v>0</v>
+      </c>
+      <c r="S722" s="7">
+        <v>1.6296374031265399</v>
+      </c>
+      <c r="T722" t="b">
+        <v>1</v>
+      </c>
+      <c r="U722" s="2">
+        <v>15</v>
+      </c>
+      <c r="V722" s="2">
+        <v>5</v>
+      </c>
+      <c r="W722" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="723" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A723" s="10">
+        <v>722</v>
+      </c>
+      <c r="B723" s="7">
+        <v>0</v>
+      </c>
+      <c r="C723" s="7">
+        <v>7.69668762440556</v>
+      </c>
+      <c r="D723" s="7">
+        <v>9.3909707101749405</v>
+      </c>
+      <c r="E723" s="7">
+        <v>0</v>
+      </c>
+      <c r="F723" s="7">
+        <v>0</v>
+      </c>
+      <c r="G723" s="7">
+        <v>0</v>
+      </c>
+      <c r="H723" s="7">
+        <v>0</v>
+      </c>
+      <c r="I723" s="7">
+        <v>0</v>
+      </c>
+      <c r="J723" s="7">
+        <v>0</v>
+      </c>
+      <c r="K723" s="7">
+        <v>0</v>
+      </c>
+      <c r="L723" s="7">
+        <v>0</v>
+      </c>
+      <c r="M723" s="7">
+        <v>0</v>
+      </c>
+      <c r="N723" s="7">
+        <v>0</v>
+      </c>
+      <c r="O723" s="7">
+        <v>0</v>
+      </c>
+      <c r="P723" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q723" s="7">
+        <v>2.70807542397562</v>
+      </c>
+      <c r="R723" s="7">
+        <v>0</v>
+      </c>
+      <c r="S723" s="7">
+        <v>2.5890391416031302</v>
+      </c>
+      <c r="T723" t="b">
+        <v>1</v>
+      </c>
+      <c r="U723" s="2">
+        <v>14</v>
+      </c>
+      <c r="V723" s="2">
+        <v>11</v>
+      </c>
+      <c r="W723" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="724" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A724" s="10">
+        <v>723</v>
+      </c>
+      <c r="B724" s="7">
+        <v>0</v>
+      </c>
+      <c r="C724" s="7">
+        <v>0</v>
+      </c>
+      <c r="D724" s="7">
+        <v>12.711987270969299</v>
+      </c>
+      <c r="E724" s="7">
+        <v>0</v>
+      </c>
+      <c r="F724" s="7">
+        <v>0</v>
+      </c>
+      <c r="G724" s="7">
+        <v>8.8221420980801302</v>
+      </c>
+      <c r="H724" s="7">
+        <v>0</v>
+      </c>
+      <c r="I724" s="7">
+        <v>0</v>
+      </c>
+      <c r="J724" s="7">
+        <v>0</v>
+      </c>
+      <c r="K724" s="7">
+        <v>0</v>
+      </c>
+      <c r="L724" s="7">
+        <v>0</v>
+      </c>
+      <c r="M724" s="7">
+        <v>0</v>
+      </c>
+      <c r="N724" s="7">
+        <v>0</v>
+      </c>
+      <c r="O724" s="7">
+        <v>0</v>
+      </c>
+      <c r="P724" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q724" s="7">
+        <v>2.85933718493501</v>
+      </c>
+      <c r="R724" s="7">
+        <v>0</v>
+      </c>
+      <c r="S724" s="7">
+        <v>3.1197112477235298</v>
+      </c>
+      <c r="T724" t="b">
+        <v>0</v>
+      </c>
+      <c r="U724" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V724" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W724" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="725" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A725" s="10">
+        <v>724</v>
+      </c>
+      <c r="B725" s="7">
+        <v>12.331110323774899</v>
+      </c>
+      <c r="C725" s="7">
+        <v>0</v>
+      </c>
+      <c r="D725" s="7">
+        <v>8.8990074581806304</v>
+      </c>
+      <c r="E725" s="7">
+        <v>0</v>
+      </c>
+      <c r="F725" s="7">
+        <v>0</v>
+      </c>
+      <c r="G725" s="7">
+        <v>0</v>
+      </c>
+      <c r="H725" s="7">
+        <v>0</v>
+      </c>
+      <c r="I725" s="7">
+        <v>0</v>
+      </c>
+      <c r="J725" s="7">
+        <v>0</v>
+      </c>
+      <c r="K725" s="7">
+        <v>0</v>
+      </c>
+      <c r="L725" s="7">
+        <v>0</v>
+      </c>
+      <c r="M725" s="7">
+        <v>0</v>
+      </c>
+      <c r="N725" s="7">
+        <v>0</v>
+      </c>
+      <c r="O725" s="7">
+        <v>0</v>
+      </c>
+      <c r="P725" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q725" s="7">
+        <v>1.8405181262252801</v>
+      </c>
+      <c r="R725" s="7">
+        <v>0</v>
+      </c>
+      <c r="S725" s="7">
+        <v>2.4459992364223901</v>
+      </c>
+      <c r="T725" t="b">
+        <v>0</v>
+      </c>
+      <c r="U725" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V725" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W725" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="726" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A726" s="10">
+        <v>725</v>
+      </c>
+      <c r="B726" s="7">
+        <v>0</v>
+      </c>
+      <c r="C726" s="7">
+        <v>13.2894331132447</v>
+      </c>
+      <c r="D726" s="7">
+        <v>0</v>
+      </c>
+      <c r="E726" s="7">
+        <v>0</v>
+      </c>
+      <c r="F726" s="7">
+        <v>0</v>
+      </c>
+      <c r="G726" s="7">
+        <v>0</v>
+      </c>
+      <c r="H726" s="7">
+        <v>0</v>
+      </c>
+      <c r="I726" s="7">
+        <v>0</v>
+      </c>
+      <c r="J726" s="7">
+        <v>12.498349544076101</v>
+      </c>
+      <c r="K726" s="7">
+        <v>0</v>
+      </c>
+      <c r="L726" s="7">
+        <v>0</v>
+      </c>
+      <c r="M726" s="7">
+        <v>0</v>
+      </c>
+      <c r="N726" s="7">
+        <v>0</v>
+      </c>
+      <c r="O726" s="7">
+        <v>0</v>
+      </c>
+      <c r="P726" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q726" s="7">
+        <v>1.99336678893748</v>
+      </c>
+      <c r="R726" s="7">
+        <v>0</v>
+      </c>
+      <c r="S726" s="7">
+        <v>2.5775256364508201</v>
+      </c>
+      <c r="T726" t="b">
+        <v>1</v>
+      </c>
+      <c r="U726" s="2">
+        <v>16</v>
+      </c>
+      <c r="V726" s="2">
+        <v>10</v>
+      </c>
+      <c r="W726" s="12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="727" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A727" s="10">
+        <v>726</v>
+      </c>
+      <c r="B727" s="7">
+        <v>0</v>
+      </c>
+      <c r="C727" s="7">
+        <v>9.8968972623355</v>
+      </c>
+      <c r="D727" s="7">
+        <v>0</v>
+      </c>
+      <c r="E727" s="7">
+        <v>0</v>
+      </c>
+      <c r="F727" s="7">
+        <v>0</v>
+      </c>
+      <c r="G727" s="7">
+        <v>0</v>
+      </c>
+      <c r="H727" s="7">
+        <v>0</v>
+      </c>
+      <c r="I727" s="7">
+        <v>0</v>
+      </c>
+      <c r="J727" s="7">
+        <v>0</v>
+      </c>
+      <c r="K727" s="7">
+        <v>0</v>
+      </c>
+      <c r="L727" s="7">
+        <v>8.86446605512287</v>
+      </c>
+      <c r="M727" s="7">
+        <v>0</v>
+      </c>
+      <c r="N727" s="7">
+        <v>0</v>
+      </c>
+      <c r="O727" s="7">
+        <v>0</v>
+      </c>
+      <c r="P727" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q727" s="7">
+        <v>2.7799039712165601</v>
+      </c>
+      <c r="R727" s="7">
+        <v>0</v>
+      </c>
+      <c r="S727" s="7">
+        <v>1.5613326385069299</v>
+      </c>
+      <c r="T727" t="b">
+        <v>0</v>
+      </c>
+      <c r="U727" s="2" t="str">
+        <f t="shared" si="40"/>
+        <v>NA</v>
+      </c>
+      <c r="V727" s="2" t="str">
+        <f t="shared" si="41"/>
+        <v>NA</v>
+      </c>
+      <c r="W727" s="12" t="str">
+        <f t="shared" si="42"/>
+        <v>NA</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:W715">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="A1:W727">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U580">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U569">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>4000</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53032,9 +53869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0992AFC5-60E2-AE4E-A4C6-1068A8E518A1}">
   <dimension ref="A1:W140"/>
   <sheetViews>
-    <sheetView zoomScale="75" workbookViewId="0">
-      <pane ySplit="41" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <pane ySplit="41" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -63174,7 +64011,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD127 A140:XFD1048576 A128:A139 T128:XFD139">
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
       <formula>$T1=TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Dataset updated till S798
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AFB152-A688-0D47-8F01-96D3B5110CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3467847-61C3-E947-840E-2960EC1A0029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
   <sheets>
     <sheet name="PhDFormulationsDataset_2023" sheetId="3" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -658,7 +658,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A769" zoomScale="106" workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W795" sqref="W795"/>
+      <selection pane="topRight" activeCell="X799" sqref="X799"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -61900,13 +61900,11 @@
       <c r="V796" s="1">
         <v>4</v>
       </c>
-      <c r="W796" s="1" t="str">
-        <f t="shared" si="59"/>
-        <v/>
-      </c>
-      <c r="X796" s="1" t="str">
-        <f t="shared" si="60"/>
-        <v/>
+      <c r="W796" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X796" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="797" spans="1:26" x14ac:dyDescent="0.2">
@@ -61976,13 +61974,11 @@
       <c r="V797" s="1">
         <v>2</v>
       </c>
-      <c r="W797" s="1" t="str">
-        <f t="shared" si="59"/>
-        <v/>
-      </c>
-      <c r="X797" s="1" t="str">
-        <f t="shared" si="60"/>
-        <v/>
+      <c r="W797" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X797" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="798" spans="1:26" x14ac:dyDescent="0.2">
@@ -62052,13 +62048,11 @@
       <c r="V798" s="1">
         <v>61</v>
       </c>
-      <c r="W798" s="1" t="str">
-        <f t="shared" si="59"/>
-        <v/>
-      </c>
-      <c r="X798" s="1" t="str">
-        <f t="shared" si="60"/>
-        <v/>
+      <c r="W798" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X798" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="799" spans="1:26" x14ac:dyDescent="0.2">
@@ -62128,13 +62122,11 @@
       <c r="V799" s="1">
         <v>2</v>
       </c>
-      <c r="W799" s="1" t="str">
-        <f t="shared" si="59"/>
-        <v/>
-      </c>
-      <c r="X799" s="1" t="str">
-        <f t="shared" si="60"/>
-        <v/>
+      <c r="W799" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X799" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dataset updated till S822 - final samplegit add .
</commit_message>
<xml_diff>
--- a/PhDFormulationsDataset_2023.xlsx
+++ b/PhDFormulationsDataset_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ac2349/GitHub/formulations-prep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3467847-61C3-E947-840E-2960EC1A0029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAF672B-4434-E240-8A88-AA2E2B7D21E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{44BDF354-F4F0-754D-8169-479863DA8206}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -149,9 +149,6 @@
   </si>
   <si>
     <t>NEWTONIAN</t>
-  </si>
-  <si>
-    <t>SHEAR-THICK</t>
   </si>
   <si>
     <t xml:space="preserve">LOW </t>
@@ -654,11 +651,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D7A413F-453F-F64F-BD2C-3CD20486E015}">
-  <dimension ref="A1:Z799"/>
+  <dimension ref="A1:Z823"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A769" zoomScale="106" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="X799" sqref="X799"/>
+    <sheetView tabSelected="1" topLeftCell="A787" zoomScale="106" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="W823" sqref="W823"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1315,7 +1312,7 @@
       </c>
       <c r="Y8" s="1"/>
       <c r="Z8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
@@ -1393,7 +1390,7 @@
       </c>
       <c r="Y9" s="1"/>
       <c r="Z9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
@@ -2704,7 +2701,7 @@
         <v>6</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X26" s="1" t="s">
         <v>37</v>
@@ -2857,7 +2854,7 @@
         <v>1</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X28" s="1" t="s">
         <v>37</v>
@@ -2932,7 +2929,7 @@
         <v>4</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X29" s="1" t="s">
         <v>37</v>
@@ -4816,7 +4813,7 @@
         <v>17</v>
       </c>
       <c r="W53" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X53" s="1" t="s">
         <v>37</v>
@@ -8747,7 +8744,7 @@
         <v>1</v>
       </c>
       <c r="W103" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X103" s="1" t="s">
         <v>37</v>
@@ -8822,7 +8819,7 @@
         <v>0</v>
       </c>
       <c r="W104" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X104" s="1" t="s">
         <v>37</v>
@@ -9292,7 +9289,7 @@
         <v>1</v>
       </c>
       <c r="W110" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X110" s="1" t="s">
         <v>37</v>
@@ -9446,7 +9443,7 @@
         <v>0</v>
       </c>
       <c r="W112" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X112" s="1" t="s">
         <v>37</v>
@@ -11848,7 +11845,7 @@
         <v>1</v>
       </c>
       <c r="W143" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X143" s="6" t="s">
         <v>37</v>
@@ -12534,7 +12531,7 @@
         <v>2</v>
       </c>
       <c r="W152" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X152" s="6" t="s">
         <v>37</v>
@@ -12834,7 +12831,7 @@
         <v>0</v>
       </c>
       <c r="W156" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X156" s="6" t="s">
         <v>37</v>
@@ -13138,7 +13135,7 @@
         <v>1</v>
       </c>
       <c r="W160" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X160" s="6" t="s">
         <v>37</v>
@@ -13520,7 +13517,7 @@
         <v>0</v>
       </c>
       <c r="W165" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X165" s="6" t="s">
         <v>37</v>
@@ -13898,7 +13895,7 @@
         <v>45</v>
       </c>
       <c r="W170" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X170" s="6" t="s">
         <v>37</v>
@@ -14662,7 +14659,7 @@
         <v>0</v>
       </c>
       <c r="W180" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X180" s="6" t="s">
         <v>37</v>
@@ -14736,7 +14733,7 @@
         <v>0</v>
       </c>
       <c r="W181" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X181" s="6" t="s">
         <v>37</v>
@@ -15348,7 +15345,7 @@
         <v>0</v>
       </c>
       <c r="W189" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X189" s="6" t="s">
         <v>37</v>
@@ -15422,7 +15419,7 @@
         <v>0</v>
       </c>
       <c r="W190" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X190" s="6" t="s">
         <v>37</v>
@@ -15496,7 +15493,7 @@
         <v>1</v>
       </c>
       <c r="W191" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X191" s="6" t="s">
         <v>37</v>
@@ -15570,7 +15567,7 @@
         <v>0</v>
       </c>
       <c r="W192" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X192" s="6" t="s">
         <v>37</v>
@@ -15644,7 +15641,7 @@
         <v>12</v>
       </c>
       <c r="W193" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X193" s="6" t="s">
         <v>37</v>
@@ -16778,7 +16775,7 @@
         <v>1</v>
       </c>
       <c r="W208" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X208" s="6" t="s">
         <v>37</v>
@@ -16926,7 +16923,7 @@
         <v>1</v>
       </c>
       <c r="W210" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X210" s="6" t="s">
         <v>37</v>
@@ -17542,7 +17539,7 @@
         <v>2</v>
       </c>
       <c r="W218" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X218" s="6" t="s">
         <v>35</v>
@@ -19784,7 +19781,7 @@
         <v>2</v>
       </c>
       <c r="W247" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X247" s="6" t="s">
         <v>37</v>
@@ -19932,7 +19929,7 @@
         <v>1</v>
       </c>
       <c r="W249" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X249" s="6" t="s">
         <v>37</v>
@@ -20318,7 +20315,7 @@
         <v>1</v>
       </c>
       <c r="W254" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X254" s="6" t="s">
         <v>37</v>
@@ -20392,7 +20389,7 @@
         <v>1</v>
       </c>
       <c r="W255" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X255" s="6" t="s">
         <v>37</v>
@@ -21390,7 +21387,7 @@
         <v>0</v>
       </c>
       <c r="W268" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X268" s="6" t="s">
         <v>37</v>
@@ -21700,7 +21697,7 @@
         <v>35</v>
       </c>
       <c r="Z272" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="273" spans="1:24" x14ac:dyDescent="0.2">
@@ -22149,7 +22146,7 @@
         <v>0</v>
       </c>
       <c r="W278" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X278" s="6" t="s">
         <v>37</v>
@@ -22223,7 +22220,7 @@
         <v>2</v>
       </c>
       <c r="W279" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X279" s="6" t="s">
         <v>37</v>
@@ -22297,7 +22294,7 @@
         <v>2</v>
       </c>
       <c r="W280" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X280" s="6" t="s">
         <v>37</v>
@@ -22371,7 +22368,7 @@
         <v>1</v>
       </c>
       <c r="W281" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X281" s="6" t="s">
         <v>37</v>
@@ -22445,7 +22442,7 @@
         <v>1</v>
       </c>
       <c r="W282" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X282" s="6" t="s">
         <v>37</v>
@@ -22519,7 +22516,7 @@
         <v>0</v>
       </c>
       <c r="W283" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X283" s="6" t="s">
         <v>37</v>
@@ -22667,7 +22664,7 @@
         <v>0</v>
       </c>
       <c r="W285" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X285" s="6" t="s">
         <v>37</v>
@@ -22741,7 +22738,7 @@
         <v>1</v>
       </c>
       <c r="W286" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X286" s="6" t="s">
         <v>37</v>
@@ -22815,7 +22812,7 @@
         <v>1</v>
       </c>
       <c r="W287" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X287" s="6" t="s">
         <v>37</v>
@@ -22889,7 +22886,7 @@
         <v>2</v>
       </c>
       <c r="W288" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X288" s="6" t="s">
         <v>37</v>
@@ -22963,7 +22960,7 @@
         <v>1</v>
       </c>
       <c r="W289" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X289" s="6" t="s">
         <v>37</v>
@@ -23037,7 +23034,7 @@
         <v>0</v>
       </c>
       <c r="W290" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X290" s="6" t="s">
         <v>37</v>
@@ -23185,7 +23182,7 @@
         <v>0</v>
       </c>
       <c r="W292" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X292" s="6" t="s">
         <v>37</v>
@@ -23259,7 +23256,7 @@
         <v>0</v>
       </c>
       <c r="W293" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X293" s="6" t="s">
         <v>37</v>
@@ -23333,7 +23330,7 @@
         <v>2</v>
       </c>
       <c r="W294" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X294" s="6" t="s">
         <v>37</v>
@@ -23407,7 +23404,7 @@
         <v>1</v>
       </c>
       <c r="W295" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X295" s="6" t="s">
         <v>37</v>
@@ -23481,7 +23478,7 @@
         <v>0</v>
       </c>
       <c r="W296" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X296" s="6" t="s">
         <v>37</v>
@@ -23555,7 +23552,7 @@
         <v>1</v>
       </c>
       <c r="W297" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X297" s="6" t="s">
         <v>37</v>
@@ -23629,7 +23626,7 @@
         <v>0</v>
       </c>
       <c r="W298" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X298" s="6" t="s">
         <v>37</v>
@@ -23703,7 +23700,7 @@
         <v>1</v>
       </c>
       <c r="W299" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X299" s="6" t="s">
         <v>37</v>
@@ -23931,7 +23928,7 @@
         <v>35</v>
       </c>
       <c r="Z302" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="303" spans="1:26" x14ac:dyDescent="0.2">
@@ -24002,7 +23999,7 @@
         <v>0</v>
       </c>
       <c r="W303" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X303" s="6" t="s">
         <v>37</v>
@@ -24154,7 +24151,7 @@
         <v>3</v>
       </c>
       <c r="W305" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X305" s="6" t="s">
         <v>37</v>
@@ -24228,7 +24225,7 @@
         <v>0</v>
       </c>
       <c r="W306" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X306" s="6" t="s">
         <v>37</v>
@@ -24380,7 +24377,7 @@
         <v>1</v>
       </c>
       <c r="W308" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X308" s="6" t="s">
         <v>37</v>
@@ -24532,7 +24529,7 @@
         <v>0</v>
       </c>
       <c r="W310" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X310" s="6" t="s">
         <v>37</v>
@@ -24837,7 +24834,7 @@
         <v>0</v>
       </c>
       <c r="W314" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X314" s="6" t="s">
         <v>37</v>
@@ -24989,7 +24986,7 @@
         <v>1</v>
       </c>
       <c r="W316" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X316" s="6" t="s">
         <v>37</v>
@@ -25063,7 +25060,7 @@
         <v>2</v>
       </c>
       <c r="W317" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X317" s="6" t="s">
         <v>37</v>
@@ -25217,7 +25214,7 @@
         <v>35</v>
       </c>
       <c r="Z319" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="320" spans="1:26" x14ac:dyDescent="0.2">
@@ -25518,7 +25515,7 @@
         <v>0</v>
       </c>
       <c r="W323" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X323" s="6" t="s">
         <v>37</v>
@@ -25904,7 +25901,7 @@
         <v>8</v>
       </c>
       <c r="W328" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X328" s="6" t="s">
         <v>37</v>
@@ -25978,7 +25975,7 @@
         <v>1</v>
       </c>
       <c r="W329" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X329" s="6" t="s">
         <v>37</v>
@@ -26052,7 +26049,7 @@
         <v>0</v>
       </c>
       <c r="W330" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X330" s="6" t="s">
         <v>37</v>
@@ -26126,7 +26123,7 @@
         <v>1</v>
       </c>
       <c r="W331" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X331" s="6" t="s">
         <v>37</v>
@@ -26200,7 +26197,7 @@
         <v>1</v>
       </c>
       <c r="W332" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X332" s="6" t="s">
         <v>37</v>
@@ -26274,7 +26271,7 @@
         <v>1</v>
       </c>
       <c r="W333" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X333" s="6" t="s">
         <v>37</v>
@@ -26728,7 +26725,7 @@
         <v>35</v>
       </c>
       <c r="Z339" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="340" spans="1:26" x14ac:dyDescent="0.2">
@@ -26873,7 +26870,7 @@
         <v>0</v>
       </c>
       <c r="W341" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X341" s="6" t="s">
         <v>37</v>
@@ -27099,7 +27096,7 @@
         <v>0</v>
       </c>
       <c r="W344" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X344" s="6" t="s">
         <v>37</v>
@@ -27789,7 +27786,7 @@
         <v>0</v>
       </c>
       <c r="W353" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X353" s="6" t="s">
         <v>37</v>
@@ -28089,7 +28086,7 @@
         <v>3</v>
       </c>
       <c r="W357" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X357" s="6" t="s">
         <v>37</v>
@@ -28237,7 +28234,7 @@
         <v>1</v>
       </c>
       <c r="W359" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X359" s="6" t="s">
         <v>37</v>
@@ -28389,7 +28386,7 @@
         <v>1</v>
       </c>
       <c r="W361" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X361" s="6" t="s">
         <v>37</v>
@@ -28463,7 +28460,7 @@
         <v>2</v>
       </c>
       <c r="W362" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X362" s="6" t="s">
         <v>37</v>
@@ -28690,7 +28687,7 @@
         <v>3</v>
       </c>
       <c r="W365" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X365" s="1" t="s">
         <v>37</v>
@@ -29002,7 +28999,7 @@
         <v>1</v>
       </c>
       <c r="W369" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X369" s="1" t="s">
         <v>37</v>
@@ -29314,7 +29311,7 @@
         <v>1</v>
       </c>
       <c r="W373" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X373" s="1" t="s">
         <v>37</v>
@@ -29855,7 +29852,7 @@
         <v>2</v>
       </c>
       <c r="W380" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X380" s="1" t="s">
         <v>37</v>
@@ -32923,7 +32920,7 @@
         <v>34</v>
       </c>
       <c r="X419" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y419" s="1"/>
     </row>
@@ -32995,7 +32992,7 @@
         <v>0</v>
       </c>
       <c r="W420" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X420" s="1" t="s">
         <v>37</v>
@@ -34883,7 +34880,7 @@
         <v>1</v>
       </c>
       <c r="W444" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X444" s="1" t="s">
         <v>37</v>
@@ -35590,7 +35587,7 @@
         <v>1</v>
       </c>
       <c r="W453" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X453" s="1" t="s">
         <v>37</v>
@@ -41131,7 +41128,7 @@
         <v>1</v>
       </c>
       <c r="W524" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X524" s="6" t="s">
         <v>37</v>
@@ -41279,7 +41276,7 @@
         <v>12</v>
       </c>
       <c r="W526" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X526" s="6" t="s">
         <v>37</v>
@@ -41430,7 +41427,7 @@
         <v>22</v>
       </c>
       <c r="W528" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X528" s="6" t="s">
         <v>37</v>
@@ -41504,7 +41501,7 @@
         <v>1</v>
       </c>
       <c r="W529" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X529" s="6" t="s">
         <v>37</v>
@@ -41812,7 +41809,7 @@
         <v>1</v>
       </c>
       <c r="W533" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X533" s="6" t="s">
         <v>37</v>
@@ -41886,7 +41883,7 @@
         <v>4</v>
       </c>
       <c r="W534" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X534" s="6" t="s">
         <v>37</v>
@@ -41960,7 +41957,7 @@
         <v>0</v>
       </c>
       <c r="W535" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X535" s="6" t="s">
         <v>37</v>
@@ -42268,7 +42265,7 @@
         <v>183</v>
       </c>
       <c r="W539" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X539" s="6" t="s">
         <v>37</v>
@@ -42420,7 +42417,7 @@
         <v>0</v>
       </c>
       <c r="W541" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X541" s="6" t="s">
         <v>37</v>
@@ -42724,7 +42721,7 @@
         <v>0</v>
       </c>
       <c r="W545" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X545" s="6" t="s">
         <v>37</v>
@@ -43032,7 +43029,7 @@
         <v>1</v>
       </c>
       <c r="W549" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X549" s="6" t="s">
         <v>37</v>
@@ -43788,7 +43785,7 @@
         <v>0</v>
       </c>
       <c r="W559" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X559" s="6" t="s">
         <v>37</v>
@@ -44089,7 +44086,7 @@
         <v>0</v>
       </c>
       <c r="W563" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X563" s="6" t="s">
         <v>37</v>
@@ -44163,7 +44160,7 @@
         <v>0</v>
       </c>
       <c r="W564" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X564" s="6" t="s">
         <v>37</v>
@@ -44237,7 +44234,7 @@
         <v>1</v>
       </c>
       <c r="W565" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X565" s="6" t="s">
         <v>37</v>
@@ -45228,7 +45225,7 @@
         <v>1</v>
       </c>
       <c r="W578" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X578" s="6" t="s">
         <v>37</v>
@@ -45302,7 +45299,7 @@
         <v>1</v>
       </c>
       <c r="W579" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X579" s="6" t="s">
         <v>37</v>
@@ -47320,7 +47317,7 @@
         <v>37</v>
       </c>
       <c r="Z605" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="606" spans="1:26" x14ac:dyDescent="0.2">
@@ -49021,7 +49018,7 @@
         <v>0</v>
       </c>
       <c r="W627" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X627" s="6" t="s">
         <v>37</v>
@@ -49329,7 +49326,7 @@
         <v>1</v>
       </c>
       <c r="W631" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X631" s="6" t="s">
         <v>37</v>
@@ -49481,7 +49478,7 @@
         <v>0</v>
       </c>
       <c r="W633" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X633" s="6" t="s">
         <v>37</v>
@@ -49633,7 +49630,7 @@
         <v>1</v>
       </c>
       <c r="W635" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X635" s="6" t="s">
         <v>37</v>
@@ -50311,7 +50308,7 @@
         <v>1</v>
       </c>
       <c r="W644" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X644" s="6" t="s">
         <v>37</v>
@@ -50463,7 +50460,7 @@
         <v>0</v>
       </c>
       <c r="W646" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X646" s="6" t="s">
         <v>37</v>
@@ -50537,7 +50534,7 @@
         <v>1</v>
       </c>
       <c r="W647" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X647" s="6" t="s">
         <v>37</v>
@@ -50689,7 +50686,7 @@
         <v>2</v>
       </c>
       <c r="W649" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X649" s="6" t="s">
         <v>37</v>
@@ -50763,7 +50760,7 @@
         <v>1</v>
       </c>
       <c r="W650" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X650" s="6" t="s">
         <v>37</v>
@@ -51071,7 +51068,7 @@
         <v>0</v>
       </c>
       <c r="W654" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X654" s="6" t="s">
         <v>37</v>
@@ -51145,7 +51142,7 @@
         <v>0</v>
       </c>
       <c r="W655" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X655" s="6" t="s">
         <v>37</v>
@@ -51297,7 +51294,7 @@
         <v>0</v>
       </c>
       <c r="W657" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X657" s="6" t="s">
         <v>37</v>
@@ -51527,7 +51524,7 @@
         <v>2</v>
       </c>
       <c r="W660" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X660" s="6" t="s">
         <v>37</v>
@@ -51757,7 +51754,7 @@
         <v>0</v>
       </c>
       <c r="W663" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X663" s="6" t="s">
         <v>37</v>
@@ -52539,7 +52536,7 @@
         <v>35</v>
       </c>
       <c r="Z673" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="674" spans="1:26" x14ac:dyDescent="0.2">
@@ -52610,7 +52607,7 @@
         <v>0</v>
       </c>
       <c r="W674" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X674" s="6" t="s">
         <v>37</v>
@@ -53542,7 +53539,7 @@
         <v>778</v>
       </c>
       <c r="W686" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X686" s="6" t="s">
         <v>37</v>
@@ -53775,7 +53772,7 @@
         <v>36</v>
       </c>
       <c r="X689" s="6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="Z689" s="3" t="s">
         <v>24</v>
@@ -54083,7 +54080,7 @@
         <v>0</v>
       </c>
       <c r="W693" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X693" s="6" t="s">
         <v>37</v>
@@ -54773,7 +54770,7 @@
         <v>0</v>
       </c>
       <c r="W702" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X702" s="6" t="s">
         <v>37</v>
@@ -54847,7 +54844,7 @@
         <v>2</v>
       </c>
       <c r="W703" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X703" s="6" t="s">
         <v>37</v>
@@ -55615,7 +55612,7 @@
         <v>0</v>
       </c>
       <c r="W713" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X713" s="6" t="s">
         <v>37</v>
@@ -55689,7 +55686,7 @@
         <v>1</v>
       </c>
       <c r="W714" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X714" s="6" t="s">
         <v>37</v>
@@ -55841,7 +55838,7 @@
         <v>0</v>
       </c>
       <c r="W716" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X716" s="6" t="s">
         <v>37</v>
@@ -55915,7 +55912,7 @@
         <v>0</v>
       </c>
       <c r="W717" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X717" s="6" t="s">
         <v>37</v>
@@ -56145,7 +56142,7 @@
         <v>0</v>
       </c>
       <c r="W720" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X720" s="6" t="s">
         <v>37</v>
@@ -56293,7 +56290,7 @@
         <v>1</v>
       </c>
       <c r="W722" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X722" s="6" t="s">
         <v>37</v>
@@ -56597,7 +56594,7 @@
         <v>1</v>
       </c>
       <c r="W726" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X726" s="6" t="s">
         <v>37</v>
@@ -56823,7 +56820,7 @@
         <v>3</v>
       </c>
       <c r="W729" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X729" s="6" t="s">
         <v>37</v>
@@ -56975,7 +56972,7 @@
         <v>0</v>
       </c>
       <c r="W731" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X731" s="6" t="s">
         <v>37</v>
@@ -57049,7 +57046,7 @@
         <v>1</v>
       </c>
       <c r="W732" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X732" s="6" t="s">
         <v>37</v>
@@ -57123,7 +57120,7 @@
         <v>1</v>
       </c>
       <c r="W733" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X733" s="6" t="s">
         <v>37</v>
@@ -57197,7 +57194,7 @@
         <v>2</v>
       </c>
       <c r="W734" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X734" s="6" t="s">
         <v>37</v>
@@ -57497,7 +57494,7 @@
         <v>1</v>
       </c>
       <c r="W738" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X738" s="6" t="s">
         <v>37</v>
@@ -57645,7 +57642,7 @@
         <v>0</v>
       </c>
       <c r="W740" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X740" s="6" t="s">
         <v>37</v>
@@ -57719,7 +57716,7 @@
         <v>0</v>
       </c>
       <c r="W741" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X741" s="6" t="s">
         <v>37</v>
@@ -57871,7 +57868,7 @@
         <v>1</v>
       </c>
       <c r="W743" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X743" s="6" t="s">
         <v>37</v>
@@ -57945,7 +57942,7 @@
         <v>1</v>
       </c>
       <c r="W744" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X744" s="6" t="s">
         <v>37</v>
@@ -58093,7 +58090,7 @@
         <v>0</v>
       </c>
       <c r="W746" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X746" s="6" t="s">
         <v>37</v>
@@ -58167,7 +58164,7 @@
         <v>0</v>
       </c>
       <c r="W747" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X747" s="6" t="s">
         <v>37</v>
@@ -58241,7 +58238,7 @@
         <v>0</v>
       </c>
       <c r="W748" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X748" s="6" t="s">
         <v>37</v>
@@ -58315,7 +58312,7 @@
         <v>0</v>
       </c>
       <c r="W749" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X749" s="6" t="s">
         <v>37</v>
@@ -58545,7 +58542,7 @@
         <v>1</v>
       </c>
       <c r="W752" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X752" s="6" t="s">
         <v>37</v>
@@ -58770,7 +58767,7 @@
         <v>1</v>
       </c>
       <c r="W755" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X755" s="6" t="s">
         <v>37</v>
@@ -58921,7 +58918,7 @@
         <v>0</v>
       </c>
       <c r="W757" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X757" s="6" t="s">
         <v>37</v>
@@ -59300,7 +59297,7 @@
         <v>1</v>
       </c>
       <c r="W762" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X762" s="6" t="s">
         <v>37</v>
@@ -59605,7 +59602,7 @@
         <v>1</v>
       </c>
       <c r="W766" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X766" s="6" t="s">
         <v>35</v>
@@ -59679,7 +59676,7 @@
         <v>3</v>
       </c>
       <c r="W767" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X767" s="6" t="s">
         <v>37</v>
@@ -59760,7 +59757,7 @@
         <v>35</v>
       </c>
       <c r="Z768" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="769" spans="1:24" x14ac:dyDescent="0.2">
@@ -60292,7 +60289,7 @@
         <v>1</v>
       </c>
       <c r="W775" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X775" s="6" t="s">
         <v>37</v>
@@ -60366,7 +60363,7 @@
         <v>1</v>
       </c>
       <c r="W776" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X776" s="1" t="s">
         <v>37</v>
@@ -60442,11 +60439,11 @@
         <v>NA</v>
       </c>
       <c r="W777" s="1" t="str">
-        <f t="shared" ref="W777:W799" si="59">IF(T777=FALSE, "NA", "")</f>
+        <f t="shared" ref="W777:W795" si="59">IF(T777=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="X777" s="1" t="str">
-        <f t="shared" ref="X777:X799" si="60">IF(T777=FALSE, "NA", "")</f>
+        <f t="shared" ref="X777:X795" si="60">IF(T777=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
     </row>
@@ -61280,7 +61277,7 @@
         <v>0</v>
       </c>
       <c r="U788" s="15" t="str">
-        <f t="shared" ref="U788:U795" si="63">IF(T788=FALSE, "NA", "")</f>
+        <f t="shared" ref="U788:U794" si="63">IF(T788=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V788" s="15" t="str">
@@ -61297,7 +61294,7 @@
       </c>
       <c r="Y788" s="16"/>
       <c r="Z788" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="789" spans="1:26" x14ac:dyDescent="0.2">
@@ -61817,7 +61814,7 @@
         <v>0</v>
       </c>
       <c r="U795" s="1" t="str">
-        <f t="shared" si="63"/>
+        <f>IF(T795=FALSE, "NA", "")</f>
         <v>NA</v>
       </c>
       <c r="V795" s="1" t="str">
@@ -61975,7 +61972,7 @@
         <v>2</v>
       </c>
       <c r="W797" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X797" s="1" t="s">
         <v>37</v>
@@ -62123,14 +62120,1846 @@
         <v>2</v>
       </c>
       <c r="W799" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="X799" s="1" t="s">
         <v>37</v>
       </c>
     </row>
+    <row r="800" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A800" s="4">
+        <v>799</v>
+      </c>
+      <c r="B800" s="2">
+        <v>0</v>
+      </c>
+      <c r="C800" s="2">
+        <v>0</v>
+      </c>
+      <c r="D800" s="2">
+        <v>0</v>
+      </c>
+      <c r="E800" s="2">
+        <v>0</v>
+      </c>
+      <c r="F800" s="2">
+        <v>0</v>
+      </c>
+      <c r="G800" s="2">
+        <v>0</v>
+      </c>
+      <c r="H800" s="2">
+        <v>0</v>
+      </c>
+      <c r="I800" s="2">
+        <v>9.8849153412904194</v>
+      </c>
+      <c r="J800" s="2">
+        <v>0</v>
+      </c>
+      <c r="K800" s="2">
+        <v>9.0329254184544503</v>
+      </c>
+      <c r="L800" s="2">
+        <v>0</v>
+      </c>
+      <c r="M800" s="2">
+        <v>0</v>
+      </c>
+      <c r="N800" s="2">
+        <v>0</v>
+      </c>
+      <c r="O800" s="2">
+        <v>0</v>
+      </c>
+      <c r="P800" s="2">
+        <v>1.1375134274423699</v>
+      </c>
+      <c r="Q800" s="2">
+        <v>0</v>
+      </c>
+      <c r="R800" s="2">
+        <v>0</v>
+      </c>
+      <c r="S800" s="2">
+        <v>4.2548600686431799</v>
+      </c>
+      <c r="T800" t="b">
+        <v>0</v>
+      </c>
+      <c r="U800" s="1" t="str">
+        <f>IF(T800=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V800" s="1" t="str">
+        <f>IF(T800=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W800" s="1" t="str">
+        <f>IF(T800=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="X800" s="6" t="str">
+        <f>IF(T800=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="801" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A801" s="4">
+        <v>800</v>
+      </c>
+      <c r="B801" s="2">
+        <v>0</v>
+      </c>
+      <c r="C801" s="2">
+        <v>0</v>
+      </c>
+      <c r="D801" s="2">
+        <v>0</v>
+      </c>
+      <c r="E801" s="2">
+        <v>0</v>
+      </c>
+      <c r="F801" s="2">
+        <v>0</v>
+      </c>
+      <c r="G801" s="2">
+        <v>7.3929889163801201</v>
+      </c>
+      <c r="H801" s="2">
+        <v>0</v>
+      </c>
+      <c r="I801" s="2">
+        <v>8.9487222208703798</v>
+      </c>
+      <c r="J801" s="2">
+        <v>0</v>
+      </c>
+      <c r="K801" s="2">
+        <v>0</v>
+      </c>
+      <c r="L801" s="2">
+        <v>0</v>
+      </c>
+      <c r="M801" s="2">
+        <v>0</v>
+      </c>
+      <c r="N801" s="2">
+        <v>0</v>
+      </c>
+      <c r="O801" s="2">
+        <v>0</v>
+      </c>
+      <c r="P801" s="2">
+        <v>2.6371332415136401</v>
+      </c>
+      <c r="Q801" s="2">
+        <v>0</v>
+      </c>
+      <c r="R801" s="2">
+        <v>0</v>
+      </c>
+      <c r="S801" s="2">
+        <v>1.79815922830652</v>
+      </c>
+      <c r="T801" t="b">
+        <v>0</v>
+      </c>
+      <c r="U801" s="1" t="str">
+        <f t="shared" ref="U801:U822" si="64">IF(T801=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="V801" s="1" t="str">
+        <f t="shared" ref="V801:V822" si="65">IF(T801=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="W801" s="1" t="str">
+        <f t="shared" ref="W801:W823" si="66">IF(T801=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+      <c r="X801" s="6" t="str">
+        <f t="shared" ref="X801:X823" si="67">IF(T801=FALSE, "NA", "")</f>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="802" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A802" s="4">
+        <v>801</v>
+      </c>
+      <c r="B802" s="2">
+        <v>10.1799192294447</v>
+      </c>
+      <c r="C802" s="2">
+        <v>0</v>
+      </c>
+      <c r="D802" s="2">
+        <v>0</v>
+      </c>
+      <c r="E802" s="2">
+        <v>11.113497212085701</v>
+      </c>
+      <c r="F802" s="2">
+        <v>0</v>
+      </c>
+      <c r="G802" s="2">
+        <v>0</v>
+      </c>
+      <c r="H802" s="2">
+        <v>0</v>
+      </c>
+      <c r="I802" s="2">
+        <v>0</v>
+      </c>
+      <c r="J802" s="2">
+        <v>0</v>
+      </c>
+      <c r="K802" s="2">
+        <v>0</v>
+      </c>
+      <c r="L802" s="2">
+        <v>0</v>
+      </c>
+      <c r="M802" s="2">
+        <v>0</v>
+      </c>
+      <c r="N802" s="2">
+        <v>0</v>
+      </c>
+      <c r="O802" s="2">
+        <v>0</v>
+      </c>
+      <c r="P802" s="2">
+        <v>1.4081551648824999</v>
+      </c>
+      <c r="Q802" s="2">
+        <v>0</v>
+      </c>
+      <c r="R802" s="2">
+        <v>0</v>
+      </c>
+      <c r="S802" s="2">
+        <v>1.5877860199923599</v>
+      </c>
+      <c r="T802" t="b">
+        <v>1</v>
+      </c>
+      <c r="U802" s="1">
+        <v>28</v>
+      </c>
+      <c r="V802" s="1">
+        <v>3</v>
+      </c>
+      <c r="W802" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X802" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="803" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A803" s="4">
+        <v>802</v>
+      </c>
+      <c r="B803" s="2">
+        <v>0</v>
+      </c>
+      <c r="C803" s="2">
+        <v>0</v>
+      </c>
+      <c r="D803" s="2">
+        <v>0</v>
+      </c>
+      <c r="E803" s="2">
+        <v>0</v>
+      </c>
+      <c r="F803" s="2">
+        <v>0</v>
+      </c>
+      <c r="G803" s="2">
+        <v>0</v>
+      </c>
+      <c r="H803" s="2">
+        <v>11.8854178833758</v>
+      </c>
+      <c r="I803" s="2">
+        <v>12.175234723389201</v>
+      </c>
+      <c r="J803" s="2">
+        <v>0</v>
+      </c>
+      <c r="K803" s="2">
+        <v>0</v>
+      </c>
+      <c r="L803" s="2">
+        <v>0</v>
+      </c>
+      <c r="M803" s="2">
+        <v>0</v>
+      </c>
+      <c r="N803" s="2">
+        <v>0</v>
+      </c>
+      <c r="O803" s="2">
+        <v>0</v>
+      </c>
+      <c r="P803" s="2">
+        <v>3.0933312553613601</v>
+      </c>
+      <c r="Q803" s="2">
+        <v>0</v>
+      </c>
+      <c r="R803" s="2">
+        <v>0</v>
+      </c>
+      <c r="S803" s="2">
+        <v>3.3860755382031398</v>
+      </c>
+      <c r="T803" t="b">
+        <v>1</v>
+      </c>
+      <c r="U803" s="1">
+        <v>717</v>
+      </c>
+      <c r="V803" s="1">
+        <v>54</v>
+      </c>
+      <c r="W803" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X803" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="804" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A804" s="4">
+        <v>803</v>
+      </c>
+      <c r="B804" s="2">
+        <v>0</v>
+      </c>
+      <c r="C804" s="2">
+        <v>0</v>
+      </c>
+      <c r="D804" s="2">
+        <v>0</v>
+      </c>
+      <c r="E804" s="2">
+        <v>0</v>
+      </c>
+      <c r="F804" s="2">
+        <v>0</v>
+      </c>
+      <c r="G804" s="2">
+        <v>0</v>
+      </c>
+      <c r="H804" s="2">
+        <v>12.4100019679996</v>
+      </c>
+      <c r="I804" s="2">
+        <v>0</v>
+      </c>
+      <c r="J804" s="2">
+        <v>7.9153945313568403</v>
+      </c>
+      <c r="K804" s="2">
+        <v>0</v>
+      </c>
+      <c r="L804" s="2">
+        <v>0</v>
+      </c>
+      <c r="M804" s="2">
+        <v>0</v>
+      </c>
+      <c r="N804" s="2">
+        <v>0</v>
+      </c>
+      <c r="O804" s="2">
+        <v>0</v>
+      </c>
+      <c r="P804" s="2">
+        <v>2.29615814698044</v>
+      </c>
+      <c r="Q804" s="2">
+        <v>0</v>
+      </c>
+      <c r="R804" s="2">
+        <v>0</v>
+      </c>
+      <c r="S804" s="2">
+        <v>1.4265493168474399</v>
+      </c>
+      <c r="T804" t="b">
+        <v>1</v>
+      </c>
+      <c r="U804" s="1">
+        <v>20</v>
+      </c>
+      <c r="V804" s="1">
+        <v>1</v>
+      </c>
+      <c r="W804" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X804" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="805" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A805" s="4">
+        <v>804</v>
+      </c>
+      <c r="B805" s="2">
+        <v>12.600782614546199</v>
+      </c>
+      <c r="C805" s="2">
+        <v>0</v>
+      </c>
+      <c r="D805" s="2">
+        <v>0</v>
+      </c>
+      <c r="E805" s="2">
+        <v>9.2496266309246007</v>
+      </c>
+      <c r="F805" s="2">
+        <v>0</v>
+      </c>
+      <c r="G805" s="2">
+        <v>0</v>
+      </c>
+      <c r="H805" s="2">
+        <v>0</v>
+      </c>
+      <c r="I805" s="2">
+        <v>0</v>
+      </c>
+      <c r="J805" s="2">
+        <v>0</v>
+      </c>
+      <c r="K805" s="2">
+        <v>0</v>
+      </c>
+      <c r="L805" s="2">
+        <v>0</v>
+      </c>
+      <c r="M805" s="2">
+        <v>0</v>
+      </c>
+      <c r="N805" s="2">
+        <v>0</v>
+      </c>
+      <c r="O805" s="2">
+        <v>0</v>
+      </c>
+      <c r="P805" s="2">
+        <v>2.8000637840078499</v>
+      </c>
+      <c r="Q805" s="2">
+        <v>0</v>
+      </c>
+      <c r="R805" s="2">
+        <v>0</v>
+      </c>
+      <c r="S805" s="2">
+        <v>4.6634690632769402</v>
+      </c>
+      <c r="T805" t="b">
+        <v>0</v>
+      </c>
+      <c r="U805" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V805" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W805" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X805" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="806" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A806" s="4">
+        <v>805</v>
+      </c>
+      <c r="B806" s="2">
+        <v>0</v>
+      </c>
+      <c r="C806" s="2">
+        <v>0</v>
+      </c>
+      <c r="D806" s="2">
+        <v>10.943258618625</v>
+      </c>
+      <c r="E806" s="2">
+        <v>0</v>
+      </c>
+      <c r="F806" s="2">
+        <v>0</v>
+      </c>
+      <c r="G806" s="2">
+        <v>0</v>
+      </c>
+      <c r="H806" s="2">
+        <v>13.2027529055212</v>
+      </c>
+      <c r="I806" s="2">
+        <v>0</v>
+      </c>
+      <c r="J806" s="2">
+        <v>0</v>
+      </c>
+      <c r="K806" s="2">
+        <v>0</v>
+      </c>
+      <c r="L806" s="2">
+        <v>0</v>
+      </c>
+      <c r="M806" s="2">
+        <v>0</v>
+      </c>
+      <c r="N806" s="2">
+        <v>0</v>
+      </c>
+      <c r="O806" s="2">
+        <v>0</v>
+      </c>
+      <c r="P806" s="2">
+        <v>1.9905549267095499</v>
+      </c>
+      <c r="Q806" s="2">
+        <v>0</v>
+      </c>
+      <c r="R806" s="2">
+        <v>0</v>
+      </c>
+      <c r="S806" s="2">
+        <v>1.60455378122598</v>
+      </c>
+      <c r="T806" t="b">
+        <v>1</v>
+      </c>
+      <c r="U806" s="1">
+        <v>14</v>
+      </c>
+      <c r="V806" s="1">
+        <v>0</v>
+      </c>
+      <c r="W806" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X806" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="807" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A807" s="4">
+        <v>806</v>
+      </c>
+      <c r="B807" s="2">
+        <v>0</v>
+      </c>
+      <c r="C807" s="2">
+        <v>0</v>
+      </c>
+      <c r="D807" s="2">
+        <v>0</v>
+      </c>
+      <c r="E807" s="2">
+        <v>0</v>
+      </c>
+      <c r="F807" s="2">
+        <v>7.5933940478487303</v>
+      </c>
+      <c r="G807" s="2">
+        <v>0</v>
+      </c>
+      <c r="H807" s="2">
+        <v>8.7831793457706198</v>
+      </c>
+      <c r="I807" s="2">
+        <v>0</v>
+      </c>
+      <c r="J807" s="2">
+        <v>0</v>
+      </c>
+      <c r="K807" s="2">
+        <v>0</v>
+      </c>
+      <c r="L807" s="2">
+        <v>0</v>
+      </c>
+      <c r="M807" s="2">
+        <v>0</v>
+      </c>
+      <c r="N807" s="2">
+        <v>0</v>
+      </c>
+      <c r="O807" s="2">
+        <v>0</v>
+      </c>
+      <c r="P807" s="2">
+        <v>1.0565854287101499</v>
+      </c>
+      <c r="Q807" s="2">
+        <v>0</v>
+      </c>
+      <c r="R807" s="2">
+        <v>0</v>
+      </c>
+      <c r="S807" s="2">
+        <v>4.5718601725704602</v>
+      </c>
+      <c r="T807" t="b">
+        <v>0</v>
+      </c>
+      <c r="U807" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V807" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W807" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X807" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="808" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A808" s="4">
+        <v>807</v>
+      </c>
+      <c r="B808" s="2">
+        <v>0</v>
+      </c>
+      <c r="C808" s="2">
+        <v>0</v>
+      </c>
+      <c r="D808" s="2">
+        <v>0</v>
+      </c>
+      <c r="E808" s="2">
+        <v>0</v>
+      </c>
+      <c r="F808" s="2">
+        <v>10.6241066529776</v>
+      </c>
+      <c r="G808" s="2">
+        <v>0</v>
+      </c>
+      <c r="H808" s="2">
+        <v>0</v>
+      </c>
+      <c r="I808" s="2">
+        <v>0</v>
+      </c>
+      <c r="J808" s="2">
+        <v>0</v>
+      </c>
+      <c r="K808" s="2">
+        <v>0</v>
+      </c>
+      <c r="L808" s="2">
+        <v>0</v>
+      </c>
+      <c r="M808" s="2">
+        <v>12.2533150463554</v>
+      </c>
+      <c r="N808" s="2">
+        <v>0</v>
+      </c>
+      <c r="O808" s="2">
+        <v>0</v>
+      </c>
+      <c r="P808" s="2">
+        <v>1.0399730603675901</v>
+      </c>
+      <c r="Q808" s="2">
+        <v>0</v>
+      </c>
+      <c r="R808" s="2">
+        <v>0</v>
+      </c>
+      <c r="S808" s="2">
+        <v>4.7704730835956699</v>
+      </c>
+      <c r="T808" t="b">
+        <v>0</v>
+      </c>
+      <c r="U808" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V808" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W808" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X808" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="809" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A809" s="4">
+        <v>808</v>
+      </c>
+      <c r="B809" s="2">
+        <v>0</v>
+      </c>
+      <c r="C809" s="2">
+        <v>0</v>
+      </c>
+      <c r="D809" s="2">
+        <v>0</v>
+      </c>
+      <c r="E809" s="2">
+        <v>7.0305956957785503</v>
+      </c>
+      <c r="F809" s="2">
+        <v>0</v>
+      </c>
+      <c r="G809" s="2">
+        <v>0</v>
+      </c>
+      <c r="H809" s="2">
+        <v>0</v>
+      </c>
+      <c r="I809" s="2">
+        <v>0</v>
+      </c>
+      <c r="J809" s="2">
+        <v>9.5745810582094393</v>
+      </c>
+      <c r="K809" s="2">
+        <v>0</v>
+      </c>
+      <c r="L809" s="2">
+        <v>0</v>
+      </c>
+      <c r="M809" s="2">
+        <v>0</v>
+      </c>
+      <c r="N809" s="2">
+        <v>0</v>
+      </c>
+      <c r="O809" s="2">
+        <v>0</v>
+      </c>
+      <c r="P809" s="2">
+        <v>1.62387384519796</v>
+      </c>
+      <c r="Q809" s="2">
+        <v>0</v>
+      </c>
+      <c r="R809" s="2">
+        <v>0</v>
+      </c>
+      <c r="S809" s="2">
+        <v>2.0078811068909701</v>
+      </c>
+      <c r="T809" t="b">
+        <v>0</v>
+      </c>
+      <c r="U809" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V809" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W809" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X809" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="810" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A810" s="4">
+        <v>809</v>
+      </c>
+      <c r="B810" s="2">
+        <v>0</v>
+      </c>
+      <c r="C810" s="2">
+        <v>11.498051764838101</v>
+      </c>
+      <c r="D810" s="2">
+        <v>8.8228898329739707</v>
+      </c>
+      <c r="E810" s="2">
+        <v>0</v>
+      </c>
+      <c r="F810" s="2">
+        <v>0</v>
+      </c>
+      <c r="G810" s="2">
+        <v>0</v>
+      </c>
+      <c r="H810" s="2">
+        <v>0</v>
+      </c>
+      <c r="I810" s="2">
+        <v>0</v>
+      </c>
+      <c r="J810" s="2">
+        <v>0</v>
+      </c>
+      <c r="K810" s="2">
+        <v>0</v>
+      </c>
+      <c r="L810" s="2">
+        <v>0</v>
+      </c>
+      <c r="M810" s="2">
+        <v>0</v>
+      </c>
+      <c r="N810" s="2">
+        <v>0</v>
+      </c>
+      <c r="O810" s="2">
+        <v>0</v>
+      </c>
+      <c r="P810" s="2">
+        <v>1.41969577375168</v>
+      </c>
+      <c r="Q810" s="2">
+        <v>0</v>
+      </c>
+      <c r="R810" s="2">
+        <v>0</v>
+      </c>
+      <c r="S810" s="2">
+        <v>2.3546173808564999</v>
+      </c>
+      <c r="T810" t="b">
+        <v>1</v>
+      </c>
+      <c r="U810" s="1">
+        <v>14</v>
+      </c>
+      <c r="V810" s="1">
+        <v>0</v>
+      </c>
+      <c r="W810" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X810" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="811" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A811" s="4">
+        <v>810</v>
+      </c>
+      <c r="B811" s="2">
+        <v>10.053106366939801</v>
+      </c>
+      <c r="C811" s="2">
+        <v>0</v>
+      </c>
+      <c r="D811" s="2">
+        <v>0</v>
+      </c>
+      <c r="E811" s="2">
+        <v>0</v>
+      </c>
+      <c r="F811" s="2">
+        <v>0</v>
+      </c>
+      <c r="G811" s="2">
+        <v>0</v>
+      </c>
+      <c r="H811" s="2">
+        <v>0</v>
+      </c>
+      <c r="I811" s="2">
+        <v>0</v>
+      </c>
+      <c r="J811" s="2">
+        <v>0</v>
+      </c>
+      <c r="K811" s="2">
+        <v>0</v>
+      </c>
+      <c r="L811" s="2">
+        <v>11.6386466059423</v>
+      </c>
+      <c r="M811" s="2">
+        <v>0</v>
+      </c>
+      <c r="N811" s="2">
+        <v>0</v>
+      </c>
+      <c r="O811" s="2">
+        <v>0</v>
+      </c>
+      <c r="P811" s="2">
+        <v>2.2523585675655902</v>
+      </c>
+      <c r="Q811" s="2">
+        <v>0</v>
+      </c>
+      <c r="R811" s="2">
+        <v>0</v>
+      </c>
+      <c r="S811" s="2">
+        <v>1.36218239105687</v>
+      </c>
+      <c r="T811" t="b">
+        <v>1</v>
+      </c>
+      <c r="U811" s="1">
+        <v>3876</v>
+      </c>
+      <c r="V811" s="1">
+        <v>317</v>
+      </c>
+      <c r="W811" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="X811" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="812" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A812" s="4">
+        <v>811</v>
+      </c>
+      <c r="B812" s="2">
+        <v>0</v>
+      </c>
+      <c r="C812" s="2">
+        <v>9.8118348722457096</v>
+      </c>
+      <c r="D812" s="2">
+        <v>0</v>
+      </c>
+      <c r="E812" s="2">
+        <v>0</v>
+      </c>
+      <c r="F812" s="2">
+        <v>0</v>
+      </c>
+      <c r="G812" s="2">
+        <v>0</v>
+      </c>
+      <c r="H812" s="2">
+        <v>0</v>
+      </c>
+      <c r="I812" s="2">
+        <v>0</v>
+      </c>
+      <c r="J812" s="2">
+        <v>0</v>
+      </c>
+      <c r="K812" s="2">
+        <v>0</v>
+      </c>
+      <c r="L812" s="2">
+        <v>10.567359132065601</v>
+      </c>
+      <c r="M812" s="2">
+        <v>0</v>
+      </c>
+      <c r="N812" s="2">
+        <v>0</v>
+      </c>
+      <c r="O812" s="2">
+        <v>0</v>
+      </c>
+      <c r="P812" s="2">
+        <v>2.6573095664077</v>
+      </c>
+      <c r="Q812" s="2">
+        <v>0</v>
+      </c>
+      <c r="R812" s="2">
+        <v>0</v>
+      </c>
+      <c r="S812" s="2">
+        <v>2.9592198551733002</v>
+      </c>
+      <c r="T812" t="b">
+        <v>0</v>
+      </c>
+      <c r="U812" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V812" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W812" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X812" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="813" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A813" s="4">
+        <v>812</v>
+      </c>
+      <c r="B813" s="2">
+        <v>0</v>
+      </c>
+      <c r="C813" s="2">
+        <v>0</v>
+      </c>
+      <c r="D813" s="2">
+        <v>9.3988809746029407</v>
+      </c>
+      <c r="E813" s="2">
+        <v>0</v>
+      </c>
+      <c r="F813" s="2">
+        <v>0</v>
+      </c>
+      <c r="G813" s="2">
+        <v>0</v>
+      </c>
+      <c r="H813" s="2">
+        <v>0</v>
+      </c>
+      <c r="I813" s="2">
+        <v>0</v>
+      </c>
+      <c r="J813" s="2">
+        <v>10.0366371145633</v>
+      </c>
+      <c r="K813" s="2">
+        <v>0</v>
+      </c>
+      <c r="L813" s="2">
+        <v>0</v>
+      </c>
+      <c r="M813" s="2">
+        <v>0</v>
+      </c>
+      <c r="N813" s="2">
+        <v>0</v>
+      </c>
+      <c r="O813" s="2">
+        <v>0</v>
+      </c>
+      <c r="P813" s="2">
+        <v>2.98572155146497</v>
+      </c>
+      <c r="Q813" s="2">
+        <v>0</v>
+      </c>
+      <c r="R813" s="2">
+        <v>0</v>
+      </c>
+      <c r="S813" s="2">
+        <v>1.62447318669129</v>
+      </c>
+      <c r="T813" t="b">
+        <v>1</v>
+      </c>
+      <c r="U813" s="1">
+        <v>13</v>
+      </c>
+      <c r="V813" s="1">
+        <v>0</v>
+      </c>
+      <c r="W813" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X813" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="814" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A814" s="4">
+        <v>813</v>
+      </c>
+      <c r="B814" s="2">
+        <v>0</v>
+      </c>
+      <c r="C814" s="2">
+        <v>0</v>
+      </c>
+      <c r="D814" s="2">
+        <v>0</v>
+      </c>
+      <c r="E814" s="2">
+        <v>0</v>
+      </c>
+      <c r="F814" s="2">
+        <v>0</v>
+      </c>
+      <c r="G814" s="2">
+        <v>0</v>
+      </c>
+      <c r="H814" s="2">
+        <v>0</v>
+      </c>
+      <c r="I814" s="2">
+        <v>0</v>
+      </c>
+      <c r="J814" s="2">
+        <v>8.2792233059921294</v>
+      </c>
+      <c r="K814" s="2">
+        <v>0</v>
+      </c>
+      <c r="L814" s="2">
+        <v>0</v>
+      </c>
+      <c r="M814" s="2">
+        <v>12.231034044228799</v>
+      </c>
+      <c r="N814" s="2">
+        <v>0</v>
+      </c>
+      <c r="O814" s="2">
+        <v>0</v>
+      </c>
+      <c r="P814" s="2">
+        <v>1.7506441655104501</v>
+      </c>
+      <c r="Q814" s="2">
+        <v>0</v>
+      </c>
+      <c r="R814" s="2">
+        <v>0</v>
+      </c>
+      <c r="S814" s="2">
+        <v>3.0068125182234602</v>
+      </c>
+      <c r="T814" t="b">
+        <v>1</v>
+      </c>
+      <c r="U814" s="1">
+        <v>255</v>
+      </c>
+      <c r="V814" s="1">
+        <v>33</v>
+      </c>
+      <c r="W814" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="X814" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="815" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A815" s="4">
+        <v>814</v>
+      </c>
+      <c r="B815" s="2">
+        <v>0</v>
+      </c>
+      <c r="C815" s="2">
+        <v>0</v>
+      </c>
+      <c r="D815" s="2">
+        <v>0</v>
+      </c>
+      <c r="E815" s="2">
+        <v>7.53280892312468</v>
+      </c>
+      <c r="F815" s="2">
+        <v>0</v>
+      </c>
+      <c r="G815" s="2">
+        <v>0</v>
+      </c>
+      <c r="H815" s="2">
+        <v>0</v>
+      </c>
+      <c r="I815" s="2">
+        <v>5.9367872848597401</v>
+      </c>
+      <c r="J815" s="2">
+        <v>0</v>
+      </c>
+      <c r="K815" s="2">
+        <v>0</v>
+      </c>
+      <c r="L815" s="2">
+        <v>0</v>
+      </c>
+      <c r="M815" s="2">
+        <v>0</v>
+      </c>
+      <c r="N815" s="2">
+        <v>0</v>
+      </c>
+      <c r="O815" s="2">
+        <v>0</v>
+      </c>
+      <c r="P815" s="2">
+        <v>2.39403245739731</v>
+      </c>
+      <c r="Q815" s="2">
+        <v>0</v>
+      </c>
+      <c r="R815" s="2">
+        <v>0</v>
+      </c>
+      <c r="S815" s="2">
+        <v>4.6847625433859799</v>
+      </c>
+      <c r="T815" t="b">
+        <v>0</v>
+      </c>
+      <c r="U815" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V815" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W815" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X815" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="816" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A816" s="4">
+        <v>815</v>
+      </c>
+      <c r="B816" s="2">
+        <v>0</v>
+      </c>
+      <c r="C816" s="2">
+        <v>0</v>
+      </c>
+      <c r="D816" s="2">
+        <v>12.269966345256099</v>
+      </c>
+      <c r="E816" s="2">
+        <v>0</v>
+      </c>
+      <c r="F816" s="2">
+        <v>0</v>
+      </c>
+      <c r="G816" s="2">
+        <v>0</v>
+      </c>
+      <c r="H816" s="2">
+        <v>0</v>
+      </c>
+      <c r="I816" s="2">
+        <v>0</v>
+      </c>
+      <c r="J816" s="2">
+        <v>0</v>
+      </c>
+      <c r="K816" s="2">
+        <v>8.3352349280238602</v>
+      </c>
+      <c r="L816" s="2">
+        <v>0</v>
+      </c>
+      <c r="M816" s="2">
+        <v>0</v>
+      </c>
+      <c r="N816" s="2">
+        <v>0</v>
+      </c>
+      <c r="O816" s="2">
+        <v>0</v>
+      </c>
+      <c r="P816" s="2">
+        <v>1.73423138246891</v>
+      </c>
+      <c r="Q816" s="2">
+        <v>0</v>
+      </c>
+      <c r="R816" s="2">
+        <v>0</v>
+      </c>
+      <c r="S816" s="2">
+        <v>4.7024112217554004</v>
+      </c>
+      <c r="T816" t="b">
+        <v>0</v>
+      </c>
+      <c r="U816" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V816" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W816" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X816" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="817" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A817" s="4">
+        <v>816</v>
+      </c>
+      <c r="B817" s="2">
+        <v>0</v>
+      </c>
+      <c r="C817" s="2">
+        <v>0</v>
+      </c>
+      <c r="D817" s="2">
+        <v>7.3675982553050599</v>
+      </c>
+      <c r="E817" s="2">
+        <v>0</v>
+      </c>
+      <c r="F817" s="2">
+        <v>0</v>
+      </c>
+      <c r="G817" s="2">
+        <v>0</v>
+      </c>
+      <c r="H817" s="2">
+        <v>0</v>
+      </c>
+      <c r="I817" s="2">
+        <v>0</v>
+      </c>
+      <c r="J817" s="2">
+        <v>0</v>
+      </c>
+      <c r="K817" s="2">
+        <v>11.7747184563056</v>
+      </c>
+      <c r="L817" s="2">
+        <v>0</v>
+      </c>
+      <c r="M817" s="2">
+        <v>0</v>
+      </c>
+      <c r="N817" s="2">
+        <v>0</v>
+      </c>
+      <c r="O817" s="2">
+        <v>0</v>
+      </c>
+      <c r="P817" s="2">
+        <v>2.9903693964748901</v>
+      </c>
+      <c r="Q817" s="2">
+        <v>0</v>
+      </c>
+      <c r="R817" s="2">
+        <v>0</v>
+      </c>
+      <c r="S817" s="2">
+        <v>2.1936786650720599</v>
+      </c>
+      <c r="T817" t="b">
+        <v>0</v>
+      </c>
+      <c r="U817" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V817" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W817" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X817" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="818" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A818" s="4">
+        <v>817</v>
+      </c>
+      <c r="B818" s="2">
+        <v>7.9320625074463003</v>
+      </c>
+      <c r="C818" s="2">
+        <v>0</v>
+      </c>
+      <c r="D818" s="2">
+        <v>0</v>
+      </c>
+      <c r="E818" s="2">
+        <v>0</v>
+      </c>
+      <c r="F818" s="2">
+        <v>9.2936603137546907</v>
+      </c>
+      <c r="G818" s="2">
+        <v>0</v>
+      </c>
+      <c r="H818" s="2">
+        <v>0</v>
+      </c>
+      <c r="I818" s="2">
+        <v>0</v>
+      </c>
+      <c r="J818" s="2">
+        <v>0</v>
+      </c>
+      <c r="K818" s="2">
+        <v>0</v>
+      </c>
+      <c r="L818" s="2">
+        <v>0</v>
+      </c>
+      <c r="M818" s="2">
+        <v>0</v>
+      </c>
+      <c r="N818" s="2">
+        <v>0</v>
+      </c>
+      <c r="O818" s="2">
+        <v>0</v>
+      </c>
+      <c r="P818" s="2">
+        <v>1.2566391383775699</v>
+      </c>
+      <c r="Q818" s="2">
+        <v>0</v>
+      </c>
+      <c r="R818" s="2">
+        <v>0</v>
+      </c>
+      <c r="S818" s="2">
+        <v>4.4483723281843401</v>
+      </c>
+      <c r="T818" t="b">
+        <v>0</v>
+      </c>
+      <c r="U818" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V818" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W818" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X818" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="819" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A819" s="4">
+        <v>818</v>
+      </c>
+      <c r="B819" s="2">
+        <v>6.6149454660182299</v>
+      </c>
+      <c r="C819" s="2">
+        <v>0</v>
+      </c>
+      <c r="D819" s="2">
+        <v>0</v>
+      </c>
+      <c r="E819" s="2">
+        <v>0</v>
+      </c>
+      <c r="F819" s="2">
+        <v>0</v>
+      </c>
+      <c r="G819" s="2">
+        <v>0</v>
+      </c>
+      <c r="H819" s="2">
+        <v>0</v>
+      </c>
+      <c r="I819" s="2">
+        <v>0</v>
+      </c>
+      <c r="J819" s="2">
+        <v>0</v>
+      </c>
+      <c r="K819" s="2">
+        <v>0</v>
+      </c>
+      <c r="L819" s="2">
+        <v>0</v>
+      </c>
+      <c r="M819" s="2">
+        <v>12.6963269345418</v>
+      </c>
+      <c r="N819" s="2">
+        <v>0</v>
+      </c>
+      <c r="O819" s="2">
+        <v>0</v>
+      </c>
+      <c r="P819" s="2">
+        <v>2.215382679657</v>
+      </c>
+      <c r="Q819" s="2">
+        <v>0</v>
+      </c>
+      <c r="R819" s="2">
+        <v>0</v>
+      </c>
+      <c r="S819" s="2">
+        <v>4.0979379144830004</v>
+      </c>
+      <c r="T819" t="b">
+        <v>0</v>
+      </c>
+      <c r="U819" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V819" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W819" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X819" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="820" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A820" s="4">
+        <v>819</v>
+      </c>
+      <c r="B820" s="2">
+        <v>0</v>
+      </c>
+      <c r="C820" s="2">
+        <v>0</v>
+      </c>
+      <c r="D820" s="2">
+        <v>0</v>
+      </c>
+      <c r="E820" s="2">
+        <v>0</v>
+      </c>
+      <c r="F820" s="2">
+        <v>0</v>
+      </c>
+      <c r="G820" s="2">
+        <v>12.3716394863928</v>
+      </c>
+      <c r="H820" s="2">
+        <v>0</v>
+      </c>
+      <c r="I820" s="2">
+        <v>0</v>
+      </c>
+      <c r="J820" s="2">
+        <v>0</v>
+      </c>
+      <c r="K820" s="2">
+        <v>0</v>
+      </c>
+      <c r="L820" s="2">
+        <v>9.0266118011276806</v>
+      </c>
+      <c r="M820" s="2">
+        <v>0</v>
+      </c>
+      <c r="N820" s="2">
+        <v>0</v>
+      </c>
+      <c r="O820" s="2">
+        <v>0</v>
+      </c>
+      <c r="P820" s="2">
+        <v>1.2022744165510499</v>
+      </c>
+      <c r="Q820" s="2">
+        <v>0</v>
+      </c>
+      <c r="R820" s="2">
+        <v>0</v>
+      </c>
+      <c r="S820" s="2">
+        <v>3.4939161579029299</v>
+      </c>
+      <c r="T820" t="b">
+        <v>0</v>
+      </c>
+      <c r="U820" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V820" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W820" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X820" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="821" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A821" s="4">
+        <v>820</v>
+      </c>
+      <c r="B821" s="2">
+        <v>0</v>
+      </c>
+      <c r="C821" s="2">
+        <v>0</v>
+      </c>
+      <c r="D821" s="2">
+        <v>12.2701047970652</v>
+      </c>
+      <c r="E821" s="2">
+        <v>0</v>
+      </c>
+      <c r="F821" s="2">
+        <v>8.7926854139318493</v>
+      </c>
+      <c r="G821" s="2">
+        <v>0</v>
+      </c>
+      <c r="H821" s="2">
+        <v>0</v>
+      </c>
+      <c r="I821" s="2">
+        <v>0</v>
+      </c>
+      <c r="J821" s="2">
+        <v>0</v>
+      </c>
+      <c r="K821" s="2">
+        <v>0</v>
+      </c>
+      <c r="L821" s="2">
+        <v>0</v>
+      </c>
+      <c r="M821" s="2">
+        <v>0</v>
+      </c>
+      <c r="N821" s="2">
+        <v>0</v>
+      </c>
+      <c r="O821" s="2">
+        <v>0</v>
+      </c>
+      <c r="P821" s="2">
+        <v>1.95414192308767</v>
+      </c>
+      <c r="Q821" s="2">
+        <v>0</v>
+      </c>
+      <c r="R821" s="2">
+        <v>0</v>
+      </c>
+      <c r="S821" s="2">
+        <v>2.45935910320298</v>
+      </c>
+      <c r="T821" t="b">
+        <v>1</v>
+      </c>
+      <c r="U821" s="1">
+        <v>14</v>
+      </c>
+      <c r="V821" s="1">
+        <v>0</v>
+      </c>
+      <c r="W821" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="X821" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="822" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A822" s="4">
+        <v>821</v>
+      </c>
+      <c r="B822" s="2">
+        <v>0</v>
+      </c>
+      <c r="C822" s="2">
+        <v>0</v>
+      </c>
+      <c r="D822" s="2">
+        <v>0</v>
+      </c>
+      <c r="E822" s="2">
+        <v>0</v>
+      </c>
+      <c r="F822" s="2">
+        <v>9.0916108202257906</v>
+      </c>
+      <c r="G822" s="2">
+        <v>0</v>
+      </c>
+      <c r="H822" s="2">
+        <v>0</v>
+      </c>
+      <c r="I822" s="2">
+        <v>9.2256198236257099</v>
+      </c>
+      <c r="J822" s="2">
+        <v>0</v>
+      </c>
+      <c r="K822" s="2">
+        <v>0</v>
+      </c>
+      <c r="L822" s="2">
+        <v>0</v>
+      </c>
+      <c r="M822" s="2">
+        <v>0</v>
+      </c>
+      <c r="N822" s="2">
+        <v>0</v>
+      </c>
+      <c r="O822" s="2">
+        <v>0</v>
+      </c>
+      <c r="P822" s="2">
+        <v>1.8001209411952701</v>
+      </c>
+      <c r="Q822" s="2">
+        <v>0</v>
+      </c>
+      <c r="R822" s="2">
+        <v>0</v>
+      </c>
+      <c r="S822" s="2">
+        <v>3.56023919480845</v>
+      </c>
+      <c r="T822" t="b">
+        <v>0</v>
+      </c>
+      <c r="U822" s="1" t="str">
+        <f t="shared" si="64"/>
+        <v>NA</v>
+      </c>
+      <c r="V822" s="1" t="str">
+        <f t="shared" si="65"/>
+        <v>NA</v>
+      </c>
+      <c r="W822" s="1" t="str">
+        <f t="shared" si="66"/>
+        <v>NA</v>
+      </c>
+      <c r="X822" s="6" t="str">
+        <f t="shared" si="67"/>
+        <v>NA</v>
+      </c>
+    </row>
+    <row r="823" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A823" s="4">
+        <v>822</v>
+      </c>
+      <c r="B823" s="2">
+        <v>0</v>
+      </c>
+      <c r="C823" s="2">
+        <v>0</v>
+      </c>
+      <c r="D823" s="2">
+        <v>12.0934437052746</v>
+      </c>
+      <c r="E823" s="2">
+        <v>0</v>
+      </c>
+      <c r="F823" s="2">
+        <v>0</v>
+      </c>
+      <c r="G823" s="2">
+        <v>0</v>
+      </c>
+      <c r="H823" s="2">
+        <v>12.017020576820901</v>
+      </c>
+      <c r="I823" s="2">
+        <v>0</v>
+      </c>
+      <c r="J823" s="2">
+        <v>0</v>
+      </c>
+      <c r="K823" s="2">
+        <v>0</v>
+      </c>
+      <c r="L823" s="2">
+        <v>0</v>
+      </c>
+      <c r="M823" s="2">
+        <v>0</v>
+      </c>
+      <c r="N823" s="2">
+        <v>0</v>
+      </c>
+      <c r="O823" s="2">
+        <v>0</v>
+      </c>
+      <c r="P823" s="2">
+        <v>2.7483925756329799</v>
+      </c>
+      <c r="Q823" s="2">
+        <v>0</v>
+      </c>
+      <c r="R823" s="2">
+        <v>0</v>
+      </c>
+      <c r="S823" s="2">
+        <v>0.25818624477527402</v>
+      </c>
+      <c r="T823" t="b">
+        <v>1</v>
+      </c>
+      <c r="U823" s="1">
+        <v>15</v>
+      </c>
+      <c r="V823" s="1">
+        <v>1</v>
+      </c>
+      <c r="W823" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X823" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:Y799">
+  <conditionalFormatting sqref="A1:Y823">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$T1=TRUE</formula>
     </cfRule>

</xml_diff>